<commit_message>
Add flags for SF Bernie and SF Sersa
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/HD/Users/tm/Documents/Code/swgoh-shard-payout/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CAC38817-8CDE-8E46-9544-61E4A6B255F1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C013C5-23DB-A740-96E4-266679754C96}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15640" yWindow="1140" windowWidth="28800" windowHeight="15080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="280" yWindow="7420" windowWidth="28800" windowHeight="15080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,10 @@
   <definedNames>
     <definedName name="Z_6B6C704A_4C22_4616_B5BC_59850AE98E27_.wvu.Cols" localSheetId="0" hidden="1">Sheet1!$C:$D,Sheet1!$F:$G</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <customWorkbookViews>
+    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="124">
   <si>
     <t>Name</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>https://swgoh.gg/u/rikk91/</t>
+  </si>
+  <si>
+    <t>:flat_at:</t>
   </si>
 </sst>
 </file>
@@ -1454,7 +1457,7 @@
   <dimension ref="A1:V49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2274,7 +2277,7 @@
         <v>16</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>48</v>
+        <v>123</v>
       </c>
       <c r="G11" s="31" t="s">
         <v>92</v>
@@ -2353,7 +2356,7 @@
         <v>17</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="G12" s="31" t="s">
         <v>100</v>
@@ -5145,11 +5148,11 @@
     <sortCondition ref="D2:D38"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
+      <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
-      <selection sqref="A1:XFD1048576"/>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Update Movan Lipost flag to rage
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C013C5-23DB-A740-96E4-266679754C96}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D7FE16-2260-9949-9340-9AA0A7F50CDB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="7420" windowWidth="28800" windowHeight="15080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5480" yWindow="6540" windowWidth="28800" windowHeight="15080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1457,7 +1457,7 @@
   <dimension ref="A1:V49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2197,8 +2197,8 @@
       <c r="E10" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>95</v>
+      <c r="F10" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="G10" s="31" t="s">
         <v>122</v>
@@ -5148,11 +5148,11 @@
     <sortCondition ref="D2:D38"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Correct SF Sersa flag
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D7FE16-2260-9949-9340-9AA0A7F50CDB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6F0E56-E9C3-6C46-8715-637CF64EA0EB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="6540" windowWidth="28800" windowHeight="15080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12560" yWindow="5220" windowWidth="28800" windowHeight="15080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <customWorkbookViews>
+    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -405,7 +405,7 @@
     <t>https://swgoh.gg/u/rikk91/</t>
   </si>
   <si>
-    <t>:flat_at:</t>
+    <t>:flag_at:</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1457,7 @@
   <dimension ref="A1:V49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5148,11 +5148,11 @@
     <sortCondition ref="D2:D38"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
+      <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
-      <selection sqref="A1:XFD1048576"/>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Update flags for Darth Dentist, Kael Varlie, Eddie, Wookiefecker
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD5BEA6-0AFB-3842-8A9B-0230D8BA527B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFA2674-5B0E-D143-830A-FC8F3A494B61}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17700" yWindow="6260" windowWidth="28800" windowHeight="15080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="138">
   <si>
     <t>Name</t>
   </si>
@@ -258,9 +258,6 @@
     <t>Raucous</t>
   </si>
   <si>
-    <t>Eddie</t>
-  </si>
-  <si>
     <t>PDT</t>
   </si>
   <si>
@@ -406,6 +403,51 @@
   </si>
   <si>
     <t>:flag_at:</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/darkness39/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/landogerton/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/spook1322/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/fajhajaba/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/zombiegnome/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/jvu420/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/droopy/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/chiefnorbitthegreat/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/raucous1/</t>
+  </si>
+  <si>
+    <t>Eddie (IGN Aaron)</t>
+  </si>
+  <si>
+    <t>:flag_tw:</t>
+  </si>
+  <si>
+    <t>:flag_gb:</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/varlie/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/broly/</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
   </si>
 </sst>
 </file>
@@ -415,7 +457,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,8 +516,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -512,8 +562,20 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF305496"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -710,12 +772,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="dashDot">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -769,6 +864,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -781,40 +878,14 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="46">
     <dxf>
       <fill>
         <patternFill>
@@ -1457,7 +1528,7 @@
   <dimension ref="A1:V49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1570,7 +1641,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="6" t="s">
@@ -1634,7 +1705,7 @@
     <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18"/>
       <c r="B3" s="38" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="C3" s="7">
         <v>2</v>
@@ -1643,10 +1714,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="6" t="s">
@@ -1708,7 +1779,7 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="41" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="19" t="s">
@@ -1721,13 +1792,13 @@
         <v>3</v>
       </c>
       <c r="E4" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="G4" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H4" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -1789,7 +1860,7 @@
       </c>
     </row>
     <row r="5" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="39"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="19" t="s">
         <v>42</v>
       </c>
@@ -1806,7 +1877,7 @@
         <v>19</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -1868,7 +1939,7 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="39"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="13" t="s">
         <v>43</v>
       </c>
@@ -1879,13 +1950,13 @@
         <v>5</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H6" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -1947,7 +2018,7 @@
       </c>
     </row>
     <row r="7" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="19" t="s">
         <v>44</v>
       </c>
@@ -1961,10 +2032,10 @@
         <v>20</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H7" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2026,7 +2097,7 @@
       </c>
     </row>
     <row r="8" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="13" t="s">
         <v>45</v>
       </c>
@@ -2040,10 +2111,10 @@
         <v>16</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H8" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2105,7 +2176,7 @@
       </c>
     </row>
     <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="39"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="19" t="s">
         <v>46</v>
       </c>
@@ -2116,13 +2187,13 @@
         <v>8</v>
       </c>
       <c r="E9" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="G9" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H9" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2184,9 +2255,9 @@
       </c>
     </row>
     <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="39"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" s="7">
         <v>13</v>
@@ -2195,13 +2266,13 @@
         <v>13</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H10" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2263,7 +2334,7 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="39"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="19" t="s">
         <v>49</v>
       </c>
@@ -2277,10 +2348,10 @@
         <v>16</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H11" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2342,7 +2413,7 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="39"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="19" t="s">
         <v>50</v>
       </c>
@@ -2359,7 +2430,7 @@
         <v>19</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H12" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2421,7 +2492,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="39"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="19" t="s">
         <v>51</v>
       </c>
@@ -2438,7 +2509,7 @@
         <v>48</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H13" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2500,7 +2571,7 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="39"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="19" t="s">
         <v>52</v>
       </c>
@@ -2517,7 +2588,7 @@
         <v>48</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H14" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2579,7 +2650,7 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="19" t="s">
         <v>53</v>
       </c>
@@ -2596,7 +2667,7 @@
         <v>48</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H15" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2658,7 +2729,7 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="39"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="13" t="s">
         <v>54</v>
       </c>
@@ -2675,7 +2746,7 @@
         <v>22</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H16" s="29" t="s">
         <v>12</v>
@@ -2736,7 +2807,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="39"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="19" t="s">
         <v>55</v>
       </c>
@@ -2750,10 +2821,10 @@
         <v>31</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H17" s="31" t="s">
         <v>12</v>
@@ -2814,7 +2885,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="19" t="s">
         <v>56</v>
       </c>
@@ -2828,10 +2899,10 @@
         <v>31</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H18" s="31" t="s">
         <v>12</v>
@@ -2892,9 +2963,9 @@
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="40"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C19" s="7">
         <v>18</v>
@@ -2903,13 +2974,13 @@
         <v>18</v>
       </c>
       <c r="E19" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="G19" s="36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H19" s="31" t="s">
         <v>12</v>
@@ -2970,11 +3041,11 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="43" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" s="7">
         <v>19</v>
@@ -2983,13 +3054,13 @@
         <v>19</v>
       </c>
       <c r="E20" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="G20" s="36" t="s">
         <v>98</v>
-      </c>
-      <c r="G20" s="36" t="s">
-        <v>99</v>
       </c>
       <c r="H20" s="31" t="s">
         <v>12</v>
@@ -3050,7 +3121,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="19" t="s">
         <v>57</v>
       </c>
@@ -3061,13 +3132,13 @@
         <v>20</v>
       </c>
       <c r="E21" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>110</v>
-      </c>
       <c r="G21" s="36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H21" s="31" t="s">
         <v>12</v>
@@ -3128,7 +3199,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="19" t="s">
         <v>32</v>
       </c>
@@ -3145,7 +3216,7 @@
         <v>22</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H22" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3207,7 +3278,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="19" t="s">
         <v>33</v>
       </c>
@@ -3224,7 +3295,7 @@
         <v>22</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H23" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3286,7 +3357,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="19" t="s">
         <v>34</v>
       </c>
@@ -3303,7 +3374,7 @@
         <v>22</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H24" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3365,7 +3436,7 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="19" t="s">
         <v>35</v>
       </c>
@@ -3382,7 +3453,7 @@
         <v>22</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H25" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3444,7 +3515,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="13" t="s">
         <v>36</v>
       </c>
@@ -3461,7 +3532,7 @@
         <v>22</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H26" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3523,7 +3594,7 @@
       </c>
     </row>
     <row r="27" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="19" t="s">
         <v>37</v>
       </c>
@@ -3540,7 +3611,7 @@
         <v>22</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H27" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3602,7 +3673,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="42"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="13" t="s">
         <v>38</v>
       </c>
@@ -3619,7 +3690,7 @@
         <v>22</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H28" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3681,7 +3752,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="42"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="13" t="s">
         <v>39</v>
       </c>
@@ -3694,10 +3765,12 @@
       <c r="E29" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G29" s="23"/>
+      <c r="F29" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>135</v>
+      </c>
       <c r="H29" s="31" t="str">
         <f>Sheet2!$A$9</f>
         <v>EDT</v>
@@ -3758,7 +3831,7 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="19" t="s">
         <v>47</v>
       </c>
@@ -3775,7 +3848,7 @@
         <v>48</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H30" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3837,9 +3910,9 @@
       </c>
     </row>
     <row r="31" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="42"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C31" s="7">
         <v>30</v>
@@ -3854,7 +3927,7 @@
         <v>48</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H31" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3916,7 +3989,7 @@
       </c>
     </row>
     <row r="32" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="42"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="19" t="s">
         <v>58</v>
       </c>
@@ -3933,10 +4006,10 @@
         <v>22</v>
       </c>
       <c r="G32" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H32" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I32" s="24">
         <v>0</v>
@@ -3994,7 +4067,7 @@
       </c>
     </row>
     <row r="33" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="42"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="19" t="s">
         <v>59</v>
       </c>
@@ -4011,10 +4084,10 @@
         <v>22</v>
       </c>
       <c r="G33" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H33" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I33" s="24">
         <v>0</v>
@@ -4072,7 +4145,7 @@
       </c>
     </row>
     <row r="34" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="42"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="19" t="s">
         <v>60</v>
       </c>
@@ -4082,15 +4155,15 @@
       <c r="D34" s="7">
         <v>33</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>77</v>
+      <c r="F34" s="46" t="s">
+        <v>22</v>
       </c>
       <c r="G34" s="31"/>
       <c r="H34" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I34" s="24">
         <v>0</v>
@@ -4148,7 +4221,7 @@
       </c>
     </row>
     <row r="35" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="37" t="s">
         <v>61</v>
       </c>
@@ -4162,11 +4235,13 @@
         <v>30</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G35" s="31"/>
+        <v>76</v>
+      </c>
+      <c r="G35" s="31" t="s">
+        <v>136</v>
+      </c>
       <c r="H35" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I35" s="24">
         <v>0</v>
@@ -4224,7 +4299,7 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="42"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="19" t="s">
         <v>62</v>
       </c>
@@ -4238,11 +4313,11 @@
         <v>30</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G36" s="31"/>
       <c r="H36" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I36" s="24">
         <v>0</v>
@@ -4300,7 +4375,7 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="42"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="37" t="s">
         <v>63</v>
       </c>
@@ -4317,10 +4392,10 @@
         <v>22</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H37" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I37" s="24">
         <v>0</v>
@@ -4378,7 +4453,7 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="42"/>
+      <c r="A38" s="44"/>
       <c r="B38" s="19" t="s">
         <v>64</v>
       </c>
@@ -4391,12 +4466,14 @@
       <c r="E38" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F38" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G38" s="31"/>
+      <c r="F38" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" s="31" t="s">
+        <v>123</v>
+      </c>
       <c r="H38" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I38" s="24">
         <v>0</v>
@@ -4454,7 +4531,7 @@
       </c>
     </row>
     <row r="39" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="42"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="37" t="s">
         <v>65</v>
       </c>
@@ -4467,12 +4544,14 @@
       <c r="E39" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F39" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G39" s="29"/>
+      <c r="F39" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>124</v>
+      </c>
       <c r="H39" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I39" s="24">
         <v>0</v>
@@ -4530,7 +4609,7 @@
       </c>
     </row>
     <row r="40" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="42"/>
+      <c r="A40" s="44"/>
       <c r="B40" s="19" t="s">
         <v>66</v>
       </c>
@@ -4544,11 +4623,13 @@
         <v>30</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G40" s="31"/>
+        <v>76</v>
+      </c>
+      <c r="G40" s="31" t="s">
+        <v>125</v>
+      </c>
       <c r="H40" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I40" s="24">
         <v>0</v>
@@ -4606,7 +4687,7 @@
       </c>
     </row>
     <row r="41" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="42"/>
+      <c r="A41" s="44"/>
       <c r="B41" s="37" t="s">
         <v>67</v>
       </c>
@@ -4622,9 +4703,11 @@
       <c r="F41" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G41" s="31"/>
+      <c r="G41" s="31" t="s">
+        <v>126</v>
+      </c>
       <c r="H41" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I41" s="24">
         <v>0</v>
@@ -4682,7 +4765,7 @@
       </c>
     </row>
     <row r="42" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="42"/>
+      <c r="A42" s="44"/>
       <c r="B42" s="19" t="s">
         <v>68</v>
       </c>
@@ -4696,9 +4779,11 @@
         <v>30</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G42" s="36"/>
+        <v>76</v>
+      </c>
+      <c r="G42" s="36" t="s">
+        <v>127</v>
+      </c>
       <c r="H42" s="31" t="s">
         <v>13</v>
       </c>
@@ -4758,7 +4843,7 @@
       </c>
     </row>
     <row r="43" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="42"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="37" t="s">
         <v>69</v>
       </c>
@@ -4834,7 +4919,7 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="42"/>
+      <c r="A44" s="44"/>
       <c r="B44" s="19" t="s">
         <v>70</v>
       </c>
@@ -4850,9 +4935,11 @@
       <c r="F44" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G44" s="9"/>
+      <c r="G44" s="39" t="s">
+        <v>128</v>
+      </c>
       <c r="H44" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I44" s="24">
         <v>8.3333333333333329E-2</v>
@@ -4910,7 +4997,7 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="42"/>
+      <c r="A45" s="44"/>
       <c r="B45" s="37" t="s">
         <v>71</v>
       </c>
@@ -4924,11 +5011,13 @@
         <v>30</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G45" s="9"/>
+        <v>76</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="H45" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I45" s="24">
         <v>8.3333333333333329E-2</v>
@@ -4986,7 +5075,7 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="42"/>
+      <c r="A46" s="44"/>
       <c r="B46" s="19" t="s">
         <v>72</v>
       </c>
@@ -4999,12 +5088,14 @@
       <c r="E46" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F46" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G46" s="22"/>
+      <c r="F46" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" s="22" t="s">
+        <v>130</v>
+      </c>
       <c r="H46" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I46" s="24">
         <v>8.3333333333333329E-2</v>
@@ -5062,7 +5153,7 @@
       </c>
     </row>
     <row r="47" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="42"/>
+      <c r="A47" s="44"/>
       <c r="B47" s="37" t="s">
         <v>73</v>
       </c>
@@ -5075,12 +5166,14 @@
       <c r="E47" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F47" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G47" s="23"/>
+      <c r="F47" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" s="23" t="s">
+        <v>131</v>
+      </c>
       <c r="H47" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I47" s="24">
         <v>8.3333333333333329E-2</v>
@@ -5138,21 +5231,21 @@
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A48" s="42"/>
+      <c r="A48" s="44"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="42"/>
+      <c r="A49" s="44"/>
     </row>
   </sheetData>
   <sortState ref="B2:V38">
     <sortCondition ref="D2:D38"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -5161,251 +5254,231 @@
     <mergeCell ref="A20:A49"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:L3 K4:V47">
-    <cfRule type="expression" dxfId="49" priority="99">
+    <cfRule type="expression" dxfId="45" priority="102">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V3">
-    <cfRule type="expression" dxfId="48" priority="101">
+    <cfRule type="expression" dxfId="44" priority="104">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24:V36 G24:G47 E30:V31 B19:B36 E19:V23 C19:D47 K32:V47 E24:F36 B2:V18">
-    <cfRule type="expression" dxfId="47" priority="105">
+  <conditionalFormatting sqref="H24:V36 G24:G43 E30:V31 B19:B36 E19:V23 C19:D47 K32:V47 B2:V18 G45:G47 E24:F33 E35:F36">
+    <cfRule type="expression" dxfId="43" priority="108">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37 J37:V37">
-    <cfRule type="expression" dxfId="46" priority="82">
+    <cfRule type="expression" dxfId="42" priority="85">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38 J38:V38">
-    <cfRule type="expression" dxfId="45" priority="80">
+    <cfRule type="expression" dxfId="41" priority="83">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39 J39:V39">
-    <cfRule type="expression" dxfId="44" priority="78">
+    <cfRule type="expression" dxfId="40" priority="81">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40 J40:V40">
-    <cfRule type="expression" dxfId="43" priority="76">
+    <cfRule type="expression" dxfId="39" priority="79">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41 J41:V41">
-    <cfRule type="expression" dxfId="42" priority="74">
+    <cfRule type="expression" dxfId="38" priority="77">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42 J42:V42">
-    <cfRule type="expression" dxfId="41" priority="72">
+    <cfRule type="expression" dxfId="37" priority="75">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43 J43:V43 E43:F43 H43">
-    <cfRule type="expression" dxfId="40" priority="70">
+    <cfRule type="expression" dxfId="36" priority="73">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" dxfId="39" priority="68">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E38">
-    <cfRule type="expression" dxfId="38" priority="67">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="37" priority="66">
+    <cfRule type="expression" dxfId="35" priority="71">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="36" priority="65">
+    <cfRule type="expression" dxfId="34" priority="68">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="expression" dxfId="35" priority="64">
+    <cfRule type="expression" dxfId="33" priority="67">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42 H42">
-    <cfRule type="expression" dxfId="34" priority="63">
+    <cfRule type="expression" dxfId="32" priority="66">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44 J44:V44">
-    <cfRule type="expression" dxfId="33" priority="61">
+    <cfRule type="expression" dxfId="31" priority="64">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45 J45:V45 E45">
-    <cfRule type="expression" dxfId="32" priority="59">
+    <cfRule type="expression" dxfId="30" priority="62">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44:F44 H44">
-    <cfRule type="expression" dxfId="31" priority="57">
+    <cfRule type="expression" dxfId="29" priority="60">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46 J46:V46">
-    <cfRule type="expression" dxfId="30" priority="55">
+    <cfRule type="expression" dxfId="28" priority="58">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47 J47:V47 E47">
-    <cfRule type="expression" dxfId="29" priority="53">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
-    <cfRule type="expression" dxfId="28" priority="51">
+    <cfRule type="expression" dxfId="27" priority="56">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41">
-    <cfRule type="expression" dxfId="27" priority="45">
+    <cfRule type="expression" dxfId="26" priority="48">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="expression" dxfId="26" priority="35">
+    <cfRule type="expression" dxfId="25" priority="38">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="25" priority="34">
+    <cfRule type="expression" dxfId="24" priority="37">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="expression" dxfId="24" priority="33">
+    <cfRule type="expression" dxfId="23" priority="36">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="23" priority="32">
+    <cfRule type="expression" dxfId="22" priority="35">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41">
-    <cfRule type="expression" dxfId="22" priority="31">
+    <cfRule type="expression" dxfId="21" priority="34">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="21" priority="30">
+    <cfRule type="expression" dxfId="20" priority="33">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="20" priority="29">
+    <cfRule type="expression" dxfId="19" priority="32">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="19" priority="28">
+    <cfRule type="expression" dxfId="18" priority="31">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="18" priority="21">
+    <cfRule type="expression" dxfId="17" priority="24">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="17" priority="20">
+    <cfRule type="expression" dxfId="16" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="expression" dxfId="16" priority="19">
+    <cfRule type="expression" dxfId="15" priority="22">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="14" priority="21">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="expression" dxfId="14" priority="17">
+    <cfRule type="expression" dxfId="13" priority="20">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="12" priority="19">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45">
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="11" priority="18">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="10" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="10" priority="13">
+    <cfRule type="expression" dxfId="9" priority="16">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="8" priority="15">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="8" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F38">
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="7" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45">
-    <cfRule type="expression" dxfId="3" priority="5">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39:F39">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38:F38">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46:F46">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update payout with Punisher09brm
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFA2674-5B0E-D143-830A-FC8F3A494B61}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A52C65-636F-3948-BA59-F70965D545AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17700" yWindow="6260" windowWidth="28800" windowHeight="15080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="1240" windowWidth="25760" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <customWorkbookViews>
+    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="149">
   <si>
     <t>Name</t>
   </si>
@@ -216,9 +216,6 @@
     <t>Sideous</t>
   </si>
   <si>
-    <t>Darth Dentist</t>
-  </si>
-  <si>
     <t>Broly</t>
   </si>
   <si>
@@ -448,6 +445,42 @@
   </si>
   <si>
     <t>Taiwan</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/darkdentist/</t>
+  </si>
+  <si>
+    <t>Dark Dentist</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/loohoo/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/trueno0917/</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>:flag_ca:</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/miguelangel1506/</t>
+  </si>
+  <si>
+    <t>DarthSlappyJedi</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/darthslappyjedi/</t>
+  </si>
+  <si>
+    <t>EDT</t>
+  </si>
+  <si>
+    <t>Punisher09brm</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/punisher09brm/</t>
   </si>
 </sst>
 </file>
@@ -575,7 +608,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -805,12 +838,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -866,6 +910,12 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -878,14 +928,27 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="48">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF920000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1525,10 +1588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V49"/>
+  <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1612,15 +1675,15 @@
         <v>EDT</v>
       </c>
       <c r="T1" s="3" t="str">
-        <f>H32</f>
+        <f>H34</f>
         <v>CDT</v>
       </c>
       <c r="U1" s="3" t="str">
-        <f>H35</f>
+        <f>H37</f>
         <v>CDT</v>
       </c>
       <c r="V1" s="3" t="str">
-        <f>H36</f>
+        <f>H38</f>
         <v>CDT</v>
       </c>
     </row>
@@ -1641,9 +1704,11 @@
         <v>26</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>140</v>
+      </c>
       <c r="H2" s="6" t="s">
         <v>27</v>
       </c>
@@ -1705,7 +1770,7 @@
     <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18"/>
       <c r="B3" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C3" s="7">
         <v>2</v>
@@ -1714,10 +1779,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="6" t="s">
@@ -1778,8 +1843,8 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="45" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="19" t="s">
@@ -1792,13 +1857,13 @@
         <v>3</v>
       </c>
       <c r="E4" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="G4" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H4" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -1859,8 +1924,8 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="41"/>
+    <row r="5" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="45"/>
       <c r="B5" s="19" t="s">
         <v>42</v>
       </c>
@@ -1877,7 +1942,7 @@
         <v>19</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H5" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -1938,8 +2003,8 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="41"/>
+    <row r="6" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="45"/>
       <c r="B6" s="13" t="s">
         <v>43</v>
       </c>
@@ -1950,13 +2015,13 @@
         <v>5</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H6" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2017,8 +2082,8 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="41"/>
+    <row r="7" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="45"/>
       <c r="B7" s="19" t="s">
         <v>44</v>
       </c>
@@ -2032,10 +2097,10 @@
         <v>20</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H7" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2096,8 +2161,8 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="41"/>
+    <row r="8" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="45"/>
       <c r="B8" s="13" t="s">
         <v>45</v>
       </c>
@@ -2111,10 +2176,10 @@
         <v>16</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H8" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2175,8 +2240,8 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="41"/>
+    <row r="9" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="45"/>
       <c r="B9" s="19" t="s">
         <v>46</v>
       </c>
@@ -2187,13 +2252,13 @@
         <v>8</v>
       </c>
       <c r="E9" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="G9" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H9" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2255,9 +2320,9 @@
       </c>
     </row>
     <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="41"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C10" s="7">
         <v>13</v>
@@ -2266,13 +2331,13 @@
         <v>13</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H10" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2333,8 +2398,8 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="41"/>
+    <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="45"/>
       <c r="B11" s="19" t="s">
         <v>49</v>
       </c>
@@ -2348,10 +2413,10 @@
         <v>16</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H11" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2413,7 +2478,7 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="41"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="19" t="s">
         <v>50</v>
       </c>
@@ -2430,7 +2495,7 @@
         <v>19</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H12" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2492,7 +2557,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="41"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="19" t="s">
         <v>51</v>
       </c>
@@ -2509,7 +2574,7 @@
         <v>48</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H13" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2571,7 +2636,7 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="41"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="19" t="s">
         <v>52</v>
       </c>
@@ -2588,7 +2653,7 @@
         <v>48</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H14" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2650,7 +2715,7 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="41"/>
+      <c r="A15" s="45"/>
       <c r="B15" s="19" t="s">
         <v>53</v>
       </c>
@@ -2667,7 +2732,7 @@
         <v>48</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H15" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2729,7 +2794,7 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="41"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="13" t="s">
         <v>54</v>
       </c>
@@ -2746,7 +2811,7 @@
         <v>22</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H16" s="29" t="s">
         <v>12</v>
@@ -2807,7 +2872,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="41"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="19" t="s">
         <v>55</v>
       </c>
@@ -2821,10 +2886,10 @@
         <v>31</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H17" s="31" t="s">
         <v>12</v>
@@ -2885,7 +2950,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="41"/>
+      <c r="A18" s="45"/>
       <c r="B18" s="19" t="s">
         <v>56</v>
       </c>
@@ -2899,10 +2964,10 @@
         <v>31</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H18" s="31" t="s">
         <v>12</v>
@@ -2963,9 +3028,9 @@
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C19" s="7">
         <v>18</v>
@@ -2974,13 +3039,13 @@
         <v>18</v>
       </c>
       <c r="E19" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="G19" s="36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H19" s="31" t="s">
         <v>12</v>
@@ -3041,11 +3106,11 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="47" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" s="7">
         <v>19</v>
@@ -3054,13 +3119,13 @@
         <v>19</v>
       </c>
       <c r="E20" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="G20" s="36" t="s">
         <v>97</v>
-      </c>
-      <c r="G20" s="36" t="s">
-        <v>98</v>
       </c>
       <c r="H20" s="31" t="s">
         <v>12</v>
@@ -3121,7 +3186,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="44"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="19" t="s">
         <v>57</v>
       </c>
@@ -3132,13 +3197,13 @@
         <v>20</v>
       </c>
       <c r="E21" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="G21" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H21" s="31" t="s">
         <v>12</v>
@@ -3199,7 +3264,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="44"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="19" t="s">
         <v>32</v>
       </c>
@@ -3216,7 +3281,7 @@
         <v>22</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H22" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3277,8 +3342,8 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
+    <row r="23" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="48"/>
       <c r="B23" s="19" t="s">
         <v>33</v>
       </c>
@@ -3295,7 +3360,7 @@
         <v>22</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H23" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3356,8 +3421,8 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="44"/>
+    <row r="24" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="48"/>
       <c r="B24" s="19" t="s">
         <v>34</v>
       </c>
@@ -3374,7 +3439,7 @@
         <v>22</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H24" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3435,8 +3500,8 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
+    <row r="25" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="48"/>
       <c r="B25" s="19" t="s">
         <v>35</v>
       </c>
@@ -3453,7 +3518,7 @@
         <v>22</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H25" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3514,8 +3579,8 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
+    <row r="26" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="48"/>
       <c r="B26" s="13" t="s">
         <v>36</v>
       </c>
@@ -3532,7 +3597,7 @@
         <v>22</v>
       </c>
       <c r="G26" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H26" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3593,8 +3658,8 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
+    <row r="27" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="48"/>
       <c r="B27" s="19" t="s">
         <v>37</v>
       </c>
@@ -3611,7 +3676,7 @@
         <v>22</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H27" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3672,8 +3737,8 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
+    <row r="28" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="48"/>
       <c r="B28" s="13" t="s">
         <v>38</v>
       </c>
@@ -3690,7 +3755,7 @@
         <v>22</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H28" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3751,8 +3816,8 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
+    <row r="29" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="48"/>
       <c r="B29" s="13" t="s">
         <v>39</v>
       </c>
@@ -3769,7 +3834,7 @@
         <v>22</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H29" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3830,25 +3895,25 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
-      <c r="B30" s="19" t="s">
-        <v>47</v>
+    <row r="30" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="48"/>
+      <c r="B30" s="13" t="s">
+        <v>147</v>
       </c>
       <c r="C30" s="7">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="7">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>30</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>86</v>
+        <v>22</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>148</v>
       </c>
       <c r="H30" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3857,68 +3922,68 @@
       <c r="I30" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J30" s="28" t="s">
+      <c r="J30" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K30" s="26">
+      <c r="K30" s="33">
         <f>$I30+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L30" s="24">
+      <c r="L30" s="17">
         <f>$I30+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M30" s="24">
+      <c r="M30" s="17">
         <f>$I30+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N30" s="24">
+      <c r="N30" s="17">
         <f>$I30+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O30" s="24">
+      <c r="O30" s="17">
         <f>$I30+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P30" s="24">
+      <c r="P30" s="17">
         <f>$I30+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q30" s="24">
+      <c r="Q30" s="17">
         <f>$I30+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R30" s="24">
+      <c r="R30" s="17">
         <f>$I30+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S30" s="24">
+      <c r="S30" s="17">
         <f>$I30+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T30" s="24">
+      <c r="T30" s="17">
         <f>$I30+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U30" s="24">
+      <c r="U30" s="17">
         <f>$I30+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V30" s="24">
+      <c r="V30" s="17">
         <f>$I30+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="44"/>
+    <row r="31" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="48"/>
       <c r="B31" s="19" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="C31" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>30</v>
@@ -3926,8 +3991,8 @@
       <c r="F31" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G31" s="23" t="s">
-        <v>116</v>
+      <c r="G31" s="22" t="s">
+        <v>85</v>
       </c>
       <c r="H31" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3988,182 +4053,185 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="44"/>
+    <row r="32" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="48"/>
       <c r="B32" s="19" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="C32" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>30</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G32" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="H32" s="31" t="s">
-        <v>75</v>
+        <v>48</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32" s="31" t="str">
+        <f>Sheet2!$A$9</f>
+        <v>EDT</v>
       </c>
       <c r="I32" s="24">
-        <v>0</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="J32" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K32" s="26">
         <f>$I32+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
+        <v>1.375</v>
       </c>
       <c r="L32" s="24">
         <f>$I32+Sheet2!B$2/24</f>
-        <v>0.375</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="M32" s="24">
         <f>$I32+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="N32" s="24">
         <f>$I32+Sheet2!B$4/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="O32" s="24">
         <f>$I32+Sheet2!B$5/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="P32" s="24">
         <f>$I32+Sheet2!B$6/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="Q32" s="24">
         <f>$I32+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="R32" s="24">
         <f>$I32+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>1</v>
       </c>
       <c r="S32" s="24">
         <f>$I32+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="T32" s="24">
         <f>$I32+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="U32" s="24">
         <f>$I32+Sheet2!B$11/24</f>
-        <v>-0.25</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="V32" s="24">
         <f>$I32+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="44"/>
+        <v>0.66666666666666674</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="48"/>
       <c r="B33" s="19" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
       <c r="C33" s="7">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D33" s="7">
-        <v>32</v>
-      </c>
-      <c r="E33" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="42" t="s">
         <v>22</v>
       </c>
       <c r="G33" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="H33" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="I33" s="24">
-        <v>0</v>
-      </c>
-      <c r="J33" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="H33" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="I33" s="43">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="J33" s="44" t="s">
         <v>15</v>
       </c>
       <c r="K33" s="26">
         <f>$I33+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
+        <v>1.375</v>
       </c>
       <c r="L33" s="24">
         <f>$I33+Sheet2!B$2/24</f>
-        <v>0.375</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="M33" s="24">
         <f>$I33+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="N33" s="24">
         <f>$I33+Sheet2!B$4/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="O33" s="24">
         <f>$I33+Sheet2!B$5/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="P33" s="24">
         <f>$I33+Sheet2!B$6/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="Q33" s="24">
         <f>$I33+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="R33" s="24">
         <f>$I33+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>1</v>
       </c>
       <c r="S33" s="24">
         <f>$I33+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="T33" s="24">
         <f>$I33+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="U33" s="24">
         <f>$I33+Sheet2!B$11/24</f>
-        <v>-0.25</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="V33" s="24">
         <f>$I33+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="44"/>
+        <v>0.66666666666666674</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="48"/>
       <c r="B34" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C34" s="7">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D34" s="7">
-        <v>33</v>
-      </c>
-      <c r="E34" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F34" s="46" t="s">
+      <c r="F34" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="31"/>
+      <c r="G34" s="29" t="s">
+        <v>118</v>
+      </c>
       <c r="H34" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I34" s="24">
         <v>0</v>
@@ -4220,33 +4288,33 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="44"/>
-      <c r="B35" s="37" t="s">
-        <v>61</v>
+    <row r="35" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="48"/>
+      <c r="B35" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="C35" s="7">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D35" s="7">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>76</v>
+      <c r="F35" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="G35" s="31" t="s">
-        <v>136</v>
+        <v>81</v>
       </c>
       <c r="H35" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I35" s="24">
         <v>0</v>
       </c>
-      <c r="J35" s="30" t="s">
+      <c r="J35" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K35" s="26">
@@ -4298,31 +4366,33 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="44"/>
+    <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="48"/>
       <c r="B36" s="19" t="s">
-        <v>62</v>
+        <v>138</v>
       </c>
       <c r="C36" s="7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D36" s="7">
-        <v>35</v>
-      </c>
-      <c r="E36" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F36" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G36" s="31"/>
+      <c r="F36" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="31" t="s">
+        <v>137</v>
+      </c>
       <c r="H36" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I36" s="24">
         <v>0</v>
       </c>
-      <c r="J36" s="30" t="s">
+      <c r="J36" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K36" s="26">
@@ -4374,28 +4444,28 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="44"/>
+    <row r="37" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="48"/>
       <c r="B37" s="37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C37" s="7">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D37" s="7">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="20" t="s">
-        <v>22</v>
+      <c r="F37" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="H37" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I37" s="24">
         <v>0</v>
@@ -4452,28 +4522,28 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="44"/>
+    <row r="38" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="48"/>
       <c r="B38" s="19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C38" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D38" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E38" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F38" s="20" t="s">
-        <v>22</v>
+      <c r="F38" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="G38" s="31" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="H38" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I38" s="24">
         <v>0</v>
@@ -4530,16 +4600,16 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="44"/>
+    <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="48"/>
       <c r="B39" s="37" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C39" s="7">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D39" s="7">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E39" s="15" t="s">
         <v>30</v>
@@ -4547,11 +4617,11 @@
       <c r="F39" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="29" t="s">
-        <v>124</v>
+      <c r="G39" s="31" t="s">
+        <v>76</v>
       </c>
       <c r="H39" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I39" s="24">
         <v>0</v>
@@ -4608,28 +4678,28 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="44"/>
+    <row r="40" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="48"/>
       <c r="B40" s="19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C40" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D40" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E40" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F40" s="7" t="s">
-        <v>76</v>
+      <c r="F40" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="G40" s="31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H40" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I40" s="24">
         <v>0</v>
@@ -4686,28 +4756,28 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="44"/>
+    <row r="41" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="48"/>
       <c r="B41" s="37" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C41" s="7">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D41" s="7">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E41" s="15" t="s">
         <v>30</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G41" s="31" t="s">
-        <v>126</v>
+        <v>22</v>
+      </c>
+      <c r="G41" s="29" t="s">
+        <v>123</v>
       </c>
       <c r="H41" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I41" s="24">
         <v>0</v>
@@ -4764,338 +4834,340 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="44"/>
+    <row r="42" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="48"/>
       <c r="B42" s="19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C42" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D42" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>30</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G42" s="36" t="s">
-        <v>127</v>
+        <v>75</v>
+      </c>
+      <c r="G42" s="31" t="s">
+        <v>124</v>
       </c>
       <c r="H42" s="31" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="I42" s="24">
-        <v>4.1666666666666664E-2</v>
+        <v>0</v>
       </c>
       <c r="J42" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K42" s="26">
         <f>$I42+Sheet2!B$1/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L42" s="24">
         <f>$I42+Sheet2!B$2/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="M42" s="24">
         <f>$I42+Sheet2!B$3/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N42" s="24">
         <f>$I42+Sheet2!B$4/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="O42" s="24">
         <f>$I42+Sheet2!B$5/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="P42" s="24">
         <f>$I42+Sheet2!B$6/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="Q42" s="24">
         <f>$I42+Sheet2!B$7/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R42" s="24">
         <f>$I42+Sheet2!B$8/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="S42" s="24">
         <f>$I42+Sheet2!B$9/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="T42" s="24">
         <f>$I42+Sheet2!B$10/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="U42" s="24">
         <f>$I42+Sheet2!B$11/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.25</v>
       </c>
       <c r="V42" s="24">
         <f>$I42+Sheet2!B$12/24</f>
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="44"/>
+        <v>-0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="48"/>
       <c r="B43" s="37" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C43" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D43" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E43" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F43" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G43" s="36"/>
-      <c r="H43" s="37" t="s">
-        <v>13</v>
+      <c r="F43" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G43" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="H43" s="31" t="s">
+        <v>74</v>
       </c>
       <c r="I43" s="24">
-        <v>4.1666666666666664E-2</v>
+        <v>0</v>
       </c>
       <c r="J43" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K43" s="26">
         <f>$I43+Sheet2!B$1/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L43" s="24">
         <f>$I43+Sheet2!B$2/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="M43" s="24">
         <f>$I43+Sheet2!B$3/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N43" s="24">
         <f>$I43+Sheet2!B$4/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="O43" s="24">
         <f>$I43+Sheet2!B$5/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="P43" s="24">
         <f>$I43+Sheet2!B$6/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="Q43" s="24">
         <f>$I43+Sheet2!B$7/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R43" s="24">
         <f>$I43+Sheet2!B$8/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="S43" s="24">
         <f>$I43+Sheet2!B$9/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="T43" s="24">
         <f>$I43+Sheet2!B$10/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="U43" s="24">
         <f>$I43+Sheet2!B$11/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.25</v>
       </c>
       <c r="V43" s="24">
         <f>$I43+Sheet2!B$12/24</f>
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="44"/>
+        <v>-0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="48"/>
       <c r="B44" s="19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C44" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D44" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44" s="39" t="s">
-        <v>128</v>
+        <v>141</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G44" s="36" t="s">
+        <v>126</v>
       </c>
       <c r="H44" s="31" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="I44" s="24">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J44" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K44" s="26">
         <f>$I44+Sheet2!B$1/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="L44" s="24">
         <f>$I44+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M44" s="24">
         <f>$I44+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="N44" s="24">
         <f>$I44+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="O44" s="24">
         <f>$I44+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P44" s="24">
         <f>$I44+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q44" s="24">
         <f>$I44+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="R44" s="24">
         <f>$I44+Sheet2!B$8/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S44" s="24">
         <f>$I44+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="T44" s="24">
         <f>$I44+Sheet2!B$10/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="U44" s="24">
         <f>$I44+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="V44" s="24">
         <f>$I44+Sheet2!B$12/24</f>
-        <v>-0.20833333333333337</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="44"/>
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="48"/>
       <c r="B45" s="37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C45" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D45" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E45" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F45" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="H45" s="31" t="s">
-        <v>74</v>
+      <c r="F45" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H45" s="37" t="s">
+        <v>13</v>
       </c>
       <c r="I45" s="24">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J45" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K45" s="26">
         <f>$I45+Sheet2!B$1/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="L45" s="24">
         <f>$I45+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M45" s="24">
         <f>$I45+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="N45" s="24">
         <f>$I45+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="O45" s="24">
         <f>$I45+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P45" s="24">
         <f>$I45+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q45" s="24">
         <f>$I45+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="R45" s="24">
         <f>$I45+Sheet2!B$8/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S45" s="24">
         <f>$I45+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="T45" s="24">
         <f>$I45+Sheet2!B$10/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="U45" s="24">
         <f>$I45+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="V45" s="24">
         <f>$I45+Sheet2!B$12/24</f>
-        <v>-0.20833333333333337</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="44"/>
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="48"/>
       <c r="B46" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C46" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D46" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E46" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="F46" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G46" s="22" t="s">
-        <v>130</v>
+      <c r="G46" s="39" t="s">
+        <v>127</v>
       </c>
       <c r="H46" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I46" s="24">
         <v>8.3333333333333329E-2</v>
@@ -5152,28 +5224,28 @@
         <v>-0.20833333333333337</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="44"/>
+    <row r="47" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="48"/>
       <c r="B47" s="37" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C47" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D47" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E47" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F47" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="G47" s="23" t="s">
-        <v>131</v>
+      <c r="F47" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="H47" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I47" s="24">
         <v>8.3333333333333329E-2</v>
@@ -5230,256 +5302,422 @@
         <v>-0.20833333333333337</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A48" s="44"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="44"/>
+    <row r="48" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="48"/>
+      <c r="B48" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" s="7">
+        <v>45</v>
+      </c>
+      <c r="D48" s="7">
+        <v>45</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H48" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="I48" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J48" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K48" s="26">
+        <f>$I48+Sheet2!B$1/24</f>
+        <v>0.5</v>
+      </c>
+      <c r="L48" s="24">
+        <f>$I48+Sheet2!B$2/24</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M48" s="24">
+        <f>$I48+Sheet2!B$3/24</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="N48" s="24">
+        <f>$I48+Sheet2!B$4/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="O48" s="24">
+        <f>$I48+Sheet2!B$5/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P48" s="24">
+        <f>$I48+Sheet2!B$6/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="Q48" s="24">
+        <f>$I48+Sheet2!B$7/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R48" s="24">
+        <f>$I48+Sheet2!B$8/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="S48" s="24">
+        <f>$I48+Sheet2!B$9/24</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="T48" s="24">
+        <f>$I48+Sheet2!B$10/24</f>
+        <v>-0.125</v>
+      </c>
+      <c r="U48" s="24">
+        <f>$I48+Sheet2!B$11/24</f>
+        <v>-0.16666666666666669</v>
+      </c>
+      <c r="V48" s="24">
+        <f>$I48+Sheet2!B$12/24</f>
+        <v>-0.20833333333333337</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="48"/>
+      <c r="B49" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" s="7">
+        <v>46</v>
+      </c>
+      <c r="D49" s="7">
+        <v>46</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F49" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H49" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="I49" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J49" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K49" s="26">
+        <f>$I49+Sheet2!B$1/24</f>
+        <v>0.5</v>
+      </c>
+      <c r="L49" s="24">
+        <f>$I49+Sheet2!B$2/24</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M49" s="24">
+        <f>$I49+Sheet2!B$3/24</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="N49" s="24">
+        <f>$I49+Sheet2!B$4/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="O49" s="24">
+        <f>$I49+Sheet2!B$5/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P49" s="24">
+        <f>$I49+Sheet2!B$6/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="Q49" s="24">
+        <f>$I49+Sheet2!B$7/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R49" s="24">
+        <f>$I49+Sheet2!B$8/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="S49" s="24">
+        <f>$I49+Sheet2!B$9/24</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="T49" s="24">
+        <f>$I49+Sheet2!B$10/24</f>
+        <v>-0.125</v>
+      </c>
+      <c r="U49" s="24">
+        <f>$I49+Sheet2!B$11/24</f>
+        <v>-0.16666666666666669</v>
+      </c>
+      <c r="V49" s="24">
+        <f>$I49+Sheet2!B$12/24</f>
+        <v>-0.20833333333333337</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A50" s="48"/>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A51" s="48"/>
     </row>
   </sheetData>
-  <sortState ref="B2:V38">
-    <sortCondition ref="D2:D38"/>
+  <sortState ref="B2:V40">
+    <sortCondition ref="D2:D40"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
+      <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
-      <selection sqref="A1:XFD1048576"/>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
     <mergeCell ref="A4:A19"/>
-    <mergeCell ref="A20:A49"/>
+    <mergeCell ref="A20:A51"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L3 K4:V47">
-    <cfRule type="expression" dxfId="45" priority="102">
+  <conditionalFormatting sqref="K2:L3 K4:V29 K31:V49">
+    <cfRule type="expression" dxfId="47" priority="104">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V3">
-    <cfRule type="expression" dxfId="44" priority="104">
+    <cfRule type="expression" dxfId="46" priority="106">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24:V36 G24:G43 E30:V31 B19:B36 E19:V23 C19:D47 K32:V47 B2:V18 G45:G47 E24:F33 E35:F36">
-    <cfRule type="expression" dxfId="43" priority="108">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37 J37:V37">
-    <cfRule type="expression" dxfId="42" priority="85">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38 J38:V38">
-    <cfRule type="expression" dxfId="41" priority="83">
+  <conditionalFormatting sqref="G47:G49 E37:F38 E34:F35 B2:V29 H34:V38 K33:V49 G31:G45 C31:D49 B31:B38 E31:V32">
+    <cfRule type="expression" dxfId="45" priority="110">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39 J39:V39">
-    <cfRule type="expression" dxfId="40" priority="81">
+    <cfRule type="expression" dxfId="44" priority="87">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40 J40:V40">
-    <cfRule type="expression" dxfId="39" priority="79">
+    <cfRule type="expression" dxfId="43" priority="85">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41 J41:V41">
-    <cfRule type="expression" dxfId="38" priority="77">
+    <cfRule type="expression" dxfId="42" priority="83">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42 J42:V42">
-    <cfRule type="expression" dxfId="37" priority="75">
+    <cfRule type="expression" dxfId="41" priority="81">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43 J43:V43 E43:F43 H43">
-    <cfRule type="expression" dxfId="36" priority="73">
+  <conditionalFormatting sqref="B43 J43:V43">
+    <cfRule type="expression" dxfId="40" priority="79">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="expression" dxfId="35" priority="71">
+  <conditionalFormatting sqref="B44 J44:V44">
+    <cfRule type="expression" dxfId="39" priority="77">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
+  <conditionalFormatting sqref="B45 J45:V45 E45:F45 H45">
+    <cfRule type="expression" dxfId="38" priority="75">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="expression" dxfId="37" priority="73">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="expression" dxfId="36" priority="70">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="expression" dxfId="35" priority="69">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44 H44">
     <cfRule type="expression" dxfId="34" priority="68">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="expression" dxfId="33" priority="67">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42 H42">
-    <cfRule type="expression" dxfId="32" priority="66">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B44 J44:V44">
-    <cfRule type="expression" dxfId="31" priority="64">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45 J45:V45 E45">
-    <cfRule type="expression" dxfId="30" priority="62">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44:F44 H44">
-    <cfRule type="expression" dxfId="29" priority="60">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B46 J46:V46">
-    <cfRule type="expression" dxfId="28" priority="58">
+    <cfRule type="expression" dxfId="33" priority="66">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47 J47:V47 E47">
-    <cfRule type="expression" dxfId="27" priority="56">
+    <cfRule type="expression" dxfId="32" priority="64">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41">
-    <cfRule type="expression" dxfId="26" priority="48">
+  <conditionalFormatting sqref="E46:F46 H46">
+    <cfRule type="expression" dxfId="31" priority="62">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
+  <conditionalFormatting sqref="B48 J48:V48">
+    <cfRule type="expression" dxfId="30" priority="60">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49 J49:V49 E49">
+    <cfRule type="expression" dxfId="29" priority="58">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43">
+    <cfRule type="expression" dxfId="28" priority="50">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="expression" dxfId="27" priority="40">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="expression" dxfId="26" priority="39">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
     <cfRule type="expression" dxfId="25" priority="38">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
+  <conditionalFormatting sqref="I42">
     <cfRule type="expression" dxfId="24" priority="37">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
+  <conditionalFormatting sqref="I43">
     <cfRule type="expression" dxfId="23" priority="36">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
+  <conditionalFormatting sqref="I44">
     <cfRule type="expression" dxfId="22" priority="35">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
+  <conditionalFormatting sqref="I45">
     <cfRule type="expression" dxfId="21" priority="34">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
+  <conditionalFormatting sqref="I46">
     <cfRule type="expression" dxfId="20" priority="33">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="19" priority="32">
+  <conditionalFormatting sqref="H39">
+    <cfRule type="expression" dxfId="19" priority="26">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="18" priority="31">
+  <conditionalFormatting sqref="H40">
+    <cfRule type="expression" dxfId="18" priority="25">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
+  <conditionalFormatting sqref="H41">
     <cfRule type="expression" dxfId="17" priority="24">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38">
+  <conditionalFormatting sqref="H42">
     <cfRule type="expression" dxfId="16" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
+  <conditionalFormatting sqref="H43">
     <cfRule type="expression" dxfId="15" priority="22">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
+  <conditionalFormatting sqref="H47">
     <cfRule type="expression" dxfId="14" priority="21">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H41">
+  <conditionalFormatting sqref="I47">
     <cfRule type="expression" dxfId="13" priority="20">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H45">
+  <conditionalFormatting sqref="H48">
     <cfRule type="expression" dxfId="12" priority="19">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
+  <conditionalFormatting sqref="I48">
     <cfRule type="expression" dxfId="11" priority="18">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H46">
+  <conditionalFormatting sqref="H49">
     <cfRule type="expression" dxfId="10" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
+  <conditionalFormatting sqref="I49">
     <cfRule type="expression" dxfId="9" priority="16">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
-    <cfRule type="expression" dxfId="8" priority="15">
+  <conditionalFormatting sqref="F42">
+    <cfRule type="expression" dxfId="8" priority="12">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="7" priority="14">
+  <conditionalFormatting sqref="F44">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
+  <conditionalFormatting sqref="F47">
     <cfRule type="expression" dxfId="6" priority="10">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F42">
-    <cfRule type="expression" dxfId="5" priority="9">
+  <conditionalFormatting sqref="F39">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F45">
-    <cfRule type="expression" dxfId="4" priority="8">
+  <conditionalFormatting sqref="E41:F41">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F37">
+  <conditionalFormatting sqref="E40:F40">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39:F39">
+  <conditionalFormatting sqref="E48:F48">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E38:F38">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>MOD(ROW(),2)=1</formula>
+  <conditionalFormatting sqref="K30:V30">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>K$1=$H30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46:F46">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="B30:V30">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update Movan Lipost time zone
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm/Documents/Code/swgoh-squad-arena-payout-bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A52C65-636F-3948-BA59-F70965D545AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA38C6F-4A05-9544-A107-9AE36EDAEBE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="1240" windowWidth="25760" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,12 +29,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="152">
   <si>
     <t>Name</t>
   </si>
@@ -481,6 +486,15 @@
   </si>
   <si>
     <t>https://swgoh.gg/u/punisher09brm/</t>
+  </si>
+  <si>
+    <t>:flag_ru:</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>PETT</t>
   </si>
 </sst>
 </file>
@@ -854,7 +868,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -919,6 +933,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -933,19 +950,11 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="47">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1590,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1651,19 +1660,19 @@
         <v>9</v>
       </c>
       <c r="N1" s="3" t="str">
-        <f>H4</f>
+        <f>H5</f>
         <v>CEST</v>
       </c>
       <c r="O1" s="3" t="str">
-        <f>H6</f>
-        <v>CEST</v>
-      </c>
-      <c r="P1" s="3" t="str">
         <f>H7</f>
         <v>CEST</v>
       </c>
+      <c r="P1" s="3" t="str">
+        <f>H8</f>
+        <v>CEST</v>
+      </c>
       <c r="Q1" s="3" t="str">
-        <f>H8</f>
+        <f>H9</f>
         <v>CEST</v>
       </c>
       <c r="R1" s="3" t="str">
@@ -1843,106 +1852,105 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="45" t="s">
-        <v>29</v>
-      </c>
+    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="45"/>
       <c r="B4" s="19" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="C4" s="7">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D4" s="7">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="H4" s="29" t="str">
-        <f>Sheet2!$A$7</f>
-        <v>CEST</v>
+        <v>149</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>151</v>
       </c>
       <c r="I4" s="24">
-        <v>0.70833333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="J4" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="26">
         <f>$I4+Sheet2!B$1/24</f>
-        <v>1.125</v>
+        <v>0.91666666666666674</v>
       </c>
       <c r="L4" s="24">
         <f>$I4+Sheet2!B$2/24</f>
-        <v>1.0833333333333335</v>
+        <v>0.875</v>
       </c>
       <c r="M4" s="24">
         <f>$I4+Sheet2!B$3/24</f>
-        <v>1.0416666666666667</v>
+        <v>0.83333333333333326</v>
       </c>
       <c r="N4" s="24">
         <f>$I4+Sheet2!B$4/24</f>
-        <v>0.83333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="O4" s="24">
         <f>$I4+Sheet2!B$5/24</f>
-        <v>0.83333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="P4" s="24">
         <f>$I4+Sheet2!B$6/24</f>
-        <v>0.83333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="Q4" s="24">
         <f>$I4+Sheet2!B$7/24</f>
-        <v>0.79166666666666674</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="R4" s="24">
         <f>$I4+Sheet2!B$8/24</f>
-        <v>0.75</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="S4" s="24">
         <f>$I4+Sheet2!B$9/24</f>
-        <v>0.54166666666666674</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="T4" s="24">
         <f>$I4+Sheet2!B$10/24</f>
-        <v>0.5</v>
+        <v>0.29166666666666663</v>
       </c>
       <c r="U4" s="24">
         <f>$I4+Sheet2!B$11/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.25</v>
       </c>
       <c r="V4" s="24">
         <f>$I4+Sheet2!B$12/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.20833333333333331</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="45"/>
+      <c r="A5" s="46" t="s">
+        <v>29</v>
+      </c>
       <c r="B5" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>77</v>
+        <v>105</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>87</v>
       </c>
       <c r="H5" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -1954,7 +1962,7 @@
       <c r="J5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="26">
         <f>$I5+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
@@ -2004,24 +2012,24 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="45"/>
-      <c r="B6" s="13" t="s">
-        <v>43</v>
+      <c r="A6" s="46"/>
+      <c r="B6" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="C6" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="7">
-        <v>5</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>88</v>
+        <v>4</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>77</v>
       </c>
       <c r="H6" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2033,74 +2041,74 @@
       <c r="J6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="12">
         <f>$I6+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="24">
         <f>$I6+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="24">
         <f>$I6+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N6" s="17">
+      <c r="N6" s="24">
         <f>$I6+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O6" s="17">
+      <c r="O6" s="24">
         <f>$I6+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P6" s="17">
+      <c r="P6" s="24">
         <f>$I6+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="Q6" s="24">
         <f>$I6+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R6" s="17">
+      <c r="R6" s="24">
         <f>$I6+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S6" s="17">
+      <c r="S6" s="24">
         <f>$I6+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T6" s="17">
+      <c r="T6" s="24">
         <f>$I6+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U6" s="17">
+      <c r="U6" s="24">
         <f>$I6+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V6" s="17">
+      <c r="V6" s="24">
         <f>$I6+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="45"/>
-      <c r="B7" s="19" t="s">
-        <v>44</v>
+      <c r="A7" s="46"/>
+      <c r="B7" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C7" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="7">
-        <v>6</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>109</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>86</v>
+        <v>114</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="H7" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2112,74 +2120,74 @@
       <c r="J7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="27">
         <f>$I7+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L7" s="24">
+      <c r="L7" s="17">
         <f>$I7+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M7" s="24">
+      <c r="M7" s="17">
         <f>$I7+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="17">
         <f>$I7+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O7" s="24">
+      <c r="O7" s="17">
         <f>$I7+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P7" s="24">
+      <c r="P7" s="17">
         <f>$I7+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q7" s="24">
+      <c r="Q7" s="17">
         <f>$I7+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R7" s="24">
+      <c r="R7" s="17">
         <f>$I7+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S7" s="24">
+      <c r="S7" s="17">
         <f>$I7+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T7" s="24">
+      <c r="T7" s="17">
         <f>$I7+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U7" s="24">
+      <c r="U7" s="17">
         <f>$I7+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V7" s="24">
+      <c r="V7" s="17">
         <f>$I7+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="45"/>
-      <c r="B8" s="13" t="s">
-        <v>45</v>
+      <c r="A8" s="46"/>
+      <c r="B8" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="C8" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="7">
-        <v>7</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>89</v>
+        <v>110</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="H8" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2188,156 +2196,156 @@
       <c r="I8" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="J8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="27">
+      <c r="K8" s="26">
         <f>$I8+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="24">
         <f>$I8+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="24">
         <f>$I8+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="24">
         <f>$I8+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="24">
         <f>$I8+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="24">
         <f>$I8+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="Q8" s="24">
         <f>$I8+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R8" s="17">
+      <c r="R8" s="24">
         <f>$I8+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S8" s="17">
+      <c r="S8" s="24">
         <f>$I8+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T8" s="17">
+      <c r="T8" s="24">
         <f>$I8+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U8" s="17">
+      <c r="U8" s="24">
         <f>$I8+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V8" s="17">
+      <c r="V8" s="24">
         <f>$I8+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="45"/>
-      <c r="B9" s="19" t="s">
-        <v>46</v>
+      <c r="A9" s="46"/>
+      <c r="B9" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="C9" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="7">
-        <v>8</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>92</v>
+        <v>7</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" s="31" t="str">
+        <v>75</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="29" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
       <c r="I9" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="27">
         <f>$I9+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L9" s="24">
+      <c r="L9" s="17">
         <f>$I9+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M9" s="24">
+      <c r="M9" s="17">
         <f>$I9+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="17">
         <f>$I9+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O9" s="24">
+      <c r="O9" s="17">
         <f>$I9+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P9" s="24">
+      <c r="P9" s="17">
         <f>$I9+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q9" s="24">
+      <c r="Q9" s="17">
         <f>$I9+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R9" s="24">
+      <c r="R9" s="17">
         <f>$I9+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S9" s="24">
+      <c r="S9" s="17">
         <f>$I9+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T9" s="24">
+      <c r="T9" s="17">
         <f>$I9+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U9" s="24">
+      <c r="U9" s="17">
         <f>$I9+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V9" s="24">
+      <c r="V9" s="17">
         <f>$I9+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="45"/>
+    <row r="10" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="46"/>
       <c r="B10" s="19" t="s">
-        <v>119</v>
+        <v>46</v>
       </c>
       <c r="C10" s="7">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D10" s="7">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="20" t="s">
-        <v>48</v>
+      <c r="F10" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="H10" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2346,7 +2354,7 @@
       <c r="I10" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="26">
@@ -2399,7 +2407,7 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="45"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="19" t="s">
         <v>49</v>
       </c>
@@ -2478,7 +2486,7 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="19" t="s">
         <v>50</v>
       </c>
@@ -2557,7 +2565,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="19" t="s">
         <v>51</v>
       </c>
@@ -2636,7 +2644,7 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="45"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="19" t="s">
         <v>52</v>
       </c>
@@ -2715,7 +2723,7 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="45"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="19" t="s">
         <v>53</v>
       </c>
@@ -2794,7 +2802,7 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="45"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="13" t="s">
         <v>54</v>
       </c>
@@ -2872,7 +2880,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="45"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="19" t="s">
         <v>55</v>
       </c>
@@ -2950,7 +2958,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="45"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="19" t="s">
         <v>56</v>
       </c>
@@ -3028,7 +3036,7 @@
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="34" t="s">
         <v>112</v>
       </c>
@@ -3106,7 +3114,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="48" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="19" t="s">
@@ -3186,7 +3194,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="48"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="19" t="s">
         <v>57</v>
       </c>
@@ -3264,7 +3272,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="48"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="19" t="s">
         <v>32</v>
       </c>
@@ -3343,7 +3351,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="48"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="19" t="s">
         <v>33</v>
       </c>
@@ -3422,7 +3430,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="48"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="19" t="s">
         <v>34</v>
       </c>
@@ -3501,7 +3509,7 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="48"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="19" t="s">
         <v>35</v>
       </c>
@@ -3580,7 +3588,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="48"/>
+      <c r="A26" s="49"/>
       <c r="B26" s="13" t="s">
         <v>36</v>
       </c>
@@ -3659,7 +3667,7 @@
       </c>
     </row>
     <row r="27" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="48"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="19" t="s">
         <v>37</v>
       </c>
@@ -3738,7 +3746,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="48"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="13" t="s">
         <v>38</v>
       </c>
@@ -3817,7 +3825,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="48"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="13" t="s">
         <v>39</v>
       </c>
@@ -3896,7 +3904,7 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="48"/>
+      <c r="A30" s="49"/>
       <c r="B30" s="13" t="s">
         <v>147</v>
       </c>
@@ -3975,7 +3983,7 @@
       </c>
     </row>
     <row r="31" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="48"/>
+      <c r="A31" s="49"/>
       <c r="B31" s="19" t="s">
         <v>47</v>
       </c>
@@ -4054,7 +4062,7 @@
       </c>
     </row>
     <row r="32" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="48"/>
+      <c r="A32" s="49"/>
       <c r="B32" s="19" t="s">
         <v>116</v>
       </c>
@@ -4133,7 +4141,7 @@
       </c>
     </row>
     <row r="33" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="48"/>
+      <c r="A33" s="49"/>
       <c r="B33" s="19" t="s">
         <v>144</v>
       </c>
@@ -4211,7 +4219,7 @@
       </c>
     </row>
     <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="48"/>
+      <c r="A34" s="49"/>
       <c r="B34" s="19" t="s">
         <v>58</v>
       </c>
@@ -4289,7 +4297,7 @@
       </c>
     </row>
     <row r="35" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="48"/>
+      <c r="A35" s="49"/>
       <c r="B35" s="19" t="s">
         <v>59</v>
       </c>
@@ -4367,7 +4375,7 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="48"/>
+      <c r="A36" s="49"/>
       <c r="B36" s="19" t="s">
         <v>138</v>
       </c>
@@ -4445,7 +4453,7 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="48"/>
+      <c r="A37" s="49"/>
       <c r="B37" s="37" t="s">
         <v>60</v>
       </c>
@@ -4523,7 +4531,7 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="48"/>
+      <c r="A38" s="49"/>
       <c r="B38" s="19" t="s">
         <v>61</v>
       </c>
@@ -4601,7 +4609,7 @@
       </c>
     </row>
     <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="48"/>
+      <c r="A39" s="49"/>
       <c r="B39" s="37" t="s">
         <v>62</v>
       </c>
@@ -4679,7 +4687,7 @@
       </c>
     </row>
     <row r="40" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="48"/>
+      <c r="A40" s="49"/>
       <c r="B40" s="19" t="s">
         <v>63</v>
       </c>
@@ -4757,7 +4765,7 @@
       </c>
     </row>
     <row r="41" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="48"/>
+      <c r="A41" s="49"/>
       <c r="B41" s="37" t="s">
         <v>64</v>
       </c>
@@ -4835,7 +4843,7 @@
       </c>
     </row>
     <row r="42" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="48"/>
+      <c r="A42" s="49"/>
       <c r="B42" s="19" t="s">
         <v>65</v>
       </c>
@@ -4913,7 +4921,7 @@
       </c>
     </row>
     <row r="43" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="48"/>
+      <c r="A43" s="49"/>
       <c r="B43" s="37" t="s">
         <v>66</v>
       </c>
@@ -4991,7 +4999,7 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="48"/>
+      <c r="A44" s="49"/>
       <c r="B44" s="19" t="s">
         <v>67</v>
       </c>
@@ -5069,7 +5077,7 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="48"/>
+      <c r="A45" s="49"/>
       <c r="B45" s="37" t="s">
         <v>68</v>
       </c>
@@ -5147,7 +5155,7 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="48"/>
+      <c r="A46" s="49"/>
       <c r="B46" s="19" t="s">
         <v>69</v>
       </c>
@@ -5225,7 +5233,7 @@
       </c>
     </row>
     <row r="47" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="48"/>
+      <c r="A47" s="49"/>
       <c r="B47" s="37" t="s">
         <v>70</v>
       </c>
@@ -5303,7 +5311,7 @@
       </c>
     </row>
     <row r="48" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="48"/>
+      <c r="A48" s="49"/>
       <c r="B48" s="19" t="s">
         <v>71</v>
       </c>
@@ -5381,7 +5389,7 @@
       </c>
     </row>
     <row r="49" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="48"/>
+      <c r="A49" s="49"/>
       <c r="B49" s="37" t="s">
         <v>72</v>
       </c>
@@ -5459,10 +5467,10 @@
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A50" s="48"/>
+      <c r="A50" s="49"/>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A51" s="48"/>
+      <c r="A51" s="49"/>
     </row>
   </sheetData>
   <sortState ref="B2:V40">
@@ -5478,242 +5486,237 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
-    <mergeCell ref="A4:A19"/>
+    <mergeCell ref="A5:A19"/>
     <mergeCell ref="A20:A51"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L3 K4:V29 K31:V49">
-    <cfRule type="expression" dxfId="47" priority="104">
+  <conditionalFormatting sqref="K2:L4 K4:V49">
+    <cfRule type="expression" dxfId="46" priority="104">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:V3">
-    <cfRule type="expression" dxfId="46" priority="106">
+  <conditionalFormatting sqref="K2:V4">
+    <cfRule type="expression" dxfId="45" priority="106">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G47:G49 E37:F38 E34:F35 B2:V29 H34:V38 K33:V49 G31:G45 C31:D49 B31:B38 E31:V32">
-    <cfRule type="expression" dxfId="45" priority="110">
+  <conditionalFormatting sqref="G47:G49 E37:F38 E34:F35 H34:V38 K33:V49 G31:G45 C31:D49 B31:B38 E31:V32 B2:V29">
+    <cfRule type="expression" dxfId="44" priority="110">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39 J39:V39">
-    <cfRule type="expression" dxfId="44" priority="87">
+    <cfRule type="expression" dxfId="43" priority="87">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40 J40:V40">
-    <cfRule type="expression" dxfId="43" priority="85">
+    <cfRule type="expression" dxfId="42" priority="85">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41 J41:V41">
-    <cfRule type="expression" dxfId="42" priority="83">
+    <cfRule type="expression" dxfId="41" priority="83">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42 J42:V42">
-    <cfRule type="expression" dxfId="41" priority="81">
+    <cfRule type="expression" dxfId="40" priority="81">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43 J43:V43">
-    <cfRule type="expression" dxfId="40" priority="79">
+    <cfRule type="expression" dxfId="39" priority="79">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44 J44:V44">
-    <cfRule type="expression" dxfId="39" priority="77">
+    <cfRule type="expression" dxfId="38" priority="77">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45 J45:V45 E45:F45 H45">
-    <cfRule type="expression" dxfId="38" priority="75">
+    <cfRule type="expression" dxfId="37" priority="75">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="37" priority="73">
+    <cfRule type="expression" dxfId="36" priority="73">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="expression" dxfId="36" priority="70">
+    <cfRule type="expression" dxfId="35" priority="70">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="expression" dxfId="35" priority="69">
+    <cfRule type="expression" dxfId="34" priority="69">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44 H44">
-    <cfRule type="expression" dxfId="34" priority="68">
+    <cfRule type="expression" dxfId="33" priority="68">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46 J46:V46">
-    <cfRule type="expression" dxfId="33" priority="66">
+    <cfRule type="expression" dxfId="32" priority="66">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47 J47:V47 E47">
-    <cfRule type="expression" dxfId="32" priority="64">
+    <cfRule type="expression" dxfId="31" priority="64">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46:F46 H46">
-    <cfRule type="expression" dxfId="31" priority="62">
+    <cfRule type="expression" dxfId="30" priority="62">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48 J48:V48">
-    <cfRule type="expression" dxfId="30" priority="60">
+    <cfRule type="expression" dxfId="29" priority="60">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49 J49:V49 E49">
-    <cfRule type="expression" dxfId="29" priority="58">
+    <cfRule type="expression" dxfId="28" priority="58">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="28" priority="50">
+    <cfRule type="expression" dxfId="27" priority="50">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="expression" dxfId="27" priority="40">
+    <cfRule type="expression" dxfId="26" priority="40">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="26" priority="39">
+    <cfRule type="expression" dxfId="25" priority="39">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41">
-    <cfRule type="expression" dxfId="25" priority="38">
+    <cfRule type="expression" dxfId="24" priority="38">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="24" priority="37">
+    <cfRule type="expression" dxfId="23" priority="37">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="23" priority="36">
+    <cfRule type="expression" dxfId="22" priority="36">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="22" priority="35">
+    <cfRule type="expression" dxfId="21" priority="35">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45">
-    <cfRule type="expression" dxfId="21" priority="34">
+    <cfRule type="expression" dxfId="20" priority="34">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="20" priority="33">
+    <cfRule type="expression" dxfId="19" priority="33">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="expression" dxfId="19" priority="26">
+    <cfRule type="expression" dxfId="18" priority="26">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="expression" dxfId="18" priority="25">
+    <cfRule type="expression" dxfId="17" priority="25">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="expression" dxfId="17" priority="24">
+    <cfRule type="expression" dxfId="16" priority="24">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="expression" dxfId="16" priority="23">
+    <cfRule type="expression" dxfId="15" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="expression" dxfId="15" priority="22">
+    <cfRule type="expression" dxfId="14" priority="22">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="expression" dxfId="14" priority="21">
+    <cfRule type="expression" dxfId="13" priority="21">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="13" priority="20">
+    <cfRule type="expression" dxfId="12" priority="20">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="expression" dxfId="12" priority="19">
+    <cfRule type="expression" dxfId="11" priority="19">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="11" priority="18">
+    <cfRule type="expression" dxfId="10" priority="18">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="expression" dxfId="10" priority="17">
+    <cfRule type="expression" dxfId="9" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="expression" dxfId="9" priority="16">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42">
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="7" priority="12">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44">
-    <cfRule type="expression" dxfId="7" priority="11">
+    <cfRule type="expression" dxfId="6" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47">
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="5" priority="10">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41:F41">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40:F40">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:F48">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30:V30">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>K$1=$H30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:V30">
@@ -5731,7 +5734,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Correct Movan Lipost TZ to 11 UTC/GMT instead of 12 UCT/GMT
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA38C6F-4A05-9544-A107-9AE36EDAEBE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF9460C-A099-054B-99C9-0709FCF35E51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="1240" windowWidth="25760" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -494,7 +494,7 @@
     <t>Russia</t>
   </si>
   <si>
-    <t>PETT</t>
+    <t>VLAS</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -1876,58 +1876,58 @@
         <v>151</v>
       </c>
       <c r="I4" s="24">
-        <v>0.5</v>
+        <v>11.458333333333334</v>
       </c>
       <c r="J4" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="26">
         <f>$I4+Sheet2!B$1/24</f>
-        <v>0.91666666666666674</v>
+        <v>11.875</v>
       </c>
       <c r="L4" s="24">
         <f>$I4+Sheet2!B$2/24</f>
-        <v>0.875</v>
+        <v>11.833333333333334</v>
       </c>
       <c r="M4" s="24">
         <f>$I4+Sheet2!B$3/24</f>
-        <v>0.83333333333333326</v>
+        <v>11.791666666666668</v>
       </c>
       <c r="N4" s="24">
         <f>$I4+Sheet2!B$4/24</f>
-        <v>0.625</v>
+        <v>11.583333333333334</v>
       </c>
       <c r="O4" s="24">
         <f>$I4+Sheet2!B$5/24</f>
-        <v>0.625</v>
+        <v>11.583333333333334</v>
       </c>
       <c r="P4" s="24">
         <f>$I4+Sheet2!B$6/24</f>
-        <v>0.625</v>
+        <v>11.583333333333334</v>
       </c>
       <c r="Q4" s="24">
         <f>$I4+Sheet2!B$7/24</f>
-        <v>0.58333333333333337</v>
+        <v>11.541666666666668</v>
       </c>
       <c r="R4" s="24">
         <f>$I4+Sheet2!B$8/24</f>
-        <v>0.54166666666666663</v>
+        <v>11.5</v>
       </c>
       <c r="S4" s="24">
         <f>$I4+Sheet2!B$9/24</f>
-        <v>0.33333333333333337</v>
+        <v>11.291666666666668</v>
       </c>
       <c r="T4" s="24">
         <f>$I4+Sheet2!B$10/24</f>
-        <v>0.29166666666666663</v>
+        <v>11.25</v>
       </c>
       <c r="U4" s="24">
         <f>$I4+Sheet2!B$11/24</f>
-        <v>0.25</v>
+        <v>11.208333333333334</v>
       </c>
       <c r="V4" s="24">
         <f>$I4+Sheet2!B$12/24</f>
-        <v>0.20833333333333331</v>
+        <v>11.166666666666668</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="17" x14ac:dyDescent="0.2">
@@ -5477,11 +5477,11 @@
     <sortCondition ref="D2:D40"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Sort each payout by IGN alphabetical order
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF9460C-A099-054B-99C9-0709FCF35E51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECF0470-F7B0-BF4B-9A33-11695E2CB0F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="1240" windowWidth="25760" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="1240" windowWidth="33700" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="154">
   <si>
     <t>Name</t>
   </si>
@@ -495,6 +495,12 @@
   </si>
   <si>
     <t>VLAS</t>
+  </si>
+  <si>
+    <t>PSUlion</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/psulion/</t>
   </si>
 </sst>
 </file>
@@ -868,7 +874,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -929,6 +935,9 @@
     <xf numFmtId="164" fontId="7" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1597,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V51"/>
+  <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:V39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1660,11 +1669,11 @@
         <v>9</v>
       </c>
       <c r="N1" s="3" t="str">
-        <f>H5</f>
+        <f>H11</f>
         <v>CEST</v>
       </c>
       <c r="O1" s="3" t="str">
-        <f>H7</f>
+        <f>H6</f>
         <v>CEST</v>
       </c>
       <c r="P1" s="3" t="str">
@@ -1672,27 +1681,27 @@
         <v>CEST</v>
       </c>
       <c r="Q1" s="3" t="str">
-        <f>H9</f>
+        <f>H12</f>
         <v>CEST</v>
       </c>
       <c r="R1" s="3" t="str">
-        <f>H19</f>
+        <f>H18</f>
         <v>BST</v>
       </c>
       <c r="S1" s="3" t="str">
-        <f>H22</f>
+        <f>H32</f>
         <v>EDT</v>
       </c>
       <c r="T1" s="3" t="str">
-        <f>H34</f>
+        <f>H42</f>
         <v>CDT</v>
       </c>
       <c r="U1" s="3" t="str">
-        <f>H37</f>
+        <f>H36</f>
         <v>CDT</v>
       </c>
       <c r="V1" s="3" t="str">
-        <f>H38</f>
+        <f>H39</f>
         <v>CDT</v>
       </c>
     </row>
@@ -1858,7 +1867,7 @@
         <v>119</v>
       </c>
       <c r="C4" s="7">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D4" s="7">
         <v>13</v>
@@ -1930,39 +1939,37 @@
         <v>11.166666666666668</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="s">
-        <v>29</v>
-      </c>
+    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="46"/>
       <c r="B5" s="19" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C5" s="7">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D5" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" s="29" t="str">
+        <v>20</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="31" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
       <c r="I5" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="12">
         <f>$I5+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
@@ -2012,24 +2019,26 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
-      <c r="B6" s="19" t="s">
-        <v>42</v>
+      <c r="A6" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C6" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" s="7">
-        <v>4</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>77</v>
+        <v>2</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="H6" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2041,74 +2050,74 @@
       <c r="J6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="27">
         <f>$I6+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L6" s="24">
+      <c r="L6" s="17">
         <f>$I6+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M6" s="24">
+      <c r="M6" s="17">
         <f>$I6+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="17">
         <f>$I6+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6" s="17">
         <f>$I6+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P6" s="24">
+      <c r="P6" s="17">
         <f>$I6+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q6" s="24">
+      <c r="Q6" s="17">
         <f>$I6+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R6" s="24">
+      <c r="R6" s="17">
         <f>$I6+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S6" s="24">
+      <c r="S6" s="17">
         <f>$I6+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T6" s="24">
+      <c r="T6" s="17">
         <f>$I6+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U6" s="24">
+      <c r="U6" s="17">
         <f>$I6+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V6" s="24">
+      <c r="V6" s="17">
         <f>$I6+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="46"/>
-      <c r="B7" s="13" t="s">
-        <v>43</v>
+      <c r="A7" s="47"/>
+      <c r="B7" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="C7" s="7">
         <v>5</v>
       </c>
       <c r="D7" s="7">
-        <v>5</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>88</v>
+        <v>3</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>77</v>
       </c>
       <c r="H7" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2120,65 +2129,65 @@
       <c r="J7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="12">
         <f>$I7+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="24">
         <f>$I7+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="24">
         <f>$I7+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N7" s="17">
+      <c r="N7" s="24">
         <f>$I7+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O7" s="17">
+      <c r="O7" s="24">
         <f>$I7+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P7" s="17">
+      <c r="P7" s="24">
         <f>$I7+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q7" s="17">
+      <c r="Q7" s="24">
         <f>$I7+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R7" s="17">
+      <c r="R7" s="24">
         <f>$I7+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S7" s="17">
+      <c r="S7" s="24">
         <f>$I7+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T7" s="17">
+      <c r="T7" s="24">
         <f>$I7+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U7" s="17">
+      <c r="U7" s="24">
         <f>$I7+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V7" s="17">
+      <c r="V7" s="24">
         <f>$I7+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="46"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="19" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>20</v>
@@ -2248,104 +2257,104 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="46"/>
-      <c r="B9" s="13" t="s">
-        <v>45</v>
+    <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="47"/>
+      <c r="B9" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="C9" s="7">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D9" s="7">
-        <v>7</v>
-      </c>
-      <c r="E9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="29" t="str">
+      <c r="F9" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="31" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
       <c r="I9" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="27">
+      <c r="K9" s="26">
         <f>$I9+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="24">
         <f>$I9+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="24">
         <f>$I9+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N9" s="17">
+      <c r="N9" s="24">
         <f>$I9+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O9" s="17">
+      <c r="O9" s="24">
         <f>$I9+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P9" s="17">
+      <c r="P9" s="24">
         <f>$I9+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q9" s="17">
+      <c r="Q9" s="24">
         <f>$I9+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R9" s="17">
+      <c r="R9" s="24">
         <f>$I9+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S9" s="17">
+      <c r="S9" s="24">
         <f>$I9+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T9" s="17">
+      <c r="T9" s="24">
         <f>$I9+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U9" s="17">
+      <c r="U9" s="24">
         <f>$I9+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V9" s="17">
+      <c r="V9" s="24">
         <f>$I9+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="46"/>
+    <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="47"/>
       <c r="B10" s="19" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C10" s="7">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D10" s="7">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>93</v>
+        <v>18</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="H10" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2354,10 +2363,10 @@
       <c r="I10" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="26">
+      <c r="K10" s="12">
         <f>$I10+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
@@ -2407,26 +2416,26 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="46"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="19" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C11" s="7">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D11" s="7">
-        <v>9</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="H11" s="31" t="str">
+        <v>3</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="29" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
@@ -2436,7 +2445,7 @@
       <c r="J11" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="26">
         <f>$I11+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
@@ -2485,104 +2494,104 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="46"/>
-      <c r="B12" s="19" t="s">
-        <v>50</v>
+    <row r="12" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="47"/>
+      <c r="B12" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="C12" s="7">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12" s="7">
-        <v>10</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" s="31" t="str">
+        <v>7</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="29" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
       <c r="I12" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J12" s="32" t="s">
+      <c r="J12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="26">
+      <c r="K12" s="27">
         <f>$I12+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L12" s="24">
+      <c r="L12" s="17">
         <f>$I12+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M12" s="24">
+      <c r="M12" s="17">
         <f>$I12+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N12" s="24">
+      <c r="N12" s="17">
         <f>$I12+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O12" s="24">
+      <c r="O12" s="17">
         <f>$I12+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P12" s="24">
+      <c r="P12" s="17">
         <f>$I12+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q12" s="24">
+      <c r="Q12" s="17">
         <f>$I12+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R12" s="24">
+      <c r="R12" s="17">
         <f>$I12+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S12" s="24">
+      <c r="S12" s="17">
         <f>$I12+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T12" s="24">
+      <c r="T12" s="17">
         <f>$I12+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U12" s="24">
+      <c r="U12" s="17">
         <f>$I12+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V12" s="24">
+      <c r="V12" s="17">
         <f>$I12+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="46"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="7">
         <v>11</v>
       </c>
       <c r="D13" s="7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="H13" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2594,7 +2603,7 @@
       <c r="J13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="26">
         <f>$I13+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
@@ -2643,25 +2652,25 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="46"/>
+    <row r="14" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="47"/>
       <c r="B14" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C14" s="7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" s="7">
-        <v>12</v>
-      </c>
-      <c r="E14" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="H14" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2670,10 +2679,10 @@
       <c r="I14" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="26">
+      <c r="K14" s="12">
         <f>$I14+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
@@ -2722,25 +2731,25 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="46"/>
+    <row r="15" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="47"/>
       <c r="B15" s="19" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C15" s="7">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D15" s="7">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>48</v>
+        <v>92</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="H15" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2749,10 +2758,10 @@
       <c r="I15" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J15" s="32" t="s">
+      <c r="J15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="26">
         <f>$I15+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
@@ -2801,181 +2810,181 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="46"/>
-      <c r="B16" s="13" t="s">
-        <v>54</v>
+    <row r="16" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="47"/>
+      <c r="B16" s="19" t="s">
+        <v>56</v>
       </c>
       <c r="C16" s="7">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D16" s="7">
-        <v>15</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="H16" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="H16" s="31" t="s">
         <v>12</v>
       </c>
       <c r="I16" s="17">
         <v>0.75</v>
       </c>
-      <c r="J16" s="30" t="s">
+      <c r="J16" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="33">
+      <c r="K16" s="26">
         <f>$I16+Sheet2!B$1/24</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="24">
         <f>$I16+Sheet2!B$2/24</f>
         <v>1.125</v>
       </c>
-      <c r="M16" s="17">
+      <c r="M16" s="24">
         <f>$I16+Sheet2!B$3/24</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="N16" s="17">
+      <c r="N16" s="24">
         <f>$I16+Sheet2!B$4/24</f>
         <v>0.875</v>
       </c>
-      <c r="O16" s="17">
+      <c r="O16" s="24">
         <f>$I16+Sheet2!B$5/24</f>
         <v>0.875</v>
       </c>
-      <c r="P16" s="17">
+      <c r="P16" s="24">
         <f>$I16+Sheet2!B$6/24</f>
         <v>0.875</v>
       </c>
-      <c r="Q16" s="17">
+      <c r="Q16" s="24">
         <f>$I16+Sheet2!B$7/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R16" s="17">
+      <c r="R16" s="24">
         <f>$I16+Sheet2!B$8/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="S16" s="17">
+      <c r="S16" s="24">
         <f>$I16+Sheet2!B$9/24</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="T16" s="17">
+      <c r="T16" s="24">
         <f>$I16+Sheet2!B$10/24</f>
         <v>0.54166666666666663</v>
       </c>
-      <c r="U16" s="17">
+      <c r="U16" s="24">
         <f>$I16+Sheet2!B$11/24</f>
         <v>0.5</v>
       </c>
-      <c r="V16" s="17">
+      <c r="V16" s="24">
         <f>$I16+Sheet2!B$12/24</f>
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="46"/>
-      <c r="B17" s="19" t="s">
-        <v>55</v>
+      <c r="A17" s="47"/>
+      <c r="B17" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="C17" s="7">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="7">
-        <v>16</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H17" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="29" t="s">
         <v>12</v>
       </c>
       <c r="I17" s="17">
         <v>0.75</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="26">
+      <c r="K17" s="33">
         <f>$I17+Sheet2!B$1/24</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L17" s="24">
+      <c r="L17" s="17">
         <f>$I17+Sheet2!B$2/24</f>
         <v>1.125</v>
       </c>
-      <c r="M17" s="24">
+      <c r="M17" s="17">
         <f>$I17+Sheet2!B$3/24</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="N17" s="24">
+      <c r="N17" s="17">
         <f>$I17+Sheet2!B$4/24</f>
         <v>0.875</v>
       </c>
-      <c r="O17" s="24">
+      <c r="O17" s="17">
         <f>$I17+Sheet2!B$5/24</f>
         <v>0.875</v>
       </c>
-      <c r="P17" s="24">
+      <c r="P17" s="17">
         <f>$I17+Sheet2!B$6/24</f>
         <v>0.875</v>
       </c>
-      <c r="Q17" s="24">
+      <c r="Q17" s="17">
         <f>$I17+Sheet2!B$7/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R17" s="24">
+      <c r="R17" s="17">
         <f>$I17+Sheet2!B$8/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="S17" s="24">
+      <c r="S17" s="17">
         <f>$I17+Sheet2!B$9/24</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="T17" s="24">
+      <c r="T17" s="17">
         <f>$I17+Sheet2!B$10/24</f>
         <v>0.54166666666666663</v>
       </c>
-      <c r="U17" s="24">
+      <c r="U17" s="17">
         <f>$I17+Sheet2!B$11/24</f>
         <v>0.5</v>
       </c>
-      <c r="V17" s="24">
+      <c r="V17" s="17">
         <f>$I17+Sheet2!B$12/24</f>
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46"/>
-      <c r="B18" s="19" t="s">
-        <v>56</v>
+      <c r="A18" s="47"/>
+      <c r="B18" s="34" t="s">
+        <v>112</v>
       </c>
       <c r="C18" s="7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" s="7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>103</v>
+        <v>106</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>113</v>
       </c>
       <c r="H18" s="31" t="s">
         <v>12</v>
@@ -3037,23 +3046,23 @@
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="47"/>
-      <c r="B19" s="34" t="s">
-        <v>112</v>
+      <c r="B19" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="C19" s="7">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" s="7">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G19" s="36" t="s">
-        <v>113</v>
+        <v>133</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>102</v>
       </c>
       <c r="H19" s="31" t="s">
         <v>12</v>
@@ -3114,9 +3123,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="48" t="s">
-        <v>21</v>
-      </c>
+      <c r="A20" s="48"/>
       <c r="B20" s="19" t="s">
         <v>94</v>
       </c>
@@ -3194,7 +3201,9 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
+      <c r="A21" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="B21" s="19" t="s">
         <v>57</v>
       </c>
@@ -3271,25 +3280,25 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49"/>
+    <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="50"/>
       <c r="B22" s="19" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="C22" s="7">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D22" s="7">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>30</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>83</v>
+        <v>48</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>115</v>
       </c>
       <c r="H22" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3350,34 +3359,33 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="49"/>
+    <row r="23" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="50"/>
       <c r="B23" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="7">
         <v>33</v>
       </c>
-      <c r="C23" s="7">
+      <c r="D23" s="7">
+        <v>47</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="7">
-        <v>22</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="H23" s="31" t="str">
-        <f>Sheet2!$A$9</f>
-        <v>EDT</v>
-      </c>
-      <c r="I23" s="24">
+      <c r="G23" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="H23" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="I23" s="43">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J23" s="28" t="s">
+      <c r="J23" s="44" t="s">
         <v>15</v>
       </c>
       <c r="K23" s="26">
@@ -3430,15 +3438,15 @@
       </c>
     </row>
     <row r="24" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="49"/>
-      <c r="B24" s="19" t="s">
-        <v>34</v>
+      <c r="A24" s="50"/>
+      <c r="B24" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="C24" s="7">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D24" s="7">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>30</v>
@@ -3446,8 +3454,8 @@
       <c r="F24" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G24" s="9" t="s">
-        <v>79</v>
+      <c r="G24" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="H24" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3459,7 +3467,7 @@
       <c r="J24" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="26">
+      <c r="K24" s="12">
         <f>$I24+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
@@ -3509,15 +3517,15 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="49"/>
-      <c r="B25" s="19" t="s">
-        <v>35</v>
+      <c r="A25" s="50"/>
+      <c r="B25" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="C25" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D25" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>30</v>
@@ -3525,8 +3533,8 @@
       <c r="F25" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>80</v>
+      <c r="G25" s="22" t="s">
+        <v>117</v>
       </c>
       <c r="H25" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3588,15 +3596,15 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="49"/>
-      <c r="B26" s="13" t="s">
-        <v>36</v>
+      <c r="A26" s="50"/>
+      <c r="B26" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="C26" s="7">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D26" s="7">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>30</v>
@@ -3604,8 +3612,8 @@
       <c r="F26" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G26" s="22" t="s">
-        <v>117</v>
+      <c r="G26" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="H26" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3667,15 +3675,15 @@
       </c>
     </row>
     <row r="27" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="49"/>
-      <c r="B27" s="19" t="s">
-        <v>37</v>
+      <c r="A27" s="50"/>
+      <c r="B27" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="C27" s="7">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D27" s="7">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>30</v>
@@ -3684,7 +3692,7 @@
         <v>22</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="H27" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3693,68 +3701,68 @@
       <c r="I27" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J27" s="28" t="s">
+      <c r="J27" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K27" s="12">
+      <c r="K27" s="33">
         <f>$I27+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L27" s="24">
+      <c r="L27" s="17">
         <f>$I27+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M27" s="24">
+      <c r="M27" s="17">
         <f>$I27+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N27" s="24">
+      <c r="N27" s="17">
         <f>$I27+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O27" s="24">
+      <c r="O27" s="17">
         <f>$I27+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P27" s="24">
+      <c r="P27" s="17">
         <f>$I27+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q27" s="24">
+      <c r="Q27" s="17">
         <f>$I27+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R27" s="24">
+      <c r="R27" s="17">
         <f>$I27+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S27" s="24">
+      <c r="S27" s="17">
         <f>$I27+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T27" s="24">
+      <c r="T27" s="17">
         <f>$I27+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U27" s="24">
+      <c r="U27" s="17">
         <f>$I27+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V27" s="24">
+      <c r="V27" s="17">
         <f>$I27+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="49"/>
-      <c r="B28" s="13" t="s">
-        <v>38</v>
+      <c r="A28" s="50"/>
+      <c r="B28" s="19" t="s">
+        <v>35</v>
       </c>
       <c r="C28" s="7">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D28" s="7">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>30</v>
@@ -3762,8 +3770,8 @@
       <c r="F28" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G28" s="16" t="s">
-        <v>78</v>
+      <c r="G28" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="H28" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3775,7 +3783,7 @@
       <c r="J28" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K28" s="12">
+      <c r="K28" s="26">
         <f>$I28+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
@@ -3825,15 +3833,15 @@
       </c>
     </row>
     <row r="29" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="49"/>
-      <c r="B29" s="13" t="s">
-        <v>39</v>
+      <c r="A29" s="50"/>
+      <c r="B29" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="C29" s="7">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D29" s="7">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>30</v>
@@ -3842,7 +3850,7 @@
         <v>22</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="H29" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3851,77 +3859,77 @@
       <c r="I29" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J29" s="30" t="s">
+      <c r="J29" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K29" s="33">
+      <c r="K29" s="12">
         <f>$I29+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L29" s="17">
+      <c r="L29" s="24">
         <f>$I29+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M29" s="17">
+      <c r="M29" s="24">
         <f>$I29+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N29" s="17">
+      <c r="N29" s="24">
         <f>$I29+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O29" s="17">
+      <c r="O29" s="24">
         <f>$I29+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P29" s="17">
+      <c r="P29" s="24">
         <f>$I29+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q29" s="17">
+      <c r="Q29" s="24">
         <f>$I29+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R29" s="17">
+      <c r="R29" s="24">
         <f>$I29+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S29" s="17">
+      <c r="S29" s="24">
         <f>$I29+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T29" s="17">
+      <c r="T29" s="24">
         <f>$I29+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U29" s="17">
+      <c r="U29" s="24">
         <f>$I29+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V29" s="17">
+      <c r="V29" s="24">
         <f>$I29+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="49"/>
-      <c r="B30" s="13" t="s">
-        <v>147</v>
+      <c r="A30" s="50"/>
+      <c r="B30" s="19" t="s">
+        <v>152</v>
       </c>
       <c r="C30" s="7">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D30" s="7">
-        <v>28</v>
-      </c>
-      <c r="E30" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="F30" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="23" t="s">
-        <v>148</v>
+      <c r="G30" s="31" t="s">
+        <v>153</v>
       </c>
       <c r="H30" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3930,77 +3938,77 @@
       <c r="I30" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J30" s="30" t="s">
+      <c r="J30" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K30" s="33">
+      <c r="K30" s="26">
         <f>$I30+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L30" s="17">
+      <c r="L30" s="24">
         <f>$I30+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M30" s="17">
+      <c r="M30" s="24">
         <f>$I30+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N30" s="17">
+      <c r="N30" s="24">
         <f>$I30+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O30" s="17">
+      <c r="O30" s="24">
         <f>$I30+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P30" s="17">
+      <c r="P30" s="24">
         <f>$I30+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q30" s="17">
+      <c r="Q30" s="24">
         <f>$I30+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R30" s="17">
+      <c r="R30" s="24">
         <f>$I30+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S30" s="17">
+      <c r="S30" s="24">
         <f>$I30+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T30" s="17">
+      <c r="T30" s="24">
         <f>$I30+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U30" s="17">
+      <c r="U30" s="24">
         <f>$I30+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V30" s="17">
+      <c r="V30" s="24">
         <f>$I30+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="49"/>
-      <c r="B31" s="19" t="s">
-        <v>47</v>
+      <c r="A31" s="50"/>
+      <c r="B31" s="13" t="s">
+        <v>147</v>
       </c>
       <c r="C31" s="7">
         <v>29</v>
       </c>
       <c r="D31" s="7">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>30</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G31" s="22" t="s">
-        <v>85</v>
+        <v>22</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>148</v>
       </c>
       <c r="H31" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4009,77 +4017,77 @@
       <c r="I31" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J31" s="28" t="s">
+      <c r="J31" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K31" s="26">
+      <c r="K31" s="33">
         <f>$I31+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L31" s="24">
+      <c r="L31" s="17">
         <f>$I31+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M31" s="24">
+      <c r="M31" s="17">
         <f>$I31+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N31" s="24">
+      <c r="N31" s="17">
         <f>$I31+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O31" s="24">
+      <c r="O31" s="17">
         <f>$I31+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P31" s="24">
+      <c r="P31" s="17">
         <f>$I31+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q31" s="24">
+      <c r="Q31" s="17">
         <f>$I31+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R31" s="24">
+      <c r="R31" s="17">
         <f>$I31+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S31" s="24">
+      <c r="S31" s="17">
         <f>$I31+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T31" s="24">
+      <c r="T31" s="17">
         <f>$I31+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U31" s="24">
+      <c r="U31" s="17">
         <f>$I31+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V31" s="24">
+      <c r="V31" s="17">
         <f>$I31+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="49"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="19" t="s">
-        <v>116</v>
+        <v>32</v>
       </c>
       <c r="C32" s="7">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D32" s="7">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>30</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G32" s="23" t="s">
-        <v>115</v>
+        <v>22</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="H32" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4141,32 +4149,33 @@
       </c>
     </row>
     <row r="33" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="49"/>
+      <c r="A33" s="50"/>
       <c r="B33" s="19" t="s">
-        <v>144</v>
+        <v>33</v>
       </c>
       <c r="C33" s="7">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D33" s="7">
-        <v>47</v>
-      </c>
-      <c r="E33" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="42" t="s">
+      <c r="F33" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G33" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="H33" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="I33" s="43">
+      <c r="G33" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H33" s="31" t="str">
+        <f>Sheet2!$A$9</f>
+        <v>EDT</v>
+      </c>
+      <c r="I33" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J33" s="44" t="s">
+      <c r="J33" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K33" s="26">
@@ -4219,93 +4228,94 @@
       </c>
     </row>
     <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="49"/>
+      <c r="A34" s="50"/>
       <c r="B34" s="19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C34" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D34" s="7">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E34" s="15" t="s">
         <v>30</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G34" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="H34" s="31" t="s">
-        <v>74</v>
+        <v>48</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" s="31" t="str">
+        <f>Sheet2!$A$9</f>
+        <v>EDT</v>
       </c>
       <c r="I34" s="24">
-        <v>0</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="J34" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K34" s="26">
         <f>$I34+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
+        <v>1.375</v>
       </c>
       <c r="L34" s="24">
         <f>$I34+Sheet2!B$2/24</f>
-        <v>0.375</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="M34" s="24">
         <f>$I34+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="N34" s="24">
         <f>$I34+Sheet2!B$4/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="O34" s="24">
         <f>$I34+Sheet2!B$5/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="P34" s="24">
         <f>$I34+Sheet2!B$6/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="Q34" s="24">
         <f>$I34+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="R34" s="24">
         <f>$I34+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>1</v>
       </c>
       <c r="S34" s="24">
         <f>$I34+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="T34" s="24">
         <f>$I34+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="U34" s="24">
         <f>$I34+Sheet2!B$11/24</f>
-        <v>-0.25</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="V34" s="24">
         <f>$I34+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="49"/>
-      <c r="B35" s="19" t="s">
-        <v>59</v>
+      <c r="A35" s="50"/>
+      <c r="B35" s="37" t="s">
+        <v>62</v>
       </c>
       <c r="C35" s="7">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D35" s="7">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>30</v>
@@ -4314,7 +4324,7 @@
         <v>22</v>
       </c>
       <c r="G35" s="31" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H35" s="31" t="s">
         <v>74</v>
@@ -4322,7 +4332,7 @@
       <c r="I35" s="24">
         <v>0</v>
       </c>
-      <c r="J35" s="28" t="s">
+      <c r="J35" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K35" s="26">
@@ -4375,24 +4385,24 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="49"/>
-      <c r="B36" s="19" t="s">
-        <v>138</v>
+      <c r="A36" s="50"/>
+      <c r="B36" s="37" t="s">
+        <v>60</v>
       </c>
       <c r="C36" s="7">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D36" s="7">
-        <v>33</v>
-      </c>
-      <c r="E36" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F36" s="42" t="s">
-        <v>22</v>
+      <c r="F36" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="G36" s="31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H36" s="31" t="s">
         <v>74</v>
@@ -4400,7 +4410,7 @@
       <c r="I36" s="24">
         <v>0</v>
       </c>
-      <c r="J36" s="28" t="s">
+      <c r="J36" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K36" s="26">
@@ -4453,24 +4463,24 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="49"/>
-      <c r="B37" s="37" t="s">
-        <v>60</v>
+      <c r="A37" s="50"/>
+      <c r="B37" s="19" t="s">
+        <v>138</v>
       </c>
       <c r="C37" s="7">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D37" s="7">
-        <v>34</v>
-      </c>
-      <c r="E37" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="7" t="s">
-        <v>75</v>
+      <c r="F37" s="42" t="s">
+        <v>22</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H37" s="31" t="s">
         <v>74</v>
@@ -4478,7 +4488,7 @@
       <c r="I37" s="24">
         <v>0</v>
       </c>
-      <c r="J37" s="30" t="s">
+      <c r="J37" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K37" s="26">
@@ -4531,24 +4541,24 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="49"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C38" s="7">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D38" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E38" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F38" s="7" t="s">
-        <v>75</v>
+      <c r="F38" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="G38" s="31" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="H38" s="31" t="s">
         <v>74</v>
@@ -4609,24 +4619,24 @@
       </c>
     </row>
     <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="49"/>
-      <c r="B39" s="37" t="s">
-        <v>62</v>
+      <c r="A39" s="50"/>
+      <c r="B39" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="C39" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D39" s="7">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E39" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F39" s="20" t="s">
-        <v>22</v>
+      <c r="F39" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="G39" s="31" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="H39" s="31" t="s">
         <v>74</v>
@@ -4687,15 +4697,15 @@
       </c>
     </row>
     <row r="40" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="49"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C40" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D40" s="7">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E40" s="15" t="s">
         <v>30</v>
@@ -4704,7 +4714,7 @@
         <v>22</v>
       </c>
       <c r="G40" s="31" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="H40" s="31" t="s">
         <v>74</v>
@@ -4712,7 +4722,7 @@
       <c r="I40" s="24">
         <v>0</v>
       </c>
-      <c r="J40" s="30" t="s">
+      <c r="J40" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K40" s="26">
@@ -4764,103 +4774,28 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="49"/>
-      <c r="B41" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="7">
-        <v>38</v>
-      </c>
-      <c r="D41" s="7">
-        <v>38</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="H41" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="I41" s="24">
-        <v>0</v>
-      </c>
-      <c r="J41" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="K41" s="26">
-        <f>$I41+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="L41" s="24">
-        <f>$I41+Sheet2!B$2/24</f>
-        <v>0.375</v>
-      </c>
-      <c r="M41" s="24">
-        <f>$I41+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="N41" s="24">
-        <f>$I41+Sheet2!B$4/24</f>
-        <v>0.125</v>
-      </c>
-      <c r="O41" s="24">
-        <f>$I41+Sheet2!B$5/24</f>
-        <v>0.125</v>
-      </c>
-      <c r="P41" s="24">
-        <f>$I41+Sheet2!B$6/24</f>
-        <v>0.125</v>
-      </c>
-      <c r="Q41" s="24">
-        <f>$I41+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="R41" s="24">
-        <f>$I41+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="S41" s="24">
-        <f>$I41+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
-      </c>
-      <c r="T41" s="24">
-        <f>$I41+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
-      </c>
-      <c r="U41" s="24">
-        <f>$I41+Sheet2!B$11/24</f>
-        <v>-0.25</v>
-      </c>
-      <c r="V41" s="24">
-        <f>$I41+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
-      </c>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A41" s="50"/>
     </row>
     <row r="42" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="49"/>
+      <c r="A42" s="50"/>
       <c r="B42" s="19" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C42" s="7">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D42" s="7">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F42" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G42" s="31" t="s">
-        <v>124</v>
+      <c r="F42" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="29" t="s">
+        <v>118</v>
       </c>
       <c r="H42" s="31" t="s">
         <v>74</v>
@@ -4868,7 +4803,7 @@
       <c r="I42" s="24">
         <v>0</v>
       </c>
-      <c r="J42" s="30" t="s">
+      <c r="J42" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K42" s="26">
@@ -4920,25 +4855,25 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="49"/>
+    <row r="43" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="50"/>
       <c r="B43" s="37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C43" s="7">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D43" s="7">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E43" s="15" t="s">
         <v>30</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G43" s="31" t="s">
-        <v>125</v>
+        <v>22</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>123</v>
       </c>
       <c r="H43" s="31" t="s">
         <v>74</v>
@@ -4999,336 +4934,336 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="49"/>
+      <c r="A44" s="50"/>
       <c r="B44" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C44" s="7">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D44" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G44" s="36" t="s">
-        <v>126</v>
+        <v>75</v>
+      </c>
+      <c r="G44" s="31" t="s">
+        <v>124</v>
       </c>
       <c r="H44" s="31" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="I44" s="24">
-        <v>4.1666666666666664E-2</v>
+        <v>0</v>
       </c>
       <c r="J44" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K44" s="26">
         <f>$I44+Sheet2!B$1/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L44" s="24">
         <f>$I44+Sheet2!B$2/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="M44" s="24">
         <f>$I44+Sheet2!B$3/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N44" s="24">
         <f>$I44+Sheet2!B$4/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="O44" s="24">
         <f>$I44+Sheet2!B$5/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="P44" s="24">
         <f>$I44+Sheet2!B$6/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="Q44" s="24">
         <f>$I44+Sheet2!B$7/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R44" s="24">
         <f>$I44+Sheet2!B$8/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="S44" s="24">
         <f>$I44+Sheet2!B$9/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="T44" s="24">
         <f>$I44+Sheet2!B$10/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="U44" s="24">
         <f>$I44+Sheet2!B$11/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.25</v>
       </c>
       <c r="V44" s="24">
         <f>$I44+Sheet2!B$12/24</f>
-        <v>-0.25</v>
+        <v>-0.29166666666666669</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="49"/>
+      <c r="A45" s="50"/>
       <c r="B45" s="37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C45" s="7">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D45" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E45" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F45" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G45" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="H45" s="37" t="s">
-        <v>13</v>
+      <c r="F45" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G45" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>74</v>
       </c>
       <c r="I45" s="24">
-        <v>4.1666666666666664E-2</v>
+        <v>0</v>
       </c>
       <c r="J45" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K45" s="26">
         <f>$I45+Sheet2!B$1/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L45" s="24">
         <f>$I45+Sheet2!B$2/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="M45" s="24">
         <f>$I45+Sheet2!B$3/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N45" s="24">
         <f>$I45+Sheet2!B$4/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="O45" s="24">
         <f>$I45+Sheet2!B$5/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="P45" s="24">
         <f>$I45+Sheet2!B$6/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="Q45" s="24">
         <f>$I45+Sheet2!B$7/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R45" s="24">
         <f>$I45+Sheet2!B$8/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="S45" s="24">
         <f>$I45+Sheet2!B$9/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="T45" s="24">
         <f>$I45+Sheet2!B$10/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="U45" s="24">
         <f>$I45+Sheet2!B$11/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.25</v>
       </c>
       <c r="V45" s="24">
         <f>$I45+Sheet2!B$12/24</f>
-        <v>-0.25</v>
+        <v>-0.29166666666666669</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="49"/>
+      <c r="A46" s="50"/>
       <c r="B46" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C46" s="7">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D46" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G46" s="39" t="s">
-        <v>127</v>
+        <v>141</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G46" s="36" t="s">
+        <v>126</v>
       </c>
       <c r="H46" s="31" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="I46" s="24">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J46" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K46" s="26">
         <f>$I46+Sheet2!B$1/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="L46" s="24">
         <f>$I46+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M46" s="24">
         <f>$I46+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="N46" s="24">
         <f>$I46+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="O46" s="24">
         <f>$I46+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P46" s="24">
         <f>$I46+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q46" s="24">
         <f>$I46+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="R46" s="24">
         <f>$I46+Sheet2!B$8/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S46" s="24">
         <f>$I46+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="T46" s="24">
         <f>$I46+Sheet2!B$10/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="U46" s="24">
         <f>$I46+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="V46" s="24">
         <f>$I46+Sheet2!B$12/24</f>
-        <v>-0.20833333333333337</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="49"/>
+      <c r="A47" s="50"/>
       <c r="B47" s="37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C47" s="7">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D47" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E47" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F47" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="H47" s="31" t="s">
-        <v>73</v>
+      <c r="F47" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H47" s="37" t="s">
+        <v>13</v>
       </c>
       <c r="I47" s="24">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J47" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K47" s="26">
         <f>$I47+Sheet2!B$1/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="L47" s="24">
         <f>$I47+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M47" s="24">
         <f>$I47+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="N47" s="24">
         <f>$I47+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="O47" s="24">
         <f>$I47+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P47" s="24">
         <f>$I47+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q47" s="24">
         <f>$I47+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="R47" s="24">
         <f>$I47+Sheet2!B$8/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S47" s="24">
         <f>$I47+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="T47" s="24">
         <f>$I47+Sheet2!B$10/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="U47" s="24">
         <f>$I47+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="V47" s="24">
         <f>$I47+Sheet2!B$12/24</f>
-        <v>-0.20833333333333337</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="49"/>
+      <c r="A48" s="50"/>
       <c r="B48" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C48" s="7">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D48" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E48" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F48" s="20" t="s">
+      <c r="F48" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G48" s="22" t="s">
-        <v>129</v>
+      <c r="G48" s="39" t="s">
+        <v>127</v>
       </c>
       <c r="H48" s="31" t="s">
         <v>73</v>
@@ -5389,24 +5324,24 @@
       </c>
     </row>
     <row r="49" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="49"/>
+      <c r="A49" s="50"/>
       <c r="B49" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C49" s="7">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D49" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E49" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F49" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="G49" s="23" t="s">
-        <v>130</v>
+      <c r="F49" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="H49" s="31" t="s">
         <v>73</v>
@@ -5466,15 +5401,171 @@
         <v>-0.20833333333333337</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A50" s="49"/>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A51" s="49"/>
+    <row r="50" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="50"/>
+      <c r="B50" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="7">
+        <v>48</v>
+      </c>
+      <c r="D50" s="7">
+        <v>45</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F50" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H50" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="I50" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J50" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K50" s="26">
+        <f>$I50+Sheet2!B$1/24</f>
+        <v>0.5</v>
+      </c>
+      <c r="L50" s="24">
+        <f>$I50+Sheet2!B$2/24</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M50" s="24">
+        <f>$I50+Sheet2!B$3/24</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="N50" s="24">
+        <f>$I50+Sheet2!B$4/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="O50" s="24">
+        <f>$I50+Sheet2!B$5/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P50" s="24">
+        <f>$I50+Sheet2!B$6/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="Q50" s="24">
+        <f>$I50+Sheet2!B$7/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R50" s="24">
+        <f>$I50+Sheet2!B$8/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="S50" s="24">
+        <f>$I50+Sheet2!B$9/24</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="T50" s="24">
+        <f>$I50+Sheet2!B$10/24</f>
+        <v>-0.125</v>
+      </c>
+      <c r="U50" s="24">
+        <f>$I50+Sheet2!B$11/24</f>
+        <v>-0.16666666666666669</v>
+      </c>
+      <c r="V50" s="24">
+        <f>$I50+Sheet2!B$12/24</f>
+        <v>-0.20833333333333337</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="50"/>
+      <c r="B51" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="7">
+        <v>49</v>
+      </c>
+      <c r="D51" s="7">
+        <v>46</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F51" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G51" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H51" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="I51" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J51" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K51" s="26">
+        <f>$I51+Sheet2!B$1/24</f>
+        <v>0.5</v>
+      </c>
+      <c r="L51" s="24">
+        <f>$I51+Sheet2!B$2/24</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M51" s="24">
+        <f>$I51+Sheet2!B$3/24</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="N51" s="24">
+        <f>$I51+Sheet2!B$4/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="O51" s="24">
+        <f>$I51+Sheet2!B$5/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P51" s="24">
+        <f>$I51+Sheet2!B$6/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="Q51" s="24">
+        <f>$I51+Sheet2!B$7/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R51" s="24">
+        <f>$I51+Sheet2!B$8/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="S51" s="24">
+        <f>$I51+Sheet2!B$9/24</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="T51" s="24">
+        <f>$I51+Sheet2!B$10/24</f>
+        <v>-0.125</v>
+      </c>
+      <c r="U51" s="24">
+        <f>$I51+Sheet2!B$11/24</f>
+        <v>-0.16666666666666669</v>
+      </c>
+      <c r="V51" s="24">
+        <f>$I51+Sheet2!B$12/24</f>
+        <v>-0.20833333333333337</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A52" s="50"/>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A53" s="50"/>
     </row>
   </sheetData>
-  <sortState ref="B2:V40">
-    <sortCondition ref="D2:D40"/>
+  <sortState ref="B2:V42">
+    <sortCondition ref="D2:D42"/>
   </sortState>
   <customSheetViews>
     <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
@@ -5486,10 +5577,10 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
-    <mergeCell ref="A5:A19"/>
-    <mergeCell ref="A20:A51"/>
+    <mergeCell ref="A6:A20"/>
+    <mergeCell ref="A21:A53"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L4 K4:V49">
+  <conditionalFormatting sqref="K2:L4 K42:V51 K4:V40">
     <cfRule type="expression" dxfId="46" priority="104">
       <formula>K$1=$H2</formula>
     </cfRule>
@@ -5499,227 +5590,227 @@
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G47:G49 E37:F38 E34:F35 H34:V38 K33:V49 G31:G45 C31:D49 B31:B38 E31:V32 B2:V29">
+  <conditionalFormatting sqref="G49:G51 B2:V22 K23:V23 G30:V30 G23 B23:D23 B24:V29 B30:D30 C31 B32:V34 K35:V35 G35 C35:D35 B36:V36 G37:V37 B37:D37 K43:V51 K38:V38 G43:G47 G38 C43:D51 C38:D38 B42:V42 B39:V40">
     <cfRule type="expression" dxfId="44" priority="110">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39 J39:V39">
+  <conditionalFormatting sqref="B35 J35:V35">
     <cfRule type="expression" dxfId="43" priority="87">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B40 J40:V40">
+  <conditionalFormatting sqref="B38 J38:V38">
     <cfRule type="expression" dxfId="42" priority="85">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B41 J41:V41">
+  <conditionalFormatting sqref="B43 J43:V43">
     <cfRule type="expression" dxfId="41" priority="83">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42 J42:V42">
+  <conditionalFormatting sqref="B44 J44:V44">
     <cfRule type="expression" dxfId="40" priority="81">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43 J43:V43">
+  <conditionalFormatting sqref="B45 J45:V45">
     <cfRule type="expression" dxfId="39" priority="79">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44 J44:V44">
+  <conditionalFormatting sqref="B46 J46:V46">
     <cfRule type="expression" dxfId="38" priority="77">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45 J45:V45 E45:F45 H45">
+  <conditionalFormatting sqref="B47 J47:V47 E47:F47 H47">
     <cfRule type="expression" dxfId="37" priority="75">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
+  <conditionalFormatting sqref="E35">
     <cfRule type="expression" dxfId="36" priority="73">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
+  <conditionalFormatting sqref="E44">
     <cfRule type="expression" dxfId="35" priority="70">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
+  <conditionalFormatting sqref="E45">
     <cfRule type="expression" dxfId="34" priority="69">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E44 H44">
+  <conditionalFormatting sqref="E46 H46">
     <cfRule type="expression" dxfId="33" priority="68">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B46 J46:V46">
+  <conditionalFormatting sqref="B48 J48:V48">
     <cfRule type="expression" dxfId="32" priority="66">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47 J47:V47 E47">
+  <conditionalFormatting sqref="B49 J49:V49 E49">
     <cfRule type="expression" dxfId="31" priority="64">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46:F46 H46">
+  <conditionalFormatting sqref="E48:F48 H48">
     <cfRule type="expression" dxfId="30" priority="62">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48 J48:V48">
+  <conditionalFormatting sqref="B50 J50:V50">
     <cfRule type="expression" dxfId="29" priority="60">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49 J49:V49 E49">
+  <conditionalFormatting sqref="B51 J51:V51 E51">
     <cfRule type="expression" dxfId="28" priority="58">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
+  <conditionalFormatting sqref="F45">
     <cfRule type="expression" dxfId="27" priority="50">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
+  <conditionalFormatting sqref="I35">
     <cfRule type="expression" dxfId="26" priority="40">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
+  <conditionalFormatting sqref="I38">
     <cfRule type="expression" dxfId="25" priority="39">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
+  <conditionalFormatting sqref="I43">
     <cfRule type="expression" dxfId="24" priority="38">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
+  <conditionalFormatting sqref="I44">
     <cfRule type="expression" dxfId="23" priority="37">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
+  <conditionalFormatting sqref="I45">
     <cfRule type="expression" dxfId="22" priority="36">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
+  <conditionalFormatting sqref="I46">
     <cfRule type="expression" dxfId="21" priority="35">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
+  <conditionalFormatting sqref="I47">
     <cfRule type="expression" dxfId="20" priority="34">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
+  <conditionalFormatting sqref="I48">
     <cfRule type="expression" dxfId="19" priority="33">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
+  <conditionalFormatting sqref="H35">
     <cfRule type="expression" dxfId="18" priority="26">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
+  <conditionalFormatting sqref="H38">
     <cfRule type="expression" dxfId="17" priority="25">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H41">
+  <conditionalFormatting sqref="H43">
     <cfRule type="expression" dxfId="16" priority="24">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H42">
+  <conditionalFormatting sqref="H44">
     <cfRule type="expression" dxfId="15" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
+  <conditionalFormatting sqref="H45">
     <cfRule type="expression" dxfId="14" priority="22">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
+  <conditionalFormatting sqref="H49">
     <cfRule type="expression" dxfId="13" priority="21">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
+  <conditionalFormatting sqref="I49">
     <cfRule type="expression" dxfId="12" priority="20">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
+  <conditionalFormatting sqref="H50">
     <cfRule type="expression" dxfId="11" priority="19">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I48">
+  <conditionalFormatting sqref="I50">
     <cfRule type="expression" dxfId="10" priority="18">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H49">
+  <conditionalFormatting sqref="H51">
     <cfRule type="expression" dxfId="9" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I49">
+  <conditionalFormatting sqref="I51">
     <cfRule type="expression" dxfId="8" priority="16">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F42">
+  <conditionalFormatting sqref="F44">
     <cfRule type="expression" dxfId="7" priority="12">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F44">
+  <conditionalFormatting sqref="F46">
     <cfRule type="expression" dxfId="6" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
+  <conditionalFormatting sqref="F49">
     <cfRule type="expression" dxfId="5" priority="10">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
+  <conditionalFormatting sqref="F35">
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41:F41">
+  <conditionalFormatting sqref="E43:F43">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40:F40">
+  <conditionalFormatting sqref="E38:F38">
     <cfRule type="expression" dxfId="2" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48:F48">
+  <conditionalFormatting sqref="E50:F50">
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:V30">
+  <conditionalFormatting sqref="B31 D31:V31">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Resolve minor sorting error with PDT timezone
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECF0470-F7B0-BF4B-9A33-11695E2CB0F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93777D04-7F28-8548-BE40-4A84DD680C52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="1240" windowWidth="33700" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:V39"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1693,7 +1693,7 @@
         <v>EDT</v>
       </c>
       <c r="T1" s="3" t="str">
-        <f>H42</f>
+        <f>H44</f>
         <v>CDT</v>
       </c>
       <c r="U1" s="3" t="str">
@@ -1701,7 +1701,7 @@
         <v>CDT</v>
       </c>
       <c r="V1" s="3" t="str">
-        <f>H39</f>
+        <f>H41</f>
         <v>CDT</v>
       </c>
     </row>
@@ -1870,7 +1870,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="7">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>150</v>
@@ -1945,10 +1945,10 @@
         <v>53</v>
       </c>
       <c r="C5" s="7">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D5" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>20</v>
@@ -2026,10 +2026,10 @@
         <v>43</v>
       </c>
       <c r="C6" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>109</v>
@@ -2105,10 +2105,10 @@
         <v>42</v>
       </c>
       <c r="C7" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>18</v>
@@ -2187,7 +2187,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>20</v>
@@ -2263,10 +2263,10 @@
         <v>52</v>
       </c>
       <c r="C9" s="7">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D9" s="7">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>16</v>
@@ -2342,10 +2342,10 @@
         <v>51</v>
       </c>
       <c r="C10" s="7">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" s="7">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>18</v>
@@ -2421,10 +2421,10 @@
         <v>41</v>
       </c>
       <c r="C11" s="7">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D11" s="7">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>105</v>
@@ -2500,10 +2500,10 @@
         <v>45</v>
       </c>
       <c r="C12" s="7">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D12" s="7">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>16</v>
@@ -2579,10 +2579,10 @@
         <v>50</v>
       </c>
       <c r="C13" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" s="7">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>17</v>
@@ -2658,10 +2658,10 @@
         <v>49</v>
       </c>
       <c r="C14" s="7">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D14" s="7">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>16</v>
@@ -2737,10 +2737,10 @@
         <v>46</v>
       </c>
       <c r="C15" s="7">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D15" s="7">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E15" s="21" t="s">
         <v>92</v>
@@ -2816,10 +2816,10 @@
         <v>56</v>
       </c>
       <c r="C16" s="7">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D16" s="7">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>31</v>
@@ -2894,10 +2894,10 @@
         <v>54</v>
       </c>
       <c r="C17" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D17" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>30</v>
@@ -2972,10 +2972,10 @@
         <v>112</v>
       </c>
       <c r="C18" s="7">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="7">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>105</v>
@@ -3050,10 +3050,10 @@
         <v>55</v>
       </c>
       <c r="C19" s="7">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D19" s="7">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E19" s="21" t="s">
         <v>31</v>
@@ -3286,10 +3286,10 @@
         <v>116</v>
       </c>
       <c r="C22" s="7">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D22" s="7">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>30</v>
@@ -3365,10 +3365,10 @@
         <v>144</v>
       </c>
       <c r="C23" s="7">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D23" s="7">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="E23" s="41" t="s">
         <v>30</v>
@@ -3443,10 +3443,10 @@
         <v>38</v>
       </c>
       <c r="C24" s="7">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D24" s="7">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>30</v>
@@ -3522,10 +3522,10 @@
         <v>36</v>
       </c>
       <c r="C25" s="7">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="7">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>30</v>
@@ -3601,10 +3601,10 @@
         <v>34</v>
       </c>
       <c r="C26" s="7">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D26" s="7">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>30</v>
@@ -3680,10 +3680,10 @@
         <v>39</v>
       </c>
       <c r="C27" s="7">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D27" s="7">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>30</v>
@@ -3759,10 +3759,10 @@
         <v>35</v>
       </c>
       <c r="C28" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D28" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>30</v>
@@ -3838,10 +3838,10 @@
         <v>37</v>
       </c>
       <c r="C29" s="7">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D29" s="7">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>30</v>
@@ -3917,10 +3917,10 @@
         <v>152</v>
       </c>
       <c r="C30" s="7">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D30" s="7">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E30" s="41" t="s">
         <v>30</v>
@@ -3996,10 +3996,10 @@
         <v>147</v>
       </c>
       <c r="C31" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D31" s="7">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>30</v>
@@ -4075,10 +4075,10 @@
         <v>32</v>
       </c>
       <c r="C32" s="7">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D32" s="7">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>30</v>
@@ -4154,10 +4154,10 @@
         <v>33</v>
       </c>
       <c r="C33" s="7">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D33" s="7">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E33" s="15" t="s">
         <v>30</v>
@@ -4233,10 +4233,10 @@
         <v>47</v>
       </c>
       <c r="C34" s="7">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D34" s="7">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E34" s="15" t="s">
         <v>30</v>
@@ -4312,10 +4312,10 @@
         <v>62</v>
       </c>
       <c r="C35" s="7">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D35" s="7">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>30</v>
@@ -4390,10 +4390,10 @@
         <v>60</v>
       </c>
       <c r="C36" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D36" s="7">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E36" s="15" t="s">
         <v>30</v>
@@ -4471,7 +4471,7 @@
         <v>36</v>
       </c>
       <c r="D37" s="7">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E37" s="41" t="s">
         <v>30</v>
@@ -4546,7 +4546,7 @@
         <v>63</v>
       </c>
       <c r="C38" s="7">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D38" s="7">
         <v>37</v>
@@ -4620,23 +4620,23 @@
     </row>
     <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="50"/>
-      <c r="B39" s="19" t="s">
-        <v>61</v>
+      <c r="B39" s="37" t="s">
+        <v>66</v>
       </c>
       <c r="C39" s="7">
         <v>38</v>
       </c>
       <c r="D39" s="7">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E39" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F39" s="7" t="s">
-        <v>75</v>
+      <c r="F39" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="G39" s="31" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="H39" s="31" t="s">
         <v>74</v>
@@ -4698,14 +4698,14 @@
     </row>
     <row r="40" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="50"/>
-      <c r="B40" s="19" t="s">
-        <v>59</v>
+      <c r="B40" s="37" t="s">
+        <v>64</v>
       </c>
       <c r="C40" s="7">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D40" s="7">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E40" s="15" t="s">
         <v>30</v>
@@ -4713,8 +4713,8 @@
       <c r="F40" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G40" s="31" t="s">
-        <v>81</v>
+      <c r="G40" s="29" t="s">
+        <v>123</v>
       </c>
       <c r="H40" s="31" t="s">
         <v>74</v>
@@ -4722,7 +4722,7 @@
       <c r="I40" s="24">
         <v>0</v>
       </c>
-      <c r="J40" s="28" t="s">
+      <c r="J40" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K40" s="26">
@@ -4774,19 +4774,94 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="50"/>
+      <c r="B41" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="7">
+        <v>40</v>
+      </c>
+      <c r="D41" s="7">
+        <v>40</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I41" s="24">
+        <v>0</v>
+      </c>
+      <c r="J41" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K41" s="26">
+        <f>$I41+Sheet2!B$1/24</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L41" s="24">
+        <f>$I41+Sheet2!B$2/24</f>
+        <v>0.375</v>
+      </c>
+      <c r="M41" s="24">
+        <f>$I41+Sheet2!B$3/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N41" s="24">
+        <f>$I41+Sheet2!B$4/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="O41" s="24">
+        <f>$I41+Sheet2!B$5/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="P41" s="24">
+        <f>$I41+Sheet2!B$6/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="Q41" s="24">
+        <f>$I41+Sheet2!B$7/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="R41" s="24">
+        <f>$I41+Sheet2!B$8/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S41" s="24">
+        <f>$I41+Sheet2!B$9/24</f>
+        <v>-0.16666666666666666</v>
+      </c>
+      <c r="T41" s="24">
+        <f>$I41+Sheet2!B$10/24</f>
+        <v>-0.20833333333333334</v>
+      </c>
+      <c r="U41" s="24">
+        <f>$I41+Sheet2!B$11/24</f>
+        <v>-0.25</v>
+      </c>
+      <c r="V41" s="24">
+        <f>$I41+Sheet2!B$12/24</f>
+        <v>-0.29166666666666669</v>
+      </c>
     </row>
     <row r="42" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="50"/>
       <c r="B42" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C42" s="7">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D42" s="7">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>30</v>
@@ -4794,8 +4869,8 @@
       <c r="F42" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G42" s="29" t="s">
-        <v>118</v>
+      <c r="G42" s="31" t="s">
+        <v>81</v>
       </c>
       <c r="H42" s="31" t="s">
         <v>74</v>
@@ -4857,23 +4932,23 @@
     </row>
     <row r="43" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="50"/>
-      <c r="B43" s="37" t="s">
-        <v>64</v>
+      <c r="B43" s="19" t="s">
+        <v>65</v>
       </c>
       <c r="C43" s="7">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D43" s="7">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E43" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F43" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G43" s="29" t="s">
-        <v>123</v>
+      <c r="F43" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G43" s="31" t="s">
+        <v>124</v>
       </c>
       <c r="H43" s="31" t="s">
         <v>74</v>
@@ -4936,22 +5011,22 @@
     <row r="44" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="50"/>
       <c r="B44" s="19" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C44" s="7">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D44" s="7">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E44" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F44" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G44" s="31" t="s">
-        <v>124</v>
+      <c r="F44" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="29" t="s">
+        <v>118</v>
       </c>
       <c r="H44" s="31" t="s">
         <v>74</v>
@@ -4959,7 +5034,7 @@
       <c r="I44" s="24">
         <v>0</v>
       </c>
-      <c r="J44" s="30" t="s">
+      <c r="J44" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K44" s="26">
@@ -5013,103 +5088,103 @@
     </row>
     <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="50"/>
-      <c r="B45" s="37" t="s">
-        <v>66</v>
+      <c r="B45" s="19" t="s">
+        <v>67</v>
       </c>
       <c r="C45" s="7">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D45" s="7">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F45" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G45" s="31" t="s">
-        <v>125</v>
+        <v>141</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G45" s="36" t="s">
+        <v>126</v>
       </c>
       <c r="H45" s="31" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="I45" s="24">
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J45" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K45" s="26">
         <f>$I45+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="L45" s="24">
         <f>$I45+Sheet2!B$2/24</f>
-        <v>0.375</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M45" s="24">
         <f>$I45+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="N45" s="24">
         <f>$I45+Sheet2!B$4/24</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="O45" s="24">
         <f>$I45+Sheet2!B$5/24</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P45" s="24">
         <f>$I45+Sheet2!B$6/24</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q45" s="24">
         <f>$I45+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
       <c r="R45" s="24">
         <f>$I45+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S45" s="24">
         <f>$I45+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
+        <v>-0.125</v>
       </c>
       <c r="T45" s="24">
         <f>$I45+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="U45" s="24">
         <f>$I45+Sheet2!B$11/24</f>
-        <v>-0.25</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="V45" s="24">
         <f>$I45+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="50"/>
-      <c r="B46" s="19" t="s">
-        <v>67</v>
+      <c r="B46" s="37" t="s">
+        <v>68</v>
       </c>
       <c r="C46" s="7">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D46" s="7">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>142</v>
+        <v>30</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="G46" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="H46" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="H46" s="37" t="s">
         <v>13</v>
       </c>
       <c r="I46" s="24">
@@ -5169,101 +5244,101 @@
     </row>
     <row r="47" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="50"/>
-      <c r="B47" s="37" t="s">
-        <v>68</v>
+      <c r="B47" s="19" t="s">
+        <v>71</v>
       </c>
       <c r="C47" s="7">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D47" s="7">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E47" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F47" s="14" t="s">
+      <c r="F47" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G47" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="H47" s="37" t="s">
-        <v>13</v>
+      <c r="G47" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="H47" s="31" t="s">
+        <v>73</v>
       </c>
       <c r="I47" s="24">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="J47" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K47" s="26">
         <f>$I47+Sheet2!B$1/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="L47" s="24">
         <f>$I47+Sheet2!B$2/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="M47" s="24">
         <f>$I47+Sheet2!B$3/24</f>
-        <v>0.375</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="N47" s="24">
         <f>$I47+Sheet2!B$4/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="O47" s="24">
         <f>$I47+Sheet2!B$5/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="P47" s="24">
         <f>$I47+Sheet2!B$6/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="Q47" s="24">
         <f>$I47+Sheet2!B$7/24</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="R47" s="24">
         <f>$I47+Sheet2!B$8/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
       <c r="S47" s="24">
         <f>$I47+Sheet2!B$9/24</f>
-        <v>-0.125</v>
+        <v>-8.3333333333333329E-2</v>
       </c>
       <c r="T47" s="24">
         <f>$I47+Sheet2!B$10/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.125</v>
       </c>
       <c r="U47" s="24">
         <f>$I47+Sheet2!B$11/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="V47" s="24">
         <f>$I47+Sheet2!B$12/24</f>
-        <v>-0.25</v>
+        <v>-0.20833333333333337</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="50"/>
-      <c r="B48" s="19" t="s">
-        <v>69</v>
+      <c r="B48" s="37" t="s">
+        <v>70</v>
       </c>
       <c r="C48" s="7">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D48" s="7">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E48" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F48" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G48" s="39" t="s">
-        <v>127</v>
+      <c r="F48" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="H48" s="31" t="s">
         <v>73</v>
@@ -5325,23 +5400,23 @@
     </row>
     <row r="49" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="50"/>
-      <c r="B49" s="37" t="s">
-        <v>70</v>
+      <c r="B49" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="C49" s="7">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D49" s="7">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E49" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F49" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>128</v>
+      <c r="F49" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49" s="39" t="s">
+        <v>127</v>
       </c>
       <c r="H49" s="31" t="s">
         <v>73</v>
@@ -5403,23 +5478,23 @@
     </row>
     <row r="50" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="50"/>
-      <c r="B50" s="19" t="s">
-        <v>71</v>
+      <c r="B50" s="37" t="s">
+        <v>72</v>
       </c>
       <c r="C50" s="7">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D50" s="7">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E50" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F50" s="20" t="s">
+      <c r="F50" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G50" s="22" t="s">
-        <v>129</v>
+      <c r="G50" s="23" t="s">
+        <v>130</v>
       </c>
       <c r="H50" s="31" t="s">
         <v>73</v>
@@ -5479,83 +5554,8 @@
         <v>-0.20833333333333337</v>
       </c>
     </row>
-    <row r="51" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="50"/>
-      <c r="B51" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" s="7">
-        <v>49</v>
-      </c>
-      <c r="D51" s="7">
-        <v>46</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F51" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="G51" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="H51" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="I51" s="24">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="J51" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="K51" s="26">
-        <f>$I51+Sheet2!B$1/24</f>
-        <v>0.5</v>
-      </c>
-      <c r="L51" s="24">
-        <f>$I51+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="M51" s="24">
-        <f>$I51+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
-      </c>
-      <c r="N51" s="24">
-        <f>$I51+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
-      </c>
-      <c r="O51" s="24">
-        <f>$I51+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
-      </c>
-      <c r="P51" s="24">
-        <f>$I51+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
-      </c>
-      <c r="Q51" s="24">
-        <f>$I51+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="R51" s="24">
-        <f>$I51+Sheet2!B$8/24</f>
-        <v>0.125</v>
-      </c>
-      <c r="S51" s="24">
-        <f>$I51+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
-      </c>
-      <c r="T51" s="24">
-        <f>$I51+Sheet2!B$10/24</f>
-        <v>-0.125</v>
-      </c>
-      <c r="U51" s="24">
-        <f>$I51+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
-      </c>
-      <c r="V51" s="24">
-        <f>$I51+Sheet2!B$12/24</f>
-        <v>-0.20833333333333337</v>
-      </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="50"/>
@@ -5580,7 +5580,7 @@
     <mergeCell ref="A6:A20"/>
     <mergeCell ref="A21:A53"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L4 K42:V51 K4:V40">
+  <conditionalFormatting sqref="K2:L4 K4:V50">
     <cfRule type="expression" dxfId="46" priority="104">
       <formula>K$1=$H2</formula>
     </cfRule>
@@ -5590,7 +5590,7 @@
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G49:G51 B2:V22 K23:V23 G30:V30 G23 B23:D23 B24:V29 B30:D30 C31 B32:V34 K35:V35 G35 C35:D35 B36:V36 G37:V37 B37:D37 K43:V51 K38:V38 G43:G47 G38 C43:D51 C38:D38 B42:V42 B39:V40">
+  <conditionalFormatting sqref="B2:V3 K23:V23 G30:V30 G23 B32:B34 K35:V35 G35 G37:V37 B36:B37 K38:V40 G38:G40 B41:B42 B44 K43:V43 G43 G50 G45:G48 K45:V50 E44:V44 E41:V42 E36:V36 E32:V34 E24:V29 B4:B30 E4:V22 C4:D50">
     <cfRule type="expression" dxfId="44" priority="110">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -5605,27 +5605,27 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43 J43:V43">
+  <conditionalFormatting sqref="B40 J40:V40">
     <cfRule type="expression" dxfId="41" priority="83">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44 J44:V44">
+  <conditionalFormatting sqref="B43 J43:V43">
     <cfRule type="expression" dxfId="40" priority="81">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45 J45:V45">
+  <conditionalFormatting sqref="B39 J39:V39">
     <cfRule type="expression" dxfId="39" priority="79">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B46 J46:V46">
+  <conditionalFormatting sqref="B45 J45:V45">
     <cfRule type="expression" dxfId="38" priority="77">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47 J47:V47 E47:F47 H47">
+  <conditionalFormatting sqref="B46 J46:V46 E46:F46 H46">
     <cfRule type="expression" dxfId="37" priority="75">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -5635,47 +5635,47 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
+  <conditionalFormatting sqref="E43">
     <cfRule type="expression" dxfId="35" priority="70">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
+  <conditionalFormatting sqref="E39">
     <cfRule type="expression" dxfId="34" priority="69">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46 H46">
+  <conditionalFormatting sqref="E45 H45">
     <cfRule type="expression" dxfId="33" priority="68">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48 J48:V48">
+  <conditionalFormatting sqref="B49 J49:V49">
     <cfRule type="expression" dxfId="32" priority="66">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49 J49:V49 E49">
+  <conditionalFormatting sqref="B48 J48:V48 E48">
     <cfRule type="expression" dxfId="31" priority="64">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48:F48 H48">
+  <conditionalFormatting sqref="E49:F49 H49">
     <cfRule type="expression" dxfId="30" priority="62">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50 J50:V50">
+  <conditionalFormatting sqref="B47 J47:V47">
     <cfRule type="expression" dxfId="29" priority="60">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51 J51:V51 E51">
+  <conditionalFormatting sqref="B50 J50:V50 E50">
     <cfRule type="expression" dxfId="28" priority="58">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F45">
+  <conditionalFormatting sqref="F39">
     <cfRule type="expression" dxfId="27" priority="50">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -5690,32 +5690,32 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
+  <conditionalFormatting sqref="I40">
     <cfRule type="expression" dxfId="24" priority="38">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
+  <conditionalFormatting sqref="I43">
     <cfRule type="expression" dxfId="23" priority="37">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
+  <conditionalFormatting sqref="I39">
     <cfRule type="expression" dxfId="22" priority="36">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
+  <conditionalFormatting sqref="I45">
     <cfRule type="expression" dxfId="21" priority="35">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
+  <conditionalFormatting sqref="I46">
     <cfRule type="expression" dxfId="20" priority="34">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I48">
+  <conditionalFormatting sqref="I49">
     <cfRule type="expression" dxfId="19" priority="33">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -5730,62 +5730,62 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
+  <conditionalFormatting sqref="H40">
     <cfRule type="expression" dxfId="16" priority="24">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H44">
+  <conditionalFormatting sqref="H43">
     <cfRule type="expression" dxfId="15" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H45">
+  <conditionalFormatting sqref="H39">
     <cfRule type="expression" dxfId="14" priority="22">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H49">
+  <conditionalFormatting sqref="H48">
     <cfRule type="expression" dxfId="13" priority="21">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I49">
+  <conditionalFormatting sqref="I48">
     <cfRule type="expression" dxfId="12" priority="20">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
+  <conditionalFormatting sqref="H47">
     <cfRule type="expression" dxfId="11" priority="19">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I50">
+  <conditionalFormatting sqref="I47">
     <cfRule type="expression" dxfId="10" priority="18">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
+  <conditionalFormatting sqref="H50">
     <cfRule type="expression" dxfId="9" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I51">
+  <conditionalFormatting sqref="I50">
     <cfRule type="expression" dxfId="8" priority="16">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F44">
+  <conditionalFormatting sqref="F43">
     <cfRule type="expression" dxfId="7" priority="12">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F46">
+  <conditionalFormatting sqref="F45">
     <cfRule type="expression" dxfId="6" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
+  <conditionalFormatting sqref="F48">
     <cfRule type="expression" dxfId="5" priority="10">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -5795,7 +5795,7 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E43:F43">
+  <conditionalFormatting sqref="E40:F40">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -5805,12 +5805,12 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50:F50">
+  <conditionalFormatting sqref="E47:F47">
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31 D31:V31">
+  <conditionalFormatting sqref="B31 E31:V31">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add temporary excel file to gitignore list
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93777D04-7F28-8548-BE40-4A84DD680C52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CC74DA-6132-284F-92F9-D4E2ED63A47D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="1240" windowWidth="33700" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1609,7 +1609,7 @@
   <dimension ref="A1:V53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add BigHoov, update StormTrooper Gary country, flag and time zone
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CC74DA-6132-284F-92F9-D4E2ED63A47D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E357A0E-043A-D648-A9FC-A12F057B8C35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="1240" windowWidth="33700" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="740" windowWidth="33700" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <customWorkbookViews>
+    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="157">
   <si>
     <t>Name</t>
   </si>
@@ -119,9 +119,6 @@
     <t>5/11</t>
   </si>
   <si>
-    <t>Guam</t>
-  </si>
-  <si>
     <t>ChST</t>
   </si>
   <si>
@@ -501,6 +498,18 @@
   </si>
   <si>
     <t>https://swgoh.gg/u/psulion/</t>
+  </si>
+  <si>
+    <t>BigHoov (HS)</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/u/bighoov/</t>
+  </si>
+  <si>
+    <t>:flag_hk:</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
   </si>
 </sst>
 </file>
@@ -959,7 +968,57 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="54">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF920000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1606,10 +1665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V53"/>
+  <dimension ref="A1:V54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1660,10 +1719,10 @@
         <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>9</v>
@@ -1693,15 +1752,15 @@
         <v>EDT</v>
       </c>
       <c r="T1" s="3" t="str">
-        <f>H44</f>
+        <f>H45</f>
         <v>CDT</v>
       </c>
       <c r="U1" s="3" t="str">
-        <f>H36</f>
+        <f>H37</f>
         <v>CDT</v>
       </c>
       <c r="V1" s="3" t="str">
-        <f>H41</f>
+        <f>H42</f>
         <v>CDT</v>
       </c>
     </row>
@@ -1710,7 +1769,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -1719,13 +1778,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>26</v>
+        <v>156</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>27</v>
@@ -1788,7 +1847,7 @@
     <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18"/>
       <c r="B3" s="38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" s="7">
         <v>2</v>
@@ -1797,14 +1856,14 @@
         <v>2</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I3" s="10">
         <v>0.41666666666666669</v>
@@ -1864,7 +1923,7 @@
     <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="45"/>
       <c r="B4" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="7">
         <v>3</v>
@@ -1873,16 +1932,16 @@
         <v>3</v>
       </c>
       <c r="E4" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="29" t="s">
         <v>150</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="G4" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>151</v>
       </c>
       <c r="I4" s="24">
         <v>11.458333333333334</v>
@@ -1942,7 +2001,7 @@
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="46"/>
       <c r="B5" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="7">
         <v>4</v>
@@ -1954,10 +2013,10 @@
         <v>20</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H5" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2020,10 +2079,10 @@
     </row>
     <row r="6" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="7">
         <v>5</v>
@@ -2032,13 +2091,13 @@
         <v>5</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H6" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2102,7 +2161,7 @@
     <row r="7" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="47"/>
       <c r="B7" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="7">
         <v>6</v>
@@ -2117,7 +2176,7 @@
         <v>19</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H7" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2181,7 +2240,7 @@
     <row r="8" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="47"/>
       <c r="B8" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="7">
         <v>7</v>
@@ -2193,10 +2252,10 @@
         <v>20</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2260,7 +2319,7 @@
     <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="47"/>
       <c r="B9" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="7">
         <v>8</v>
@@ -2272,10 +2331,10 @@
         <v>16</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H9" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2339,7 +2398,7 @@
     <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="47"/>
       <c r="B10" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="7">
         <v>9</v>
@@ -2351,10 +2410,10 @@
         <v>18</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H10" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2418,7 +2477,7 @@
     <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
       <c r="B11" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="7">
         <v>10</v>
@@ -2427,13 +2486,13 @@
         <v>10</v>
       </c>
       <c r="E11" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="G11" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H11" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2497,7 +2556,7 @@
     <row r="12" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="47"/>
       <c r="B12" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="7">
         <v>11</v>
@@ -2509,10 +2568,10 @@
         <v>16</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H12" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2576,7 +2635,7 @@
     <row r="13" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="47"/>
       <c r="B13" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="7">
         <v>12</v>
@@ -2591,7 +2650,7 @@
         <v>19</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H13" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2655,7 +2714,7 @@
     <row r="14" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
       <c r="B14" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="7">
         <v>13</v>
@@ -2667,10 +2726,10 @@
         <v>16</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2734,7 +2793,7 @@
     <row r="15" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="47"/>
       <c r="B15" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="7">
         <v>14</v>
@@ -2743,13 +2802,13 @@
         <v>14</v>
       </c>
       <c r="E15" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>93</v>
-      </c>
       <c r="G15" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H15" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2813,7 +2872,7 @@
     <row r="16" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="47"/>
       <c r="B16" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="7">
         <v>15</v>
@@ -2822,13 +2881,13 @@
         <v>15</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16" s="31" t="s">
         <v>12</v>
@@ -2891,7 +2950,7 @@
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="47"/>
       <c r="B17" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="7">
         <v>16</v>
@@ -2900,13 +2959,13 @@
         <v>16</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>22</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H17" s="29" t="s">
         <v>12</v>
@@ -2969,7 +3028,7 @@
     <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="47"/>
       <c r="B18" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="7">
         <v>17</v>
@@ -2978,13 +3037,13 @@
         <v>17</v>
       </c>
       <c r="E18" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="G18" s="36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H18" s="31" t="s">
         <v>12</v>
@@ -3047,7 +3106,7 @@
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="47"/>
       <c r="B19" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="7">
         <v>18</v>
@@ -3056,13 +3115,13 @@
         <v>18</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H19" s="31" t="s">
         <v>12</v>
@@ -3125,7 +3184,7 @@
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="48"/>
       <c r="B20" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" s="7">
         <v>19</v>
@@ -3134,13 +3193,13 @@
         <v>19</v>
       </c>
       <c r="E20" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="G20" s="36" t="s">
         <v>96</v>
-      </c>
-      <c r="G20" s="36" t="s">
-        <v>97</v>
       </c>
       <c r="H20" s="31" t="s">
         <v>12</v>
@@ -3205,7 +3264,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="7">
         <v>20</v>
@@ -3214,13 +3273,13 @@
         <v>20</v>
       </c>
       <c r="E21" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="G21" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H21" s="31" t="s">
         <v>12</v>
@@ -3283,7 +3342,7 @@
     <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="50"/>
       <c r="B22" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C22" s="7">
         <v>21</v>
@@ -3292,13 +3351,13 @@
         <v>21</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H22" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3362,7 +3421,7 @@
     <row r="23" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="50"/>
       <c r="B23" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C23" s="7">
         <v>22</v>
@@ -3371,16 +3430,16 @@
         <v>22</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23" s="42" t="s">
         <v>22</v>
       </c>
       <c r="G23" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="H23" s="42" t="s">
         <v>145</v>
-      </c>
-      <c r="H23" s="42" t="s">
-        <v>146</v>
       </c>
       <c r="I23" s="43">
         <v>0.95833333333333337</v>
@@ -3440,7 +3499,7 @@
     <row r="24" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="50"/>
       <c r="B24" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="7">
         <v>23</v>
@@ -3449,13 +3508,13 @@
         <v>23</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24" s="20" t="s">
         <v>22</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H24" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3519,7 +3578,7 @@
     <row r="25" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="50"/>
       <c r="B25" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="7">
         <v>24</v>
@@ -3528,13 +3587,13 @@
         <v>24</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F25" s="20" t="s">
         <v>22</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H25" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3598,7 +3657,7 @@
     <row r="26" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="50"/>
       <c r="B26" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="7">
         <v>25</v>
@@ -3607,13 +3666,13 @@
         <v>25</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F26" s="20" t="s">
         <v>22</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H26" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3677,7 +3736,7 @@
     <row r="27" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="50"/>
       <c r="B27" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="7">
         <v>26</v>
@@ -3686,13 +3745,13 @@
         <v>26</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F27" s="20" t="s">
         <v>22</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H27" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3756,7 +3815,7 @@
     <row r="28" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="50"/>
       <c r="B28" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="7">
         <v>27</v>
@@ -3765,13 +3824,13 @@
         <v>27</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F28" s="20" t="s">
         <v>22</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H28" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3835,7 +3894,7 @@
     <row r="29" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="50"/>
       <c r="B29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="7">
         <v>28</v>
@@ -3844,13 +3903,13 @@
         <v>28</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F29" s="20" t="s">
         <v>22</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H29" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3914,7 +3973,7 @@
     <row r="30" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="50"/>
       <c r="B30" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C30" s="7">
         <v>29</v>
@@ -3923,13 +3982,13 @@
         <v>29</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F30" s="42" t="s">
         <v>22</v>
       </c>
       <c r="G30" s="31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H30" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3993,7 +4052,7 @@
     <row r="31" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="50"/>
       <c r="B31" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C31" s="7">
         <v>30</v>
@@ -4002,13 +4061,13 @@
         <v>30</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F31" s="20" t="s">
         <v>22</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H31" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4072,7 +4131,7 @@
     <row r="32" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="50"/>
       <c r="B32" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="7">
         <v>31</v>
@@ -4081,13 +4140,13 @@
         <v>31</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F32" s="20" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H32" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4151,7 +4210,7 @@
     <row r="33" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="50"/>
       <c r="B33" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="7">
         <v>32</v>
@@ -4160,13 +4219,13 @@
         <v>32</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F33" s="20" t="s">
         <v>22</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H33" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4230,7 +4289,7 @@
     <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="50"/>
       <c r="B34" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="7">
         <v>33</v>
@@ -4239,13 +4298,13 @@
         <v>33</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H34" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4309,7 +4368,7 @@
     <row r="35" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="50"/>
       <c r="B35" s="37" t="s">
-        <v>62</v>
+        <v>153</v>
       </c>
       <c r="C35" s="7">
         <v>34</v>
@@ -4318,16 +4377,16 @@
         <v>34</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F35" s="20" t="s">
         <v>22</v>
       </c>
       <c r="G35" s="31" t="s">
-        <v>76</v>
+        <v>154</v>
       </c>
       <c r="H35" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I35" s="24">
         <v>0</v>
@@ -4387,25 +4446,25 @@
     <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="50"/>
       <c r="B36" s="37" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C36" s="7">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="7">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="G36" s="31" t="s">
-        <v>135</v>
-      </c>
       <c r="H36" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I36" s="24">
         <v>0</v>
@@ -4464,31 +4523,31 @@
     </row>
     <row r="37" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="50"/>
-      <c r="B37" s="19" t="s">
-        <v>138</v>
+      <c r="B37" s="37" t="s">
+        <v>59</v>
       </c>
       <c r="C37" s="7">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="7">
-        <v>36</v>
-      </c>
-      <c r="E37" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="F37" s="42" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H37" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I37" s="24">
         <v>0</v>
       </c>
-      <c r="J37" s="28" t="s">
+      <c r="J37" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K37" s="26">
@@ -4543,30 +4602,30 @@
     <row r="38" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="50"/>
       <c r="B38" s="19" t="s">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="C38" s="7">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="7">
-        <v>37</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F38" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="42" t="s">
         <v>22</v>
       </c>
       <c r="G38" s="31" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="H38" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I38" s="24">
         <v>0</v>
       </c>
-      <c r="J38" s="30" t="s">
+      <c r="J38" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K38" s="26">
@@ -4620,26 +4679,26 @@
     </row>
     <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="50"/>
-      <c r="B39" s="37" t="s">
-        <v>66</v>
+      <c r="B39" s="19" t="s">
+        <v>62</v>
       </c>
       <c r="C39" s="7">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39" s="7">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="G39" s="31" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H39" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I39" s="24">
         <v>0</v>
@@ -4699,25 +4758,25 @@
     <row r="40" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="50"/>
       <c r="B40" s="37" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C40" s="7">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40" s="7">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="29" t="s">
-        <v>123</v>
+        <v>47</v>
+      </c>
+      <c r="G40" s="31" t="s">
+        <v>124</v>
       </c>
       <c r="H40" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I40" s="24">
         <v>0</v>
@@ -4776,26 +4835,26 @@
     </row>
     <row r="41" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="50"/>
-      <c r="B41" s="19" t="s">
-        <v>61</v>
+      <c r="B41" s="37" t="s">
+        <v>63</v>
       </c>
       <c r="C41" s="7">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41" s="7">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G41" s="31" t="s">
-        <v>143</v>
+        <v>29</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="29" t="s">
+        <v>122</v>
       </c>
       <c r="H41" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I41" s="24">
         <v>0</v>
@@ -4855,30 +4914,30 @@
     <row r="42" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="50"/>
       <c r="B42" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C42" s="7">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D42" s="7">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>22</v>
+        <v>29</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="G42" s="31" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="H42" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I42" s="24">
         <v>0</v>
       </c>
-      <c r="J42" s="28" t="s">
+      <c r="J42" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K42" s="26">
@@ -4930,33 +4989,33 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="50"/>
       <c r="B43" s="19" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C43" s="7">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D43" s="7">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>75</v>
+        <v>29</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="G43" s="31" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="H43" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I43" s="24">
         <v>0</v>
       </c>
-      <c r="J43" s="30" t="s">
+      <c r="J43" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K43" s="26">
@@ -5008,33 +5067,33 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="50"/>
       <c r="B44" s="19" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C44" s="7">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D44" s="7">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F44" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44" s="29" t="s">
-        <v>118</v>
+        <v>29</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="31" t="s">
+        <v>123</v>
       </c>
       <c r="H44" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I44" s="24">
         <v>0</v>
       </c>
-      <c r="J44" s="28" t="s">
+      <c r="J44" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K44" s="26">
@@ -5089,102 +5148,102 @@
     <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="50"/>
       <c r="B45" s="19" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C45" s="7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D45" s="7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G45" s="36" t="s">
-        <v>126</v>
+        <v>29</v>
+      </c>
+      <c r="F45" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" s="29" t="s">
+        <v>117</v>
       </c>
       <c r="H45" s="31" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="I45" s="24">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J45" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="J45" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K45" s="26">
         <f>$I45+Sheet2!B$1/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L45" s="24">
         <f>$I45+Sheet2!B$2/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="M45" s="24">
         <f>$I45+Sheet2!B$3/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N45" s="24">
         <f>$I45+Sheet2!B$4/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="O45" s="24">
         <f>$I45+Sheet2!B$5/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="P45" s="24">
         <f>$I45+Sheet2!B$6/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="Q45" s="24">
         <f>$I45+Sheet2!B$7/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R45" s="24">
         <f>$I45+Sheet2!B$8/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="S45" s="24">
         <f>$I45+Sheet2!B$9/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="T45" s="24">
         <f>$I45+Sheet2!B$10/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="U45" s="24">
         <f>$I45+Sheet2!B$11/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.25</v>
       </c>
       <c r="V45" s="24">
         <f>$I45+Sheet2!B$12/24</f>
-        <v>-0.25</v>
+        <v>-0.29166666666666669</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="50"/>
-      <c r="B46" s="37" t="s">
-        <v>68</v>
+      <c r="B46" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="C46" s="7">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D46" s="7">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>22</v>
+        <v>140</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>141</v>
       </c>
       <c r="G46" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="H46" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="H46" s="31" t="s">
         <v>13</v>
       </c>
       <c r="I46" s="24">
@@ -5244,104 +5303,104 @@
     </row>
     <row r="47" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="50"/>
-      <c r="B47" s="19" t="s">
-        <v>71</v>
+      <c r="B47" s="37" t="s">
+        <v>67</v>
       </c>
       <c r="C47" s="7">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D47" s="7">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F47" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G47" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H47" s="31" t="s">
-        <v>73</v>
+      <c r="G47" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="H47" s="37" t="s">
+        <v>13</v>
       </c>
       <c r="I47" s="24">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J47" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K47" s="26">
         <f>$I47+Sheet2!B$1/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="L47" s="24">
         <f>$I47+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M47" s="24">
         <f>$I47+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="N47" s="24">
         <f>$I47+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="O47" s="24">
         <f>$I47+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P47" s="24">
         <f>$I47+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q47" s="24">
         <f>$I47+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="R47" s="24">
         <f>$I47+Sheet2!B$8/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S47" s="24">
         <f>$I47+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="T47" s="24">
         <f>$I47+Sheet2!B$10/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="U47" s="24">
         <f>$I47+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="V47" s="24">
         <f>$I47+Sheet2!B$12/24</f>
-        <v>-0.20833333333333337</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="50"/>
-      <c r="B48" s="37" t="s">
+      <c r="B48" s="19" t="s">
         <v>70</v>
       </c>
       <c r="C48" s="7">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" s="7">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G48" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="22" t="s">
         <v>128</v>
       </c>
       <c r="H48" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I48" s="24">
         <v>8.3333333333333329E-2</v>
@@ -5400,26 +5459,26 @@
     </row>
     <row r="49" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="50"/>
-      <c r="B49" s="19" t="s">
+      <c r="B49" s="37" t="s">
         <v>69</v>
       </c>
       <c r="C49" s="7">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D49" s="7">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G49" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G49" s="9" t="s">
         <v>127</v>
       </c>
       <c r="H49" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I49" s="24">
         <v>8.3333333333333329E-2</v>
@@ -5478,26 +5537,26 @@
     </row>
     <row r="50" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="50"/>
-      <c r="B50" s="37" t="s">
+      <c r="B50" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="7">
+        <v>48</v>
+      </c>
+      <c r="D50" s="7">
+        <v>48</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="H50" s="31" t="s">
         <v>72</v>
-      </c>
-      <c r="C50" s="7">
-        <v>49</v>
-      </c>
-      <c r="D50" s="7">
-        <v>49</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F50" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="G50" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="H50" s="31" t="s">
-        <v>73</v>
       </c>
       <c r="I50" s="24">
         <v>8.3333333333333329E-2</v>
@@ -5554,8 +5613,83 @@
         <v>-0.20833333333333337</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="50"/>
+      <c r="B51" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="7">
+        <v>49</v>
+      </c>
+      <c r="D51" s="7">
+        <v>49</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G51" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="H51" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="I51" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J51" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K51" s="26">
+        <f>$I51+Sheet2!B$1/24</f>
+        <v>0.5</v>
+      </c>
+      <c r="L51" s="24">
+        <f>$I51+Sheet2!B$2/24</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M51" s="24">
+        <f>$I51+Sheet2!B$3/24</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="N51" s="24">
+        <f>$I51+Sheet2!B$4/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="O51" s="24">
+        <f>$I51+Sheet2!B$5/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P51" s="24">
+        <f>$I51+Sheet2!B$6/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="Q51" s="24">
+        <f>$I51+Sheet2!B$7/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R51" s="24">
+        <f>$I51+Sheet2!B$8/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="S51" s="24">
+        <f>$I51+Sheet2!B$9/24</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="T51" s="24">
+        <f>$I51+Sheet2!B$10/24</f>
+        <v>-0.125</v>
+      </c>
+      <c r="U51" s="24">
+        <f>$I51+Sheet2!B$11/24</f>
+        <v>-0.16666666666666669</v>
+      </c>
+      <c r="V51" s="24">
+        <f>$I51+Sheet2!B$12/24</f>
+        <v>-0.20833333333333337</v>
+      </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="50"/>
@@ -5563,255 +5697,293 @@
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" s="50"/>
     </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A54" s="50"/>
+    </row>
   </sheetData>
-  <sortState ref="B2:V42">
-    <sortCondition ref="D2:D42"/>
+  <sortState ref="B2:V43">
+    <sortCondition ref="D2:D43"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
+      <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
-      <selection sqref="A1:XFD1048576"/>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
     <mergeCell ref="A6:A20"/>
-    <mergeCell ref="A21:A53"/>
+    <mergeCell ref="A21:A54"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L4 K4:V50">
-    <cfRule type="expression" dxfId="46" priority="104">
+  <conditionalFormatting sqref="K2:L4 K4:V34 K36:V51">
+    <cfRule type="expression" dxfId="53" priority="111">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V4">
-    <cfRule type="expression" dxfId="45" priority="106">
+    <cfRule type="expression" dxfId="52" priority="113">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:V3 K23:V23 G30:V30 G23 B32:B34 K35:V35 G35 G37:V37 B36:B37 K38:V40 G38:G40 B41:B42 B44 K43:V43 G43 G50 G45:G48 K45:V50 E44:V44 E41:V42 E36:V36 E32:V34 E24:V29 B4:B30 E4:V22 C4:D50">
-    <cfRule type="expression" dxfId="44" priority="110">
+  <conditionalFormatting sqref="B2:V3 K23:V23 G30:V30 G23 B32:B34 K36:V36 G36 G38:V38 B37:B38 K39:V41 G39:G41 B42:B43 B45 K44:V44 G44 G51 G46:G49 K46:V51 E45:V45 E42:V43 E37:V37 E32:V34 E24:V29 B4:B30 E4:V22 C4:D34 C36:D51">
+    <cfRule type="expression" dxfId="51" priority="117">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36 J36:V36">
+    <cfRule type="expression" dxfId="50" priority="94">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39 J39:V39">
+    <cfRule type="expression" dxfId="49" priority="92">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41 J41:V41">
+    <cfRule type="expression" dxfId="48" priority="90">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44 J44:V44">
+    <cfRule type="expression" dxfId="47" priority="88">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40 J40:V40">
+    <cfRule type="expression" dxfId="46" priority="86">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46 J46:V46">
+    <cfRule type="expression" dxfId="45" priority="84">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47 J47:V47 E47:F47 H47">
+    <cfRule type="expression" dxfId="44" priority="82">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="expression" dxfId="43" priority="80">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="expression" dxfId="42" priority="77">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="expression" dxfId="41" priority="76">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46 H46">
+    <cfRule type="expression" dxfId="40" priority="75">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50 J50:V50">
+    <cfRule type="expression" dxfId="39" priority="73">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49 J49:V49 E49">
+    <cfRule type="expression" dxfId="38" priority="71">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50:F50 H50">
+    <cfRule type="expression" dxfId="37" priority="69">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48 J48:V48">
+    <cfRule type="expression" dxfId="36" priority="67">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B51 J51:V51 E51">
+    <cfRule type="expression" dxfId="35" priority="65">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40">
+    <cfRule type="expression" dxfId="34" priority="57">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="expression" dxfId="33" priority="47">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="expression" dxfId="32" priority="46">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
+    <cfRule type="expression" dxfId="31" priority="45">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="expression" dxfId="30" priority="44">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="expression" dxfId="29" priority="43">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I46">
+    <cfRule type="expression" dxfId="28" priority="42">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I47">
+    <cfRule type="expression" dxfId="27" priority="41">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50">
+    <cfRule type="expression" dxfId="26" priority="40">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
+    <cfRule type="expression" dxfId="25" priority="33">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H39">
+    <cfRule type="expression" dxfId="24" priority="32">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H41">
+    <cfRule type="expression" dxfId="23" priority="31">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H44">
+    <cfRule type="expression" dxfId="22" priority="30">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H40">
+    <cfRule type="expression" dxfId="21" priority="29">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H49">
+    <cfRule type="expression" dxfId="20" priority="28">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I49">
+    <cfRule type="expression" dxfId="19" priority="27">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H48">
+    <cfRule type="expression" dxfId="18" priority="26">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I48">
+    <cfRule type="expression" dxfId="17" priority="25">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H51">
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I51">
+    <cfRule type="expression" dxfId="15" priority="23">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44">
+    <cfRule type="expression" dxfId="14" priority="19">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46">
+    <cfRule type="expression" dxfId="13" priority="18">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F49">
+    <cfRule type="expression" dxfId="12" priority="17">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F36">
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41:F41">
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39:F39">
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48:F48">
+    <cfRule type="expression" dxfId="8" priority="10">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31 E31:V31">
+    <cfRule type="expression" dxfId="7" priority="9">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K35:V35">
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>K$1=$H35</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K35:V35 G35 C35:D35">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35 J35:V35">
-    <cfRule type="expression" dxfId="43" priority="87">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38 J38:V38">
-    <cfRule type="expression" dxfId="42" priority="85">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40 J40:V40">
-    <cfRule type="expression" dxfId="41" priority="83">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B43 J43:V43">
-    <cfRule type="expression" dxfId="40" priority="81">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39 J39:V39">
-    <cfRule type="expression" dxfId="39" priority="79">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45 J45:V45">
-    <cfRule type="expression" dxfId="38" priority="77">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46 J46:V46 E46:F46 H46">
-    <cfRule type="expression" dxfId="37" priority="75">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" dxfId="36" priority="73">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
-    <cfRule type="expression" dxfId="35" priority="70">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="34" priority="69">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45 H45">
-    <cfRule type="expression" dxfId="33" priority="68">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49 J49:V49">
-    <cfRule type="expression" dxfId="32" priority="66">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B48 J48:V48 E48">
-    <cfRule type="expression" dxfId="31" priority="64">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49:F49 H49">
-    <cfRule type="expression" dxfId="30" priority="62">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47 J47:V47">
-    <cfRule type="expression" dxfId="29" priority="60">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B50 J50:V50 E50">
-    <cfRule type="expression" dxfId="28" priority="58">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
-    <cfRule type="expression" dxfId="27" priority="50">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="expression" dxfId="26" priority="40">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="25" priority="39">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="24" priority="38">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="23" priority="37">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="expression" dxfId="22" priority="36">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
-    <cfRule type="expression" dxfId="21" priority="35">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="20" priority="34">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I49">
-    <cfRule type="expression" dxfId="19" priority="33">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="18" priority="26">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="17" priority="25">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
-    <cfRule type="expression" dxfId="16" priority="24">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
-    <cfRule type="expression" dxfId="15" priority="23">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
-    <cfRule type="expression" dxfId="14" priority="22">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
-    <cfRule type="expression" dxfId="13" priority="21">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="12" priority="20">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
-    <cfRule type="expression" dxfId="11" priority="19">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="10" priority="18">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="9" priority="17">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I50">
-    <cfRule type="expression" dxfId="8" priority="16">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="7" priority="12">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45">
-    <cfRule type="expression" dxfId="6" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48">
-    <cfRule type="expression" dxfId="5" priority="10">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35">
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40:F40">
-    <cfRule type="expression" dxfId="3" priority="5">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E38:F38">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47:F47">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B31 E31:V31">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5838,7 +6010,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1">
         <v>10</v>
@@ -5849,7 +6021,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>9</v>

</xml_diff>

<commit_message>
Add time zone headings on payout schedule
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31518659-5B1E-CC46-9967-73DDAC2E3746}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1B54A5-4E6A-F84C-B8CF-DF31A0703226}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="740" windowWidth="33700" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="168">
   <si>
     <t>Name</t>
   </si>
@@ -516,6 +516,33 @@
   </si>
   <si>
     <t>https://swgoh.gg/u/spell/</t>
+  </si>
+  <si>
+    <t>TZ EST</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">:clock1: </t>
+  </si>
+  <si>
+    <t>:clock2:</t>
+  </si>
+  <si>
+    <t>TZ CEST</t>
+  </si>
+  <si>
+    <t>TZ BST</t>
+  </si>
+  <si>
+    <t>:clock7:</t>
+  </si>
+  <si>
+    <t>TZ CST</t>
+  </si>
+  <si>
+    <t>:clock8:</t>
   </si>
 </sst>
 </file>
@@ -889,7 +916,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -960,6 +987,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -974,11 +1004,56 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="60">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF920000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF920000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF920000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1019,9 +1094,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1671,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V55"/>
+  <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1734,39 +1808,39 @@
         <v>9</v>
       </c>
       <c r="N1" s="3" t="str">
-        <f>H11</f>
-        <v>CEST</v>
-      </c>
-      <c r="O1" s="3" t="str">
-        <f>H6</f>
-        <v>CEST</v>
-      </c>
-      <c r="P1" s="3" t="str">
-        <f>H8</f>
-        <v>CEST</v>
-      </c>
-      <c r="Q1" s="3" t="str">
         <f>H12</f>
         <v>CEST</v>
       </c>
+      <c r="O1" s="3" t="str">
+        <f>H7</f>
+        <v>CEST</v>
+      </c>
+      <c r="P1" s="3" t="str">
+        <f>H9</f>
+        <v>CEST</v>
+      </c>
+      <c r="Q1" s="3" t="str">
+        <f>H13</f>
+        <v>CEST</v>
+      </c>
       <c r="R1" s="3" t="str">
-        <f>H18</f>
+        <f>H21</f>
         <v>BST</v>
       </c>
       <c r="S1" s="3" t="str">
-        <f>H33</f>
+        <f>H36</f>
         <v>EDT</v>
       </c>
       <c r="T1" s="3" t="str">
-        <f>H46</f>
+        <f>H50</f>
         <v>CDT</v>
       </c>
       <c r="U1" s="3" t="str">
-        <f>H38</f>
+        <f>H42</f>
         <v>CDT</v>
       </c>
       <c r="V1" s="3" t="str">
-        <f>H43</f>
+        <f>H47</f>
         <v>CDT</v>
       </c>
     </row>
@@ -2005,9 +2079,9 @@
       </c>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="46"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="19" t="s">
-        <v>52</v>
+        <v>163</v>
       </c>
       <c r="C5" s="7">
         <v>4</v>
@@ -2015,14 +2089,12 @@
       <c r="D5" s="7">
         <v>4</v>
       </c>
-      <c r="E5" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>47</v>
+      <c r="E5" s="21"/>
+      <c r="F5" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="H5" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2083,12 +2155,10 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>42</v>
+    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="46"/>
+      <c r="B6" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="C6" s="7">
         <v>5</v>
@@ -2096,78 +2166,80 @@
       <c r="D6" s="7">
         <v>5</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="H6" s="29" t="str">
+      <c r="E6" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="31" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
       <c r="I6" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="12">
         <f>$I6+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="24">
         <f>$I6+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="24">
         <f>$I6+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N6" s="17">
+      <c r="N6" s="24">
         <f>$I6+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O6" s="17">
+      <c r="O6" s="24">
         <f>$I6+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P6" s="17">
+      <c r="P6" s="24">
         <f>$I6+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="Q6" s="24">
         <f>$I6+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R6" s="17">
+      <c r="R6" s="24">
         <f>$I6+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S6" s="17">
+      <c r="S6" s="24">
         <f>$I6+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T6" s="17">
+      <c r="T6" s="24">
         <f>$I6+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U6" s="17">
+      <c r="U6" s="24">
         <f>$I6+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V6" s="17">
+      <c r="V6" s="24">
         <f>$I6+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
-      <c r="B7" s="19" t="s">
-        <v>41</v>
+      <c r="A7" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="C7" s="7">
         <v>6</v>
@@ -2175,14 +2247,14 @@
       <c r="D7" s="7">
         <v>6</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>76</v>
+      <c r="E7" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>87</v>
       </c>
       <c r="H7" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2194,59 +2266,59 @@
       <c r="J7" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="27">
         <f>$I7+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L7" s="24">
+      <c r="L7" s="17">
         <f>$I7+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M7" s="24">
+      <c r="M7" s="17">
         <f>$I7+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="17">
         <f>$I7+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O7" s="24">
+      <c r="O7" s="17">
         <f>$I7+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P7" s="24">
+      <c r="P7" s="17">
         <f>$I7+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q7" s="24">
+      <c r="Q7" s="17">
         <f>$I7+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R7" s="24">
+      <c r="R7" s="17">
         <f>$I7+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S7" s="24">
+      <c r="S7" s="17">
         <f>$I7+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T7" s="24">
+      <c r="T7" s="17">
         <f>$I7+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U7" s="24">
+      <c r="U7" s="17">
         <f>$I7+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V7" s="24">
+      <c r="V7" s="17">
         <f>$I7+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="7">
         <v>7</v>
@@ -2255,13 +2327,13 @@
         <v>7</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>109</v>
+        <v>18</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H8" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2273,7 +2345,7 @@
       <c r="J8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="12">
         <f>$I8+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
@@ -2322,10 +2394,10 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
+    <row r="9" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="48"/>
       <c r="B9" s="19" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C9" s="7">
         <v>8</v>
@@ -2334,22 +2406,22 @@
         <v>8</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="H9" s="31" t="str">
+        <v>20</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="29" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
       <c r="I9" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K9" s="26">
@@ -2402,9 +2474,9 @@
       </c>
     </row>
     <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="47"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" s="7">
         <v>9</v>
@@ -2413,13 +2485,13 @@
         <v>9</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>47</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="H10" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2431,7 +2503,7 @@
       <c r="J10" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="26">
         <f>$I10+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
@@ -2480,10 +2552,10 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="47"/>
+    <row r="11" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="48"/>
       <c r="B11" s="19" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C11" s="7">
         <v>10</v>
@@ -2492,25 +2564,25 @@
         <v>10</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="H11" s="29" t="str">
+        <v>18</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="31" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
       <c r="I11" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="12">
         <f>$I11+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
@@ -2560,9 +2632,9 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="47"/>
-      <c r="B12" s="13" t="s">
-        <v>44</v>
+      <c r="A12" s="48"/>
+      <c r="B12" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="C12" s="7">
         <v>11</v>
@@ -2570,14 +2642,14 @@
       <c r="D12" s="7">
         <v>11</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>16</v>
+      <c r="E12" s="21" t="s">
+        <v>104</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>88</v>
+        <v>105</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="H12" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2586,62 +2658,62 @@
       <c r="I12" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J12" s="30" t="s">
+      <c r="J12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="27">
+      <c r="K12" s="26">
         <f>$I12+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L12" s="17">
+      <c r="L12" s="24">
         <f>$I12+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="24">
         <f>$I12+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N12" s="17">
+      <c r="N12" s="24">
         <f>$I12+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O12" s="17">
+      <c r="O12" s="24">
         <f>$I12+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P12" s="17">
+      <c r="P12" s="24">
         <f>$I12+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q12" s="17">
+      <c r="Q12" s="24">
         <f>$I12+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R12" s="17">
+      <c r="R12" s="24">
         <f>$I12+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S12" s="17">
+      <c r="S12" s="24">
         <f>$I12+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T12" s="17">
+      <c r="T12" s="24">
         <f>$I12+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U12" s="17">
+      <c r="U12" s="24">
         <f>$I12+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V12" s="17">
+      <c r="V12" s="24">
         <f>$I12+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="47"/>
-      <c r="B13" s="19" t="s">
-        <v>49</v>
+    <row r="13" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="48"/>
+      <c r="B13" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="C13" s="7">
         <v>12</v>
@@ -2649,78 +2721,78 @@
       <c r="D13" s="7">
         <v>12</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="H13" s="31" t="str">
+      <c r="E13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="29" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
       <c r="I13" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="26">
+      <c r="K13" s="27">
         <f>$I13+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L13" s="24">
+      <c r="L13" s="17">
         <f>$I13+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M13" s="24">
+      <c r="M13" s="17">
         <f>$I13+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13" s="17">
         <f>$I13+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O13" s="24">
+      <c r="O13" s="17">
         <f>$I13+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P13" s="24">
+      <c r="P13" s="17">
         <f>$I13+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q13" s="24">
+      <c r="Q13" s="17">
         <f>$I13+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R13" s="24">
+      <c r="R13" s="17">
         <f>$I13+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S13" s="24">
+      <c r="S13" s="17">
         <f>$I13+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T13" s="24">
+      <c r="T13" s="17">
         <f>$I13+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U13" s="24">
+      <c r="U13" s="17">
         <f>$I13+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V13" s="24">
+      <c r="V13" s="17">
         <f>$I13+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="47"/>
+    <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="48"/>
       <c r="B14" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" s="7">
         <v>13</v>
@@ -2728,14 +2800,14 @@
       <c r="D14" s="7">
         <v>13</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>16</v>
+      <c r="E14" s="21" t="s">
+        <v>17</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>120</v>
+        <v>19</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="H14" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2744,10 +2816,10 @@
       <c r="I14" s="24">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="26">
         <f>$I14+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
@@ -2797,9 +2869,9 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="47"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="19" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C15" s="7">
         <v>14</v>
@@ -2807,14 +2879,14 @@
       <c r="D15" s="7">
         <v>14</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>92</v>
+      <c r="E15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="H15" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2826,7 +2898,7 @@
       <c r="J15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="26">
+      <c r="K15" s="12">
         <f>$I15+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
@@ -2876,9 +2948,9 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="47"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="19" t="s">
-        <v>55</v>
+        <v>157</v>
       </c>
       <c r="C16" s="7">
         <v>15</v>
@@ -2887,76 +2959,77 @@
         <v>15</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>74</v>
+        <v>18</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H16" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="17">
-        <v>0.75</v>
+        <v>158</v>
+      </c>
+      <c r="H16" s="31" t="str">
+        <f>Sheet2!$A$7</f>
+        <v>CEST</v>
+      </c>
+      <c r="I16" s="24">
+        <v>0.70833333333333337</v>
       </c>
       <c r="J16" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="12">
         <f>$I16+Sheet2!B$1/24</f>
-        <v>1.1666666666666667</v>
+        <v>1.125</v>
       </c>
       <c r="L16" s="24">
         <f>$I16+Sheet2!B$2/24</f>
-        <v>1.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="M16" s="24">
         <f>$I16+Sheet2!B$3/24</f>
-        <v>1.0833333333333333</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="N16" s="24">
         <f>$I16+Sheet2!B$4/24</f>
-        <v>0.875</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="O16" s="24">
         <f>$I16+Sheet2!B$5/24</f>
-        <v>0.875</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="P16" s="24">
         <f>$I16+Sheet2!B$6/24</f>
-        <v>0.875</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="Q16" s="24">
         <f>$I16+Sheet2!B$7/24</f>
-        <v>0.83333333333333337</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="R16" s="24">
         <f>$I16+Sheet2!B$8/24</f>
-        <v>0.79166666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="S16" s="24">
         <f>$I16+Sheet2!B$9/24</f>
-        <v>0.58333333333333337</v>
+        <v>0.54166666666666674</v>
       </c>
       <c r="T16" s="24">
         <f>$I16+Sheet2!B$10/24</f>
-        <v>0.54166666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="U16" s="24">
         <f>$I16+Sheet2!B$11/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="V16" s="24">
         <f>$I16+Sheet2!B$12/24</f>
-        <v>0.45833333333333331</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="47"/>
-      <c r="B17" s="13" t="s">
-        <v>53</v>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="48"/>
+      <c r="B17" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="C17" s="7">
         <v>16</v>
@@ -2964,93 +3037,86 @@
       <c r="D17" s="7">
         <v>16</v>
       </c>
-      <c r="E17" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="17">
+      <c r="E17" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="31" t="str">
+        <f>Sheet2!$A$7</f>
+        <v>CEST</v>
+      </c>
+      <c r="I17" s="24">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="26">
+        <f>$I17+Sheet2!B$1/24</f>
+        <v>1.125</v>
+      </c>
+      <c r="L17" s="24">
+        <f>$I17+Sheet2!B$2/24</f>
+        <v>1.0833333333333335</v>
+      </c>
+      <c r="M17" s="24">
+        <f>$I17+Sheet2!B$3/24</f>
+        <v>1.0416666666666667</v>
+      </c>
+      <c r="N17" s="24">
+        <f>$I17+Sheet2!B$4/24</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="O17" s="24">
+        <f>$I17+Sheet2!B$5/24</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="P17" s="24">
+        <f>$I17+Sheet2!B$6/24</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="Q17" s="24">
+        <f>$I17+Sheet2!B$7/24</f>
+        <v>0.79166666666666674</v>
+      </c>
+      <c r="R17" s="24">
+        <f>$I17+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="J17" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="33">
-        <f>$I17+Sheet2!B$1/24</f>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="L17" s="17">
-        <f>$I17+Sheet2!B$2/24</f>
-        <v>1.125</v>
-      </c>
-      <c r="M17" s="17">
-        <f>$I17+Sheet2!B$3/24</f>
-        <v>1.0833333333333333</v>
-      </c>
-      <c r="N17" s="17">
-        <f>$I17+Sheet2!B$4/24</f>
-        <v>0.875</v>
-      </c>
-      <c r="O17" s="17">
-        <f>$I17+Sheet2!B$5/24</f>
-        <v>0.875</v>
-      </c>
-      <c r="P17" s="17">
-        <f>$I17+Sheet2!B$6/24</f>
-        <v>0.875</v>
-      </c>
-      <c r="Q17" s="17">
-        <f>$I17+Sheet2!B$7/24</f>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="R17" s="17">
-        <f>$I17+Sheet2!B$8/24</f>
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="S17" s="17">
+      <c r="S17" s="24">
         <f>$I17+Sheet2!B$9/24</f>
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="T17" s="17">
+        <v>0.54166666666666674</v>
+      </c>
+      <c r="T17" s="24">
         <f>$I17+Sheet2!B$10/24</f>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="U17" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="U17" s="24">
         <f>$I17+Sheet2!B$11/24</f>
-        <v>0.5</v>
-      </c>
-      <c r="V17" s="17">
+        <v>0.45833333333333337</v>
+      </c>
+      <c r="V17" s="24">
         <f>$I17+Sheet2!B$12/24</f>
-        <v>0.45833333333333331</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="47"/>
-      <c r="B18" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="C18" s="7">
-        <v>17</v>
-      </c>
-      <c r="D18" s="7">
-        <v>17</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>104</v>
-      </c>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="48"/>
+      <c r="B18" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" s="36" t="s">
-        <v>112</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="G18" s="31"/>
       <c r="H18" s="31" t="s">
         <v>12</v>
       </c>
@@ -3109,25 +3175,25 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="47"/>
+    <row r="19" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="48"/>
       <c r="B19" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C19" s="7">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="7">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" s="21" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H19" s="31" t="s">
         <v>12</v>
@@ -3188,419 +3254,413 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="47"/>
-      <c r="B20" s="19" t="s">
-        <v>157</v>
+      <c r="A20" s="48"/>
+      <c r="B20" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="C20" s="7">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="7">
-        <v>19</v>
-      </c>
-      <c r="E20" s="21" t="s">
         <v>18</v>
       </c>
+      <c r="E20" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="F20" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="H20" s="31" t="str">
-        <f>Sheet2!$A$7</f>
-        <v>CEST</v>
+        <v>22</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>12</v>
       </c>
       <c r="I20" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="J20" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="33">
+        <f>$I20+Sheet2!B$1/24</f>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="L20" s="17">
+        <f>$I20+Sheet2!B$2/24</f>
+        <v>1.125</v>
+      </c>
+      <c r="M20" s="17">
+        <f>$I20+Sheet2!B$3/24</f>
+        <v>1.0833333333333333</v>
+      </c>
+      <c r="N20" s="17">
+        <f>$I20+Sheet2!B$4/24</f>
+        <v>0.875</v>
+      </c>
+      <c r="O20" s="17">
+        <f>$I20+Sheet2!B$5/24</f>
+        <v>0.875</v>
+      </c>
+      <c r="P20" s="17">
+        <f>$I20+Sheet2!B$6/24</f>
+        <v>0.875</v>
+      </c>
+      <c r="Q20" s="17">
+        <f>$I20+Sheet2!B$7/24</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="R20" s="17">
+        <f>$I20+Sheet2!B$8/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="J20" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="26">
-        <f>$I20+Sheet2!B$1/24</f>
-        <v>1.2083333333333333</v>
-      </c>
-      <c r="L20" s="24">
-        <f>$I20+Sheet2!B$2/24</f>
-        <v>1.1666666666666665</v>
-      </c>
-      <c r="M20" s="24">
-        <f>$I20+Sheet2!B$3/24</f>
-        <v>1.125</v>
-      </c>
-      <c r="N20" s="24">
-        <f>$I20+Sheet2!B$4/24</f>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="O20" s="24">
-        <f>$I20+Sheet2!B$5/24</f>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="P20" s="24">
-        <f>$I20+Sheet2!B$6/24</f>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="Q20" s="24">
-        <f>$I20+Sheet2!B$7/24</f>
-        <v>0.875</v>
-      </c>
-      <c r="R20" s="24">
-        <f>$I20+Sheet2!B$8/24</f>
-        <v>0.83333333333333326</v>
-      </c>
-      <c r="S20" s="24">
+      <c r="S20" s="17">
         <f>$I20+Sheet2!B$9/24</f>
-        <v>0.625</v>
-      </c>
-      <c r="T20" s="24">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="T20" s="17">
         <f>$I20+Sheet2!B$10/24</f>
-        <v>0.58333333333333326</v>
-      </c>
-      <c r="U20" s="24">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="U20" s="17">
         <f>$I20+Sheet2!B$11/24</f>
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="V20" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="V20" s="17">
         <f>$I20+Sheet2!B$12/24</f>
-        <v>0.49999999999999994</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="48"/>
-      <c r="B21" s="19" t="s">
-        <v>93</v>
+      <c r="B21" s="34" t="s">
+        <v>111</v>
       </c>
       <c r="C21" s="7">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="7">
-        <v>20</v>
-      </c>
-      <c r="E21" s="35" t="s">
-        <v>94</v>
+        <v>19</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>104</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="G21" s="36" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="H21" s="31" t="s">
         <v>12</v>
       </c>
       <c r="I21" s="17">
-        <v>0.79166666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="J21" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K21" s="26">
         <f>$I21+Sheet2!B$1/24</f>
-        <v>1.2083333333333333</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="L21" s="24">
         <f>$I21+Sheet2!B$2/24</f>
-        <v>1.1666666666666665</v>
+        <v>1.125</v>
       </c>
       <c r="M21" s="24">
         <f>$I21+Sheet2!B$3/24</f>
-        <v>1.125</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="N21" s="24">
         <f>$I21+Sheet2!B$4/24</f>
-        <v>0.91666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="O21" s="24">
         <f>$I21+Sheet2!B$5/24</f>
-        <v>0.91666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="P21" s="24">
         <f>$I21+Sheet2!B$6/24</f>
-        <v>0.91666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="Q21" s="24">
         <f>$I21+Sheet2!B$7/24</f>
-        <v>0.875</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="R21" s="24">
         <f>$I21+Sheet2!B$8/24</f>
-        <v>0.83333333333333326</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="S21" s="24">
         <f>$I21+Sheet2!B$9/24</f>
-        <v>0.625</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="T21" s="24">
         <f>$I21+Sheet2!B$10/24</f>
-        <v>0.58333333333333326</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="U21" s="24">
         <f>$I21+Sheet2!B$11/24</f>
-        <v>0.54166666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="V21" s="24">
         <f>$I21+Sheet2!B$12/24</f>
-        <v>0.49999999999999994</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49" t="s">
-        <v>21</v>
-      </c>
+      <c r="A22" s="48"/>
       <c r="B22" s="19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C22" s="7">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="7">
-        <v>21</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>106</v>
+        <v>20</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" s="36" t="s">
-        <v>100</v>
+        <v>132</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>101</v>
       </c>
       <c r="H22" s="31" t="s">
         <v>12</v>
       </c>
       <c r="I22" s="17">
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
       <c r="J22" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K22" s="26">
         <f>$I22+Sheet2!B$1/24</f>
-        <v>1.2916666666666667</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="L22" s="24">
         <f>$I22+Sheet2!B$2/24</f>
-        <v>1.25</v>
+        <v>1.125</v>
       </c>
       <c r="M22" s="24">
         <f>$I22+Sheet2!B$3/24</f>
-        <v>1.2083333333333333</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="N22" s="24">
         <f>$I22+Sheet2!B$4/24</f>
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="O22" s="24">
         <f>$I22+Sheet2!B$5/24</f>
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="P22" s="24">
         <f>$I22+Sheet2!B$6/24</f>
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="Q22" s="24">
         <f>$I22+Sheet2!B$7/24</f>
-        <v>0.95833333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="R22" s="24">
         <f>$I22+Sheet2!B$8/24</f>
-        <v>0.91666666666666663</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="S22" s="24">
         <f>$I22+Sheet2!B$9/24</f>
-        <v>0.70833333333333337</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="T22" s="24">
         <f>$I22+Sheet2!B$10/24</f>
-        <v>0.66666666666666663</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="U22" s="24">
         <f>$I22+Sheet2!B$11/24</f>
-        <v>0.625</v>
+        <v>0.5</v>
       </c>
       <c r="V22" s="24">
         <f>$I22+Sheet2!B$12/24</f>
-        <v>0.58333333333333326</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="19" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C23" s="7">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="7">
-        <v>22</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="H23" s="31" t="str">
-        <f>Sheet2!$A$9</f>
-        <v>EDT</v>
-      </c>
-      <c r="I23" s="24">
-        <v>0.95833333333333337</v>
+        <v>21</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="17">
+        <v>0.79166666666666663</v>
       </c>
       <c r="J23" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K23" s="26">
         <f>$I23+Sheet2!B$1/24</f>
-        <v>1.375</v>
+        <v>1.2083333333333333</v>
       </c>
       <c r="L23" s="24">
         <f>$I23+Sheet2!B$2/24</f>
-        <v>1.3333333333333335</v>
+        <v>1.1666666666666665</v>
       </c>
       <c r="M23" s="24">
         <f>$I23+Sheet2!B$3/24</f>
-        <v>1.2916666666666667</v>
+        <v>1.125</v>
       </c>
       <c r="N23" s="24">
         <f>$I23+Sheet2!B$4/24</f>
-        <v>1.0833333333333335</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="O23" s="24">
         <f>$I23+Sheet2!B$5/24</f>
-        <v>1.0833333333333335</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="P23" s="24">
         <f>$I23+Sheet2!B$6/24</f>
-        <v>1.0833333333333335</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="Q23" s="24">
         <f>$I23+Sheet2!B$7/24</f>
-        <v>1.0416666666666667</v>
+        <v>0.875</v>
       </c>
       <c r="R23" s="24">
         <f>$I23+Sheet2!B$8/24</f>
-        <v>1</v>
+        <v>0.83333333333333326</v>
       </c>
       <c r="S23" s="24">
         <f>$I23+Sheet2!B$9/24</f>
-        <v>0.79166666666666674</v>
+        <v>0.625</v>
       </c>
       <c r="T23" s="24">
         <f>$I23+Sheet2!B$10/24</f>
-        <v>0.75</v>
+        <v>0.58333333333333326</v>
       </c>
       <c r="U23" s="24">
         <f>$I23+Sheet2!B$11/24</f>
-        <v>0.70833333333333337</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="V23" s="24">
         <f>$I23+Sheet2!B$12/24</f>
-        <v>0.66666666666666674</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="50"/>
+        <v>0.49999999999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="50" t="s">
+        <v>21</v>
+      </c>
       <c r="B24" s="19" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
       <c r="C24" s="7">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="7">
-        <v>23</v>
-      </c>
-      <c r="E24" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="G24" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="H24" s="42" t="s">
-        <v>145</v>
-      </c>
-      <c r="I24" s="43">
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="J24" s="44" t="s">
+      <c r="E24" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="17">
+        <v>0.875</v>
+      </c>
+      <c r="J24" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K24" s="26">
         <f>$I24+Sheet2!B$1/24</f>
-        <v>1.375</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="L24" s="24">
         <f>$I24+Sheet2!B$2/24</f>
-        <v>1.3333333333333335</v>
+        <v>1.25</v>
       </c>
       <c r="M24" s="24">
         <f>$I24+Sheet2!B$3/24</f>
-        <v>1.2916666666666667</v>
+        <v>1.2083333333333333</v>
       </c>
       <c r="N24" s="24">
         <f>$I24+Sheet2!B$4/24</f>
-        <v>1.0833333333333335</v>
+        <v>1</v>
       </c>
       <c r="O24" s="24">
         <f>$I24+Sheet2!B$5/24</f>
-        <v>1.0833333333333335</v>
+        <v>1</v>
       </c>
       <c r="P24" s="24">
         <f>$I24+Sheet2!B$6/24</f>
-        <v>1.0833333333333335</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="24">
         <f>$I24+Sheet2!B$7/24</f>
-        <v>1.0416666666666667</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="R24" s="24">
         <f>$I24+Sheet2!B$8/24</f>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="S24" s="24">
         <f>$I24+Sheet2!B$9/24</f>
-        <v>0.79166666666666674</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="T24" s="24">
         <f>$I24+Sheet2!B$10/24</f>
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="U24" s="24">
         <f>$I24+Sheet2!B$11/24</f>
-        <v>0.70833333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="V24" s="24">
         <f>$I24+Sheet2!B$12/24</f>
-        <v>0.66666666666666674</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="50"/>
-      <c r="B25" s="13" t="s">
-        <v>37</v>
+        <v>0.58333333333333326</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="51"/>
+      <c r="B25" s="19" t="s">
+        <v>159</v>
       </c>
       <c r="C25" s="7">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="7">
-        <v>24</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>77</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G25" s="31"/>
       <c r="H25" s="31" t="str">
         <f>Sheet2!$A$9</f>
         <v>EDT</v>
@@ -3611,7 +3671,7 @@
       <c r="J25" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K25" s="12">
+      <c r="K25" s="26">
         <f>$I25+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
@@ -3660,25 +3720,25 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="50"/>
-      <c r="B26" s="13" t="s">
-        <v>35</v>
+    <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="51"/>
+      <c r="B26" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="C26" s="7">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="7">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>29</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="22" t="s">
-        <v>116</v>
+        <v>47</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>114</v>
       </c>
       <c r="H26" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3739,34 +3799,33 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="50"/>
+    <row r="27" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="51"/>
       <c r="B27" s="19" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="C27" s="7">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="7">
-        <v>26</v>
-      </c>
-      <c r="E27" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H27" s="31" t="str">
-        <f>Sheet2!$A$9</f>
-        <v>EDT</v>
-      </c>
-      <c r="I27" s="24">
+      <c r="G27" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="H27" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="I27" s="43">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J27" s="28" t="s">
+      <c r="J27" s="44" t="s">
         <v>15</v>
       </c>
       <c r="K27" s="26">
@@ -3819,15 +3878,15 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="50"/>
+      <c r="A28" s="51"/>
       <c r="B28" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="7">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="7">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>29</v>
@@ -3835,8 +3894,8 @@
       <c r="F28" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G28" s="23" t="s">
-        <v>133</v>
+      <c r="G28" s="16" t="s">
+        <v>77</v>
       </c>
       <c r="H28" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3845,68 +3904,68 @@
       <c r="I28" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J28" s="30" t="s">
+      <c r="J28" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K28" s="33">
+      <c r="K28" s="12">
         <f>$I28+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L28" s="17">
+      <c r="L28" s="24">
         <f>$I28+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M28" s="17">
+      <c r="M28" s="24">
         <f>$I28+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N28" s="17">
+      <c r="N28" s="24">
         <f>$I28+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O28" s="17">
+      <c r="O28" s="24">
         <f>$I28+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P28" s="17">
+      <c r="P28" s="24">
         <f>$I28+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q28" s="17">
+      <c r="Q28" s="24">
         <f>$I28+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R28" s="17">
+      <c r="R28" s="24">
         <f>$I28+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S28" s="17">
+      <c r="S28" s="24">
         <f>$I28+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T28" s="17">
+      <c r="T28" s="24">
         <f>$I28+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U28" s="17">
+      <c r="U28" s="24">
         <f>$I28+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V28" s="17">
+      <c r="V28" s="24">
         <f>$I28+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="50"/>
-      <c r="B29" s="19" t="s">
-        <v>34</v>
+      <c r="A29" s="51"/>
+      <c r="B29" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="C29" s="7">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" s="7">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>29</v>
@@ -3914,8 +3973,8 @@
       <c r="F29" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="9" t="s">
-        <v>79</v>
+      <c r="G29" s="22" t="s">
+        <v>116</v>
       </c>
       <c r="H29" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -3977,15 +4036,15 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="50"/>
+      <c r="A30" s="51"/>
       <c r="B30" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C30" s="7">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="7">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>29</v>
@@ -3993,8 +4052,8 @@
       <c r="F30" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="23" t="s">
-        <v>110</v>
+      <c r="G30" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="H30" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4006,7 +4065,7 @@
       <c r="J30" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K30" s="12">
+      <c r="K30" s="26">
         <f>$I30+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
@@ -4056,24 +4115,24 @@
       </c>
     </row>
     <row r="31" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="50"/>
-      <c r="B31" s="19" t="s">
-        <v>151</v>
+      <c r="A31" s="51"/>
+      <c r="B31" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="C31" s="7">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" s="7">
-        <v>30</v>
-      </c>
-      <c r="E31" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="42" t="s">
+      <c r="E31" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="31" t="s">
-        <v>152</v>
+      <c r="G31" s="23" t="s">
+        <v>133</v>
       </c>
       <c r="H31" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4082,68 +4141,68 @@
       <c r="I31" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J31" s="28" t="s">
+      <c r="J31" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K31" s="26">
+      <c r="K31" s="33">
         <f>$I31+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L31" s="24">
+      <c r="L31" s="17">
         <f>$I31+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M31" s="24">
+      <c r="M31" s="17">
         <f>$I31+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N31" s="24">
+      <c r="N31" s="17">
         <f>$I31+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O31" s="24">
+      <c r="O31" s="17">
         <f>$I31+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P31" s="24">
+      <c r="P31" s="17">
         <f>$I31+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q31" s="24">
+      <c r="Q31" s="17">
         <f>$I31+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R31" s="24">
+      <c r="R31" s="17">
         <f>$I31+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S31" s="24">
+      <c r="S31" s="17">
         <f>$I31+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T31" s="24">
+      <c r="T31" s="17">
         <f>$I31+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U31" s="24">
+      <c r="U31" s="17">
         <f>$I31+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V31" s="24">
+      <c r="V31" s="17">
         <f>$I31+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="50"/>
-      <c r="B32" s="13" t="s">
-        <v>146</v>
+      <c r="A32" s="51"/>
+      <c r="B32" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="C32" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>29</v>
@@ -4151,8 +4210,8 @@
       <c r="F32" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="23" t="s">
-        <v>147</v>
+      <c r="G32" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="H32" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4161,68 +4220,68 @@
       <c r="I32" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J32" s="30" t="s">
+      <c r="J32" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K32" s="33">
+      <c r="K32" s="26">
         <f>$I32+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L32" s="17">
+      <c r="L32" s="24">
         <f>$I32+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M32" s="17">
+      <c r="M32" s="24">
         <f>$I32+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N32" s="17">
+      <c r="N32" s="24">
         <f>$I32+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O32" s="17">
+      <c r="O32" s="24">
         <f>$I32+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P32" s="17">
+      <c r="P32" s="24">
         <f>$I32+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q32" s="17">
+      <c r="Q32" s="24">
         <f>$I32+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R32" s="17">
+      <c r="R32" s="24">
         <f>$I32+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S32" s="17">
+      <c r="S32" s="24">
         <f>$I32+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T32" s="17">
+      <c r="T32" s="24">
         <f>$I32+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U32" s="17">
+      <c r="U32" s="24">
         <f>$I32+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V32" s="17">
+      <c r="V32" s="24">
         <f>$I32+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="50"/>
+      <c r="A33" s="51"/>
       <c r="B33" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="7">
         <v>31</v>
       </c>
-      <c r="C33" s="7">
-        <v>32</v>
-      </c>
       <c r="D33" s="7">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E33" s="15" t="s">
         <v>29</v>
@@ -4230,8 +4289,8 @@
       <c r="F33" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G33" s="9" t="s">
-        <v>82</v>
+      <c r="G33" s="23" t="s">
+        <v>110</v>
       </c>
       <c r="H33" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4243,7 +4302,7 @@
       <c r="J33" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K33" s="26">
+      <c r="K33" s="12">
         <f>$I33+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
@@ -4293,24 +4352,24 @@
       </c>
     </row>
     <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="50"/>
+      <c r="A34" s="51"/>
       <c r="B34" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" s="7">
         <v>32</v>
       </c>
-      <c r="C34" s="7">
-        <v>33</v>
-      </c>
       <c r="D34" s="7">
-        <v>33</v>
-      </c>
-      <c r="E34" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="9" t="s">
-        <v>83</v>
+      <c r="G34" s="31" t="s">
+        <v>152</v>
       </c>
       <c r="H34" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4372,24 +4431,24 @@
       </c>
     </row>
     <row r="35" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="50"/>
-      <c r="B35" s="19" t="s">
-        <v>46</v>
+      <c r="A35" s="51"/>
+      <c r="B35" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="C35" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="7">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>29</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G35" s="22" t="s">
-        <v>84</v>
+        <v>22</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>147</v>
       </c>
       <c r="H35" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4398,68 +4457,68 @@
       <c r="I35" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J35" s="28" t="s">
+      <c r="J35" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K35" s="26">
+      <c r="K35" s="33">
         <f>$I35+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L35" s="24">
+      <c r="L35" s="17">
         <f>$I35+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M35" s="24">
+      <c r="M35" s="17">
         <f>$I35+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N35" s="24">
+      <c r="N35" s="17">
         <f>$I35+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O35" s="24">
+      <c r="O35" s="17">
         <f>$I35+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P35" s="24">
+      <c r="P35" s="17">
         <f>$I35+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q35" s="24">
+      <c r="Q35" s="17">
         <f>$I35+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R35" s="24">
+      <c r="R35" s="17">
         <f>$I35+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S35" s="24">
+      <c r="S35" s="17">
         <f>$I35+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T35" s="24">
+      <c r="T35" s="17">
         <f>$I35+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U35" s="24">
+      <c r="U35" s="17">
         <f>$I35+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V35" s="24">
+      <c r="V35" s="17">
         <f>$I35+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="50"/>
-      <c r="B36" s="37" t="s">
-        <v>153</v>
+      <c r="A36" s="51"/>
+      <c r="B36" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="C36" s="7">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="7">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E36" s="15" t="s">
         <v>29</v>
@@ -4467,77 +4526,78 @@
       <c r="F36" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="H36" s="31" t="s">
-        <v>73</v>
+      <c r="G36" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H36" s="31" t="str">
+        <f>Sheet2!$A$9</f>
+        <v>EDT</v>
       </c>
       <c r="I36" s="24">
-        <v>0</v>
-      </c>
-      <c r="J36" s="30" t="s">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="J36" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K36" s="26">
         <f>$I36+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
+        <v>1.375</v>
       </c>
       <c r="L36" s="24">
         <f>$I36+Sheet2!B$2/24</f>
-        <v>0.375</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="M36" s="24">
         <f>$I36+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="N36" s="24">
         <f>$I36+Sheet2!B$4/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="O36" s="24">
         <f>$I36+Sheet2!B$5/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="P36" s="24">
         <f>$I36+Sheet2!B$6/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="Q36" s="24">
         <f>$I36+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="R36" s="24">
         <f>$I36+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>1</v>
       </c>
       <c r="S36" s="24">
         <f>$I36+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="T36" s="24">
         <f>$I36+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="U36" s="24">
         <f>$I36+Sheet2!B$11/24</f>
-        <v>-0.25</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="V36" s="24">
         <f>$I36+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="37" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="50"/>
-      <c r="B37" s="37" t="s">
-        <v>61</v>
+      <c r="A37" s="51"/>
+      <c r="B37" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="C37" s="7">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="7">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>29</v>
@@ -4545,172 +4605,166 @@
       <c r="F37" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="H37" s="31" t="s">
-        <v>73</v>
+      <c r="G37" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H37" s="31" t="str">
+        <f>Sheet2!$A$9</f>
+        <v>EDT</v>
       </c>
       <c r="I37" s="24">
-        <v>0</v>
-      </c>
-      <c r="J37" s="30" t="s">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="J37" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K37" s="26">
         <f>$I37+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
+        <v>1.375</v>
       </c>
       <c r="L37" s="24">
         <f>$I37+Sheet2!B$2/24</f>
-        <v>0.375</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="M37" s="24">
         <f>$I37+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="N37" s="24">
         <f>$I37+Sheet2!B$4/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="O37" s="24">
         <f>$I37+Sheet2!B$5/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="P37" s="24">
         <f>$I37+Sheet2!B$6/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="Q37" s="24">
         <f>$I37+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="R37" s="24">
         <f>$I37+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>1</v>
       </c>
       <c r="S37" s="24">
         <f>$I37+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="T37" s="24">
         <f>$I37+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="U37" s="24">
         <f>$I37+Sheet2!B$11/24</f>
-        <v>-0.25</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="V37" s="24">
         <f>$I37+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="50"/>
-      <c r="B38" s="37" t="s">
-        <v>59</v>
+      <c r="A38" s="51"/>
+      <c r="B38" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="C38" s="7">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="7">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E38" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F38" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G38" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="H38" s="31" t="s">
-        <v>73</v>
+      <c r="F38" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H38" s="31" t="str">
+        <f>Sheet2!$A$9</f>
+        <v>EDT</v>
       </c>
       <c r="I38" s="24">
-        <v>0</v>
-      </c>
-      <c r="J38" s="30" t="s">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="J38" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K38" s="26">
         <f>$I38+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
+        <v>1.375</v>
       </c>
       <c r="L38" s="24">
         <f>$I38+Sheet2!B$2/24</f>
-        <v>0.375</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="M38" s="24">
         <f>$I38+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="N38" s="24">
         <f>$I38+Sheet2!B$4/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="O38" s="24">
         <f>$I38+Sheet2!B$5/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="P38" s="24">
         <f>$I38+Sheet2!B$6/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="Q38" s="24">
         <f>$I38+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="R38" s="24">
         <f>$I38+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>1</v>
       </c>
       <c r="S38" s="24">
         <f>$I38+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="T38" s="24">
         <f>$I38+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="U38" s="24">
         <f>$I38+Sheet2!B$11/24</f>
-        <v>-0.25</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="V38" s="24">
         <f>$I38+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="50"/>
+      <c r="A39" s="51"/>
       <c r="B39" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="7">
-        <v>38</v>
-      </c>
-      <c r="D39" s="7">
-        <v>38</v>
-      </c>
-      <c r="E39" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="F39" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="G39" s="31" t="s">
-        <v>136</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="G39" s="9"/>
       <c r="H39" s="31" t="s">
         <v>73</v>
       </c>
       <c r="I39" s="24">
         <v>0</v>
       </c>
-      <c r="J39" s="28" t="s">
+      <c r="J39" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K39" s="26">
@@ -4763,15 +4817,15 @@
       </c>
     </row>
     <row r="40" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="50"/>
-      <c r="B40" s="19" t="s">
-        <v>62</v>
+      <c r="A40" s="51"/>
+      <c r="B40" s="37" t="s">
+        <v>153</v>
       </c>
       <c r="C40" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D40" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E40" s="15" t="s">
         <v>29</v>
@@ -4780,7 +4834,7 @@
         <v>22</v>
       </c>
       <c r="G40" s="31" t="s">
-        <v>121</v>
+        <v>154</v>
       </c>
       <c r="H40" s="31" t="s">
         <v>73</v>
@@ -4841,24 +4895,24 @@
       </c>
     </row>
     <row r="41" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="50"/>
+      <c r="A41" s="51"/>
       <c r="B41" s="37" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C41" s="7">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D41" s="7">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E41" s="15" t="s">
         <v>29</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>124</v>
+        <v>75</v>
       </c>
       <c r="H41" s="31" t="s">
         <v>73</v>
@@ -4919,24 +4973,24 @@
       </c>
     </row>
     <row r="42" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="50"/>
+      <c r="A42" s="51"/>
       <c r="B42" s="37" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C42" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D42" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F42" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G42" s="29" t="s">
-        <v>122</v>
+      <c r="F42" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G42" s="31" t="s">
+        <v>134</v>
       </c>
       <c r="H42" s="31" t="s">
         <v>73</v>
@@ -4997,24 +5051,24 @@
       </c>
     </row>
     <row r="43" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="50"/>
+      <c r="A43" s="51"/>
       <c r="B43" s="19" t="s">
-        <v>60</v>
+        <v>137</v>
       </c>
       <c r="C43" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D43" s="7">
-        <v>42</v>
-      </c>
-      <c r="E43" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F43" s="7" t="s">
-        <v>74</v>
+      <c r="F43" s="42" t="s">
+        <v>22</v>
       </c>
       <c r="G43" s="31" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="H43" s="31" t="s">
         <v>73</v>
@@ -5022,7 +5076,7 @@
       <c r="I43" s="24">
         <v>0</v>
       </c>
-      <c r="J43" s="30" t="s">
+      <c r="J43" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K43" s="26">
@@ -5075,15 +5129,15 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="50"/>
+      <c r="A44" s="51"/>
       <c r="B44" s="19" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C44" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D44" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E44" s="15" t="s">
         <v>29</v>
@@ -5092,7 +5146,7 @@
         <v>22</v>
       </c>
       <c r="G44" s="31" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="H44" s="31" t="s">
         <v>73</v>
@@ -5100,7 +5154,7 @@
       <c r="I44" s="24">
         <v>0</v>
       </c>
-      <c r="J44" s="28" t="s">
+      <c r="J44" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K44" s="26">
@@ -5152,25 +5206,25 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="45" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="50"/>
-      <c r="B45" s="19" t="s">
-        <v>64</v>
+    <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="51"/>
+      <c r="B45" s="37" t="s">
+        <v>65</v>
       </c>
       <c r="C45" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D45" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E45" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F45" s="7" t="s">
-        <v>74</v>
+      <c r="F45" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="G45" s="31" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H45" s="31" t="s">
         <v>73</v>
@@ -5231,15 +5285,15 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="50"/>
-      <c r="B46" s="19" t="s">
-        <v>57</v>
+      <c r="A46" s="51"/>
+      <c r="B46" s="37" t="s">
+        <v>63</v>
       </c>
       <c r="C46" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D46" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E46" s="15" t="s">
         <v>29</v>
@@ -5248,7 +5302,7 @@
         <v>22</v>
       </c>
       <c r="G46" s="29" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="H46" s="31" t="s">
         <v>73</v>
@@ -5256,7 +5310,7 @@
       <c r="I46" s="24">
         <v>0</v>
       </c>
-      <c r="J46" s="28" t="s">
+      <c r="J46" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K46" s="26">
@@ -5309,485 +5363,797 @@
       </c>
     </row>
     <row r="47" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="50"/>
+      <c r="A47" s="51"/>
       <c r="B47" s="19" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C47" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D47" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>140</v>
+        <v>29</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="G47" s="36" t="s">
-        <v>125</v>
+        <v>74</v>
+      </c>
+      <c r="G47" s="31" t="s">
+        <v>142</v>
       </c>
       <c r="H47" s="31" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="I47" s="24">
-        <v>4.1666666666666664E-2</v>
+        <v>0</v>
       </c>
       <c r="J47" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K47" s="26">
         <f>$I47+Sheet2!B$1/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L47" s="24">
         <f>$I47+Sheet2!B$2/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="M47" s="24">
         <f>$I47+Sheet2!B$3/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N47" s="24">
         <f>$I47+Sheet2!B$4/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="O47" s="24">
         <f>$I47+Sheet2!B$5/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="P47" s="24">
         <f>$I47+Sheet2!B$6/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="Q47" s="24">
         <f>$I47+Sheet2!B$7/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R47" s="24">
         <f>$I47+Sheet2!B$8/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="S47" s="24">
         <f>$I47+Sheet2!B$9/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="T47" s="24">
         <f>$I47+Sheet2!B$10/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="U47" s="24">
         <f>$I47+Sheet2!B$11/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.25</v>
       </c>
       <c r="V47" s="24">
         <f>$I47+Sheet2!B$12/24</f>
-        <v>-0.25</v>
+        <v>-0.29166666666666669</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="50"/>
-      <c r="B48" s="37" t="s">
-        <v>67</v>
+      <c r="A48" s="51"/>
+      <c r="B48" s="19" t="s">
+        <v>58</v>
       </c>
       <c r="C48" s="7">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D48" s="7">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E48" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="F48" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G48" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="H48" s="37" t="s">
-        <v>13</v>
+      <c r="G48" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="H48" s="31" t="s">
+        <v>73</v>
       </c>
       <c r="I48" s="24">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J48" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="J48" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K48" s="26">
         <f>$I48+Sheet2!B$1/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L48" s="24">
         <f>$I48+Sheet2!B$2/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="M48" s="24">
         <f>$I48+Sheet2!B$3/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N48" s="24">
         <f>$I48+Sheet2!B$4/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="O48" s="24">
         <f>$I48+Sheet2!B$5/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="P48" s="24">
         <f>$I48+Sheet2!B$6/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="Q48" s="24">
         <f>$I48+Sheet2!B$7/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R48" s="24">
         <f>$I48+Sheet2!B$8/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="S48" s="24">
         <f>$I48+Sheet2!B$9/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="T48" s="24">
         <f>$I48+Sheet2!B$10/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="U48" s="24">
         <f>$I48+Sheet2!B$11/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.25</v>
       </c>
       <c r="V48" s="24">
         <f>$I48+Sheet2!B$12/24</f>
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="50"/>
+        <v>-0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="51"/>
       <c r="B49" s="19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C49" s="7">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D49" s="7">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E49" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F49" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G49" s="22" t="s">
-        <v>128</v>
+      <c r="F49" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G49" s="31" t="s">
+        <v>123</v>
       </c>
       <c r="H49" s="31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I49" s="24">
-        <v>8.3333333333333329E-2</v>
+        <v>0</v>
       </c>
       <c r="J49" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K49" s="26">
         <f>$I49+Sheet2!B$1/24</f>
-        <v>0.5</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L49" s="24">
         <f>$I49+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="M49" s="24">
         <f>$I49+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N49" s="24">
         <f>$I49+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.125</v>
       </c>
       <c r="O49" s="24">
         <f>$I49+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.125</v>
       </c>
       <c r="P49" s="24">
         <f>$I49+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.125</v>
       </c>
       <c r="Q49" s="24">
         <f>$I49+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R49" s="24">
         <f>$I49+Sheet2!B$8/24</f>
-        <v>0.125</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="S49" s="24">
         <f>$I49+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="T49" s="24">
         <f>$I49+Sheet2!B$10/24</f>
-        <v>-0.125</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="U49" s="24">
         <f>$I49+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.25</v>
       </c>
       <c r="V49" s="24">
         <f>$I49+Sheet2!B$12/24</f>
-        <v>-0.20833333333333337</v>
+        <v>-0.29166666666666669</v>
       </c>
     </row>
     <row r="50" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="50"/>
-      <c r="B50" s="37" t="s">
-        <v>69</v>
+      <c r="A50" s="51"/>
+      <c r="B50" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="C50" s="7">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D50" s="7">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E50" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F50" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>127</v>
+      <c r="F50" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" s="29" t="s">
+        <v>117</v>
       </c>
       <c r="H50" s="31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I50" s="24">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="J50" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="J50" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K50" s="26">
         <f>$I50+Sheet2!B$1/24</f>
-        <v>0.5</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L50" s="24">
         <f>$I50+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="M50" s="24">
         <f>$I50+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N50" s="24">
         <f>$I50+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.125</v>
       </c>
       <c r="O50" s="24">
         <f>$I50+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.125</v>
       </c>
       <c r="P50" s="24">
         <f>$I50+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.125</v>
       </c>
       <c r="Q50" s="24">
         <f>$I50+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R50" s="24">
         <f>$I50+Sheet2!B$8/24</f>
-        <v>0.125</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="S50" s="24">
         <f>$I50+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="T50" s="24">
         <f>$I50+Sheet2!B$10/24</f>
-        <v>-0.125</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="U50" s="24">
         <f>$I50+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.25</v>
       </c>
       <c r="V50" s="24">
         <f>$I50+Sheet2!B$12/24</f>
-        <v>-0.20833333333333337</v>
+        <v>-0.29166666666666669</v>
       </c>
     </row>
     <row r="51" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="50"/>
+      <c r="A51" s="51"/>
       <c r="B51" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C51" s="7">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D51" s="7">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G51" s="39" t="s">
-        <v>126</v>
+        <v>140</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G51" s="36" t="s">
+        <v>125</v>
       </c>
       <c r="H51" s="31" t="s">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="I51" s="24">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J51" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K51" s="26">
         <f>$I51+Sheet2!B$1/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="L51" s="24">
         <f>$I51+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M51" s="24">
         <f>$I51+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="N51" s="24">
         <f>$I51+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="O51" s="24">
         <f>$I51+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P51" s="24">
         <f>$I51+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q51" s="24">
         <f>$I51+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="R51" s="24">
         <f>$I51+Sheet2!B$8/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S51" s="24">
         <f>$I51+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="T51" s="24">
         <f>$I51+Sheet2!B$10/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="U51" s="24">
         <f>$I51+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="V51" s="24">
         <f>$I51+Sheet2!B$12/24</f>
-        <v>-0.20833333333333337</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="52" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="50"/>
+      <c r="A52" s="51"/>
       <c r="B52" s="37" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C52" s="7">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D52" s="7">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E52" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F52" s="40" t="s">
+      <c r="F52" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G52" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="H52" s="31" t="s">
-        <v>72</v>
+      <c r="G52" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="H52" s="37" t="s">
+        <v>13</v>
       </c>
       <c r="I52" s="24">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J52" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K52" s="26">
         <f>$I52+Sheet2!B$1/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="L52" s="24">
         <f>$I52+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M52" s="24">
         <f>$I52+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="N52" s="24">
         <f>$I52+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="O52" s="24">
         <f>$I52+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P52" s="24">
         <f>$I52+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q52" s="24">
         <f>$I52+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="R52" s="24">
         <f>$I52+Sheet2!B$8/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S52" s="24">
         <f>$I52+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="T52" s="24">
         <f>$I52+Sheet2!B$10/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="U52" s="24">
         <f>$I52+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="V52" s="24">
         <f>$I52+Sheet2!B$12/24</f>
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="51"/>
+      <c r="B53" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="7">
+        <v>50</v>
+      </c>
+      <c r="D53" s="7">
+        <v>50</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="H53" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="I53" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J53" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K53" s="26">
+        <f>$I53+Sheet2!B$1/24</f>
+        <v>0.5</v>
+      </c>
+      <c r="L53" s="24">
+        <f>$I53+Sheet2!B$2/24</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M53" s="24">
+        <f>$I53+Sheet2!B$3/24</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="N53" s="24">
+        <f>$I53+Sheet2!B$4/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="O53" s="24">
+        <f>$I53+Sheet2!B$5/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P53" s="24">
+        <f>$I53+Sheet2!B$6/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="Q53" s="24">
+        <f>$I53+Sheet2!B$7/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R53" s="24">
+        <f>$I53+Sheet2!B$8/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="S53" s="24">
+        <f>$I53+Sheet2!B$9/24</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="T53" s="24">
+        <f>$I53+Sheet2!B$10/24</f>
+        <v>-0.125</v>
+      </c>
+      <c r="U53" s="24">
+        <f>$I53+Sheet2!B$11/24</f>
+        <v>-0.16666666666666669</v>
+      </c>
+      <c r="V53" s="24">
+        <f>$I53+Sheet2!B$12/24</f>
         <v>-0.20833333333333337</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A53" s="50"/>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A54" s="50"/>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A55" s="50"/>
+    <row r="54" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="51"/>
+      <c r="B54" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="7">
+        <v>51</v>
+      </c>
+      <c r="D54" s="7">
+        <v>51</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H54" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="I54" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J54" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K54" s="26">
+        <f>$I54+Sheet2!B$1/24</f>
+        <v>0.5</v>
+      </c>
+      <c r="L54" s="24">
+        <f>$I54+Sheet2!B$2/24</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M54" s="24">
+        <f>$I54+Sheet2!B$3/24</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="N54" s="24">
+        <f>$I54+Sheet2!B$4/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="O54" s="24">
+        <f>$I54+Sheet2!B$5/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P54" s="24">
+        <f>$I54+Sheet2!B$6/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="Q54" s="24">
+        <f>$I54+Sheet2!B$7/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R54" s="24">
+        <f>$I54+Sheet2!B$8/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="S54" s="24">
+        <f>$I54+Sheet2!B$9/24</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="T54" s="24">
+        <f>$I54+Sheet2!B$10/24</f>
+        <v>-0.125</v>
+      </c>
+      <c r="U54" s="24">
+        <f>$I54+Sheet2!B$11/24</f>
+        <v>-0.16666666666666669</v>
+      </c>
+      <c r="V54" s="24">
+        <f>$I54+Sheet2!B$12/24</f>
+        <v>-0.20833333333333337</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="51"/>
+      <c r="B55" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C55" s="7">
+        <v>52</v>
+      </c>
+      <c r="D55" s="7">
+        <v>52</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="H55" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="I55" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J55" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K55" s="26">
+        <f>$I55+Sheet2!B$1/24</f>
+        <v>0.5</v>
+      </c>
+      <c r="L55" s="24">
+        <f>$I55+Sheet2!B$2/24</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M55" s="24">
+        <f>$I55+Sheet2!B$3/24</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="N55" s="24">
+        <f>$I55+Sheet2!B$4/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="O55" s="24">
+        <f>$I55+Sheet2!B$5/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P55" s="24">
+        <f>$I55+Sheet2!B$6/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="Q55" s="24">
+        <f>$I55+Sheet2!B$7/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R55" s="24">
+        <f>$I55+Sheet2!B$8/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="S55" s="24">
+        <f>$I55+Sheet2!B$9/24</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="T55" s="24">
+        <f>$I55+Sheet2!B$10/24</f>
+        <v>-0.125</v>
+      </c>
+      <c r="U55" s="24">
+        <f>$I55+Sheet2!B$11/24</f>
+        <v>-0.16666666666666669</v>
+      </c>
+      <c r="V55" s="24">
+        <f>$I55+Sheet2!B$12/24</f>
+        <v>-0.20833333333333337</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="51"/>
+      <c r="B56" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="7">
+        <v>53</v>
+      </c>
+      <c r="D56" s="7">
+        <v>53</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F56" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="H56" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="I56" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J56" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K56" s="26">
+        <f>$I56+Sheet2!B$1/24</f>
+        <v>0.5</v>
+      </c>
+      <c r="L56" s="24">
+        <f>$I56+Sheet2!B$2/24</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M56" s="24">
+        <f>$I56+Sheet2!B$3/24</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="N56" s="24">
+        <f>$I56+Sheet2!B$4/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="O56" s="24">
+        <f>$I56+Sheet2!B$5/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P56" s="24">
+        <f>$I56+Sheet2!B$6/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="Q56" s="24">
+        <f>$I56+Sheet2!B$7/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R56" s="24">
+        <f>$I56+Sheet2!B$8/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="S56" s="24">
+        <f>$I56+Sheet2!B$9/24</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="T56" s="24">
+        <f>$I56+Sheet2!B$10/24</f>
+        <v>-0.125</v>
+      </c>
+      <c r="U56" s="24">
+        <f>$I56+Sheet2!B$11/24</f>
+        <v>-0.16666666666666669</v>
+      </c>
+      <c r="V56" s="24">
+        <f>$I56+Sheet2!B$12/24</f>
+        <v>-0.20833333333333337</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A57" s="51"/>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A58" s="51"/>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A59" s="51"/>
     </row>
   </sheetData>
-  <sortState ref="B2:V44">
-    <sortCondition ref="D2:D44"/>
+  <sortState ref="B2:V48">
+    <sortCondition ref="D2:D48"/>
   </sortState>
   <customSheetViews>
     <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
@@ -5799,275 +6165,305 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
-    <mergeCell ref="A6:A21"/>
-    <mergeCell ref="A22:A55"/>
+    <mergeCell ref="A7:A23"/>
+    <mergeCell ref="A24:A59"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L4 K37:V52 K4:V35">
-    <cfRule type="expression" dxfId="53" priority="111">
+  <conditionalFormatting sqref="K2:L5 K4:V15 K17:V38 K40:V56">
+    <cfRule type="expression" dxfId="59" priority="117">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:V4">
-    <cfRule type="expression" dxfId="52" priority="113">
+  <conditionalFormatting sqref="K2:V5">
+    <cfRule type="expression" dxfId="58" priority="119">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:V3 K24:V24 G31:V31 G24 B33:B35 K37:V37 G37 G39:V39 B38:B39 K40:V42 G40:G42 B43:B44 B46 K45:V45 G45 G52 G47:G50 K47:V52 E46:V46 E43:V44 E38:V38 E33:V35 E25:V30 B4:B31 E4:V23 C4:D52">
-    <cfRule type="expression" dxfId="51" priority="117">
+  <conditionalFormatting sqref="K27:V27 G34:V34 G27 B36:B39 K41:V41 G41 G43:V43 B42:B43 K44:V46 G44:G46 B47:B48 B50 K49:V49 G49 G56 G51:G54 K51:V56 E50:V50 E47:V48 E42:V42 E36:V38 E28:V33 B2:V4 B5:B34 C5:D56 E5:V26 E39:G39">
+    <cfRule type="expression" dxfId="57" priority="123">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37 J37:V37">
-    <cfRule type="expression" dxfId="50" priority="94">
+  <conditionalFormatting sqref="B41 J41:V41">
+    <cfRule type="expression" dxfId="56" priority="100">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44 J44:V44">
+    <cfRule type="expression" dxfId="55" priority="98">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46 J46:V46">
+    <cfRule type="expression" dxfId="54" priority="96">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49 J49:V49">
+    <cfRule type="expression" dxfId="53" priority="94">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45 J45:V45">
+    <cfRule type="expression" dxfId="52" priority="92">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B51 J51:V51">
+    <cfRule type="expression" dxfId="51" priority="90">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52 J52:V52 E52:F52 H52">
+    <cfRule type="expression" dxfId="50" priority="88">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="expression" dxfId="49" priority="86">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49">
+    <cfRule type="expression" dxfId="48" priority="83">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="expression" dxfId="47" priority="82">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51 H51">
+    <cfRule type="expression" dxfId="46" priority="81">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B55 J55:V55">
+    <cfRule type="expression" dxfId="45" priority="79">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54 J54:V54 E54">
+    <cfRule type="expression" dxfId="44" priority="77">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55:F55 H55">
+    <cfRule type="expression" dxfId="43" priority="75">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53 J53:V53">
+    <cfRule type="expression" dxfId="42" priority="73">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B56 J56:V56 E56">
+    <cfRule type="expression" dxfId="41" priority="71">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45">
+    <cfRule type="expression" dxfId="40" priority="63">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
+    <cfRule type="expression" dxfId="39" priority="53">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="expression" dxfId="38" priority="52">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I46">
+    <cfRule type="expression" dxfId="37" priority="51">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I49">
+    <cfRule type="expression" dxfId="36" priority="50">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I45">
+    <cfRule type="expression" dxfId="35" priority="49">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I51">
+    <cfRule type="expression" dxfId="34" priority="48">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I52">
+    <cfRule type="expression" dxfId="33" priority="47">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I55">
+    <cfRule type="expression" dxfId="32" priority="46">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H41">
+    <cfRule type="expression" dxfId="31" priority="39">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H44">
+    <cfRule type="expression" dxfId="30" priority="38">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H46">
+    <cfRule type="expression" dxfId="29" priority="37">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H49">
+    <cfRule type="expression" dxfId="28" priority="36">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45">
+    <cfRule type="expression" dxfId="27" priority="35">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H54">
+    <cfRule type="expression" dxfId="26" priority="34">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I54">
+    <cfRule type="expression" dxfId="25" priority="33">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53">
+    <cfRule type="expression" dxfId="24" priority="32">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I53">
+    <cfRule type="expression" dxfId="23" priority="31">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H56">
+    <cfRule type="expression" dxfId="22" priority="30">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I56">
+    <cfRule type="expression" dxfId="21" priority="29">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F49">
+    <cfRule type="expression" dxfId="20" priority="25">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F51">
+    <cfRule type="expression" dxfId="19" priority="24">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F54">
+    <cfRule type="expression" dxfId="18" priority="23">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41">
+    <cfRule type="expression" dxfId="17" priority="19">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46:F46">
+    <cfRule type="expression" dxfId="16" priority="18">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44:F44">
+    <cfRule type="expression" dxfId="15" priority="17">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53:F53">
+    <cfRule type="expression" dxfId="14" priority="16">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35 E35:V35">
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K40:V40 G40">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40 J40:V40">
-    <cfRule type="expression" dxfId="49" priority="92">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42 J42:V42">
-    <cfRule type="expression" dxfId="48" priority="90">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45 J45:V45">
-    <cfRule type="expression" dxfId="47" priority="88">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B41 J41:V41">
-    <cfRule type="expression" dxfId="46" priority="86">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47 J47:V47">
-    <cfRule type="expression" dxfId="45" priority="84">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B48 J48:V48 E48:F48 H48">
-    <cfRule type="expression" dxfId="44" priority="82">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="expression" dxfId="43" priority="80">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="expression" dxfId="42" priority="77">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="expression" dxfId="41" priority="76">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47 H47">
-    <cfRule type="expression" dxfId="40" priority="75">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B51 J51:V51">
-    <cfRule type="expression" dxfId="39" priority="73">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B50 J50:V50 E50">
-    <cfRule type="expression" dxfId="38" priority="71">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51:F51 H51">
-    <cfRule type="expression" dxfId="37" priority="69">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49 J49:V49">
-    <cfRule type="expression" dxfId="36" priority="67">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52 J52:V52 E52">
-    <cfRule type="expression" dxfId="35" priority="65">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F41">
-    <cfRule type="expression" dxfId="34" priority="57">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="expression" dxfId="33" priority="47">
+  <conditionalFormatting sqref="E40">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="32" priority="46">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="31" priority="45">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
-    <cfRule type="expression" dxfId="30" priority="44">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
-    <cfRule type="expression" dxfId="29" priority="43">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="28" priority="42">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="27" priority="41">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I51">
-    <cfRule type="expression" dxfId="26" priority="40">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="25" priority="33">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="expression" dxfId="24" priority="32">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H42">
-    <cfRule type="expression" dxfId="23" priority="31">
+  <conditionalFormatting sqref="F40">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H45">
-    <cfRule type="expression" dxfId="22" priority="30">
-      <formula>MOD(ROW(),2)=1</formula>
+  <conditionalFormatting sqref="K16:V16">
+    <cfRule type="expression" dxfId="6" priority="127">
+      <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H41">
-    <cfRule type="expression" dxfId="21" priority="29">
-      <formula>MOD(ROW(),2)=1</formula>
+  <conditionalFormatting sqref="K16:V16">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>K$1=$H16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="20" priority="28">
-      <formula>MOD(ROW(),2)=1</formula>
+  <conditionalFormatting sqref="K39:V39">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>K$1=$H39</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I50">
-    <cfRule type="expression" dxfId="19" priority="27">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H49">
-    <cfRule type="expression" dxfId="18" priority="26">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I49">
-    <cfRule type="expression" dxfId="17" priority="25">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H52">
-    <cfRule type="expression" dxfId="16" priority="24">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I52">
-    <cfRule type="expression" dxfId="15" priority="23">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45">
-    <cfRule type="expression" dxfId="14" priority="19">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
-    <cfRule type="expression" dxfId="13" priority="18">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F50">
-    <cfRule type="expression" dxfId="12" priority="17">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F37">
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42:F42">
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40:F40">
-    <cfRule type="expression" dxfId="9" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49:F49">
-    <cfRule type="expression" dxfId="8" priority="10">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32 E32:V32">
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K36:V36">
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>K$1=$H36</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K36:V36 G36">
-    <cfRule type="expression" dxfId="5" priority="7">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36 J36:V36">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
+  <conditionalFormatting sqref="K39:V39">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
+  <conditionalFormatting sqref="J39:V39">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
+  <conditionalFormatting sqref="I39">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F36">
+  <conditionalFormatting sqref="H39">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added seth997 swgoh URL
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE28AD51-4BBF-4E48-9A98-A0A738A1281C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7B3A1C-37D9-DB49-8363-5FD09EF12862}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14140" yWindow="9040" windowWidth="33700" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <customWorkbookViews>
+    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="187">
   <si>
     <t>Name</t>
   </si>
@@ -592,6 +592,9 @@
   </si>
   <si>
     <t>:clock10:</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/411913448/</t>
   </si>
 </sst>
 </file>
@@ -1039,6 +1042,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1051,7 +1055,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1929,8 +1932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2633,7 +2636,7 @@
       </c>
     </row>
     <row r="10" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="50" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -2714,7 +2717,7 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="49"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="19" t="s">
         <v>173</v>
       </c>
@@ -2726,7 +2729,7 @@
       <c r="F11" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="G11" s="53" t="s">
+      <c r="G11" s="49" t="s">
         <v>176</v>
       </c>
       <c r="H11" s="29" t="str">
@@ -2789,7 +2792,7 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="49"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="19" t="s">
         <v>41</v>
       </c>
@@ -2868,7 +2871,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="49"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="19" t="s">
         <v>43</v>
       </c>
@@ -2947,7 +2950,7 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="49"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="19" t="s">
         <v>51</v>
       </c>
@@ -3026,7 +3029,7 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="19" t="s">
         <v>50</v>
       </c>
@@ -3105,7 +3108,7 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="49"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="19" t="s">
         <v>40</v>
       </c>
@@ -3184,7 +3187,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="49"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="13" t="s">
         <v>44</v>
       </c>
@@ -3263,7 +3266,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="49"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="19" t="s">
         <v>49</v>
       </c>
@@ -3342,7 +3345,7 @@
       </c>
     </row>
     <row r="19" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="49"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="19" t="s">
         <v>48</v>
       </c>
@@ -3421,7 +3424,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="49"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="19" t="s">
         <v>157</v>
       </c>
@@ -3500,7 +3503,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="19" t="s">
         <v>172</v>
       </c>
@@ -3516,7 +3519,9 @@
       <c r="F21" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="9"/>
+      <c r="G21" s="9" t="s">
+        <v>186</v>
+      </c>
       <c r="H21" s="31" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
@@ -3577,7 +3582,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="49"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="19" t="s">
         <v>169</v>
       </c>
@@ -3656,7 +3661,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="49"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="19" t="s">
         <v>45</v>
       </c>
@@ -3735,7 +3740,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="49"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="19" t="s">
         <v>164</v>
       </c>
@@ -3809,7 +3814,7 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="49"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="19" t="s">
         <v>55</v>
       </c>
@@ -3887,7 +3892,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="49"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="13" t="s">
         <v>53</v>
       </c>
@@ -3965,7 +3970,7 @@
       </c>
     </row>
     <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="49"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="34" t="s">
         <v>111</v>
       </c>
@@ -4043,7 +4048,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="49"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="19" t="s">
         <v>54</v>
       </c>
@@ -4121,7 +4126,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="50"/>
+      <c r="A29" s="51"/>
       <c r="B29" s="19" t="s">
         <v>93</v>
       </c>
@@ -4199,7 +4204,7 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="52" t="s">
         <v>21</v>
       </c>
       <c r="B30" s="19" t="s">
@@ -4279,7 +4284,7 @@
       </c>
     </row>
     <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="52"/>
+      <c r="A31" s="53"/>
       <c r="B31" s="19" t="s">
         <v>159</v>
       </c>
@@ -4354,7 +4359,7 @@
       </c>
     </row>
     <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="52"/>
+      <c r="A32" s="53"/>
       <c r="B32" s="19" t="s">
         <v>115</v>
       </c>
@@ -4433,7 +4438,7 @@
       </c>
     </row>
     <row r="33" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="52"/>
+      <c r="A33" s="53"/>
       <c r="B33" s="19" t="s">
         <v>143</v>
       </c>
@@ -4511,7 +4516,7 @@
       </c>
     </row>
     <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="52"/>
+      <c r="A34" s="53"/>
       <c r="B34" s="13" t="s">
         <v>37</v>
       </c>
@@ -4590,7 +4595,7 @@
       </c>
     </row>
     <row r="35" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="52"/>
+      <c r="A35" s="53"/>
       <c r="B35" s="13" t="s">
         <v>35</v>
       </c>
@@ -4669,7 +4674,7 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="52"/>
+      <c r="A36" s="53"/>
       <c r="B36" s="19" t="s">
         <v>33</v>
       </c>
@@ -4748,7 +4753,7 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="52"/>
+      <c r="A37" s="53"/>
       <c r="B37" s="13" t="s">
         <v>38</v>
       </c>
@@ -4827,7 +4832,7 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="52"/>
+      <c r="A38" s="53"/>
       <c r="B38" s="19" t="s">
         <v>34</v>
       </c>
@@ -4906,7 +4911,7 @@
       </c>
     </row>
     <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="52"/>
+      <c r="A39" s="53"/>
       <c r="B39" s="19" t="s">
         <v>36</v>
       </c>
@@ -4985,7 +4990,7 @@
       </c>
     </row>
     <row r="40" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="52"/>
+      <c r="A40" s="53"/>
       <c r="B40" s="19" t="s">
         <v>151</v>
       </c>
@@ -5064,7 +5069,7 @@
       </c>
     </row>
     <row r="41" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="52"/>
+      <c r="A41" s="53"/>
       <c r="B41" s="13" t="s">
         <v>146</v>
       </c>
@@ -5143,7 +5148,7 @@
       </c>
     </row>
     <row r="42" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="52"/>
+      <c r="A42" s="53"/>
       <c r="B42" s="19" t="s">
         <v>31</v>
       </c>
@@ -5222,7 +5227,7 @@
       </c>
     </row>
     <row r="43" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="52"/>
+      <c r="A43" s="53"/>
       <c r="B43" s="19" t="s">
         <v>32</v>
       </c>
@@ -5301,7 +5306,7 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="52"/>
+      <c r="A44" s="53"/>
       <c r="B44" s="19" t="s">
         <v>46</v>
       </c>
@@ -5380,7 +5385,7 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="52"/>
+      <c r="A45" s="53"/>
       <c r="B45" s="19" t="s">
         <v>166</v>
       </c>
@@ -5454,7 +5459,7 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="52"/>
+      <c r="A46" s="53"/>
       <c r="B46" s="37" t="s">
         <v>153</v>
       </c>
@@ -5532,7 +5537,7 @@
       </c>
     </row>
     <row r="47" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="52"/>
+      <c r="A47" s="53"/>
       <c r="B47" s="37" t="s">
         <v>61</v>
       </c>
@@ -5610,7 +5615,7 @@
       </c>
     </row>
     <row r="48" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="52"/>
+      <c r="A48" s="53"/>
       <c r="B48" s="37" t="s">
         <v>59</v>
       </c>
@@ -5688,7 +5693,7 @@
       </c>
     </row>
     <row r="49" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="52"/>
+      <c r="A49" s="53"/>
       <c r="B49" s="19" t="s">
         <v>137</v>
       </c>
@@ -5766,7 +5771,7 @@
       </c>
     </row>
     <row r="50" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="52"/>
+      <c r="A50" s="53"/>
       <c r="B50" s="19" t="s">
         <v>62</v>
       </c>
@@ -5844,7 +5849,7 @@
       </c>
     </row>
     <row r="51" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="52"/>
+      <c r="A51" s="53"/>
       <c r="B51" s="37" t="s">
         <v>65</v>
       </c>
@@ -5922,7 +5927,7 @@
       </c>
     </row>
     <row r="52" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="52"/>
+      <c r="A52" s="53"/>
       <c r="B52" s="37" t="s">
         <v>63</v>
       </c>
@@ -6000,7 +6005,7 @@
       </c>
     </row>
     <row r="53" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="52"/>
+      <c r="A53" s="53"/>
       <c r="B53" s="19" t="s">
         <v>60</v>
       </c>
@@ -6078,7 +6083,7 @@
       </c>
     </row>
     <row r="54" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="52"/>
+      <c r="A54" s="53"/>
       <c r="B54" s="19" t="s">
         <v>58</v>
       </c>
@@ -6156,7 +6161,7 @@
       </c>
     </row>
     <row r="55" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="52"/>
+      <c r="A55" s="53"/>
       <c r="B55" s="19" t="s">
         <v>64</v>
       </c>
@@ -6234,7 +6239,7 @@
       </c>
     </row>
     <row r="56" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="52"/>
+      <c r="A56" s="53"/>
       <c r="B56" s="19" t="s">
         <v>57</v>
       </c>
@@ -6312,7 +6317,7 @@
       </c>
     </row>
     <row r="57" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="52"/>
+      <c r="A57" s="53"/>
       <c r="B57" s="19" t="s">
         <v>183</v>
       </c>
@@ -6386,7 +6391,7 @@
       </c>
     </row>
     <row r="58" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="52"/>
+      <c r="A58" s="53"/>
       <c r="B58" s="19" t="s">
         <v>66</v>
       </c>
@@ -6464,7 +6469,7 @@
       </c>
     </row>
     <row r="59" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="52"/>
+      <c r="A59" s="53"/>
       <c r="B59" s="37" t="s">
         <v>67</v>
       </c>
@@ -6542,7 +6547,7 @@
       </c>
     </row>
     <row r="60" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="52"/>
+      <c r="A60" s="53"/>
       <c r="B60" s="19" t="s">
         <v>184</v>
       </c>
@@ -6616,7 +6621,7 @@
       </c>
     </row>
     <row r="61" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="52"/>
+      <c r="A61" s="53"/>
       <c r="B61" s="19" t="s">
         <v>70</v>
       </c>
@@ -6694,7 +6699,7 @@
       </c>
     </row>
     <row r="62" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="52"/>
+      <c r="A62" s="53"/>
       <c r="B62" s="37" t="s">
         <v>69</v>
       </c>
@@ -6772,7 +6777,7 @@
       </c>
     </row>
     <row r="63" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="52"/>
+      <c r="A63" s="53"/>
       <c r="B63" s="19" t="s">
         <v>68</v>
       </c>
@@ -6850,7 +6855,7 @@
       </c>
     </row>
     <row r="64" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="52"/>
+      <c r="A64" s="53"/>
       <c r="B64" s="37" t="s">
         <v>71</v>
       </c>
@@ -6928,24 +6933,24 @@
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="52"/>
+      <c r="A65" s="53"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="52"/>
+      <c r="A66" s="53"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="52"/>
+      <c r="A67" s="53"/>
     </row>
   </sheetData>
   <sortState ref="B2:V54">
     <sortCondition ref="D2:D54"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
+      <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
-      <selection sqref="A1:XFD1048576"/>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Add ski and mang
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CDB155-76DC-4E46-83F6-6D77BD3D22A1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CFE03A-3069-FB41-9C50-A735AA9E4BD8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14140" yWindow="9040" windowWidth="33700" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <customWorkbookViews>
+    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="193">
   <si>
     <t>Name</t>
   </si>
@@ -261,54 +261,6 @@
     <t>:smiley:</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/bonesaw/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/disgrace/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/dogman/</t>
-  </si>
-  <si>
-    <t>&lt;https://swgoh.gg/u/mistborn/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;https://swgoh.gg/u/cmansfield30/&gt;</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/sideous/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/thanatos85/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/t-m/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/tuggspeedman/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/whippo/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/doc1974/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/lokonew/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/boro/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/mrblonde/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/sersa/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/kuesko/</t>
-  </si>
-  <si>
     <t>Italy</t>
   </si>
   <si>
@@ -324,30 +276,6 @@
     <t>:flag_bz:</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/tchacabr/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/berne123/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/wild/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/phamous/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/sylar4/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/wookiefecker/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/mariopeartree/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/axlr/</t>
-  </si>
-  <si>
     <t>Spain</t>
   </si>
   <si>
@@ -366,66 +294,21 @@
     <t>:flag_pl:</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/mortisbs/</t>
-  </si>
-  <si>
     <t>Tantema VVV</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/ferlondon76/</t>
-  </si>
-  <si>
     <t>:flag_sk:</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/darthhemrhoid/</t>
-  </si>
-  <si>
     <t>DarthHemRhoid</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/jedichew/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/yodanhodaka/</t>
-  </si>
-  <si>
     <t>Movan Lipost</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/rikk91/</t>
-  </si>
-  <si>
     <t>:flag_at:</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/darkness39/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/landogerton/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/spook1322/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/fajhajaba/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/zombiegnome/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/jvu420/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/droopy/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/chiefnorbitthegreat/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/raucous1/</t>
-  </si>
-  <si>
     <t>Eddie (IGN Aaron)</t>
   </si>
   <si>
@@ -435,51 +318,27 @@
     <t>:flag_gb:</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/varlie/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/broly/</t>
-  </si>
-  <si>
     <t>Taiwan</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/darkdentist/</t>
-  </si>
-  <si>
     <t>Dark Dentist</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/loohoo/</t>
-  </si>
-  <si>
-    <t>https://swgoh.gg/u/trueno0917/</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
     <t>:flag_ca:</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/miguelangel1506/</t>
-  </si>
-  <si>
     <t>DarthSlappyJedi</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/darthslappyjedi/</t>
-  </si>
-  <si>
     <t>EDT</t>
   </si>
   <si>
     <t>Punisher09brm</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/punisher09brm/</t>
-  </si>
-  <si>
     <t>:flag_ru:</t>
   </si>
   <si>
@@ -492,15 +351,9 @@
     <t>PSUlion</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/psulion/</t>
-  </si>
-  <si>
     <t>BigHoov (HS)</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/bighoov/</t>
-  </si>
-  <si>
     <t>:flag_hk:</t>
   </si>
   <si>
@@ -510,9 +363,6 @@
     <t>spell</t>
   </si>
   <si>
-    <t>https://swgoh.gg/u/spell/</t>
-  </si>
-  <si>
     <t>TZ EST</t>
   </si>
   <si>
@@ -601,6 +451,168 @@
   </si>
   <si>
     <t>https://swgoh.gg/p/865686499/</t>
+  </si>
+  <si>
+    <t>ski</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/123599797/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/979333176/</t>
+  </si>
+  <si>
+    <t>mang</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/267375252/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/121297475/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/119951554/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/829286233/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/535791581/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/274888747/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/117242282/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/353582613/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/768432229/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/382359167/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/513244519/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/454756465/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/514139651/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/261159659/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/584959796/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/652562743/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/531586268/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/854688879/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/162883938/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/741784458/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/968876577/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/976267739/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/915462152/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/117214579/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/493542499/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/121914893/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/753175275/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/128229281/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/838653979/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/865644997/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/191155833/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/259284386/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/662216351/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/215672729/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/545256144/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/972272138/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/157812467/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/285698128/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/596968217/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/284612418/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/997429163/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/179595464/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/132182242/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/416881399/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/262521353/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/382162328/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/545415194/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/346575984/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/597177222/</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/959656473/</t>
   </si>
 </sst>
 </file>
@@ -974,7 +986,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1061,19 +1073,19 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="79">
     <dxf>
       <fill>
         <patternFill>
@@ -1950,10 +1962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V68"/>
+  <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D65"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2029,23 +2041,23 @@
         <v>CEST</v>
       </c>
       <c r="R1" s="3" t="str">
-        <f>H28</f>
+        <f>H29</f>
         <v>BST</v>
       </c>
       <c r="S1" s="3" t="str">
-        <f>H43</f>
+        <f>H45</f>
         <v>EDT</v>
       </c>
       <c r="T1" s="3" t="str">
-        <f>H57</f>
+        <f>H59</f>
         <v>CDT</v>
       </c>
       <c r="U1" s="3" t="str">
-        <f>H49</f>
+        <f>H51</f>
         <v>CDT</v>
       </c>
       <c r="V1" s="3" t="str">
-        <f>H54</f>
+        <f>H56</f>
         <v>CDT</v>
       </c>
     </row>
@@ -2054,7 +2066,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -2064,10 +2076,10 @@
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="7" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>27</v>
@@ -2139,13 +2151,13 @@
         <v>2</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>27</v>
@@ -2208,7 +2220,7 @@
     <row r="4" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="48"/>
       <c r="B4" s="38" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="C4" s="7">
         <v>3</v>
@@ -2218,7 +2230,7 @@
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="7" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="6" t="s">
@@ -2282,7 +2294,7 @@
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18"/>
       <c r="B5" s="38" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="C5" s="7">
         <v>4</v>
@@ -2291,10 +2303,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="6" t="s">
@@ -2358,7 +2370,7 @@
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
       <c r="B6" s="38" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="C6" s="7">
         <v>5</v>
@@ -2368,11 +2380,11 @@
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="7" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="29" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="I6" s="24">
         <v>11.458333333333334</v>
@@ -2432,7 +2444,7 @@
     <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="45"/>
       <c r="B7" s="19" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C7" s="7">
         <v>6</v>
@@ -2441,16 +2453,16 @@
         <v>6</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="I7" s="24">
         <v>11.458333333333334</v>
@@ -2510,7 +2522,7 @@
     <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="47"/>
       <c r="B8" s="19" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C8" s="7">
         <v>7</v>
@@ -2520,10 +2532,10 @@
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="7" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="H8" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2602,7 +2614,7 @@
         <v>47</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="H9" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -2677,13 +2689,13 @@
         <v>9</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="H10" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2747,7 +2759,7 @@
     <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="50"/>
       <c r="B11" s="19" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="C11" s="7">
         <v>10</v>
@@ -2756,13 +2768,13 @@
         <v>10</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="G11" s="49" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="H11" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2841,7 +2853,7 @@
         <v>19</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>76</v>
+        <v>148</v>
       </c>
       <c r="H12" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2917,10 +2929,10 @@
         <v>20</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>85</v>
+        <v>149</v>
       </c>
       <c r="H13" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -2998,8 +3010,8 @@
       <c r="F14" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="31" t="s">
-        <v>98</v>
+      <c r="G14" s="54" t="s">
+        <v>150</v>
       </c>
       <c r="H14" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -3078,7 +3090,7 @@
         <v>47</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
       <c r="H15" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -3151,13 +3163,13 @@
         <v>15</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="H16" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -3221,7 +3233,7 @@
     <row r="17" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="50"/>
       <c r="B17" s="19" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="C17" s="7">
         <v>16</v>
@@ -3230,13 +3242,13 @@
         <v>16</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
       <c r="H17" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -3315,7 +3327,7 @@
         <v>74</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>88</v>
+        <v>153</v>
       </c>
       <c r="H18" s="29" t="str">
         <f>Sheet2!$A$7</f>
@@ -3394,7 +3406,7 @@
         <v>19</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="H19" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -3470,10 +3482,10 @@
         <v>16</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>89</v>
+        <v>155</v>
       </c>
       <c r="H20" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -3537,7 +3549,7 @@
     <row r="21" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="50"/>
       <c r="B21" s="19" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
       <c r="C21" s="7">
         <v>20</v>
@@ -3552,7 +3564,7 @@
         <v>19</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H21" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -3616,7 +3628,7 @@
     <row r="22" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="50"/>
       <c r="B22" s="19" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="C22" s="7">
         <v>21</v>
@@ -3625,13 +3637,13 @@
         <v>21</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="H22" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -3695,7 +3707,7 @@
     <row r="23" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="50"/>
       <c r="B23" s="19" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="C23" s="7">
         <v>22</v>
@@ -3707,10 +3719,10 @@
         <v>29</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="H23" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -3783,13 +3795,13 @@
         <v>23</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="G24" s="31" t="s">
-        <v>81</v>
+        <v>157</v>
       </c>
       <c r="H24" s="31" t="str">
         <f>Sheet2!$A$7</f>
@@ -3853,7 +3865,7 @@
     <row r="25" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="50"/>
       <c r="B25" s="19" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="C25" s="7">
         <v>24</v>
@@ -3863,7 +3875,7 @@
       </c>
       <c r="E25" s="21"/>
       <c r="F25" s="7" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31" t="s">
@@ -3927,7 +3939,7 @@
     <row r="26" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="50"/>
       <c r="B26" s="19" t="s">
-        <v>55</v>
+        <v>142</v>
       </c>
       <c r="C26" s="7">
         <v>25</v>
@@ -3936,13 +3948,13 @@
         <v>25</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="H26" s="31" t="s">
         <v>12</v>
@@ -4002,10 +4014,10 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="50"/>
-      <c r="B27" s="13" t="s">
-        <v>53</v>
+      <c r="B27" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="C27" s="7">
         <v>26</v>
@@ -4013,77 +4025,77 @@
       <c r="D27" s="7">
         <v>26</v>
       </c>
-      <c r="E27" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="H27" s="29" t="s">
+      <c r="E27" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="H27" s="31" t="s">
         <v>12</v>
       </c>
       <c r="I27" s="17">
         <v>0.75</v>
       </c>
-      <c r="J27" s="30" t="s">
+      <c r="J27" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K27" s="33">
+      <c r="K27" s="26">
         <f>$I27+Sheet2!B$1/24</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L27" s="17">
+      <c r="L27" s="24">
         <f>$I27+Sheet2!B$2/24</f>
         <v>1.125</v>
       </c>
-      <c r="M27" s="17">
+      <c r="M27" s="24">
         <f>$I27+Sheet2!B$3/24</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="N27" s="17">
+      <c r="N27" s="24">
         <f>$I27+Sheet2!B$4/24</f>
         <v>0.875</v>
       </c>
-      <c r="O27" s="17">
+      <c r="O27" s="24">
         <f>$I27+Sheet2!B$5/24</f>
         <v>0.875</v>
       </c>
-      <c r="P27" s="17">
+      <c r="P27" s="24">
         <f>$I27+Sheet2!B$6/24</f>
         <v>0.875</v>
       </c>
-      <c r="Q27" s="17">
+      <c r="Q27" s="24">
         <f>$I27+Sheet2!B$7/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R27" s="17">
+      <c r="R27" s="24">
         <f>$I27+Sheet2!B$8/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="S27" s="17">
+      <c r="S27" s="24">
         <f>$I27+Sheet2!B$9/24</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="T27" s="17">
+      <c r="T27" s="24">
         <f>$I27+Sheet2!B$10/24</f>
         <v>0.54166666666666663</v>
       </c>
-      <c r="U27" s="17">
+      <c r="U27" s="24">
         <f>$I27+Sheet2!B$11/24</f>
         <v>0.5</v>
       </c>
-      <c r="V27" s="17">
+      <c r="V27" s="24">
         <f>$I27+Sheet2!B$12/24</f>
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="50"/>
-      <c r="B28" s="34" t="s">
-        <v>111</v>
+      <c r="B28" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="C28" s="7">
         <v>27</v>
@@ -4091,77 +4103,77 @@
       <c r="D28" s="7">
         <v>27</v>
       </c>
-      <c r="E28" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="H28" s="31" t="s">
+      <c r="E28" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="H28" s="29" t="s">
         <v>12</v>
       </c>
       <c r="I28" s="17">
         <v>0.75</v>
       </c>
-      <c r="J28" s="28" t="s">
+      <c r="J28" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K28" s="26">
+      <c r="K28" s="33">
         <f>$I28+Sheet2!B$1/24</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L28" s="24">
+      <c r="L28" s="17">
         <f>$I28+Sheet2!B$2/24</f>
         <v>1.125</v>
       </c>
-      <c r="M28" s="24">
+      <c r="M28" s="17">
         <f>$I28+Sheet2!B$3/24</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="N28" s="24">
+      <c r="N28" s="17">
         <f>$I28+Sheet2!B$4/24</f>
         <v>0.875</v>
       </c>
-      <c r="O28" s="24">
+      <c r="O28" s="17">
         <f>$I28+Sheet2!B$5/24</f>
         <v>0.875</v>
       </c>
-      <c r="P28" s="24">
+      <c r="P28" s="17">
         <f>$I28+Sheet2!B$6/24</f>
         <v>0.875</v>
       </c>
-      <c r="Q28" s="24">
+      <c r="Q28" s="17">
         <f>$I28+Sheet2!B$7/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R28" s="24">
+      <c r="R28" s="17">
         <f>$I28+Sheet2!B$8/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="S28" s="24">
+      <c r="S28" s="17">
         <f>$I28+Sheet2!B$9/24</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="T28" s="24">
+      <c r="T28" s="17">
         <f>$I28+Sheet2!B$10/24</f>
         <v>0.54166666666666663</v>
       </c>
-      <c r="U28" s="24">
+      <c r="U28" s="17">
         <f>$I28+Sheet2!B$11/24</f>
         <v>0.5</v>
       </c>
-      <c r="V28" s="24">
+      <c r="V28" s="17">
         <f>$I28+Sheet2!B$12/24</f>
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="50"/>
-      <c r="B29" s="19" t="s">
-        <v>54</v>
+      <c r="B29" s="34" t="s">
+        <v>86</v>
       </c>
       <c r="C29" s="7">
         <v>28</v>
@@ -4170,13 +4182,13 @@
         <v>28</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="G29" s="31" t="s">
-        <v>101</v>
+        <v>81</v>
+      </c>
+      <c r="G29" s="36" t="s">
+        <v>160</v>
       </c>
       <c r="H29" s="31" t="s">
         <v>12</v>
@@ -4237,9 +4249,9 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="51"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="19" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="C30" s="7">
         <v>29</v>
@@ -4247,79 +4259,77 @@
       <c r="D30" s="7">
         <v>29</v>
       </c>
-      <c r="E30" s="35" t="s">
-        <v>94</v>
+      <c r="E30" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G30" s="36" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>161</v>
       </c>
       <c r="H30" s="31" t="s">
         <v>12</v>
       </c>
       <c r="I30" s="17">
-        <v>0.79166666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="J30" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K30" s="26">
         <f>$I30+Sheet2!B$1/24</f>
-        <v>1.2083333333333333</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="L30" s="24">
         <f>$I30+Sheet2!B$2/24</f>
-        <v>1.1666666666666665</v>
+        <v>1.125</v>
       </c>
       <c r="M30" s="24">
         <f>$I30+Sheet2!B$3/24</f>
-        <v>1.125</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="N30" s="24">
         <f>$I30+Sheet2!B$4/24</f>
-        <v>0.91666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="O30" s="24">
         <f>$I30+Sheet2!B$5/24</f>
-        <v>0.91666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="P30" s="24">
         <f>$I30+Sheet2!B$6/24</f>
-        <v>0.91666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="Q30" s="24">
         <f>$I30+Sheet2!B$7/24</f>
-        <v>0.875</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="R30" s="24">
         <f>$I30+Sheet2!B$8/24</f>
-        <v>0.83333333333333326</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="S30" s="24">
         <f>$I30+Sheet2!B$9/24</f>
-        <v>0.625</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="T30" s="24">
         <f>$I30+Sheet2!B$10/24</f>
-        <v>0.58333333333333326</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="U30" s="24">
         <f>$I30+Sheet2!B$11/24</f>
-        <v>0.54166666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="V30" s="24">
         <f>$I30+Sheet2!B$12/24</f>
-        <v>0.49999999999999994</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="52" t="s">
-        <v>21</v>
-      </c>
+      <c r="A31" s="51"/>
       <c r="B31" s="19" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C31" s="7">
         <v>30</v>
@@ -4328,76 +4338,78 @@
         <v>30</v>
       </c>
       <c r="E31" s="35" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="G31" s="36" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="H31" s="31" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="17">
-        <v>0.875</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="J31" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K31" s="26">
         <f>$I31+Sheet2!B$1/24</f>
-        <v>1.2916666666666667</v>
+        <v>1.2083333333333333</v>
       </c>
       <c r="L31" s="24">
         <f>$I31+Sheet2!B$2/24</f>
-        <v>1.25</v>
+        <v>1.1666666666666665</v>
       </c>
       <c r="M31" s="24">
         <f>$I31+Sheet2!B$3/24</f>
-        <v>1.2083333333333333</v>
+        <v>1.125</v>
       </c>
       <c r="N31" s="24">
         <f>$I31+Sheet2!B$4/24</f>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="O31" s="24">
         <f>$I31+Sheet2!B$5/24</f>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="P31" s="24">
         <f>$I31+Sheet2!B$6/24</f>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="Q31" s="24">
         <f>$I31+Sheet2!B$7/24</f>
-        <v>0.95833333333333337</v>
+        <v>0.875</v>
       </c>
       <c r="R31" s="24">
         <f>$I31+Sheet2!B$8/24</f>
-        <v>0.91666666666666663</v>
+        <v>0.83333333333333326</v>
       </c>
       <c r="S31" s="24">
         <f>$I31+Sheet2!B$9/24</f>
-        <v>0.70833333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="T31" s="24">
         <f>$I31+Sheet2!B$10/24</f>
-        <v>0.66666666666666663</v>
+        <v>0.58333333333333326</v>
       </c>
       <c r="U31" s="24">
         <f>$I31+Sheet2!B$11/24</f>
-        <v>0.625</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="V31" s="24">
         <f>$I31+Sheet2!B$12/24</f>
-        <v>0.58333333333333326</v>
+        <v>0.49999999999999994</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="53"/>
+      <c r="A32" s="52" t="s">
+        <v>21</v>
+      </c>
       <c r="B32" s="19" t="s">
-        <v>159</v>
+        <v>56</v>
       </c>
       <c r="C32" s="7">
         <v>31</v>
@@ -4405,74 +4417,77 @@
       <c r="D32" s="7">
         <v>31</v>
       </c>
-      <c r="E32" s="21"/>
+      <c r="E32" s="35" t="s">
+        <v>82</v>
+      </c>
       <c r="F32" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31" t="str">
-        <f>Sheet2!$A$9</f>
-        <v>EDT</v>
-      </c>
-      <c r="I32" s="24">
-        <v>0.95833333333333337</v>
+        <v>83</v>
+      </c>
+      <c r="G32" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="17">
+        <v>0.875</v>
       </c>
       <c r="J32" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K32" s="26">
         <f>$I32+Sheet2!B$1/24</f>
-        <v>1.375</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="L32" s="24">
         <f>$I32+Sheet2!B$2/24</f>
-        <v>1.3333333333333335</v>
+        <v>1.25</v>
       </c>
       <c r="M32" s="24">
         <f>$I32+Sheet2!B$3/24</f>
-        <v>1.2916666666666667</v>
+        <v>1.2083333333333333</v>
       </c>
       <c r="N32" s="24">
         <f>$I32+Sheet2!B$4/24</f>
-        <v>1.0833333333333335</v>
+        <v>1</v>
       </c>
       <c r="O32" s="24">
         <f>$I32+Sheet2!B$5/24</f>
-        <v>1.0833333333333335</v>
+        <v>1</v>
       </c>
       <c r="P32" s="24">
         <f>$I32+Sheet2!B$6/24</f>
-        <v>1.0833333333333335</v>
+        <v>1</v>
       </c>
       <c r="Q32" s="24">
         <f>$I32+Sheet2!B$7/24</f>
-        <v>1.0416666666666667</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="R32" s="24">
         <f>$I32+Sheet2!B$8/24</f>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="S32" s="24">
         <f>$I32+Sheet2!B$9/24</f>
-        <v>0.79166666666666674</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="T32" s="24">
         <f>$I32+Sheet2!B$10/24</f>
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="U32" s="24">
         <f>$I32+Sheet2!B$11/24</f>
-        <v>0.70833333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="V32" s="24">
         <f>$I32+Sheet2!B$12/24</f>
-        <v>0.66666666666666674</v>
+        <v>0.58333333333333326</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="53"/>
       <c r="B33" s="19" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C33" s="7">
         <v>32</v>
@@ -4480,15 +4495,11 @@
       <c r="D33" s="7">
         <v>32</v>
       </c>
-      <c r="E33" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G33" s="23" t="s">
-        <v>114</v>
-      </c>
+      <c r="E33" s="21"/>
+      <c r="F33" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33" s="31"/>
       <c r="H33" s="31" t="str">
         <f>Sheet2!$A$9</f>
         <v>EDT</v>
@@ -4548,10 +4559,10 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="53"/>
       <c r="B34" s="19" t="s">
-        <v>143</v>
+        <v>88</v>
       </c>
       <c r="C34" s="7">
         <v>33</v>
@@ -4559,22 +4570,23 @@
       <c r="D34" s="7">
         <v>33</v>
       </c>
-      <c r="E34" s="41" t="s">
+      <c r="E34" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="G34" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="H34" s="42" t="s">
-        <v>145</v>
-      </c>
-      <c r="I34" s="43">
+      <c r="F34" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="H34" s="31" t="str">
+        <f>Sheet2!$A$9</f>
+        <v>EDT</v>
+      </c>
+      <c r="I34" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J34" s="44" t="s">
+      <c r="J34" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K34" s="26">
@@ -4626,10 +4638,10 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="53"/>
-      <c r="B35" s="13" t="s">
-        <v>37</v>
+      <c r="B35" s="19" t="s">
+        <v>98</v>
       </c>
       <c r="C35" s="7">
         <v>34</v>
@@ -4637,26 +4649,25 @@
       <c r="D35" s="7">
         <v>34</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="G35" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="H35" s="31" t="str">
-        <f>Sheet2!$A$9</f>
-        <v>EDT</v>
-      </c>
-      <c r="I35" s="24">
+      <c r="G35" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="H35" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35" s="43">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J35" s="28" t="s">
+      <c r="J35" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="K35" s="12">
+      <c r="K35" s="26">
         <f>$I35+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
@@ -4708,7 +4719,7 @@
     <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="53"/>
       <c r="B36" s="13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C36" s="7">
         <v>35</v>
@@ -4722,8 +4733,8 @@
       <c r="F36" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="22" t="s">
-        <v>116</v>
+      <c r="G36" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="H36" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4735,7 +4746,7 @@
       <c r="J36" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="26">
+      <c r="K36" s="12">
         <f>$I36+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
@@ -4786,8 +4797,8 @@
     </row>
     <row r="37" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="53"/>
-      <c r="B37" s="19" t="s">
-        <v>33</v>
+      <c r="B37" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="C37" s="7">
         <v>36</v>
@@ -4801,8 +4812,8 @@
       <c r="F37" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="9" t="s">
-        <v>78</v>
+      <c r="G37" s="22" t="s">
+        <v>167</v>
       </c>
       <c r="H37" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4865,8 +4876,8 @@
     </row>
     <row r="38" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="53"/>
-      <c r="B38" s="13" t="s">
-        <v>38</v>
+      <c r="B38" s="19" t="s">
+        <v>33</v>
       </c>
       <c r="C38" s="7">
         <v>37</v>
@@ -4880,8 +4891,8 @@
       <c r="F38" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G38" s="23" t="s">
-        <v>133</v>
+      <c r="G38" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="H38" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4890,62 +4901,62 @@
       <c r="I38" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J38" s="30" t="s">
+      <c r="J38" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K38" s="33">
+      <c r="K38" s="26">
         <f>$I38+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L38" s="17">
+      <c r="L38" s="24">
         <f>$I38+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M38" s="17">
+      <c r="M38" s="24">
         <f>$I38+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N38" s="17">
+      <c r="N38" s="24">
         <f>$I38+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O38" s="17">
+      <c r="O38" s="24">
         <f>$I38+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P38" s="17">
+      <c r="P38" s="24">
         <f>$I38+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q38" s="17">
+      <c r="Q38" s="24">
         <f>$I38+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R38" s="17">
+      <c r="R38" s="24">
         <f>$I38+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S38" s="17">
+      <c r="S38" s="24">
         <f>$I38+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T38" s="17">
+      <c r="T38" s="24">
         <f>$I38+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U38" s="17">
+      <c r="U38" s="24">
         <f>$I38+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V38" s="17">
+      <c r="V38" s="24">
         <f>$I38+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="53"/>
-      <c r="B39" s="19" t="s">
-        <v>34</v>
+      <c r="B39" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="C39" s="7">
         <v>38</v>
@@ -4959,8 +4970,8 @@
       <c r="F39" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G39" s="9" t="s">
-        <v>79</v>
+      <c r="G39" s="23" t="s">
+        <v>169</v>
       </c>
       <c r="H39" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -4969,54 +4980,54 @@
       <c r="I39" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J39" s="28" t="s">
+      <c r="J39" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K39" s="26">
+      <c r="K39" s="33">
         <f>$I39+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L39" s="24">
+      <c r="L39" s="17">
         <f>$I39+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M39" s="24">
+      <c r="M39" s="17">
         <f>$I39+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N39" s="24">
+      <c r="N39" s="17">
         <f>$I39+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O39" s="24">
+      <c r="O39" s="17">
         <f>$I39+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P39" s="24">
+      <c r="P39" s="17">
         <f>$I39+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q39" s="24">
+      <c r="Q39" s="17">
         <f>$I39+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R39" s="24">
+      <c r="R39" s="17">
         <f>$I39+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S39" s="24">
+      <c r="S39" s="17">
         <f>$I39+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T39" s="24">
+      <c r="T39" s="17">
         <f>$I39+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U39" s="24">
+      <c r="U39" s="17">
         <f>$I39+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V39" s="24">
+      <c r="V39" s="17">
         <f>$I39+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
@@ -5024,7 +5035,7 @@
     <row r="40" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="53"/>
       <c r="B40" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C40" s="7">
         <v>39</v>
@@ -5038,8 +5049,8 @@
       <c r="F40" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G40" s="23" t="s">
-        <v>110</v>
+      <c r="G40" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="H40" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -5051,7 +5062,7 @@
       <c r="J40" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K40" s="12">
+      <c r="K40" s="26">
         <f>$I40+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
@@ -5103,7 +5114,7 @@
     <row r="41" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="53"/>
       <c r="B41" s="19" t="s">
-        <v>151</v>
+        <v>36</v>
       </c>
       <c r="C41" s="7">
         <v>40</v>
@@ -5111,14 +5122,14 @@
       <c r="D41" s="7">
         <v>40</v>
       </c>
-      <c r="E41" s="41" t="s">
+      <c r="E41" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F41" s="42" t="s">
+      <c r="F41" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G41" s="31" t="s">
-        <v>152</v>
+      <c r="G41" s="23" t="s">
+        <v>171</v>
       </c>
       <c r="H41" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -5130,7 +5141,7 @@
       <c r="J41" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K41" s="26">
+      <c r="K41" s="12">
         <f>$I41+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
@@ -5181,8 +5192,8 @@
     </row>
     <row r="42" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="53"/>
-      <c r="B42" s="13" t="s">
-        <v>146</v>
+      <c r="B42" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="C42" s="7">
         <v>41</v>
@@ -5190,14 +5201,14 @@
       <c r="D42" s="7">
         <v>41</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="F42" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="G42" s="23" t="s">
-        <v>147</v>
+      <c r="G42" s="31" t="s">
+        <v>172</v>
       </c>
       <c r="H42" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -5206,62 +5217,62 @@
       <c r="I42" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J42" s="30" t="s">
+      <c r="J42" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K42" s="33">
+      <c r="K42" s="26">
         <f>$I42+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L42" s="17">
+      <c r="L42" s="24">
         <f>$I42+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M42" s="17">
+      <c r="M42" s="24">
         <f>$I42+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N42" s="17">
+      <c r="N42" s="24">
         <f>$I42+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O42" s="17">
+      <c r="O42" s="24">
         <f>$I42+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P42" s="17">
+      <c r="P42" s="24">
         <f>$I42+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q42" s="17">
+      <c r="Q42" s="24">
         <f>$I42+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R42" s="17">
+      <c r="R42" s="24">
         <f>$I42+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S42" s="17">
+      <c r="S42" s="24">
         <f>$I42+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T42" s="17">
+      <c r="T42" s="24">
         <f>$I42+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U42" s="17">
+      <c r="U42" s="24">
         <f>$I42+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V42" s="17">
+      <c r="V42" s="24">
         <f>$I42+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="43" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="53"/>
-      <c r="B43" s="19" t="s">
-        <v>31</v>
+      <c r="B43" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="C43" s="7">
         <v>42</v>
@@ -5275,8 +5286,8 @@
       <c r="F43" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G43" s="9" t="s">
-        <v>82</v>
+      <c r="G43" s="23" t="s">
+        <v>141</v>
       </c>
       <c r="H43" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -5285,54 +5296,54 @@
       <c r="I43" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J43" s="28" t="s">
+      <c r="J43" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K43" s="26">
+      <c r="K43" s="33">
         <f>$I43+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L43" s="24">
+      <c r="L43" s="17">
         <f>$I43+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M43" s="24">
+      <c r="M43" s="17">
         <f>$I43+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N43" s="24">
+      <c r="N43" s="17">
         <f>$I43+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O43" s="24">
+      <c r="O43" s="17">
         <f>$I43+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P43" s="24">
+      <c r="P43" s="17">
         <f>$I43+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q43" s="24">
+      <c r="Q43" s="17">
         <f>$I43+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R43" s="24">
+      <c r="R43" s="17">
         <f>$I43+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S43" s="24">
+      <c r="S43" s="17">
         <f>$I43+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T43" s="24">
+      <c r="T43" s="17">
         <f>$I43+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U43" s="24">
+      <c r="U43" s="17">
         <f>$I43+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V43" s="24">
+      <c r="V43" s="17">
         <f>$I43+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
@@ -5340,7 +5351,7 @@
     <row r="44" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="53"/>
       <c r="B44" s="19" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="C44" s="7">
         <v>43</v>
@@ -5354,8 +5365,8 @@
       <c r="F44" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>83</v>
+      <c r="G44" s="56" t="s">
+        <v>140</v>
       </c>
       <c r="H44" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -5364,54 +5375,54 @@
       <c r="I44" s="24">
         <v>0.95833333333333337</v>
       </c>
-      <c r="J44" s="28" t="s">
+      <c r="J44" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K44" s="26">
+      <c r="K44" s="33">
         <f>$I44+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
-      <c r="L44" s="24">
+      <c r="L44" s="17">
         <f>$I44+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="M44" s="24">
+      <c r="M44" s="17">
         <f>$I44+Sheet2!B$3/24</f>
         <v>1.2916666666666667</v>
       </c>
-      <c r="N44" s="24">
+      <c r="N44" s="17">
         <f>$I44+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="O44" s="24">
+      <c r="O44" s="17">
         <f>$I44+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P44" s="24">
+      <c r="P44" s="17">
         <f>$I44+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q44" s="24">
+      <c r="Q44" s="17">
         <f>$I44+Sheet2!B$7/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="R44" s="24">
+      <c r="R44" s="17">
         <f>$I44+Sheet2!B$8/24</f>
         <v>1</v>
       </c>
-      <c r="S44" s="24">
+      <c r="S44" s="17">
         <f>$I44+Sheet2!B$9/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="T44" s="24">
+      <c r="T44" s="17">
         <f>$I44+Sheet2!B$10/24</f>
         <v>0.75</v>
       </c>
-      <c r="U44" s="24">
+      <c r="U44" s="17">
         <f>$I44+Sheet2!B$11/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="V44" s="24">
+      <c r="V44" s="17">
         <f>$I44+Sheet2!B$12/24</f>
         <v>0.66666666666666674</v>
       </c>
@@ -5419,7 +5430,7 @@
     <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="53"/>
       <c r="B45" s="19" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C45" s="7">
         <v>44</v>
@@ -5431,10 +5442,10 @@
         <v>29</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G45" s="22" t="s">
-        <v>84</v>
+        <v>22</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="H45" s="31" t="str">
         <f>Sheet2!$A$9</f>
@@ -5498,7 +5509,7 @@
     <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="53"/>
       <c r="B46" s="19" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="C46" s="7">
         <v>45</v>
@@ -5506,73 +5517,78 @@
       <c r="D46" s="7">
         <v>45</v>
       </c>
-      <c r="E46" s="15"/>
+      <c r="E46" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="F46" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="G46" s="9"/>
-      <c r="H46" s="31" t="s">
-        <v>73</v>
+        <v>22</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="H46" s="31" t="str">
+        <f>Sheet2!$A$9</f>
+        <v>EDT</v>
       </c>
       <c r="I46" s="24">
-        <v>0</v>
-      </c>
-      <c r="J46" s="30" t="s">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="J46" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K46" s="26">
         <f>$I46+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
+        <v>1.375</v>
       </c>
       <c r="L46" s="24">
         <f>$I46+Sheet2!B$2/24</f>
-        <v>0.375</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="M46" s="24">
         <f>$I46+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="N46" s="24">
         <f>$I46+Sheet2!B$4/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="O46" s="24">
         <f>$I46+Sheet2!B$5/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="P46" s="24">
         <f>$I46+Sheet2!B$6/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="Q46" s="24">
         <f>$I46+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="R46" s="24">
         <f>$I46+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>1</v>
       </c>
       <c r="S46" s="24">
         <f>$I46+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="T46" s="24">
         <f>$I46+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="U46" s="24">
         <f>$I46+Sheet2!B$11/24</f>
-        <v>-0.25</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="V46" s="24">
         <f>$I46+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="53"/>
-      <c r="B47" s="37" t="s">
-        <v>153</v>
+      <c r="B47" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="C47" s="7">
         <v>46</v>
@@ -5584,73 +5600,74 @@
         <v>29</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G47" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="H47" s="31" t="s">
-        <v>73</v>
+        <v>47</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="H47" s="31" t="str">
+        <f>Sheet2!$A$9</f>
+        <v>EDT</v>
       </c>
       <c r="I47" s="24">
-        <v>0</v>
-      </c>
-      <c r="J47" s="30" t="s">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="J47" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K47" s="26">
         <f>$I47+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
+        <v>1.375</v>
       </c>
       <c r="L47" s="24">
         <f>$I47+Sheet2!B$2/24</f>
-        <v>0.375</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="M47" s="24">
         <f>$I47+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="N47" s="24">
         <f>$I47+Sheet2!B$4/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="O47" s="24">
         <f>$I47+Sheet2!B$5/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="P47" s="24">
         <f>$I47+Sheet2!B$6/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="Q47" s="24">
         <f>$I47+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="R47" s="24">
         <f>$I47+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>1</v>
       </c>
       <c r="S47" s="24">
         <f>$I47+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="T47" s="24">
         <f>$I47+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="U47" s="24">
         <f>$I47+Sheet2!B$11/24</f>
-        <v>-0.25</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="V47" s="24">
         <f>$I47+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="53"/>
-      <c r="B48" s="37" t="s">
-        <v>61</v>
+      <c r="B48" s="19" t="s">
+        <v>116</v>
       </c>
       <c r="C48" s="7">
         <v>47</v>
@@ -5658,15 +5675,11 @@
       <c r="D48" s="7">
         <v>47</v>
       </c>
-      <c r="E48" s="15" t="s">
-        <v>29</v>
-      </c>
+      <c r="E48" s="15"/>
       <c r="F48" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G48" s="31" t="s">
-        <v>75</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="G48" s="9"/>
       <c r="H48" s="31" t="s">
         <v>73</v>
       </c>
@@ -5728,7 +5741,7 @@
     <row r="49" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="53"/>
       <c r="B49" s="37" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="C49" s="7">
         <v>48</v>
@@ -5739,11 +5752,11 @@
       <c r="E49" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F49" s="7" t="s">
-        <v>74</v>
+      <c r="F49" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="G49" s="31" t="s">
-        <v>134</v>
+        <v>176</v>
       </c>
       <c r="H49" s="31" t="s">
         <v>73</v>
@@ -5805,8 +5818,8 @@
     </row>
     <row r="50" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="53"/>
-      <c r="B50" s="19" t="s">
-        <v>137</v>
+      <c r="B50" s="37" t="s">
+        <v>61</v>
       </c>
       <c r="C50" s="7">
         <v>49</v>
@@ -5814,14 +5827,14 @@
       <c r="D50" s="7">
         <v>49</v>
       </c>
-      <c r="E50" s="41" t="s">
+      <c r="E50" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F50" s="42" t="s">
+      <c r="F50" s="20" t="s">
         <v>22</v>
       </c>
       <c r="G50" s="31" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="H50" s="31" t="s">
         <v>73</v>
@@ -5829,7 +5842,7 @@
       <c r="I50" s="24">
         <v>0</v>
       </c>
-      <c r="J50" s="28" t="s">
+      <c r="J50" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K50" s="26">
@@ -5883,8 +5896,8 @@
     </row>
     <row r="51" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="53"/>
-      <c r="B51" s="19" t="s">
-        <v>62</v>
+      <c r="B51" s="37" t="s">
+        <v>59</v>
       </c>
       <c r="C51" s="7">
         <v>50</v>
@@ -5895,11 +5908,11 @@
       <c r="E51" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="20" t="s">
-        <v>22</v>
+      <c r="F51" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="G51" s="31" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="H51" s="31" t="s">
         <v>73</v>
@@ -5961,8 +5974,8 @@
     </row>
     <row r="52" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="53"/>
-      <c r="B52" s="37" t="s">
-        <v>65</v>
+      <c r="B52" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="C52" s="7">
         <v>51</v>
@@ -5970,14 +5983,14 @@
       <c r="D52" s="7">
         <v>51</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E52" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F52" s="20" t="s">
-        <v>47</v>
+      <c r="F52" s="42" t="s">
+        <v>22</v>
       </c>
       <c r="G52" s="31" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
       <c r="H52" s="31" t="s">
         <v>73</v>
@@ -5985,7 +5998,7 @@
       <c r="I52" s="24">
         <v>0</v>
       </c>
-      <c r="J52" s="30" t="s">
+      <c r="J52" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K52" s="26">
@@ -6039,8 +6052,8 @@
     </row>
     <row r="53" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="53"/>
-      <c r="B53" s="37" t="s">
-        <v>63</v>
+      <c r="B53" s="19" t="s">
+        <v>62</v>
       </c>
       <c r="C53" s="7">
         <v>52</v>
@@ -6054,8 +6067,8 @@
       <c r="F53" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G53" s="29" t="s">
-        <v>122</v>
+      <c r="G53" s="31" t="s">
+        <v>180</v>
       </c>
       <c r="H53" s="31" t="s">
         <v>73</v>
@@ -6117,8 +6130,8 @@
     </row>
     <row r="54" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="53"/>
-      <c r="B54" s="19" t="s">
-        <v>60</v>
+      <c r="B54" s="37" t="s">
+        <v>65</v>
       </c>
       <c r="C54" s="7">
         <v>53</v>
@@ -6129,11 +6142,11 @@
       <c r="E54" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F54" s="7" t="s">
-        <v>168</v>
+      <c r="F54" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="G54" s="31" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="H54" s="31" t="s">
         <v>73</v>
@@ -6195,8 +6208,8 @@
     </row>
     <row r="55" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="53"/>
-      <c r="B55" s="19" t="s">
-        <v>58</v>
+      <c r="B55" s="37" t="s">
+        <v>63</v>
       </c>
       <c r="C55" s="7">
         <v>54</v>
@@ -6210,8 +6223,8 @@
       <c r="F55" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G55" s="31" t="s">
-        <v>80</v>
+      <c r="G55" s="29" t="s">
+        <v>182</v>
       </c>
       <c r="H55" s="31" t="s">
         <v>73</v>
@@ -6219,7 +6232,7 @@
       <c r="I55" s="24">
         <v>0</v>
       </c>
-      <c r="J55" s="28" t="s">
+      <c r="J55" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K55" s="26">
@@ -6271,10 +6284,10 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="56" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="53"/>
       <c r="B56" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C56" s="7">
         <v>55</v>
@@ -6286,10 +6299,10 @@
         <v>29</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="G56" s="31" t="s">
-        <v>123</v>
+        <v>183</v>
       </c>
       <c r="H56" s="31" t="s">
         <v>73</v>
@@ -6352,7 +6365,7 @@
     <row r="57" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="53"/>
       <c r="B57" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C57" s="7">
         <v>56</v>
@@ -6366,8 +6379,8 @@
       <c r="F57" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G57" s="29" t="s">
-        <v>117</v>
+      <c r="G57" s="31" t="s">
+        <v>184</v>
       </c>
       <c r="H57" s="31" t="s">
         <v>73</v>
@@ -6427,10 +6440,10 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="58" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="53"/>
       <c r="B58" s="19" t="s">
-        <v>183</v>
+        <v>64</v>
       </c>
       <c r="C58" s="7">
         <v>57</v>
@@ -6438,73 +6451,77 @@
       <c r="D58" s="7">
         <v>57</v>
       </c>
-      <c r="E58" s="15"/>
-      <c r="F58" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="G58" s="31"/>
+      <c r="E58" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G58" s="31" t="s">
+        <v>185</v>
+      </c>
       <c r="H58" s="31" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="I58" s="24">
-        <v>4.1666666666666664E-2</v>
+        <v>0</v>
       </c>
       <c r="J58" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K58" s="26">
         <f>$I58+Sheet2!B$1/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L58" s="24">
         <f>$I58+Sheet2!B$2/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="M58" s="24">
         <f>$I58+Sheet2!B$3/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N58" s="24">
         <f>$I58+Sheet2!B$4/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="O58" s="24">
         <f>$I58+Sheet2!B$5/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="P58" s="24">
         <f>$I58+Sheet2!B$6/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="Q58" s="24">
         <f>$I58+Sheet2!B$7/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R58" s="24">
         <f>$I58+Sheet2!B$8/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="S58" s="24">
         <f>$I58+Sheet2!B$9/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="T58" s="24">
         <f>$I58+Sheet2!B$10/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="U58" s="24">
         <f>$I58+Sheet2!B$11/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.25</v>
       </c>
       <c r="V58" s="24">
         <f>$I58+Sheet2!B$12/24</f>
-        <v>-0.25</v>
+        <v>-0.29166666666666669</v>
       </c>
     </row>
     <row r="59" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="53"/>
       <c r="B59" s="19" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C59" s="7">
         <v>58</v>
@@ -6513,76 +6530,76 @@
         <v>58</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="G59" s="36" t="s">
-        <v>125</v>
+        <v>29</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G59" s="29" t="s">
+        <v>186</v>
       </c>
       <c r="H59" s="31" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="I59" s="24">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J59" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="J59" s="28" t="s">
         <v>15</v>
       </c>
       <c r="K59" s="26">
         <f>$I59+Sheet2!B$1/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L59" s="24">
         <f>$I59+Sheet2!B$2/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="M59" s="24">
         <f>$I59+Sheet2!B$3/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N59" s="24">
         <f>$I59+Sheet2!B$4/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="O59" s="24">
         <f>$I59+Sheet2!B$5/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="P59" s="24">
         <f>$I59+Sheet2!B$6/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="Q59" s="24">
         <f>$I59+Sheet2!B$7/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R59" s="24">
         <f>$I59+Sheet2!B$8/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="S59" s="24">
         <f>$I59+Sheet2!B$9/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="T59" s="24">
         <f>$I59+Sheet2!B$10/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="U59" s="24">
         <f>$I59+Sheet2!B$11/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.25</v>
       </c>
       <c r="V59" s="24">
         <f>$I59+Sheet2!B$12/24</f>
-        <v>-0.25</v>
+        <v>-0.29166666666666669</v>
       </c>
     </row>
     <row r="60" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="53"/>
-      <c r="B60" s="37" t="s">
-        <v>67</v>
+      <c r="B60" s="19" t="s">
+        <v>133</v>
       </c>
       <c r="C60" s="7">
         <v>59</v>
@@ -6590,16 +6607,12 @@
       <c r="D60" s="7">
         <v>59</v>
       </c>
-      <c r="E60" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G60" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="H60" s="37" t="s">
+      <c r="E60" s="15"/>
+      <c r="F60" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="G60" s="31"/>
+      <c r="H60" s="31" t="s">
         <v>13</v>
       </c>
       <c r="I60" s="24">
@@ -6660,7 +6673,7 @@
     <row r="61" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="53"/>
       <c r="B61" s="19" t="s">
-        <v>184</v>
+        <v>66</v>
       </c>
       <c r="C61" s="7">
         <v>60</v>
@@ -6668,73 +6681,77 @@
       <c r="D61" s="7">
         <v>60</v>
       </c>
-      <c r="E61" s="15"/>
-      <c r="F61" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="G61" s="31"/>
+      <c r="E61" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G61" s="36" t="s">
+        <v>187</v>
+      </c>
       <c r="H61" s="31" t="s">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="I61" s="24">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J61" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K61" s="26">
         <f>$I61+Sheet2!B$1/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="L61" s="24">
         <f>$I61+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M61" s="24">
         <f>$I61+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="N61" s="24">
         <f>$I61+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="O61" s="24">
         <f>$I61+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P61" s="24">
         <f>$I61+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q61" s="24">
         <f>$I61+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="R61" s="24">
         <f>$I61+Sheet2!B$8/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S61" s="24">
         <f>$I61+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="T61" s="24">
         <f>$I61+Sheet2!B$10/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="U61" s="24">
         <f>$I61+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="V61" s="24">
         <f>$I61+Sheet2!B$12/24</f>
-        <v>-0.20833333333333337</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="62" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="53"/>
-      <c r="B62" s="19" t="s">
-        <v>70</v>
+      <c r="B62" s="37" t="s">
+        <v>67</v>
       </c>
       <c r="C62" s="7">
         <v>61</v>
@@ -6745,74 +6762,74 @@
       <c r="E62" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F62" s="20" t="s">
+      <c r="F62" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G62" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="H62" s="31" t="s">
-        <v>72</v>
+      <c r="G62" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="H62" s="37" t="s">
+        <v>13</v>
       </c>
       <c r="I62" s="24">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J62" s="30" t="s">
         <v>15</v>
       </c>
       <c r="K62" s="26">
         <f>$I62+Sheet2!B$1/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="L62" s="24">
         <f>$I62+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M62" s="24">
         <f>$I62+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="N62" s="24">
         <f>$I62+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="O62" s="24">
         <f>$I62+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P62" s="24">
         <f>$I62+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q62" s="24">
         <f>$I62+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="R62" s="24">
         <f>$I62+Sheet2!B$8/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S62" s="24">
         <f>$I62+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="T62" s="24">
         <f>$I62+Sheet2!B$10/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="U62" s="24">
         <f>$I62+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="V62" s="24">
         <f>$I62+Sheet2!B$12/24</f>
-        <v>-0.20833333333333337</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="63" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="53"/>
-      <c r="B63" s="37" t="s">
-        <v>69</v>
+      <c r="B63" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="C63" s="7">
         <v>62</v>
@@ -6820,15 +6837,11 @@
       <c r="D63" s="7">
         <v>62</v>
       </c>
-      <c r="E63" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G63" s="9" t="s">
-        <v>127</v>
-      </c>
+      <c r="E63" s="15"/>
+      <c r="F63" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="G63" s="31"/>
       <c r="H63" s="31" t="s">
         <v>72</v>
       </c>
@@ -6890,7 +6903,7 @@
     <row r="64" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="53"/>
       <c r="B64" s="19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C64" s="7">
         <v>63</v>
@@ -6901,11 +6914,11 @@
       <c r="E64" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F64" s="14" t="s">
+      <c r="F64" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G64" s="39" t="s">
-        <v>126</v>
+      <c r="G64" s="22" t="s">
+        <v>189</v>
       </c>
       <c r="H64" s="31" t="s">
         <v>72</v>
@@ -6968,7 +6981,7 @@
     <row r="65" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="53"/>
       <c r="B65" s="37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C65" s="7">
         <v>64</v>
@@ -6979,11 +6992,11 @@
       <c r="E65" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F65" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="G65" s="23" t="s">
-        <v>129</v>
+      <c r="F65" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="H65" s="31" t="s">
         <v>72</v>
@@ -7043,419 +7056,575 @@
         <v>-0.20833333333333337</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="53"/>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B66" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C66" s="7">
+        <v>65</v>
+      </c>
+      <c r="D66" s="7">
+        <v>65</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G66" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="H66" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="I66" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J66" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K66" s="26">
+        <f>$I66+Sheet2!B$1/24</f>
+        <v>0.5</v>
+      </c>
+      <c r="L66" s="24">
+        <f>$I66+Sheet2!B$2/24</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M66" s="24">
+        <f>$I66+Sheet2!B$3/24</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="N66" s="24">
+        <f>$I66+Sheet2!B$4/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="O66" s="24">
+        <f>$I66+Sheet2!B$5/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P66" s="24">
+        <f>$I66+Sheet2!B$6/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="Q66" s="24">
+        <f>$I66+Sheet2!B$7/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R66" s="24">
+        <f>$I66+Sheet2!B$8/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="S66" s="24">
+        <f>$I66+Sheet2!B$9/24</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="T66" s="24">
+        <f>$I66+Sheet2!B$10/24</f>
+        <v>-0.125</v>
+      </c>
+      <c r="U66" s="24">
+        <f>$I66+Sheet2!B$11/24</f>
+        <v>-0.16666666666666669</v>
+      </c>
+      <c r="V66" s="24">
+        <f>$I66+Sheet2!B$12/24</f>
+        <v>-0.20833333333333337</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="53"/>
+      <c r="B67" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" s="7">
+        <v>66</v>
+      </c>
+      <c r="D67" s="7">
+        <v>66</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F67" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G67" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="H67" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="I67" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J67" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K67" s="26">
+        <f>$I67+Sheet2!B$1/24</f>
+        <v>0.5</v>
+      </c>
+      <c r="L67" s="24">
+        <f>$I67+Sheet2!B$2/24</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M67" s="24">
+        <f>$I67+Sheet2!B$3/24</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="N67" s="24">
+        <f>$I67+Sheet2!B$4/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="O67" s="24">
+        <f>$I67+Sheet2!B$5/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="P67" s="24">
+        <f>$I67+Sheet2!B$6/24</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="Q67" s="24">
+        <f>$I67+Sheet2!B$7/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R67" s="24">
+        <f>$I67+Sheet2!B$8/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="S67" s="24">
+        <f>$I67+Sheet2!B$9/24</f>
+        <v>-8.3333333333333329E-2</v>
+      </c>
+      <c r="T67" s="24">
+        <f>$I67+Sheet2!B$10/24</f>
+        <v>-0.125</v>
+      </c>
+      <c r="U67" s="24">
+        <f>$I67+Sheet2!B$11/24</f>
+        <v>-0.16666666666666669</v>
+      </c>
+      <c r="V67" s="24">
+        <f>$I67+Sheet2!B$12/24</f>
+        <v>-0.20833333333333337</v>
+      </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" s="53"/>
     </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A69" s="53"/>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A70" s="53"/>
+    </row>
   </sheetData>
-  <sortState ref="B2:V55">
-    <sortCondition ref="D2:D55"/>
+  <sortState ref="B2:V57">
+    <sortCondition ref="D2:D57"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
-    <mergeCell ref="A10:A30"/>
-    <mergeCell ref="A31:A68"/>
+    <mergeCell ref="A10:A31"/>
+    <mergeCell ref="A32:A70"/>
   </mergeCells>
-  <conditionalFormatting sqref="K24:V57 K2:L8 K59:V60 K62:V65 K6:V20">
-    <cfRule type="expression" dxfId="79" priority="141">
+  <conditionalFormatting sqref="K2:L8 K61:V62 K64:V67 K6:V20 K24:V59">
+    <cfRule type="expression" dxfId="78" priority="141">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V8">
-    <cfRule type="expression" dxfId="78" priority="143">
+    <cfRule type="expression" dxfId="77" priority="143">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K34:V34 G41:V41 G34 B43:B46 K48:V48 G48 G50:V50 B49:B50 K51:V53 G51:G53 B54:B55 K56:V56 G56 G65 K59:V60 E54:V55 E43:V45 E35:V40 E46:G46 E24:V33 B24:B41 H22:V22 H2:V2 B3:V3 G58:G63 K62:V65 E18:V21 G17:V17 B4:B21 E4:V16 C5:D5 C7:D7 C9:D9 C11:D11 C13:D13 C15:D15 C17:D17 C19:D19 C21:D21 C23:D23 C25:D25 C27:D27 C29:D29 C31:D31 C33:D33 C35:D35 C37:D37 C39:D39 C41:D41 C43:D43 C45:D45 C47:D47 C49:V49 C51:D51 C53:D53 C55:D55 B57:V57 C59:D59 C61:D61 C63:D63 C65:D65">
-    <cfRule type="expression" dxfId="77" priority="147">
+  <conditionalFormatting sqref="K35:V35 G42:V42 G35 B45:B48 K50:V50 G50 G52:V52 B51:B52 K53:V55 G53:G55 B56:B57 K58:V58 G58 G67 K61:V62 E56:V57 E45:V47 E36:V41 E48:G48 B24:B42 H22:V22 H2:V2 B3:V3 G60:G65 K64:V67 E18:V21 G17:V17 B4:B21 E4:V16 C5:D5 E24:V34 C7:D7 C11:D11 C15:D15 C19:D19 C23:D23 C27:D27 C31:D31 C35:D35 C39:D39 C43:D43 C47:D47 C51:V51 C55:D55 B59:V59 C63:D63 C67:D67 C9:D9 C13:D13 C17:D17 C21:D21 C25:D25 C29:D29 C33:D33 C37:D37 C41:D41 C45:D45 C49:D49 C53:D53 C57:D57 C61:D61 C65:D65">
+    <cfRule type="expression" dxfId="76" priority="147">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48 J48:V48">
-    <cfRule type="expression" dxfId="76" priority="124">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B51 J51:V51">
-    <cfRule type="expression" dxfId="75" priority="122">
+  <conditionalFormatting sqref="B50 J50:V50">
+    <cfRule type="expression" dxfId="75" priority="124">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53 J53:V53">
-    <cfRule type="expression" dxfId="74" priority="120">
+    <cfRule type="expression" dxfId="74" priority="122">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B56 J56:V56">
-    <cfRule type="expression" dxfId="73" priority="118">
+  <conditionalFormatting sqref="B55 J55:V55">
+    <cfRule type="expression" dxfId="73" priority="120">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B52 J52:V52">
-    <cfRule type="expression" dxfId="72" priority="116">
+  <conditionalFormatting sqref="B58 J58:V58">
+    <cfRule type="expression" dxfId="72" priority="118">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B59 J59:V59">
-    <cfRule type="expression" dxfId="71" priority="114">
+  <conditionalFormatting sqref="B54 J54:V54">
+    <cfRule type="expression" dxfId="71" priority="116">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B60 J60:V60 E60:F60 H60">
-    <cfRule type="expression" dxfId="70" priority="112">
+  <conditionalFormatting sqref="B61 J61:V61">
+    <cfRule type="expression" dxfId="70" priority="114">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
-    <cfRule type="expression" dxfId="69" priority="110">
+  <conditionalFormatting sqref="B62 J62:V62 E62:F62 H62">
+    <cfRule type="expression" dxfId="69" priority="112">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
-    <cfRule type="expression" dxfId="68" priority="107">
+  <conditionalFormatting sqref="E50">
+    <cfRule type="expression" dxfId="68" priority="110">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="expression" dxfId="67" priority="106">
+  <conditionalFormatting sqref="E58">
+    <cfRule type="expression" dxfId="67" priority="107">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E59 H59">
-    <cfRule type="expression" dxfId="66" priority="105">
+  <conditionalFormatting sqref="E54">
+    <cfRule type="expression" dxfId="66" priority="106">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E61 H61">
+    <cfRule type="expression" dxfId="65" priority="105">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B66 J66:V66">
+    <cfRule type="expression" dxfId="64" priority="103">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B65 J65:V65 E65">
+    <cfRule type="expression" dxfId="63" priority="101">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66:F66 H66">
+    <cfRule type="expression" dxfId="62" priority="99">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64 J64:V64">
-    <cfRule type="expression" dxfId="65" priority="103">
+    <cfRule type="expression" dxfId="61" priority="97">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B63 J63:V63 E63">
-    <cfRule type="expression" dxfId="64" priority="101">
+  <conditionalFormatting sqref="B67 J67:V67 E67">
+    <cfRule type="expression" dxfId="60" priority="95">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E64:F64 H64">
-    <cfRule type="expression" dxfId="63" priority="99">
+  <conditionalFormatting sqref="F54">
+    <cfRule type="expression" dxfId="59" priority="87">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B62 J62:V62">
-    <cfRule type="expression" dxfId="62" priority="97">
+  <conditionalFormatting sqref="I50">
+    <cfRule type="expression" dxfId="58" priority="77">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B65 J65:V65 E65">
-    <cfRule type="expression" dxfId="61" priority="95">
+  <conditionalFormatting sqref="I53">
+    <cfRule type="expression" dxfId="57" priority="76">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F52">
-    <cfRule type="expression" dxfId="60" priority="87">
+  <conditionalFormatting sqref="I55">
+    <cfRule type="expression" dxfId="56" priority="75">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I58">
+    <cfRule type="expression" dxfId="55" priority="74">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I54">
+    <cfRule type="expression" dxfId="54" priority="73">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I61">
+    <cfRule type="expression" dxfId="53" priority="72">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I62">
+    <cfRule type="expression" dxfId="52" priority="71">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I66">
+    <cfRule type="expression" dxfId="51" priority="70">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H50">
+    <cfRule type="expression" dxfId="50" priority="63">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53">
+    <cfRule type="expression" dxfId="49" priority="62">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H55">
+    <cfRule type="expression" dxfId="48" priority="61">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H58">
+    <cfRule type="expression" dxfId="47" priority="60">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H54">
+    <cfRule type="expression" dxfId="46" priority="59">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H65">
+    <cfRule type="expression" dxfId="45" priority="58">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I65">
+    <cfRule type="expression" dxfId="44" priority="57">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H64">
+    <cfRule type="expression" dxfId="43" priority="56">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I64">
+    <cfRule type="expression" dxfId="42" priority="55">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H67">
+    <cfRule type="expression" dxfId="41" priority="54">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I67">
+    <cfRule type="expression" dxfId="40" priority="53">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F58">
+    <cfRule type="expression" dxfId="39" priority="49">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F61">
+    <cfRule type="expression" dxfId="38" priority="48">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F65">
+    <cfRule type="expression" dxfId="37" priority="47">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F50">
+    <cfRule type="expression" dxfId="36" priority="43">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55:F55">
+    <cfRule type="expression" dxfId="35" priority="42">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53:F53">
+    <cfRule type="expression" dxfId="34" priority="41">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64:F64">
+    <cfRule type="expression" dxfId="33" priority="40">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43:B44 E43:V44">
+    <cfRule type="expression" dxfId="32" priority="39">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:V49 G49">
+    <cfRule type="expression" dxfId="31" priority="37">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49 J49:V49">
+    <cfRule type="expression" dxfId="30" priority="35">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49">
+    <cfRule type="expression" dxfId="29" priority="34">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I49">
+    <cfRule type="expression" dxfId="28" priority="33">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H49">
+    <cfRule type="expression" dxfId="27" priority="32">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F49">
+    <cfRule type="expression" dxfId="26" priority="31">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:V22">
+    <cfRule type="expression" dxfId="25" priority="151">
+      <formula>K$1=#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:V22">
+    <cfRule type="expression" dxfId="24" priority="30">
+      <formula>K$1=$H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48:V48">
+    <cfRule type="expression" dxfId="23" priority="28">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J48:V48">
+    <cfRule type="expression" dxfId="22" priority="27">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="59" priority="77">
+    <cfRule type="expression" dxfId="21" priority="26">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I51">
-    <cfRule type="expression" dxfId="58" priority="76">
+  <conditionalFormatting sqref="H48">
+    <cfRule type="expression" dxfId="20" priority="25">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I53">
-    <cfRule type="expression" dxfId="57" priority="75">
+  <conditionalFormatting sqref="B22 G22">
+    <cfRule type="expression" dxfId="19" priority="21">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I56">
-    <cfRule type="expression" dxfId="56" priority="74">
+  <conditionalFormatting sqref="H23:V23">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I52">
-    <cfRule type="expression" dxfId="55" priority="73">
+  <conditionalFormatting sqref="K23:V23">
+    <cfRule type="expression" dxfId="17" priority="20">
+      <formula>K$1=#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23:V23">
+    <cfRule type="expression" dxfId="16" priority="18">
+      <formula>K$1=$H23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23 E23:G23">
+    <cfRule type="expression" dxfId="15" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I59">
-    <cfRule type="expression" dxfId="54" priority="72">
+  <conditionalFormatting sqref="E22:F22">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:G2 C4:D4 C6:D6 C10:D10 C14:D14 C18:D18 C22:D22 C26:D26 C30:D30 C34:D34 C38:D38 C42:D42 C46:D46 C50:D50 C54:D54 C58:D58 C62:D62 C66:D66 C8:D8 C12:D12 C16:D16 C20:D20 C24:D24 C28:D28 C32:D32 C36:D36 C40:D40 C44:D44 C48:D48 C52:D52 C56:D56 C60:D60 C64:D64">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B60 E60:F60">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K60:V60">
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>K$1=$H60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K60:V60">
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J60:V60">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H60">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I60">
-    <cfRule type="expression" dxfId="53" priority="71">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I64">
-    <cfRule type="expression" dxfId="52" priority="70">
+  <conditionalFormatting sqref="B63 E63:F63">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
-    <cfRule type="expression" dxfId="51" priority="63">
+  <conditionalFormatting sqref="K63:V63">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>K$1=$H63</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63:V63">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
-    <cfRule type="expression" dxfId="50" priority="62">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H53">
-    <cfRule type="expression" dxfId="49" priority="61">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H56">
-    <cfRule type="expression" dxfId="48" priority="60">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H52">
-    <cfRule type="expression" dxfId="47" priority="59">
+  <conditionalFormatting sqref="J63:V63">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="46" priority="58">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="45" priority="57">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H62">
-    <cfRule type="expression" dxfId="44" priority="56">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I62">
-    <cfRule type="expression" dxfId="43" priority="55">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H65">
-    <cfRule type="expression" dxfId="42" priority="54">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
-    <cfRule type="expression" dxfId="41" priority="53">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F56">
-    <cfRule type="expression" dxfId="40" priority="49">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F59">
-    <cfRule type="expression" dxfId="39" priority="48">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F63">
-    <cfRule type="expression" dxfId="38" priority="47">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48">
-    <cfRule type="expression" dxfId="37" priority="43">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53:F53">
-    <cfRule type="expression" dxfId="36" priority="42">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51:F51">
-    <cfRule type="expression" dxfId="35" priority="41">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E62:F62">
-    <cfRule type="expression" dxfId="34" priority="40">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B42 E42:V42">
-    <cfRule type="expression" dxfId="33" priority="39">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K47:V47 G47">
-    <cfRule type="expression" dxfId="32" priority="37">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47 J47:V47">
-    <cfRule type="expression" dxfId="31" priority="35">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="30" priority="34">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="29" priority="33">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
-    <cfRule type="expression" dxfId="28" priority="32">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
-    <cfRule type="expression" dxfId="27" priority="31">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:V22">
-    <cfRule type="expression" dxfId="26" priority="151">
-      <formula>K$1=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:V22">
-    <cfRule type="expression" dxfId="25" priority="30">
-      <formula>K$1=$H21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K46:V46">
-    <cfRule type="expression" dxfId="24" priority="28">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J46:V46">
-    <cfRule type="expression" dxfId="23" priority="27">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="22" priority="26">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H46">
-    <cfRule type="expression" dxfId="21" priority="25">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22 G22">
-    <cfRule type="expression" dxfId="20" priority="21">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23:V23">
-    <cfRule type="expression" dxfId="19" priority="19">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23:V23">
-    <cfRule type="expression" dxfId="18" priority="20">
-      <formula>K$1=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23:V23">
-    <cfRule type="expression" dxfId="17" priority="18">
-      <formula>K$1=$H23</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23 E23:G23">
-    <cfRule type="expression" dxfId="16" priority="17">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22:F22">
-    <cfRule type="expression" dxfId="15" priority="15">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G2 C4:D4 C6:D6 C8:D8 C10:D10 C12:D12 C14:D14 C16:D16 C18:D18 C20:D20 C22:D22 C24:D24 C26:D26 C28:D28 C30:D30 C32:D32 C34:D34 C36:D36 C38:D38 C40:D40 C42:D42 C44:D44 C46:D46 C48:D48 C50:D50 C52:D52 C54:D54 C56:D56 C58:D58 C60:D60 C62:D62 C64:D64">
-    <cfRule type="expression" dxfId="14" priority="14">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B58 E58:F58">
-    <cfRule type="expression" dxfId="13" priority="13">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K58:V58">
-    <cfRule type="expression" dxfId="12" priority="11">
-      <formula>K$1=$H58</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K58:V58">
-    <cfRule type="expression" dxfId="11" priority="12">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J58:V58">
-    <cfRule type="expression" dxfId="10" priority="10">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H58">
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I58">
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B61 E61:F61">
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K61:V61">
-    <cfRule type="expression" dxfId="6" priority="5">
-      <formula>K$1=$H61</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K61:V61">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J61:V61">
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H61">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I61">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add missing timezone information
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A610C41-8320-6048-B83D-80FE8AA8568C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94286119-903C-FE45-99F4-88D2AACF153D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16900" yWindow="7800" windowWidth="23920" windowHeight="18280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="203">
   <si>
     <t>Name</t>
   </si>
@@ -1118,7 +1118,22 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="81">
+  <dxfs count="83">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF920000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2012,8 +2027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4467,21 +4482,63 @@
         <v>195</v>
       </c>
       <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="24"/>
-      <c r="S32" s="24"/>
-      <c r="T32" s="24"/>
-      <c r="U32" s="24"/>
-      <c r="V32" s="24"/>
+      <c r="H32" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="17">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="J32" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="K32" s="26">
+        <f>$I32+Sheet2!B$1/24</f>
+        <v>1.25</v>
+      </c>
+      <c r="L32" s="24">
+        <f>$I32+Sheet2!B$2/24</f>
+        <v>1.2083333333333335</v>
+      </c>
+      <c r="M32" s="24">
+        <f>$I32+Sheet2!B$3/24</f>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="N32" s="24">
+        <f>$I32+Sheet2!B$4/24</f>
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="O32" s="24">
+        <f>$I32+Sheet2!B$5/24</f>
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="P32" s="24">
+        <f>$I32+Sheet2!B$6/24</f>
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="Q32" s="24">
+        <f>$I32+Sheet2!B$7/24</f>
+        <v>0.91666666666666674</v>
+      </c>
+      <c r="R32" s="24">
+        <f>$I32+Sheet2!B$8/24</f>
+        <v>0.875</v>
+      </c>
+      <c r="S32" s="24">
+        <f>$I32+Sheet2!B$9/24</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="T32" s="24">
+        <f>$I32+Sheet2!B$10/24</f>
+        <v>0.625</v>
+      </c>
+      <c r="U32" s="24">
+        <f>$I32+Sheet2!B$11/24</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="V32" s="24">
+        <f>$I32+Sheet2!B$12/24</f>
+        <v>0.54166666666666674</v>
+      </c>
     </row>
     <row r="33" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="53"/>
@@ -4655,21 +4712,63 @@
         <v>191</v>
       </c>
       <c r="G35" s="36"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="24"/>
-      <c r="O35" s="24"/>
-      <c r="P35" s="24"/>
-      <c r="Q35" s="24"/>
-      <c r="R35" s="24"/>
-      <c r="S35" s="24"/>
-      <c r="T35" s="24"/>
-      <c r="U35" s="24"/>
-      <c r="V35" s="24"/>
+      <c r="H35" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="17">
+        <v>0.875</v>
+      </c>
+      <c r="J35" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35" s="26">
+        <f>$I35+Sheet2!B$1/24</f>
+        <v>1.2916666666666667</v>
+      </c>
+      <c r="L35" s="24">
+        <f>$I35+Sheet2!B$2/24</f>
+        <v>1.25</v>
+      </c>
+      <c r="M35" s="24">
+        <f>$I35+Sheet2!B$3/24</f>
+        <v>1.2083333333333333</v>
+      </c>
+      <c r="N35" s="24">
+        <f>$I35+Sheet2!B$4/24</f>
+        <v>1</v>
+      </c>
+      <c r="O35" s="24">
+        <f>$I35+Sheet2!B$5/24</f>
+        <v>1</v>
+      </c>
+      <c r="P35" s="24">
+        <f>$I35+Sheet2!B$6/24</f>
+        <v>1</v>
+      </c>
+      <c r="Q35" s="24">
+        <f>$I35+Sheet2!B$7/24</f>
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="R35" s="24">
+        <f>$I35+Sheet2!B$8/24</f>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="S35" s="24">
+        <f>$I35+Sheet2!B$9/24</f>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="T35" s="24">
+        <f>$I35+Sheet2!B$10/24</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="U35" s="24">
+        <f>$I35+Sheet2!B$11/24</f>
+        <v>0.625</v>
+      </c>
+      <c r="V35" s="24">
+        <f>$I35+Sheet2!B$12/24</f>
+        <v>0.58333333333333326</v>
+      </c>
     </row>
     <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="55" t="s">
@@ -7583,407 +7682,417 @@
     <mergeCell ref="A10:A34"/>
     <mergeCell ref="A36:A75"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L8 K66:V67 K69:V72 K25:V32 K34:V64 K6:V21">
-    <cfRule type="expression" dxfId="80" priority="143">
+  <conditionalFormatting sqref="K2:L8 K66:V67 K69:V72 K25:V31 K6:V21 K34:V64">
+    <cfRule type="expression" dxfId="82" priority="145">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V8">
-    <cfRule type="expression" dxfId="79" priority="145">
+    <cfRule type="expression" dxfId="81" priority="147">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K39:V39 G46:V46 G39 B49:B52 K54:V54 G54 B55:B57 K58:V60 G58:G60 B61:B62 K63:V63 G63 G72 K66:V67 E61:V62 E49:V51 E40:V45 E52:G52 B25:B32 H23:V23 H2:V2 B3:V3 G65:G70 K69:V72 E19:V22 G18:V18 B4:B22 B64 E25:V32 G56:V57 E34:V38 B34:B46 E4:V17 E64:V64 C5:D5 C7:D7 C9:D9 C11:D11 C13:D13 C15:D15 C17:D17 C19:D19 C21:D21 C23:D23 C25:D25 C27:D27 C29:D29 C31:D31 C33:D33 C35:D35 C37:D37 C39:D39 C41:D41 C43:D43 C45:D45 C47:D47 C49:D49 C51:D51 C53:D53 C55:V55 C57:D57 C59:D59 C61:D61 C63:D63 C65:D65 C67:D67 C69:D69 C71:D71">
-    <cfRule type="expression" dxfId="78" priority="149">
+  <conditionalFormatting sqref="K39:V39 G46:V46 G39 B49:B52 K54:V54 G54 B55:B57 K58:V60 G58:G60 B61:B62 K63:V63 G63 G72 K66:V67 E61:V62 E49:V51 E40:V45 E52:G52 B25:B32 H23:V23 H2:V2 B3:V3 G65:G70 K69:V72 E19:V22 G18:V18 B4:B22 B64 E25:V31 G56:V57 B34:B46 E4:V17 E64:V64 C5:D5 C7:D7 C9:D9 C11:D11 C13:D13 C15:D15 C17:D17 C19:D19 C21:D21 C23:D23 C25:D25 C27:D27 C29:D29 C31:D31 C33:D33 C35:D35 C37:D37 C39:D39 C41:D41 C43:D43 C45:D45 C47:D47 C49:D49 C51:D51 C53:D53 C55:V55 C57:D57 C59:D59 C61:D61 C63:D63 C65:D65 C67:D67 C69:D69 C71:D71 E34:V38 E32:G32">
+    <cfRule type="expression" dxfId="80" priority="151">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54 J54:V54">
-    <cfRule type="expression" dxfId="77" priority="126">
+    <cfRule type="expression" dxfId="79" priority="128">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58 J58:V58">
-    <cfRule type="expression" dxfId="76" priority="124">
+    <cfRule type="expression" dxfId="78" priority="126">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60 J60:V60">
-    <cfRule type="expression" dxfId="75" priority="122">
+    <cfRule type="expression" dxfId="77" priority="124">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63 J63:V63">
-    <cfRule type="expression" dxfId="74" priority="120">
+    <cfRule type="expression" dxfId="76" priority="122">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59 J59:V59">
-    <cfRule type="expression" dxfId="73" priority="118">
+    <cfRule type="expression" dxfId="75" priority="120">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66 J66:V66">
-    <cfRule type="expression" dxfId="72" priority="116">
+    <cfRule type="expression" dxfId="74" priority="118">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67 J67:V67 E67:F67 H67">
-    <cfRule type="expression" dxfId="71" priority="114">
+    <cfRule type="expression" dxfId="73" priority="116">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54">
-    <cfRule type="expression" dxfId="70" priority="112">
+    <cfRule type="expression" dxfId="72" priority="114">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
+    <cfRule type="expression" dxfId="71" priority="111">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
+    <cfRule type="expression" dxfId="70" priority="110">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66 H66">
     <cfRule type="expression" dxfId="69" priority="109">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E59">
-    <cfRule type="expression" dxfId="68" priority="108">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66 H66">
-    <cfRule type="expression" dxfId="67" priority="107">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B71 J71:V71">
-    <cfRule type="expression" dxfId="66" priority="105">
+    <cfRule type="expression" dxfId="68" priority="107">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70 J70:V70 E70">
-    <cfRule type="expression" dxfId="65" priority="103">
+    <cfRule type="expression" dxfId="67" priority="105">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E71:F71 H71">
-    <cfRule type="expression" dxfId="64" priority="101">
+    <cfRule type="expression" dxfId="66" priority="103">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69 J69:V69">
-    <cfRule type="expression" dxfId="63" priority="99">
+    <cfRule type="expression" dxfId="65" priority="101">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72 J72:V72 E72">
-    <cfRule type="expression" dxfId="62" priority="97">
+    <cfRule type="expression" dxfId="64" priority="99">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59">
-    <cfRule type="expression" dxfId="61" priority="89">
+    <cfRule type="expression" dxfId="63" priority="91">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54">
+    <cfRule type="expression" dxfId="62" priority="81">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I58">
+    <cfRule type="expression" dxfId="61" priority="80">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I60">
     <cfRule type="expression" dxfId="60" priority="79">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I58">
+  <conditionalFormatting sqref="I63">
     <cfRule type="expression" dxfId="59" priority="78">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I60">
+  <conditionalFormatting sqref="I59">
     <cfRule type="expression" dxfId="58" priority="77">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I63">
+  <conditionalFormatting sqref="I66">
     <cfRule type="expression" dxfId="57" priority="76">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I59">
+  <conditionalFormatting sqref="I67">
     <cfRule type="expression" dxfId="56" priority="75">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I66">
+  <conditionalFormatting sqref="I71">
     <cfRule type="expression" dxfId="55" priority="74">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I67">
-    <cfRule type="expression" dxfId="54" priority="73">
+  <conditionalFormatting sqref="H54">
+    <cfRule type="expression" dxfId="54" priority="67">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I71">
-    <cfRule type="expression" dxfId="53" priority="72">
+  <conditionalFormatting sqref="H58">
+    <cfRule type="expression" dxfId="53" priority="66">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H54">
+  <conditionalFormatting sqref="H60">
     <cfRule type="expression" dxfId="52" priority="65">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H58">
+  <conditionalFormatting sqref="H63">
     <cfRule type="expression" dxfId="51" priority="64">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H60">
+  <conditionalFormatting sqref="H59">
     <cfRule type="expression" dxfId="50" priority="63">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H63">
+  <conditionalFormatting sqref="H70">
     <cfRule type="expression" dxfId="49" priority="62">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H59">
+  <conditionalFormatting sqref="I70">
     <cfRule type="expression" dxfId="48" priority="61">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H70">
+  <conditionalFormatting sqref="H69">
     <cfRule type="expression" dxfId="47" priority="60">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I70">
+  <conditionalFormatting sqref="I69">
     <cfRule type="expression" dxfId="46" priority="59">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H69">
+  <conditionalFormatting sqref="H72">
     <cfRule type="expression" dxfId="45" priority="58">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I69">
+  <conditionalFormatting sqref="I72">
     <cfRule type="expression" dxfId="44" priority="57">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H72">
-    <cfRule type="expression" dxfId="43" priority="56">
+  <conditionalFormatting sqref="F63">
+    <cfRule type="expression" dxfId="43" priority="53">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I72">
-    <cfRule type="expression" dxfId="42" priority="55">
+  <conditionalFormatting sqref="F66">
+    <cfRule type="expression" dxfId="42" priority="52">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F63">
+  <conditionalFormatting sqref="F70">
     <cfRule type="expression" dxfId="41" priority="51">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F66">
-    <cfRule type="expression" dxfId="40" priority="50">
+  <conditionalFormatting sqref="F54">
+    <cfRule type="expression" dxfId="40" priority="47">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F70">
-    <cfRule type="expression" dxfId="39" priority="49">
+  <conditionalFormatting sqref="E60:F60">
+    <cfRule type="expression" dxfId="39" priority="46">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F54">
+  <conditionalFormatting sqref="E58:F58">
     <cfRule type="expression" dxfId="38" priority="45">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E60:F60">
+  <conditionalFormatting sqref="E69:F69">
     <cfRule type="expression" dxfId="37" priority="44">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E58:F58">
+  <conditionalFormatting sqref="B47:B48 E47:V48">
     <cfRule type="expression" dxfId="36" priority="43">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69:F69">
-    <cfRule type="expression" dxfId="35" priority="42">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47:B48 E47:V48">
-    <cfRule type="expression" dxfId="34" priority="41">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K53:V53 G53">
-    <cfRule type="expression" dxfId="33" priority="39">
+    <cfRule type="expression" dxfId="35" priority="41">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53 J53:V53">
+    <cfRule type="expression" dxfId="34" priority="39">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule type="expression" dxfId="33" priority="38">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I53">
     <cfRule type="expression" dxfId="32" priority="37">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
+  <conditionalFormatting sqref="H53">
     <cfRule type="expression" dxfId="31" priority="36">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I53">
+  <conditionalFormatting sqref="F53">
     <cfRule type="expression" dxfId="30" priority="35">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H53">
-    <cfRule type="expression" dxfId="29" priority="34">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F53">
-    <cfRule type="expression" dxfId="28" priority="33">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K22:V23">
-    <cfRule type="expression" dxfId="27" priority="153">
+    <cfRule type="expression" dxfId="29" priority="155">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:V23">
-    <cfRule type="expression" dxfId="26" priority="32">
+    <cfRule type="expression" dxfId="28" priority="34">
       <formula>K$1=$H22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:V52">
+    <cfRule type="expression" dxfId="27" priority="32">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J52:V52">
+    <cfRule type="expression" dxfId="26" priority="31">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I52">
     <cfRule type="expression" dxfId="25" priority="30">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J52:V52">
+  <conditionalFormatting sqref="H52">
     <cfRule type="expression" dxfId="24" priority="29">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I52">
-    <cfRule type="expression" dxfId="23" priority="28">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H52">
-    <cfRule type="expression" dxfId="22" priority="27">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B23 G23">
-    <cfRule type="expression" dxfId="21" priority="23">
+    <cfRule type="expression" dxfId="23" priority="25">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:V24">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24:V24">
-    <cfRule type="expression" dxfId="19" priority="22">
+    <cfRule type="expression" dxfId="21" priority="24">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24:V24">
-    <cfRule type="expression" dxfId="18" priority="20">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>K$1=$H24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24 E24:G24">
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="19" priority="21">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:F23">
+    <cfRule type="expression" dxfId="18" priority="19">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:G2 C4:D4 C6:D6 C8:D8 C10:D10 C12:D12 C14:D14 C16:D16 C18:D18 C20:D20 C22:D22 C24:D24 C26:D26 C28:D28 C30:D30 C32:D32 C34:D34 C36:D36 C38:D38 C40:D40 C42:D42 C44:D44 C46:D46 C48:D48 C50:D50 C52:D52 C54:D54 C56:D56 C58:D58 C60:D60 C62:D62 C64:D64 C66:D66 C68:D68 C70:D70 C72:D72">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B65 E65:F65">
     <cfRule type="expression" dxfId="16" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G2 C4:D4 C6:D6 C8:D8 C10:D10 C12:D12 C14:D14 C16:D16 C18:D18 C20:D20 C22:D22 C24:D24 C26:D26 C28:D28 C30:D30 C32:D32 C34:D34 C36:D36 C38:D38 C40:D40 C42:D42 C44:D44 C46:D46 C48:D48 C50:D50 C52:D52 C54:D54 C56:D56 C58:D58 C60:D60 C62:D62 C64:D64 C66:D66 C68:D68 C70:D70 C72:D72">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B65 E65:F65">
-    <cfRule type="expression" dxfId="14" priority="15">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K65:V65">
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="15" priority="15">
       <formula>K$1=$H65</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65:V65">
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J65:V65">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H65">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I65">
     <cfRule type="expression" dxfId="11" priority="12">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H65">
+  <conditionalFormatting sqref="B68 E68:F68">
     <cfRule type="expression" dxfId="10" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B68 E68:F68">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K68:V68">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>K$1=$H68</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68:V68">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68:V68">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H68">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I68">
     <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H68">
+  <conditionalFormatting sqref="E18:F18">
     <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I68">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:F18">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K33:V33">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>K$1=$H33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33 E33:V33">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32:V32">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>K$1=$H32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32:V32">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Move KoS Mistborn payout
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800F73B9-6512-AB4E-AE3B-ED118C47F080}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0853CFD5-61D2-A947-B2A1-9FC2C2693185}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20200" yWindow="1560" windowWidth="25720" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1177,7 +1177,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="261">
+  <dxfs count="259">
     <dxf>
       <fill>
         <patternFill>
@@ -1216,6 +1216,20 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
@@ -1238,6 +1252,27 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
@@ -1254,27 +1289,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
@@ -1286,36 +1300,6 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3338,8 +3322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3401,7 +3385,7 @@
         <v>9</v>
       </c>
       <c r="N1" s="3" t="str">
-        <f>H28</f>
+        <f>H27</f>
         <v>CET</v>
       </c>
       <c r="O1" s="3" t="str">
@@ -3409,15 +3393,15 @@
         <v>CXT</v>
       </c>
       <c r="P1" s="3" t="str">
-        <f>H20</f>
+        <f>H19</f>
         <v>EET</v>
       </c>
       <c r="Q1" s="3" t="str">
-        <f>H30</f>
+        <f>H29</f>
         <v>CET</v>
       </c>
       <c r="R1" s="3" t="str">
-        <f>H36</f>
+        <f>H35</f>
         <v>GMT</v>
       </c>
       <c r="S1" s="3" t="str">
@@ -4582,174 +4566,174 @@
       </c>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="49"/>
-      <c r="B17" s="18" t="s">
-        <v>31</v>
+      <c r="A17" s="43"/>
+      <c r="B17" s="36" t="s">
+        <v>207</v>
       </c>
       <c r="C17" s="7">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="D17" s="7">
-        <v>51</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>206</v>
+        <v>15</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="27" t="s">
+        <v>209</v>
       </c>
       <c r="I17" s="23">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="J17" s="24" t="s">
+        <v>0.625</v>
+      </c>
+      <c r="J17" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="25">
         <f>$I17+Sheet2!B$1/24</f>
-        <v>1</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="L17" s="23">
         <f>$I17+Sheet2!B$2/24</f>
-        <v>0.95833333333333337</v>
+        <v>1</v>
       </c>
       <c r="M17" s="23">
         <f>$I17+Sheet2!B$3/24</f>
-        <v>0.91666666666666674</v>
+        <v>0.95833333333333326</v>
       </c>
       <c r="N17" s="23">
         <f>$I17+Sheet2!B$4/24</f>
-        <v>0.70833333333333337</v>
+        <v>0.75</v>
       </c>
       <c r="O17" s="23">
         <f>$I17+Sheet2!B$5/24</f>
-        <v>0.70833333333333337</v>
+        <v>0.75</v>
       </c>
       <c r="P17" s="23">
         <f>$I17+Sheet2!B$6/24</f>
-        <v>0.70833333333333337</v>
+        <v>0.75</v>
       </c>
       <c r="Q17" s="23">
         <f>$I17+Sheet2!B$7/24</f>
-        <v>0.66666666666666674</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="R17" s="23">
         <f>$I17+Sheet2!B$8/24</f>
-        <v>0.625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S17" s="23">
         <f>$I17+Sheet2!B$9/24</f>
-        <v>0.41666666666666674</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="T17" s="23">
         <f>$I17+Sheet2!B$10/24</f>
-        <v>0.375</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="U17" s="23">
         <f>$I17+Sheet2!B$11/24</f>
-        <v>0.33333333333333337</v>
+        <v>0.375</v>
       </c>
       <c r="V17" s="23">
         <f>$I17+Sheet2!B$12/24</f>
-        <v>0.29166666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="43"/>
-      <c r="B18" s="36" t="s">
-        <v>207</v>
+      <c r="A18" s="47"/>
+      <c r="B18" s="18" t="s">
+        <v>210</v>
       </c>
       <c r="C18" s="7">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D18" s="7">
-        <v>15</v>
-      </c>
-      <c r="E18" s="8"/>
+        <v>17</v>
+      </c>
+      <c r="E18" s="20"/>
       <c r="F18" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="27" t="s">
-        <v>209</v>
+        <v>211</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>212</v>
       </c>
       <c r="I18" s="23">
-        <v>0.625</v>
-      </c>
-      <c r="J18" s="26" t="s">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J18" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="11">
         <f>$I18+Sheet2!B$1/24</f>
-        <v>1.0416666666666667</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="L18" s="23">
         <f>$I18+Sheet2!B$2/24</f>
-        <v>1</v>
+        <v>1.0416666666666665</v>
       </c>
       <c r="M18" s="23">
         <f>$I18+Sheet2!B$3/24</f>
-        <v>0.95833333333333326</v>
+        <v>1</v>
       </c>
       <c r="N18" s="23">
         <f>$I18+Sheet2!B$4/24</f>
-        <v>0.75</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="O18" s="23">
         <f>$I18+Sheet2!B$5/24</f>
-        <v>0.75</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="P18" s="23">
         <f>$I18+Sheet2!B$6/24</f>
-        <v>0.75</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="Q18" s="23">
         <f>$I18+Sheet2!B$7/24</f>
-        <v>0.70833333333333337</v>
+        <v>0.75</v>
       </c>
       <c r="R18" s="23">
         <f>$I18+Sheet2!B$8/24</f>
-        <v>0.66666666666666663</v>
+        <v>0.70833333333333326</v>
       </c>
       <c r="S18" s="23">
         <f>$I18+Sheet2!B$9/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="T18" s="23">
         <f>$I18+Sheet2!B$10/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.45833333333333326</v>
       </c>
       <c r="U18" s="23">
         <f>$I18+Sheet2!B$11/24</f>
-        <v>0.375</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="V18" s="23">
         <f>$I18+Sheet2!B$12/24</f>
-        <v>0.33333333333333331</v>
+        <v>0.37499999999999994</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="47"/>
       <c r="B19" s="18" t="s">
-        <v>210</v>
+        <v>41</v>
       </c>
       <c r="C19" s="7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D19" s="7">
-        <v>17</v>
-      </c>
-      <c r="E19" s="20"/>
+        <v>18</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>19</v>
+      </c>
       <c r="F19" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>104</v>
+        <v>81</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="H19" s="29" t="s">
         <v>212</v>
@@ -4812,22 +4796,22 @@
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="47"/>
       <c r="B20" s="18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C20" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D20" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>137</v>
+        <v>72</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>145</v>
       </c>
       <c r="H20" s="29" t="s">
         <v>212</v>
@@ -4888,100 +4872,100 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="47"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="18" t="s">
-        <v>43</v>
+        <v>185</v>
       </c>
       <c r="C21" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D21" s="7">
-        <v>19</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>71</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E21" s="20"/>
       <c r="F21" s="7" t="s">
-        <v>72</v>
+        <v>213</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>145</v>
+        <v>104</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I21" s="23">
-        <v>0.66666666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="J21" s="30" t="s">
         <v>14</v>
       </c>
       <c r="K21" s="11">
         <f>$I21+Sheet2!B$1/24</f>
-        <v>1.0833333333333333</v>
+        <v>1.125</v>
       </c>
       <c r="L21" s="23">
         <f>$I21+Sheet2!B$2/24</f>
-        <v>1.0416666666666665</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="M21" s="23">
         <f>$I21+Sheet2!B$3/24</f>
-        <v>1</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="N21" s="23">
         <f>$I21+Sheet2!B$4/24</f>
-        <v>0.79166666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="O21" s="23">
         <f>$I21+Sheet2!B$5/24</f>
-        <v>0.79166666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="P21" s="23">
         <f>$I21+Sheet2!B$6/24</f>
-        <v>0.79166666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="Q21" s="23">
         <f>$I21+Sheet2!B$7/24</f>
-        <v>0.75</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="R21" s="23">
         <f>$I21+Sheet2!B$8/24</f>
-        <v>0.70833333333333326</v>
+        <v>0.75</v>
       </c>
       <c r="S21" s="23">
         <f>$I21+Sheet2!B$9/24</f>
-        <v>0.5</v>
+        <v>0.54166666666666674</v>
       </c>
       <c r="T21" s="23">
         <f>$I21+Sheet2!B$10/24</f>
-        <v>0.45833333333333326</v>
+        <v>0.5</v>
       </c>
       <c r="U21" s="23">
         <f>$I21+Sheet2!B$11/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="V21" s="23">
         <f>$I21+Sheet2!B$12/24</f>
-        <v>0.37499999999999994</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="18" t="s">
-        <v>185</v>
+        <v>50</v>
       </c>
       <c r="C22" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D22" s="7">
-        <v>20</v>
-      </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="7" t="s">
-        <v>213</v>
+        <v>21</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="H22" s="29" t="s">
         <v>214</v>
@@ -5041,25 +5025,25 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="41"/>
+    <row r="23" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="50" t="s">
+        <v>26</v>
+      </c>
       <c r="B23" s="18" t="s">
-        <v>50</v>
+        <v>190</v>
       </c>
       <c r="C23" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D23" s="7">
-        <v>21</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>19</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E23" s="20"/>
       <c r="F23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="29" t="s">
-        <v>134</v>
+      <c r="G23" s="48" t="s">
+        <v>191</v>
       </c>
       <c r="H23" s="29" t="s">
         <v>214</v>
@@ -5074,70 +5058,70 @@
         <f>$I23+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L23" s="23">
+      <c r="L23" s="16">
         <f>$I23+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M23" s="23">
+      <c r="M23" s="16">
         <f>$I23+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N23" s="23">
+      <c r="N23" s="16">
         <f>$I23+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O23" s="23">
+      <c r="O23" s="16">
         <f>$I23+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P23" s="23">
+      <c r="P23" s="16">
         <f>$I23+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q23" s="23">
+      <c r="Q23" s="16">
         <f>$I23+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R23" s="23">
+      <c r="R23" s="16">
         <f>$I23+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S23" s="23">
+      <c r="S23" s="16">
         <f>$I23+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T23" s="23">
+      <c r="T23" s="16">
         <f>$I23+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U23" s="23">
+      <c r="U23" s="16">
         <f>$I23+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V23" s="23">
+      <c r="V23" s="16">
         <f>$I23+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="50" t="s">
-        <v>26</v>
-      </c>
+      <c r="A24" s="50"/>
       <c r="B24" s="18" t="s">
-        <v>190</v>
+        <v>114</v>
       </c>
       <c r="C24" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D24" s="7">
-        <v>22</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G24" s="48" t="s">
-        <v>191</v>
+        <v>23</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>117</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>214</v>
@@ -5200,22 +5184,22 @@
     <row r="25" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="50"/>
       <c r="B25" s="18" t="s">
-        <v>114</v>
+        <v>49</v>
       </c>
       <c r="C25" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D25" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>117</v>
+        <v>15</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="44" t="s">
+        <v>138</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>214</v>
@@ -5230,47 +5214,47 @@
         <f>$I25+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L25" s="16">
+      <c r="L25" s="23">
         <f>$I25+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M25" s="16">
+      <c r="M25" s="23">
         <f>$I25+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N25" s="16">
+      <c r="N25" s="23">
         <f>$I25+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O25" s="16">
+      <c r="O25" s="23">
         <f>$I25+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P25" s="16">
+      <c r="P25" s="23">
         <f>$I25+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q25" s="16">
+      <c r="Q25" s="23">
         <f>$I25+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R25" s="16">
+      <c r="R25" s="23">
         <f>$I25+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S25" s="16">
+      <c r="S25" s="23">
         <f>$I25+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T25" s="16">
+      <c r="T25" s="23">
         <f>$I25+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U25" s="16">
+      <c r="U25" s="23">
         <f>$I25+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V25" s="16">
+      <c r="V25" s="23">
         <f>$I25+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
@@ -5278,22 +5262,22 @@
     <row r="26" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="50"/>
       <c r="B26" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D26" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G26" s="44" t="s">
-        <v>138</v>
+      <c r="G26" s="29" t="s">
+        <v>139</v>
       </c>
       <c r="H26" s="29" t="s">
         <v>214</v>
@@ -5356,22 +5340,22 @@
     <row r="27" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="50"/>
       <c r="B27" s="18" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C27" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D27" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" s="29" t="s">
-        <v>139</v>
+        <v>76</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="H27" s="29" t="s">
         <v>214</v>
@@ -5434,22 +5418,22 @@
     <row r="28" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="50"/>
       <c r="B28" s="18" t="s">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="C28" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D28" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="21" t="s">
-        <v>140</v>
+        <v>72</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="H28" s="29" t="s">
         <v>214</v>
@@ -5511,23 +5495,23 @@
     </row>
     <row r="29" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="50"/>
-      <c r="B29" s="18" t="s">
-        <v>125</v>
+      <c r="B29" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="C29" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D29" s="7">
-        <v>27</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>71</v>
+        <v>28</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>126</v>
+        <v>70</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>141</v>
       </c>
       <c r="H29" s="29" t="s">
         <v>214</v>
@@ -5542,70 +5526,70 @@
         <f>$I29+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L29" s="23">
+      <c r="L29" s="16">
         <f>$I29+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M29" s="23">
+      <c r="M29" s="16">
         <f>$I29+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N29" s="23">
+      <c r="N29" s="16">
         <f>$I29+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O29" s="23">
+      <c r="O29" s="16">
         <f>$I29+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P29" s="23">
+      <c r="P29" s="16">
         <f>$I29+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q29" s="23">
+      <c r="Q29" s="16">
         <f>$I29+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R29" s="23">
+      <c r="R29" s="16">
         <f>$I29+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S29" s="23">
+      <c r="S29" s="16">
         <f>$I29+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T29" s="23">
+      <c r="T29" s="16">
         <f>$I29+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U29" s="23">
+      <c r="U29" s="16">
         <f>$I29+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V29" s="23">
+      <c r="V29" s="16">
         <f>$I29+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="50"/>
-      <c r="B30" s="12" t="s">
-        <v>42</v>
+      <c r="B30" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="C30" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D30" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F30" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" s="27" t="s">
-        <v>141</v>
+      <c r="F30" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>143</v>
       </c>
       <c r="H30" s="29" t="s">
         <v>214</v>
@@ -5620,145 +5604,145 @@
         <f>$I30+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L30" s="16">
+      <c r="L30" s="23">
         <f>$I30+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M30" s="16">
+      <c r="M30" s="23">
         <f>$I30+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N30" s="16">
+      <c r="N30" s="23">
         <f>$I30+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O30" s="16">
+      <c r="O30" s="23">
         <f>$I30+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P30" s="16">
+      <c r="P30" s="23">
         <f>$I30+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q30" s="16">
+      <c r="Q30" s="23">
         <f>$I30+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R30" s="16">
+      <c r="R30" s="23">
         <f>$I30+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S30" s="16">
+      <c r="S30" s="23">
         <f>$I30+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T30" s="16">
+      <c r="T30" s="23">
         <f>$I30+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U30" s="16">
+      <c r="U30" s="23">
         <f>$I30+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V30" s="16">
+      <c r="V30" s="23">
         <f>$I30+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="50"/>
       <c r="B31" s="18" t="s">
-        <v>46</v>
+        <v>215</v>
       </c>
       <c r="C31" s="7">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D31" s="7">
-        <v>29</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G31" s="29" t="s">
-        <v>143</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E31" s="20"/>
+      <c r="F31" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="G31" s="29"/>
       <c r="H31" s="29" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="I31" s="23">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="J31" s="30" t="s">
+        <v>0.75</v>
+      </c>
+      <c r="J31" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K31" s="11">
+      <c r="K31" s="25">
         <f>$I31+Sheet2!B$1/24</f>
-        <v>1.125</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="L31" s="23">
         <f>$I31+Sheet2!B$2/24</f>
-        <v>1.0833333333333335</v>
+        <v>1.125</v>
       </c>
       <c r="M31" s="23">
         <f>$I31+Sheet2!B$3/24</f>
-        <v>1.0416666666666667</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="N31" s="23">
         <f>$I31+Sheet2!B$4/24</f>
-        <v>0.83333333333333337</v>
+        <v>0.875</v>
       </c>
       <c r="O31" s="23">
         <f>$I31+Sheet2!B$5/24</f>
-        <v>0.83333333333333337</v>
+        <v>0.875</v>
       </c>
       <c r="P31" s="23">
         <f>$I31+Sheet2!B$6/24</f>
-        <v>0.83333333333333337</v>
+        <v>0.875</v>
       </c>
       <c r="Q31" s="23">
         <f>$I31+Sheet2!B$7/24</f>
-        <v>0.79166666666666674</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="R31" s="23">
         <f>$I31+Sheet2!B$8/24</f>
-        <v>0.75</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="S31" s="23">
         <f>$I31+Sheet2!B$9/24</f>
-        <v>0.54166666666666674</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="T31" s="23">
         <f>$I31+Sheet2!B$10/24</f>
-        <v>0.5</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="U31" s="23">
         <f>$I31+Sheet2!B$11/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="V31" s="23">
         <f>$I31+Sheet2!B$12/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="50"/>
       <c r="B32" s="18" t="s">
-        <v>215</v>
+        <v>130</v>
       </c>
       <c r="C32" s="7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D32" s="7">
-        <v>31</v>
-      </c>
-      <c r="E32" s="20"/>
+        <v>32</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>115</v>
+      </c>
       <c r="F32" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="G32" s="29"/>
+        <v>116</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>131</v>
+      </c>
       <c r="H32" s="29" t="s">
         <v>217</v>
       </c>
@@ -5820,22 +5804,22 @@
     <row r="33" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="50"/>
       <c r="B33" s="18" t="s">
-        <v>130</v>
+        <v>53</v>
       </c>
       <c r="C33" s="7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D33" s="7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>115</v>
+        <v>28</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="G33" s="29" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="H33" s="29" t="s">
         <v>217</v>
@@ -5897,23 +5881,23 @@
     </row>
     <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="50"/>
-      <c r="B34" s="18" t="s">
-        <v>53</v>
+      <c r="B34" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="C34" s="7">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D34" s="7">
-        <v>33</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G34" s="29" t="s">
-        <v>146</v>
+        <v>34</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="27" t="s">
+        <v>147</v>
       </c>
       <c r="H34" s="29" t="s">
         <v>217</v>
@@ -5921,77 +5905,77 @@
       <c r="I34" s="23">
         <v>0.75</v>
       </c>
-      <c r="J34" s="26" t="s">
+      <c r="J34" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="K34" s="25">
+      <c r="K34" s="31">
         <f>$I34+Sheet2!B$1/24</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L34" s="23">
+      <c r="L34" s="16">
         <f>$I34+Sheet2!B$2/24</f>
         <v>1.125</v>
       </c>
-      <c r="M34" s="23">
+      <c r="M34" s="16">
         <f>$I34+Sheet2!B$3/24</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="N34" s="23">
+      <c r="N34" s="16">
         <f>$I34+Sheet2!B$4/24</f>
         <v>0.875</v>
       </c>
-      <c r="O34" s="23">
+      <c r="O34" s="16">
         <f>$I34+Sheet2!B$5/24</f>
         <v>0.875</v>
       </c>
-      <c r="P34" s="23">
+      <c r="P34" s="16">
         <f>$I34+Sheet2!B$6/24</f>
         <v>0.875</v>
       </c>
-      <c r="Q34" s="23">
+      <c r="Q34" s="16">
         <f>$I34+Sheet2!B$7/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R34" s="23">
+      <c r="R34" s="16">
         <f>$I34+Sheet2!B$8/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="S34" s="23">
+      <c r="S34" s="16">
         <f>$I34+Sheet2!B$9/24</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="T34" s="23">
+      <c r="T34" s="16">
         <f>$I34+Sheet2!B$10/24</f>
         <v>0.54166666666666663</v>
       </c>
-      <c r="U34" s="23">
+      <c r="U34" s="16">
         <f>$I34+Sheet2!B$11/24</f>
         <v>0.5</v>
       </c>
-      <c r="V34" s="23">
+      <c r="V34" s="16">
         <f>$I34+Sheet2!B$12/24</f>
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="50"/>
-      <c r="B35" s="12" t="s">
-        <v>51</v>
+      <c r="B35" s="32" t="s">
+        <v>82</v>
       </c>
       <c r="C35" s="7">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D35" s="7">
-        <v>34</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="27" t="s">
-        <v>147</v>
+        <v>35</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>148</v>
       </c>
       <c r="H35" s="29" t="s">
         <v>217</v>
@@ -5999,77 +5983,77 @@
       <c r="I35" s="23">
         <v>0.75</v>
       </c>
-      <c r="J35" s="28" t="s">
+      <c r="J35" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K35" s="31">
+      <c r="K35" s="25">
         <f>$I35+Sheet2!B$1/24</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="L35" s="16">
+      <c r="L35" s="23">
         <f>$I35+Sheet2!B$2/24</f>
         <v>1.125</v>
       </c>
-      <c r="M35" s="16">
+      <c r="M35" s="23">
         <f>$I35+Sheet2!B$3/24</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="N35" s="16">
+      <c r="N35" s="23">
         <f>$I35+Sheet2!B$4/24</f>
         <v>0.875</v>
       </c>
-      <c r="O35" s="16">
+      <c r="O35" s="23">
         <f>$I35+Sheet2!B$5/24</f>
         <v>0.875</v>
       </c>
-      <c r="P35" s="16">
+      <c r="P35" s="23">
         <f>$I35+Sheet2!B$6/24</f>
         <v>0.875</v>
       </c>
-      <c r="Q35" s="16">
+      <c r="Q35" s="23">
         <f>$I35+Sheet2!B$7/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R35" s="16">
+      <c r="R35" s="23">
         <f>$I35+Sheet2!B$8/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="S35" s="16">
+      <c r="S35" s="23">
         <f>$I35+Sheet2!B$9/24</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="T35" s="16">
+      <c r="T35" s="23">
         <f>$I35+Sheet2!B$10/24</f>
         <v>0.54166666666666663</v>
       </c>
-      <c r="U35" s="16">
+      <c r="U35" s="23">
         <f>$I35+Sheet2!B$11/24</f>
         <v>0.5</v>
       </c>
-      <c r="V35" s="16">
+      <c r="V35" s="23">
         <f>$I35+Sheet2!B$12/24</f>
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="50"/>
-      <c r="B36" s="32" t="s">
-        <v>82</v>
+      <c r="B36" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="C36" s="7">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D36" s="7">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G36" s="34" t="s">
-        <v>148</v>
+        <v>89</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>149</v>
       </c>
       <c r="H36" s="29" t="s">
         <v>217</v>
@@ -6132,171 +6116,171 @@
     <row r="37" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="50"/>
       <c r="B37" s="18" t="s">
-        <v>52</v>
+        <v>218</v>
       </c>
       <c r="C37" s="7">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D37" s="7">
-        <v>36</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>28</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E37" s="20"/>
       <c r="F37" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G37" s="29" t="s">
-        <v>149</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="G37" s="29"/>
       <c r="H37" s="29" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="I37" s="23">
-        <v>0.75</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="J37" s="26" t="s">
         <v>14</v>
       </c>
       <c r="K37" s="25">
         <f>$I37+Sheet2!B$1/24</f>
-        <v>1.1666666666666667</v>
+        <v>1.2083333333333333</v>
       </c>
       <c r="L37" s="23">
         <f>$I37+Sheet2!B$2/24</f>
-        <v>1.125</v>
+        <v>1.1666666666666665</v>
       </c>
       <c r="M37" s="23">
         <f>$I37+Sheet2!B$3/24</f>
-        <v>1.0833333333333333</v>
+        <v>1.125</v>
       </c>
       <c r="N37" s="23">
         <f>$I37+Sheet2!B$4/24</f>
-        <v>0.875</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="O37" s="23">
         <f>$I37+Sheet2!B$5/24</f>
-        <v>0.875</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="P37" s="23">
         <f>$I37+Sheet2!B$6/24</f>
-        <v>0.875</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="Q37" s="23">
         <f>$I37+Sheet2!B$7/24</f>
-        <v>0.83333333333333337</v>
+        <v>0.875</v>
       </c>
       <c r="R37" s="23">
         <f>$I37+Sheet2!B$8/24</f>
-        <v>0.79166666666666663</v>
+        <v>0.83333333333333326</v>
       </c>
       <c r="S37" s="23">
         <f>$I37+Sheet2!B$9/24</f>
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="T37" s="23">
         <f>$I37+Sheet2!B$10/24</f>
-        <v>0.54166666666666663</v>
+        <v>0.58333333333333326</v>
       </c>
       <c r="U37" s="23">
         <f>$I37+Sheet2!B$11/24</f>
-        <v>0.5</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="V37" s="23">
         <f>$I37+Sheet2!B$12/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.49999999999999994</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="50"/>
       <c r="B38" s="18" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C38" s="7">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D38" s="7">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="7" t="s">
-        <v>105</v>
+        <v>221</v>
       </c>
       <c r="G38" s="29"/>
       <c r="H38" s="29" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="I38" s="23">
-        <v>0.79166666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="J38" s="26" t="s">
         <v>14</v>
       </c>
       <c r="K38" s="25">
         <f>$I38+Sheet2!B$1/24</f>
-        <v>1.2083333333333333</v>
+        <v>1.25</v>
       </c>
       <c r="L38" s="23">
         <f>$I38+Sheet2!B$2/24</f>
-        <v>1.1666666666666665</v>
+        <v>1.2083333333333335</v>
       </c>
       <c r="M38" s="23">
         <f>$I38+Sheet2!B$3/24</f>
-        <v>1.125</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="N38" s="23">
         <f>$I38+Sheet2!B$4/24</f>
-        <v>0.91666666666666663</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="O38" s="23">
         <f>$I38+Sheet2!B$5/24</f>
-        <v>0.91666666666666663</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="P38" s="23">
         <f>$I38+Sheet2!B$6/24</f>
-        <v>0.91666666666666663</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="Q38" s="23">
         <f>$I38+Sheet2!B$7/24</f>
-        <v>0.875</v>
+        <v>0.91666666666666674</v>
       </c>
       <c r="R38" s="23">
         <f>$I38+Sheet2!B$8/24</f>
-        <v>0.83333333333333326</v>
+        <v>0.875</v>
       </c>
       <c r="S38" s="23">
         <f>$I38+Sheet2!B$9/24</f>
-        <v>0.625</v>
+        <v>0.66666666666666674</v>
       </c>
       <c r="T38" s="23">
         <f>$I38+Sheet2!B$10/24</f>
-        <v>0.58333333333333326</v>
+        <v>0.625</v>
       </c>
       <c r="U38" s="23">
         <f>$I38+Sheet2!B$11/24</f>
-        <v>0.54166666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="V38" s="23">
         <f>$I38+Sheet2!B$12/24</f>
-        <v>0.49999999999999994</v>
+        <v>0.54166666666666674</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="50"/>
       <c r="B39" s="18" t="s">
-        <v>220</v>
+        <v>31</v>
       </c>
       <c r="C39" s="7">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D39" s="7">
-        <v>38</v>
-      </c>
-      <c r="E39" s="20"/>
-      <c r="F39" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="G39" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>156</v>
+      </c>
       <c r="H39" s="29" t="s">
         <v>222</v>
       </c>
@@ -9908,1309 +9892,1289 @@
     <sortCondition ref="D2:D70"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
-    <mergeCell ref="A24:A47"/>
+    <mergeCell ref="A23:A47"/>
     <mergeCell ref="A48:A84"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L3 L10:V10 K11:L14 K5:L8 L9 K13:V16 L17:V17 K18:V40 K42:V85 L41:V41">
-    <cfRule type="expression" dxfId="260" priority="583">
+  <conditionalFormatting sqref="K2:L3 L10:V10 K11:L14 K5:L8 L9 K13:V38 K40:V85 L39:V39">
+    <cfRule type="expression" dxfId="258" priority="586">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:V3 K5:V8 K11:V15 L9:V10 K16 K22:V22 K18:V19 K20:K21 K23:K31">
-    <cfRule type="expression" dxfId="259" priority="585">
+  <conditionalFormatting sqref="K2:V3 K5:V8 K11:V15 L9:V10 K16 K21:V21 K17:V18 K19:K20 K22:K30">
+    <cfRule type="expression" dxfId="257" priority="588">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K50:V50 G50 G61 B62:B64 G71 G85 E59:G59 G29 B72 E72:G72 E62:G62 B3 E3:H3 H7 E16:G17 J18:V18 L10:V10 E20:G21 L20:V21 E22:H22 E30:G31 J22:V22 E32:H32 J32:V36 E42:G42 K42:V42 B42:B45 E47:G47 J47:V47 G63:G67 B68:B70 E68:G70 K57:V57 L61:V72 K74:V74 K83:V83 G73:G77 G83 K76:V77 K79:V80 K85:V85 L37:V37 E33:G37 E51:H51 J51:V51 E48:V49 G56:V56 H2 J2:V3 E43:H45 J43:V45 E58:V58 C57:G57 B80:G80 B11:B14 E11:H14 J11:V14 B20:B37 E24:G28 C23:G23 J80:V80 C6:D6 B5:G5 B16:B18 E18:H18 C19:D19 B9:G10 E53:V55 B47:B59 C52:V52 B17:G17 L16:V17 L23:V31 L41:V41">
-    <cfRule type="expression" dxfId="258" priority="589">
+  <conditionalFormatting sqref="K50:V50 G50 G61 B62:B64 G71 G85 E59:G59 G28 B72 E72:G72 E62:G62 B3 E3:H3 H7 J17:V17 L10:V10 E19:G20 L19:V20 E21:H21 E29:G30 J21:V21 E31:H31 J31:V35 E42:G42 K42:V42 B42:B45 E47:G47 J47:V47 G63:G67 B68:B70 E68:G70 K57:V57 L61:V72 K74:V74 K83:V83 G73:G77 G83 K76:V77 K79:V80 K85:V85 L36:V36 E32:G36 E51:H51 J51:V51 E48:V49 G56:V56 H2 J2:V3 E43:H45 J43:V45 E58:V58 C57:G57 B80:G80 B11:B14 E11:H14 J11:V14 B19:B36 E23:G27 C22:G22 J80:V80 C6:D6 B5:G5 E17:H17 C18:D18 B9:G10 E53:V55 B47:B59 C52:V52 L22:V30 L41:V41 E16:G16 B16:B17 L16:V16 L39:V39 C15:D16 B39:G39">
+    <cfRule type="expression" dxfId="256" priority="592">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61 L61:V61">
-    <cfRule type="expression" dxfId="257" priority="566">
+    <cfRule type="expression" dxfId="255" priority="569">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65 L65:V65">
-    <cfRule type="expression" dxfId="256" priority="564">
+    <cfRule type="expression" dxfId="254" priority="567">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67 L67:V67">
-    <cfRule type="expression" dxfId="255" priority="562">
+    <cfRule type="expression" dxfId="253" priority="565">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71 L71:V71">
-    <cfRule type="expression" dxfId="254" priority="560">
+    <cfRule type="expression" dxfId="252" priority="563">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66 L66:V66">
-    <cfRule type="expression" dxfId="253" priority="558">
+    <cfRule type="expression" dxfId="251" priority="561">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74 K74:V74">
-    <cfRule type="expression" dxfId="252" priority="556">
+    <cfRule type="expression" dxfId="250" priority="559">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83 K83:V83 E83:F83">
-    <cfRule type="expression" dxfId="251" priority="554">
+    <cfRule type="expression" dxfId="249" priority="557">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="expression" dxfId="250" priority="552">
+    <cfRule type="expression" dxfId="248" priority="555">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E71">
-    <cfRule type="expression" dxfId="249" priority="549">
+    <cfRule type="expression" dxfId="247" priority="552">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="expression" dxfId="248" priority="548">
+    <cfRule type="expression" dxfId="246" priority="551">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74">
-    <cfRule type="expression" dxfId="247" priority="547">
+    <cfRule type="expression" dxfId="245" priority="550">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79:B80 J79:V80">
-    <cfRule type="expression" dxfId="246" priority="545">
+    <cfRule type="expression" dxfId="244" priority="548">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77 J77:V77 E77">
-    <cfRule type="expression" dxfId="245" priority="543">
+    <cfRule type="expression" dxfId="243" priority="546">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E79:F80">
-    <cfRule type="expression" dxfId="244" priority="541">
+    <cfRule type="expression" dxfId="242" priority="544">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76 J76:V76">
-    <cfRule type="expression" dxfId="243" priority="539">
+    <cfRule type="expression" dxfId="241" priority="542">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85 J85:V85 E85">
-    <cfRule type="expression" dxfId="242" priority="537">
+    <cfRule type="expression" dxfId="240" priority="540">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66">
-    <cfRule type="expression" dxfId="241" priority="529">
+    <cfRule type="expression" dxfId="239" priority="532">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59:V59">
-    <cfRule type="expression" dxfId="240" priority="469">
+    <cfRule type="expression" dxfId="238" priority="472">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F74">
-    <cfRule type="expression" dxfId="239" priority="490">
+    <cfRule type="expression" dxfId="237" priority="493">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71">
-    <cfRule type="expression" dxfId="238" priority="491">
+    <cfRule type="expression" dxfId="236" priority="494">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73 E73:F73">
-    <cfRule type="expression" dxfId="237" priority="455">
+    <cfRule type="expression" dxfId="235" priority="458">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="expression" dxfId="236" priority="476">
+    <cfRule type="expression" dxfId="234" priority="479">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65:F65">
-    <cfRule type="expression" dxfId="235" priority="483">
+    <cfRule type="expression" dxfId="233" priority="486">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60 L60:V60">
-    <cfRule type="expression" dxfId="234" priority="477">
+    <cfRule type="expression" dxfId="232" priority="480">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F77">
-    <cfRule type="expression" dxfId="233" priority="489">
+    <cfRule type="expression" dxfId="231" priority="492">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61">
-    <cfRule type="expression" dxfId="232" priority="485">
+    <cfRule type="expression" dxfId="230" priority="488">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67:F67">
-    <cfRule type="expression" dxfId="231" priority="484">
+    <cfRule type="expression" dxfId="229" priority="487">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76:F76">
-    <cfRule type="expression" dxfId="230" priority="482">
+    <cfRule type="expression" dxfId="228" priority="485">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L60:V60 G60">
-    <cfRule type="expression" dxfId="229" priority="479">
+    <cfRule type="expression" dxfId="227" priority="482">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:V7">
-    <cfRule type="expression" dxfId="228" priority="424">
+    <cfRule type="expression" dxfId="226" priority="427">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60">
-    <cfRule type="expression" dxfId="227" priority="473">
+    <cfRule type="expression" dxfId="225" priority="476">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:V45 L41:V41">
-    <cfRule type="expression" dxfId="226" priority="593">
+    <cfRule type="expression" dxfId="224" priority="596">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59:V59">
-    <cfRule type="expression" dxfId="225" priority="470">
+    <cfRule type="expression" dxfId="223" priority="473">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:V10">
-    <cfRule type="expression" dxfId="224" priority="415">
+    <cfRule type="expression" dxfId="222" priority="418">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41 G41">
-    <cfRule type="expression" dxfId="223" priority="463">
+    <cfRule type="expression" dxfId="221" priority="466">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H14 J13:V14">
-    <cfRule type="expression" dxfId="222" priority="461">
+    <cfRule type="expression" dxfId="220" priority="464">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:V14">
-    <cfRule type="expression" dxfId="221" priority="462">
+    <cfRule type="expression" dxfId="219" priority="465">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B14 E13:G14">
-    <cfRule type="expression" dxfId="220" priority="459">
+    <cfRule type="expression" dxfId="218" priority="462">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41:F41">
-    <cfRule type="expression" dxfId="219" priority="457">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G3 B7 E7:G7 C8:D13 C15:D17 C21:D22 C24:D25 C27:D28 C30:D34 C36:D37 C66:D67 C39:D41 C69:D70 C43:D44 C72:D73 C46:D47 C75:D76 C49:D50 C78:D80 C82:D83 C54:D55 C85:D85 C59:D60 C62:D64">
-    <cfRule type="expression" dxfId="218" priority="456">
+    <cfRule type="expression" dxfId="217" priority="460">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:G3 B7 E7:G7 C8:D13 C20:D21 C23:D24 C26:D27 C29:D33 C35:D36 C66:D67 C38:D41 C69:D70 C43:D44 C72:D73 C46:D47 C75:D76 C49:D50 C78:D80 C82:D83 C54:D55 C85:D85 C59:D60 C62:D64">
+    <cfRule type="expression" dxfId="216" priority="459">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73:V73">
-    <cfRule type="expression" dxfId="217" priority="454">
+    <cfRule type="expression" dxfId="215" priority="457">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J73:V73">
-    <cfRule type="expression" dxfId="216" priority="452">
+    <cfRule type="expression" dxfId="214" priority="455">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73">
-    <cfRule type="expression" dxfId="215" priority="451">
+    <cfRule type="expression" dxfId="213" priority="454">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J75:V75">
-    <cfRule type="expression" dxfId="214" priority="446">
+    <cfRule type="expression" dxfId="212" priority="449">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75 E75:F75">
-    <cfRule type="expression" dxfId="213" priority="449">
+    <cfRule type="expression" dxfId="211" priority="452">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K75:V75">
-    <cfRule type="expression" dxfId="212" priority="448">
+    <cfRule type="expression" dxfId="210" priority="451">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75">
-    <cfRule type="expression" dxfId="211" priority="445">
+    <cfRule type="expression" dxfId="209" priority="448">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="210" priority="438">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29:F29">
-    <cfRule type="expression" dxfId="209" priority="443">
+    <cfRule type="expression" dxfId="208" priority="441">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28:F28">
+    <cfRule type="expression" dxfId="207" priority="446">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40:B41 E40:E41 L40:V41 G40:G41">
-    <cfRule type="expression" dxfId="208" priority="442">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:G4 C7:D7 C14:D14 C18:D18 C20:D20 C26:D26 C29:D29 C35:D35 C65:D65 C38:D38 C68:D68 C41:D42 C71:D71 C45:D45 C74:D74 C48:D48 C77:D77 C51:D51 C81:D81 C53:D53 C84:D84 C56:D56 C58:D58 C61:D61">
-    <cfRule type="expression" dxfId="207" priority="437">
+    <cfRule type="expression" dxfId="206" priority="445">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:G4 C7:D7 C14:D14 C17:D17 C19:D19 C25:D25 C28:D28 C34:D34 C65:D65 C37:D37 C68:D68 C41:D42 C71:D71 C45:D45 C74:D74 C48:D48 C77:D77 C51:D51 C81:D81 C53:D53 C84:D84 C56:D56 C58:D58 C61:D61">
+    <cfRule type="expression" dxfId="205" priority="440">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="206" priority="436">
+    <cfRule type="expression" dxfId="204" priority="439">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 E6:H6 J6:V6">
-    <cfRule type="expression" dxfId="205" priority="434">
+    <cfRule type="expression" dxfId="203" priority="437">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:V5">
-    <cfRule type="expression" dxfId="204" priority="431">
+    <cfRule type="expression" dxfId="202" priority="434">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:L4">
-    <cfRule type="expression" dxfId="203" priority="426">
+    <cfRule type="expression" dxfId="201" priority="429">
       <formula>K$1=$H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:V4">
-    <cfRule type="expression" dxfId="202" priority="427">
+    <cfRule type="expression" dxfId="200" priority="430">
       <formula>K$1=$I4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:V4">
-    <cfRule type="expression" dxfId="201" priority="428">
+    <cfRule type="expression" dxfId="199" priority="431">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="200" priority="421">
+    <cfRule type="expression" dxfId="198" priority="424">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 E8:G10">
-    <cfRule type="expression" dxfId="199" priority="420">
+    <cfRule type="expression" dxfId="197" priority="423">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:K8">
-    <cfRule type="expression" dxfId="198" priority="418">
+    <cfRule type="expression" dxfId="196" priority="421">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:H15 J15:V15">
-    <cfRule type="expression" dxfId="197" priority="410">
+    <cfRule type="expression" dxfId="195" priority="413">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15 J15:V15">
-    <cfRule type="expression" dxfId="196" priority="407">
+    <cfRule type="expression" dxfId="194" priority="410">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:V15">
-    <cfRule type="expression" dxfId="195" priority="408">
+    <cfRule type="expression" dxfId="193" priority="411">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:G15">
-    <cfRule type="expression" dxfId="194" priority="406">
+    <cfRule type="expression" dxfId="192" priority="409">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="193" priority="264">
+    <cfRule type="expression" dxfId="191" priority="267">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="192" priority="403">
+    <cfRule type="expression" dxfId="190" priority="406">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="191" priority="400">
+    <cfRule type="expression" dxfId="189" priority="403">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="190" priority="401">
+    <cfRule type="expression" dxfId="188" priority="404">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42 J42">
-    <cfRule type="expression" dxfId="189" priority="301">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19 E19:H19 J19:V19">
-    <cfRule type="expression" dxfId="188" priority="396">
+    <cfRule type="expression" dxfId="187" priority="304">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18 E18:H18 J18:V18">
+    <cfRule type="expression" dxfId="186" priority="399">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="187" priority="252">
+    <cfRule type="expression" dxfId="185" priority="255">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25 J25:K25">
+    <cfRule type="expression" dxfId="184" priority="361">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57 J57">
+    <cfRule type="expression" dxfId="183" priority="294">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H59:J59">
+    <cfRule type="expression" dxfId="182" priority="293">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19 J19:K19">
+    <cfRule type="expression" dxfId="181" priority="388">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20 J20:K20">
+    <cfRule type="expression" dxfId="180" priority="383">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K60">
+    <cfRule type="expression" dxfId="179" priority="288">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K60">
+    <cfRule type="expression" dxfId="178" priority="287">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22 J22:K22">
+    <cfRule type="expression" dxfId="177" priority="376">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K61">
+    <cfRule type="expression" dxfId="176" priority="284">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23 J23:K23">
+    <cfRule type="expression" dxfId="175" priority="371">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H61 J61">
+    <cfRule type="expression" dxfId="174" priority="282">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24 J24:K24">
+    <cfRule type="expression" dxfId="173" priority="366">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="expression" dxfId="172" priority="279">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62 J62">
+    <cfRule type="expression" dxfId="171" priority="278">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="expression" dxfId="170" priority="276">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="expression" dxfId="169" priority="275">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26 J26:K26">
-    <cfRule type="expression" dxfId="186" priority="358">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H57 J57">
-    <cfRule type="expression" dxfId="185" priority="291">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H59:J59">
-    <cfRule type="expression" dxfId="184" priority="290">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20 J20:K20">
-    <cfRule type="expression" dxfId="183" priority="385">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21 J21:K21">
-    <cfRule type="expression" dxfId="182" priority="380">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K60">
-    <cfRule type="expression" dxfId="181" priority="285">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K60">
-    <cfRule type="expression" dxfId="180" priority="284">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23 J23:K23">
-    <cfRule type="expression" dxfId="179" priority="373">
+    <cfRule type="expression" dxfId="168" priority="356">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="expression" dxfId="167" priority="272">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27 J27:K27">
+    <cfRule type="expression" dxfId="166" priority="351">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H64 J64">
+    <cfRule type="expression" dxfId="165" priority="270">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28 J28:K28">
+    <cfRule type="expression" dxfId="164" priority="346">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H65 J65">
+    <cfRule type="expression" dxfId="163" priority="266">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29 J29:K29">
+    <cfRule type="expression" dxfId="162" priority="341">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K66">
+    <cfRule type="expression" dxfId="161" priority="264">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K66">
+    <cfRule type="expression" dxfId="160" priority="263">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30 J30:K30">
+    <cfRule type="expression" dxfId="159" priority="336">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67">
+    <cfRule type="expression" dxfId="158" priority="260">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H67 J67">
+    <cfRule type="expression" dxfId="157" priority="258">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32">
+    <cfRule type="expression" dxfId="156" priority="324">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K68">
+    <cfRule type="expression" dxfId="155" priority="256">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33">
+    <cfRule type="expression" dxfId="154" priority="321">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="expression" dxfId="153" priority="318">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H68 J68">
+    <cfRule type="expression" dxfId="152" priority="254">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="expression" dxfId="151" priority="315">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37 J37:V37 E37:H37">
+    <cfRule type="expression" dxfId="150" priority="312">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J38:V38 B38:B41 E40:E41 E38:H38 G40:G41 E39:G39 L39:V41">
+    <cfRule type="expression" dxfId="149" priority="308">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K70">
+    <cfRule type="expression" dxfId="148" priority="252">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K70">
+    <cfRule type="expression" dxfId="147" priority="251">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46:G46 B46">
+    <cfRule type="expression" dxfId="146" priority="301">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I78">
+    <cfRule type="expression" dxfId="145" priority="158">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H46 J46:V46">
+    <cfRule type="expression" dxfId="144" priority="298">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H47">
+    <cfRule type="expression" dxfId="143" priority="297">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H50 J50">
+    <cfRule type="expression" dxfId="142" priority="296">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72">
+    <cfRule type="expression" dxfId="141" priority="244">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="140" priority="247">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H70 J70">
+    <cfRule type="expression" dxfId="139" priority="250">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H60 J60">
+    <cfRule type="expression" dxfId="138" priority="286">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K61">
-    <cfRule type="expression" dxfId="178" priority="281">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24 J24:K24">
-    <cfRule type="expression" dxfId="177" priority="368">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H61 J61">
-    <cfRule type="expression" dxfId="176" priority="279">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25 J25:K25">
-    <cfRule type="expression" dxfId="175" priority="363">
+    <cfRule type="expression" dxfId="137" priority="283">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62">
-    <cfRule type="expression" dxfId="174" priority="276">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H62 J62">
-    <cfRule type="expression" dxfId="173" priority="275">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="172" priority="273">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="171" priority="272">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27 J27:K27">
-    <cfRule type="expression" dxfId="170" priority="353">
+    <cfRule type="expression" dxfId="136" priority="280">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H63 J63">
+    <cfRule type="expression" dxfId="135" priority="274">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="169" priority="269">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H28 J28:K28">
-    <cfRule type="expression" dxfId="168" priority="348">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H64 J64">
-    <cfRule type="expression" dxfId="167" priority="267">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29 J29:K29">
-    <cfRule type="expression" dxfId="166" priority="343">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H65 J65">
-    <cfRule type="expression" dxfId="165" priority="263">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H30 J30:K30">
-    <cfRule type="expression" dxfId="164" priority="338">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="163" priority="261">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="162" priority="260">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H31 J31:K31">
-    <cfRule type="expression" dxfId="161" priority="333">
+    <cfRule type="expression" dxfId="134" priority="271">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65">
+    <cfRule type="expression" dxfId="133" priority="268">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66 J66">
+    <cfRule type="expression" dxfId="132" priority="262">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="160" priority="257">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="158" priority="255">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H33">
-    <cfRule type="expression" dxfId="157" priority="321">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="156" priority="253">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="155" priority="318">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="154" priority="315">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H68 J68">
-    <cfRule type="expression" dxfId="153" priority="251">
+    <cfRule type="expression" dxfId="131" priority="259">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="130" priority="248">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H71 J71">
+    <cfRule type="expression" dxfId="129" priority="246">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72">
+    <cfRule type="expression" dxfId="128" priority="243">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H72 J72">
+    <cfRule type="expression" dxfId="127" priority="242">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="expression" dxfId="126" priority="240">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="expression" dxfId="125" priority="239">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H69 J69">
+    <cfRule type="expression" dxfId="124" priority="238">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J74">
+    <cfRule type="expression" dxfId="123" priority="236">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H74">
+    <cfRule type="expression" dxfId="122" priority="235">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G78">
+    <cfRule type="expression" dxfId="121" priority="233">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J78:V78">
+    <cfRule type="expression" dxfId="120" priority="228">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B78 E78:F78">
+    <cfRule type="expression" dxfId="119" priority="230">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K78:V78">
+    <cfRule type="expression" dxfId="118" priority="229">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H78">
+    <cfRule type="expression" dxfId="117" priority="227">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H76">
+    <cfRule type="expression" dxfId="116" priority="224">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H77">
+    <cfRule type="expression" dxfId="115" priority="222">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G81">
+    <cfRule type="expression" dxfId="114" priority="219">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="expression" dxfId="113" priority="76">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J81:V81">
+    <cfRule type="expression" dxfId="112" priority="214">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B81 E81:F81">
+    <cfRule type="expression" dxfId="111" priority="216">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81:V81">
+    <cfRule type="expression" dxfId="110" priority="215">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H81">
+    <cfRule type="expression" dxfId="109" priority="213">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H79">
+    <cfRule type="expression" dxfId="108" priority="211">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G82">
+    <cfRule type="expression" dxfId="107" priority="209">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="expression" dxfId="106" priority="66">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J82:V82">
+    <cfRule type="expression" dxfId="105" priority="204">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82 E82:F82">
+    <cfRule type="expression" dxfId="104" priority="206">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82:V82">
+    <cfRule type="expression" dxfId="103" priority="205">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H82">
+    <cfRule type="expression" dxfId="102" priority="203">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J83">
+    <cfRule type="expression" dxfId="101" priority="201">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H83">
+    <cfRule type="expression" dxfId="100" priority="200">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G84">
+    <cfRule type="expression" dxfId="99" priority="198">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="expression" dxfId="98" priority="55">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J84:V84">
+    <cfRule type="expression" dxfId="97" priority="193">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B84 E84:F84">
+    <cfRule type="expression" dxfId="96" priority="195">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K84:V84">
+    <cfRule type="expression" dxfId="95" priority="194">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H84">
+    <cfRule type="expression" dxfId="94" priority="192">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K40">
+    <cfRule type="expression" dxfId="93" priority="190">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H40 J40">
+    <cfRule type="expression" dxfId="92" priority="188">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36:K36">
+    <cfRule type="expression" dxfId="91" priority="185">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="152" priority="312">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38 J38:V38 E38:H38">
-    <cfRule type="expression" dxfId="151" priority="309">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J39:V39 L40:V41 B39:B41 E40:E41 E39:H39 G40:G41">
-    <cfRule type="expression" dxfId="150" priority="305">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="149" priority="249">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="148" priority="248">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46:G46 B46">
-    <cfRule type="expression" dxfId="147" priority="298">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I78">
-    <cfRule type="expression" dxfId="146" priority="155">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H46 J46:V46">
-    <cfRule type="expression" dxfId="145" priority="295">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
-    <cfRule type="expression" dxfId="144" priority="294">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H50 J50">
-    <cfRule type="expression" dxfId="143" priority="293">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="142" priority="241">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="141" priority="244">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H70 J70">
-    <cfRule type="expression" dxfId="140" priority="247">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H60 J60">
-    <cfRule type="expression" dxfId="139" priority="283">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K61">
-    <cfRule type="expression" dxfId="138" priority="280">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="expression" dxfId="137" priority="277">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H63 J63">
-    <cfRule type="expression" dxfId="136" priority="271">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="135" priority="268">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="134" priority="265">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H66 J66">
-    <cfRule type="expression" dxfId="133" priority="259">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="132" priority="256">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="131" priority="245">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H71 J71">
-    <cfRule type="expression" dxfId="130" priority="243">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="129" priority="240">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H72 J72">
-    <cfRule type="expression" dxfId="128" priority="239">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="127" priority="237">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="126" priority="236">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H69 J69">
-    <cfRule type="expression" dxfId="125" priority="235">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J74">
-    <cfRule type="expression" dxfId="124" priority="233">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H74">
-    <cfRule type="expression" dxfId="123" priority="232">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G78">
-    <cfRule type="expression" dxfId="122" priority="230">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J78:V78">
-    <cfRule type="expression" dxfId="121" priority="225">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B78 E78:F78">
-    <cfRule type="expression" dxfId="120" priority="227">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K78:V78">
-    <cfRule type="expression" dxfId="119" priority="226">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H78">
-    <cfRule type="expression" dxfId="118" priority="224">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H76">
-    <cfRule type="expression" dxfId="117" priority="221">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="116" priority="219">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G81">
-    <cfRule type="expression" dxfId="115" priority="216">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="114" priority="73">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J81:V81">
-    <cfRule type="expression" dxfId="113" priority="211">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B81 E81:F81">
-    <cfRule type="expression" dxfId="112" priority="213">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="111" priority="212">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H81">
-    <cfRule type="expression" dxfId="110" priority="210">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H79">
-    <cfRule type="expression" dxfId="109" priority="208">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G82">
-    <cfRule type="expression" dxfId="108" priority="206">
+    <cfRule type="expression" dxfId="90" priority="183">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I46">
+    <cfRule type="expression" dxfId="89" priority="41">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50">
+    <cfRule type="expression" dxfId="88" priority="179">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I51">
+    <cfRule type="expression" dxfId="87" priority="178">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I57">
+    <cfRule type="expression" dxfId="86" priority="177">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I60">
+    <cfRule type="expression" dxfId="85" priority="176">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I61">
+    <cfRule type="expression" dxfId="84" priority="175">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I62">
+    <cfRule type="expression" dxfId="83" priority="174">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I63">
+    <cfRule type="expression" dxfId="82" priority="173">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I64">
+    <cfRule type="expression" dxfId="81" priority="172">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I65">
+    <cfRule type="expression" dxfId="80" priority="171">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I66">
+    <cfRule type="expression" dxfId="79" priority="170">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I67">
+    <cfRule type="expression" dxfId="78" priority="169">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I68">
+    <cfRule type="expression" dxfId="77" priority="168">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I69">
+    <cfRule type="expression" dxfId="76" priority="167">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I70">
+    <cfRule type="expression" dxfId="75" priority="166">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I71">
+    <cfRule type="expression" dxfId="74" priority="165">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I72">
+    <cfRule type="expression" dxfId="73" priority="164">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I73">
+    <cfRule type="expression" dxfId="72" priority="163">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I74">
+    <cfRule type="expression" dxfId="71" priority="162">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I75">
+    <cfRule type="expression" dxfId="70" priority="161">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I76">
+    <cfRule type="expression" dxfId="69" priority="160">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I77">
+    <cfRule type="expression" dxfId="68" priority="159">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I79">
+    <cfRule type="expression" dxfId="67" priority="157">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I81">
+    <cfRule type="expression" dxfId="66" priority="156">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I82">
+    <cfRule type="expression" dxfId="65" priority="155">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I83">
+    <cfRule type="expression" dxfId="64" priority="154">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I84">
+    <cfRule type="expression" dxfId="63" priority="153">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I85">
+    <cfRule type="expression" dxfId="62" priority="152">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H85">
+    <cfRule type="expression" dxfId="61" priority="151">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="expression" dxfId="60" priority="150">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="expression" dxfId="59" priority="149">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="expression" dxfId="58" priority="148">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="expression" dxfId="57" priority="147">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="expression" dxfId="56" priority="146">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="expression" dxfId="55" priority="145">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="expression" dxfId="54" priority="144">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="expression" dxfId="53" priority="143">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="expression" dxfId="52" priority="75">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="expression" dxfId="51" priority="74">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="expression" dxfId="50" priority="73">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="expression" dxfId="49" priority="72">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="expression" dxfId="48" priority="71">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="107" priority="63">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J82:V82">
-    <cfRule type="expression" dxfId="106" priority="201">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B82 E82:F82">
-    <cfRule type="expression" dxfId="105" priority="203">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82:V82">
-    <cfRule type="expression" dxfId="104" priority="202">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H82">
-    <cfRule type="expression" dxfId="103" priority="200">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J83">
-    <cfRule type="expression" dxfId="102" priority="198">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H83">
-    <cfRule type="expression" dxfId="101" priority="197">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G84">
-    <cfRule type="expression" dxfId="100" priority="195">
+    <cfRule type="expression" dxfId="47" priority="65">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="expression" dxfId="46" priority="69">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="expression" dxfId="45" priority="68">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="expression" dxfId="44" priority="67">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="expression" dxfId="43" priority="64">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="expression" dxfId="42" priority="63">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="expression" dxfId="41" priority="62">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="expression" dxfId="40" priority="61">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="expression" dxfId="39" priority="60">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="expression" dxfId="38" priority="59">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="expression" dxfId="37" priority="58">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30">
+    <cfRule type="expression" dxfId="36" priority="57">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="99" priority="52">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J84:V84">
-    <cfRule type="expression" dxfId="98" priority="190">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B84 E84:F84">
-    <cfRule type="expression" dxfId="97" priority="192">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K84:V84">
-    <cfRule type="expression" dxfId="96" priority="191">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H84">
-    <cfRule type="expression" dxfId="95" priority="189">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K40">
-    <cfRule type="expression" dxfId="94" priority="187">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H40 J40">
-    <cfRule type="expression" dxfId="93" priority="185">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J37:K37">
-    <cfRule type="expression" dxfId="92" priority="182">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="91" priority="180">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="90" priority="38">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I50">
-    <cfRule type="expression" dxfId="89" priority="176">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I51">
-    <cfRule type="expression" dxfId="88" priority="175">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I57">
-    <cfRule type="expression" dxfId="87" priority="174">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I60">
-    <cfRule type="expression" dxfId="86" priority="173">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I61">
-    <cfRule type="expression" dxfId="85" priority="172">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I62">
-    <cfRule type="expression" dxfId="84" priority="171">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="83" priority="170">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I64">
-    <cfRule type="expression" dxfId="82" priority="169">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
-    <cfRule type="expression" dxfId="81" priority="168">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I66">
-    <cfRule type="expression" dxfId="80" priority="167">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I67">
-    <cfRule type="expression" dxfId="79" priority="166">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I68">
-    <cfRule type="expression" dxfId="78" priority="165">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="77" priority="164">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="76" priority="163">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I71">
-    <cfRule type="expression" dxfId="75" priority="162">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I72">
-    <cfRule type="expression" dxfId="74" priority="161">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I73">
-    <cfRule type="expression" dxfId="73" priority="160">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I74">
-    <cfRule type="expression" dxfId="72" priority="159">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I75">
-    <cfRule type="expression" dxfId="71" priority="158">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="expression" dxfId="70" priority="157">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I77">
-    <cfRule type="expression" dxfId="69" priority="156">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I79">
-    <cfRule type="expression" dxfId="68" priority="154">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I81">
-    <cfRule type="expression" dxfId="67" priority="153">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I82">
-    <cfRule type="expression" dxfId="66" priority="152">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I83">
-    <cfRule type="expression" dxfId="65" priority="151">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I84">
-    <cfRule type="expression" dxfId="64" priority="150">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I85">
-    <cfRule type="expression" dxfId="63" priority="149">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H85">
-    <cfRule type="expression" dxfId="62" priority="148">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="61" priority="147">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="60" priority="146">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="expression" dxfId="59" priority="145">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="58" priority="144">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="57" priority="143">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="56" priority="142">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="55" priority="141">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="54" priority="140">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="53" priority="72">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="expression" dxfId="52" priority="71">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="expression" dxfId="51" priority="70">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="50" priority="69">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="49" priority="68">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="48" priority="62">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
-    <cfRule type="expression" dxfId="47" priority="66">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="expression" dxfId="46" priority="65">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="expression" dxfId="45" priority="64">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="44" priority="61">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="expression" dxfId="43" priority="60">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
-    <cfRule type="expression" dxfId="42" priority="59">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
-    <cfRule type="expression" dxfId="41" priority="58">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="40" priority="57">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="39" priority="56">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="expression" dxfId="38" priority="55">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="expression" dxfId="37" priority="54">
+    <cfRule type="expression" dxfId="35" priority="54">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I47">
+    <cfRule type="expression" dxfId="34" priority="40">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="35" priority="51">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="34" priority="37">
+    <cfRule type="expression" dxfId="33" priority="52">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="33" priority="49">
+    <cfRule type="expression" dxfId="32" priority="51">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="expression" dxfId="32" priority="48">
+    <cfRule type="expression" dxfId="31" priority="50">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="expression" dxfId="31" priority="47">
+    <cfRule type="expression" dxfId="30" priority="49">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="expression" dxfId="30" priority="46">
+    <cfRule type="expression" dxfId="29" priority="48">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="29" priority="45">
+    <cfRule type="expression" dxfId="28" priority="47">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="expression" dxfId="27" priority="46">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I42">
+    <cfRule type="expression" dxfId="26" priority="45">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43">
+    <cfRule type="expression" dxfId="25" priority="44">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="expression" dxfId="24" priority="43">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I45">
+    <cfRule type="expression" dxfId="23" priority="42">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:V10">
+    <cfRule type="expression" dxfId="22" priority="32">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="expression" dxfId="21" priority="21">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H80">
+    <cfRule type="expression" dxfId="20" priority="30">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I80">
+    <cfRule type="expression" dxfId="19" priority="29">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:K9">
+    <cfRule type="expression" dxfId="18" priority="20">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="expression" dxfId="17" priority="19">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="16" priority="22">
+      <formula>K$1=$H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="15" priority="23">
+      <formula>K$1=$I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="14" priority="17">
+      <formula>K$1=$H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="13" priority="18">
+      <formula>K$1=$I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:K10">
+    <cfRule type="expression" dxfId="11" priority="15">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40:F41">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41:K41 H41">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K39">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>K$1=$H39</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J39:K39 H39">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="expression" dxfId="28" priority="44">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="27" priority="43">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="26" priority="42">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="25" priority="41">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="24" priority="40">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
-    <cfRule type="expression" dxfId="23" priority="39">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L9:V10">
-    <cfRule type="expression" dxfId="22" priority="29">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="21" priority="18">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H80">
-    <cfRule type="expression" dxfId="20" priority="27">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I80">
-    <cfRule type="expression" dxfId="19" priority="26">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:K9">
-    <cfRule type="expression" dxfId="18" priority="17">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="17" priority="16">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="16" priority="19">
-      <formula>K$1=$H9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="15" priority="20">
-      <formula>K$1=$I9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="14" priority="14">
-      <formula>K$1=$H10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="13" priority="15">
-      <formula>K$1=$I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="12" priority="13">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
-    <cfRule type="expression" dxfId="11" priority="12">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="10" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>K$1=$H17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="expression" dxfId="8" priority="10">
-      <formula>K$1=$I17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17 J17:K17">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17 J17:K17">
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="expression" dxfId="5" priority="7">
-      <formula>K$1=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F40:F41">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K41">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>K$1=$H41</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J41:K41 H41">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
TchacaBR is now Richard01
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E70EA02-6B32-2A4D-A4B3-CEC978EEA3DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93DC16E-309E-F343-B99B-8EE4A71A07D9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19820" yWindow="2700" windowWidth="25720" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -32,6 +32,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -260,9 +261,6 @@
     <t>:flag_it:</t>
   </si>
   <si>
-    <t>TchacaBR</t>
-  </si>
-  <si>
     <t>Brazil</t>
   </si>
   <si>
@@ -756,6 +754,9 @@
   </si>
   <si>
     <t>AOE</t>
+  </si>
+  <si>
+    <t>Richard01</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1183,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="270">
+  <dxfs count="262">
     <dxf>
       <fill>
         <patternFill>
@@ -1202,64 +1203,6 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3408,7 +3351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
@@ -3512,7 +3455,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -3522,10 +3465,10 @@
       </c>
       <c r="E2" s="20"/>
       <c r="F2" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>12</v>
@@ -3603,7 +3546,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>12</v>
@@ -3666,7 +3609,7 @@
     <row r="4" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C4" s="7">
         <v>3</v>
@@ -3676,13 +3619,13 @@
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="I4" s="23">
         <v>0.33333333333333331</v>
@@ -3742,7 +3685,7 @@
     <row r="5" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="7">
         <v>4</v>
@@ -3752,10 +3695,10 @@
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>25</v>
@@ -3827,13 +3770,13 @@
         <v>5</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>25</v>
@@ -3896,7 +3839,7 @@
     <row r="7" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C7" s="7">
         <v>6</v>
@@ -3906,11 +3849,11 @@
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G7" s="29"/>
       <c r="H7" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I7" s="23">
         <v>0.41666666666666669</v>
@@ -3970,7 +3913,7 @@
     <row r="8" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C8" s="7">
         <v>7</v>
@@ -3980,11 +3923,11 @@
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G8" s="29"/>
       <c r="H8" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I8" s="23">
         <v>0.45833333333333331</v>
@@ -4053,16 +3996,16 @@
         <v>8</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I9" s="23">
         <v>0.45833333333333331</v>
@@ -4122,7 +4065,7 @@
     <row r="10" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
       <c r="B10" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="7">
         <v>9</v>
@@ -4131,16 +4074,16 @@
         <v>9</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I10" s="23">
         <v>0.45833333333333331</v>
@@ -4200,7 +4143,7 @@
     <row r="11" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="43"/>
       <c r="B11" s="36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C11" s="7">
         <v>10</v>
@@ -4210,11 +4153,11 @@
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I11" s="23">
         <v>0.5</v>
@@ -4274,7 +4217,7 @@
     <row r="12" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12" s="7">
         <v>11</v>
@@ -4283,14 +4226,14 @@
         <v>11</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I12" s="23">
         <v>0.5</v>
@@ -4350,7 +4293,7 @@
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="47"/>
       <c r="B13" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" s="7">
         <v>12</v>
@@ -4362,13 +4305,13 @@
         <v>27</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I13" s="23">
         <v>0.5</v>
@@ -4428,7 +4371,7 @@
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
       <c r="B14" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C14" s="7">
         <v>13</v>
@@ -4438,11 +4381,11 @@
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I14" s="23">
         <v>0.54166666666666663</v>
@@ -4502,7 +4445,7 @@
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="47"/>
       <c r="B15" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C15" s="7">
         <v>14</v>
@@ -4512,11 +4455,11 @@
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I15" s="23">
         <v>0.58333333333333337</v>
@@ -4591,10 +4534,10 @@
         <v>18</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I16" s="23">
         <v>0.58333333333333337</v>
@@ -4654,7 +4597,7 @@
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="43"/>
       <c r="B17" s="36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C17" s="7">
         <v>16</v>
@@ -4664,7 +4607,7 @@
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="27" t="s">
@@ -4743,7 +4686,7 @@
         <v>20</v>
       </c>
       <c r="G18" s="45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H18" s="27" t="s">
         <v>10</v>
@@ -4806,7 +4749,7 @@
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="47"/>
       <c r="B19" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C19" s="7">
         <v>18</v>
@@ -4816,13 +4759,13 @@
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="29" t="s">
         <v>210</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="H19" s="29" t="s">
-        <v>211</v>
       </c>
       <c r="I19" s="23">
         <v>0.66666666666666663</v>
@@ -4894,13 +4837,13 @@
         <v>19</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H20" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I20" s="23">
         <v>0.66666666666666663</v>
@@ -4975,10 +4918,10 @@
         <v>72</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I21" s="23">
         <v>0.66666666666666663</v>
@@ -5038,7 +4981,7 @@
     <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="42"/>
       <c r="B22" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C22" s="7">
         <v>21</v>
@@ -5048,13 +4991,13 @@
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22" s="29" t="s">
         <v>212</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="H22" s="29" t="s">
-        <v>213</v>
       </c>
       <c r="I22" s="23">
         <v>0.70833333333333337</v>
@@ -5129,10 +5072,10 @@
         <v>45</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H23" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I23" s="23">
         <v>0.70833333333333337</v>
@@ -5194,7 +5137,7 @@
         <v>26</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C24" s="7">
         <v>23</v>
@@ -5207,10 +5150,10 @@
         <v>45</v>
       </c>
       <c r="G24" s="48" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I24" s="23">
         <v>0.70833333333333337</v>
@@ -5270,7 +5213,7 @@
     <row r="25" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="51"/>
       <c r="B25" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" s="7">
         <v>24</v>
@@ -5279,16 +5222,16 @@
         <v>24</v>
       </c>
       <c r="E25" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="G25" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="G25" s="22" t="s">
-        <v>117</v>
-      </c>
       <c r="H25" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I25" s="23">
         <v>0.70833333333333337</v>
@@ -5363,10 +5306,10 @@
         <v>45</v>
       </c>
       <c r="G26" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I26" s="23">
         <v>0.70833333333333337</v>
@@ -5441,10 +5384,10 @@
         <v>45</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I27" s="23">
         <v>0.70833333333333337</v>
@@ -5513,16 +5456,16 @@
         <v>27</v>
       </c>
       <c r="E28" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="G28" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I28" s="23">
         <v>0.70833333333333337</v>
@@ -5582,7 +5525,7 @@
     <row r="29" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="51"/>
       <c r="B29" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C29" s="7">
         <v>28</v>
@@ -5597,10 +5540,10 @@
         <v>72</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H29" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I29" s="23">
         <v>0.70833333333333337</v>
@@ -5675,10 +5618,10 @@
         <v>70</v>
       </c>
       <c r="G30" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H30" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I30" s="23">
         <v>0.70833333333333337</v>
@@ -5750,13 +5693,13 @@
         <v>15</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G31" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H31" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I31" s="23">
         <v>0.70833333333333337</v>
@@ -5816,7 +5759,7 @@
     <row r="32" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="51"/>
       <c r="B32" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C32" s="7">
         <v>31</v>
@@ -5826,11 +5769,11 @@
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G32" s="29"/>
       <c r="H32" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I32" s="23">
         <v>0.75</v>
@@ -5890,7 +5833,7 @@
     <row r="33" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="51"/>
       <c r="B33" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C33" s="7">
         <v>32</v>
@@ -5899,16 +5842,16 @@
         <v>32</v>
       </c>
       <c r="E33" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="F33" s="7" t="s">
-        <v>116</v>
-      </c>
       <c r="G33" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H33" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I33" s="23">
         <v>0.75</v>
@@ -5983,10 +5926,10 @@
         <v>70</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I34" s="23">
         <v>0.75</v>
@@ -6061,10 +6004,10 @@
         <v>20</v>
       </c>
       <c r="G35" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H35" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I35" s="23">
         <v>0.75</v>
@@ -6124,7 +6067,7 @@
     <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="51"/>
       <c r="B36" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C36" s="7">
         <v>35</v>
@@ -6133,16 +6076,16 @@
         <v>35</v>
       </c>
       <c r="E36" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F36" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="G36" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H36" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I36" s="23">
         <v>0.75</v>
@@ -6214,13 +6157,13 @@
         <v>28</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G37" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H37" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I37" s="23">
         <v>0.75</v>
@@ -6280,7 +6223,7 @@
     <row r="38" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="51"/>
       <c r="B38" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C38" s="7">
         <v>37</v>
@@ -6290,11 +6233,11 @@
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G38" s="29"/>
       <c r="H38" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I38" s="23">
         <v>0.79166666666666663</v>
@@ -6354,7 +6297,7 @@
     <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="51"/>
       <c r="B39" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C39" s="7">
         <v>55</v>
@@ -6369,10 +6312,10 @@
         <v>20</v>
       </c>
       <c r="G39" s="46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H39" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I39" s="23">
         <v>0.79166666666666663</v>
@@ -6432,7 +6375,7 @@
     <row r="40" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="51"/>
       <c r="B40" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C40" s="7">
         <v>38</v>
@@ -6442,11 +6385,11 @@
       </c>
       <c r="E40" s="20"/>
       <c r="F40" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G40" s="29"/>
       <c r="H40" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I40" s="23">
         <v>0.83333333333333337</v>
@@ -6521,10 +6464,10 @@
         <v>20</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H41" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I41" s="23">
         <v>0.83333333333333337</v>
@@ -6584,7 +6527,7 @@
     <row r="42" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="51"/>
       <c r="B42" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C42" s="7">
         <v>40</v>
@@ -6593,16 +6536,16 @@
         <v>40</v>
       </c>
       <c r="E42" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F42" s="19" t="s">
         <v>45</v>
       </c>
       <c r="G42" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H42" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I42" s="23">
         <v>0.83333333333333337</v>
@@ -6662,7 +6605,7 @@
     <row r="43" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="51"/>
       <c r="B43" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C43" s="7">
         <v>41</v>
@@ -6677,10 +6620,10 @@
         <v>72</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H43" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I43" s="23">
         <v>0.83333333333333337</v>
@@ -6740,7 +6683,7 @@
     <row r="44" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="51"/>
       <c r="B44" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C44" s="7">
         <v>43</v>
@@ -6750,11 +6693,11 @@
       </c>
       <c r="E44" s="33"/>
       <c r="F44" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G44" s="34"/>
       <c r="H44" s="29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I44" s="23">
         <v>0.875</v>
@@ -6814,7 +6757,7 @@
     <row r="45" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="51"/>
       <c r="B45" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" s="7">
         <v>44</v>
@@ -6829,10 +6772,10 @@
         <v>18</v>
       </c>
       <c r="G45" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H45" s="29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I45" s="23">
         <v>0.875</v>
@@ -6892,7 +6835,7 @@
     <row r="46" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="51"/>
       <c r="B46" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C46" s="7">
         <v>45</v>
@@ -6902,11 +6845,11 @@
       </c>
       <c r="E46" s="20"/>
       <c r="F46" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G46" s="29"/>
       <c r="H46" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I46" s="23">
         <v>0.91666666666666663</v>
@@ -6981,10 +6924,10 @@
         <v>20</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H47" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I47" s="23">
         <v>0.91666666666666663</v>
@@ -7044,7 +6987,7 @@
     <row r="48" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="52"/>
       <c r="B48" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C48" s="7">
         <v>47</v>
@@ -7054,11 +6997,11 @@
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G48" s="29"/>
       <c r="H48" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I48" s="23">
         <v>0.95833333333333337</v>
@@ -7118,7 +7061,7 @@
     <row r="49" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="52"/>
       <c r="B49" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C49" s="7">
         <v>48</v>
@@ -7133,10 +7076,10 @@
         <v>45</v>
       </c>
       <c r="G49" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H49" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I49" s="23">
         <v>0.95833333333333337</v>
@@ -7196,7 +7139,7 @@
     <row r="50" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="52"/>
       <c r="B50" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C50" s="7">
         <v>49</v>
@@ -7211,10 +7154,10 @@
         <v>20</v>
       </c>
       <c r="G50" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H50" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I50" s="23">
         <v>0.95833333333333337</v>
@@ -7289,10 +7232,10 @@
         <v>20</v>
       </c>
       <c r="G51" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H51" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I51" s="23">
         <v>0.95833333333333337</v>
@@ -7367,10 +7310,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H52" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I52" s="23">
         <v>0.95833333333333337</v>
@@ -7445,10 +7388,10 @@
         <v>20</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H53" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I53" s="23">
         <v>0.95833333333333337</v>
@@ -7523,10 +7466,10 @@
         <v>20</v>
       </c>
       <c r="G54" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H54" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I54" s="23">
         <v>0.95833333333333337</v>
@@ -7586,7 +7529,7 @@
     <row r="55" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="52"/>
       <c r="B55" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C55" s="7">
         <v>54</v>
@@ -7601,10 +7544,10 @@
         <v>20</v>
       </c>
       <c r="G55" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H55" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I55" s="23">
         <v>0.95833333333333337</v>
@@ -7679,10 +7622,10 @@
         <v>45</v>
       </c>
       <c r="G56" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H56" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I56" s="23">
         <v>0.95833333333333337</v>
@@ -7742,7 +7685,7 @@
     <row r="57" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="52"/>
       <c r="B57" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C57" s="7">
         <v>57</v>
@@ -7752,7 +7695,7 @@
       </c>
       <c r="E57" s="14"/>
       <c r="F57" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G57" s="9"/>
       <c r="H57" s="29" t="s">
@@ -7816,7 +7759,7 @@
     <row r="58" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="52"/>
       <c r="B58" s="35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C58" s="7">
         <v>58</v>
@@ -7831,7 +7774,7 @@
         <v>20</v>
       </c>
       <c r="G58" s="29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H58" s="29" t="s">
         <v>9</v>
@@ -7909,7 +7852,7 @@
         <v>20</v>
       </c>
       <c r="G59" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H59" s="29" t="s">
         <v>9</v>
@@ -7987,7 +7930,7 @@
         <v>70</v>
       </c>
       <c r="G60" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H60" s="29" t="s">
         <v>9</v>
@@ -8050,7 +7993,7 @@
     <row r="61" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="52"/>
       <c r="B61" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C61" s="7">
         <v>61</v>
@@ -8065,7 +8008,7 @@
         <v>20</v>
       </c>
       <c r="G61" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H61" s="29" t="s">
         <v>9</v>
@@ -8128,7 +8071,7 @@
     <row r="62" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="52"/>
       <c r="B62" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C62" s="7">
         <v>62</v>
@@ -8143,7 +8086,7 @@
         <v>20</v>
       </c>
       <c r="G62" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H62" s="29" t="s">
         <v>9</v>
@@ -8221,7 +8164,7 @@
         <v>20</v>
       </c>
       <c r="G63" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H63" s="29" t="s">
         <v>9</v>
@@ -8299,7 +8242,7 @@
         <v>45</v>
       </c>
       <c r="G64" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H64" s="29" t="s">
         <v>9</v>
@@ -8377,7 +8320,7 @@
         <v>20</v>
       </c>
       <c r="G65" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H65" s="29" t="s">
         <v>9</v>
@@ -8452,10 +8395,10 @@
         <v>27</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G66" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H66" s="29" t="s">
         <v>9</v>
@@ -8518,7 +8461,7 @@
     <row r="67" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="52"/>
       <c r="B67" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C67" s="7">
         <v>67</v>
@@ -8533,7 +8476,7 @@
         <v>20</v>
       </c>
       <c r="G67" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H67" s="29" t="s">
         <v>9</v>
@@ -8611,7 +8554,7 @@
         <v>20</v>
       </c>
       <c r="G68" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H68" s="29" t="s">
         <v>9</v>
@@ -8689,7 +8632,7 @@
         <v>70</v>
       </c>
       <c r="G69" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H69" s="29" t="s">
         <v>9</v>
@@ -8767,7 +8710,7 @@
         <v>20</v>
       </c>
       <c r="G70" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H70" s="29" t="s">
         <v>9</v>
@@ -8830,7 +8773,7 @@
     <row r="71" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="52"/>
       <c r="B71" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C71" s="7">
         <v>71</v>
@@ -8840,11 +8783,11 @@
       </c>
       <c r="E71" s="14"/>
       <c r="F71" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G71" s="29"/>
       <c r="H71" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I71" s="23">
         <v>4.1666666666666664E-2</v>
@@ -8913,16 +8856,16 @@
         <v>72</v>
       </c>
       <c r="E72" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="F72" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F72" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="G72" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H72" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I72" s="23">
         <v>4.1666666666666664E-2</v>
@@ -8991,16 +8934,16 @@
         <v>73</v>
       </c>
       <c r="E73" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F73" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F73" s="7" t="s">
-        <v>93</v>
-      </c>
       <c r="G73" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H73" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I73" s="23">
         <v>4.1666666666666664E-2</v>
@@ -9060,7 +9003,7 @@
     <row r="74" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="52"/>
       <c r="B74" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C74" s="7">
         <v>74</v>
@@ -9070,11 +9013,11 @@
       </c>
       <c r="E74" s="14"/>
       <c r="F74" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G74" s="29"/>
       <c r="H74" s="29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I74" s="23">
         <v>8.3333333333333329E-2</v>
@@ -9149,10 +9092,10 @@
         <v>20</v>
       </c>
       <c r="G75" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H75" s="29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I75" s="23">
         <v>8.3333333333333329E-2</v>
@@ -9227,10 +9170,10 @@
         <v>70</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H76" s="29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I76" s="23">
         <v>8.3333333333333329E-2</v>
@@ -9290,7 +9233,7 @@
     <row r="77" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="52"/>
       <c r="B77" s="18" t="s">
-        <v>73</v>
+        <v>238</v>
       </c>
       <c r="C77" s="7">
         <v>42</v>
@@ -9299,16 +9242,16 @@
         <v>42</v>
       </c>
       <c r="E77" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F77" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F77" s="7" t="s">
-        <v>75</v>
-      </c>
       <c r="G77" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H77" s="29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I77" s="23">
         <v>8.3333333333333329E-2</v>
@@ -9368,7 +9311,7 @@
     <row r="78" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="52"/>
       <c r="B78" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C78" s="7">
         <v>77</v>
@@ -9378,11 +9321,11 @@
       </c>
       <c r="E78" s="14"/>
       <c r="F78" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G78" s="29"/>
       <c r="H78" s="29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I78" s="23">
         <v>0.125</v>
@@ -9457,10 +9400,10 @@
         <v>20</v>
       </c>
       <c r="G79" s="37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H79" s="29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I79" s="23">
         <v>0.125</v>
@@ -9535,10 +9478,10 @@
         <v>20</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H80" s="29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I80" s="23">
         <v>0.125</v>
@@ -9598,7 +9541,7 @@
     <row r="81" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="52"/>
       <c r="B81" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C81" s="7">
         <v>80</v>
@@ -9608,11 +9551,11 @@
       </c>
       <c r="E81" s="14"/>
       <c r="F81" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G81" s="29"/>
       <c r="H81" s="29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I81" s="23">
         <v>0.16666666666666666</v>
@@ -9672,7 +9615,7 @@
     <row r="82" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="52"/>
       <c r="B82" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C82" s="7">
         <v>81</v>
@@ -9682,11 +9625,11 @@
       </c>
       <c r="E82" s="14"/>
       <c r="F82" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G82" s="29"/>
       <c r="H82" s="29" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I82" s="23">
         <v>0.20833333333333334</v>
@@ -9761,10 +9704,10 @@
         <v>20</v>
       </c>
       <c r="G83" s="34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H83" s="29" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I83" s="23">
         <v>0.20833333333333334</v>
@@ -9824,7 +9767,7 @@
     <row r="84" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="52"/>
       <c r="B84" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C84" s="7">
         <v>83</v>
@@ -9834,11 +9777,11 @@
       </c>
       <c r="E84" s="14"/>
       <c r="F84" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G84" s="29"/>
       <c r="H84" s="29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I84" s="23">
         <v>0.25</v>
@@ -9912,10 +9855,10 @@
         <v>20</v>
       </c>
       <c r="G85" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H85" s="29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I85" s="23">
         <v>0.25</v>
@@ -9973,15 +9916,15 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:V68">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:V68">
     <sortCondition ref="D2:D68"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -9990,1282 +9933,1282 @@
     <mergeCell ref="A48:A84"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V38 L39:V39 K40:V76 K78:V85">
-    <cfRule type="expression" dxfId="269" priority="618">
+    <cfRule type="expression" dxfId="261" priority="618">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K22:V22 K17:V17 K19:V19 K20:K21 K23:K31">
-    <cfRule type="expression" dxfId="268" priority="620">
+    <cfRule type="expression" dxfId="260" priority="620">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K50:V50 G50 G59 B60:B62 G69 G85 E57:G57 G29 B70 E70:G70 B3 E3:H3 H7 L10:V10 E20:G21 L20:V21 E22:H22 E30:G31 J22:V22 E32:H32 J32:V36 E47:G47 J47:V47 G61:G65 B66:B68 E66:G68 L39:V39 L59:V70 K73:V73 K83:V83 G83 K75:V76 K79:V80 K85:V85 L37:V37 E33:G37 E48:V49 G55:V55 H2 J2:V3 E39:G39 B80 J11:V14 B20:B37 E23:G28 J80:V80 B5:G5 E51:V54 L23:V31 L43:V43 L16:V16 L41:V41 B41 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V45 L72:V72 E44:H45 B9:B14 E18:G18 E9:G10 C9:D9 C13:D13 C17:H17 C21:D21 E41:G41 E80:G80 C25:D25 C45:D45 C64:D64 C85:D85 C29:D29 C49:D49 C68:D68 C33:D33 C53:D53 B72:G72 C37:D37 C56:V56 C76:D77 C60:G60 C81:D81 B47:B57 B39 B44:B45 C42:D43 G71:G76 B73:F73 C74:D74 B77:G77">
-    <cfRule type="expression" dxfId="267" priority="624">
+    <cfRule type="expression" dxfId="259" priority="624">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59 L59:V59">
-    <cfRule type="expression" dxfId="266" priority="601">
+    <cfRule type="expression" dxfId="258" priority="601">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63 L63:V63">
-    <cfRule type="expression" dxfId="265" priority="599">
+    <cfRule type="expression" dxfId="257" priority="599">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65 L65:V65">
-    <cfRule type="expression" dxfId="264" priority="597">
+    <cfRule type="expression" dxfId="256" priority="597">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69 L69:V69">
-    <cfRule type="expression" dxfId="263" priority="595">
+    <cfRule type="expression" dxfId="255" priority="595">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64 L64:V64">
-    <cfRule type="expression" dxfId="262" priority="593">
+    <cfRule type="expression" dxfId="254" priority="593">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73:V73">
-    <cfRule type="expression" dxfId="261" priority="591">
+    <cfRule type="expression" dxfId="253" priority="591">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83 K83:V83 E83:F83">
-    <cfRule type="expression" dxfId="260" priority="589">
+    <cfRule type="expression" dxfId="252" priority="589">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59">
-    <cfRule type="expression" dxfId="259" priority="587">
+    <cfRule type="expression" dxfId="251" priority="587">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69">
-    <cfRule type="expression" dxfId="258" priority="584">
+    <cfRule type="expression" dxfId="250" priority="584">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" dxfId="257" priority="583">
+    <cfRule type="expression" dxfId="249" priority="583">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79:B80 J79:V80">
-    <cfRule type="expression" dxfId="256" priority="580">
+    <cfRule type="expression" dxfId="248" priority="580">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76:B77 J76:V76 E76:E77">
-    <cfRule type="expression" dxfId="255" priority="578">
+    <cfRule type="expression" dxfId="247" priority="578">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E79:F80">
-    <cfRule type="expression" dxfId="254" priority="576">
+    <cfRule type="expression" dxfId="246" priority="576">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75 J75:V75">
-    <cfRule type="expression" dxfId="253" priority="574">
+    <cfRule type="expression" dxfId="245" priority="574">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85 J85:V85 E85">
-    <cfRule type="expression" dxfId="252" priority="572">
+    <cfRule type="expression" dxfId="244" priority="572">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64">
-    <cfRule type="expression" dxfId="251" priority="564">
+    <cfRule type="expression" dxfId="243" priority="564">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K57:V57">
-    <cfRule type="expression" dxfId="250" priority="504">
+    <cfRule type="expression" dxfId="242" priority="504">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F69">
-    <cfRule type="expression" dxfId="249" priority="526">
+    <cfRule type="expression" dxfId="241" priority="526">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71:B72 E71:F72">
-    <cfRule type="expression" dxfId="248" priority="490">
+    <cfRule type="expression" dxfId="240" priority="490">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58">
-    <cfRule type="expression" dxfId="247" priority="511">
+    <cfRule type="expression" dxfId="239" priority="511">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63:F63">
-    <cfRule type="expression" dxfId="246" priority="518">
+    <cfRule type="expression" dxfId="238" priority="518">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58 L58:V58">
-    <cfRule type="expression" dxfId="245" priority="512">
+    <cfRule type="expression" dxfId="237" priority="512">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F76:F77">
-    <cfRule type="expression" dxfId="244" priority="524">
+    <cfRule type="expression" dxfId="236" priority="524">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59">
-    <cfRule type="expression" dxfId="243" priority="520">
+    <cfRule type="expression" dxfId="235" priority="520">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65:F65">
-    <cfRule type="expression" dxfId="242" priority="519">
+    <cfRule type="expression" dxfId="234" priority="519">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E75:F75">
-    <cfRule type="expression" dxfId="241" priority="517">
+    <cfRule type="expression" dxfId="233" priority="517">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58:V58 G58">
-    <cfRule type="expression" dxfId="240" priority="514">
+    <cfRule type="expression" dxfId="232" priority="514">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:V7">
-    <cfRule type="expression" dxfId="239" priority="459">
+    <cfRule type="expression" dxfId="231" priority="459">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F58">
-    <cfRule type="expression" dxfId="238" priority="508">
+    <cfRule type="expression" dxfId="230" priority="508">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:V45 L43:V43">
-    <cfRule type="expression" dxfId="237" priority="628">
+    <cfRule type="expression" dxfId="229" priority="628">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K57:V57">
-    <cfRule type="expression" dxfId="236" priority="505">
+    <cfRule type="expression" dxfId="228" priority="505">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:V10">
-    <cfRule type="expression" dxfId="235" priority="450">
+    <cfRule type="expression" dxfId="227" priority="450">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43 G43">
-    <cfRule type="expression" dxfId="234" priority="498">
+    <cfRule type="expression" dxfId="226" priority="498">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H14 J13:V14 L18:V18">
-    <cfRule type="expression" dxfId="233" priority="496">
+    <cfRule type="expression" dxfId="225" priority="496">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:V14 L18:V18">
-    <cfRule type="expression" dxfId="232" priority="497">
+    <cfRule type="expression" dxfId="224" priority="497">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43:F43">
-    <cfRule type="expression" dxfId="231" priority="492">
+    <cfRule type="expression" dxfId="223" priority="492">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:G3 B7 E7:G7 C6:D7 C10:D11 C14:D15 C18:D19 C22:D23 C61:D62 C82:D83 C26:D27 C46:D47 C65:D66 C30:D31 C50:D51 C69:D70 C34:D35 C54:D55 C38:D40 C57:D58 C78:D79">
-    <cfRule type="expression" dxfId="230" priority="491">
+    <cfRule type="expression" dxfId="222" priority="491">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71:V71 L72:V72">
-    <cfRule type="expression" dxfId="229" priority="489">
+    <cfRule type="expression" dxfId="221" priority="489">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J71:V71 L72:V72">
-    <cfRule type="expression" dxfId="228" priority="487">
+    <cfRule type="expression" dxfId="220" priority="487">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71">
-    <cfRule type="expression" dxfId="227" priority="486">
+    <cfRule type="expression" dxfId="219" priority="486">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J74:V74">
-    <cfRule type="expression" dxfId="226" priority="481">
+    <cfRule type="expression" dxfId="218" priority="481">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74 E74:F74">
-    <cfRule type="expression" dxfId="225" priority="484">
+    <cfRule type="expression" dxfId="217" priority="484">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74:V74">
-    <cfRule type="expression" dxfId="224" priority="483">
+    <cfRule type="expression" dxfId="216" priority="483">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74">
-    <cfRule type="expression" dxfId="223" priority="480">
+    <cfRule type="expression" dxfId="215" priority="480">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="222" priority="473">
+    <cfRule type="expression" dxfId="214" priority="473">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:F29">
-    <cfRule type="expression" dxfId="221" priority="478">
+    <cfRule type="expression" dxfId="213" priority="478">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42:B43 E42:E43 L42:V43 G42:G43">
-    <cfRule type="expression" dxfId="220" priority="477">
+    <cfRule type="expression" dxfId="212" priority="477">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:G4 C8:D8 C12:D12 C16:D16 C20:D20 C24:D24 C44:D44 C63:D63 C84:D84 C28:D28 C48:D48 C67:D67 C32:D32 C52:D52 C71:D71 C36:D36 C39:D39 C75:D75 C41:D41 C59:D59 C80:D80">
-    <cfRule type="expression" dxfId="219" priority="472">
+    <cfRule type="expression" dxfId="211" priority="472">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="218" priority="471">
+    <cfRule type="expression" dxfId="210" priority="471">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 E6:H6 J6:V6">
-    <cfRule type="expression" dxfId="217" priority="469">
+    <cfRule type="expression" dxfId="209" priority="469">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:V5">
-    <cfRule type="expression" dxfId="216" priority="466">
+    <cfRule type="expression" dxfId="208" priority="466">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:L4">
-    <cfRule type="expression" dxfId="215" priority="461">
+    <cfRule type="expression" dxfId="207" priority="461">
       <formula>K$1=$H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:V4">
-    <cfRule type="expression" dxfId="214" priority="462">
+    <cfRule type="expression" dxfId="206" priority="462">
       <formula>K$1=$I4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:V4">
-    <cfRule type="expression" dxfId="213" priority="463">
+    <cfRule type="expression" dxfId="205" priority="463">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="212" priority="456">
+    <cfRule type="expression" dxfId="204" priority="456">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 E8:G10">
-    <cfRule type="expression" dxfId="211" priority="455">
+    <cfRule type="expression" dxfId="203" priority="455">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:K8">
-    <cfRule type="expression" dxfId="210" priority="453">
+    <cfRule type="expression" dxfId="202" priority="453">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:H15 J15:V15">
-    <cfRule type="expression" dxfId="209" priority="445">
+    <cfRule type="expression" dxfId="201" priority="445">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15 J15:V15">
-    <cfRule type="expression" dxfId="208" priority="442">
+    <cfRule type="expression" dxfId="200" priority="442">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:V15">
-    <cfRule type="expression" dxfId="207" priority="443">
+    <cfRule type="expression" dxfId="199" priority="443">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:G15">
-    <cfRule type="expression" dxfId="206" priority="441">
+    <cfRule type="expression" dxfId="198" priority="441">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="205" priority="299">
+    <cfRule type="expression" dxfId="197" priority="299">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="204" priority="438">
+    <cfRule type="expression" dxfId="196" priority="438">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="203" priority="435">
+    <cfRule type="expression" dxfId="195" priority="435">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="202" priority="436">
+    <cfRule type="expression" dxfId="194" priority="436">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46 J46:V46">
-    <cfRule type="expression" dxfId="201" priority="330">
+    <cfRule type="expression" dxfId="193" priority="330">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19 E19:H19 J19:V19">
-    <cfRule type="expression" dxfId="200" priority="431">
+    <cfRule type="expression" dxfId="192" priority="431">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="199" priority="287">
+    <cfRule type="expression" dxfId="191" priority="287">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26 J26:K26">
-    <cfRule type="expression" dxfId="198" priority="393">
+    <cfRule type="expression" dxfId="190" priority="393">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:J57">
-    <cfRule type="expression" dxfId="197" priority="325">
+    <cfRule type="expression" dxfId="189" priority="325">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20 J20:K20">
-    <cfRule type="expression" dxfId="196" priority="420">
+    <cfRule type="expression" dxfId="188" priority="420">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21 J21:K21">
-    <cfRule type="expression" dxfId="195" priority="415">
+    <cfRule type="expression" dxfId="187" priority="415">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
-    <cfRule type="expression" dxfId="194" priority="320">
+    <cfRule type="expression" dxfId="186" priority="320">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
-    <cfRule type="expression" dxfId="193" priority="319">
+    <cfRule type="expression" dxfId="185" priority="319">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23 J23:K23">
-    <cfRule type="expression" dxfId="192" priority="408">
+    <cfRule type="expression" dxfId="184" priority="408">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59">
-    <cfRule type="expression" dxfId="191" priority="316">
+    <cfRule type="expression" dxfId="183" priority="316">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24 J24:K24">
-    <cfRule type="expression" dxfId="190" priority="403">
+    <cfRule type="expression" dxfId="182" priority="403">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59 J59">
-    <cfRule type="expression" dxfId="189" priority="314">
+    <cfRule type="expression" dxfId="181" priority="314">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25 J25:K25">
-    <cfRule type="expression" dxfId="188" priority="398">
+    <cfRule type="expression" dxfId="180" priority="398">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K60">
-    <cfRule type="expression" dxfId="187" priority="311">
+    <cfRule type="expression" dxfId="179" priority="311">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H60 J60">
-    <cfRule type="expression" dxfId="186" priority="310">
+    <cfRule type="expression" dxfId="178" priority="310">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K61">
-    <cfRule type="expression" dxfId="185" priority="308">
+    <cfRule type="expression" dxfId="177" priority="308">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K61">
-    <cfRule type="expression" dxfId="184" priority="307">
+    <cfRule type="expression" dxfId="176" priority="307">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27 J27:K27">
-    <cfRule type="expression" dxfId="183" priority="388">
+    <cfRule type="expression" dxfId="175" priority="388">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62">
-    <cfRule type="expression" dxfId="182" priority="304">
+    <cfRule type="expression" dxfId="174" priority="304">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28 J28:K28">
-    <cfRule type="expression" dxfId="181" priority="383">
+    <cfRule type="expression" dxfId="173" priority="383">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62 J62">
-    <cfRule type="expression" dxfId="180" priority="302">
+    <cfRule type="expression" dxfId="172" priority="302">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29 J29:K29">
-    <cfRule type="expression" dxfId="179" priority="378">
+    <cfRule type="expression" dxfId="171" priority="378">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63 J63">
-    <cfRule type="expression" dxfId="178" priority="298">
+    <cfRule type="expression" dxfId="170" priority="298">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30 J30:K30">
-    <cfRule type="expression" dxfId="177" priority="373">
+    <cfRule type="expression" dxfId="169" priority="373">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="176" priority="296">
+    <cfRule type="expression" dxfId="168" priority="296">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="175" priority="295">
+    <cfRule type="expression" dxfId="167" priority="295">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31 J31:K31">
-    <cfRule type="expression" dxfId="174" priority="368">
+    <cfRule type="expression" dxfId="166" priority="368">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="173" priority="292">
+    <cfRule type="expression" dxfId="165" priority="292">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65 J65">
-    <cfRule type="expression" dxfId="172" priority="290">
+    <cfRule type="expression" dxfId="164" priority="290">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="expression" dxfId="171" priority="356">
+    <cfRule type="expression" dxfId="163" priority="356">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="170" priority="288">
+    <cfRule type="expression" dxfId="162" priority="288">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="169" priority="353">
+    <cfRule type="expression" dxfId="161" priority="353">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="168" priority="350">
+    <cfRule type="expression" dxfId="160" priority="350">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66 J66">
-    <cfRule type="expression" dxfId="167" priority="286">
+    <cfRule type="expression" dxfId="159" priority="286">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="166" priority="347">
+    <cfRule type="expression" dxfId="158" priority="347">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38:B39 J38:V38 E38:H38 E39:G39 L39:V39">
-    <cfRule type="expression" dxfId="165" priority="344">
+    <cfRule type="expression" dxfId="157" priority="344">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J40:V40 B40:B43 E42:E43 E40:H40 G42:G43 E41:G41 L41:V43">
-    <cfRule type="expression" dxfId="164" priority="340">
+    <cfRule type="expression" dxfId="156" priority="340">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="163" priority="284">
+    <cfRule type="expression" dxfId="155" priority="284">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="162" priority="283">
+    <cfRule type="expression" dxfId="154" priority="283">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46:G46 B46">
-    <cfRule type="expression" dxfId="161" priority="333">
+    <cfRule type="expression" dxfId="153" priority="333">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I78">
-    <cfRule type="expression" dxfId="160" priority="190">
+    <cfRule type="expression" dxfId="152" priority="190">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="expression" dxfId="159" priority="329">
+    <cfRule type="expression" dxfId="151" priority="329">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50 J50">
-    <cfRule type="expression" dxfId="158" priority="328">
+    <cfRule type="expression" dxfId="150" priority="328">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="157" priority="276">
+    <cfRule type="expression" dxfId="149" priority="276">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="156" priority="279">
+    <cfRule type="expression" dxfId="148" priority="279">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68 J68">
-    <cfRule type="expression" dxfId="155" priority="282">
+    <cfRule type="expression" dxfId="147" priority="282">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58 J58">
-    <cfRule type="expression" dxfId="154" priority="318">
+    <cfRule type="expression" dxfId="146" priority="318">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59">
-    <cfRule type="expression" dxfId="153" priority="315">
+    <cfRule type="expression" dxfId="145" priority="315">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K60">
-    <cfRule type="expression" dxfId="152" priority="312">
+    <cfRule type="expression" dxfId="144" priority="312">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61 J61">
-    <cfRule type="expression" dxfId="151" priority="306">
+    <cfRule type="expression" dxfId="143" priority="306">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62">
-    <cfRule type="expression" dxfId="150" priority="303">
+    <cfRule type="expression" dxfId="142" priority="303">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="149" priority="300">
+    <cfRule type="expression" dxfId="141" priority="300">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64 J64">
-    <cfRule type="expression" dxfId="148" priority="294">
+    <cfRule type="expression" dxfId="140" priority="294">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="147" priority="291">
+    <cfRule type="expression" dxfId="139" priority="291">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="146" priority="280">
+    <cfRule type="expression" dxfId="138" priority="280">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69 J69">
-    <cfRule type="expression" dxfId="145" priority="278">
+    <cfRule type="expression" dxfId="137" priority="278">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="144" priority="275">
+    <cfRule type="expression" dxfId="136" priority="275">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70 J70">
-    <cfRule type="expression" dxfId="143" priority="274">
+    <cfRule type="expression" dxfId="135" priority="274">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="142" priority="272">
+    <cfRule type="expression" dxfId="134" priority="272">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="141" priority="271">
+    <cfRule type="expression" dxfId="133" priority="271">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="140" priority="270">
+    <cfRule type="expression" dxfId="132" priority="270">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J73">
-    <cfRule type="expression" dxfId="139" priority="268">
+    <cfRule type="expression" dxfId="131" priority="268">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73">
-    <cfRule type="expression" dxfId="138" priority="267">
+    <cfRule type="expression" dxfId="130" priority="267">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G78">
-    <cfRule type="expression" dxfId="137" priority="265">
+    <cfRule type="expression" dxfId="129" priority="265">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J78:V78">
-    <cfRule type="expression" dxfId="136" priority="260">
+    <cfRule type="expression" dxfId="128" priority="260">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78 E78:F78">
-    <cfRule type="expression" dxfId="135" priority="262">
+    <cfRule type="expression" dxfId="127" priority="262">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K78:V78">
-    <cfRule type="expression" dxfId="134" priority="261">
+    <cfRule type="expression" dxfId="126" priority="261">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78">
-    <cfRule type="expression" dxfId="133" priority="259">
+    <cfRule type="expression" dxfId="125" priority="259">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75">
-    <cfRule type="expression" dxfId="132" priority="256">
+    <cfRule type="expression" dxfId="124" priority="256">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H76">
-    <cfRule type="expression" dxfId="131" priority="254">
+    <cfRule type="expression" dxfId="123" priority="254">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81">
-    <cfRule type="expression" dxfId="130" priority="251">
+    <cfRule type="expression" dxfId="122" priority="251">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="129" priority="108">
+    <cfRule type="expression" dxfId="121" priority="108">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:V81">
-    <cfRule type="expression" dxfId="128" priority="246">
+    <cfRule type="expression" dxfId="120" priority="246">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81 E81:F81">
-    <cfRule type="expression" dxfId="127" priority="248">
+    <cfRule type="expression" dxfId="119" priority="248">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="126" priority="247">
+    <cfRule type="expression" dxfId="118" priority="247">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81">
-    <cfRule type="expression" dxfId="125" priority="245">
+    <cfRule type="expression" dxfId="117" priority="245">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79">
-    <cfRule type="expression" dxfId="124" priority="243">
+    <cfRule type="expression" dxfId="116" priority="243">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82">
-    <cfRule type="expression" dxfId="123" priority="241">
+    <cfRule type="expression" dxfId="115" priority="241">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="122" priority="98">
+    <cfRule type="expression" dxfId="114" priority="98">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J82:V82">
-    <cfRule type="expression" dxfId="121" priority="236">
+    <cfRule type="expression" dxfId="113" priority="236">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82 E82:F82">
-    <cfRule type="expression" dxfId="120" priority="238">
+    <cfRule type="expression" dxfId="112" priority="238">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K82:V82">
-    <cfRule type="expression" dxfId="119" priority="237">
+    <cfRule type="expression" dxfId="111" priority="237">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="expression" dxfId="118" priority="235">
+    <cfRule type="expression" dxfId="110" priority="235">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J83">
-    <cfRule type="expression" dxfId="117" priority="233">
+    <cfRule type="expression" dxfId="109" priority="233">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="expression" dxfId="116" priority="232">
+    <cfRule type="expression" dxfId="108" priority="232">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G84">
-    <cfRule type="expression" dxfId="115" priority="230">
+    <cfRule type="expression" dxfId="107" priority="230">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="114" priority="87">
+    <cfRule type="expression" dxfId="106" priority="87">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J84:V84">
-    <cfRule type="expression" dxfId="113" priority="225">
+    <cfRule type="expression" dxfId="105" priority="225">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84 E84:F84">
-    <cfRule type="expression" dxfId="112" priority="227">
+    <cfRule type="expression" dxfId="104" priority="227">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K84:V84">
-    <cfRule type="expression" dxfId="111" priority="226">
+    <cfRule type="expression" dxfId="103" priority="226">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H84">
-    <cfRule type="expression" dxfId="110" priority="224">
+    <cfRule type="expression" dxfId="102" priority="224">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="expression" dxfId="109" priority="222">
+    <cfRule type="expression" dxfId="101" priority="222">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42 J42">
-    <cfRule type="expression" dxfId="108" priority="220">
+    <cfRule type="expression" dxfId="100" priority="220">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:K37">
-    <cfRule type="expression" dxfId="107" priority="217">
+    <cfRule type="expression" dxfId="99" priority="217">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="106" priority="215">
+    <cfRule type="expression" dxfId="98" priority="215">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="105" priority="73">
+    <cfRule type="expression" dxfId="97" priority="73">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50">
-    <cfRule type="expression" dxfId="104" priority="211">
+    <cfRule type="expression" dxfId="96" priority="211">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I62">
-    <cfRule type="expression" dxfId="103" priority="204">
+    <cfRule type="expression" dxfId="95" priority="204">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I58">
-    <cfRule type="expression" dxfId="102" priority="208">
+    <cfRule type="expression" dxfId="94" priority="208">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I59">
-    <cfRule type="expression" dxfId="101" priority="207">
+    <cfRule type="expression" dxfId="93" priority="207">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I60">
-    <cfRule type="expression" dxfId="100" priority="206">
+    <cfRule type="expression" dxfId="92" priority="206">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61">
-    <cfRule type="expression" dxfId="99" priority="205">
+    <cfRule type="expression" dxfId="91" priority="205">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="98" priority="203">
+    <cfRule type="expression" dxfId="90" priority="203">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64">
-    <cfRule type="expression" dxfId="97" priority="202">
+    <cfRule type="expression" dxfId="89" priority="202">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I65">
-    <cfRule type="expression" dxfId="96" priority="201">
+    <cfRule type="expression" dxfId="88" priority="201">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I66">
-    <cfRule type="expression" dxfId="95" priority="200">
+    <cfRule type="expression" dxfId="87" priority="200">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I67">
-    <cfRule type="expression" dxfId="94" priority="199">
+    <cfRule type="expression" dxfId="86" priority="199">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I68">
-    <cfRule type="expression" dxfId="93" priority="198">
+    <cfRule type="expression" dxfId="85" priority="198">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="92" priority="197">
+    <cfRule type="expression" dxfId="84" priority="197">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="91" priority="196">
+    <cfRule type="expression" dxfId="83" priority="196">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I71">
-    <cfRule type="expression" dxfId="90" priority="195">
+    <cfRule type="expression" dxfId="82" priority="195">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I73">
-    <cfRule type="expression" dxfId="89" priority="194">
+    <cfRule type="expression" dxfId="81" priority="194">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74">
-    <cfRule type="expression" dxfId="88" priority="193">
+    <cfRule type="expression" dxfId="80" priority="193">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I75">
-    <cfRule type="expression" dxfId="87" priority="192">
+    <cfRule type="expression" dxfId="79" priority="192">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76">
-    <cfRule type="expression" dxfId="86" priority="191">
+    <cfRule type="expression" dxfId="78" priority="191">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I79">
-    <cfRule type="expression" dxfId="85" priority="189">
+    <cfRule type="expression" dxfId="77" priority="189">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81">
-    <cfRule type="expression" dxfId="84" priority="188">
+    <cfRule type="expression" dxfId="76" priority="188">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I82">
-    <cfRule type="expression" dxfId="83" priority="187">
+    <cfRule type="expression" dxfId="75" priority="187">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I83">
-    <cfRule type="expression" dxfId="82" priority="186">
+    <cfRule type="expression" dxfId="74" priority="186">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I84">
-    <cfRule type="expression" dxfId="81" priority="185">
+    <cfRule type="expression" dxfId="73" priority="185">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I85">
-    <cfRule type="expression" dxfId="80" priority="184">
+    <cfRule type="expression" dxfId="72" priority="184">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="expression" dxfId="79" priority="183">
+    <cfRule type="expression" dxfId="71" priority="183">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="78" priority="182">
+    <cfRule type="expression" dxfId="70" priority="182">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="77" priority="181">
+    <cfRule type="expression" dxfId="69" priority="181">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="expression" dxfId="76" priority="180">
+    <cfRule type="expression" dxfId="68" priority="180">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="75" priority="179">
+    <cfRule type="expression" dxfId="67" priority="179">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="74" priority="178">
+    <cfRule type="expression" dxfId="66" priority="178">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="73" priority="177">
+    <cfRule type="expression" dxfId="65" priority="177">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="72" priority="176">
+    <cfRule type="expression" dxfId="64" priority="176">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="71" priority="175">
+    <cfRule type="expression" dxfId="63" priority="175">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="70" priority="107">
+    <cfRule type="expression" dxfId="62" priority="107">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="expression" dxfId="69" priority="106">
+    <cfRule type="expression" dxfId="61" priority="106">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="expression" dxfId="68" priority="105">
+    <cfRule type="expression" dxfId="60" priority="105">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="67" priority="104">
+    <cfRule type="expression" dxfId="59" priority="104">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="66" priority="103">
+    <cfRule type="expression" dxfId="58" priority="103">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="65" priority="97">
+    <cfRule type="expression" dxfId="57" priority="97">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="expression" dxfId="64" priority="101">
+    <cfRule type="expression" dxfId="56" priority="101">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" dxfId="63" priority="100">
+    <cfRule type="expression" dxfId="55" priority="100">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="expression" dxfId="62" priority="99">
+    <cfRule type="expression" dxfId="54" priority="99">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="61" priority="96">
+    <cfRule type="expression" dxfId="53" priority="96">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="expression" dxfId="60" priority="95">
+    <cfRule type="expression" dxfId="52" priority="95">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26">
-    <cfRule type="expression" dxfId="59" priority="94">
+    <cfRule type="expression" dxfId="51" priority="94">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="expression" dxfId="58" priority="93">
+    <cfRule type="expression" dxfId="50" priority="93">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="57" priority="92">
+    <cfRule type="expression" dxfId="49" priority="92">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="56" priority="91">
+    <cfRule type="expression" dxfId="48" priority="91">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="expression" dxfId="55" priority="90">
+    <cfRule type="expression" dxfId="47" priority="90">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31">
-    <cfRule type="expression" dxfId="54" priority="89">
+    <cfRule type="expression" dxfId="46" priority="89">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="53" priority="86">
+    <cfRule type="expression" dxfId="45" priority="86">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="52" priority="72">
+    <cfRule type="expression" dxfId="44" priority="72">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="51" priority="84">
+    <cfRule type="expression" dxfId="43" priority="84">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="expression" dxfId="50" priority="83">
+    <cfRule type="expression" dxfId="42" priority="83">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="expression" dxfId="49" priority="82">
+    <cfRule type="expression" dxfId="41" priority="82">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="expression" dxfId="48" priority="81">
+    <cfRule type="expression" dxfId="40" priority="81">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="47" priority="80">
+    <cfRule type="expression" dxfId="39" priority="80">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="46" priority="79">
+    <cfRule type="expression" dxfId="38" priority="79">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="45" priority="78">
+    <cfRule type="expression" dxfId="37" priority="78">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="44" priority="76">
+    <cfRule type="expression" dxfId="36" priority="76">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45">
-    <cfRule type="expression" dxfId="43" priority="74">
+    <cfRule type="expression" dxfId="35" priority="74">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:V10">
-    <cfRule type="expression" dxfId="42" priority="64">
+    <cfRule type="expression" dxfId="34" priority="64">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="41" priority="53">
+    <cfRule type="expression" dxfId="33" priority="53">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80">
-    <cfRule type="expression" dxfId="40" priority="62">
+    <cfRule type="expression" dxfId="32" priority="62">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I80">
-    <cfRule type="expression" dxfId="39" priority="61">
+    <cfRule type="expression" dxfId="31" priority="61">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:K9">
-    <cfRule type="expression" dxfId="38" priority="52">
+    <cfRule type="expression" dxfId="30" priority="52">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="37" priority="51">
+    <cfRule type="expression" dxfId="29" priority="51">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="36" priority="54">
+    <cfRule type="expression" dxfId="28" priority="54">
       <formula>K$1=$H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="35" priority="55">
+    <cfRule type="expression" dxfId="27" priority="55">
       <formula>K$1=$I9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="34" priority="49">
+    <cfRule type="expression" dxfId="26" priority="49">
       <formula>K$1=$H10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="33" priority="50">
+    <cfRule type="expression" dxfId="25" priority="50">
       <formula>K$1=$I10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="32" priority="48">
+    <cfRule type="expression" dxfId="24" priority="48">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10:K10">
-    <cfRule type="expression" dxfId="31" priority="47">
+    <cfRule type="expression" dxfId="23" priority="47">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="30" priority="46">
+    <cfRule type="expression" dxfId="22" priority="46">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:F43">
-    <cfRule type="expression" dxfId="29" priority="39">
+    <cfRule type="expression" dxfId="21" priority="39">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43:K43 H43">
-    <cfRule type="expression" dxfId="28" priority="37">
+    <cfRule type="expression" dxfId="20" priority="37">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="27" priority="36">
+    <cfRule type="expression" dxfId="19" priority="36">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:K41 H41">
-    <cfRule type="expression" dxfId="26" priority="34">
+    <cfRule type="expression" dxfId="18" priority="34">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41">
-    <cfRule type="expression" dxfId="25" priority="33">
+    <cfRule type="expression" dxfId="17" priority="33">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="24" priority="24">
+    <cfRule type="expression" dxfId="16" priority="24">
       <formula>K$1=$H18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="23" priority="25">
+    <cfRule type="expression" dxfId="15" priority="25">
       <formula>K$1=$I18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18 J18:K18">
-    <cfRule type="expression" dxfId="22" priority="26">
+    <cfRule type="expression" dxfId="14" priority="26">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="21" priority="23">
+    <cfRule type="expression" dxfId="13" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="12" priority="21">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J72:K72">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="11" priority="20">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="10" priority="19">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I72">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="9" priority="18">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="8" priority="17">
       <formula>K$1=$H39</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39:K39 H39">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="7" priority="16">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="6" priority="15">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Move Joseph Howan up 1 hour
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0640421-B2B7-EB48-818E-D0C23C6134E1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5029BCB7-C3B3-544C-81C9-646C2F0FA6DD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17560" yWindow="6120" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1095,7 +1095,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1183,6 +1183,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1191,7 +1194,14 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="269">
+  <dxfs count="270">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1216,149 +1226,149 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3408,8 +3418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4958,24 +4968,24 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="47"/>
+      <c r="A21" s="52"/>
       <c r="B21" s="18" t="s">
-        <v>43</v>
+        <v>235</v>
       </c>
       <c r="C21" s="7">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D21" s="7">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>141</v>
+        <v>236</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="G21" s="51" t="s">
+        <v>238</v>
       </c>
       <c r="H21" s="29" t="s">
         <v>206</v>
@@ -5036,100 +5046,100 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="18" t="s">
-        <v>180</v>
+        <v>43</v>
       </c>
       <c r="C22" s="7">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="7">
-        <v>21</v>
-      </c>
-      <c r="E22" s="20"/>
+        <v>20</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="F22" s="7" t="s">
-        <v>207</v>
+        <v>71</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I22" s="23">
-        <v>0.70833333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J22" s="30" t="s">
         <v>14</v>
       </c>
       <c r="K22" s="11">
         <f>$I22+Sheet2!B$1/24</f>
-        <v>1.125</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="L22" s="23">
         <f>$I22+Sheet2!B$2/24</f>
-        <v>1.0833333333333335</v>
+        <v>1.0416666666666665</v>
       </c>
       <c r="M22" s="23">
         <f>$I22+Sheet2!B$3/24</f>
-        <v>1.0416666666666667</v>
+        <v>1</v>
       </c>
       <c r="N22" s="23">
         <f>$I22+Sheet2!B$4/24</f>
-        <v>0.83333333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="O22" s="23">
         <f>$I22+Sheet2!B$5/24</f>
-        <v>0.83333333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="P22" s="23">
         <f>$I22+Sheet2!B$6/24</f>
-        <v>0.83333333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="Q22" s="23">
         <f>$I22+Sheet2!B$7/24</f>
-        <v>0.79166666666666674</v>
+        <v>0.75</v>
       </c>
       <c r="R22" s="23">
         <f>$I22+Sheet2!B$8/24</f>
-        <v>0.75</v>
+        <v>0.70833333333333326</v>
       </c>
       <c r="S22" s="23">
         <f>$I22+Sheet2!B$9/24</f>
-        <v>0.54166666666666674</v>
+        <v>0.5</v>
       </c>
       <c r="T22" s="23">
         <f>$I22+Sheet2!B$10/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333326</v>
       </c>
       <c r="U22" s="23">
         <f>$I22+Sheet2!B$11/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="V22" s="23">
         <f>$I22+Sheet2!B$12/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.37499999999999994</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="41"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="18" t="s">
-        <v>50</v>
+        <v>180</v>
       </c>
       <c r="C23" s="7">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="7">
-        <v>22</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>45</v>
+        <v>21</v>
+      </c>
+      <c r="E23" s="20"/>
+      <c r="F23" s="7" t="s">
+        <v>207</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H23" s="29" t="s">
         <v>208</v>
@@ -5189,25 +5199,25 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="52" t="s">
-        <v>26</v>
-      </c>
+    <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="41"/>
       <c r="B24" s="18" t="s">
-        <v>185</v>
+        <v>50</v>
       </c>
       <c r="C24" s="7">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="7">
-        <v>23</v>
-      </c>
-      <c r="E24" s="20"/>
+        <v>22</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>19</v>
+      </c>
       <c r="F24" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="48" t="s">
-        <v>186</v>
+      <c r="G24" s="29" t="s">
+        <v>130</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>208</v>
@@ -5222,70 +5232,70 @@
         <f>$I24+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L24" s="16">
+      <c r="L24" s="23">
         <f>$I24+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M24" s="16">
+      <c r="M24" s="23">
         <f>$I24+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N24" s="16">
+      <c r="N24" s="23">
         <f>$I24+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O24" s="16">
+      <c r="O24" s="23">
         <f>$I24+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P24" s="16">
+      <c r="P24" s="23">
         <f>$I24+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q24" s="16">
+      <c r="Q24" s="23">
         <f>$I24+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R24" s="16">
+      <c r="R24" s="23">
         <f>$I24+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S24" s="16">
+      <c r="S24" s="23">
         <f>$I24+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T24" s="16">
+      <c r="T24" s="23">
         <f>$I24+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U24" s="16">
+      <c r="U24" s="23">
         <f>$I24+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V24" s="16">
+      <c r="V24" s="23">
         <f>$I24+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="52"/>
+      <c r="A25" s="53" t="s">
+        <v>26</v>
+      </c>
       <c r="B25" s="18" t="s">
-        <v>110</v>
+        <v>185</v>
       </c>
       <c r="C25" s="7">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="7">
-        <v>24</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>113</v>
+        <v>23</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="F25" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>208</v>
@@ -5346,24 +5356,24 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="52"/>
+      <c r="A26" s="53"/>
       <c r="B26" s="18" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="C26" s="7">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="7">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G26" s="44" t="s">
-        <v>134</v>
+        <v>111</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>113</v>
       </c>
       <c r="H26" s="29" t="s">
         <v>208</v>
@@ -5378,70 +5388,70 @@
         <f>$I26+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="L26" s="23">
+      <c r="L26" s="16">
         <f>$I26+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="M26" s="23">
+      <c r="M26" s="16">
         <f>$I26+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="N26" s="23">
+      <c r="N26" s="16">
         <f>$I26+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="O26" s="23">
+      <c r="O26" s="16">
         <f>$I26+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P26" s="23">
+      <c r="P26" s="16">
         <f>$I26+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q26" s="23">
+      <c r="Q26" s="16">
         <f>$I26+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="R26" s="23">
+      <c r="R26" s="16">
         <f>$I26+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="S26" s="23">
+      <c r="S26" s="16">
         <f>$I26+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="T26" s="23">
+      <c r="T26" s="16">
         <f>$I26+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="U26" s="23">
+      <c r="U26" s="16">
         <f>$I26+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="V26" s="23">
+      <c r="V26" s="16">
         <f>$I26+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="52"/>
+      <c r="A27" s="53"/>
       <c r="B27" s="18" t="s">
-        <v>235</v>
+        <v>49</v>
       </c>
       <c r="C27" s="7">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="7">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>236</v>
+        <v>15</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="G27" s="51" t="s">
-        <v>238</v>
+        <v>45</v>
+      </c>
+      <c r="G27" s="44" t="s">
+        <v>134</v>
       </c>
       <c r="H27" s="29" t="s">
         <v>208</v>
@@ -5502,7 +5512,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="52"/>
+      <c r="A28" s="53"/>
       <c r="B28" s="18" t="s">
         <v>48</v>
       </c>
@@ -5580,7 +5590,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="52"/>
+      <c r="A29" s="53"/>
       <c r="B29" s="18" t="s">
         <v>38</v>
       </c>
@@ -5658,7 +5668,7 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="52"/>
+      <c r="A30" s="53"/>
       <c r="B30" s="18" t="s">
         <v>121</v>
       </c>
@@ -5736,7 +5746,7 @@
       </c>
     </row>
     <row r="31" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="52"/>
+      <c r="A31" s="53"/>
       <c r="B31" s="12" t="s">
         <v>42</v>
       </c>
@@ -5814,7 +5824,7 @@
       </c>
     </row>
     <row r="32" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="52"/>
+      <c r="A32" s="53"/>
       <c r="B32" s="18" t="s">
         <v>46</v>
       </c>
@@ -5892,7 +5902,7 @@
       </c>
     </row>
     <row r="33" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="52"/>
+      <c r="A33" s="53"/>
       <c r="B33" s="18" t="s">
         <v>209</v>
       </c>
@@ -5966,7 +5976,7 @@
       </c>
     </row>
     <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="52"/>
+      <c r="A34" s="53"/>
       <c r="B34" s="18" t="s">
         <v>126</v>
       </c>
@@ -6044,7 +6054,7 @@
       </c>
     </row>
     <row r="35" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="52"/>
+      <c r="A35" s="53"/>
       <c r="B35" s="18" t="s">
         <v>53</v>
       </c>
@@ -6122,7 +6132,7 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="52"/>
+      <c r="A36" s="53"/>
       <c r="B36" s="12" t="s">
         <v>51</v>
       </c>
@@ -6200,7 +6210,7 @@
       </c>
     </row>
     <row r="37" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="52"/>
+      <c r="A37" s="53"/>
       <c r="B37" s="32" t="s">
         <v>80</v>
       </c>
@@ -6278,7 +6288,7 @@
       </c>
     </row>
     <row r="38" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="52"/>
+      <c r="A38" s="53"/>
       <c r="B38" s="18" t="s">
         <v>52</v>
       </c>
@@ -6356,7 +6366,7 @@
       </c>
     </row>
     <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="52"/>
+      <c r="A39" s="53"/>
       <c r="B39" s="18" t="s">
         <v>212</v>
       </c>
@@ -6430,7 +6440,7 @@
       </c>
     </row>
     <row r="40" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="52"/>
+      <c r="A40" s="53"/>
       <c r="B40" s="18" t="s">
         <v>123</v>
       </c>
@@ -6508,7 +6518,7 @@
       </c>
     </row>
     <row r="41" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="52"/>
+      <c r="A41" s="53"/>
       <c r="B41" s="18" t="s">
         <v>214</v>
       </c>
@@ -6582,7 +6592,7 @@
       </c>
     </row>
     <row r="42" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="52"/>
+      <c r="A42" s="53"/>
       <c r="B42" s="18" t="s">
         <v>31</v>
       </c>
@@ -6660,7 +6670,7 @@
       </c>
     </row>
     <row r="43" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="52"/>
+      <c r="A43" s="53"/>
       <c r="B43" s="18" t="s">
         <v>183</v>
       </c>
@@ -6738,7 +6748,7 @@
       </c>
     </row>
     <row r="44" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="52"/>
+      <c r="A44" s="53"/>
       <c r="B44" s="18" t="s">
         <v>178</v>
       </c>
@@ -6812,7 +6822,7 @@
       </c>
     </row>
     <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="52"/>
+      <c r="A45" s="53"/>
       <c r="B45" s="18" t="s">
         <v>239</v>
       </c>
@@ -6890,7 +6900,7 @@
       </c>
     </row>
     <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="52"/>
+      <c r="A46" s="53"/>
       <c r="B46" s="18" t="s">
         <v>109</v>
       </c>
@@ -6968,7 +6978,7 @@
       </c>
     </row>
     <row r="47" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="52"/>
+      <c r="A47" s="53"/>
       <c r="B47" s="18" t="s">
         <v>98</v>
       </c>
@@ -7046,7 +7056,7 @@
       </c>
     </row>
     <row r="48" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="52"/>
+      <c r="A48" s="53"/>
       <c r="B48" s="18" t="s">
         <v>218</v>
       </c>
@@ -7120,7 +7130,7 @@
       </c>
     </row>
     <row r="49" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="52"/>
+      <c r="A49" s="53"/>
       <c r="B49" s="18" t="s">
         <v>30</v>
       </c>
@@ -7198,7 +7208,7 @@
       </c>
     </row>
     <row r="50" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="53"/>
+      <c r="A50" s="54"/>
       <c r="B50" s="18" t="s">
         <v>99</v>
       </c>
@@ -7272,7 +7282,7 @@
       </c>
     </row>
     <row r="51" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="53"/>
+      <c r="A51" s="54"/>
       <c r="B51" s="18" t="s">
         <v>82</v>
       </c>
@@ -7350,7 +7360,7 @@
       </c>
     </row>
     <row r="52" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="53"/>
+      <c r="A52" s="54"/>
       <c r="B52" s="18" t="s">
         <v>90</v>
       </c>
@@ -7428,7 +7438,7 @@
       </c>
     </row>
     <row r="53" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="53"/>
+      <c r="A53" s="54"/>
       <c r="B53" s="12" t="s">
         <v>33</v>
       </c>
@@ -7506,7 +7516,7 @@
       </c>
     </row>
     <row r="54" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="53"/>
+      <c r="A54" s="54"/>
       <c r="B54" s="12" t="s">
         <v>36</v>
       </c>
@@ -7584,7 +7594,7 @@
       </c>
     </row>
     <row r="55" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="53"/>
+      <c r="A55" s="54"/>
       <c r="B55" s="18" t="s">
         <v>32</v>
       </c>
@@ -7662,7 +7672,7 @@
       </c>
     </row>
     <row r="56" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="53"/>
+      <c r="A56" s="54"/>
       <c r="B56" s="18" t="s">
         <v>34</v>
       </c>
@@ -7740,7 +7750,7 @@
       </c>
     </row>
     <row r="57" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="53"/>
+      <c r="A57" s="54"/>
       <c r="B57" s="18" t="s">
         <v>94</v>
       </c>
@@ -7818,7 +7828,7 @@
       </c>
     </row>
     <row r="58" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="53"/>
+      <c r="A58" s="54"/>
       <c r="B58" s="18" t="s">
         <v>44</v>
       </c>
@@ -7896,7 +7906,7 @@
       </c>
     </row>
     <row r="59" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="53"/>
+      <c r="A59" s="54"/>
       <c r="B59" s="18" t="s">
         <v>103</v>
       </c>
@@ -7970,7 +7980,7 @@
       </c>
     </row>
     <row r="60" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="53"/>
+      <c r="A60" s="54"/>
       <c r="B60" s="35" t="s">
         <v>95</v>
       </c>
@@ -8048,7 +8058,7 @@
       </c>
     </row>
     <row r="61" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="53"/>
+      <c r="A61" s="54"/>
       <c r="B61" s="35" t="s">
         <v>59</v>
       </c>
@@ -8126,7 +8136,7 @@
       </c>
     </row>
     <row r="62" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="53"/>
+      <c r="A62" s="54"/>
       <c r="B62" s="35" t="s">
         <v>57</v>
       </c>
@@ -8204,7 +8214,7 @@
       </c>
     </row>
     <row r="63" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="53"/>
+      <c r="A63" s="54"/>
       <c r="B63" s="18" t="s">
         <v>89</v>
       </c>
@@ -8282,7 +8292,7 @@
       </c>
     </row>
     <row r="64" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="53"/>
+      <c r="A64" s="54"/>
       <c r="B64" s="18" t="s">
         <v>181</v>
       </c>
@@ -8360,7 +8370,7 @@
       </c>
     </row>
     <row r="65" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="53"/>
+      <c r="A65" s="54"/>
       <c r="B65" s="18" t="s">
         <v>60</v>
       </c>
@@ -8438,7 +8448,7 @@
       </c>
     </row>
     <row r="66" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="53"/>
+      <c r="A66" s="54"/>
       <c r="B66" s="35" t="s">
         <v>63</v>
       </c>
@@ -8516,7 +8526,7 @@
       </c>
     </row>
     <row r="67" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="53"/>
+      <c r="A67" s="54"/>
       <c r="B67" s="35" t="s">
         <v>61</v>
       </c>
@@ -8594,7 +8604,7 @@
       </c>
     </row>
     <row r="68" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="53"/>
+      <c r="A68" s="54"/>
       <c r="B68" s="18" t="s">
         <v>58</v>
       </c>
@@ -8672,7 +8682,7 @@
       </c>
     </row>
     <row r="69" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="53"/>
+      <c r="A69" s="54"/>
       <c r="B69" s="12" t="s">
         <v>91</v>
       </c>
@@ -8750,7 +8760,7 @@
       </c>
     </row>
     <row r="70" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="53"/>
+      <c r="A70" s="54"/>
       <c r="B70" s="18" t="s">
         <v>56</v>
       </c>
@@ -8828,7 +8838,7 @@
       </c>
     </row>
     <row r="71" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="53"/>
+      <c r="A71" s="54"/>
       <c r="B71" s="18" t="s">
         <v>62</v>
       </c>
@@ -8906,7 +8916,7 @@
       </c>
     </row>
     <row r="72" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="53"/>
+      <c r="A72" s="54"/>
       <c r="B72" s="18" t="s">
         <v>55</v>
       </c>
@@ -8984,7 +8994,7 @@
       </c>
     </row>
     <row r="73" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="53"/>
+      <c r="A73" s="54"/>
       <c r="B73" s="18" t="s">
         <v>117</v>
       </c>
@@ -9058,7 +9068,7 @@
       </c>
     </row>
     <row r="74" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="53"/>
+      <c r="A74" s="54"/>
       <c r="B74" s="18" t="s">
         <v>54</v>
       </c>
@@ -9136,7 +9146,7 @@
       </c>
     </row>
     <row r="75" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="53"/>
+      <c r="A75" s="54"/>
       <c r="B75" s="18" t="s">
         <v>118</v>
       </c>
@@ -9210,7 +9220,7 @@
       </c>
     </row>
     <row r="76" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="53"/>
+      <c r="A76" s="54"/>
       <c r="B76" s="18" t="s">
         <v>67</v>
       </c>
@@ -9288,7 +9298,7 @@
       </c>
     </row>
     <row r="77" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="53"/>
+      <c r="A77" s="54"/>
       <c r="B77" s="35" t="s">
         <v>66</v>
       </c>
@@ -9366,7 +9376,7 @@
       </c>
     </row>
     <row r="78" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="53"/>
+      <c r="A78" s="54"/>
       <c r="B78" s="18" t="s">
         <v>234</v>
       </c>
@@ -9444,7 +9454,7 @@
       </c>
     </row>
     <row r="79" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="53"/>
+      <c r="A79" s="54"/>
       <c r="B79" s="18" t="s">
         <v>223</v>
       </c>
@@ -9518,7 +9528,7 @@
       </c>
     </row>
     <row r="80" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="53"/>
+      <c r="A80" s="54"/>
       <c r="B80" s="18" t="s">
         <v>65</v>
       </c>
@@ -9596,7 +9606,7 @@
       </c>
     </row>
     <row r="81" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="53"/>
+      <c r="A81" s="54"/>
       <c r="B81" s="18" t="s">
         <v>29</v>
       </c>
@@ -9674,7 +9684,7 @@
       </c>
     </row>
     <row r="82" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="53"/>
+      <c r="A82" s="54"/>
       <c r="B82" s="18" t="s">
         <v>226</v>
       </c>
@@ -9748,7 +9758,7 @@
       </c>
     </row>
     <row r="83" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="53"/>
+      <c r="A83" s="54"/>
       <c r="B83" s="18" t="s">
         <v>229</v>
       </c>
@@ -9822,7 +9832,7 @@
       </c>
     </row>
     <row r="84" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="53"/>
+      <c r="A84" s="54"/>
       <c r="B84" s="35" t="s">
         <v>64</v>
       </c>
@@ -9900,7 +9910,7 @@
       </c>
     </row>
     <row r="85" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="53"/>
+      <c r="A85" s="54"/>
       <c r="B85" s="18" t="s">
         <v>232</v>
       </c>
@@ -10055,1355 +10065,1360 @@
     <sortCondition ref="D2:D70"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
-    <mergeCell ref="A24:A49"/>
+    <mergeCell ref="A25:A49"/>
     <mergeCell ref="A50:A85"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 L40:V40 K41:V44 K19:V39 K46:V86">
-    <cfRule type="expression" dxfId="268" priority="635">
+  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V86">
+    <cfRule type="expression" dxfId="269" priority="640">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K22:V22 K17:V17 K19:V19 K20:K21 K23:K32">
-    <cfRule type="expression" dxfId="267" priority="637">
+  <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K17:V17 K19:V19 K23:V23 K20 K24:K32 K22">
+    <cfRule type="expression" dxfId="268" priority="642">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K52:V52 G52 G61 B62:B64 G71 G86 E59:G59 G30 B72 E72:G72 B3 E3:H3 H7 L10:V10 E20:G21 L20:V21 E22:H22 E31:G32 J22:V22 E33:H33 J33:V37 E49:G49 J49:V49 G63:G67 B68:B70 E68:G70 L40:V40 L61:V72 K84:V84 G84 K76:V77 K80:V81 K86:V86 L38:V38 E34:G38 E50:V51 G57:V57 H2 J2:V3 E40:G40 B81 J11:V14 B20:B26 E23:G26 J81:V81 B5 E53:V56 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L74:V74 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E81:G81 B74 E58:V58 E62:G62 B49:B59 B40 B44:B45 B78 B47 J47:V47 G73:G77 E28:G29 B28:B38 L23:V32 E44:H44 E45:G45 E5:G5 E47:H47 E78:G78 E74:G74">
-    <cfRule type="expression" dxfId="266" priority="641">
+  <conditionalFormatting sqref="K52:V52 G52 G61 B62:B64 G71 G86 E59:G59 G30 B72 E72:G72 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E49:G49 J49:V49 G63:G67 B68:B70 E68:G70 L40:V40 L61:V72 K84:V84 G84 K76:V77 K80:V81 K86:V86 L38:V38 E34:G38 E50:V51 G57:V57 H2 J2:V3 E40:G40 B81 J11:V14 J81:V81 B5 E53:V56 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L74:V74 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E81:G81 B74 E58:V58 E62:G62 B49:B59 B40 B44:B45 B78 B47 J47:V47 G73:G77 E24:G29 B20:B38 E44:H44 E45:G45 E5:G5 E47:H47 E78:G78 E74:G74 L24:V32 L20:V20 C4:D86 L22:V22">
+    <cfRule type="expression" dxfId="267" priority="646">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61 L61:V61">
-    <cfRule type="expression" dxfId="265" priority="618">
+    <cfRule type="expression" dxfId="266" priority="623">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65 L65:V65">
-    <cfRule type="expression" dxfId="264" priority="616">
+    <cfRule type="expression" dxfId="265" priority="621">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67 L67:V67">
-    <cfRule type="expression" dxfId="263" priority="614">
+    <cfRule type="expression" dxfId="264" priority="619">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71 L71:V71">
-    <cfRule type="expression" dxfId="262" priority="612">
+    <cfRule type="expression" dxfId="263" priority="617">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66 L66:V66">
-    <cfRule type="expression" dxfId="261" priority="610">
+    <cfRule type="expression" dxfId="262" priority="615">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84 K84:V84 E84:F84">
-    <cfRule type="expression" dxfId="260" priority="606">
+    <cfRule type="expression" dxfId="261" priority="611">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="expression" dxfId="259" priority="604">
+    <cfRule type="expression" dxfId="260" priority="609">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E71">
-    <cfRule type="expression" dxfId="258" priority="601">
+    <cfRule type="expression" dxfId="259" priority="606">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="expression" dxfId="257" priority="600">
+    <cfRule type="expression" dxfId="258" priority="605">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:B81 J80:V81">
-    <cfRule type="expression" dxfId="256" priority="597">
+    <cfRule type="expression" dxfId="257" priority="602">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77:B78 J77:V77 E77:E78">
-    <cfRule type="expression" dxfId="255" priority="595">
+    <cfRule type="expression" dxfId="256" priority="600">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E80:F81">
-    <cfRule type="expression" dxfId="254" priority="593">
+    <cfRule type="expression" dxfId="255" priority="598">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76 J76:V76">
-    <cfRule type="expression" dxfId="253" priority="591">
+    <cfRule type="expression" dxfId="254" priority="596">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86 J86:V86 E86">
-    <cfRule type="expression" dxfId="252" priority="589">
+    <cfRule type="expression" dxfId="253" priority="594">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66">
-    <cfRule type="expression" dxfId="251" priority="581">
+    <cfRule type="expression" dxfId="252" priority="586">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59:V59">
-    <cfRule type="expression" dxfId="250" priority="521">
+    <cfRule type="expression" dxfId="251" priority="526">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71">
-    <cfRule type="expression" dxfId="249" priority="543">
+    <cfRule type="expression" dxfId="250" priority="548">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73:B74 E73:F74">
-    <cfRule type="expression" dxfId="248" priority="507">
+    <cfRule type="expression" dxfId="249" priority="512">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="expression" dxfId="247" priority="528">
+    <cfRule type="expression" dxfId="248" priority="533">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65:F65">
-    <cfRule type="expression" dxfId="246" priority="535">
+    <cfRule type="expression" dxfId="247" priority="540">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60 L60:V60">
-    <cfRule type="expression" dxfId="245" priority="529">
+    <cfRule type="expression" dxfId="246" priority="534">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F77:F78">
-    <cfRule type="expression" dxfId="244" priority="541">
+    <cfRule type="expression" dxfId="245" priority="546">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61">
-    <cfRule type="expression" dxfId="243" priority="537">
+    <cfRule type="expression" dxfId="244" priority="542">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67:F67">
-    <cfRule type="expression" dxfId="242" priority="536">
+    <cfRule type="expression" dxfId="243" priority="541">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76:F76">
-    <cfRule type="expression" dxfId="241" priority="534">
+    <cfRule type="expression" dxfId="242" priority="539">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L60:V60 G60">
-    <cfRule type="expression" dxfId="240" priority="531">
+    <cfRule type="expression" dxfId="241" priority="536">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:V7">
-    <cfRule type="expression" dxfId="239" priority="476">
+    <cfRule type="expression" dxfId="240" priority="481">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60">
-    <cfRule type="expression" dxfId="238" priority="525">
+    <cfRule type="expression" dxfId="239" priority="530">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:V47">
-    <cfRule type="expression" dxfId="237" priority="645">
+    <cfRule type="expression" dxfId="238" priority="650">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59:V59">
-    <cfRule type="expression" dxfId="236" priority="522">
+    <cfRule type="expression" dxfId="237" priority="527">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:V10">
-    <cfRule type="expression" dxfId="235" priority="467">
+    <cfRule type="expression" dxfId="236" priority="472">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H14 J13:V14 L18:V18">
-    <cfRule type="expression" dxfId="234" priority="513">
+    <cfRule type="expression" dxfId="235" priority="518">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:V14 L18:V18">
-    <cfRule type="expression" dxfId="233" priority="514">
+    <cfRule type="expression" dxfId="234" priority="519">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G3 B7 E7:G7 C4:D86">
-    <cfRule type="expression" dxfId="232" priority="508">
+  <conditionalFormatting sqref="B2:G3 B7 E7:G7">
+    <cfRule type="expression" dxfId="233" priority="513">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73:V73 L74:V74">
-    <cfRule type="expression" dxfId="231" priority="506">
+    <cfRule type="expression" dxfId="232" priority="511">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J73:V73 L74:V74">
-    <cfRule type="expression" dxfId="230" priority="504">
+    <cfRule type="expression" dxfId="231" priority="509">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73">
+    <cfRule type="expression" dxfId="230" priority="508">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J75:V75">
     <cfRule type="expression" dxfId="229" priority="503">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J75:V75">
-    <cfRule type="expression" dxfId="228" priority="498">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B75 E75:F75">
-    <cfRule type="expression" dxfId="227" priority="501">
+    <cfRule type="expression" dxfId="228" priority="506">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K75:V75">
-    <cfRule type="expression" dxfId="226" priority="500">
+    <cfRule type="expression" dxfId="227" priority="505">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75">
-    <cfRule type="expression" dxfId="225" priority="497">
+    <cfRule type="expression" dxfId="226" priority="502">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="224" priority="490">
+    <cfRule type="expression" dxfId="225" priority="495">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:F30">
-    <cfRule type="expression" dxfId="223" priority="495">
+    <cfRule type="expression" dxfId="224" priority="500">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43 E43 L43:V43 G43">
+    <cfRule type="expression" dxfId="223" priority="499">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4 E4:G4">
     <cfRule type="expression" dxfId="222" priority="494">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4 E4:G4">
-    <cfRule type="expression" dxfId="221" priority="489">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="220" priority="488">
+    <cfRule type="expression" dxfId="221" priority="493">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 E6:H6 J6:V6">
-    <cfRule type="expression" dxfId="219" priority="486">
+    <cfRule type="expression" dxfId="220" priority="491">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:V5">
+    <cfRule type="expression" dxfId="219" priority="488">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:L4">
     <cfRule type="expression" dxfId="218" priority="483">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:L4">
-    <cfRule type="expression" dxfId="217" priority="478">
       <formula>K$1=$H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:V4">
-    <cfRule type="expression" dxfId="216" priority="479">
+    <cfRule type="expression" dxfId="217" priority="484">
       <formula>K$1=$I4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:V4">
-    <cfRule type="expression" dxfId="215" priority="480">
+    <cfRule type="expression" dxfId="216" priority="485">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="214" priority="473">
+    <cfRule type="expression" dxfId="215" priority="478">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 E8:G10">
-    <cfRule type="expression" dxfId="213" priority="472">
+    <cfRule type="expression" dxfId="214" priority="477">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:K8">
-    <cfRule type="expression" dxfId="212" priority="470">
+    <cfRule type="expression" dxfId="213" priority="475">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:H15 J15:V15">
-    <cfRule type="expression" dxfId="211" priority="462">
+    <cfRule type="expression" dxfId="212" priority="467">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15 J15:V15">
-    <cfRule type="expression" dxfId="210" priority="459">
+    <cfRule type="expression" dxfId="211" priority="464">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:V15">
-    <cfRule type="expression" dxfId="209" priority="460">
+    <cfRule type="expression" dxfId="210" priority="465">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:G15">
-    <cfRule type="expression" dxfId="208" priority="458">
+    <cfRule type="expression" dxfId="209" priority="463">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="207" priority="316">
+    <cfRule type="expression" dxfId="208" priority="321">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="206" priority="455">
+    <cfRule type="expression" dxfId="207" priority="460">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="205" priority="452">
+    <cfRule type="expression" dxfId="206" priority="457">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="204" priority="453">
+    <cfRule type="expression" dxfId="205" priority="458">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48 J48:V48">
-    <cfRule type="expression" dxfId="203" priority="347">
+    <cfRule type="expression" dxfId="204" priority="352">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19 E19:H19 J19:V19">
-    <cfRule type="expression" dxfId="202" priority="448">
+    <cfRule type="expression" dxfId="203" priority="453">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="201" priority="304">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26 J26:K26 K27">
-    <cfRule type="expression" dxfId="200" priority="410">
+    <cfRule type="expression" dxfId="202" priority="309">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27 J27:K27">
+    <cfRule type="expression" dxfId="201" priority="415">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:J59">
-    <cfRule type="expression" dxfId="199" priority="342">
+    <cfRule type="expression" dxfId="200" priority="347">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20 J20:K20">
+    <cfRule type="expression" dxfId="199" priority="442">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22 J22:K22">
     <cfRule type="expression" dxfId="198" priority="437">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K60">
+    <cfRule type="expression" dxfId="197" priority="342">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K60">
+    <cfRule type="expression" dxfId="196" priority="341">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24 J24:K24">
+    <cfRule type="expression" dxfId="195" priority="430">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K61">
+    <cfRule type="expression" dxfId="194" priority="338">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25 J25:K25">
+    <cfRule type="expression" dxfId="193" priority="425">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H61 J61">
+    <cfRule type="expression" dxfId="192" priority="336">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26 J26:K26">
+    <cfRule type="expression" dxfId="191" priority="420">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="expression" dxfId="190" priority="333">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62 J62">
+    <cfRule type="expression" dxfId="189" priority="332">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="expression" dxfId="188" priority="330">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="expression" dxfId="187" priority="329">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28 J28:K28">
+    <cfRule type="expression" dxfId="186" priority="410">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="expression" dxfId="185" priority="326">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29 J29:K29">
+    <cfRule type="expression" dxfId="184" priority="405">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H64 J64">
+    <cfRule type="expression" dxfId="183" priority="324">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30 J30:K30">
+    <cfRule type="expression" dxfId="182" priority="400">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H65 J65">
+    <cfRule type="expression" dxfId="181" priority="320">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31 J31:K31">
+    <cfRule type="expression" dxfId="180" priority="395">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K66">
+    <cfRule type="expression" dxfId="179" priority="318">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K66">
+    <cfRule type="expression" dxfId="178" priority="317">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32 J32:K32">
+    <cfRule type="expression" dxfId="177" priority="390">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67">
+    <cfRule type="expression" dxfId="176" priority="314">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H67 J67">
+    <cfRule type="expression" dxfId="175" priority="312">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="expression" dxfId="174" priority="378">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K68">
+    <cfRule type="expression" dxfId="173" priority="310">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="expression" dxfId="172" priority="375">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
+    <cfRule type="expression" dxfId="171" priority="372">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H68 J68">
+    <cfRule type="expression" dxfId="170" priority="308">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H37">
+    <cfRule type="expression" dxfId="169" priority="369">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:B40 J39:V39 E39:H39 E40:G40 L40:V40">
+    <cfRule type="expression" dxfId="168" priority="366">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41:V41 B41:B43 E43 E41:H41 G43 E42:G42 L42:V43">
+    <cfRule type="expression" dxfId="167" priority="362">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K70">
+    <cfRule type="expression" dxfId="166" priority="306">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K70">
+    <cfRule type="expression" dxfId="165" priority="305">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48:G48 B48">
+    <cfRule type="expression" dxfId="164" priority="355">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I79">
+    <cfRule type="expression" dxfId="163" priority="212">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H49">
+    <cfRule type="expression" dxfId="162" priority="351">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H52 J52">
+    <cfRule type="expression" dxfId="161" priority="350">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72">
+    <cfRule type="expression" dxfId="160" priority="298">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="159" priority="301">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H70 J70">
+    <cfRule type="expression" dxfId="158" priority="304">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H60 J60">
+    <cfRule type="expression" dxfId="157" priority="340">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K61">
+    <cfRule type="expression" dxfId="156" priority="337">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="expression" dxfId="155" priority="334">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H63 J63">
+    <cfRule type="expression" dxfId="154" priority="328">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="expression" dxfId="153" priority="325">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65">
+    <cfRule type="expression" dxfId="152" priority="322">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66 J66">
+    <cfRule type="expression" dxfId="151" priority="316">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67">
+    <cfRule type="expression" dxfId="150" priority="313">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="149" priority="302">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H71 J71">
+    <cfRule type="expression" dxfId="148" priority="300">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72">
+    <cfRule type="expression" dxfId="147" priority="297">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H72 J72">
+    <cfRule type="expression" dxfId="146" priority="296">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="expression" dxfId="145" priority="294">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="expression" dxfId="144" priority="293">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H69 J69">
+    <cfRule type="expression" dxfId="143" priority="292">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G79">
+    <cfRule type="expression" dxfId="142" priority="287">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J79:V79">
+    <cfRule type="expression" dxfId="141" priority="282">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B79 E79:F79">
+    <cfRule type="expression" dxfId="140" priority="284">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K79:V79">
+    <cfRule type="expression" dxfId="139" priority="283">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H79">
+    <cfRule type="expression" dxfId="138" priority="281">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H76">
+    <cfRule type="expression" dxfId="137" priority="278">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H77">
+    <cfRule type="expression" dxfId="136" priority="276">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G82">
+    <cfRule type="expression" dxfId="135" priority="273">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="expression" dxfId="134" priority="130">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J82:V82">
+    <cfRule type="expression" dxfId="133" priority="268">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82 E82:F82">
+    <cfRule type="expression" dxfId="132" priority="270">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82:V82">
+    <cfRule type="expression" dxfId="131" priority="269">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H82">
+    <cfRule type="expression" dxfId="130" priority="267">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H80">
+    <cfRule type="expression" dxfId="129" priority="265">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G83">
+    <cfRule type="expression" dxfId="128" priority="263">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="expression" dxfId="127" priority="120">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J83:V83">
+    <cfRule type="expression" dxfId="126" priority="258">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83 E83:F83">
+    <cfRule type="expression" dxfId="125" priority="260">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K83:V83">
+    <cfRule type="expression" dxfId="124" priority="259">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H83">
+    <cfRule type="expression" dxfId="123" priority="257">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J84">
+    <cfRule type="expression" dxfId="122" priority="255">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H84">
+    <cfRule type="expression" dxfId="121" priority="254">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G85">
+    <cfRule type="expression" dxfId="120" priority="252">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33">
+    <cfRule type="expression" dxfId="119" priority="109">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J85:V85">
+    <cfRule type="expression" dxfId="118" priority="247">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B85 E85:F85">
+    <cfRule type="expression" dxfId="117" priority="249">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K85:V85">
+    <cfRule type="expression" dxfId="116" priority="248">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H85">
+    <cfRule type="expression" dxfId="115" priority="246">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K43">
+    <cfRule type="expression" dxfId="114" priority="244">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43 J43">
+    <cfRule type="expression" dxfId="113" priority="242">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J38:K38">
+    <cfRule type="expression" dxfId="112" priority="239">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H38">
+    <cfRule type="expression" dxfId="111" priority="237">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I48">
+    <cfRule type="expression" dxfId="110" priority="95">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I52">
+    <cfRule type="expression" dxfId="109" priority="233">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I64">
+    <cfRule type="expression" dxfId="108" priority="226">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I60">
+    <cfRule type="expression" dxfId="107" priority="230">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I61">
+    <cfRule type="expression" dxfId="106" priority="229">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I62">
+    <cfRule type="expression" dxfId="105" priority="228">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I63">
+    <cfRule type="expression" dxfId="104" priority="227">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I65">
+    <cfRule type="expression" dxfId="103" priority="225">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I66">
+    <cfRule type="expression" dxfId="102" priority="224">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I67">
+    <cfRule type="expression" dxfId="101" priority="223">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I68">
+    <cfRule type="expression" dxfId="100" priority="222">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I69">
+    <cfRule type="expression" dxfId="99" priority="221">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I70">
+    <cfRule type="expression" dxfId="98" priority="220">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I71">
+    <cfRule type="expression" dxfId="97" priority="219">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I72">
+    <cfRule type="expression" dxfId="96" priority="218">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I73">
+    <cfRule type="expression" dxfId="95" priority="217">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I75">
+    <cfRule type="expression" dxfId="94" priority="215">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I76">
+    <cfRule type="expression" dxfId="93" priority="214">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I77">
+    <cfRule type="expression" dxfId="92" priority="213">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I80">
+    <cfRule type="expression" dxfId="91" priority="211">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I82">
+    <cfRule type="expression" dxfId="90" priority="210">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I83">
+    <cfRule type="expression" dxfId="89" priority="209">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I84">
+    <cfRule type="expression" dxfId="88" priority="208">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I85">
+    <cfRule type="expression" dxfId="87" priority="207">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I86">
+    <cfRule type="expression" dxfId="86" priority="206">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H86">
+    <cfRule type="expression" dxfId="85" priority="205">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="expression" dxfId="84" priority="204">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="expression" dxfId="83" priority="203">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="expression" dxfId="82" priority="202">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="expression" dxfId="81" priority="201">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="expression" dxfId="80" priority="200">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="expression" dxfId="79" priority="199">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="expression" dxfId="78" priority="198">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="expression" dxfId="77" priority="197">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="expression" dxfId="76" priority="129">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="expression" dxfId="75" priority="128">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="expression" dxfId="74" priority="127">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="expression" dxfId="73" priority="126">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="expression" dxfId="72" priority="125">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="expression" dxfId="71" priority="119">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="expression" dxfId="70" priority="123">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="expression" dxfId="69" priority="122">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
+    <cfRule type="expression" dxfId="68" priority="121">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="expression" dxfId="67" priority="118">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="expression" dxfId="66" priority="117">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="expression" dxfId="65" priority="116">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="expression" dxfId="64" priority="115">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="expression" dxfId="63" priority="114">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30">
+    <cfRule type="expression" dxfId="62" priority="113">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="expression" dxfId="61" priority="112">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="expression" dxfId="60" priority="111">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
+    <cfRule type="expression" dxfId="59" priority="108">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I49">
+    <cfRule type="expression" dxfId="58" priority="94">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
+    <cfRule type="expression" dxfId="57" priority="106">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="expression" dxfId="56" priority="105">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="expression" dxfId="55" priority="104">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38">
+    <cfRule type="expression" dxfId="54" priority="103">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="expression" dxfId="53" priority="102">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
+    <cfRule type="expression" dxfId="52" priority="101">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43">
+    <cfRule type="expression" dxfId="51" priority="100">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="expression" dxfId="50" priority="98">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I47">
+    <cfRule type="expression" dxfId="49" priority="96">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:V10">
+    <cfRule type="expression" dxfId="48" priority="86">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="expression" dxfId="47" priority="75">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H81">
+    <cfRule type="expression" dxfId="46" priority="84">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I81">
+    <cfRule type="expression" dxfId="45" priority="83">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:K9">
+    <cfRule type="expression" dxfId="44" priority="74">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="expression" dxfId="43" priority="73">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="42" priority="76">
+      <formula>K$1=$H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="41" priority="77">
+      <formula>K$1=$I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="40" priority="71">
+      <formula>K$1=$H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="39" priority="72">
+      <formula>K$1=$I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="expression" dxfId="38" priority="70">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:K10">
+    <cfRule type="expression" dxfId="37" priority="69">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="expression" dxfId="36" priority="68">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43">
+    <cfRule type="expression" dxfId="35" priority="61">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42:K42 H42">
+    <cfRule type="expression" dxfId="34" priority="56">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I42">
+    <cfRule type="expression" dxfId="33" priority="55">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="32" priority="46">
+      <formula>K$1=$H18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="31" priority="47">
+      <formula>K$1=$I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18 J18:K18">
+    <cfRule type="expression" dxfId="30" priority="48">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="expression" dxfId="29" priority="45">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K74">
+    <cfRule type="expression" dxfId="28" priority="43">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J74:K74">
+    <cfRule type="expression" dxfId="27" priority="42">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H74">
+    <cfRule type="expression" dxfId="26" priority="41">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I74">
+    <cfRule type="expression" dxfId="25" priority="40">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40:K40 H40">
+    <cfRule type="expression" dxfId="24" priority="38">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="expression" dxfId="23" priority="37">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J78">
+    <cfRule type="expression" dxfId="22" priority="28">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H78">
+    <cfRule type="expression" dxfId="21" priority="27">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I78">
+    <cfRule type="expression" dxfId="20" priority="26">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K78:V78">
+    <cfRule type="expression" dxfId="19" priority="25">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K78:V78">
+    <cfRule type="expression" dxfId="18" priority="23">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46 G46">
+    <cfRule type="expression" dxfId="17" priority="21">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46:F46">
+    <cfRule type="expression" dxfId="16" priority="20">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46 E46 G46">
+    <cfRule type="expression" dxfId="15" priority="19">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46 E46 G46">
+    <cfRule type="expression" dxfId="14" priority="18">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46">
+    <cfRule type="expression" dxfId="13" priority="17">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J46:V46 H46">
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I46">
+    <cfRule type="expression" dxfId="11" priority="14">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21 E21:G21">
+    <cfRule type="expression" dxfId="10" priority="13">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45:F45">
+    <cfRule type="expression" dxfId="7" priority="9">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J45:V45 H45">
+    <cfRule type="expression" dxfId="6" priority="8">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I45">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:V21">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>K$1=$H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>K$1=$I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L21:V21">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H21 J21:K21">
-    <cfRule type="expression" dxfId="197" priority="432">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K60">
-    <cfRule type="expression" dxfId="196" priority="337">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K60">
-    <cfRule type="expression" dxfId="195" priority="336">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23 J23:K23">
-    <cfRule type="expression" dxfId="194" priority="425">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K61">
-    <cfRule type="expression" dxfId="193" priority="333">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24 J24:K24">
-    <cfRule type="expression" dxfId="192" priority="420">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H61 J61">
-    <cfRule type="expression" dxfId="191" priority="331">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25 J25:K25">
-    <cfRule type="expression" dxfId="190" priority="415">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="expression" dxfId="189" priority="328">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H62 J62">
-    <cfRule type="expression" dxfId="188" priority="327">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="187" priority="325">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="186" priority="324">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H28 J28:K28">
-    <cfRule type="expression" dxfId="185" priority="405">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="184" priority="321">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29 J29:K29">
-    <cfRule type="expression" dxfId="183" priority="400">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H64 J64">
-    <cfRule type="expression" dxfId="182" priority="319">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H30 J30:K30">
-    <cfRule type="expression" dxfId="181" priority="395">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H65 J65">
-    <cfRule type="expression" dxfId="180" priority="315">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H31 J31:K31">
-    <cfRule type="expression" dxfId="179" priority="390">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="178" priority="313">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="177" priority="312">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H32 J32:K32">
-    <cfRule type="expression" dxfId="176" priority="385">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="175" priority="309">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="174" priority="307">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="173" priority="373">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="172" priority="305">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="171" priority="370">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="170" priority="367">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H68 J68">
-    <cfRule type="expression" dxfId="169" priority="303">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="168" priority="364">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39:B40 J39:V39 E39:H39 E40:G40 L40:V40">
-    <cfRule type="expression" dxfId="167" priority="361">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J41:V41 B41:B43 E43 E41:H41 G43 E42:G42 L42:V43">
-    <cfRule type="expression" dxfId="166" priority="357">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="165" priority="301">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="164" priority="300">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E48:G48 B48">
-    <cfRule type="expression" dxfId="163" priority="350">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I79">
-    <cfRule type="expression" dxfId="162" priority="207">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H49">
-    <cfRule type="expression" dxfId="161" priority="346">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H52 J52">
-    <cfRule type="expression" dxfId="160" priority="345">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="159" priority="293">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="158" priority="296">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H70 J70">
-    <cfRule type="expression" dxfId="157" priority="299">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H60 J60">
-    <cfRule type="expression" dxfId="156" priority="335">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K61">
-    <cfRule type="expression" dxfId="155" priority="332">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="expression" dxfId="154" priority="329">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H63 J63">
-    <cfRule type="expression" dxfId="153" priority="323">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="152" priority="320">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="151" priority="317">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H66 J66">
-    <cfRule type="expression" dxfId="150" priority="311">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="149" priority="308">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="148" priority="297">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H71 J71">
-    <cfRule type="expression" dxfId="147" priority="295">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="146" priority="292">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H72 J72">
-    <cfRule type="expression" dxfId="145" priority="291">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="144" priority="289">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="143" priority="288">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H69 J69">
-    <cfRule type="expression" dxfId="142" priority="287">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G79">
-    <cfRule type="expression" dxfId="141" priority="282">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J79:V79">
-    <cfRule type="expression" dxfId="140" priority="277">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B79 E79:F79">
-    <cfRule type="expression" dxfId="139" priority="279">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K79:V79">
-    <cfRule type="expression" dxfId="138" priority="278">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H79">
-    <cfRule type="expression" dxfId="137" priority="276">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H76">
-    <cfRule type="expression" dxfId="136" priority="273">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="135" priority="271">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G82">
-    <cfRule type="expression" dxfId="134" priority="268">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="133" priority="125">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J82:V82">
-    <cfRule type="expression" dxfId="132" priority="263">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B82 E82:F82">
-    <cfRule type="expression" dxfId="131" priority="265">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82:V82">
-    <cfRule type="expression" dxfId="130" priority="264">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H82">
-    <cfRule type="expression" dxfId="129" priority="262">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H80">
-    <cfRule type="expression" dxfId="128" priority="260">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G83">
-    <cfRule type="expression" dxfId="127" priority="258">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="126" priority="115">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J83:V83">
-    <cfRule type="expression" dxfId="125" priority="253">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B83 E83:F83">
-    <cfRule type="expression" dxfId="124" priority="255">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K83:V83">
-    <cfRule type="expression" dxfId="123" priority="254">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H83">
-    <cfRule type="expression" dxfId="122" priority="252">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J84">
-    <cfRule type="expression" dxfId="121" priority="250">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H84">
-    <cfRule type="expression" dxfId="120" priority="249">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G85">
-    <cfRule type="expression" dxfId="119" priority="247">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="118" priority="104">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J85:V85">
-    <cfRule type="expression" dxfId="117" priority="242">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B85 E85:F85">
-    <cfRule type="expression" dxfId="116" priority="244">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K85:V85">
-    <cfRule type="expression" dxfId="115" priority="243">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H85">
-    <cfRule type="expression" dxfId="114" priority="241">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K43">
-    <cfRule type="expression" dxfId="113" priority="239">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H43 J43">
-    <cfRule type="expression" dxfId="112" priority="237">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J38:K38">
-    <cfRule type="expression" dxfId="111" priority="234">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="110" priority="232">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="109" priority="90">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I52">
-    <cfRule type="expression" dxfId="108" priority="228">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I64">
-    <cfRule type="expression" dxfId="107" priority="221">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I60">
-    <cfRule type="expression" dxfId="106" priority="225">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I61">
-    <cfRule type="expression" dxfId="105" priority="224">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I62">
-    <cfRule type="expression" dxfId="104" priority="223">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="103" priority="222">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
-    <cfRule type="expression" dxfId="102" priority="220">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I66">
-    <cfRule type="expression" dxfId="101" priority="219">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I67">
-    <cfRule type="expression" dxfId="100" priority="218">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I68">
-    <cfRule type="expression" dxfId="99" priority="217">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="98" priority="216">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="97" priority="215">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I71">
-    <cfRule type="expression" dxfId="96" priority="214">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I72">
-    <cfRule type="expression" dxfId="95" priority="213">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I73">
-    <cfRule type="expression" dxfId="94" priority="212">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I75">
-    <cfRule type="expression" dxfId="93" priority="210">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="expression" dxfId="92" priority="209">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I77">
-    <cfRule type="expression" dxfId="91" priority="208">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I80">
-    <cfRule type="expression" dxfId="90" priority="206">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I82">
-    <cfRule type="expression" dxfId="89" priority="205">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I83">
-    <cfRule type="expression" dxfId="88" priority="204">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I84">
-    <cfRule type="expression" dxfId="87" priority="203">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I85">
-    <cfRule type="expression" dxfId="86" priority="202">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I86">
-    <cfRule type="expression" dxfId="85" priority="201">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H86">
-    <cfRule type="expression" dxfId="84" priority="200">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="83" priority="199">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="82" priority="198">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="expression" dxfId="81" priority="197">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="80" priority="196">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="79" priority="195">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="78" priority="194">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="77" priority="193">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="76" priority="192">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="75" priority="124">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="expression" dxfId="74" priority="123">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="expression" dxfId="73" priority="122">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="72" priority="121">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="71" priority="120">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="70" priority="114">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
-    <cfRule type="expression" dxfId="69" priority="118">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="expression" dxfId="68" priority="117">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="expression" dxfId="67" priority="116">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="66" priority="113">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="expression" dxfId="65" priority="112">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
-    <cfRule type="expression" dxfId="64" priority="111">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="63" priority="110">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="62" priority="109">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="expression" dxfId="61" priority="108">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="expression" dxfId="60" priority="107">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="59" priority="106">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="58" priority="103">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I49">
-    <cfRule type="expression" dxfId="57" priority="89">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="expression" dxfId="56" priority="101">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
-    <cfRule type="expression" dxfId="55" priority="100">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="expression" dxfId="54" priority="99">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="53" priority="98">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="expression" dxfId="52" priority="97">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
-    <cfRule type="expression" dxfId="51" priority="96">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="50" priority="95">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="49" priority="93">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="48" priority="91">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L9:V10">
-    <cfRule type="expression" dxfId="47" priority="81">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="46" priority="70">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H81">
-    <cfRule type="expression" dxfId="45" priority="79">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I81">
-    <cfRule type="expression" dxfId="44" priority="78">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:K9">
-    <cfRule type="expression" dxfId="43" priority="69">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="42" priority="68">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="41" priority="71">
-      <formula>K$1=$H9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="40" priority="72">
-      <formula>K$1=$I9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="39" priority="66">
-      <formula>K$1=$H10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="38" priority="67">
-      <formula>K$1=$I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="37" priority="65">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
-    <cfRule type="expression" dxfId="36" priority="64">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="35" priority="63">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="34" priority="56">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J42:K42 H42">
-    <cfRule type="expression" dxfId="33" priority="51">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="32" priority="50">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="31" priority="41">
-      <formula>K$1=$H18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="30" priority="42">
-      <formula>K$1=$I18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18 J18:K18">
-    <cfRule type="expression" dxfId="29" priority="43">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="28" priority="40">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="27" priority="38">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J74:K74">
-    <cfRule type="expression" dxfId="26" priority="37">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H74">
-    <cfRule type="expression" dxfId="25" priority="36">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I74">
-    <cfRule type="expression" dxfId="24" priority="35">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K40">
-    <cfRule type="expression" dxfId="23" priority="34">
-      <formula>K$1=$H40</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J40:K40 H40">
-    <cfRule type="expression" dxfId="22" priority="33">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="21" priority="32">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J78">
-    <cfRule type="expression" dxfId="20" priority="23">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H78">
-    <cfRule type="expression" dxfId="19" priority="22">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I78">
-    <cfRule type="expression" dxfId="18" priority="21">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K78:V78">
-    <cfRule type="expression" dxfId="17" priority="20">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K78:V78">
-    <cfRule type="expression" dxfId="16" priority="18">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46 G46">
-    <cfRule type="expression" dxfId="14" priority="16">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46:F46">
-    <cfRule type="expression" dxfId="13" priority="15">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46 E46 G46">
-    <cfRule type="expression" dxfId="12" priority="14">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46 E46 G46">
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46">
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J46:V46 H46">
-    <cfRule type="expression" dxfId="9" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27 E27:G27">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27 J27">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45:F45">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K45:V45">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>K$1=$H45</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J45:V45 H45">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G27" r:id="rId1" xr:uid="{441BD375-4CFE-1440-B1DD-3FDA85827C47}"/>
+    <hyperlink ref="G21" r:id="rId1" xr:uid="{441BD375-4CFE-1440-B1DD-3FDA85827C47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Update join and sort column values
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5029BCB7-C3B3-544C-81C9-646C2F0FA6DD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664E5041-DA5E-8841-836E-FE8C44E3213B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17560" yWindow="6120" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1194,7 +1194,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="270">
+  <dxfs count="268">
     <dxf>
       <fill>
         <patternFill>
@@ -1229,20 +1229,6 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3418,8 +3404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4973,10 +4959,10 @@
         <v>235</v>
       </c>
       <c r="C21" s="7">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D21" s="7">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>236</v>
@@ -5051,10 +5037,10 @@
         <v>43</v>
       </c>
       <c r="C22" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D22" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>70</v>
@@ -5129,10 +5115,10 @@
         <v>180</v>
       </c>
       <c r="C23" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D23" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="7" t="s">
@@ -5205,10 +5191,10 @@
         <v>50</v>
       </c>
       <c r="C24" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D24" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>19</v>
@@ -5285,10 +5271,10 @@
         <v>185</v>
       </c>
       <c r="C25" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D25" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="19" t="s">
@@ -5361,10 +5347,10 @@
         <v>110</v>
       </c>
       <c r="C26" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D26" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>111</v>
@@ -5439,10 +5425,10 @@
         <v>49</v>
       </c>
       <c r="C27" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D27" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>15</v>
@@ -10065,11 +10051,11 @@
     <sortCondition ref="D2:D70"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
+      <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
-      <selection sqref="A1:XFD1048576"/>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -10078,1302 +10064,1302 @@
     <mergeCell ref="A50:A85"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V86">
-    <cfRule type="expression" dxfId="269" priority="640">
+    <cfRule type="expression" dxfId="267" priority="640">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K17:V17 K19:V19 K23:V23 K20 K24:K32 K22">
-    <cfRule type="expression" dxfId="268" priority="642">
+    <cfRule type="expression" dxfId="266" priority="642">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K52:V52 G52 G61 B62:B64 G71 G86 E59:G59 G30 B72 E72:G72 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E49:G49 J49:V49 G63:G67 B68:B70 E68:G70 L40:V40 L61:V72 K84:V84 G84 K76:V77 K80:V81 K86:V86 L38:V38 E34:G38 E50:V51 G57:V57 H2 J2:V3 E40:G40 B81 J11:V14 J81:V81 B5 E53:V56 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L74:V74 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E81:G81 B74 E58:V58 E62:G62 B49:B59 B40 B44:B45 B78 B47 J47:V47 G73:G77 E24:G29 B20:B38 E44:H44 E45:G45 E5:G5 E47:H47 E78:G78 E74:G74 L24:V32 L20:V20 C4:D86 L22:V22">
-    <cfRule type="expression" dxfId="267" priority="646">
+  <conditionalFormatting sqref="K52:V52 G52 G61 B62:B64 G71 G86 E59:G59 G30 B72 E72:G72 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E49:G49 J49:V49 G63:G67 B68:B70 E68:G70 L40:V40 L61:V72 K84:V84 G84 K76:V77 K80:V81 K86:V86 L38:V38 E34:G38 E50:V51 G57:V57 H2 J2:V3 E40:G40 B81 J11:V14 J81:V81 B5 E53:V56 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L74:V74 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E81:G81 B74 E58:V58 E62:G62 B49:B59 B40 B44:B45 B78 B47 J47:V47 G73:G77 E24:G29 B20:B38 E44:H44 E45:G45 E5:G5 E47:H47 E78:G78 E74:G74 L24:V32 L20:V20 L22:V22">
+    <cfRule type="expression" dxfId="265" priority="646">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61 L61:V61">
-    <cfRule type="expression" dxfId="266" priority="623">
+    <cfRule type="expression" dxfId="264" priority="623">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65 L65:V65">
-    <cfRule type="expression" dxfId="265" priority="621">
+    <cfRule type="expression" dxfId="263" priority="621">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67 L67:V67">
-    <cfRule type="expression" dxfId="264" priority="619">
+    <cfRule type="expression" dxfId="262" priority="619">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71 L71:V71">
-    <cfRule type="expression" dxfId="263" priority="617">
+    <cfRule type="expression" dxfId="261" priority="617">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66 L66:V66">
-    <cfRule type="expression" dxfId="262" priority="615">
+    <cfRule type="expression" dxfId="260" priority="615">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84 K84:V84 E84:F84">
-    <cfRule type="expression" dxfId="261" priority="611">
+    <cfRule type="expression" dxfId="259" priority="611">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="expression" dxfId="260" priority="609">
+    <cfRule type="expression" dxfId="258" priority="609">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E71">
-    <cfRule type="expression" dxfId="259" priority="606">
+    <cfRule type="expression" dxfId="257" priority="606">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="expression" dxfId="258" priority="605">
+    <cfRule type="expression" dxfId="256" priority="605">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:B81 J80:V81">
-    <cfRule type="expression" dxfId="257" priority="602">
+    <cfRule type="expression" dxfId="255" priority="602">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77:B78 J77:V77 E77:E78">
-    <cfRule type="expression" dxfId="256" priority="600">
+    <cfRule type="expression" dxfId="254" priority="600">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E80:F81">
-    <cfRule type="expression" dxfId="255" priority="598">
+    <cfRule type="expression" dxfId="253" priority="598">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76 J76:V76">
-    <cfRule type="expression" dxfId="254" priority="596">
+    <cfRule type="expression" dxfId="252" priority="596">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86 J86:V86 E86">
-    <cfRule type="expression" dxfId="253" priority="594">
+    <cfRule type="expression" dxfId="251" priority="594">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66">
-    <cfRule type="expression" dxfId="252" priority="586">
+    <cfRule type="expression" dxfId="250" priority="586">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59:V59">
-    <cfRule type="expression" dxfId="251" priority="526">
+    <cfRule type="expression" dxfId="249" priority="526">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71">
-    <cfRule type="expression" dxfId="250" priority="548">
+    <cfRule type="expression" dxfId="248" priority="548">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73:B74 E73:F74">
-    <cfRule type="expression" dxfId="249" priority="512">
+    <cfRule type="expression" dxfId="247" priority="512">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="expression" dxfId="248" priority="533">
+    <cfRule type="expression" dxfId="246" priority="533">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65:F65">
-    <cfRule type="expression" dxfId="247" priority="540">
+    <cfRule type="expression" dxfId="245" priority="540">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60 L60:V60">
-    <cfRule type="expression" dxfId="246" priority="534">
+    <cfRule type="expression" dxfId="244" priority="534">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F77:F78">
-    <cfRule type="expression" dxfId="245" priority="546">
+    <cfRule type="expression" dxfId="243" priority="546">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61">
-    <cfRule type="expression" dxfId="244" priority="542">
+    <cfRule type="expression" dxfId="242" priority="542">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67:F67">
-    <cfRule type="expression" dxfId="243" priority="541">
+    <cfRule type="expression" dxfId="241" priority="541">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76:F76">
-    <cfRule type="expression" dxfId="242" priority="539">
+    <cfRule type="expression" dxfId="240" priority="539">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L60:V60 G60">
-    <cfRule type="expression" dxfId="241" priority="536">
+    <cfRule type="expression" dxfId="239" priority="536">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:V7">
-    <cfRule type="expression" dxfId="240" priority="481">
+    <cfRule type="expression" dxfId="238" priority="481">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60">
-    <cfRule type="expression" dxfId="239" priority="530">
+    <cfRule type="expression" dxfId="237" priority="530">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:V47">
-    <cfRule type="expression" dxfId="238" priority="650">
+    <cfRule type="expression" dxfId="236" priority="650">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59:V59">
-    <cfRule type="expression" dxfId="237" priority="527">
+    <cfRule type="expression" dxfId="235" priority="527">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:V10">
-    <cfRule type="expression" dxfId="236" priority="472">
+    <cfRule type="expression" dxfId="234" priority="472">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H14 J13:V14 L18:V18">
-    <cfRule type="expression" dxfId="235" priority="518">
+    <cfRule type="expression" dxfId="233" priority="518">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:V14 L18:V18">
-    <cfRule type="expression" dxfId="234" priority="519">
+    <cfRule type="expression" dxfId="232" priority="519">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G3 B7 E7:G7">
-    <cfRule type="expression" dxfId="233" priority="513">
+  <conditionalFormatting sqref="B2:G3 B7 E7:G7 C4:D86">
+    <cfRule type="expression" dxfId="231" priority="513">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73:V73 L74:V74">
-    <cfRule type="expression" dxfId="232" priority="511">
+    <cfRule type="expression" dxfId="230" priority="511">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J73:V73 L74:V74">
-    <cfRule type="expression" dxfId="231" priority="509">
+    <cfRule type="expression" dxfId="229" priority="509">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73">
-    <cfRule type="expression" dxfId="230" priority="508">
+    <cfRule type="expression" dxfId="228" priority="508">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J75:V75">
-    <cfRule type="expression" dxfId="229" priority="503">
+    <cfRule type="expression" dxfId="227" priority="503">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75 E75:F75">
-    <cfRule type="expression" dxfId="228" priority="506">
+    <cfRule type="expression" dxfId="226" priority="506">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K75:V75">
-    <cfRule type="expression" dxfId="227" priority="505">
+    <cfRule type="expression" dxfId="225" priority="505">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75">
-    <cfRule type="expression" dxfId="226" priority="502">
+    <cfRule type="expression" dxfId="224" priority="502">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="225" priority="495">
+    <cfRule type="expression" dxfId="223" priority="495">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:F30">
-    <cfRule type="expression" dxfId="224" priority="500">
+    <cfRule type="expression" dxfId="222" priority="500">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43 E43 L43:V43 G43">
-    <cfRule type="expression" dxfId="223" priority="499">
+    <cfRule type="expression" dxfId="221" priority="499">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4 E4:G4">
-    <cfRule type="expression" dxfId="222" priority="494">
+    <cfRule type="expression" dxfId="220" priority="494">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="221" priority="493">
+    <cfRule type="expression" dxfId="219" priority="493">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 E6:H6 J6:V6">
-    <cfRule type="expression" dxfId="220" priority="491">
+    <cfRule type="expression" dxfId="218" priority="491">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:V5">
-    <cfRule type="expression" dxfId="219" priority="488">
+    <cfRule type="expression" dxfId="217" priority="488">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:L4">
-    <cfRule type="expression" dxfId="218" priority="483">
+    <cfRule type="expression" dxfId="216" priority="483">
       <formula>K$1=$H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:V4">
-    <cfRule type="expression" dxfId="217" priority="484">
+    <cfRule type="expression" dxfId="215" priority="484">
       <formula>K$1=$I4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:V4">
-    <cfRule type="expression" dxfId="216" priority="485">
+    <cfRule type="expression" dxfId="214" priority="485">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="215" priority="478">
+    <cfRule type="expression" dxfId="213" priority="478">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 E8:G10">
-    <cfRule type="expression" dxfId="214" priority="477">
+    <cfRule type="expression" dxfId="212" priority="477">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:K8">
-    <cfRule type="expression" dxfId="213" priority="475">
+    <cfRule type="expression" dxfId="211" priority="475">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:H15 J15:V15">
-    <cfRule type="expression" dxfId="212" priority="467">
+    <cfRule type="expression" dxfId="210" priority="467">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15 J15:V15">
-    <cfRule type="expression" dxfId="211" priority="464">
+    <cfRule type="expression" dxfId="209" priority="464">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:V15">
-    <cfRule type="expression" dxfId="210" priority="465">
+    <cfRule type="expression" dxfId="208" priority="465">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:G15">
-    <cfRule type="expression" dxfId="209" priority="463">
+    <cfRule type="expression" dxfId="207" priority="463">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="208" priority="321">
+    <cfRule type="expression" dxfId="206" priority="321">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="207" priority="460">
+    <cfRule type="expression" dxfId="205" priority="460">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="206" priority="457">
+    <cfRule type="expression" dxfId="204" priority="457">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="205" priority="458">
+    <cfRule type="expression" dxfId="203" priority="458">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48 J48:V48">
-    <cfRule type="expression" dxfId="204" priority="352">
+    <cfRule type="expression" dxfId="202" priority="352">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19 E19:H19 J19:V19">
-    <cfRule type="expression" dxfId="203" priority="453">
+    <cfRule type="expression" dxfId="201" priority="453">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="202" priority="309">
+    <cfRule type="expression" dxfId="200" priority="309">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27 J27:K27">
-    <cfRule type="expression" dxfId="201" priority="415">
+    <cfRule type="expression" dxfId="199" priority="415">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:J59">
-    <cfRule type="expression" dxfId="200" priority="347">
+    <cfRule type="expression" dxfId="198" priority="347">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20 J20:K20">
-    <cfRule type="expression" dxfId="199" priority="442">
+    <cfRule type="expression" dxfId="197" priority="442">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22 J22:K22">
-    <cfRule type="expression" dxfId="198" priority="437">
+    <cfRule type="expression" dxfId="196" priority="437">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K60">
-    <cfRule type="expression" dxfId="197" priority="342">
+    <cfRule type="expression" dxfId="195" priority="342">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K60">
-    <cfRule type="expression" dxfId="196" priority="341">
+    <cfRule type="expression" dxfId="194" priority="341">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24 J24:K24">
-    <cfRule type="expression" dxfId="195" priority="430">
+    <cfRule type="expression" dxfId="193" priority="430">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K61">
-    <cfRule type="expression" dxfId="194" priority="338">
+    <cfRule type="expression" dxfId="192" priority="338">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25 J25:K25">
-    <cfRule type="expression" dxfId="193" priority="425">
+    <cfRule type="expression" dxfId="191" priority="425">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61 J61">
-    <cfRule type="expression" dxfId="192" priority="336">
+    <cfRule type="expression" dxfId="190" priority="336">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26 J26:K26">
-    <cfRule type="expression" dxfId="191" priority="420">
+    <cfRule type="expression" dxfId="189" priority="420">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62">
-    <cfRule type="expression" dxfId="190" priority="333">
+    <cfRule type="expression" dxfId="188" priority="333">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62 J62">
-    <cfRule type="expression" dxfId="189" priority="332">
+    <cfRule type="expression" dxfId="187" priority="332">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="188" priority="330">
+    <cfRule type="expression" dxfId="186" priority="330">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="187" priority="329">
+    <cfRule type="expression" dxfId="185" priority="329">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28 J28:K28">
-    <cfRule type="expression" dxfId="186" priority="410">
+    <cfRule type="expression" dxfId="184" priority="410">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="185" priority="326">
+    <cfRule type="expression" dxfId="183" priority="326">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29 J29:K29">
-    <cfRule type="expression" dxfId="184" priority="405">
+    <cfRule type="expression" dxfId="182" priority="405">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64 J64">
-    <cfRule type="expression" dxfId="183" priority="324">
+    <cfRule type="expression" dxfId="181" priority="324">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30 J30:K30">
-    <cfRule type="expression" dxfId="182" priority="400">
+    <cfRule type="expression" dxfId="180" priority="400">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65 J65">
-    <cfRule type="expression" dxfId="181" priority="320">
+    <cfRule type="expression" dxfId="179" priority="320">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31 J31:K31">
-    <cfRule type="expression" dxfId="180" priority="395">
+    <cfRule type="expression" dxfId="178" priority="395">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="179" priority="318">
+    <cfRule type="expression" dxfId="177" priority="318">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="178" priority="317">
+    <cfRule type="expression" dxfId="176" priority="317">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32 J32:K32">
-    <cfRule type="expression" dxfId="177" priority="390">
+    <cfRule type="expression" dxfId="175" priority="390">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="176" priority="314">
+    <cfRule type="expression" dxfId="174" priority="314">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="175" priority="312">
+    <cfRule type="expression" dxfId="173" priority="312">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="174" priority="378">
+    <cfRule type="expression" dxfId="172" priority="378">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="173" priority="310">
+    <cfRule type="expression" dxfId="171" priority="310">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="172" priority="375">
+    <cfRule type="expression" dxfId="170" priority="375">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="171" priority="372">
+    <cfRule type="expression" dxfId="169" priority="372">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68 J68">
-    <cfRule type="expression" dxfId="170" priority="308">
+    <cfRule type="expression" dxfId="168" priority="308">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="169" priority="369">
+    <cfRule type="expression" dxfId="167" priority="369">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:B40 J39:V39 E39:H39 E40:G40 L40:V40">
-    <cfRule type="expression" dxfId="168" priority="366">
+    <cfRule type="expression" dxfId="166" priority="366">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:V41 B41:B43 E43 E41:H41 G43 E42:G42 L42:V43">
-    <cfRule type="expression" dxfId="167" priority="362">
+    <cfRule type="expression" dxfId="165" priority="362">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="166" priority="306">
+    <cfRule type="expression" dxfId="164" priority="306">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="165" priority="305">
+    <cfRule type="expression" dxfId="163" priority="305">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:G48 B48">
-    <cfRule type="expression" dxfId="164" priority="355">
+    <cfRule type="expression" dxfId="162" priority="355">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I79">
-    <cfRule type="expression" dxfId="163" priority="212">
+    <cfRule type="expression" dxfId="161" priority="212">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="expression" dxfId="162" priority="351">
+    <cfRule type="expression" dxfId="160" priority="351">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52 J52">
-    <cfRule type="expression" dxfId="161" priority="350">
+    <cfRule type="expression" dxfId="159" priority="350">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="160" priority="298">
+    <cfRule type="expression" dxfId="158" priority="298">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="159" priority="301">
+    <cfRule type="expression" dxfId="157" priority="301">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70 J70">
-    <cfRule type="expression" dxfId="158" priority="304">
+    <cfRule type="expression" dxfId="156" priority="304">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H60 J60">
-    <cfRule type="expression" dxfId="157" priority="340">
+    <cfRule type="expression" dxfId="155" priority="340">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K61">
-    <cfRule type="expression" dxfId="156" priority="337">
+    <cfRule type="expression" dxfId="154" priority="337">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62">
-    <cfRule type="expression" dxfId="155" priority="334">
+    <cfRule type="expression" dxfId="153" priority="334">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63 J63">
-    <cfRule type="expression" dxfId="154" priority="328">
+    <cfRule type="expression" dxfId="152" priority="328">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="153" priority="325">
+    <cfRule type="expression" dxfId="151" priority="325">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="152" priority="322">
+    <cfRule type="expression" dxfId="150" priority="322">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66 J66">
-    <cfRule type="expression" dxfId="151" priority="316">
+    <cfRule type="expression" dxfId="149" priority="316">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="150" priority="313">
+    <cfRule type="expression" dxfId="148" priority="313">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="149" priority="302">
+    <cfRule type="expression" dxfId="147" priority="302">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71 J71">
-    <cfRule type="expression" dxfId="148" priority="300">
+    <cfRule type="expression" dxfId="146" priority="300">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="147" priority="297">
+    <cfRule type="expression" dxfId="145" priority="297">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72 J72">
-    <cfRule type="expression" dxfId="146" priority="296">
+    <cfRule type="expression" dxfId="144" priority="296">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="145" priority="294">
+    <cfRule type="expression" dxfId="143" priority="294">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="144" priority="293">
+    <cfRule type="expression" dxfId="142" priority="293">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69 J69">
-    <cfRule type="expression" dxfId="143" priority="292">
+    <cfRule type="expression" dxfId="141" priority="292">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G79">
-    <cfRule type="expression" dxfId="142" priority="287">
+    <cfRule type="expression" dxfId="140" priority="287">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J79:V79">
-    <cfRule type="expression" dxfId="141" priority="282">
+    <cfRule type="expression" dxfId="139" priority="282">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79 E79:F79">
-    <cfRule type="expression" dxfId="140" priority="284">
+    <cfRule type="expression" dxfId="138" priority="284">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K79:V79">
-    <cfRule type="expression" dxfId="139" priority="283">
+    <cfRule type="expression" dxfId="137" priority="283">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79">
-    <cfRule type="expression" dxfId="138" priority="281">
+    <cfRule type="expression" dxfId="136" priority="281">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H76">
-    <cfRule type="expression" dxfId="137" priority="278">
+    <cfRule type="expression" dxfId="135" priority="278">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="136" priority="276">
+    <cfRule type="expression" dxfId="134" priority="276">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82">
-    <cfRule type="expression" dxfId="135" priority="273">
+    <cfRule type="expression" dxfId="133" priority="273">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="134" priority="130">
+    <cfRule type="expression" dxfId="132" priority="130">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J82:V82">
-    <cfRule type="expression" dxfId="133" priority="268">
+    <cfRule type="expression" dxfId="131" priority="268">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82 E82:F82">
-    <cfRule type="expression" dxfId="132" priority="270">
+    <cfRule type="expression" dxfId="130" priority="270">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K82:V82">
-    <cfRule type="expression" dxfId="131" priority="269">
+    <cfRule type="expression" dxfId="129" priority="269">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="expression" dxfId="130" priority="267">
+    <cfRule type="expression" dxfId="128" priority="267">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80">
-    <cfRule type="expression" dxfId="129" priority="265">
+    <cfRule type="expression" dxfId="127" priority="265">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G83">
-    <cfRule type="expression" dxfId="128" priority="263">
+    <cfRule type="expression" dxfId="126" priority="263">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="127" priority="120">
+    <cfRule type="expression" dxfId="125" priority="120">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J83:V83">
-    <cfRule type="expression" dxfId="126" priority="258">
+    <cfRule type="expression" dxfId="124" priority="258">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83 E83:F83">
-    <cfRule type="expression" dxfId="125" priority="260">
+    <cfRule type="expression" dxfId="123" priority="260">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K83:V83">
-    <cfRule type="expression" dxfId="124" priority="259">
+    <cfRule type="expression" dxfId="122" priority="259">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="expression" dxfId="123" priority="257">
+    <cfRule type="expression" dxfId="121" priority="257">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J84">
-    <cfRule type="expression" dxfId="122" priority="255">
+    <cfRule type="expression" dxfId="120" priority="255">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H84">
-    <cfRule type="expression" dxfId="121" priority="254">
+    <cfRule type="expression" dxfId="119" priority="254">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G85">
-    <cfRule type="expression" dxfId="120" priority="252">
+    <cfRule type="expression" dxfId="118" priority="252">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="119" priority="109">
+    <cfRule type="expression" dxfId="117" priority="109">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J85:V85">
-    <cfRule type="expression" dxfId="118" priority="247">
+    <cfRule type="expression" dxfId="116" priority="247">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85 E85:F85">
-    <cfRule type="expression" dxfId="117" priority="249">
+    <cfRule type="expression" dxfId="115" priority="249">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K85:V85">
-    <cfRule type="expression" dxfId="116" priority="248">
+    <cfRule type="expression" dxfId="114" priority="248">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="expression" dxfId="115" priority="246">
+    <cfRule type="expression" dxfId="113" priority="246">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43">
-    <cfRule type="expression" dxfId="114" priority="244">
+    <cfRule type="expression" dxfId="112" priority="244">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43 J43">
-    <cfRule type="expression" dxfId="113" priority="242">
+    <cfRule type="expression" dxfId="111" priority="242">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:K38">
-    <cfRule type="expression" dxfId="112" priority="239">
+    <cfRule type="expression" dxfId="110" priority="239">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="111" priority="237">
+    <cfRule type="expression" dxfId="109" priority="237">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="110" priority="95">
+    <cfRule type="expression" dxfId="108" priority="95">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52">
-    <cfRule type="expression" dxfId="109" priority="233">
+    <cfRule type="expression" dxfId="107" priority="233">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64">
-    <cfRule type="expression" dxfId="108" priority="226">
+    <cfRule type="expression" dxfId="106" priority="226">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I60">
-    <cfRule type="expression" dxfId="107" priority="230">
+    <cfRule type="expression" dxfId="105" priority="230">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61">
-    <cfRule type="expression" dxfId="106" priority="229">
+    <cfRule type="expression" dxfId="104" priority="229">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I62">
-    <cfRule type="expression" dxfId="105" priority="228">
+    <cfRule type="expression" dxfId="103" priority="228">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="104" priority="227">
+    <cfRule type="expression" dxfId="102" priority="227">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I65">
-    <cfRule type="expression" dxfId="103" priority="225">
+    <cfRule type="expression" dxfId="101" priority="225">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I66">
-    <cfRule type="expression" dxfId="102" priority="224">
+    <cfRule type="expression" dxfId="100" priority="224">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I67">
-    <cfRule type="expression" dxfId="101" priority="223">
+    <cfRule type="expression" dxfId="99" priority="223">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I68">
-    <cfRule type="expression" dxfId="100" priority="222">
+    <cfRule type="expression" dxfId="98" priority="222">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="99" priority="221">
+    <cfRule type="expression" dxfId="97" priority="221">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="98" priority="220">
+    <cfRule type="expression" dxfId="96" priority="220">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I71">
-    <cfRule type="expression" dxfId="97" priority="219">
+    <cfRule type="expression" dxfId="95" priority="219">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I72">
-    <cfRule type="expression" dxfId="96" priority="218">
+    <cfRule type="expression" dxfId="94" priority="218">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I73">
-    <cfRule type="expression" dxfId="95" priority="217">
+    <cfRule type="expression" dxfId="93" priority="217">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I75">
-    <cfRule type="expression" dxfId="94" priority="215">
+    <cfRule type="expression" dxfId="92" priority="215">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76">
-    <cfRule type="expression" dxfId="93" priority="214">
+    <cfRule type="expression" dxfId="91" priority="214">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I77">
-    <cfRule type="expression" dxfId="92" priority="213">
+    <cfRule type="expression" dxfId="90" priority="213">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I80">
-    <cfRule type="expression" dxfId="91" priority="211">
+    <cfRule type="expression" dxfId="89" priority="211">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I82">
-    <cfRule type="expression" dxfId="90" priority="210">
+    <cfRule type="expression" dxfId="88" priority="210">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I83">
-    <cfRule type="expression" dxfId="89" priority="209">
+    <cfRule type="expression" dxfId="87" priority="209">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I84">
-    <cfRule type="expression" dxfId="88" priority="208">
+    <cfRule type="expression" dxfId="86" priority="208">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I85">
-    <cfRule type="expression" dxfId="87" priority="207">
+    <cfRule type="expression" dxfId="85" priority="207">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I86">
-    <cfRule type="expression" dxfId="86" priority="206">
+    <cfRule type="expression" dxfId="84" priority="206">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="expression" dxfId="85" priority="205">
+    <cfRule type="expression" dxfId="83" priority="205">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="84" priority="204">
+    <cfRule type="expression" dxfId="82" priority="204">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="83" priority="203">
+    <cfRule type="expression" dxfId="81" priority="203">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="expression" dxfId="82" priority="202">
+    <cfRule type="expression" dxfId="80" priority="202">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="81" priority="201">
+    <cfRule type="expression" dxfId="79" priority="201">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="80" priority="200">
+    <cfRule type="expression" dxfId="78" priority="200">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="79" priority="199">
+    <cfRule type="expression" dxfId="77" priority="199">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="78" priority="198">
+    <cfRule type="expression" dxfId="76" priority="198">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="77" priority="197">
+    <cfRule type="expression" dxfId="75" priority="197">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="76" priority="129">
+    <cfRule type="expression" dxfId="74" priority="129">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="expression" dxfId="75" priority="128">
+    <cfRule type="expression" dxfId="73" priority="128">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="expression" dxfId="74" priority="127">
+    <cfRule type="expression" dxfId="72" priority="127">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="73" priority="126">
+    <cfRule type="expression" dxfId="71" priority="126">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="72" priority="125">
+    <cfRule type="expression" dxfId="70" priority="125">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="71" priority="119">
+    <cfRule type="expression" dxfId="69" priority="119">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="expression" dxfId="70" priority="123">
+    <cfRule type="expression" dxfId="68" priority="123">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="expression" dxfId="69" priority="122">
+    <cfRule type="expression" dxfId="67" priority="122">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="68" priority="121">
+    <cfRule type="expression" dxfId="66" priority="121">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="expression" dxfId="67" priority="118">
+    <cfRule type="expression" dxfId="65" priority="118">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26">
-    <cfRule type="expression" dxfId="66" priority="117">
+    <cfRule type="expression" dxfId="64" priority="117">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="expression" dxfId="65" priority="116">
+    <cfRule type="expression" dxfId="63" priority="116">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="64" priority="115">
+    <cfRule type="expression" dxfId="62" priority="115">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="63" priority="114">
+    <cfRule type="expression" dxfId="61" priority="114">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="expression" dxfId="62" priority="113">
+    <cfRule type="expression" dxfId="60" priority="113">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31">
-    <cfRule type="expression" dxfId="61" priority="112">
+    <cfRule type="expression" dxfId="59" priority="112">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="60" priority="111">
+    <cfRule type="expression" dxfId="58" priority="111">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="59" priority="108">
+    <cfRule type="expression" dxfId="57" priority="108">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="expression" dxfId="58" priority="94">
+    <cfRule type="expression" dxfId="56" priority="94">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="expression" dxfId="57" priority="106">
+    <cfRule type="expression" dxfId="55" priority="106">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="expression" dxfId="56" priority="105">
+    <cfRule type="expression" dxfId="54" priority="105">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="expression" dxfId="55" priority="104">
+    <cfRule type="expression" dxfId="53" priority="104">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="54" priority="103">
+    <cfRule type="expression" dxfId="52" priority="103">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39">
-    <cfRule type="expression" dxfId="53" priority="102">
+    <cfRule type="expression" dxfId="51" priority="102">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41">
-    <cfRule type="expression" dxfId="52" priority="101">
+    <cfRule type="expression" dxfId="50" priority="101">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="51" priority="100">
+    <cfRule type="expression" dxfId="49" priority="100">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="50" priority="98">
+    <cfRule type="expression" dxfId="48" priority="98">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="49" priority="96">
+    <cfRule type="expression" dxfId="47" priority="96">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:V10">
-    <cfRule type="expression" dxfId="48" priority="86">
+    <cfRule type="expression" dxfId="46" priority="86">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="47" priority="75">
+    <cfRule type="expression" dxfId="45" priority="75">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81">
-    <cfRule type="expression" dxfId="46" priority="84">
+    <cfRule type="expression" dxfId="44" priority="84">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81">
-    <cfRule type="expression" dxfId="45" priority="83">
+    <cfRule type="expression" dxfId="43" priority="83">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:K9">
-    <cfRule type="expression" dxfId="44" priority="74">
+    <cfRule type="expression" dxfId="42" priority="74">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="43" priority="73">
+    <cfRule type="expression" dxfId="41" priority="73">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="42" priority="76">
+    <cfRule type="expression" dxfId="40" priority="76">
       <formula>K$1=$H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="41" priority="77">
+    <cfRule type="expression" dxfId="39" priority="77">
       <formula>K$1=$I9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="40" priority="71">
+    <cfRule type="expression" dxfId="38" priority="71">
       <formula>K$1=$H10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="39" priority="72">
+    <cfRule type="expression" dxfId="37" priority="72">
       <formula>K$1=$I10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="38" priority="70">
+    <cfRule type="expression" dxfId="36" priority="70">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10:K10">
-    <cfRule type="expression" dxfId="37" priority="69">
+    <cfRule type="expression" dxfId="35" priority="69">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="36" priority="68">
+    <cfRule type="expression" dxfId="34" priority="68">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="35" priority="61">
+    <cfRule type="expression" dxfId="33" priority="61">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42:K42 H42">
-    <cfRule type="expression" dxfId="34" priority="56">
+    <cfRule type="expression" dxfId="32" priority="56">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="33" priority="55">
+    <cfRule type="expression" dxfId="31" priority="55">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="32" priority="46">
+    <cfRule type="expression" dxfId="30" priority="46">
       <formula>K$1=$H18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="31" priority="47">
+    <cfRule type="expression" dxfId="29" priority="47">
       <formula>K$1=$I18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18 J18:K18">
-    <cfRule type="expression" dxfId="30" priority="48">
+    <cfRule type="expression" dxfId="28" priority="48">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="29" priority="45">
+    <cfRule type="expression" dxfId="27" priority="45">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="28" priority="43">
+    <cfRule type="expression" dxfId="26" priority="43">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J74:K74">
-    <cfRule type="expression" dxfId="27" priority="42">
+    <cfRule type="expression" dxfId="25" priority="42">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74">
-    <cfRule type="expression" dxfId="26" priority="41">
+    <cfRule type="expression" dxfId="24" priority="41">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74">
-    <cfRule type="expression" dxfId="25" priority="40">
+    <cfRule type="expression" dxfId="23" priority="40">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J40:K40 H40">
-    <cfRule type="expression" dxfId="24" priority="38">
+    <cfRule type="expression" dxfId="22" priority="38">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="23" priority="37">
+    <cfRule type="expression" dxfId="21" priority="37">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J78">
-    <cfRule type="expression" dxfId="22" priority="28">
+    <cfRule type="expression" dxfId="20" priority="28">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78">
-    <cfRule type="expression" dxfId="21" priority="27">
+    <cfRule type="expression" dxfId="19" priority="27">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I78">
-    <cfRule type="expression" dxfId="20" priority="26">
+    <cfRule type="expression" dxfId="18" priority="26">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K78:V78">
-    <cfRule type="expression" dxfId="19" priority="25">
+    <cfRule type="expression" dxfId="17" priority="25">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K78:V78">
-    <cfRule type="expression" dxfId="18" priority="23">
+    <cfRule type="expression" dxfId="16" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46 G46">
-    <cfRule type="expression" dxfId="17" priority="21">
+    <cfRule type="expression" dxfId="15" priority="21">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46:F46">
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="14" priority="20">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46 E46 G46">
-    <cfRule type="expression" dxfId="15" priority="19">
+    <cfRule type="expression" dxfId="13" priority="19">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46 E46 G46">
-    <cfRule type="expression" dxfId="14" priority="18">
+    <cfRule type="expression" dxfId="12" priority="18">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46">
-    <cfRule type="expression" dxfId="13" priority="17">
+    <cfRule type="expression" dxfId="11" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J46:V46 H46">
-    <cfRule type="expression" dxfId="12" priority="16">
+    <cfRule type="expression" dxfId="10" priority="16">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="9" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21 E21:G21">
-    <cfRule type="expression" dxfId="10" priority="13">
+    <cfRule type="expression" dxfId="8" priority="13">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Correct Richard01 flag to Brazil :flag_br:
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664E5041-DA5E-8841-836E-FE8C44E3213B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C939CF6-7472-A242-90F5-3316F2E05430}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17560" yWindow="6120" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -260,9 +260,6 @@
     <t>Brazil</t>
   </si>
   <si>
-    <t>:flag_bz:</t>
-  </si>
-  <si>
     <t>Spain</t>
   </si>
   <si>
@@ -762,6 +759,9 @@
   </si>
   <si>
     <t>https://swgoh.gg/p/522439213/</t>
+  </si>
+  <si>
+    <t>:flag_br:</t>
   </si>
 </sst>
 </file>
@@ -3404,8 +3404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3508,7 +3508,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -3518,10 +3518,10 @@
       </c>
       <c r="E2" s="20"/>
       <c r="F2" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>12</v>
@@ -3599,7 +3599,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>12</v>
@@ -3662,7 +3662,7 @@
     <row r="4" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" s="7">
         <v>3</v>
@@ -3672,13 +3672,13 @@
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="I4" s="23">
         <v>0.33333333333333331</v>
@@ -3738,7 +3738,7 @@
     <row r="5" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="7">
         <v>4</v>
@@ -3748,10 +3748,10 @@
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>25</v>
@@ -3823,13 +3823,13 @@
         <v>5</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>25</v>
@@ -3892,7 +3892,7 @@
     <row r="7" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C7" s="7">
         <v>6</v>
@@ -3902,11 +3902,11 @@
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G7" s="29"/>
       <c r="H7" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I7" s="23">
         <v>0.41666666666666669</v>
@@ -3966,7 +3966,7 @@
     <row r="8" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C8" s="7">
         <v>7</v>
@@ -3976,11 +3976,11 @@
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G8" s="29"/>
       <c r="H8" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I8" s="23">
         <v>0.45833333333333331</v>
@@ -4049,16 +4049,16 @@
         <v>8</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I9" s="23">
         <v>0.45833333333333331</v>
@@ -4118,7 +4118,7 @@
     <row r="10" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
       <c r="B10" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="7">
         <v>9</v>
@@ -4127,16 +4127,16 @@
         <v>9</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I10" s="23">
         <v>0.45833333333333331</v>
@@ -4196,7 +4196,7 @@
     <row r="11" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="43"/>
       <c r="B11" s="36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C11" s="7">
         <v>10</v>
@@ -4206,11 +4206,11 @@
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I11" s="23">
         <v>0.5</v>
@@ -4270,7 +4270,7 @@
     <row r="12" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="7">
         <v>11</v>
@@ -4279,14 +4279,14 @@
         <v>11</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I12" s="23">
         <v>0.5</v>
@@ -4346,7 +4346,7 @@
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="47"/>
       <c r="B13" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" s="7">
         <v>12</v>
@@ -4358,13 +4358,13 @@
         <v>27</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I13" s="23">
         <v>0.5</v>
@@ -4424,7 +4424,7 @@
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
       <c r="B14" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C14" s="7">
         <v>13</v>
@@ -4434,11 +4434,11 @@
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I14" s="23">
         <v>0.54166666666666663</v>
@@ -4498,7 +4498,7 @@
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="47"/>
       <c r="B15" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C15" s="7">
         <v>14</v>
@@ -4508,11 +4508,11 @@
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I15" s="23">
         <v>0.58333333333333337</v>
@@ -4587,10 +4587,10 @@
         <v>18</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I16" s="23">
         <v>0.58333333333333337</v>
@@ -4650,7 +4650,7 @@
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="43"/>
       <c r="B17" s="36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C17" s="7">
         <v>16</v>
@@ -4660,7 +4660,7 @@
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="27" t="s">
@@ -4739,7 +4739,7 @@
         <v>20</v>
       </c>
       <c r="G18" s="45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H18" s="27" t="s">
         <v>10</v>
@@ -4802,7 +4802,7 @@
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="47"/>
       <c r="B19" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C19" s="7">
         <v>18</v>
@@ -4812,13 +4812,13 @@
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="29" t="s">
         <v>205</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="H19" s="29" t="s">
-        <v>206</v>
       </c>
       <c r="I19" s="23">
         <v>0.66666666666666663</v>
@@ -4890,13 +4890,13 @@
         <v>19</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H20" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I20" s="23">
         <v>0.66666666666666663</v>
@@ -4956,7 +4956,7 @@
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="52"/>
       <c r="B21" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C21" s="7">
         <v>20</v>
@@ -4965,16 +4965,16 @@
         <v>20</v>
       </c>
       <c r="E21" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="F21" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="G21" s="51" t="s">
         <v>237</v>
       </c>
-      <c r="G21" s="51" t="s">
-        <v>238</v>
-      </c>
       <c r="H21" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I21" s="23">
         <v>0.66666666666666663</v>
@@ -5049,10 +5049,10 @@
         <v>71</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I22" s="23">
         <v>0.66666666666666663</v>
@@ -5112,7 +5112,7 @@
     <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="42"/>
       <c r="B23" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C23" s="7">
         <v>22</v>
@@ -5122,13 +5122,13 @@
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" s="29" t="s">
         <v>207</v>
-      </c>
-      <c r="G23" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="H23" s="29" t="s">
-        <v>208</v>
       </c>
       <c r="I23" s="23">
         <v>0.70833333333333337</v>
@@ -5203,10 +5203,10 @@
         <v>45</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I24" s="23">
         <v>0.70833333333333337</v>
@@ -5268,7 +5268,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C25" s="7">
         <v>24</v>
@@ -5281,10 +5281,10 @@
         <v>45</v>
       </c>
       <c r="G25" s="48" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I25" s="23">
         <v>0.70833333333333337</v>
@@ -5344,7 +5344,7 @@
     <row r="26" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="53"/>
       <c r="B26" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" s="7">
         <v>25</v>
@@ -5353,16 +5353,16 @@
         <v>25</v>
       </c>
       <c r="E26" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="G26" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="G26" s="22" t="s">
-        <v>113</v>
-      </c>
       <c r="H26" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I26" s="23">
         <v>0.70833333333333337</v>
@@ -5437,10 +5437,10 @@
         <v>45</v>
       </c>
       <c r="G27" s="44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I27" s="23">
         <v>0.70833333333333337</v>
@@ -5515,10 +5515,10 @@
         <v>45</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I28" s="23">
         <v>0.70833333333333337</v>
@@ -5587,16 +5587,16 @@
         <v>28</v>
       </c>
       <c r="E29" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>75</v>
-      </c>
       <c r="G29" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H29" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I29" s="23">
         <v>0.70833333333333337</v>
@@ -5656,7 +5656,7 @@
     <row r="30" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="53"/>
       <c r="B30" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C30" s="7">
         <v>29</v>
@@ -5671,10 +5671,10 @@
         <v>71</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H30" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I30" s="23">
         <v>0.70833333333333337</v>
@@ -5749,10 +5749,10 @@
         <v>69</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H31" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I31" s="23">
         <v>0.70833333333333337</v>
@@ -5824,13 +5824,13 @@
         <v>15</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G32" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H32" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I32" s="23">
         <v>0.70833333333333337</v>
@@ -5890,7 +5890,7 @@
     <row r="33" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="53"/>
       <c r="B33" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C33" s="7">
         <v>32</v>
@@ -5900,11 +5900,11 @@
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G33" s="29"/>
       <c r="H33" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I33" s="23">
         <v>0.75</v>
@@ -5964,7 +5964,7 @@
     <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="53"/>
       <c r="B34" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C34" s="7">
         <v>33</v>
@@ -5973,16 +5973,16 @@
         <v>33</v>
       </c>
       <c r="E34" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="G34" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I34" s="23">
         <v>0.75</v>
@@ -6057,10 +6057,10 @@
         <v>69</v>
       </c>
       <c r="G35" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H35" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I35" s="23">
         <v>0.75</v>
@@ -6135,10 +6135,10 @@
         <v>20</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H36" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I36" s="23">
         <v>0.75</v>
@@ -6198,7 +6198,7 @@
     <row r="37" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="53"/>
       <c r="B37" s="32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C37" s="7">
         <v>36</v>
@@ -6207,16 +6207,16 @@
         <v>36</v>
       </c>
       <c r="E37" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="7" t="s">
-        <v>75</v>
-      </c>
       <c r="G37" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H37" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I37" s="23">
         <v>0.75</v>
@@ -6288,13 +6288,13 @@
         <v>28</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G38" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H38" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I38" s="23">
         <v>0.75</v>
@@ -6354,7 +6354,7 @@
     <row r="39" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="53"/>
       <c r="B39" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C39" s="7">
         <v>38</v>
@@ -6364,11 +6364,11 @@
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G39" s="29"/>
       <c r="H39" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I39" s="23">
         <v>0.79166666666666663</v>
@@ -6428,7 +6428,7 @@
     <row r="40" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="53"/>
       <c r="B40" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C40" s="7">
         <v>39</v>
@@ -6443,10 +6443,10 @@
         <v>20</v>
       </c>
       <c r="G40" s="46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H40" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I40" s="23">
         <v>0.79166666666666663</v>
@@ -6506,7 +6506,7 @@
     <row r="41" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="53"/>
       <c r="B41" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C41" s="7">
         <v>40</v>
@@ -6516,11 +6516,11 @@
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G41" s="29"/>
       <c r="H41" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I41" s="23">
         <v>0.83333333333333337</v>
@@ -6595,10 +6595,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H42" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I42" s="23">
         <v>0.83333333333333337</v>
@@ -6658,7 +6658,7 @@
     <row r="43" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="53"/>
       <c r="B43" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C43" s="7">
         <v>42</v>
@@ -6673,10 +6673,10 @@
         <v>45</v>
       </c>
       <c r="G43" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H43" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I43" s="23">
         <v>0.83333333333333337</v>
@@ -6736,7 +6736,7 @@
     <row r="44" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="53"/>
       <c r="B44" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C44" s="7">
         <v>43</v>
@@ -6746,11 +6746,11 @@
       </c>
       <c r="E44" s="33"/>
       <c r="F44" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G44" s="34"/>
       <c r="H44" s="29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I44" s="23">
         <v>0.875</v>
@@ -6810,7 +6810,7 @@
     <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="53"/>
       <c r="B45" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C45" s="7">
         <v>44</v>
@@ -6819,16 +6819,16 @@
         <v>44</v>
       </c>
       <c r="E45" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F45" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="G45" s="29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H45" s="29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I45" s="23">
         <v>0.875</v>
@@ -6888,7 +6888,7 @@
     <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="53"/>
       <c r="B46" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C46" s="7">
         <v>45</v>
@@ -6903,10 +6903,10 @@
         <v>71</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H46" s="29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I46" s="23">
         <v>0.875</v>
@@ -6966,7 +6966,7 @@
     <row r="47" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="53"/>
       <c r="B47" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C47" s="7">
         <v>46</v>
@@ -6981,10 +6981,10 @@
         <v>18</v>
       </c>
       <c r="G47" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H47" s="29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I47" s="23">
         <v>0.875</v>
@@ -7044,7 +7044,7 @@
     <row r="48" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="53"/>
       <c r="B48" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C48" s="7">
         <v>47</v>
@@ -7054,11 +7054,11 @@
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G48" s="29"/>
       <c r="H48" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I48" s="23">
         <v>0.91666666666666663</v>
@@ -7133,10 +7133,10 @@
         <v>20</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H49" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I49" s="23">
         <v>0.91666666666666663</v>
@@ -7196,7 +7196,7 @@
     <row r="50" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="54"/>
       <c r="B50" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C50" s="7">
         <v>49</v>
@@ -7206,11 +7206,11 @@
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G50" s="29"/>
       <c r="H50" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I50" s="23">
         <v>0.95833333333333337</v>
@@ -7270,7 +7270,7 @@
     <row r="51" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="54"/>
       <c r="B51" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C51" s="7">
         <v>50</v>
@@ -7285,10 +7285,10 @@
         <v>45</v>
       </c>
       <c r="G51" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H51" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I51" s="23">
         <v>0.95833333333333337</v>
@@ -7348,7 +7348,7 @@
     <row r="52" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="54"/>
       <c r="B52" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C52" s="7">
         <v>51</v>
@@ -7363,10 +7363,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H52" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I52" s="23">
         <v>0.95833333333333337</v>
@@ -7441,10 +7441,10 @@
         <v>20</v>
       </c>
       <c r="G53" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H53" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I53" s="23">
         <v>0.95833333333333337</v>
@@ -7519,10 +7519,10 @@
         <v>20</v>
       </c>
       <c r="G54" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H54" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I54" s="23">
         <v>0.95833333333333337</v>
@@ -7597,10 +7597,10 @@
         <v>20</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H55" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I55" s="23">
         <v>0.95833333333333337</v>
@@ -7675,10 +7675,10 @@
         <v>20</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H56" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I56" s="23">
         <v>0.95833333333333337</v>
@@ -7738,7 +7738,7 @@
     <row r="57" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="54"/>
       <c r="B57" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C57" s="7">
         <v>56</v>
@@ -7753,10 +7753,10 @@
         <v>20</v>
       </c>
       <c r="G57" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H57" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I57" s="23">
         <v>0.95833333333333337</v>
@@ -7831,10 +7831,10 @@
         <v>45</v>
       </c>
       <c r="G58" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H58" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I58" s="23">
         <v>0.95833333333333337</v>
@@ -7894,7 +7894,7 @@
     <row r="59" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="54"/>
       <c r="B59" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C59" s="7">
         <v>58</v>
@@ -7904,7 +7904,7 @@
       </c>
       <c r="E59" s="14"/>
       <c r="F59" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G59" s="9"/>
       <c r="H59" s="29" t="s">
@@ -7968,7 +7968,7 @@
     <row r="60" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="54"/>
       <c r="B60" s="35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C60" s="7">
         <v>59</v>
@@ -7983,7 +7983,7 @@
         <v>20</v>
       </c>
       <c r="G60" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H60" s="29" t="s">
         <v>9</v>
@@ -8061,7 +8061,7 @@
         <v>20</v>
       </c>
       <c r="G61" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H61" s="29" t="s">
         <v>9</v>
@@ -8139,7 +8139,7 @@
         <v>69</v>
       </c>
       <c r="G62" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H62" s="29" t="s">
         <v>9</v>
@@ -8202,7 +8202,7 @@
     <row r="63" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="54"/>
       <c r="B63" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C63" s="7">
         <v>62</v>
@@ -8217,7 +8217,7 @@
         <v>20</v>
       </c>
       <c r="G63" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H63" s="29" t="s">
         <v>9</v>
@@ -8280,7 +8280,7 @@
     <row r="64" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="54"/>
       <c r="B64" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C64" s="7">
         <v>63</v>
@@ -8295,7 +8295,7 @@
         <v>20</v>
       </c>
       <c r="G64" s="29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H64" s="29" t="s">
         <v>9</v>
@@ -8373,7 +8373,7 @@
         <v>20</v>
       </c>
       <c r="G65" s="29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H65" s="29" t="s">
         <v>9</v>
@@ -8451,7 +8451,7 @@
         <v>45</v>
       </c>
       <c r="G66" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H66" s="29" t="s">
         <v>9</v>
@@ -8529,7 +8529,7 @@
         <v>20</v>
       </c>
       <c r="G67" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H67" s="29" t="s">
         <v>9</v>
@@ -8604,10 +8604,10 @@
         <v>27</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G68" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H68" s="29" t="s">
         <v>9</v>
@@ -8670,7 +8670,7 @@
     <row r="69" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="54"/>
       <c r="B69" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C69" s="7">
         <v>68</v>
@@ -8685,7 +8685,7 @@
         <v>20</v>
       </c>
       <c r="G69" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H69" s="29" t="s">
         <v>9</v>
@@ -8763,7 +8763,7 @@
         <v>20</v>
       </c>
       <c r="G70" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H70" s="29" t="s">
         <v>9</v>
@@ -8841,7 +8841,7 @@
         <v>69</v>
       </c>
       <c r="G71" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H71" s="29" t="s">
         <v>9</v>
@@ -8919,7 +8919,7 @@
         <v>20</v>
       </c>
       <c r="G72" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H72" s="29" t="s">
         <v>9</v>
@@ -8982,7 +8982,7 @@
     <row r="73" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="54"/>
       <c r="B73" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C73" s="7">
         <v>72</v>
@@ -8992,11 +8992,11 @@
       </c>
       <c r="E73" s="14"/>
       <c r="F73" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G73" s="29"/>
       <c r="H73" s="29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I73" s="23">
         <v>4.1666666666666664E-2</v>
@@ -9065,16 +9065,16 @@
         <v>73</v>
       </c>
       <c r="E74" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F74" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F74" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="G74" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H74" s="29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I74" s="23">
         <v>4.1666666666666664E-2</v>
@@ -9134,7 +9134,7 @@
     <row r="75" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="54"/>
       <c r="B75" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C75" s="7">
         <v>74</v>
@@ -9144,11 +9144,11 @@
       </c>
       <c r="E75" s="14"/>
       <c r="F75" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G75" s="29"/>
       <c r="H75" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I75" s="23">
         <v>8.3333333333333329E-2</v>
@@ -9223,10 +9223,10 @@
         <v>20</v>
       </c>
       <c r="G76" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H76" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I76" s="23">
         <v>8.3333333333333329E-2</v>
@@ -9301,10 +9301,10 @@
         <v>69</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H77" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I77" s="23">
         <v>8.3333333333333329E-2</v>
@@ -9364,7 +9364,7 @@
     <row r="78" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="54"/>
       <c r="B78" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C78" s="7">
         <v>77</v>
@@ -9376,13 +9376,13 @@
         <v>72</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>73</v>
+        <v>240</v>
       </c>
       <c r="G78" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H78" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I78" s="23">
         <v>8.3333333333333329E-2</v>
@@ -9442,7 +9442,7 @@
     <row r="79" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="54"/>
       <c r="B79" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C79" s="7">
         <v>78</v>
@@ -9452,11 +9452,11 @@
       </c>
       <c r="E79" s="14"/>
       <c r="F79" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G79" s="29"/>
       <c r="H79" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I79" s="23">
         <v>0.125</v>
@@ -9531,10 +9531,10 @@
         <v>20</v>
       </c>
       <c r="G80" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H80" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I80" s="23">
         <v>0.125</v>
@@ -9609,10 +9609,10 @@
         <v>20</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H81" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I81" s="23">
         <v>0.125</v>
@@ -9672,7 +9672,7 @@
     <row r="82" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="54"/>
       <c r="B82" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C82" s="7">
         <v>81</v>
@@ -9682,11 +9682,11 @@
       </c>
       <c r="E82" s="14"/>
       <c r="F82" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G82" s="29"/>
       <c r="H82" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I82" s="23">
         <v>0.16666666666666666</v>
@@ -9746,7 +9746,7 @@
     <row r="83" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="54"/>
       <c r="B83" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C83" s="7">
         <v>82</v>
@@ -9756,11 +9756,11 @@
       </c>
       <c r="E83" s="14"/>
       <c r="F83" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G83" s="29"/>
       <c r="H83" s="29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I83" s="23">
         <v>0.20833333333333334</v>
@@ -9835,10 +9835,10 @@
         <v>20</v>
       </c>
       <c r="G84" s="34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H84" s="29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I84" s="23">
         <v>0.20833333333333334</v>
@@ -9898,7 +9898,7 @@
     <row r="85" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="54"/>
       <c r="B85" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C85" s="7">
         <v>84</v>
@@ -9908,11 +9908,11 @@
       </c>
       <c r="E85" s="14"/>
       <c r="F85" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G85" s="29"/>
       <c r="H85" s="29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I85" s="23">
         <v>0.25</v>
@@ -9986,10 +9986,10 @@
         <v>20</v>
       </c>
       <c r="G86" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H86" s="29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I86" s="23">
         <v>0.25</v>
@@ -10051,11 +10051,11 @@
     <sortCondition ref="D2:D70"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Move DaCoachDitka to MST
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF3BF37-6A51-4941-B5F5-B8DDC29EA39E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2419F480-363A-D140-97FA-2DDA94547316}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19460" yWindow="5940" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1208,47 +1208,60 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="274">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
+  <dxfs count="276">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3462,8 +3475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B65" sqref="A65:XFD65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3549,7 +3562,7 @@
         <v>AKST</v>
       </c>
       <c r="T1" s="3" t="str">
-        <f>H74</f>
+        <f>H73</f>
         <v>CST</v>
       </c>
       <c r="U1" s="3" t="str">
@@ -3557,7 +3570,7 @@
         <v>CST</v>
       </c>
       <c r="V1" s="3" t="str">
-        <f>H70</f>
+        <f>H69</f>
         <v>CST</v>
       </c>
     </row>
@@ -8414,13 +8427,13 @@
     <row r="65" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="55"/>
       <c r="B65" s="18" t="s">
-        <v>243</v>
+        <v>88</v>
       </c>
       <c r="C65" s="7">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D65" s="7">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E65" s="39" t="s">
         <v>27</v>
@@ -8429,7 +8442,7 @@
         <v>20</v>
       </c>
       <c r="G65" s="29" t="s">
-        <v>244</v>
+        <v>162</v>
       </c>
       <c r="H65" s="29" t="s">
         <v>9</v>
@@ -8492,13 +8505,13 @@
     <row r="66" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="55"/>
       <c r="B66" s="18" t="s">
-        <v>88</v>
+        <v>180</v>
       </c>
       <c r="C66" s="7">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D66" s="7">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E66" s="39" t="s">
         <v>27</v>
@@ -8507,7 +8520,7 @@
         <v>20</v>
       </c>
       <c r="G66" s="29" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="H66" s="29" t="s">
         <v>9</v>
@@ -8569,23 +8582,23 @@
     </row>
     <row r="67" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="55"/>
-      <c r="B67" s="18" t="s">
-        <v>180</v>
+      <c r="B67" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="C67" s="7">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D67" s="7">
-        <v>66</v>
-      </c>
-      <c r="E67" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="E67" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F67" s="40" t="s">
-        <v>20</v>
+      <c r="F67" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="G67" s="29" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="H67" s="29" t="s">
         <v>9</v>
@@ -8648,22 +8661,22 @@
     <row r="68" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="55"/>
       <c r="B68" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C68" s="7">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D68" s="7">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E68" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G68" s="29" t="s">
-        <v>164</v>
+        <v>20</v>
+      </c>
+      <c r="G68" s="27" t="s">
+        <v>165</v>
       </c>
       <c r="H68" s="29" t="s">
         <v>9</v>
@@ -8725,23 +8738,23 @@
     </row>
     <row r="69" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="55"/>
-      <c r="B69" s="35" t="s">
-        <v>61</v>
+      <c r="B69" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="C69" s="7">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D69" s="7">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E69" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F69" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G69" s="27" t="s">
-        <v>165</v>
+      <c r="F69" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G69" s="29" t="s">
+        <v>166</v>
       </c>
       <c r="H69" s="29" t="s">
         <v>9</v>
@@ -8803,23 +8816,23 @@
     </row>
     <row r="70" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="55"/>
-      <c r="B70" s="18" t="s">
-        <v>58</v>
+      <c r="B70" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="C70" s="7">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D70" s="7">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E70" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F70" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G70" s="29" t="s">
-        <v>166</v>
+      <c r="F70" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" s="22" t="s">
+        <v>124</v>
       </c>
       <c r="H70" s="29" t="s">
         <v>9</v>
@@ -8834,61 +8847,61 @@
         <f>$I70+Sheet2!B$1/24</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="L70" s="23">
+      <c r="L70" s="16">
         <f>$I70+Sheet2!B$2/24</f>
         <v>0.375</v>
       </c>
-      <c r="M70" s="23">
+      <c r="M70" s="16">
         <f>$I70+Sheet2!B$3/24</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N70" s="23">
+      <c r="N70" s="16">
         <f>$I70+Sheet2!B$4/24</f>
         <v>0.125</v>
       </c>
-      <c r="O70" s="23">
+      <c r="O70" s="16">
         <f>$I70+Sheet2!B$5/24</f>
         <v>0.125</v>
       </c>
-      <c r="P70" s="23">
+      <c r="P70" s="16">
         <f>$I70+Sheet2!B$6/24</f>
         <v>0.125</v>
       </c>
-      <c r="Q70" s="23">
+      <c r="Q70" s="16">
         <f>$I70+Sheet2!B$7/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="R70" s="23">
+      <c r="R70" s="16">
         <f>$I70+Sheet2!B$8/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="S70" s="23">
+      <c r="S70" s="16">
         <f>$I70+Sheet2!B$9/24</f>
         <v>-0.16666666666666666</v>
       </c>
-      <c r="T70" s="23">
+      <c r="T70" s="16">
         <f>$I70+Sheet2!B$10/24</f>
         <v>-0.20833333333333334</v>
       </c>
-      <c r="U70" s="23">
+      <c r="U70" s="16">
         <f>$I70+Sheet2!B$11/24</f>
         <v>-0.25</v>
       </c>
-      <c r="V70" s="23">
+      <c r="V70" s="16">
         <f>$I70+Sheet2!B$12/24</f>
         <v>-0.29166666666666669</v>
       </c>
     </row>
     <row r="71" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="55"/>
-      <c r="B71" s="12" t="s">
-        <v>90</v>
+      <c r="B71" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="C71" s="7">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D71" s="7">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E71" s="14" t="s">
         <v>27</v>
@@ -8896,8 +8909,8 @@
       <c r="F71" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G71" s="22" t="s">
-        <v>124</v>
+      <c r="G71" s="29" t="s">
+        <v>167</v>
       </c>
       <c r="H71" s="29" t="s">
         <v>9</v>
@@ -8912,70 +8925,70 @@
         <f>$I71+Sheet2!B$1/24</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="L71" s="16">
+      <c r="L71" s="23">
         <f>$I71+Sheet2!B$2/24</f>
         <v>0.375</v>
       </c>
-      <c r="M71" s="16">
+      <c r="M71" s="23">
         <f>$I71+Sheet2!B$3/24</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N71" s="16">
+      <c r="N71" s="23">
         <f>$I71+Sheet2!B$4/24</f>
         <v>0.125</v>
       </c>
-      <c r="O71" s="16">
+      <c r="O71" s="23">
         <f>$I71+Sheet2!B$5/24</f>
         <v>0.125</v>
       </c>
-      <c r="P71" s="16">
+      <c r="P71" s="23">
         <f>$I71+Sheet2!B$6/24</f>
         <v>0.125</v>
       </c>
-      <c r="Q71" s="16">
+      <c r="Q71" s="23">
         <f>$I71+Sheet2!B$7/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="R71" s="16">
+      <c r="R71" s="23">
         <f>$I71+Sheet2!B$8/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="S71" s="16">
+      <c r="S71" s="23">
         <f>$I71+Sheet2!B$9/24</f>
         <v>-0.16666666666666666</v>
       </c>
-      <c r="T71" s="16">
+      <c r="T71" s="23">
         <f>$I71+Sheet2!B$10/24</f>
         <v>-0.20833333333333334</v>
       </c>
-      <c r="U71" s="16">
+      <c r="U71" s="23">
         <f>$I71+Sheet2!B$11/24</f>
         <v>-0.25</v>
       </c>
-      <c r="V71" s="16">
+      <c r="V71" s="23">
         <f>$I71+Sheet2!B$12/24</f>
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="72" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="55"/>
       <c r="B72" s="18" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C72" s="7">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D72" s="7">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F72" s="19" t="s">
-        <v>20</v>
+      <c r="F72" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="G72" s="29" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H72" s="29" t="s">
         <v>9</v>
@@ -9035,25 +9048,25 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="73" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="55"/>
       <c r="B73" s="18" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C73" s="7">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D73" s="7">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E73" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F73" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G73" s="29" t="s">
-        <v>168</v>
+      <c r="F73" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G73" s="27" t="s">
+        <v>169</v>
       </c>
       <c r="H73" s="29" t="s">
         <v>9</v>
@@ -9116,97 +9129,97 @@
     <row r="74" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="55"/>
       <c r="B74" s="18" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="C74" s="7">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D74" s="7">
-        <v>73</v>
-      </c>
-      <c r="E74" s="14" t="s">
-        <v>27</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E74" s="14"/>
       <c r="F74" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G74" s="27" t="s">
-        <v>169</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="G74" s="29"/>
       <c r="H74" s="29" t="s">
-        <v>9</v>
+        <v>221</v>
       </c>
       <c r="I74" s="23">
-        <v>0</v>
-      </c>
-      <c r="J74" s="26" t="s">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="J74" s="28" t="s">
         <v>14</v>
       </c>
       <c r="K74" s="25">
         <f>$I74+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="L74" s="23">
         <f>$I74+Sheet2!B$2/24</f>
-        <v>0.375</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M74" s="23">
         <f>$I74+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="N74" s="23">
         <f>$I74+Sheet2!B$4/24</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="O74" s="23">
         <f>$I74+Sheet2!B$5/24</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P74" s="23">
         <f>$I74+Sheet2!B$6/24</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q74" s="23">
         <f>$I74+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
       <c r="R74" s="23">
         <f>$I74+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S74" s="23">
         <f>$I74+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
+        <v>-0.125</v>
       </c>
       <c r="T74" s="23">
         <f>$I74+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="U74" s="23">
         <f>$I74+Sheet2!B$11/24</f>
-        <v>-0.25</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="V74" s="23">
         <f>$I74+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="75" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="55"/>
       <c r="B75" s="18" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="C75" s="7">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D75" s="7">
-        <v>74</v>
-      </c>
-      <c r="E75" s="14"/>
-      <c r="F75" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="G75" s="29"/>
+        <v>75</v>
+      </c>
+      <c r="E75" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G75" s="34" t="s">
+        <v>146</v>
+      </c>
       <c r="H75" s="29" t="s">
         <v>221</v>
       </c>
@@ -9268,22 +9281,22 @@
     <row r="76" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="55"/>
       <c r="B76" s="18" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="C76" s="7">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D76" s="7">
-        <v>75</v>
-      </c>
-      <c r="E76" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G76" s="34" t="s">
-        <v>146</v>
+        <v>64</v>
+      </c>
+      <c r="E76" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F76" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G76" s="29" t="s">
+        <v>244</v>
       </c>
       <c r="H76" s="29" t="s">
         <v>221</v>
@@ -10259,15 +10272,15 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:V72">
-    <sortCondition ref="D2:D72"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:V71">
+    <sortCondition ref="D2:D71"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -10275,1373 +10288,1383 @@
     <mergeCell ref="A25:A50"/>
     <mergeCell ref="A51:A87"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V44 K46:V64 K66:V88">
-    <cfRule type="expression" dxfId="273" priority="650">
+  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V44 K46:V88">
+    <cfRule type="expression" dxfId="275" priority="658">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K17:V17 K19:V19 K23:V23 K20 K24:K32 K22">
-    <cfRule type="expression" dxfId="272" priority="652">
+    <cfRule type="expression" dxfId="274" priority="660">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K53:V53 G53 G63 B64:B67 G73 G88 E61:G61 G30 B74 E74:G74 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 B70:B72 E70:G72 L40:V40 K86:V86 G86 K78:V79 K82:V83 K88:V88 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B83 J11:V14 J83:V83 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L76:V76 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E83:G83 B76 E60:V60 E64:G64 B50:B61 B40 B44:B46 B80 B48 J48:V48 G75:G79 E24:G29 B20:B38 E5:G5 E48:H48 E80:G80 E76:G76 L24:V32 L20:V20 L22:V22 G58:V59 G66:G69 E44:H44 E45:G46 L63:V64 L66:V74">
-    <cfRule type="expression" dxfId="271" priority="656">
+  <conditionalFormatting sqref="K53:V53 G53 G63 G72 G88 E61:G61 G30 B73 E73:G73 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 B69:B71 E69:G71 L40:V40 K86:V86 G86 K78:V79 K82:V83 K88:V88 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B83 J11:V14 J83:V83 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L75:V75 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E83:G83 E60:V60 E64:G64 B50:B61 B40 B44:B46 B80 B48 J48:V48 G74:G79 E24:G29 B20:B38 E5:G5 E48:H48 E80:G80 E75:G76 L24:V32 L20:V20 L22:V22 G58:V59 G65:G68 E44:H44 E45:G46 L63:V73 B64:B66 B75:B76 C4:D88">
+    <cfRule type="expression" dxfId="273" priority="664">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63 L63:V63">
-    <cfRule type="expression" dxfId="270" priority="633">
+    <cfRule type="expression" dxfId="272" priority="641">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="expression" dxfId="269" priority="631">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B69 L69:V69">
-    <cfRule type="expression" dxfId="268" priority="629">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B73 L73:V73">
-    <cfRule type="expression" dxfId="267" priority="627">
+    <cfRule type="expression" dxfId="271" priority="639">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68 L68:V68">
-    <cfRule type="expression" dxfId="266" priority="625">
+    <cfRule type="expression" dxfId="270" priority="637">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B72 L72:V72">
+    <cfRule type="expression" dxfId="269" priority="635">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B67 L67:V67">
+    <cfRule type="expression" dxfId="268" priority="633">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86 K86:V86 E86:F86">
-    <cfRule type="expression" dxfId="265" priority="621">
+    <cfRule type="expression" dxfId="267" priority="629">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="264" priority="619">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E73">
-    <cfRule type="expression" dxfId="263" priority="616">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
-    <cfRule type="expression" dxfId="262" priority="615">
+    <cfRule type="expression" dxfId="266" priority="627">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E72">
+    <cfRule type="expression" dxfId="265" priority="624">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
+    <cfRule type="expression" dxfId="264" priority="623">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82:B83 J82:V83">
-    <cfRule type="expression" dxfId="261" priority="612">
+    <cfRule type="expression" dxfId="263" priority="620">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79:B80 J79:V79 E79:E80">
-    <cfRule type="expression" dxfId="260" priority="610">
+    <cfRule type="expression" dxfId="262" priority="618">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E82:F83">
-    <cfRule type="expression" dxfId="259" priority="608">
+    <cfRule type="expression" dxfId="261" priority="616">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78 J78:V78">
-    <cfRule type="expression" dxfId="258" priority="606">
+    <cfRule type="expression" dxfId="260" priority="614">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88 J88:V88 E88">
-    <cfRule type="expression" dxfId="257" priority="604">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F68">
-    <cfRule type="expression" dxfId="256" priority="596">
+    <cfRule type="expression" dxfId="259" priority="612">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F67">
+    <cfRule type="expression" dxfId="258" priority="604">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K61:V61">
-    <cfRule type="expression" dxfId="255" priority="536">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F73">
-    <cfRule type="expression" dxfId="254" priority="558">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B75:B76 E75:F76">
-    <cfRule type="expression" dxfId="253" priority="522">
+    <cfRule type="expression" dxfId="257" priority="544">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F72">
+    <cfRule type="expression" dxfId="256" priority="566">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B74:B76 E74:F76">
+    <cfRule type="expression" dxfId="255" priority="530">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62">
-    <cfRule type="expression" dxfId="252" priority="543">
+    <cfRule type="expression" dxfId="254" priority="551">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45:F45">
-    <cfRule type="expression" dxfId="251" priority="550">
+    <cfRule type="expression" dxfId="253" priority="558">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62 L62:V62">
-    <cfRule type="expression" dxfId="250" priority="544">
+    <cfRule type="expression" dxfId="252" priority="552">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F79:F80">
-    <cfRule type="expression" dxfId="249" priority="556">
+    <cfRule type="expression" dxfId="251" priority="564">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F63">
-    <cfRule type="expression" dxfId="248" priority="552">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69:F69">
-    <cfRule type="expression" dxfId="247" priority="551">
+    <cfRule type="expression" dxfId="250" priority="560">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68:F68">
+    <cfRule type="expression" dxfId="249" priority="559">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:F78">
-    <cfRule type="expression" dxfId="246" priority="549">
+    <cfRule type="expression" dxfId="248" priority="557">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L62:V62 G62">
-    <cfRule type="expression" dxfId="245" priority="546">
+    <cfRule type="expression" dxfId="247" priority="554">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:V7">
-    <cfRule type="expression" dxfId="244" priority="491">
+    <cfRule type="expression" dxfId="246" priority="499">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F62">
-    <cfRule type="expression" dxfId="243" priority="540">
+    <cfRule type="expression" dxfId="245" priority="548">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:V48">
-    <cfRule type="expression" dxfId="242" priority="660">
+    <cfRule type="expression" dxfId="244" priority="668">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K61:V61">
-    <cfRule type="expression" dxfId="241" priority="537">
+    <cfRule type="expression" dxfId="243" priority="545">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:V10">
-    <cfRule type="expression" dxfId="240" priority="482">
+    <cfRule type="expression" dxfId="242" priority="490">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H14 J13:V14 L18:V18">
-    <cfRule type="expression" dxfId="239" priority="528">
+    <cfRule type="expression" dxfId="241" priority="536">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:V14 L18:V18">
+    <cfRule type="expression" dxfId="240" priority="537">
+      <formula>K$1=#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:G3 B7 E7:G7">
+    <cfRule type="expression" dxfId="239" priority="531">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K74:V74 L75:V75">
     <cfRule type="expression" dxfId="238" priority="529">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J74:V74 L75:V75">
+    <cfRule type="expression" dxfId="237" priority="527">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H74">
+    <cfRule type="expression" dxfId="236" priority="526">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J77:V77">
+    <cfRule type="expression" dxfId="235" priority="521">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B77 E77:F77">
+    <cfRule type="expression" dxfId="234" priority="524">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K77:V77">
+    <cfRule type="expression" dxfId="233" priority="523">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H77">
+    <cfRule type="expression" dxfId="232" priority="520">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="expression" dxfId="231" priority="513">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30:F30">
+    <cfRule type="expression" dxfId="230" priority="518">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43 E43 L43:V43 G43">
+    <cfRule type="expression" dxfId="229" priority="517">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4 E4:G4">
+    <cfRule type="expression" dxfId="228" priority="512">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
+    <cfRule type="expression" dxfId="227" priority="511">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6 E6:H6 J6:V6">
+    <cfRule type="expression" dxfId="226" priority="509">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:V5">
+    <cfRule type="expression" dxfId="225" priority="506">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:L4">
+    <cfRule type="expression" dxfId="224" priority="501">
+      <formula>K$1=$H4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:V4">
+    <cfRule type="expression" dxfId="223" priority="502">
+      <formula>K$1=$I4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:V4">
+    <cfRule type="expression" dxfId="222" priority="503">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="expression" dxfId="221" priority="496">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:B10 E8:G10">
+    <cfRule type="expression" dxfId="220" priority="495">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8:K8">
+    <cfRule type="expression" dxfId="219" priority="493">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15 E15:H15 J15:V15">
+    <cfRule type="expression" dxfId="218" priority="485">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15 J15:V15">
+    <cfRule type="expression" dxfId="217" priority="482">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15:V15">
+    <cfRule type="expression" dxfId="216" priority="483">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G3 B7 E7:G7 C4:D88">
-    <cfRule type="expression" dxfId="237" priority="523">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K75:V75 L76:V76">
-    <cfRule type="expression" dxfId="236" priority="521">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J75:V75 L76:V76">
-    <cfRule type="expression" dxfId="235" priority="519">
+  <conditionalFormatting sqref="B15 E15:G15">
+    <cfRule type="expression" dxfId="215" priority="481">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16 J16:K16">
+    <cfRule type="expression" dxfId="214" priority="478">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16 J16:K16">
+    <cfRule type="expression" dxfId="213" priority="475">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="expression" dxfId="212" priority="476">
+      <formula>K$1=#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H49 J49:V49">
+    <cfRule type="expression" dxfId="211" priority="370">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19 E19:H19 J19:V19">
+    <cfRule type="expression" dxfId="210" priority="471">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="expression" dxfId="209" priority="327">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27 J27:K27">
+    <cfRule type="expression" dxfId="208" priority="433">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H61:J61">
+    <cfRule type="expression" dxfId="207" priority="365">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20 J20:K20">
+    <cfRule type="expression" dxfId="206" priority="460">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22 J22:K22">
+    <cfRule type="expression" dxfId="205" priority="455">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="expression" dxfId="204" priority="360">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="expression" dxfId="203" priority="359">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24 J24:K24">
+    <cfRule type="expression" dxfId="202" priority="448">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="expression" dxfId="201" priority="356">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25 J25:K25">
+    <cfRule type="expression" dxfId="200" priority="443">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H63 J63">
+    <cfRule type="expression" dxfId="199" priority="354">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26 J26:K26">
+    <cfRule type="expression" dxfId="198" priority="438">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="expression" dxfId="197" priority="351">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H64 J64">
+    <cfRule type="expression" dxfId="196" priority="350">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65">
+    <cfRule type="expression" dxfId="195" priority="348">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65">
+    <cfRule type="expression" dxfId="194" priority="347">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28 J28:K28">
+    <cfRule type="expression" dxfId="193" priority="428">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K66">
+    <cfRule type="expression" dxfId="192" priority="344">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29 J29:K29">
+    <cfRule type="expression" dxfId="191" priority="423">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66 J66">
+    <cfRule type="expression" dxfId="190" priority="342">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30 J30:K30">
+    <cfRule type="expression" dxfId="189" priority="418">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31 J31:K31">
+    <cfRule type="expression" dxfId="188" priority="413">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67">
+    <cfRule type="expression" dxfId="187" priority="336">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67">
+    <cfRule type="expression" dxfId="186" priority="335">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32 J32:K32">
+    <cfRule type="expression" dxfId="185" priority="408">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K68">
+    <cfRule type="expression" dxfId="184" priority="332">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H68 J68">
+    <cfRule type="expression" dxfId="183" priority="330">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="expression" dxfId="182" priority="396">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="expression" dxfId="181" priority="328">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="expression" dxfId="180" priority="393">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
+    <cfRule type="expression" dxfId="179" priority="390">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H69 J69">
+    <cfRule type="expression" dxfId="178" priority="326">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H37">
+    <cfRule type="expression" dxfId="177" priority="387">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:B40 J39:V39 E39:H39 E40:G40 L40:V40">
+    <cfRule type="expression" dxfId="176" priority="384">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41:V41 B41:B43 E43 E41:H41 G43 E42:G42 L42:V43">
+    <cfRule type="expression" dxfId="175" priority="380">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="174" priority="324">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="173" priority="323">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49:G49 B49">
+    <cfRule type="expression" dxfId="172" priority="373">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I81">
+    <cfRule type="expression" dxfId="171" priority="230">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H50">
+    <cfRule type="expression" dxfId="170" priority="369">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53 J53">
+    <cfRule type="expression" dxfId="169" priority="368">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K73">
+    <cfRule type="expression" dxfId="168" priority="316">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72">
+    <cfRule type="expression" dxfId="167" priority="319">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H71 J71">
+    <cfRule type="expression" dxfId="166" priority="322">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62 J62">
+    <cfRule type="expression" dxfId="165" priority="358">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="expression" dxfId="164" priority="355">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="expression" dxfId="163" priority="352">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H65 J65">
+    <cfRule type="expression" dxfId="162" priority="346">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K66">
+    <cfRule type="expression" dxfId="161" priority="343">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H67 J67">
+    <cfRule type="expression" dxfId="160" priority="334">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K68">
+    <cfRule type="expression" dxfId="159" priority="331">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72">
+    <cfRule type="expression" dxfId="158" priority="320">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H72 J72">
+    <cfRule type="expression" dxfId="157" priority="318">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K73">
+    <cfRule type="expression" dxfId="156" priority="315">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H73 J73">
+    <cfRule type="expression" dxfId="155" priority="314">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K70">
+    <cfRule type="expression" dxfId="154" priority="312">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K70">
+    <cfRule type="expression" dxfId="153" priority="311">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H70 J70">
+    <cfRule type="expression" dxfId="152" priority="310">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G81">
+    <cfRule type="expression" dxfId="151" priority="305">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J81:V81">
+    <cfRule type="expression" dxfId="150" priority="300">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B81 E81:F81">
+    <cfRule type="expression" dxfId="149" priority="302">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81:V81">
+    <cfRule type="expression" dxfId="148" priority="301">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H81">
+    <cfRule type="expression" dxfId="147" priority="299">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H78">
+    <cfRule type="expression" dxfId="146" priority="296">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H79">
+    <cfRule type="expression" dxfId="145" priority="294">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G84">
+    <cfRule type="expression" dxfId="144" priority="291">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="expression" dxfId="143" priority="148">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J84:V84">
+    <cfRule type="expression" dxfId="142" priority="286">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B84 E84:F84">
+    <cfRule type="expression" dxfId="141" priority="288">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K84:V84">
+    <cfRule type="expression" dxfId="140" priority="287">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H84">
+    <cfRule type="expression" dxfId="139" priority="285">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H82">
+    <cfRule type="expression" dxfId="138" priority="283">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G85">
+    <cfRule type="expression" dxfId="137" priority="281">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="expression" dxfId="136" priority="138">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J85:V85">
+    <cfRule type="expression" dxfId="135" priority="276">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B85 E85:F85">
+    <cfRule type="expression" dxfId="134" priority="278">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K85:V85">
+    <cfRule type="expression" dxfId="133" priority="277">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H85">
+    <cfRule type="expression" dxfId="132" priority="275">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J86">
+    <cfRule type="expression" dxfId="131" priority="273">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H86">
+    <cfRule type="expression" dxfId="130" priority="272">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G87">
+    <cfRule type="expression" dxfId="129" priority="270">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33">
+    <cfRule type="expression" dxfId="128" priority="127">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J87:V87">
+    <cfRule type="expression" dxfId="127" priority="265">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B87 E87:F87">
+    <cfRule type="expression" dxfId="126" priority="267">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K87:V87">
+    <cfRule type="expression" dxfId="125" priority="266">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H87">
+    <cfRule type="expression" dxfId="124" priority="264">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K43">
+    <cfRule type="expression" dxfId="123" priority="262">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43 J43">
+    <cfRule type="expression" dxfId="122" priority="260">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J38:K38">
+    <cfRule type="expression" dxfId="121" priority="257">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H38">
+    <cfRule type="expression" dxfId="120" priority="255">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I49">
+    <cfRule type="expression" dxfId="119" priority="113">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I53">
+    <cfRule type="expression" dxfId="118" priority="251">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I66">
+    <cfRule type="expression" dxfId="117" priority="244">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I62">
+    <cfRule type="expression" dxfId="116" priority="248">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I63">
+    <cfRule type="expression" dxfId="115" priority="247">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I64">
+    <cfRule type="expression" dxfId="114" priority="246">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I65">
+    <cfRule type="expression" dxfId="113" priority="245">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I67">
+    <cfRule type="expression" dxfId="112" priority="242">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I68">
+    <cfRule type="expression" dxfId="111" priority="241">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I69">
+    <cfRule type="expression" dxfId="110" priority="240">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I70">
+    <cfRule type="expression" dxfId="109" priority="239">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I71">
+    <cfRule type="expression" dxfId="108" priority="238">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I72">
+    <cfRule type="expression" dxfId="107" priority="237">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I73">
+    <cfRule type="expression" dxfId="106" priority="236">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I74">
+    <cfRule type="expression" dxfId="105" priority="235">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I77">
+    <cfRule type="expression" dxfId="104" priority="233">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I78">
+    <cfRule type="expression" dxfId="103" priority="232">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I79">
+    <cfRule type="expression" dxfId="102" priority="231">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I82">
+    <cfRule type="expression" dxfId="101" priority="229">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I84">
+    <cfRule type="expression" dxfId="100" priority="228">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I85">
+    <cfRule type="expression" dxfId="99" priority="227">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I86">
+    <cfRule type="expression" dxfId="98" priority="226">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I87">
+    <cfRule type="expression" dxfId="97" priority="225">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I88">
+    <cfRule type="expression" dxfId="96" priority="224">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H88">
+    <cfRule type="expression" dxfId="95" priority="223">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="expression" dxfId="94" priority="222">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="expression" dxfId="93" priority="221">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="expression" dxfId="92" priority="220">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="expression" dxfId="91" priority="219">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="expression" dxfId="90" priority="218">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="expression" dxfId="89" priority="217">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="expression" dxfId="88" priority="216">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="expression" dxfId="87" priority="215">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="expression" dxfId="86" priority="147">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="expression" dxfId="85" priority="146">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="expression" dxfId="84" priority="145">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="expression" dxfId="83" priority="144">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="expression" dxfId="82" priority="143">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="expression" dxfId="81" priority="137">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="expression" dxfId="80" priority="141">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="expression" dxfId="79" priority="140">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
+    <cfRule type="expression" dxfId="78" priority="139">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="expression" dxfId="77" priority="136">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="expression" dxfId="76" priority="135">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="expression" dxfId="75" priority="134">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="expression" dxfId="74" priority="133">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="expression" dxfId="73" priority="132">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30">
+    <cfRule type="expression" dxfId="72" priority="131">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="expression" dxfId="71" priority="130">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="expression" dxfId="70" priority="129">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
+    <cfRule type="expression" dxfId="69" priority="126">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50">
+    <cfRule type="expression" dxfId="68" priority="112">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
+    <cfRule type="expression" dxfId="67" priority="124">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="expression" dxfId="66" priority="123">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="expression" dxfId="65" priority="122">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38">
+    <cfRule type="expression" dxfId="64" priority="121">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="expression" dxfId="63" priority="120">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
+    <cfRule type="expression" dxfId="62" priority="119">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43">
+    <cfRule type="expression" dxfId="61" priority="118">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="expression" dxfId="60" priority="116">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I48">
+    <cfRule type="expression" dxfId="59" priority="114">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:V10">
+    <cfRule type="expression" dxfId="58" priority="104">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="expression" dxfId="57" priority="93">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H83">
+    <cfRule type="expression" dxfId="56" priority="102">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I83">
+    <cfRule type="expression" dxfId="55" priority="101">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:K9">
+    <cfRule type="expression" dxfId="54" priority="92">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="expression" dxfId="53" priority="91">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="52" priority="94">
+      <formula>K$1=$H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="51" priority="95">
+      <formula>K$1=$I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="50" priority="89">
+      <formula>K$1=$H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="49" priority="90">
+      <formula>K$1=$I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="expression" dxfId="48" priority="88">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:K10">
+    <cfRule type="expression" dxfId="47" priority="87">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="expression" dxfId="46" priority="86">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43">
+    <cfRule type="expression" dxfId="45" priority="79">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42:K42 H42">
+    <cfRule type="expression" dxfId="44" priority="74">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I42">
+    <cfRule type="expression" dxfId="43" priority="73">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="42" priority="64">
+      <formula>K$1=$H18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="41" priority="65">
+      <formula>K$1=$I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18 J18:K18">
+    <cfRule type="expression" dxfId="40" priority="66">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="expression" dxfId="39" priority="63">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K75">
+    <cfRule type="expression" dxfId="38" priority="61">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J75:K75">
+    <cfRule type="expression" dxfId="37" priority="60">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75">
-    <cfRule type="expression" dxfId="234" priority="518">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J77:V77">
-    <cfRule type="expression" dxfId="233" priority="513">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B77 E77:F77">
-    <cfRule type="expression" dxfId="232" priority="516">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K77:V77">
-    <cfRule type="expression" dxfId="231" priority="515">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="230" priority="512">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="229" priority="505">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30:F30">
-    <cfRule type="expression" dxfId="228" priority="510">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B43 E43 L43:V43 G43">
-    <cfRule type="expression" dxfId="227" priority="509">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4 E4:G4">
-    <cfRule type="expression" dxfId="226" priority="504">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="225" priority="503">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6 E6:H6 J6:V6">
-    <cfRule type="expression" dxfId="224" priority="501">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:V5">
-    <cfRule type="expression" dxfId="223" priority="498">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:L4">
-    <cfRule type="expression" dxfId="222" priority="493">
-      <formula>K$1=$H4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:V4">
-    <cfRule type="expression" dxfId="221" priority="494">
-      <formula>K$1=$I4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4:V4">
-    <cfRule type="expression" dxfId="220" priority="495">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="219" priority="488">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B10 E8:G10">
-    <cfRule type="expression" dxfId="218" priority="487">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8:K8">
-    <cfRule type="expression" dxfId="217" priority="485">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15 E15:H15 J15:V15">
-    <cfRule type="expression" dxfId="216" priority="477">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15 J15:V15">
-    <cfRule type="expression" dxfId="215" priority="474">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15:V15">
-    <cfRule type="expression" dxfId="214" priority="475">
-      <formula>K$1=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15 E15:G15">
-    <cfRule type="expression" dxfId="213" priority="473">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="212" priority="470">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="211" priority="467">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="210" priority="468">
-      <formula>K$1=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H49 J49:V49">
-    <cfRule type="expression" dxfId="209" priority="362">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19 E19:H19 J19:V19">
-    <cfRule type="expression" dxfId="208" priority="463">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="207" priority="319">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27 J27:K27">
-    <cfRule type="expression" dxfId="206" priority="425">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H61:J61">
-    <cfRule type="expression" dxfId="205" priority="357">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20 J20:K20">
-    <cfRule type="expression" dxfId="204" priority="452">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22 J22:K22">
-    <cfRule type="expression" dxfId="203" priority="447">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="expression" dxfId="202" priority="352">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
-    <cfRule type="expression" dxfId="201" priority="351">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24 J24:K24">
-    <cfRule type="expression" dxfId="200" priority="440">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="199" priority="348">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25 J25:K25">
-    <cfRule type="expression" dxfId="198" priority="435">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H63 J63">
-    <cfRule type="expression" dxfId="197" priority="346">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26 J26:K26">
-    <cfRule type="expression" dxfId="196" priority="430">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="195" priority="343">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H64 J64">
-    <cfRule type="expression" dxfId="194" priority="342">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="193" priority="340">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="192" priority="339">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H28 J28:K28">
-    <cfRule type="expression" dxfId="191" priority="420">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="190" priority="336">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29 J29:K29">
-    <cfRule type="expression" dxfId="189" priority="415">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="188" priority="334">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H30 J30:K30">
-    <cfRule type="expression" dxfId="187" priority="410">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H31 J31:K31">
-    <cfRule type="expression" dxfId="186" priority="405">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="185" priority="328">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="184" priority="327">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H32 J32:K32">
-    <cfRule type="expression" dxfId="183" priority="400">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="182" priority="324">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H69 J69">
-    <cfRule type="expression" dxfId="181" priority="322">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="180" priority="388">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="179" priority="320">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="178" priority="385">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="177" priority="382">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H70 J70">
-    <cfRule type="expression" dxfId="176" priority="318">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="175" priority="379">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39:B40 J39:V39 E39:H39 E40:G40 L40:V40">
-    <cfRule type="expression" dxfId="174" priority="376">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J41:V41 B41:B43 E43 E41:H41 G43 E42:G42 L42:V43">
-    <cfRule type="expression" dxfId="173" priority="372">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="172" priority="316">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="171" priority="315">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49:G49 B49">
-    <cfRule type="expression" dxfId="170" priority="365">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I81">
-    <cfRule type="expression" dxfId="169" priority="222">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="168" priority="361">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H53 J53">
-    <cfRule type="expression" dxfId="167" priority="360">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="166" priority="308">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="165" priority="311">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H72 J72">
-    <cfRule type="expression" dxfId="164" priority="314">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H62 J62">
-    <cfRule type="expression" dxfId="163" priority="350">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="162" priority="347">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="161" priority="344">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H66 J66">
-    <cfRule type="expression" dxfId="160" priority="338">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="159" priority="335">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H68 J68">
-    <cfRule type="expression" dxfId="158" priority="326">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="157" priority="323">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="156" priority="312">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H73 J73">
-    <cfRule type="expression" dxfId="155" priority="310">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="154" priority="307">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H74 J74">
-    <cfRule type="expression" dxfId="153" priority="306">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="152" priority="304">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="151" priority="303">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H71 J71">
-    <cfRule type="expression" dxfId="150" priority="302">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G81">
-    <cfRule type="expression" dxfId="149" priority="297">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J81:V81">
-    <cfRule type="expression" dxfId="148" priority="292">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B81 E81:F81">
-    <cfRule type="expression" dxfId="147" priority="294">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="146" priority="293">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H81">
-    <cfRule type="expression" dxfId="145" priority="291">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H78">
-    <cfRule type="expression" dxfId="144" priority="288">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H79">
-    <cfRule type="expression" dxfId="143" priority="286">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G84">
-    <cfRule type="expression" dxfId="142" priority="283">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="141" priority="140">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J84:V84">
-    <cfRule type="expression" dxfId="140" priority="278">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B84 E84:F84">
-    <cfRule type="expression" dxfId="139" priority="280">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K84:V84">
-    <cfRule type="expression" dxfId="138" priority="279">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H84">
-    <cfRule type="expression" dxfId="137" priority="277">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H82">
-    <cfRule type="expression" dxfId="136" priority="275">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G85">
-    <cfRule type="expression" dxfId="135" priority="273">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="134" priority="130">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J85:V85">
-    <cfRule type="expression" dxfId="133" priority="268">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B85 E85:F85">
-    <cfRule type="expression" dxfId="132" priority="270">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K85:V85">
-    <cfRule type="expression" dxfId="131" priority="269">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H85">
-    <cfRule type="expression" dxfId="130" priority="267">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J86">
-    <cfRule type="expression" dxfId="129" priority="265">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H86">
-    <cfRule type="expression" dxfId="128" priority="264">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G87">
-    <cfRule type="expression" dxfId="127" priority="262">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="126" priority="119">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J87:V87">
-    <cfRule type="expression" dxfId="125" priority="257">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B87 E87:F87">
-    <cfRule type="expression" dxfId="124" priority="259">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K87:V87">
-    <cfRule type="expression" dxfId="123" priority="258">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H87">
-    <cfRule type="expression" dxfId="122" priority="256">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K43">
-    <cfRule type="expression" dxfId="121" priority="254">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H43 J43">
-    <cfRule type="expression" dxfId="120" priority="252">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J38:K38">
-    <cfRule type="expression" dxfId="119" priority="249">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="118" priority="247">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I49">
-    <cfRule type="expression" dxfId="117" priority="105">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I53">
-    <cfRule type="expression" dxfId="116" priority="243">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I67">
-    <cfRule type="expression" dxfId="115" priority="236">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I62">
-    <cfRule type="expression" dxfId="114" priority="240">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="113" priority="239">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I64">
-    <cfRule type="expression" dxfId="112" priority="238">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I66">
-    <cfRule type="expression" dxfId="111" priority="237">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I68">
-    <cfRule type="expression" dxfId="110" priority="234">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="109" priority="233">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="108" priority="232">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I71">
-    <cfRule type="expression" dxfId="107" priority="231">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I72">
-    <cfRule type="expression" dxfId="106" priority="230">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I73">
-    <cfRule type="expression" dxfId="105" priority="229">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I74">
-    <cfRule type="expression" dxfId="104" priority="228">
+    <cfRule type="expression" dxfId="36" priority="59">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I75">
-    <cfRule type="expression" dxfId="103" priority="227">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I77">
-    <cfRule type="expression" dxfId="102" priority="225">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I78">
-    <cfRule type="expression" dxfId="101" priority="224">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I79">
-    <cfRule type="expression" dxfId="100" priority="223">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I82">
-    <cfRule type="expression" dxfId="99" priority="221">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I84">
-    <cfRule type="expression" dxfId="98" priority="220">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I85">
-    <cfRule type="expression" dxfId="97" priority="219">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I86">
-    <cfRule type="expression" dxfId="96" priority="218">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I87">
-    <cfRule type="expression" dxfId="95" priority="217">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I88">
-    <cfRule type="expression" dxfId="94" priority="216">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H88">
-    <cfRule type="expression" dxfId="93" priority="215">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="92" priority="214">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="91" priority="213">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="expression" dxfId="90" priority="212">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="89" priority="211">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="88" priority="210">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="87" priority="209">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="86" priority="208">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="85" priority="207">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="84" priority="139">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="expression" dxfId="83" priority="138">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="expression" dxfId="82" priority="137">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="81" priority="136">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="80" priority="135">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="79" priority="129">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
-    <cfRule type="expression" dxfId="78" priority="133">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="expression" dxfId="77" priority="132">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="76" priority="131">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="expression" dxfId="75" priority="128">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
-    <cfRule type="expression" dxfId="74" priority="127">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
-    <cfRule type="expression" dxfId="73" priority="126">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="72" priority="125">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="71" priority="124">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="expression" dxfId="70" priority="123">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="expression" dxfId="69" priority="122">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="68" priority="121">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="67" priority="118">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I50">
-    <cfRule type="expression" dxfId="66" priority="104">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="expression" dxfId="65" priority="116">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
-    <cfRule type="expression" dxfId="64" priority="115">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="expression" dxfId="63" priority="114">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="62" priority="113">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="expression" dxfId="61" priority="112">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
-    <cfRule type="expression" dxfId="60" priority="111">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="59" priority="110">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="58" priority="108">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="57" priority="106">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L9:V10">
-    <cfRule type="expression" dxfId="56" priority="96">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="55" priority="85">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H83">
-    <cfRule type="expression" dxfId="54" priority="94">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I83">
-    <cfRule type="expression" dxfId="53" priority="93">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:K9">
-    <cfRule type="expression" dxfId="52" priority="84">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="51" priority="83">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="50" priority="86">
-      <formula>K$1=$H9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="49" priority="87">
-      <formula>K$1=$I9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="48" priority="81">
-      <formula>K$1=$H10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="47" priority="82">
-      <formula>K$1=$I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="46" priority="80">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
-    <cfRule type="expression" dxfId="45" priority="79">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="44" priority="78">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="43" priority="71">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J42:K42 H42">
-    <cfRule type="expression" dxfId="42" priority="66">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="41" priority="65">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="40" priority="56">
-      <formula>K$1=$H18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="39" priority="57">
-      <formula>K$1=$I18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18 J18:K18">
-    <cfRule type="expression" dxfId="38" priority="58">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="37" priority="55">
+    <cfRule type="expression" dxfId="35" priority="58">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40:K40 H40">
+    <cfRule type="expression" dxfId="34" priority="56">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="expression" dxfId="33" priority="55">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J80">
+    <cfRule type="expression" dxfId="32" priority="46">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H80">
+    <cfRule type="expression" dxfId="31" priority="45">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I80">
+    <cfRule type="expression" dxfId="30" priority="44">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K80:V80">
+    <cfRule type="expression" dxfId="29" priority="43">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K80:V80">
+    <cfRule type="expression" dxfId="28" priority="41">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47 G47">
+    <cfRule type="expression" dxfId="27" priority="39">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47:F47">
+    <cfRule type="expression" dxfId="26" priority="38">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47 E47 G47">
+    <cfRule type="expression" dxfId="25" priority="37">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47 E47 G47">
+    <cfRule type="expression" dxfId="24" priority="36">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47">
+    <cfRule type="expression" dxfId="23" priority="35">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J47:V47 H47">
+    <cfRule type="expression" dxfId="22" priority="34">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I47">
+    <cfRule type="expression" dxfId="21" priority="32">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21 E21:G21">
+    <cfRule type="expression" dxfId="20" priority="31">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46:F46">
+    <cfRule type="expression" dxfId="19" priority="27">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J46:V46 H46">
+    <cfRule type="expression" dxfId="18" priority="26">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I46">
+    <cfRule type="expression" dxfId="17" priority="24">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:V21">
+    <cfRule type="expression" dxfId="16" priority="21">
+      <formula>K$1=$H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="expression" dxfId="15" priority="22">
+      <formula>K$1=$I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L21:V21">
+    <cfRule type="expression" dxfId="14" priority="23">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21 J21:K21">
+    <cfRule type="expression" dxfId="13" priority="20">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="expression" dxfId="12" priority="19">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F59">
+    <cfRule type="expression" dxfId="11" priority="18">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K45:V45">
+    <cfRule type="expression" dxfId="10" priority="16">
+      <formula>K$1=$H45</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J45:V45 H45">
+    <cfRule type="expression" dxfId="9" priority="17">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I45">
+    <cfRule type="expression" dxfId="8" priority="15">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G76">
+    <cfRule type="expression" dxfId="7" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K76">
-    <cfRule type="expression" dxfId="36" priority="53">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76:K76">
-    <cfRule type="expression" dxfId="35" priority="52">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H76">
-    <cfRule type="expression" dxfId="34" priority="51">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76">
-    <cfRule type="expression" dxfId="33" priority="50">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J40:K40 H40">
-    <cfRule type="expression" dxfId="32" priority="48">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="31" priority="47">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J80">
-    <cfRule type="expression" dxfId="30" priority="38">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H80">
-    <cfRule type="expression" dxfId="29" priority="37">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I80">
-    <cfRule type="expression" dxfId="28" priority="36">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K80:V80">
-    <cfRule type="expression" dxfId="27" priority="35">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K80:V80">
-    <cfRule type="expression" dxfId="26" priority="33">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47 G47">
-    <cfRule type="expression" dxfId="25" priority="31">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47:F47">
-    <cfRule type="expression" dxfId="24" priority="30">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47 E47 G47">
-    <cfRule type="expression" dxfId="23" priority="29">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47 E47 G47">
-    <cfRule type="expression" dxfId="22" priority="28">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
-    <cfRule type="expression" dxfId="21" priority="27">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J47:V47 H47">
-    <cfRule type="expression" dxfId="20" priority="26">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="19" priority="24">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21 E21:G21">
-    <cfRule type="expression" dxfId="18" priority="23">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46:F46">
-    <cfRule type="expression" dxfId="17" priority="19">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J46:V46 H46">
-    <cfRule type="expression" dxfId="16" priority="18">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:V21">
-    <cfRule type="expression" dxfId="14" priority="13">
-      <formula>K$1=$H21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="expression" dxfId="13" priority="14">
-      <formula>K$1=$I21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L21:V21">
-    <cfRule type="expression" dxfId="12" priority="15">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21 J21:K21">
-    <cfRule type="expression" dxfId="11" priority="12">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="expression" dxfId="10" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F59">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K45:V45">
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>K$1=$H45</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J45:V45 H45">
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65:V65">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>K$1=$H65</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G65 L65:V65">
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H65 J65">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L76:V76">
+    <cfRule type="expression" dxfId="2" priority="8">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L76:V76">
+    <cfRule type="expression" dxfId="1" priority="6">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L76:V76">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add TeslasInstrument to payout schedule
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2419F480-363A-D140-97FA-2DDA94547316}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6131E1-7781-B240-B29E-4141B93DE93E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19460" yWindow="5940" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="247">
   <si>
     <t>Name</t>
   </si>
@@ -775,6 +775,12 @@
   </si>
   <si>
     <t>https://swgoh.gg/p/557591483/</t>
+  </si>
+  <si>
+    <t>TeslasInstrument</t>
+  </si>
+  <si>
+    <t>https://swgoh.gg/p/864436423/</t>
   </si>
 </sst>
 </file>
@@ -3473,10 +3479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V88"/>
+  <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B65" sqref="A65:XFD65"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3558,19 +3564,19 @@
         <v>GMT</v>
       </c>
       <c r="S1" s="3" t="str">
-        <f>H83</f>
+        <f>H84</f>
         <v>AKST</v>
       </c>
       <c r="T1" s="3" t="str">
-        <f>H73</f>
+        <f>H74</f>
         <v>CST</v>
       </c>
       <c r="U1" s="3" t="str">
-        <f>H64</f>
+        <f>H65</f>
         <v>CST</v>
       </c>
       <c r="V1" s="3" t="str">
-        <f>H69</f>
+        <f>H70</f>
         <v>CST</v>
       </c>
     </row>
@@ -7965,20 +7971,22 @@
     <row r="59" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="55"/>
       <c r="B59" s="18" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C59" s="7">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="D59" s="7">
-        <v>58</v>
-      </c>
-      <c r="E59" s="53"/>
-      <c r="F59" s="19" t="s">
-        <v>45</v>
+        <v>99</v>
+      </c>
+      <c r="E59" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="F59" s="53" t="s">
+        <v>20</v>
       </c>
       <c r="G59" s="29" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="H59" s="29" t="s">
         <v>220</v>
@@ -8041,22 +8049,20 @@
     <row r="60" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="55"/>
       <c r="B60" s="18" t="s">
-        <v>44</v>
+        <v>241</v>
       </c>
       <c r="C60" s="7">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D60" s="7">
-        <v>59</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>27</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E60" s="53"/>
       <c r="F60" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G60" s="21" t="s">
-        <v>158</v>
+      <c r="G60" s="29" t="s">
+        <v>242</v>
       </c>
       <c r="H60" s="29" t="s">
         <v>220</v>
@@ -8119,97 +8125,97 @@
     <row r="61" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="55"/>
       <c r="B61" s="18" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="C61" s="7">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D61" s="7">
-        <v>60</v>
-      </c>
-      <c r="E61" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="F61" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="G61" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="G61" s="21" t="s">
+        <v>158</v>
+      </c>
       <c r="H61" s="29" t="s">
-        <v>9</v>
+        <v>220</v>
       </c>
       <c r="I61" s="23">
-        <v>0</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="J61" s="26" t="s">
         <v>14</v>
       </c>
       <c r="K61" s="25">
         <f>$I61+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
+        <v>1.375</v>
       </c>
       <c r="L61" s="23">
         <f>$I61+Sheet2!B$2/24</f>
-        <v>0.375</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="M61" s="23">
         <f>$I61+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="N61" s="23">
         <f>$I61+Sheet2!B$4/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="O61" s="23">
         <f>$I61+Sheet2!B$5/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="P61" s="23">
         <f>$I61+Sheet2!B$6/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="Q61" s="23">
         <f>$I61+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="R61" s="23">
         <f>$I61+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>1</v>
       </c>
       <c r="S61" s="23">
         <f>$I61+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="T61" s="23">
         <f>$I61+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="U61" s="23">
         <f>$I61+Sheet2!B$11/24</f>
-        <v>-0.25</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="V61" s="23">
         <f>$I61+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="62" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="55"/>
-      <c r="B62" s="35" t="s">
-        <v>94</v>
+      <c r="B62" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="C62" s="7">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D62" s="7">
-        <v>61</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>27</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E62" s="14"/>
       <c r="F62" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G62" s="29" t="s">
-        <v>159</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="G62" s="9"/>
       <c r="H62" s="29" t="s">
         <v>9</v>
       </c>
@@ -8271,13 +8277,13 @@
     <row r="63" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="55"/>
       <c r="B63" s="35" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="C63" s="7">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D63" s="7">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E63" s="14" t="s">
         <v>27</v>
@@ -8286,7 +8292,7 @@
         <v>20</v>
       </c>
       <c r="G63" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H63" s="29" t="s">
         <v>9</v>
@@ -8349,22 +8355,22 @@
     <row r="64" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="55"/>
       <c r="B64" s="35" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C64" s="7">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D64" s="7">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E64" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F64" s="7" t="s">
-        <v>69</v>
+      <c r="F64" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="G64" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H64" s="29" t="s">
         <v>9</v>
@@ -8426,23 +8432,23 @@
     </row>
     <row r="65" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="55"/>
-      <c r="B65" s="18" t="s">
-        <v>88</v>
+      <c r="B65" s="35" t="s">
+        <v>57</v>
       </c>
       <c r="C65" s="7">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D65" s="7">
-        <v>65</v>
-      </c>
-      <c r="E65" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="E65" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F65" s="40" t="s">
-        <v>20</v>
+      <c r="F65" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="G65" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H65" s="29" t="s">
         <v>9</v>
@@ -8505,13 +8511,13 @@
     <row r="66" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="55"/>
       <c r="B66" s="18" t="s">
-        <v>180</v>
+        <v>88</v>
       </c>
       <c r="C66" s="7">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D66" s="7">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E66" s="39" t="s">
         <v>27</v>
@@ -8520,7 +8526,7 @@
         <v>20</v>
       </c>
       <c r="G66" s="29" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="H66" s="29" t="s">
         <v>9</v>
@@ -8582,23 +8588,23 @@
     </row>
     <row r="67" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="55"/>
-      <c r="B67" s="35" t="s">
-        <v>63</v>
+      <c r="B67" s="18" t="s">
+        <v>180</v>
       </c>
       <c r="C67" s="7">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D67" s="7">
-        <v>67</v>
-      </c>
-      <c r="E67" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E67" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="F67" s="19" t="s">
-        <v>45</v>
+      <c r="F67" s="40" t="s">
+        <v>20</v>
       </c>
       <c r="G67" s="29" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="H67" s="29" t="s">
         <v>9</v>
@@ -8661,22 +8667,22 @@
     <row r="68" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="55"/>
       <c r="B68" s="35" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C68" s="7">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D68" s="7">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E68" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G68" s="27" t="s">
-        <v>165</v>
+        <v>45</v>
+      </c>
+      <c r="G68" s="29" t="s">
+        <v>164</v>
       </c>
       <c r="H68" s="29" t="s">
         <v>9</v>
@@ -8738,23 +8744,23 @@
     </row>
     <row r="69" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="55"/>
-      <c r="B69" s="18" t="s">
-        <v>58</v>
+      <c r="B69" s="35" t="s">
+        <v>61</v>
       </c>
       <c r="C69" s="7">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D69" s="7">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E69" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F69" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G69" s="29" t="s">
-        <v>166</v>
+      <c r="F69" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G69" s="27" t="s">
+        <v>165</v>
       </c>
       <c r="H69" s="29" t="s">
         <v>9</v>
@@ -8816,23 +8822,23 @@
     </row>
     <row r="70" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="55"/>
-      <c r="B70" s="12" t="s">
-        <v>90</v>
+      <c r="B70" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="C70" s="7">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D70" s="7">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E70" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F70" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G70" s="22" t="s">
-        <v>124</v>
+      <c r="F70" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G70" s="29" t="s">
+        <v>166</v>
       </c>
       <c r="H70" s="29" t="s">
         <v>9</v>
@@ -8847,61 +8853,61 @@
         <f>$I70+Sheet2!B$1/24</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="L70" s="16">
+      <c r="L70" s="23">
         <f>$I70+Sheet2!B$2/24</f>
         <v>0.375</v>
       </c>
-      <c r="M70" s="16">
+      <c r="M70" s="23">
         <f>$I70+Sheet2!B$3/24</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N70" s="16">
+      <c r="N70" s="23">
         <f>$I70+Sheet2!B$4/24</f>
         <v>0.125</v>
       </c>
-      <c r="O70" s="16">
+      <c r="O70" s="23">
         <f>$I70+Sheet2!B$5/24</f>
         <v>0.125</v>
       </c>
-      <c r="P70" s="16">
+      <c r="P70" s="23">
         <f>$I70+Sheet2!B$6/24</f>
         <v>0.125</v>
       </c>
-      <c r="Q70" s="16">
+      <c r="Q70" s="23">
         <f>$I70+Sheet2!B$7/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="R70" s="16">
+      <c r="R70" s="23">
         <f>$I70+Sheet2!B$8/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="S70" s="16">
+      <c r="S70" s="23">
         <f>$I70+Sheet2!B$9/24</f>
         <v>-0.16666666666666666</v>
       </c>
-      <c r="T70" s="16">
+      <c r="T70" s="23">
         <f>$I70+Sheet2!B$10/24</f>
         <v>-0.20833333333333334</v>
       </c>
-      <c r="U70" s="16">
+      <c r="U70" s="23">
         <f>$I70+Sheet2!B$11/24</f>
         <v>-0.25</v>
       </c>
-      <c r="V70" s="16">
+      <c r="V70" s="23">
         <f>$I70+Sheet2!B$12/24</f>
         <v>-0.29166666666666669</v>
       </c>
     </row>
     <row r="71" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="55"/>
-      <c r="B71" s="18" t="s">
-        <v>56</v>
+      <c r="B71" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="C71" s="7">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D71" s="7">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E71" s="14" t="s">
         <v>27</v>
@@ -8909,8 +8915,8 @@
       <c r="F71" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G71" s="29" t="s">
-        <v>167</v>
+      <c r="G71" s="22" t="s">
+        <v>124</v>
       </c>
       <c r="H71" s="29" t="s">
         <v>9</v>
@@ -8925,70 +8931,70 @@
         <f>$I71+Sheet2!B$1/24</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="L71" s="23">
+      <c r="L71" s="16">
         <f>$I71+Sheet2!B$2/24</f>
         <v>0.375</v>
       </c>
-      <c r="M71" s="23">
+      <c r="M71" s="16">
         <f>$I71+Sheet2!B$3/24</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N71" s="23">
+      <c r="N71" s="16">
         <f>$I71+Sheet2!B$4/24</f>
         <v>0.125</v>
       </c>
-      <c r="O71" s="23">
+      <c r="O71" s="16">
         <f>$I71+Sheet2!B$5/24</f>
         <v>0.125</v>
       </c>
-      <c r="P71" s="23">
+      <c r="P71" s="16">
         <f>$I71+Sheet2!B$6/24</f>
         <v>0.125</v>
       </c>
-      <c r="Q71" s="23">
+      <c r="Q71" s="16">
         <f>$I71+Sheet2!B$7/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="R71" s="23">
+      <c r="R71" s="16">
         <f>$I71+Sheet2!B$8/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="S71" s="23">
+      <c r="S71" s="16">
         <f>$I71+Sheet2!B$9/24</f>
         <v>-0.16666666666666666</v>
       </c>
-      <c r="T71" s="23">
+      <c r="T71" s="16">
         <f>$I71+Sheet2!B$10/24</f>
         <v>-0.20833333333333334</v>
       </c>
-      <c r="U71" s="23">
+      <c r="U71" s="16">
         <f>$I71+Sheet2!B$11/24</f>
         <v>-0.25</v>
       </c>
-      <c r="V71" s="23">
+      <c r="V71" s="16">
         <f>$I71+Sheet2!B$12/24</f>
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="72" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="55"/>
       <c r="B72" s="18" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C72" s="7">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D72" s="7">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F72" s="7" t="s">
-        <v>69</v>
+      <c r="F72" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="G72" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H72" s="29" t="s">
         <v>9</v>
@@ -9048,25 +9054,25 @@
         <v>-0.29166666666666669</v>
       </c>
     </row>
-    <row r="73" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="55"/>
       <c r="B73" s="18" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C73" s="7">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D73" s="7">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E73" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F73" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G73" s="27" t="s">
-        <v>169</v>
+      <c r="F73" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G73" s="29" t="s">
+        <v>168</v>
       </c>
       <c r="H73" s="29" t="s">
         <v>9</v>
@@ -9129,97 +9135,97 @@
     <row r="74" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="55"/>
       <c r="B74" s="18" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="C74" s="7">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D74" s="7">
-        <v>74</v>
-      </c>
-      <c r="E74" s="14"/>
+        <v>73</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="F74" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="G74" s="29"/>
+        <v>20</v>
+      </c>
+      <c r="G74" s="27" t="s">
+        <v>169</v>
+      </c>
       <c r="H74" s="29" t="s">
-        <v>221</v>
+        <v>9</v>
       </c>
       <c r="I74" s="23">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J74" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="J74" s="26" t="s">
         <v>14</v>
       </c>
       <c r="K74" s="25">
         <f>$I74+Sheet2!B$1/24</f>
-        <v>0.45833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L74" s="23">
         <f>$I74+Sheet2!B$2/24</f>
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="M74" s="23">
         <f>$I74+Sheet2!B$3/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N74" s="23">
         <f>$I74+Sheet2!B$4/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="O74" s="23">
         <f>$I74+Sheet2!B$5/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="P74" s="23">
         <f>$I74+Sheet2!B$6/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="Q74" s="23">
         <f>$I74+Sheet2!B$7/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="R74" s="23">
         <f>$I74+Sheet2!B$8/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="S74" s="23">
         <f>$I74+Sheet2!B$9/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="T74" s="23">
         <f>$I74+Sheet2!B$10/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="U74" s="23">
         <f>$I74+Sheet2!B$11/24</f>
-        <v>-0.20833333333333334</v>
+        <v>-0.25</v>
       </c>
       <c r="V74" s="23">
         <f>$I74+Sheet2!B$12/24</f>
-        <v>-0.25</v>
+        <v>-0.29166666666666669</v>
       </c>
     </row>
     <row r="75" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="55"/>
       <c r="B75" s="18" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="C75" s="7">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D75" s="7">
-        <v>75</v>
-      </c>
-      <c r="E75" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G75" s="34" t="s">
-        <v>146</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E75" s="14"/>
+      <c r="F75" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G75" s="29"/>
       <c r="H75" s="29" t="s">
         <v>221</v>
       </c>
@@ -9281,22 +9287,22 @@
     <row r="76" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="55"/>
       <c r="B76" s="18" t="s">
-        <v>243</v>
+        <v>54</v>
       </c>
       <c r="C76" s="7">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D76" s="7">
-        <v>64</v>
-      </c>
-      <c r="E76" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="F76" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="G76" s="29" t="s">
-        <v>244</v>
+        <v>75</v>
+      </c>
+      <c r="E76" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G76" s="34" t="s">
+        <v>146</v>
       </c>
       <c r="H76" s="29" t="s">
         <v>221</v>
@@ -9359,97 +9365,97 @@
     <row r="77" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="55"/>
       <c r="B77" s="18" t="s">
-        <v>117</v>
+        <v>243</v>
       </c>
       <c r="C77" s="7">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D77" s="7">
-        <v>76</v>
-      </c>
-      <c r="E77" s="14"/>
-      <c r="F77" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="G77" s="29"/>
+        <v>64</v>
+      </c>
+      <c r="E77" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F77" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G77" s="29" t="s">
+        <v>244</v>
+      </c>
       <c r="H77" s="29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I77" s="23">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="J77" s="28" t="s">
         <v>14</v>
       </c>
       <c r="K77" s="25">
         <f>$I77+Sheet2!B$1/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="L77" s="23">
         <f>$I77+Sheet2!B$2/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M77" s="23">
         <f>$I77+Sheet2!B$3/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="N77" s="23">
         <f>$I77+Sheet2!B$4/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="O77" s="23">
         <f>$I77+Sheet2!B$5/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P77" s="23">
         <f>$I77+Sheet2!B$6/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="Q77" s="23">
         <f>$I77+Sheet2!B$7/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="R77" s="23">
         <f>$I77+Sheet2!B$8/24</f>
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="S77" s="23">
         <f>$I77+Sheet2!B$9/24</f>
-        <v>-8.3333333333333329E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="T77" s="23">
         <f>$I77+Sheet2!B$10/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="U77" s="23">
         <f>$I77+Sheet2!B$11/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333334</v>
       </c>
       <c r="V77" s="23">
         <f>$I77+Sheet2!B$12/24</f>
-        <v>-0.20833333333333337</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="78" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="55"/>
       <c r="B78" s="18" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="C78" s="7">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D78" s="7">
-        <v>77</v>
-      </c>
-      <c r="E78" s="14" t="s">
-        <v>27</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E78" s="14"/>
       <c r="F78" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G78" s="21" t="s">
-        <v>171</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="G78" s="29"/>
       <c r="H78" s="29" t="s">
         <v>223</v>
       </c>
@@ -9510,23 +9516,23 @@
     </row>
     <row r="79" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="55"/>
-      <c r="B79" s="35" t="s">
-        <v>66</v>
+      <c r="B79" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="C79" s="7">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D79" s="7">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E79" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F79" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G79" s="9" t="s">
-        <v>172</v>
+      <c r="F79" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G79" s="21" t="s">
+        <v>171</v>
       </c>
       <c r="H79" s="29" t="s">
         <v>223</v>
@@ -9588,23 +9594,23 @@
     </row>
     <row r="80" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="55"/>
-      <c r="B80" s="18" t="s">
-        <v>233</v>
+      <c r="B80" s="35" t="s">
+        <v>66</v>
       </c>
       <c r="C80" s="7">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D80" s="7">
-        <v>79</v>
-      </c>
-      <c r="E80" s="33" t="s">
-        <v>72</v>
+        <v>78</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="G80" s="34" t="s">
-        <v>145</v>
+        <v>69</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>172</v>
       </c>
       <c r="H80" s="29" t="s">
         <v>223</v>
@@ -9667,97 +9673,97 @@
     <row r="81" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="55"/>
       <c r="B81" s="18" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="C81" s="7">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D81" s="7">
-        <v>80</v>
-      </c>
-      <c r="E81" s="14"/>
-      <c r="F81" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G81" s="29"/>
+        <v>79</v>
+      </c>
+      <c r="E81" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="G81" s="34" t="s">
+        <v>145</v>
+      </c>
       <c r="H81" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I81" s="23">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="J81" s="28" t="s">
         <v>14</v>
       </c>
       <c r="K81" s="25">
         <f>$I81+Sheet2!B$1/24</f>
-        <v>0.54166666666666674</v>
+        <v>0.5</v>
       </c>
       <c r="L81" s="23">
         <f>$I81+Sheet2!B$2/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="M81" s="23">
         <f>$I81+Sheet2!B$3/24</f>
-        <v>0.45833333333333331</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="N81" s="23">
         <f>$I81+Sheet2!B$4/24</f>
-        <v>0.25</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="O81" s="23">
         <f>$I81+Sheet2!B$5/24</f>
-        <v>0.25</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="P81" s="23">
         <f>$I81+Sheet2!B$6/24</f>
-        <v>0.25</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="Q81" s="23">
         <f>$I81+Sheet2!B$7/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="R81" s="23">
         <f>$I81+Sheet2!B$8/24</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="S81" s="23">
         <f>$I81+Sheet2!B$9/24</f>
-        <v>-4.1666666666666657E-2</v>
+        <v>-8.3333333333333329E-2</v>
       </c>
       <c r="T81" s="23">
         <f>$I81+Sheet2!B$10/24</f>
-        <v>-8.3333333333333343E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="U81" s="23">
         <f>$I81+Sheet2!B$11/24</f>
-        <v>-0.125</v>
+        <v>-0.16666666666666669</v>
       </c>
       <c r="V81" s="23">
         <f>$I81+Sheet2!B$12/24</f>
-        <v>-0.16666666666666669</v>
+        <v>-0.20833333333333337</v>
       </c>
     </row>
     <row r="82" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="55"/>
       <c r="B82" s="18" t="s">
-        <v>65</v>
+        <v>222</v>
       </c>
       <c r="C82" s="7">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D82" s="7">
-        <v>81</v>
-      </c>
-      <c r="E82" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F82" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G82" s="37" t="s">
-        <v>173</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E82" s="14"/>
+      <c r="F82" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="G82" s="29"/>
       <c r="H82" s="29" t="s">
         <v>224</v>
       </c>
@@ -9819,22 +9825,22 @@
     <row r="83" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="55"/>
       <c r="B83" s="18" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="C83" s="7">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D83" s="7">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E83" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F83" s="19" t="s">
+      <c r="F83" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G83" s="9" t="s">
-        <v>156</v>
+      <c r="G83" s="37" t="s">
+        <v>173</v>
       </c>
       <c r="H83" s="29" t="s">
         <v>224</v>
@@ -9842,7 +9848,7 @@
       <c r="I83" s="23">
         <v>0.125</v>
       </c>
-      <c r="J83" s="26" t="s">
+      <c r="J83" s="28" t="s">
         <v>14</v>
       </c>
       <c r="K83" s="25">
@@ -9897,171 +9903,171 @@
     <row r="84" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="55"/>
       <c r="B84" s="18" t="s">
-        <v>225</v>
+        <v>29</v>
       </c>
       <c r="C84" s="7">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D84" s="7">
-        <v>83</v>
-      </c>
-      <c r="E84" s="14"/>
+        <v>82</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="F84" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="G84" s="29"/>
+        <v>20</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>156</v>
+      </c>
       <c r="H84" s="29" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I84" s="23">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="J84" s="28" t="s">
+        <v>0.125</v>
+      </c>
+      <c r="J84" s="26" t="s">
         <v>14</v>
       </c>
       <c r="K84" s="25">
         <f>$I84+Sheet2!B$1/24</f>
-        <v>0.58333333333333337</v>
+        <v>0.54166666666666674</v>
       </c>
       <c r="L84" s="23">
         <f>$I84+Sheet2!B$2/24</f>
-        <v>0.54166666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="M84" s="23">
         <f>$I84+Sheet2!B$3/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="N84" s="23">
         <f>$I84+Sheet2!B$4/24</f>
-        <v>0.29166666666666663</v>
+        <v>0.25</v>
       </c>
       <c r="O84" s="23">
         <f>$I84+Sheet2!B$5/24</f>
-        <v>0.29166666666666663</v>
+        <v>0.25</v>
       </c>
       <c r="P84" s="23">
         <f>$I84+Sheet2!B$6/24</f>
-        <v>0.29166666666666663</v>
+        <v>0.25</v>
       </c>
       <c r="Q84" s="23">
         <f>$I84+Sheet2!B$7/24</f>
-        <v>0.25</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="R84" s="23">
         <f>$I84+Sheet2!B$8/24</f>
-        <v>0.20833333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="S84" s="23">
         <f>$I84+Sheet2!B$9/24</f>
-        <v>0</v>
+        <v>-4.1666666666666657E-2</v>
       </c>
       <c r="T84" s="23">
         <f>$I84+Sheet2!B$10/24</f>
-        <v>-4.1666666666666685E-2</v>
+        <v>-8.3333333333333343E-2</v>
       </c>
       <c r="U84" s="23">
         <f>$I84+Sheet2!B$11/24</f>
-        <v>-8.3333333333333343E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="V84" s="23">
         <f>$I84+Sheet2!B$12/24</f>
-        <v>-0.12500000000000003</v>
+        <v>-0.16666666666666669</v>
       </c>
     </row>
     <row r="85" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="55"/>
       <c r="B85" s="18" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C85" s="7">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D85" s="7">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E85" s="14"/>
       <c r="F85" s="19" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G85" s="29"/>
       <c r="H85" s="29" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="I85" s="23">
-        <v>0.20833333333333334</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="J85" s="28" t="s">
         <v>14</v>
       </c>
       <c r="K85" s="25">
         <f>$I85+Sheet2!B$1/24</f>
-        <v>0.625</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="L85" s="23">
         <f>$I85+Sheet2!B$2/24</f>
-        <v>0.58333333333333337</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="M85" s="23">
         <f>$I85+Sheet2!B$3/24</f>
-        <v>0.54166666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="N85" s="23">
         <f>$I85+Sheet2!B$4/24</f>
-        <v>0.33333333333333337</v>
+        <v>0.29166666666666663</v>
       </c>
       <c r="O85" s="23">
         <f>$I85+Sheet2!B$5/24</f>
-        <v>0.33333333333333337</v>
+        <v>0.29166666666666663</v>
       </c>
       <c r="P85" s="23">
         <f>$I85+Sheet2!B$6/24</f>
-        <v>0.33333333333333337</v>
+        <v>0.29166666666666663</v>
       </c>
       <c r="Q85" s="23">
         <f>$I85+Sheet2!B$7/24</f>
-        <v>0.29166666666666669</v>
+        <v>0.25</v>
       </c>
       <c r="R85" s="23">
         <f>$I85+Sheet2!B$8/24</f>
-        <v>0.25</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="S85" s="23">
         <f>$I85+Sheet2!B$9/24</f>
-        <v>4.1666666666666685E-2</v>
+        <v>0</v>
       </c>
       <c r="T85" s="23">
         <f>$I85+Sheet2!B$10/24</f>
-        <v>0</v>
+        <v>-4.1666666666666685E-2</v>
       </c>
       <c r="U85" s="23">
         <f>$I85+Sheet2!B$11/24</f>
-        <v>-4.1666666666666657E-2</v>
+        <v>-8.3333333333333343E-2</v>
       </c>
       <c r="V85" s="23">
         <f>$I85+Sheet2!B$12/24</f>
-        <v>-8.3333333333333343E-2</v>
+        <v>-0.12500000000000003</v>
       </c>
     </row>
     <row r="86" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="55"/>
-      <c r="B86" s="35" t="s">
-        <v>64</v>
+      <c r="B86" s="18" t="s">
+        <v>228</v>
       </c>
       <c r="C86" s="7">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D86" s="7">
-        <v>85</v>
-      </c>
-      <c r="E86" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F86" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G86" s="34" t="s">
-        <v>170</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E86" s="14"/>
+      <c r="F86" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="G86" s="29"/>
       <c r="H86" s="29" t="s">
         <v>230</v>
       </c>
@@ -10122,97 +10128,98 @@
     </row>
     <row r="87" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="55"/>
-      <c r="B87" s="18" t="s">
-        <v>231</v>
+      <c r="B87" s="35" t="s">
+        <v>64</v>
       </c>
       <c r="C87" s="7">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D87" s="7">
-        <v>86</v>
-      </c>
-      <c r="E87" s="14"/>
-      <c r="F87" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="G87" s="29"/>
+        <v>85</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F87" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G87" s="34" t="s">
+        <v>170</v>
+      </c>
       <c r="H87" s="29" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I87" s="23">
-        <v>0.25</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="J87" s="28" t="s">
         <v>14</v>
       </c>
       <c r="K87" s="25">
         <f>$I87+Sheet2!B$1/24</f>
-        <v>0.66666666666666674</v>
+        <v>0.625</v>
       </c>
       <c r="L87" s="23">
         <f>$I87+Sheet2!B$2/24</f>
-        <v>0.625</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="M87" s="23">
         <f>$I87+Sheet2!B$3/24</f>
-        <v>0.58333333333333326</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="N87" s="23">
         <f>$I87+Sheet2!B$4/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="O87" s="23">
         <f>$I87+Sheet2!B$5/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="P87" s="23">
         <f>$I87+Sheet2!B$6/24</f>
-        <v>0.375</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="Q87" s="23">
         <f>$I87+Sheet2!B$7/24</f>
-        <v>0.33333333333333331</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="R87" s="23">
         <f>$I87+Sheet2!B$8/24</f>
-        <v>0.29166666666666669</v>
+        <v>0.25</v>
       </c>
       <c r="S87" s="23">
         <f>$I87+Sheet2!B$9/24</f>
-        <v>8.3333333333333343E-2</v>
+        <v>4.1666666666666685E-2</v>
       </c>
       <c r="T87" s="23">
         <f>$I87+Sheet2!B$10/24</f>
-        <v>4.1666666666666657E-2</v>
+        <v>0</v>
       </c>
       <c r="U87" s="23">
         <f>$I87+Sheet2!B$11/24</f>
-        <v>0</v>
+        <v>-4.1666666666666657E-2</v>
       </c>
       <c r="V87" s="23">
         <f>$I87+Sheet2!B$12/24</f>
-        <v>-4.1666666666666685E-2</v>
+        <v>-8.3333333333333343E-2</v>
       </c>
     </row>
     <row r="88" spans="1:22" ht="17" x14ac:dyDescent="0.2">
-      <c r="B88" s="35" t="s">
-        <v>68</v>
+      <c r="A88" s="55"/>
+      <c r="B88" s="18" t="s">
+        <v>231</v>
       </c>
       <c r="C88" s="7">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D88" s="7">
-        <v>87</v>
-      </c>
-      <c r="E88" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F88" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="G88" s="22" t="s">
-        <v>174</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E88" s="14"/>
+      <c r="F88" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="G88" s="29"/>
       <c r="H88" s="29" t="s">
         <v>232</v>
       </c>
@@ -10271,24 +10278,101 @@
         <v>-4.1666666666666685E-2</v>
       </c>
     </row>
+    <row r="89" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="B89" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C89" s="7">
+        <v>87</v>
+      </c>
+      <c r="D89" s="7">
+        <v>87</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F89" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G89" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="H89" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="I89" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="J89" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K89" s="25">
+        <f>$I89+Sheet2!B$1/24</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="L89" s="23">
+        <f>$I89+Sheet2!B$2/24</f>
+        <v>0.625</v>
+      </c>
+      <c r="M89" s="23">
+        <f>$I89+Sheet2!B$3/24</f>
+        <v>0.58333333333333326</v>
+      </c>
+      <c r="N89" s="23">
+        <f>$I89+Sheet2!B$4/24</f>
+        <v>0.375</v>
+      </c>
+      <c r="O89" s="23">
+        <f>$I89+Sheet2!B$5/24</f>
+        <v>0.375</v>
+      </c>
+      <c r="P89" s="23">
+        <f>$I89+Sheet2!B$6/24</f>
+        <v>0.375</v>
+      </c>
+      <c r="Q89" s="23">
+        <f>$I89+Sheet2!B$7/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="R89" s="23">
+        <f>$I89+Sheet2!B$8/24</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="S89" s="23">
+        <f>$I89+Sheet2!B$9/24</f>
+        <v>8.3333333333333343E-2</v>
+      </c>
+      <c r="T89" s="23">
+        <f>$I89+Sheet2!B$10/24</f>
+        <v>4.1666666666666657E-2</v>
+      </c>
+      <c r="U89" s="23">
+        <f>$I89+Sheet2!B$11/24</f>
+        <v>0</v>
+      </c>
+      <c r="V89" s="23">
+        <f>$I89+Sheet2!B$12/24</f>
+        <v>-4.1666666666666685E-2</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:V71">
-    <sortCondition ref="D2:D71"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:V72">
+    <sortCondition ref="D2:D72"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
+      <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
-      <selection sqref="A1:XFD1048576"/>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
     <mergeCell ref="A25:A50"/>
-    <mergeCell ref="A51:A87"/>
+    <mergeCell ref="A51:A88"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V44 K46:V88">
+  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V44 K46:V89">
     <cfRule type="expression" dxfId="275" priority="658">
       <formula>K$1=$H2</formula>
     </cfRule>
@@ -10298,12 +10382,12 @@
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K53:V53 G53 G63 G72 G88 E61:G61 G30 B73 E73:G73 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 B69:B71 E69:G71 L40:V40 K86:V86 G86 K78:V79 K82:V83 K88:V88 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B83 J11:V14 J83:V83 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L75:V75 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E83:G83 E60:V60 E64:G64 B50:B61 B40 B44:B46 B80 B48 J48:V48 G74:G79 E24:G29 B20:B38 E5:G5 E48:H48 E80:G80 E75:G76 L24:V32 L20:V20 L22:V22 G58:V59 G65:G68 E44:H44 E45:G46 L63:V73 B64:B66 B75:B76 C4:D88">
+  <conditionalFormatting sqref="K53:V53 G53 G64 G73 G89 E62:G62 G30 B74 E74:G74 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 B70:B72 E70:G72 L40:V40 K87:V87 G87 K79:V80 K83:V84 K89:V89 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B84 J11:V14 J84:V84 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L76:V76 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E84:G84 E61:V61 E65:G65 B50:B62 B40 B44:B46 B81 B48 J48:V48 G75:G80 E24:G29 B20:B38 E5:G5 E48:H48 E81:G81 E76:G77 L24:V32 L20:V20 L22:V22 G66:G69 E44:H44 E45:G46 L64:V74 B65:B67 B76:B77 C4:D89 G58:V60">
     <cfRule type="expression" dxfId="273" priority="664">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B63 L63:V63">
+  <conditionalFormatting sqref="B64 L64:V64">
     <cfRule type="expression" dxfId="272" priority="641">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10313,87 +10397,87 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B69 L69:V69">
+    <cfRule type="expression" dxfId="270" priority="637">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B73 L73:V73">
+    <cfRule type="expression" dxfId="269" priority="635">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B68 L68:V68">
-    <cfRule type="expression" dxfId="270" priority="637">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B72 L72:V72">
-    <cfRule type="expression" dxfId="269" priority="635">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B67 L67:V67">
     <cfRule type="expression" dxfId="268" priority="633">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B86 K86:V86 E86:F86">
+  <conditionalFormatting sqref="B87 K87:V87 E87:F87">
     <cfRule type="expression" dxfId="267" priority="629">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
+    <cfRule type="expression" dxfId="266" priority="627">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E73">
+    <cfRule type="expression" dxfId="265" priority="624">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68">
+    <cfRule type="expression" dxfId="264" priority="623">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B84 J83:V84">
+    <cfRule type="expression" dxfId="263" priority="620">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B80:B81 J80:V80 E80:E81">
+    <cfRule type="expression" dxfId="262" priority="618">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E83:F84">
+    <cfRule type="expression" dxfId="261" priority="616">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B79 J79:V79">
+    <cfRule type="expression" dxfId="260" priority="614">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B89 J89:V89 E89">
+    <cfRule type="expression" dxfId="259" priority="612">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F68">
+    <cfRule type="expression" dxfId="258" priority="604">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62:V62">
+    <cfRule type="expression" dxfId="257" priority="544">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F73">
+    <cfRule type="expression" dxfId="256" priority="566">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B75:B77 E75:F77">
+    <cfRule type="expression" dxfId="255" priority="530">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="266" priority="627">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E72">
-    <cfRule type="expression" dxfId="265" priority="624">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E67">
-    <cfRule type="expression" dxfId="264" priority="623">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B82:B83 J82:V83">
-    <cfRule type="expression" dxfId="263" priority="620">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B79:B80 J79:V79 E79:E80">
-    <cfRule type="expression" dxfId="262" priority="618">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E82:F83">
-    <cfRule type="expression" dxfId="261" priority="616">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B78 J78:V78">
-    <cfRule type="expression" dxfId="260" priority="614">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B88 J88:V88 E88">
-    <cfRule type="expression" dxfId="259" priority="612">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F67">
-    <cfRule type="expression" dxfId="258" priority="604">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K61:V61">
-    <cfRule type="expression" dxfId="257" priority="544">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F72">
-    <cfRule type="expression" dxfId="256" priority="566">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B74:B76 E74:F76">
-    <cfRule type="expression" dxfId="255" priority="530">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E62">
     <cfRule type="expression" dxfId="254" priority="551">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10403,32 +10487,32 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B62 L62:V62">
+  <conditionalFormatting sqref="B63 L63:V63">
     <cfRule type="expression" dxfId="252" priority="552">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F79:F80">
+  <conditionalFormatting sqref="F80:F81">
     <cfRule type="expression" dxfId="251" priority="564">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F63">
+  <conditionalFormatting sqref="F64">
     <cfRule type="expression" dxfId="250" priority="560">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E68:F68">
+  <conditionalFormatting sqref="E69:F69">
     <cfRule type="expression" dxfId="249" priority="559">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E78:F78">
+  <conditionalFormatting sqref="E79:F79">
     <cfRule type="expression" dxfId="248" priority="557">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L62:V62 G62">
+  <conditionalFormatting sqref="L63:V63 G63">
     <cfRule type="expression" dxfId="247" priority="554">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10438,7 +10522,7 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F62">
+  <conditionalFormatting sqref="F63">
     <cfRule type="expression" dxfId="245" priority="548">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10448,7 +10532,7 @@
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K61:V61">
+  <conditionalFormatting sqref="K62:V62">
     <cfRule type="expression" dxfId="243" priority="545">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10473,37 +10557,37 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K74:V74 L75:V75">
+  <conditionalFormatting sqref="K75:V75 L76:V76">
     <cfRule type="expression" dxfId="238" priority="529">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J74:V74 L75:V75">
+  <conditionalFormatting sqref="J75:V75 L76:V76">
     <cfRule type="expression" dxfId="237" priority="527">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H74">
+  <conditionalFormatting sqref="H75">
     <cfRule type="expression" dxfId="236" priority="526">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J77:V77">
+  <conditionalFormatting sqref="J78:V78">
     <cfRule type="expression" dxfId="235" priority="521">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B77 E77:F77">
+  <conditionalFormatting sqref="B78 E78:F78">
     <cfRule type="expression" dxfId="234" priority="524">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K77:V77">
+  <conditionalFormatting sqref="K78:V78">
     <cfRule type="expression" dxfId="233" priority="523">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H77">
+  <conditionalFormatting sqref="H78">
     <cfRule type="expression" dxfId="232" priority="520">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10618,7 +10702,7 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
+  <conditionalFormatting sqref="K70">
     <cfRule type="expression" dxfId="209" priority="327">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10628,7 +10712,7 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H61:J61">
+  <conditionalFormatting sqref="H62:J62">
     <cfRule type="expression" dxfId="207" priority="365">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10643,12 +10727,12 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
+  <conditionalFormatting sqref="K63">
     <cfRule type="expression" dxfId="204" priority="360">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
+  <conditionalFormatting sqref="K63">
     <cfRule type="expression" dxfId="203" priority="359">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10658,7 +10742,7 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
+  <conditionalFormatting sqref="K64">
     <cfRule type="expression" dxfId="201" priority="356">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10668,7 +10752,7 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H63 J63">
+  <conditionalFormatting sqref="H64 J64">
     <cfRule type="expression" dxfId="199" priority="354">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10678,22 +10762,22 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
+  <conditionalFormatting sqref="K65">
     <cfRule type="expression" dxfId="197" priority="351">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H64 J64">
+  <conditionalFormatting sqref="H65 J65">
     <cfRule type="expression" dxfId="196" priority="350">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K65">
+  <conditionalFormatting sqref="K66">
     <cfRule type="expression" dxfId="195" priority="348">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K65">
+  <conditionalFormatting sqref="K66">
     <cfRule type="expression" dxfId="194" priority="347">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10703,7 +10787,7 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
+  <conditionalFormatting sqref="K67">
     <cfRule type="expression" dxfId="192" priority="344">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10713,7 +10797,7 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H66 J66">
+  <conditionalFormatting sqref="H67 J67">
     <cfRule type="expression" dxfId="190" priority="342">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10728,12 +10812,12 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K67">
+  <conditionalFormatting sqref="K68">
     <cfRule type="expression" dxfId="187" priority="336">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K67">
+  <conditionalFormatting sqref="K68">
     <cfRule type="expression" dxfId="186" priority="335">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10743,12 +10827,12 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
+  <conditionalFormatting sqref="K69">
     <cfRule type="expression" dxfId="184" priority="332">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H68 J68">
+  <conditionalFormatting sqref="H69 J69">
     <cfRule type="expression" dxfId="183" priority="330">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10758,7 +10842,7 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
+  <conditionalFormatting sqref="K70">
     <cfRule type="expression" dxfId="181" priority="328">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10773,7 +10857,7 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H69 J69">
+  <conditionalFormatting sqref="H70 J70">
     <cfRule type="expression" dxfId="178" priority="326">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10793,12 +10877,12 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
+  <conditionalFormatting sqref="K72">
     <cfRule type="expression" dxfId="174" priority="324">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
+  <conditionalFormatting sqref="K72">
     <cfRule type="expression" dxfId="173" priority="323">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10808,7 +10892,7 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I81">
+  <conditionalFormatting sqref="I82">
     <cfRule type="expression" dxfId="171" priority="230">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10823,127 +10907,127 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K74">
+    <cfRule type="expression" dxfId="168" priority="316">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="168" priority="316">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
     <cfRule type="expression" dxfId="167" priority="319">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H72 J72">
+    <cfRule type="expression" dxfId="166" priority="322">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H63 J63">
+    <cfRule type="expression" dxfId="165" priority="358">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="expression" dxfId="164" priority="355">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65">
+    <cfRule type="expression" dxfId="163" priority="352">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66 J66">
+    <cfRule type="expression" dxfId="162" priority="346">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67">
+    <cfRule type="expression" dxfId="161" priority="343">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H68 J68">
+    <cfRule type="expression" dxfId="160" priority="334">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="expression" dxfId="159" priority="331">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K73">
+    <cfRule type="expression" dxfId="158" priority="320">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H73 J73">
+    <cfRule type="expression" dxfId="157" priority="318">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K74">
+    <cfRule type="expression" dxfId="156" priority="315">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H74 J74">
+    <cfRule type="expression" dxfId="155" priority="314">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="154" priority="312">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="153" priority="311">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H71 J71">
-    <cfRule type="expression" dxfId="166" priority="322">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H62 J62">
-    <cfRule type="expression" dxfId="165" priority="358">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="164" priority="355">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="163" priority="352">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H65 J65">
-    <cfRule type="expression" dxfId="162" priority="346">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="161" priority="343">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="160" priority="334">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="159" priority="331">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="158" priority="320">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H72 J72">
-    <cfRule type="expression" dxfId="157" priority="318">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="156" priority="315">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H73 J73">
-    <cfRule type="expression" dxfId="155" priority="314">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="154" priority="312">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="153" priority="311">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H70 J70">
     <cfRule type="expression" dxfId="152" priority="310">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G81">
+  <conditionalFormatting sqref="G82">
     <cfRule type="expression" dxfId="151" priority="305">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J81:V81">
+  <conditionalFormatting sqref="J82:V82">
     <cfRule type="expression" dxfId="150" priority="300">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B81 E81:F81">
+  <conditionalFormatting sqref="B82 E82:F82">
     <cfRule type="expression" dxfId="149" priority="302">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K81:V81">
+  <conditionalFormatting sqref="K82:V82">
     <cfRule type="expression" dxfId="148" priority="301">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H81">
+  <conditionalFormatting sqref="H82">
     <cfRule type="expression" dxfId="147" priority="299">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H78">
+  <conditionalFormatting sqref="H79">
     <cfRule type="expression" dxfId="146" priority="296">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H79">
+  <conditionalFormatting sqref="H80">
     <cfRule type="expression" dxfId="145" priority="294">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G84">
+  <conditionalFormatting sqref="G85">
     <cfRule type="expression" dxfId="144" priority="291">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10953,32 +11037,32 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J84:V84">
+  <conditionalFormatting sqref="J85:V85">
     <cfRule type="expression" dxfId="142" priority="286">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B84 E84:F84">
+  <conditionalFormatting sqref="B85 E85:F85">
     <cfRule type="expression" dxfId="141" priority="288">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K84:V84">
+  <conditionalFormatting sqref="K85:V85">
     <cfRule type="expression" dxfId="140" priority="287">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H84">
+  <conditionalFormatting sqref="H85">
     <cfRule type="expression" dxfId="139" priority="285">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H82">
+  <conditionalFormatting sqref="H83">
     <cfRule type="expression" dxfId="138" priority="283">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G85">
+  <conditionalFormatting sqref="G86">
     <cfRule type="expression" dxfId="137" priority="281">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -10988,37 +11072,37 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J85:V85">
+  <conditionalFormatting sqref="J86:V86">
     <cfRule type="expression" dxfId="135" priority="276">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B85 E85:F85">
+  <conditionalFormatting sqref="B86 E86:F86">
     <cfRule type="expression" dxfId="134" priority="278">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K85:V85">
+  <conditionalFormatting sqref="K86:V86">
     <cfRule type="expression" dxfId="133" priority="277">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H85">
+  <conditionalFormatting sqref="H86">
     <cfRule type="expression" dxfId="132" priority="275">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J86">
+  <conditionalFormatting sqref="J87">
     <cfRule type="expression" dxfId="131" priority="273">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H86">
+  <conditionalFormatting sqref="H87">
     <cfRule type="expression" dxfId="130" priority="272">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G87">
+  <conditionalFormatting sqref="G88">
     <cfRule type="expression" dxfId="129" priority="270">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -11028,22 +11112,22 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J87:V87">
+  <conditionalFormatting sqref="J88:V88">
     <cfRule type="expression" dxfId="127" priority="265">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B87 E87:F87">
+  <conditionalFormatting sqref="B88 E88:F88">
     <cfRule type="expression" dxfId="126" priority="267">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K87:V87">
+  <conditionalFormatting sqref="K88:V88">
     <cfRule type="expression" dxfId="125" priority="266">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H87">
+  <conditionalFormatting sqref="H88">
     <cfRule type="expression" dxfId="124" priority="264">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -11078,117 +11162,117 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I67">
+    <cfRule type="expression" dxfId="117" priority="244">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I63">
+    <cfRule type="expression" dxfId="116" priority="248">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I64">
+    <cfRule type="expression" dxfId="115" priority="247">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I65">
+    <cfRule type="expression" dxfId="114" priority="246">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I66">
-    <cfRule type="expression" dxfId="117" priority="244">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I62">
-    <cfRule type="expression" dxfId="116" priority="248">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="115" priority="247">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I64">
-    <cfRule type="expression" dxfId="114" priority="246">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
     <cfRule type="expression" dxfId="113" priority="245">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I67">
+  <conditionalFormatting sqref="I68">
     <cfRule type="expression" dxfId="112" priority="242">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I68">
+  <conditionalFormatting sqref="I69">
     <cfRule type="expression" dxfId="111" priority="241">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I69">
+  <conditionalFormatting sqref="I70">
     <cfRule type="expression" dxfId="110" priority="240">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I70">
+  <conditionalFormatting sqref="I71">
     <cfRule type="expression" dxfId="109" priority="239">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I71">
+  <conditionalFormatting sqref="I72">
     <cfRule type="expression" dxfId="108" priority="238">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I72">
+  <conditionalFormatting sqref="I73">
     <cfRule type="expression" dxfId="107" priority="237">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I73">
+  <conditionalFormatting sqref="I74">
     <cfRule type="expression" dxfId="106" priority="236">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I74">
+  <conditionalFormatting sqref="I75">
     <cfRule type="expression" dxfId="105" priority="235">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I77">
+  <conditionalFormatting sqref="I78">
     <cfRule type="expression" dxfId="104" priority="233">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I78">
+  <conditionalFormatting sqref="I79">
     <cfRule type="expression" dxfId="103" priority="232">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I79">
+  <conditionalFormatting sqref="I80">
     <cfRule type="expression" dxfId="102" priority="231">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I82">
+  <conditionalFormatting sqref="I83">
     <cfRule type="expression" dxfId="101" priority="229">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I84">
+  <conditionalFormatting sqref="I85">
     <cfRule type="expression" dxfId="100" priority="228">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I85">
+  <conditionalFormatting sqref="I86">
     <cfRule type="expression" dxfId="99" priority="227">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I86">
+  <conditionalFormatting sqref="I87">
     <cfRule type="expression" dxfId="98" priority="226">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87">
+  <conditionalFormatting sqref="I88">
     <cfRule type="expression" dxfId="97" priority="225">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88">
+  <conditionalFormatting sqref="I89">
     <cfRule type="expression" dxfId="96" priority="224">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H88">
+  <conditionalFormatting sqref="H89">
     <cfRule type="expression" dxfId="95" priority="223">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -11383,12 +11467,12 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H83">
+  <conditionalFormatting sqref="H84">
     <cfRule type="expression" dxfId="56" priority="102">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I83">
+  <conditionalFormatting sqref="I84">
     <cfRule type="expression" dxfId="55" priority="101">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -11473,22 +11557,22 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K75">
+  <conditionalFormatting sqref="K76">
     <cfRule type="expression" dxfId="38" priority="61">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J75:K75">
+  <conditionalFormatting sqref="J76:K76">
     <cfRule type="expression" dxfId="37" priority="60">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H75">
+  <conditionalFormatting sqref="H76">
     <cfRule type="expression" dxfId="36" priority="59">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I75">
+  <conditionalFormatting sqref="I76">
     <cfRule type="expression" dxfId="35" priority="58">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -11503,27 +11587,27 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J80">
+  <conditionalFormatting sqref="J81">
     <cfRule type="expression" dxfId="32" priority="46">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H80">
+  <conditionalFormatting sqref="H81">
     <cfRule type="expression" dxfId="31" priority="45">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I80">
+  <conditionalFormatting sqref="I81">
     <cfRule type="expression" dxfId="30" priority="44">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K80:V80">
+  <conditionalFormatting sqref="K81:V81">
     <cfRule type="expression" dxfId="29" priority="43">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K80:V80">
+  <conditionalFormatting sqref="K81:V81">
     <cfRule type="expression" dxfId="28" priority="41">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -11608,7 +11692,7 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F59">
+  <conditionalFormatting sqref="F60">
     <cfRule type="expression" dxfId="11" priority="18">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -11628,42 +11712,42 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G76">
+  <conditionalFormatting sqref="G77">
     <cfRule type="expression" dxfId="7" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K76">
+  <conditionalFormatting sqref="K77">
     <cfRule type="expression" dxfId="6" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J76:K76">
+  <conditionalFormatting sqref="J77:K77">
     <cfRule type="expression" dxfId="5" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H76">
+  <conditionalFormatting sqref="H77">
     <cfRule type="expression" dxfId="4" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
+  <conditionalFormatting sqref="I77">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L76:V76">
+  <conditionalFormatting sqref="L77:V77">
     <cfRule type="expression" dxfId="2" priority="8">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L76:V76">
+  <conditionalFormatting sqref="L77:V77">
     <cfRule type="expression" dxfId="1" priority="6">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L76:V76">
+  <conditionalFormatting sqref="L77:V77">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Demoon moved 1 hour later
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10303"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6131E1-7781-B240-B29E-4141B93DE93E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC39E386-75FA-7443-826C-2AE55603DC8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19460" yWindow="5940" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1214,56 +1214,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="276">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="280">
     <dxf>
       <fill>
         <patternFill>
@@ -1323,6 +1274,97 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
@@ -2942,20 +2984,6 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3481,8 +3509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6887,22 +6915,22 @@
     <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="54"/>
       <c r="B45" s="18" t="s">
-        <v>60</v>
+        <v>238</v>
       </c>
       <c r="C45" s="7">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D45" s="7">
-        <v>44</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="E45" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="G45" s="29" t="s">
-        <v>163</v>
+        <v>239</v>
       </c>
       <c r="H45" s="29" t="s">
         <v>216</v>
@@ -6965,22 +6993,22 @@
     <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="54"/>
       <c r="B46" s="18" t="s">
-        <v>238</v>
+        <v>108</v>
       </c>
       <c r="C46" s="7">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D46" s="7">
-        <v>45</v>
-      </c>
-      <c r="E46" s="33" t="s">
-        <v>75</v>
+        <v>46</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>70</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G46" s="29" t="s">
-        <v>239</v>
+        <v>71</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="H46" s="29" t="s">
         <v>216</v>
@@ -7040,25 +7068,25 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="54"/>
       <c r="B47" s="18" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C47" s="7">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D47" s="7">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>119</v>
+        <v>17</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="29" t="s">
+        <v>139</v>
       </c>
       <c r="H47" s="29" t="s">
         <v>216</v>
@@ -7069,7 +7097,7 @@
       <c r="J47" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K47" s="25">
+      <c r="K47" s="11">
         <f>$I47+Sheet2!B$1/24</f>
         <v>1.2916666666666667</v>
       </c>
@@ -7121,97 +7149,97 @@
     <row r="48" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="54"/>
       <c r="B48" s="18" t="s">
-        <v>97</v>
+        <v>217</v>
       </c>
       <c r="C48" s="7">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D48" s="7">
-        <v>47</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F48" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G48" s="29" t="s">
-        <v>139</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E48" s="20"/>
+      <c r="F48" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G48" s="29"/>
       <c r="H48" s="29" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="I48" s="23">
-        <v>0.875</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="J48" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K48" s="11">
+      <c r="K48" s="25">
         <f>$I48+Sheet2!B$1/24</f>
-        <v>1.2916666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="L48" s="23">
         <f>$I48+Sheet2!B$2/24</f>
-        <v>1.25</v>
+        <v>1.2916666666666665</v>
       </c>
       <c r="M48" s="23">
         <f>$I48+Sheet2!B$3/24</f>
-        <v>1.2083333333333333</v>
+        <v>1.25</v>
       </c>
       <c r="N48" s="23">
         <f>$I48+Sheet2!B$4/24</f>
-        <v>1</v>
+        <v>1.0416666666666665</v>
       </c>
       <c r="O48" s="23">
         <f>$I48+Sheet2!B$5/24</f>
-        <v>1</v>
+        <v>1.0416666666666665</v>
       </c>
       <c r="P48" s="23">
         <f>$I48+Sheet2!B$6/24</f>
-        <v>1</v>
+        <v>1.0416666666666665</v>
       </c>
       <c r="Q48" s="23">
         <f>$I48+Sheet2!B$7/24</f>
-        <v>0.95833333333333337</v>
+        <v>1</v>
       </c>
       <c r="R48" s="23">
         <f>$I48+Sheet2!B$8/24</f>
-        <v>0.91666666666666663</v>
+        <v>0.95833333333333326</v>
       </c>
       <c r="S48" s="23">
         <f>$I48+Sheet2!B$9/24</f>
-        <v>0.70833333333333337</v>
+        <v>0.75</v>
       </c>
       <c r="T48" s="23">
         <f>$I48+Sheet2!B$10/24</f>
-        <v>0.66666666666666663</v>
+        <v>0.70833333333333326</v>
       </c>
       <c r="U48" s="23">
         <f>$I48+Sheet2!B$11/24</f>
-        <v>0.625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="V48" s="23">
         <f>$I48+Sheet2!B$12/24</f>
-        <v>0.58333333333333326</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="49" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="54"/>
       <c r="B49" s="18" t="s">
-        <v>217</v>
+        <v>60</v>
       </c>
       <c r="C49" s="7">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D49" s="7">
-        <v>48</v>
-      </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="G49" s="29"/>
+        <v>44</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="29" t="s">
+        <v>163</v>
+      </c>
       <c r="H49" s="29" t="s">
         <v>218</v>
       </c>
@@ -10360,11 +10388,11 @@
     <sortCondition ref="D2:D72"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -10372,1383 +10400,1393 @@
     <mergeCell ref="A25:A50"/>
     <mergeCell ref="A51:A88"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V44 K46:V89">
-    <cfRule type="expression" dxfId="275" priority="658">
+  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V48 K50:V89">
+    <cfRule type="expression" dxfId="279" priority="668">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K17:V17 K19:V19 K23:V23 K20 K24:K32 K22">
-    <cfRule type="expression" dxfId="274" priority="660">
+    <cfRule type="expression" dxfId="278" priority="670">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K53:V53 G53 G64 G73 G89 E62:G62 G30 B74 E74:G74 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 B70:B72 E70:G72 L40:V40 K87:V87 G87 K79:V80 K83:V84 K89:V89 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B84 J11:V14 J84:V84 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L76:V76 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E84:G84 E61:V61 E65:G65 B50:B62 B40 B44:B46 B81 B48 J48:V48 G75:G80 E24:G29 B20:B38 E5:G5 E48:H48 E81:G81 E76:G77 L24:V32 L20:V20 L22:V22 G66:G69 E44:H44 E45:G46 L64:V74 B65:B67 B76:B77 C4:D89 G58:V60">
-    <cfRule type="expression" dxfId="273" priority="664">
+  <conditionalFormatting sqref="K53:V53 G53 G64 G73 G89 E62:G62 G30 B74 E74:G74 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 B70:B72 E70:G72 L40:V40 K87:V87 G87 K79:V80 K83:V84 K89:V89 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B84 J11:V14 J84:V84 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L76:V76 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E84:G84 E61:V61 E65:G65 B50:B62 B40 B81 B47 J47:V47 G75:G80 E24:G29 B20:B38 E5:G5 E47:H47 E81:G81 E76:G77 L24:V32 L20:V20 L22:V22 G66:G69 E44:H44 L64:V74 B65:B67 B76:B77 G58:V60 C50:D89 B44:B45 E45:G45 C4:D48">
+    <cfRule type="expression" dxfId="277" priority="674">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64 L64:V64">
-    <cfRule type="expression" dxfId="272" priority="641">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
-    <cfRule type="expression" dxfId="271" priority="639">
+    <cfRule type="expression" dxfId="276" priority="651">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69 L69:V69">
-    <cfRule type="expression" dxfId="270" priority="637">
+    <cfRule type="expression" dxfId="275" priority="647">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73 L73:V73">
-    <cfRule type="expression" dxfId="269" priority="635">
+    <cfRule type="expression" dxfId="274" priority="645">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68 L68:V68">
-    <cfRule type="expression" dxfId="268" priority="633">
+    <cfRule type="expression" dxfId="273" priority="643">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87 K87:V87 E87:F87">
-    <cfRule type="expression" dxfId="267" priority="629">
+    <cfRule type="expression" dxfId="272" priority="639">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" dxfId="266" priority="627">
+    <cfRule type="expression" dxfId="271" priority="637">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E73">
+    <cfRule type="expression" dxfId="270" priority="634">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68">
+    <cfRule type="expression" dxfId="269" priority="633">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B84 J83:V84">
+    <cfRule type="expression" dxfId="268" priority="630">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B80:B81 J80:V80 E80:E81">
+    <cfRule type="expression" dxfId="267" priority="628">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E83:F84">
+    <cfRule type="expression" dxfId="266" priority="626">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B79 J79:V79">
     <cfRule type="expression" dxfId="265" priority="624">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
-    <cfRule type="expression" dxfId="264" priority="623">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B83:B84 J83:V84">
-    <cfRule type="expression" dxfId="263" priority="620">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B80:B81 J80:V80 E80:E81">
-    <cfRule type="expression" dxfId="262" priority="618">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E83:F84">
-    <cfRule type="expression" dxfId="261" priority="616">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B79 J79:V79">
-    <cfRule type="expression" dxfId="260" priority="614">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B89 J89:V89 E89">
-    <cfRule type="expression" dxfId="259" priority="612">
+    <cfRule type="expression" dxfId="264" priority="622">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F68">
-    <cfRule type="expression" dxfId="258" priority="604">
+    <cfRule type="expression" dxfId="263" priority="614">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62:V62">
-    <cfRule type="expression" dxfId="257" priority="544">
+    <cfRule type="expression" dxfId="262" priority="554">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F73">
-    <cfRule type="expression" dxfId="256" priority="566">
+    <cfRule type="expression" dxfId="261" priority="576">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75:B77 E75:F77">
-    <cfRule type="expression" dxfId="255" priority="530">
+    <cfRule type="expression" dxfId="260" priority="540">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="254" priority="551">
+    <cfRule type="expression" dxfId="259" priority="561">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B63 L63:V63">
+    <cfRule type="expression" dxfId="258" priority="562">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F80:F81">
+    <cfRule type="expression" dxfId="257" priority="574">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F64">
+    <cfRule type="expression" dxfId="256" priority="570">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69:F69">
+    <cfRule type="expression" dxfId="255" priority="569">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E79:F79">
+    <cfRule type="expression" dxfId="254" priority="567">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L63:V63 G63">
+    <cfRule type="expression" dxfId="253" priority="564">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7:V7">
+    <cfRule type="expression" dxfId="252" priority="509">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F63">
+    <cfRule type="expression" dxfId="251" priority="558">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47:V47">
+    <cfRule type="expression" dxfId="250" priority="678">
+      <formula>K$1=#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K62:V62">
+    <cfRule type="expression" dxfId="249" priority="555">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L8:V10">
+    <cfRule type="expression" dxfId="248" priority="500">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13:H14 J13:V14 L18:V18">
+    <cfRule type="expression" dxfId="247" priority="546">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13:V14 L18:V18">
+    <cfRule type="expression" dxfId="246" priority="547">
+      <formula>K$1=#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:G3 B7 E7:G7">
+    <cfRule type="expression" dxfId="245" priority="541">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K75:V75 L76:V76">
+    <cfRule type="expression" dxfId="244" priority="539">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J75:V75 L76:V76">
+    <cfRule type="expression" dxfId="243" priority="537">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H75">
+    <cfRule type="expression" dxfId="242" priority="536">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J78:V78">
+    <cfRule type="expression" dxfId="241" priority="531">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B78 E78:F78">
+    <cfRule type="expression" dxfId="240" priority="534">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K78:V78">
+    <cfRule type="expression" dxfId="239" priority="533">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H78">
+    <cfRule type="expression" dxfId="238" priority="530">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="expression" dxfId="237" priority="523">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30:F30">
+    <cfRule type="expression" dxfId="236" priority="528">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43 E43 L43:V43 G43">
+    <cfRule type="expression" dxfId="235" priority="527">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4 E4:G4">
+    <cfRule type="expression" dxfId="234" priority="522">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
+    <cfRule type="expression" dxfId="233" priority="521">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6 E6:H6 J6:V6">
+    <cfRule type="expression" dxfId="232" priority="519">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:V5">
+    <cfRule type="expression" dxfId="231" priority="516">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:L4">
+    <cfRule type="expression" dxfId="230" priority="511">
+      <formula>K$1=$H4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:V4">
+    <cfRule type="expression" dxfId="229" priority="512">
+      <formula>K$1=$I4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:V4">
+    <cfRule type="expression" dxfId="228" priority="513">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="expression" dxfId="227" priority="506">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:B10 E8:G10">
+    <cfRule type="expression" dxfId="226" priority="505">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8:K8">
+    <cfRule type="expression" dxfId="225" priority="503">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15 E15:H15 J15:V15">
+    <cfRule type="expression" dxfId="224" priority="495">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15 J15:V15">
+    <cfRule type="expression" dxfId="223" priority="492">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15:V15">
+    <cfRule type="expression" dxfId="222" priority="493">
+      <formula>K$1=#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15 E15:G15">
+    <cfRule type="expression" dxfId="221" priority="491">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16 J16:K16">
+    <cfRule type="expression" dxfId="220" priority="488">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16 J16:K16">
+    <cfRule type="expression" dxfId="219" priority="485">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="expression" dxfId="218" priority="486">
+      <formula>K$1=#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H48 J48:V48">
+    <cfRule type="expression" dxfId="217" priority="380">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19 E19:H19 J19:V19">
+    <cfRule type="expression" dxfId="216" priority="481">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K70">
+    <cfRule type="expression" dxfId="215" priority="337">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27 J27:K27">
+    <cfRule type="expression" dxfId="214" priority="443">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62:J62">
+    <cfRule type="expression" dxfId="213" priority="375">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20 J20:K20">
+    <cfRule type="expression" dxfId="212" priority="470">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22 J22:K22">
+    <cfRule type="expression" dxfId="211" priority="465">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="expression" dxfId="210" priority="370">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="expression" dxfId="209" priority="369">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24 J24:K24">
+    <cfRule type="expression" dxfId="208" priority="458">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="expression" dxfId="207" priority="366">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25 J25:K25">
+    <cfRule type="expression" dxfId="206" priority="453">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H64 J64">
+    <cfRule type="expression" dxfId="205" priority="364">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26 J26:K26">
+    <cfRule type="expression" dxfId="204" priority="448">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65">
+    <cfRule type="expression" dxfId="203" priority="361">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H65 J65">
+    <cfRule type="expression" dxfId="202" priority="360">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K66">
+    <cfRule type="expression" dxfId="201" priority="358">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K66">
+    <cfRule type="expression" dxfId="200" priority="357">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28 J28:K28">
+    <cfRule type="expression" dxfId="199" priority="438">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67">
+    <cfRule type="expression" dxfId="198" priority="354">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29 J29:K29">
+    <cfRule type="expression" dxfId="197" priority="433">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H67 J67">
+    <cfRule type="expression" dxfId="196" priority="352">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30 J30:K30">
+    <cfRule type="expression" dxfId="195" priority="428">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31 J31:K31">
+    <cfRule type="expression" dxfId="194" priority="423">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K68">
+    <cfRule type="expression" dxfId="193" priority="346">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K68">
+    <cfRule type="expression" dxfId="192" priority="345">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32 J32:K32">
+    <cfRule type="expression" dxfId="191" priority="418">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="expression" dxfId="190" priority="342">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H69 J69">
+    <cfRule type="expression" dxfId="189" priority="340">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="expression" dxfId="188" priority="406">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K70">
+    <cfRule type="expression" dxfId="187" priority="338">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="expression" dxfId="186" priority="403">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
+    <cfRule type="expression" dxfId="185" priority="400">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H70 J70">
+    <cfRule type="expression" dxfId="184" priority="336">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H37">
+    <cfRule type="expression" dxfId="183" priority="397">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:B40 J39:V39 E39:H39 E40:G40 L40:V40">
+    <cfRule type="expression" dxfId="182" priority="394">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41:V41 B41:B43 E43 E41:H41 G43 E42:G42 L42:V43">
+    <cfRule type="expression" dxfId="181" priority="390">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72">
+    <cfRule type="expression" dxfId="180" priority="334">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72">
+    <cfRule type="expression" dxfId="179" priority="333">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48:G48 B48">
+    <cfRule type="expression" dxfId="178" priority="383">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I82">
+    <cfRule type="expression" dxfId="177" priority="240">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H50">
+    <cfRule type="expression" dxfId="176" priority="379">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53 J53">
+    <cfRule type="expression" dxfId="175" priority="378">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K74">
+    <cfRule type="expression" dxfId="174" priority="326">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K73">
+    <cfRule type="expression" dxfId="173" priority="329">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H72 J72">
+    <cfRule type="expression" dxfId="172" priority="332">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H63 J63">
+    <cfRule type="expression" dxfId="171" priority="368">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="expression" dxfId="170" priority="365">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65">
+    <cfRule type="expression" dxfId="169" priority="362">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66 J66">
+    <cfRule type="expression" dxfId="168" priority="356">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67">
+    <cfRule type="expression" dxfId="167" priority="353">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H68 J68">
+    <cfRule type="expression" dxfId="166" priority="344">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="expression" dxfId="165" priority="341">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K73">
+    <cfRule type="expression" dxfId="164" priority="330">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H73 J73">
+    <cfRule type="expression" dxfId="163" priority="328">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K74">
+    <cfRule type="expression" dxfId="162" priority="325">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H74 J74">
+    <cfRule type="expression" dxfId="161" priority="324">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="160" priority="322">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="159" priority="321">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H71 J71">
+    <cfRule type="expression" dxfId="158" priority="320">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G82">
+    <cfRule type="expression" dxfId="157" priority="315">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J82:V82">
+    <cfRule type="expression" dxfId="156" priority="310">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B82 E82:F82">
+    <cfRule type="expression" dxfId="155" priority="312">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82:V82">
+    <cfRule type="expression" dxfId="154" priority="311">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H82">
+    <cfRule type="expression" dxfId="153" priority="309">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H79">
+    <cfRule type="expression" dxfId="152" priority="306">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H80">
+    <cfRule type="expression" dxfId="151" priority="304">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G85">
+    <cfRule type="expression" dxfId="150" priority="301">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="expression" dxfId="149" priority="158">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J85:V85">
+    <cfRule type="expression" dxfId="148" priority="296">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B85 E85:F85">
+    <cfRule type="expression" dxfId="147" priority="298">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K85:V85">
+    <cfRule type="expression" dxfId="146" priority="297">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H85">
+    <cfRule type="expression" dxfId="145" priority="295">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H83">
+    <cfRule type="expression" dxfId="144" priority="293">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G86">
+    <cfRule type="expression" dxfId="143" priority="291">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="expression" dxfId="142" priority="148">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J86:V86">
+    <cfRule type="expression" dxfId="141" priority="286">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B86 E86:F86">
+    <cfRule type="expression" dxfId="140" priority="288">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K86:V86">
+    <cfRule type="expression" dxfId="139" priority="287">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H86">
+    <cfRule type="expression" dxfId="138" priority="285">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J87">
+    <cfRule type="expression" dxfId="137" priority="283">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H87">
+    <cfRule type="expression" dxfId="136" priority="282">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G88">
+    <cfRule type="expression" dxfId="135" priority="280">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33">
+    <cfRule type="expression" dxfId="134" priority="137">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J88:V88">
+    <cfRule type="expression" dxfId="133" priority="275">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B88 E88:F88">
+    <cfRule type="expression" dxfId="132" priority="277">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K88:V88">
+    <cfRule type="expression" dxfId="131" priority="276">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H88">
+    <cfRule type="expression" dxfId="130" priority="274">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K43">
+    <cfRule type="expression" dxfId="129" priority="272">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43 J43">
+    <cfRule type="expression" dxfId="128" priority="270">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J38:K38">
+    <cfRule type="expression" dxfId="127" priority="267">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H38">
+    <cfRule type="expression" dxfId="126" priority="265">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I48">
+    <cfRule type="expression" dxfId="125" priority="123">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I53">
+    <cfRule type="expression" dxfId="124" priority="261">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I67">
+    <cfRule type="expression" dxfId="123" priority="254">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I63">
+    <cfRule type="expression" dxfId="122" priority="258">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I64">
+    <cfRule type="expression" dxfId="121" priority="257">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I65">
+    <cfRule type="expression" dxfId="120" priority="256">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I66">
+    <cfRule type="expression" dxfId="119" priority="255">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I68">
+    <cfRule type="expression" dxfId="118" priority="252">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I69">
+    <cfRule type="expression" dxfId="117" priority="251">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I70">
+    <cfRule type="expression" dxfId="116" priority="250">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I71">
+    <cfRule type="expression" dxfId="115" priority="249">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I72">
+    <cfRule type="expression" dxfId="114" priority="248">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I73">
+    <cfRule type="expression" dxfId="113" priority="247">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I74">
+    <cfRule type="expression" dxfId="112" priority="246">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I75">
+    <cfRule type="expression" dxfId="111" priority="245">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I78">
+    <cfRule type="expression" dxfId="110" priority="243">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I79">
+    <cfRule type="expression" dxfId="109" priority="242">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I80">
+    <cfRule type="expression" dxfId="108" priority="241">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I83">
+    <cfRule type="expression" dxfId="107" priority="239">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I85">
+    <cfRule type="expression" dxfId="106" priority="238">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I86">
+    <cfRule type="expression" dxfId="105" priority="237">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I87">
+    <cfRule type="expression" dxfId="104" priority="236">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I88">
+    <cfRule type="expression" dxfId="103" priority="235">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I89">
+    <cfRule type="expression" dxfId="102" priority="234">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H89">
+    <cfRule type="expression" dxfId="101" priority="233">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="expression" dxfId="100" priority="232">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="expression" dxfId="99" priority="231">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="expression" dxfId="98" priority="230">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="expression" dxfId="97" priority="229">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="expression" dxfId="96" priority="228">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="expression" dxfId="95" priority="227">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="expression" dxfId="94" priority="226">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="expression" dxfId="93" priority="225">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="expression" dxfId="92" priority="157">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="expression" dxfId="91" priority="156">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="expression" dxfId="90" priority="155">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="expression" dxfId="89" priority="154">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="expression" dxfId="88" priority="153">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="expression" dxfId="87" priority="147">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="expression" dxfId="86" priority="151">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="expression" dxfId="85" priority="150">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
+    <cfRule type="expression" dxfId="84" priority="149">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="expression" dxfId="83" priority="146">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="expression" dxfId="82" priority="145">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="expression" dxfId="81" priority="144">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="expression" dxfId="80" priority="143">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="expression" dxfId="79" priority="142">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30">
+    <cfRule type="expression" dxfId="78" priority="141">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="expression" dxfId="77" priority="140">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="expression" dxfId="76" priority="139">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
+    <cfRule type="expression" dxfId="75" priority="136">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50">
+    <cfRule type="expression" dxfId="74" priority="122">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
+    <cfRule type="expression" dxfId="73" priority="134">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="expression" dxfId="72" priority="133">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="expression" dxfId="71" priority="132">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38">
+    <cfRule type="expression" dxfId="70" priority="131">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="expression" dxfId="69" priority="130">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
+    <cfRule type="expression" dxfId="68" priority="129">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43">
+    <cfRule type="expression" dxfId="67" priority="128">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="expression" dxfId="66" priority="126">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I47">
+    <cfRule type="expression" dxfId="65" priority="124">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:V10">
+    <cfRule type="expression" dxfId="64" priority="114">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="expression" dxfId="63" priority="103">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H84">
+    <cfRule type="expression" dxfId="62" priority="112">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I84">
+    <cfRule type="expression" dxfId="61" priority="111">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:K9">
+    <cfRule type="expression" dxfId="60" priority="102">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="expression" dxfId="59" priority="101">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="58" priority="104">
+      <formula>K$1=$H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="57" priority="105">
+      <formula>K$1=$I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="56" priority="99">
+      <formula>K$1=$H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="55" priority="100">
+      <formula>K$1=$I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="expression" dxfId="54" priority="98">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:K10">
+    <cfRule type="expression" dxfId="53" priority="97">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="expression" dxfId="52" priority="96">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43">
+    <cfRule type="expression" dxfId="51" priority="89">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42:K42 H42">
+    <cfRule type="expression" dxfId="50" priority="84">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I42">
+    <cfRule type="expression" dxfId="49" priority="83">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="48" priority="74">
+      <formula>K$1=$H18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="47" priority="75">
+      <formula>K$1=$I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18 J18:K18">
+    <cfRule type="expression" dxfId="46" priority="76">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="expression" dxfId="45" priority="73">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K76">
+    <cfRule type="expression" dxfId="44" priority="71">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J76:K76">
+    <cfRule type="expression" dxfId="43" priority="70">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H76">
+    <cfRule type="expression" dxfId="42" priority="69">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I76">
+    <cfRule type="expression" dxfId="41" priority="68">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40:K40 H40">
+    <cfRule type="expression" dxfId="40" priority="66">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="expression" dxfId="39" priority="65">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J81">
+    <cfRule type="expression" dxfId="38" priority="56">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H81">
+    <cfRule type="expression" dxfId="37" priority="55">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I81">
+    <cfRule type="expression" dxfId="36" priority="54">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81:V81">
+    <cfRule type="expression" dxfId="35" priority="53">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81:V81">
+    <cfRule type="expression" dxfId="34" priority="51">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46 G46">
+    <cfRule type="expression" dxfId="33" priority="49">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46:F46">
+    <cfRule type="expression" dxfId="32" priority="48">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46 E46 G46">
+    <cfRule type="expression" dxfId="31" priority="47">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46 E46 G46">
+    <cfRule type="expression" dxfId="30" priority="46">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46">
+    <cfRule type="expression" dxfId="29" priority="45">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J46:V46 H46">
+    <cfRule type="expression" dxfId="28" priority="44">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I46">
+    <cfRule type="expression" dxfId="27" priority="42">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21 E21:G21">
+    <cfRule type="expression" dxfId="26" priority="41">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45:F45">
-    <cfRule type="expression" dxfId="253" priority="558">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B63 L63:V63">
-    <cfRule type="expression" dxfId="252" priority="552">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F80:F81">
-    <cfRule type="expression" dxfId="251" priority="564">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F64">
-    <cfRule type="expression" dxfId="250" priority="560">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69:F69">
-    <cfRule type="expression" dxfId="249" priority="559">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E79:F79">
-    <cfRule type="expression" dxfId="248" priority="557">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L63:V63 G63">
-    <cfRule type="expression" dxfId="247" priority="554">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7:V7">
-    <cfRule type="expression" dxfId="246" priority="499">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F63">
-    <cfRule type="expression" dxfId="245" priority="548">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K48:V48">
-    <cfRule type="expression" dxfId="244" priority="668">
-      <formula>K$1=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62:V62">
-    <cfRule type="expression" dxfId="243" priority="545">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L8:V10">
-    <cfRule type="expression" dxfId="242" priority="490">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13:H14 J13:V14 L18:V18">
-    <cfRule type="expression" dxfId="241" priority="536">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K13:V14 L18:V18">
-    <cfRule type="expression" dxfId="240" priority="537">
-      <formula>K$1=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G3 B7 E7:G7">
-    <cfRule type="expression" dxfId="239" priority="531">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K75:V75 L76:V76">
-    <cfRule type="expression" dxfId="238" priority="529">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J75:V75 L76:V76">
-    <cfRule type="expression" dxfId="237" priority="527">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H75">
-    <cfRule type="expression" dxfId="236" priority="526">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J78:V78">
-    <cfRule type="expression" dxfId="235" priority="521">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B78 E78:F78">
-    <cfRule type="expression" dxfId="234" priority="524">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K78:V78">
-    <cfRule type="expression" dxfId="233" priority="523">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H78">
-    <cfRule type="expression" dxfId="232" priority="520">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="231" priority="513">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30:F30">
-    <cfRule type="expression" dxfId="230" priority="518">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B43 E43 L43:V43 G43">
-    <cfRule type="expression" dxfId="229" priority="517">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4 E4:G4">
-    <cfRule type="expression" dxfId="228" priority="512">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="227" priority="511">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6 E6:H6 J6:V6">
-    <cfRule type="expression" dxfId="226" priority="509">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:V5">
-    <cfRule type="expression" dxfId="225" priority="506">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:L4">
-    <cfRule type="expression" dxfId="224" priority="501">
-      <formula>K$1=$H4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:V4">
-    <cfRule type="expression" dxfId="223" priority="502">
-      <formula>K$1=$I4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4:V4">
-    <cfRule type="expression" dxfId="222" priority="503">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="221" priority="496">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B10 E8:G10">
-    <cfRule type="expression" dxfId="220" priority="495">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8:K8">
-    <cfRule type="expression" dxfId="219" priority="493">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15 E15:H15 J15:V15">
-    <cfRule type="expression" dxfId="218" priority="485">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15 J15:V15">
-    <cfRule type="expression" dxfId="217" priority="482">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15:V15">
-    <cfRule type="expression" dxfId="216" priority="483">
-      <formula>K$1=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15 E15:G15">
-    <cfRule type="expression" dxfId="215" priority="481">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="214" priority="478">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="213" priority="475">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="212" priority="476">
-      <formula>K$1=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H49 J49:V49">
-    <cfRule type="expression" dxfId="211" priority="370">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19 E19:H19 J19:V19">
-    <cfRule type="expression" dxfId="210" priority="471">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="209" priority="327">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27 J27:K27">
-    <cfRule type="expression" dxfId="208" priority="433">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H62:J62">
-    <cfRule type="expression" dxfId="207" priority="365">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20 J20:K20">
-    <cfRule type="expression" dxfId="206" priority="460">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22 J22:K22">
-    <cfRule type="expression" dxfId="205" priority="455">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="204" priority="360">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="203" priority="359">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24 J24:K24">
-    <cfRule type="expression" dxfId="202" priority="448">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="201" priority="356">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25 J25:K25">
-    <cfRule type="expression" dxfId="200" priority="443">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H64 J64">
-    <cfRule type="expression" dxfId="199" priority="354">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26 J26:K26">
-    <cfRule type="expression" dxfId="198" priority="438">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="197" priority="351">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H65 J65">
-    <cfRule type="expression" dxfId="196" priority="350">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="195" priority="348">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="194" priority="347">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H28 J28:K28">
-    <cfRule type="expression" dxfId="193" priority="428">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="192" priority="344">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29 J29:K29">
-    <cfRule type="expression" dxfId="191" priority="423">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="190" priority="342">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H30 J30:K30">
-    <cfRule type="expression" dxfId="189" priority="418">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H31 J31:K31">
-    <cfRule type="expression" dxfId="188" priority="413">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="187" priority="336">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="186" priority="335">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H32 J32:K32">
-    <cfRule type="expression" dxfId="185" priority="408">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="184" priority="332">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H69 J69">
-    <cfRule type="expression" dxfId="183" priority="330">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="182" priority="396">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="181" priority="328">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="180" priority="393">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="179" priority="390">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H70 J70">
-    <cfRule type="expression" dxfId="178" priority="326">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="177" priority="387">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39:B40 J39:V39 E39:H39 E40:G40 L40:V40">
-    <cfRule type="expression" dxfId="176" priority="384">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J41:V41 B41:B43 E43 E41:H41 G43 E42:G42 L42:V43">
-    <cfRule type="expression" dxfId="175" priority="380">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="174" priority="324">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="173" priority="323">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49:G49 B49">
-    <cfRule type="expression" dxfId="172" priority="373">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I82">
-    <cfRule type="expression" dxfId="171" priority="230">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="170" priority="369">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H53 J53">
-    <cfRule type="expression" dxfId="169" priority="368">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="168" priority="316">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="167" priority="319">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H72 J72">
-    <cfRule type="expression" dxfId="166" priority="322">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H63 J63">
-    <cfRule type="expression" dxfId="165" priority="358">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="164" priority="355">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="163" priority="352">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H66 J66">
-    <cfRule type="expression" dxfId="162" priority="346">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="161" priority="343">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H68 J68">
-    <cfRule type="expression" dxfId="160" priority="334">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="159" priority="331">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="158" priority="320">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H73 J73">
-    <cfRule type="expression" dxfId="157" priority="318">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="156" priority="315">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H74 J74">
-    <cfRule type="expression" dxfId="155" priority="314">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="154" priority="312">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="153" priority="311">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H71 J71">
-    <cfRule type="expression" dxfId="152" priority="310">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G82">
-    <cfRule type="expression" dxfId="151" priority="305">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J82:V82">
-    <cfRule type="expression" dxfId="150" priority="300">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B82 E82:F82">
-    <cfRule type="expression" dxfId="149" priority="302">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82:V82">
-    <cfRule type="expression" dxfId="148" priority="301">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H82">
-    <cfRule type="expression" dxfId="147" priority="299">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H79">
-    <cfRule type="expression" dxfId="146" priority="296">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H80">
-    <cfRule type="expression" dxfId="145" priority="294">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G85">
-    <cfRule type="expression" dxfId="144" priority="291">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="143" priority="148">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J85:V85">
-    <cfRule type="expression" dxfId="142" priority="286">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B85 E85:F85">
-    <cfRule type="expression" dxfId="141" priority="288">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K85:V85">
-    <cfRule type="expression" dxfId="140" priority="287">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H85">
-    <cfRule type="expression" dxfId="139" priority="285">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H83">
-    <cfRule type="expression" dxfId="138" priority="283">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G86">
-    <cfRule type="expression" dxfId="137" priority="281">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="136" priority="138">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J86:V86">
-    <cfRule type="expression" dxfId="135" priority="276">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B86 E86:F86">
-    <cfRule type="expression" dxfId="134" priority="278">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K86:V86">
-    <cfRule type="expression" dxfId="133" priority="277">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H86">
-    <cfRule type="expression" dxfId="132" priority="275">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J87">
-    <cfRule type="expression" dxfId="131" priority="273">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H87">
-    <cfRule type="expression" dxfId="130" priority="272">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G88">
-    <cfRule type="expression" dxfId="129" priority="270">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="128" priority="127">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J88:V88">
-    <cfRule type="expression" dxfId="127" priority="265">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B88 E88:F88">
-    <cfRule type="expression" dxfId="126" priority="267">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K88:V88">
-    <cfRule type="expression" dxfId="125" priority="266">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H88">
-    <cfRule type="expression" dxfId="124" priority="264">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K43">
-    <cfRule type="expression" dxfId="123" priority="262">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H43 J43">
-    <cfRule type="expression" dxfId="122" priority="260">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J38:K38">
-    <cfRule type="expression" dxfId="121" priority="257">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="120" priority="255">
+    <cfRule type="expression" dxfId="25" priority="37">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J45:V45 H45">
+    <cfRule type="expression" dxfId="24" priority="36">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I45">
+    <cfRule type="expression" dxfId="23" priority="34">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:V21">
+    <cfRule type="expression" dxfId="22" priority="31">
+      <formula>K$1=$H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="expression" dxfId="21" priority="32">
+      <formula>K$1=$I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L21:V21">
+    <cfRule type="expression" dxfId="20" priority="33">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21 J21:K21">
+    <cfRule type="expression" dxfId="19" priority="30">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="expression" dxfId="18" priority="29">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F60">
+    <cfRule type="expression" dxfId="17" priority="28">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G77">
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K77">
+    <cfRule type="expression" dxfId="15" priority="14">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J77:K77">
+    <cfRule type="expression" dxfId="14" priority="13">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H77">
+    <cfRule type="expression" dxfId="13" priority="12">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I77">
+    <cfRule type="expression" dxfId="12" priority="11">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L77:V77">
+    <cfRule type="expression" dxfId="11" priority="18">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L77:V77">
+    <cfRule type="expression" dxfId="10" priority="16">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L77:V77">
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49:G49">
+    <cfRule type="expression" dxfId="8" priority="10">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49">
+    <cfRule type="expression" dxfId="7" priority="9">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49:F49">
+    <cfRule type="expression" dxfId="6" priority="8">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K49:V49">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>K$1=$H49</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J49:V49">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H49">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="expression" dxfId="119" priority="113">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I53">
-    <cfRule type="expression" dxfId="118" priority="251">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I67">
-    <cfRule type="expression" dxfId="117" priority="244">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="116" priority="248">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I64">
-    <cfRule type="expression" dxfId="115" priority="247">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
-    <cfRule type="expression" dxfId="114" priority="246">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I66">
-    <cfRule type="expression" dxfId="113" priority="245">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I68">
-    <cfRule type="expression" dxfId="112" priority="242">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="111" priority="241">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="110" priority="240">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I71">
-    <cfRule type="expression" dxfId="109" priority="239">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I72">
-    <cfRule type="expression" dxfId="108" priority="238">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I73">
-    <cfRule type="expression" dxfId="107" priority="237">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I74">
-    <cfRule type="expression" dxfId="106" priority="236">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I75">
-    <cfRule type="expression" dxfId="105" priority="235">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I78">
-    <cfRule type="expression" dxfId="104" priority="233">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I79">
-    <cfRule type="expression" dxfId="103" priority="232">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I80">
-    <cfRule type="expression" dxfId="102" priority="231">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I83">
-    <cfRule type="expression" dxfId="101" priority="229">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I85">
-    <cfRule type="expression" dxfId="100" priority="228">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I86">
-    <cfRule type="expression" dxfId="99" priority="227">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I87">
-    <cfRule type="expression" dxfId="98" priority="226">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I88">
-    <cfRule type="expression" dxfId="97" priority="225">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I89">
-    <cfRule type="expression" dxfId="96" priority="224">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H89">
-    <cfRule type="expression" dxfId="95" priority="223">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="94" priority="222">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="93" priority="221">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="expression" dxfId="92" priority="220">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="91" priority="219">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="90" priority="218">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="89" priority="217">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="88" priority="216">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="87" priority="215">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="86" priority="147">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="expression" dxfId="85" priority="146">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="expression" dxfId="84" priority="145">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="83" priority="144">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="82" priority="143">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="81" priority="137">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
-    <cfRule type="expression" dxfId="80" priority="141">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="expression" dxfId="79" priority="140">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="78" priority="139">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="expression" dxfId="77" priority="136">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
-    <cfRule type="expression" dxfId="76" priority="135">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
-    <cfRule type="expression" dxfId="75" priority="134">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="74" priority="133">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="73" priority="132">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="expression" dxfId="72" priority="131">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="expression" dxfId="71" priority="130">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="70" priority="129">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="69" priority="126">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I50">
-    <cfRule type="expression" dxfId="68" priority="112">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="expression" dxfId="67" priority="124">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
-    <cfRule type="expression" dxfId="66" priority="123">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="expression" dxfId="65" priority="122">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="64" priority="121">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="expression" dxfId="63" priority="120">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
-    <cfRule type="expression" dxfId="62" priority="119">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="61" priority="118">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="60" priority="116">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="59" priority="114">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L9:V10">
-    <cfRule type="expression" dxfId="58" priority="104">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="57" priority="93">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H84">
-    <cfRule type="expression" dxfId="56" priority="102">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I84">
-    <cfRule type="expression" dxfId="55" priority="101">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:K9">
-    <cfRule type="expression" dxfId="54" priority="92">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="53" priority="91">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="52" priority="94">
-      <formula>K$1=$H9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="51" priority="95">
-      <formula>K$1=$I9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="50" priority="89">
-      <formula>K$1=$H10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="49" priority="90">
-      <formula>K$1=$I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="48" priority="88">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
-    <cfRule type="expression" dxfId="47" priority="87">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="46" priority="86">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="45" priority="79">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J42:K42 H42">
-    <cfRule type="expression" dxfId="44" priority="74">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="43" priority="73">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="42" priority="64">
-      <formula>K$1=$H18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="41" priority="65">
-      <formula>K$1=$I18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18 J18:K18">
-    <cfRule type="expression" dxfId="40" priority="66">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="39" priority="63">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K76">
-    <cfRule type="expression" dxfId="38" priority="61">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J76:K76">
-    <cfRule type="expression" dxfId="37" priority="60">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H76">
-    <cfRule type="expression" dxfId="36" priority="59">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="expression" dxfId="35" priority="58">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J40:K40 H40">
-    <cfRule type="expression" dxfId="34" priority="56">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="33" priority="55">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J81">
-    <cfRule type="expression" dxfId="32" priority="46">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H81">
-    <cfRule type="expression" dxfId="31" priority="45">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I81">
-    <cfRule type="expression" dxfId="30" priority="44">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="29" priority="43">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="28" priority="41">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47 G47">
-    <cfRule type="expression" dxfId="27" priority="39">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47:F47">
-    <cfRule type="expression" dxfId="26" priority="38">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47 E47 G47">
-    <cfRule type="expression" dxfId="25" priority="37">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47 E47 G47">
-    <cfRule type="expression" dxfId="24" priority="36">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
-    <cfRule type="expression" dxfId="23" priority="35">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J47:V47 H47">
-    <cfRule type="expression" dxfId="22" priority="34">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="21" priority="32">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21 E21:G21">
-    <cfRule type="expression" dxfId="20" priority="31">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46:F46">
-    <cfRule type="expression" dxfId="19" priority="27">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J46:V46 H46">
-    <cfRule type="expression" dxfId="18" priority="26">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="17" priority="24">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:V21">
-    <cfRule type="expression" dxfId="16" priority="21">
-      <formula>K$1=$H21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="expression" dxfId="15" priority="22">
-      <formula>K$1=$I21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L21:V21">
-    <cfRule type="expression" dxfId="14" priority="23">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21 J21:K21">
-    <cfRule type="expression" dxfId="13" priority="20">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="expression" dxfId="12" priority="19">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F60">
-    <cfRule type="expression" dxfId="11" priority="18">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K45:V45">
-    <cfRule type="expression" dxfId="10" priority="16">
-      <formula>K$1=$H45</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J45:V45 H45">
-    <cfRule type="expression" dxfId="9" priority="17">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
-    <cfRule type="expression" dxfId="8" priority="15">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G77">
-    <cfRule type="expression" dxfId="7" priority="14">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K77">
-    <cfRule type="expression" dxfId="6" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J77:K77">
-    <cfRule type="expression" dxfId="5" priority="3">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="4" priority="2">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I77">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="2" priority="8">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="1" priority="6">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Move Demoon back to old payout group
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10303"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm/Documents/Code/swgoh-squad-arena-payout-bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC39E386-75FA-7443-826C-2AE55603DC8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA78F770-00C3-D440-AB59-DB88034EA68F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11600" yWindow="2680" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1214,14 +1214,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="280">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="277">
     <dxf>
       <fill>
         <patternFill>
@@ -1241,20 +1234,6 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3510,7 +3489,7 @@
   <dimension ref="A1:V89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:A50"/>
+      <selection activeCell="B50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6915,22 +6894,22 @@
     <row r="45" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="54"/>
       <c r="B45" s="18" t="s">
-        <v>238</v>
+        <v>60</v>
       </c>
       <c r="C45" s="7">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D45" s="7">
-        <v>45</v>
-      </c>
-      <c r="E45" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>76</v>
+        <v>44</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="G45" s="29" t="s">
-        <v>239</v>
+        <v>163</v>
       </c>
       <c r="H45" s="29" t="s">
         <v>216</v>
@@ -6993,22 +6972,22 @@
     <row r="46" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="54"/>
       <c r="B46" s="18" t="s">
-        <v>108</v>
+        <v>238</v>
       </c>
       <c r="C46" s="7">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" s="7">
-        <v>46</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>70</v>
+        <v>45</v>
+      </c>
+      <c r="E46" s="33" t="s">
+        <v>75</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>119</v>
+        <v>76</v>
+      </c>
+      <c r="G46" s="29" t="s">
+        <v>239</v>
       </c>
       <c r="H46" s="29" t="s">
         <v>216</v>
@@ -7068,25 +7047,25 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="54"/>
       <c r="B47" s="18" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C47" s="7">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47" s="7">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G47" s="29" t="s">
-        <v>139</v>
+        <v>70</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="H47" s="29" t="s">
         <v>216</v>
@@ -7097,7 +7076,7 @@
       <c r="J47" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K47" s="11">
+      <c r="K47" s="25">
         <f>$I47+Sheet2!B$1/24</f>
         <v>1.2916666666666667</v>
       </c>
@@ -7149,97 +7128,97 @@
     <row r="48" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="54"/>
       <c r="B48" s="18" t="s">
-        <v>217</v>
+        <v>97</v>
       </c>
       <c r="C48" s="7">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D48" s="7">
-        <v>48</v>
-      </c>
-      <c r="E48" s="20"/>
-      <c r="F48" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="G48" s="29"/>
+        <v>47</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48" s="29" t="s">
+        <v>139</v>
+      </c>
       <c r="H48" s="29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I48" s="23">
-        <v>0.91666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="J48" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K48" s="25">
+      <c r="K48" s="11">
         <f>$I48+Sheet2!B$1/24</f>
-        <v>1.3333333333333333</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="L48" s="23">
         <f>$I48+Sheet2!B$2/24</f>
-        <v>1.2916666666666665</v>
+        <v>1.25</v>
       </c>
       <c r="M48" s="23">
         <f>$I48+Sheet2!B$3/24</f>
-        <v>1.25</v>
+        <v>1.2083333333333333</v>
       </c>
       <c r="N48" s="23">
         <f>$I48+Sheet2!B$4/24</f>
-        <v>1.0416666666666665</v>
+        <v>1</v>
       </c>
       <c r="O48" s="23">
         <f>$I48+Sheet2!B$5/24</f>
-        <v>1.0416666666666665</v>
+        <v>1</v>
       </c>
       <c r="P48" s="23">
         <f>$I48+Sheet2!B$6/24</f>
-        <v>1.0416666666666665</v>
+        <v>1</v>
       </c>
       <c r="Q48" s="23">
         <f>$I48+Sheet2!B$7/24</f>
-        <v>1</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="R48" s="23">
         <f>$I48+Sheet2!B$8/24</f>
-        <v>0.95833333333333326</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="S48" s="23">
         <f>$I48+Sheet2!B$9/24</f>
-        <v>0.75</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="T48" s="23">
         <f>$I48+Sheet2!B$10/24</f>
-        <v>0.70833333333333326</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="U48" s="23">
         <f>$I48+Sheet2!B$11/24</f>
-        <v>0.66666666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="V48" s="23">
         <f>$I48+Sheet2!B$12/24</f>
-        <v>0.625</v>
+        <v>0.58333333333333326</v>
       </c>
     </row>
     <row r="49" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="54"/>
       <c r="B49" s="18" t="s">
-        <v>60</v>
+        <v>217</v>
       </c>
       <c r="C49" s="7">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D49" s="7">
-        <v>44</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F49" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G49" s="29" t="s">
-        <v>163</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E49" s="20"/>
+      <c r="F49" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G49" s="29"/>
       <c r="H49" s="29" t="s">
         <v>218</v>
       </c>
@@ -10388,11 +10367,11 @@
     <sortCondition ref="D2:D72"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
+      <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
-      <selection sqref="A1:XFD1048576"/>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -10400,1392 +10379,1387 @@
     <mergeCell ref="A25:A50"/>
     <mergeCell ref="A51:A88"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V48 K50:V89">
-    <cfRule type="expression" dxfId="279" priority="668">
+  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V44 K46:V89">
+    <cfRule type="expression" dxfId="276" priority="671">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K17:V17 K19:V19 K23:V23 K20 K24:K32 K22">
-    <cfRule type="expression" dxfId="278" priority="670">
+    <cfRule type="expression" dxfId="275" priority="673">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K53:V53 G53 G64 G73 G89 E62:G62 G30 B74 E74:G74 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 B70:B72 E70:G72 L40:V40 K87:V87 G87 K79:V80 K83:V84 K89:V89 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B84 J11:V14 J84:V84 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L76:V76 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E84:G84 E61:V61 E65:G65 B50:B62 B40 B81 B47 J47:V47 G75:G80 E24:G29 B20:B38 E5:G5 E47:H47 E81:G81 E76:G77 L24:V32 L20:V20 L22:V22 G66:G69 E44:H44 L64:V74 B65:B67 B76:B77 G58:V60 C50:D89 B44:B45 E45:G45 C4:D48">
-    <cfRule type="expression" dxfId="277" priority="674">
+  <conditionalFormatting sqref="K53:V53 G53 G64 G73 G89 E62:G62 G30 B74 E74:G74 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 B70:B72 E70:G72 L40:V40 K87:V87 G87 K79:V80 K83:V84 K89:V89 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B84 J11:V14 J84:V84 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L76:V76 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E84:G84 E61:V61 E65:G65 B50:B62 B40 B81 B48 J48:V48 G75:G80 E24:G29 B20:B38 E5:G5 E48:H48 E81:G81 E76:G77 L24:V32 L20:V20 L22:V22 G66:G69 E44:H44 L64:V74 B65:B67 B76:B77 G58:V60 B44:B46 C4:D89 E45:G46">
+    <cfRule type="expression" dxfId="274" priority="677">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64 L64:V64">
-    <cfRule type="expression" dxfId="276" priority="651">
+    <cfRule type="expression" dxfId="273" priority="654">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69 L69:V69">
-    <cfRule type="expression" dxfId="275" priority="647">
+    <cfRule type="expression" dxfId="272" priority="650">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73 L73:V73">
-    <cfRule type="expression" dxfId="274" priority="645">
+    <cfRule type="expression" dxfId="271" priority="648">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68 L68:V68">
-    <cfRule type="expression" dxfId="273" priority="643">
+    <cfRule type="expression" dxfId="270" priority="646">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87 K87:V87 E87:F87">
-    <cfRule type="expression" dxfId="272" priority="639">
+    <cfRule type="expression" dxfId="269" priority="642">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" dxfId="271" priority="637">
+    <cfRule type="expression" dxfId="268" priority="640">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E73">
-    <cfRule type="expression" dxfId="270" priority="634">
+    <cfRule type="expression" dxfId="267" priority="637">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="expression" dxfId="269" priority="633">
+    <cfRule type="expression" dxfId="266" priority="636">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:B84 J83:V84">
-    <cfRule type="expression" dxfId="268" priority="630">
+    <cfRule type="expression" dxfId="265" priority="633">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:B81 J80:V80 E80:E81">
-    <cfRule type="expression" dxfId="267" priority="628">
+    <cfRule type="expression" dxfId="264" priority="631">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E83:F84">
-    <cfRule type="expression" dxfId="266" priority="626">
+    <cfRule type="expression" dxfId="263" priority="629">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79 J79:V79">
-    <cfRule type="expression" dxfId="265" priority="624">
+    <cfRule type="expression" dxfId="262" priority="627">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89 J89:V89 E89">
-    <cfRule type="expression" dxfId="264" priority="622">
+    <cfRule type="expression" dxfId="261" priority="625">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F68">
-    <cfRule type="expression" dxfId="263" priority="614">
+    <cfRule type="expression" dxfId="260" priority="617">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62:V62">
-    <cfRule type="expression" dxfId="262" priority="554">
+    <cfRule type="expression" dxfId="259" priority="557">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F73">
-    <cfRule type="expression" dxfId="261" priority="576">
+    <cfRule type="expression" dxfId="258" priority="579">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75:B77 E75:F77">
-    <cfRule type="expression" dxfId="260" priority="540">
+    <cfRule type="expression" dxfId="257" priority="543">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="259" priority="561">
+    <cfRule type="expression" dxfId="256" priority="564">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63 L63:V63">
-    <cfRule type="expression" dxfId="258" priority="562">
+    <cfRule type="expression" dxfId="255" priority="565">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F80:F81">
-    <cfRule type="expression" dxfId="257" priority="574">
+    <cfRule type="expression" dxfId="254" priority="577">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64">
-    <cfRule type="expression" dxfId="256" priority="570">
+    <cfRule type="expression" dxfId="253" priority="573">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69:F69">
-    <cfRule type="expression" dxfId="255" priority="569">
+    <cfRule type="expression" dxfId="252" priority="572">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E79:F79">
-    <cfRule type="expression" dxfId="254" priority="567">
+    <cfRule type="expression" dxfId="251" priority="570">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63:V63 G63">
-    <cfRule type="expression" dxfId="253" priority="564">
+    <cfRule type="expression" dxfId="250" priority="567">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:V7">
-    <cfRule type="expression" dxfId="252" priority="509">
+    <cfRule type="expression" dxfId="249" priority="512">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F63">
-    <cfRule type="expression" dxfId="251" priority="558">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K47:V47">
-    <cfRule type="expression" dxfId="250" priority="678">
+    <cfRule type="expression" dxfId="248" priority="561">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K48:V48">
+    <cfRule type="expression" dxfId="247" priority="681">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62:V62">
-    <cfRule type="expression" dxfId="249" priority="555">
+    <cfRule type="expression" dxfId="246" priority="558">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:V10">
-    <cfRule type="expression" dxfId="248" priority="500">
+    <cfRule type="expression" dxfId="245" priority="503">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H14 J13:V14 L18:V18">
-    <cfRule type="expression" dxfId="247" priority="546">
+    <cfRule type="expression" dxfId="244" priority="549">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:V14 L18:V18">
-    <cfRule type="expression" dxfId="246" priority="547">
+    <cfRule type="expression" dxfId="243" priority="550">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:G3 B7 E7:G7">
-    <cfRule type="expression" dxfId="245" priority="541">
+    <cfRule type="expression" dxfId="242" priority="544">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K75:V75 L76:V76">
-    <cfRule type="expression" dxfId="244" priority="539">
+    <cfRule type="expression" dxfId="241" priority="542">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J75:V75 L76:V76">
-    <cfRule type="expression" dxfId="243" priority="537">
+    <cfRule type="expression" dxfId="240" priority="540">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75">
-    <cfRule type="expression" dxfId="242" priority="536">
+    <cfRule type="expression" dxfId="239" priority="539">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J78:V78">
-    <cfRule type="expression" dxfId="241" priority="531">
+    <cfRule type="expression" dxfId="238" priority="534">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78 E78:F78">
-    <cfRule type="expression" dxfId="240" priority="534">
+    <cfRule type="expression" dxfId="237" priority="537">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K78:V78">
-    <cfRule type="expression" dxfId="239" priority="533">
+    <cfRule type="expression" dxfId="236" priority="536">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78">
-    <cfRule type="expression" dxfId="238" priority="530">
+    <cfRule type="expression" dxfId="235" priority="533">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="237" priority="523">
+    <cfRule type="expression" dxfId="234" priority="526">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:F30">
-    <cfRule type="expression" dxfId="236" priority="528">
+    <cfRule type="expression" dxfId="233" priority="531">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43 E43 L43:V43 G43">
-    <cfRule type="expression" dxfId="235" priority="527">
+    <cfRule type="expression" dxfId="232" priority="530">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4 E4:G4">
-    <cfRule type="expression" dxfId="234" priority="522">
+    <cfRule type="expression" dxfId="231" priority="525">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="233" priority="521">
+    <cfRule type="expression" dxfId="230" priority="524">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 E6:H6 J6:V6">
-    <cfRule type="expression" dxfId="232" priority="519">
+    <cfRule type="expression" dxfId="229" priority="522">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:V5">
-    <cfRule type="expression" dxfId="231" priority="516">
+    <cfRule type="expression" dxfId="228" priority="519">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:L4">
-    <cfRule type="expression" dxfId="230" priority="511">
+    <cfRule type="expression" dxfId="227" priority="514">
       <formula>K$1=$H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:V4">
-    <cfRule type="expression" dxfId="229" priority="512">
+    <cfRule type="expression" dxfId="226" priority="515">
       <formula>K$1=$I4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:V4">
-    <cfRule type="expression" dxfId="228" priority="513">
+    <cfRule type="expression" dxfId="225" priority="516">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="227" priority="506">
+    <cfRule type="expression" dxfId="224" priority="509">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 E8:G10">
-    <cfRule type="expression" dxfId="226" priority="505">
+    <cfRule type="expression" dxfId="223" priority="508">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:K8">
-    <cfRule type="expression" dxfId="225" priority="503">
+    <cfRule type="expression" dxfId="222" priority="506">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:H15 J15:V15">
-    <cfRule type="expression" dxfId="224" priority="495">
+    <cfRule type="expression" dxfId="221" priority="498">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15 J15:V15">
-    <cfRule type="expression" dxfId="223" priority="492">
+    <cfRule type="expression" dxfId="220" priority="495">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:V15">
-    <cfRule type="expression" dxfId="222" priority="493">
+    <cfRule type="expression" dxfId="219" priority="496">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:G15">
-    <cfRule type="expression" dxfId="221" priority="491">
+    <cfRule type="expression" dxfId="218" priority="494">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="220" priority="488">
+    <cfRule type="expression" dxfId="217" priority="491">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="219" priority="485">
+    <cfRule type="expression" dxfId="216" priority="488">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="218" priority="486">
+    <cfRule type="expression" dxfId="215" priority="489">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48 J48:V48">
-    <cfRule type="expression" dxfId="217" priority="380">
+  <conditionalFormatting sqref="H49 J49:V49">
+    <cfRule type="expression" dxfId="214" priority="383">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19 E19:H19 J19:V19">
-    <cfRule type="expression" dxfId="216" priority="481">
+    <cfRule type="expression" dxfId="213" priority="484">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="215" priority="337">
+    <cfRule type="expression" dxfId="212" priority="340">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27 J27:K27">
-    <cfRule type="expression" dxfId="214" priority="443">
+    <cfRule type="expression" dxfId="211" priority="446">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62:J62">
-    <cfRule type="expression" dxfId="213" priority="375">
+    <cfRule type="expression" dxfId="210" priority="378">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20 J20:K20">
-    <cfRule type="expression" dxfId="212" priority="470">
+    <cfRule type="expression" dxfId="209" priority="473">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22 J22:K22">
-    <cfRule type="expression" dxfId="211" priority="465">
+    <cfRule type="expression" dxfId="208" priority="468">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="210" priority="370">
+    <cfRule type="expression" dxfId="207" priority="373">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="209" priority="369">
+    <cfRule type="expression" dxfId="206" priority="372">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24 J24:K24">
-    <cfRule type="expression" dxfId="208" priority="458">
+    <cfRule type="expression" dxfId="205" priority="461">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="207" priority="366">
+    <cfRule type="expression" dxfId="204" priority="369">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25 J25:K25">
-    <cfRule type="expression" dxfId="206" priority="453">
+    <cfRule type="expression" dxfId="203" priority="456">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64 J64">
-    <cfRule type="expression" dxfId="205" priority="364">
+    <cfRule type="expression" dxfId="202" priority="367">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26 J26:K26">
-    <cfRule type="expression" dxfId="204" priority="448">
+    <cfRule type="expression" dxfId="201" priority="451">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="203" priority="361">
+    <cfRule type="expression" dxfId="200" priority="364">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65 J65">
-    <cfRule type="expression" dxfId="202" priority="360">
+    <cfRule type="expression" dxfId="199" priority="363">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="201" priority="358">
+    <cfRule type="expression" dxfId="198" priority="361">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="200" priority="357">
+    <cfRule type="expression" dxfId="197" priority="360">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28 J28:K28">
-    <cfRule type="expression" dxfId="199" priority="438">
+    <cfRule type="expression" dxfId="196" priority="441">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="198" priority="354">
+    <cfRule type="expression" dxfId="195" priority="357">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29 J29:K29">
-    <cfRule type="expression" dxfId="197" priority="433">
+    <cfRule type="expression" dxfId="194" priority="436">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="196" priority="352">
+    <cfRule type="expression" dxfId="193" priority="355">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30 J30:K30">
-    <cfRule type="expression" dxfId="195" priority="428">
+    <cfRule type="expression" dxfId="192" priority="431">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31 J31:K31">
-    <cfRule type="expression" dxfId="194" priority="423">
+    <cfRule type="expression" dxfId="191" priority="426">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="193" priority="346">
+    <cfRule type="expression" dxfId="190" priority="349">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="192" priority="345">
+    <cfRule type="expression" dxfId="189" priority="348">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32 J32:K32">
-    <cfRule type="expression" dxfId="191" priority="418">
+    <cfRule type="expression" dxfId="188" priority="421">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="190" priority="342">
+    <cfRule type="expression" dxfId="187" priority="345">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69 J69">
-    <cfRule type="expression" dxfId="189" priority="340">
+    <cfRule type="expression" dxfId="186" priority="343">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="188" priority="406">
+    <cfRule type="expression" dxfId="185" priority="409">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="187" priority="338">
+    <cfRule type="expression" dxfId="184" priority="341">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="186" priority="403">
+    <cfRule type="expression" dxfId="183" priority="406">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="185" priority="400">
+    <cfRule type="expression" dxfId="182" priority="403">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70 J70">
-    <cfRule type="expression" dxfId="184" priority="336">
+    <cfRule type="expression" dxfId="181" priority="339">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="183" priority="397">
+    <cfRule type="expression" dxfId="180" priority="400">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:B40 J39:V39 E39:H39 E40:G40 L40:V40">
-    <cfRule type="expression" dxfId="182" priority="394">
+    <cfRule type="expression" dxfId="179" priority="397">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:V41 B41:B43 E43 E41:H41 G43 E42:G42 L42:V43">
-    <cfRule type="expression" dxfId="181" priority="390">
+    <cfRule type="expression" dxfId="178" priority="393">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="180" priority="334">
+    <cfRule type="expression" dxfId="177" priority="337">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="179" priority="333">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E48:G48 B48">
-    <cfRule type="expression" dxfId="178" priority="383">
+    <cfRule type="expression" dxfId="176" priority="336">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49:G49 B49">
+    <cfRule type="expression" dxfId="175" priority="386">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I82">
-    <cfRule type="expression" dxfId="177" priority="240">
+    <cfRule type="expression" dxfId="174" priority="243">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="176" priority="379">
+    <cfRule type="expression" dxfId="173" priority="382">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53 J53">
-    <cfRule type="expression" dxfId="175" priority="378">
+    <cfRule type="expression" dxfId="172" priority="381">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="174" priority="326">
+    <cfRule type="expression" dxfId="171" priority="329">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="173" priority="329">
+    <cfRule type="expression" dxfId="170" priority="332">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72 J72">
-    <cfRule type="expression" dxfId="172" priority="332">
+    <cfRule type="expression" dxfId="169" priority="335">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63 J63">
-    <cfRule type="expression" dxfId="171" priority="368">
+    <cfRule type="expression" dxfId="168" priority="371">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="170" priority="365">
+    <cfRule type="expression" dxfId="167" priority="368">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="169" priority="362">
+    <cfRule type="expression" dxfId="166" priority="365">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66 J66">
-    <cfRule type="expression" dxfId="168" priority="356">
+    <cfRule type="expression" dxfId="165" priority="359">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="167" priority="353">
+    <cfRule type="expression" dxfId="164" priority="356">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68 J68">
-    <cfRule type="expression" dxfId="166" priority="344">
+    <cfRule type="expression" dxfId="163" priority="347">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="165" priority="341">
+    <cfRule type="expression" dxfId="162" priority="344">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="164" priority="330">
+    <cfRule type="expression" dxfId="161" priority="333">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73 J73">
-    <cfRule type="expression" dxfId="163" priority="328">
+    <cfRule type="expression" dxfId="160" priority="331">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="162" priority="325">
+    <cfRule type="expression" dxfId="159" priority="328">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74 J74">
-    <cfRule type="expression" dxfId="161" priority="324">
+    <cfRule type="expression" dxfId="158" priority="327">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="160" priority="322">
+    <cfRule type="expression" dxfId="157" priority="325">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="159" priority="321">
+    <cfRule type="expression" dxfId="156" priority="324">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71 J71">
-    <cfRule type="expression" dxfId="158" priority="320">
+    <cfRule type="expression" dxfId="155" priority="323">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82">
-    <cfRule type="expression" dxfId="157" priority="315">
+    <cfRule type="expression" dxfId="154" priority="318">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J82:V82">
-    <cfRule type="expression" dxfId="156" priority="310">
+    <cfRule type="expression" dxfId="153" priority="313">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82 E82:F82">
-    <cfRule type="expression" dxfId="155" priority="312">
+    <cfRule type="expression" dxfId="152" priority="315">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K82:V82">
-    <cfRule type="expression" dxfId="154" priority="311">
+    <cfRule type="expression" dxfId="151" priority="314">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="expression" dxfId="153" priority="309">
+    <cfRule type="expression" dxfId="150" priority="312">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79">
-    <cfRule type="expression" dxfId="152" priority="306">
+    <cfRule type="expression" dxfId="149" priority="309">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80">
-    <cfRule type="expression" dxfId="151" priority="304">
+    <cfRule type="expression" dxfId="148" priority="307">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G85">
-    <cfRule type="expression" dxfId="150" priority="301">
+    <cfRule type="expression" dxfId="147" priority="304">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="149" priority="158">
+    <cfRule type="expression" dxfId="146" priority="161">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J85:V85">
-    <cfRule type="expression" dxfId="148" priority="296">
+    <cfRule type="expression" dxfId="145" priority="299">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85 E85:F85">
-    <cfRule type="expression" dxfId="147" priority="298">
+    <cfRule type="expression" dxfId="144" priority="301">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K85:V85">
-    <cfRule type="expression" dxfId="146" priority="297">
+    <cfRule type="expression" dxfId="143" priority="300">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="expression" dxfId="145" priority="295">
+    <cfRule type="expression" dxfId="142" priority="298">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="expression" dxfId="144" priority="293">
+    <cfRule type="expression" dxfId="141" priority="296">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G86">
-    <cfRule type="expression" dxfId="143" priority="291">
+    <cfRule type="expression" dxfId="140" priority="294">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="142" priority="148">
+    <cfRule type="expression" dxfId="139" priority="151">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J86:V86">
-    <cfRule type="expression" dxfId="141" priority="286">
+    <cfRule type="expression" dxfId="138" priority="289">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86 E86:F86">
-    <cfRule type="expression" dxfId="140" priority="288">
+    <cfRule type="expression" dxfId="137" priority="291">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K86:V86">
-    <cfRule type="expression" dxfId="139" priority="287">
+    <cfRule type="expression" dxfId="136" priority="290">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="expression" dxfId="138" priority="285">
+    <cfRule type="expression" dxfId="135" priority="288">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87">
-    <cfRule type="expression" dxfId="137" priority="283">
+    <cfRule type="expression" dxfId="134" priority="286">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87">
-    <cfRule type="expression" dxfId="136" priority="282">
+    <cfRule type="expression" dxfId="133" priority="285">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88">
-    <cfRule type="expression" dxfId="135" priority="280">
+    <cfRule type="expression" dxfId="132" priority="283">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="134" priority="137">
+    <cfRule type="expression" dxfId="131" priority="140">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J88:V88">
-    <cfRule type="expression" dxfId="133" priority="275">
+    <cfRule type="expression" dxfId="130" priority="278">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88 E88:F88">
-    <cfRule type="expression" dxfId="132" priority="277">
+    <cfRule type="expression" dxfId="129" priority="280">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88:V88">
-    <cfRule type="expression" dxfId="131" priority="276">
+    <cfRule type="expression" dxfId="128" priority="279">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88">
-    <cfRule type="expression" dxfId="130" priority="274">
+    <cfRule type="expression" dxfId="127" priority="277">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43">
-    <cfRule type="expression" dxfId="129" priority="272">
+    <cfRule type="expression" dxfId="126" priority="275">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43 J43">
-    <cfRule type="expression" dxfId="128" priority="270">
+    <cfRule type="expression" dxfId="125" priority="273">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:K38">
-    <cfRule type="expression" dxfId="127" priority="267">
+    <cfRule type="expression" dxfId="124" priority="270">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="126" priority="265">
+    <cfRule type="expression" dxfId="123" priority="268">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I49">
+    <cfRule type="expression" dxfId="122" priority="126">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I53">
+    <cfRule type="expression" dxfId="121" priority="264">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I67">
+    <cfRule type="expression" dxfId="120" priority="257">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I63">
+    <cfRule type="expression" dxfId="119" priority="261">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I64">
+    <cfRule type="expression" dxfId="118" priority="260">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I65">
+    <cfRule type="expression" dxfId="117" priority="259">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I66">
+    <cfRule type="expression" dxfId="116" priority="258">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I68">
+    <cfRule type="expression" dxfId="115" priority="255">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I69">
+    <cfRule type="expression" dxfId="114" priority="254">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I70">
+    <cfRule type="expression" dxfId="113" priority="253">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I71">
+    <cfRule type="expression" dxfId="112" priority="252">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I72">
+    <cfRule type="expression" dxfId="111" priority="251">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I73">
+    <cfRule type="expression" dxfId="110" priority="250">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I74">
+    <cfRule type="expression" dxfId="109" priority="249">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I75">
+    <cfRule type="expression" dxfId="108" priority="248">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I78">
+    <cfRule type="expression" dxfId="107" priority="246">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I79">
+    <cfRule type="expression" dxfId="106" priority="245">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I80">
+    <cfRule type="expression" dxfId="105" priority="244">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I83">
+    <cfRule type="expression" dxfId="104" priority="242">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I85">
+    <cfRule type="expression" dxfId="103" priority="241">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I86">
+    <cfRule type="expression" dxfId="102" priority="240">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I87">
+    <cfRule type="expression" dxfId="101" priority="239">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I88">
+    <cfRule type="expression" dxfId="100" priority="238">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I89">
+    <cfRule type="expression" dxfId="99" priority="237">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H89">
+    <cfRule type="expression" dxfId="98" priority="236">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="expression" dxfId="97" priority="235">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="expression" dxfId="96" priority="234">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="expression" dxfId="95" priority="233">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="expression" dxfId="94" priority="232">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="expression" dxfId="93" priority="231">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="expression" dxfId="92" priority="230">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="expression" dxfId="91" priority="229">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="expression" dxfId="90" priority="228">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="expression" dxfId="89" priority="160">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="expression" dxfId="88" priority="159">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="expression" dxfId="87" priority="158">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="expression" dxfId="86" priority="157">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="expression" dxfId="85" priority="156">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="expression" dxfId="84" priority="150">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="expression" dxfId="83" priority="154">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="expression" dxfId="82" priority="153">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
+    <cfRule type="expression" dxfId="81" priority="152">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="expression" dxfId="80" priority="149">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="expression" dxfId="79" priority="148">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="expression" dxfId="78" priority="147">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="expression" dxfId="77" priority="146">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="expression" dxfId="76" priority="145">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30">
+    <cfRule type="expression" dxfId="75" priority="144">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="expression" dxfId="74" priority="143">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="expression" dxfId="73" priority="142">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
+    <cfRule type="expression" dxfId="72" priority="139">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50">
+    <cfRule type="expression" dxfId="71" priority="125">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
+    <cfRule type="expression" dxfId="70" priority="137">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="expression" dxfId="69" priority="136">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="expression" dxfId="68" priority="135">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38">
+    <cfRule type="expression" dxfId="67" priority="134">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="expression" dxfId="66" priority="133">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
+    <cfRule type="expression" dxfId="65" priority="132">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43">
+    <cfRule type="expression" dxfId="64" priority="131">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="expression" dxfId="63" priority="129">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="125" priority="123">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I53">
-    <cfRule type="expression" dxfId="124" priority="261">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I67">
-    <cfRule type="expression" dxfId="123" priority="254">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="122" priority="258">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I64">
-    <cfRule type="expression" dxfId="121" priority="257">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
-    <cfRule type="expression" dxfId="120" priority="256">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I66">
-    <cfRule type="expression" dxfId="119" priority="255">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I68">
-    <cfRule type="expression" dxfId="118" priority="252">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="117" priority="251">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="116" priority="250">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I71">
-    <cfRule type="expression" dxfId="115" priority="249">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I72">
-    <cfRule type="expression" dxfId="114" priority="248">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I73">
-    <cfRule type="expression" dxfId="113" priority="247">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I74">
-    <cfRule type="expression" dxfId="112" priority="246">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I75">
-    <cfRule type="expression" dxfId="111" priority="245">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I78">
-    <cfRule type="expression" dxfId="110" priority="243">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I79">
-    <cfRule type="expression" dxfId="109" priority="242">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I80">
-    <cfRule type="expression" dxfId="108" priority="241">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I83">
-    <cfRule type="expression" dxfId="107" priority="239">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I85">
-    <cfRule type="expression" dxfId="106" priority="238">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I86">
-    <cfRule type="expression" dxfId="105" priority="237">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I87">
-    <cfRule type="expression" dxfId="104" priority="236">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I88">
-    <cfRule type="expression" dxfId="103" priority="235">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I89">
-    <cfRule type="expression" dxfId="102" priority="234">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H89">
-    <cfRule type="expression" dxfId="101" priority="233">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="100" priority="232">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="99" priority="231">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="expression" dxfId="98" priority="230">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="97" priority="229">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="96" priority="228">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="95" priority="227">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="94" priority="226">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="93" priority="225">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="92" priority="157">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="expression" dxfId="91" priority="156">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="expression" dxfId="90" priority="155">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="89" priority="154">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="88" priority="153">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="87" priority="147">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
-    <cfRule type="expression" dxfId="86" priority="151">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="expression" dxfId="85" priority="150">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="84" priority="149">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="expression" dxfId="83" priority="146">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
-    <cfRule type="expression" dxfId="82" priority="145">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
-    <cfRule type="expression" dxfId="81" priority="144">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="80" priority="143">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="79" priority="142">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="expression" dxfId="78" priority="141">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="expression" dxfId="77" priority="140">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="76" priority="139">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="75" priority="136">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I50">
-    <cfRule type="expression" dxfId="74" priority="122">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="expression" dxfId="73" priority="134">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
-    <cfRule type="expression" dxfId="72" priority="133">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="expression" dxfId="71" priority="132">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="70" priority="131">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="expression" dxfId="69" priority="130">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
-    <cfRule type="expression" dxfId="68" priority="129">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="67" priority="128">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="66" priority="126">
+    <cfRule type="expression" dxfId="62" priority="127">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:V10">
+    <cfRule type="expression" dxfId="61" priority="117">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="expression" dxfId="60" priority="106">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H84">
+    <cfRule type="expression" dxfId="59" priority="115">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I84">
+    <cfRule type="expression" dxfId="58" priority="114">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:K9">
+    <cfRule type="expression" dxfId="57" priority="105">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="expression" dxfId="56" priority="104">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="55" priority="107">
+      <formula>K$1=$H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="54" priority="108">
+      <formula>K$1=$I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="53" priority="102">
+      <formula>K$1=$H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="52" priority="103">
+      <formula>K$1=$I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="expression" dxfId="51" priority="101">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:K10">
+    <cfRule type="expression" dxfId="50" priority="100">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="expression" dxfId="49" priority="99">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43">
+    <cfRule type="expression" dxfId="48" priority="92">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42:K42 H42">
+    <cfRule type="expression" dxfId="47" priority="87">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I42">
+    <cfRule type="expression" dxfId="46" priority="86">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="45" priority="77">
+      <formula>K$1=$H18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="44" priority="78">
+      <formula>K$1=$I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18 J18:K18">
+    <cfRule type="expression" dxfId="43" priority="79">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="expression" dxfId="42" priority="76">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K76">
+    <cfRule type="expression" dxfId="41" priority="74">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J76:K76">
+    <cfRule type="expression" dxfId="40" priority="73">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H76">
+    <cfRule type="expression" dxfId="39" priority="72">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I76">
+    <cfRule type="expression" dxfId="38" priority="71">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40:K40 H40">
+    <cfRule type="expression" dxfId="37" priority="69">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="expression" dxfId="36" priority="68">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J81">
+    <cfRule type="expression" dxfId="35" priority="59">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H81">
+    <cfRule type="expression" dxfId="34" priority="58">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I81">
+    <cfRule type="expression" dxfId="33" priority="57">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81:V81">
+    <cfRule type="expression" dxfId="32" priority="56">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81:V81">
+    <cfRule type="expression" dxfId="31" priority="54">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47 G47">
+    <cfRule type="expression" dxfId="30" priority="52">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47:F47">
+    <cfRule type="expression" dxfId="29" priority="51">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47 E47 G47">
+    <cfRule type="expression" dxfId="28" priority="50">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47 E47 G47">
+    <cfRule type="expression" dxfId="27" priority="49">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47">
+    <cfRule type="expression" dxfId="26" priority="48">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J47:V47 H47">
+    <cfRule type="expression" dxfId="25" priority="47">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="65" priority="124">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L9:V10">
-    <cfRule type="expression" dxfId="64" priority="114">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="63" priority="103">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H84">
-    <cfRule type="expression" dxfId="62" priority="112">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I84">
-    <cfRule type="expression" dxfId="61" priority="111">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:K9">
-    <cfRule type="expression" dxfId="60" priority="102">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="59" priority="101">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="58" priority="104">
-      <formula>K$1=$H9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="57" priority="105">
-      <formula>K$1=$I9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="56" priority="99">
-      <formula>K$1=$H10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="55" priority="100">
-      <formula>K$1=$I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="54" priority="98">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
-    <cfRule type="expression" dxfId="53" priority="97">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="52" priority="96">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="51" priority="89">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J42:K42 H42">
-    <cfRule type="expression" dxfId="50" priority="84">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="49" priority="83">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="48" priority="74">
-      <formula>K$1=$H18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="47" priority="75">
-      <formula>K$1=$I18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18 J18:K18">
-    <cfRule type="expression" dxfId="46" priority="76">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="45" priority="73">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K76">
-    <cfRule type="expression" dxfId="44" priority="71">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J76:K76">
-    <cfRule type="expression" dxfId="43" priority="70">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H76">
-    <cfRule type="expression" dxfId="42" priority="69">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="expression" dxfId="41" priority="68">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J40:K40 H40">
-    <cfRule type="expression" dxfId="40" priority="66">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="39" priority="65">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J81">
-    <cfRule type="expression" dxfId="38" priority="56">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H81">
-    <cfRule type="expression" dxfId="37" priority="55">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I81">
-    <cfRule type="expression" dxfId="36" priority="54">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="35" priority="53">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="34" priority="51">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46 G46">
-    <cfRule type="expression" dxfId="33" priority="49">
+    <cfRule type="expression" dxfId="24" priority="45">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21 E21:G21">
+    <cfRule type="expression" dxfId="23" priority="44">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46:F46">
-    <cfRule type="expression" dxfId="32" priority="48">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46 E46 G46">
-    <cfRule type="expression" dxfId="31" priority="47">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46 E46 G46">
-    <cfRule type="expression" dxfId="30" priority="46">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46">
-    <cfRule type="expression" dxfId="29" priority="45">
+    <cfRule type="expression" dxfId="22" priority="40">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J46:V46 H46">
-    <cfRule type="expression" dxfId="28" priority="44">
+    <cfRule type="expression" dxfId="21" priority="39">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="27" priority="42">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21 E21:G21">
-    <cfRule type="expression" dxfId="26" priority="41">
+    <cfRule type="expression" dxfId="20" priority="37">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:V21">
+    <cfRule type="expression" dxfId="19" priority="34">
+      <formula>K$1=$H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="expression" dxfId="18" priority="35">
+      <formula>K$1=$I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L21:V21">
+    <cfRule type="expression" dxfId="17" priority="36">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21 J21:K21">
+    <cfRule type="expression" dxfId="16" priority="33">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="expression" dxfId="15" priority="32">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F60">
+    <cfRule type="expression" dxfId="14" priority="31">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G77">
+    <cfRule type="expression" dxfId="13" priority="27">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K77">
+    <cfRule type="expression" dxfId="12" priority="17">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J77:K77">
+    <cfRule type="expression" dxfId="11" priority="16">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H77">
+    <cfRule type="expression" dxfId="10" priority="15">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I77">
+    <cfRule type="expression" dxfId="9" priority="14">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L77:V77">
+    <cfRule type="expression" dxfId="8" priority="21">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L77:V77">
+    <cfRule type="expression" dxfId="7" priority="19">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L77:V77">
+    <cfRule type="expression" dxfId="6" priority="18">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45:G45">
+    <cfRule type="expression" dxfId="5" priority="13">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45:F45">
-    <cfRule type="expression" dxfId="25" priority="37">
-      <formula>MOD(ROW(),2)=1</formula>
+    <cfRule type="expression" dxfId="3" priority="11">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K45:V45">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>K$1=$H45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45:V45 H45">
-    <cfRule type="expression" dxfId="24" priority="36">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45">
-    <cfRule type="expression" dxfId="23" priority="34">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:V21">
-    <cfRule type="expression" dxfId="22" priority="31">
-      <formula>K$1=$H21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="expression" dxfId="21" priority="32">
-      <formula>K$1=$I21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L21:V21">
-    <cfRule type="expression" dxfId="20" priority="33">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21 J21:K21">
-    <cfRule type="expression" dxfId="19" priority="30">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="expression" dxfId="18" priority="29">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F60">
-    <cfRule type="expression" dxfId="17" priority="28">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G77">
-    <cfRule type="expression" dxfId="16" priority="24">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K77">
-    <cfRule type="expression" dxfId="15" priority="14">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J77:K77">
-    <cfRule type="expression" dxfId="14" priority="13">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="13" priority="12">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I77">
-    <cfRule type="expression" dxfId="12" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="11" priority="18">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="10" priority="16">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="9" priority="15">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49:G49">
-    <cfRule type="expression" dxfId="8" priority="10">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49:F49">
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K49:V49">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>K$1=$H49</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J49:V49">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H49">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I49">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Mark JVU420 as enemy
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA78F770-00C3-D440-AB59-DB88034EA68F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D902693-A433-BD4F-9AD0-FF60049A12C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11600" yWindow="2680" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1214,7 +1214,14 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="277">
+  <dxfs count="278">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3488,8 +3495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B50" sqref="A50:XFD50"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9843,8 +9850,8 @@
       <c r="E83" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F83" s="13" t="s">
-        <v>20</v>
+      <c r="F83" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="G83" s="37" t="s">
         <v>173</v>
@@ -10367,11 +10374,11 @@
     <sortCondition ref="D2:D72"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -10380,347 +10387,352 @@
     <mergeCell ref="A51:A88"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V44 K46:V89">
-    <cfRule type="expression" dxfId="276" priority="671">
+    <cfRule type="expression" dxfId="277" priority="672">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K17:V17 K19:V19 K23:V23 K20 K24:K32 K22">
-    <cfRule type="expression" dxfId="275" priority="673">
+    <cfRule type="expression" dxfId="276" priority="674">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K53:V53 G53 G64 G73 G89 E62:G62 G30 B74 E74:G74 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 B70:B72 E70:G72 L40:V40 K87:V87 G87 K79:V80 K83:V84 K89:V89 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B84 J11:V14 J84:V84 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L76:V76 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E84:G84 E61:V61 E65:G65 B50:B62 B40 B81 B48 J48:V48 G75:G80 E24:G29 B20:B38 E5:G5 E48:H48 E81:G81 E76:G77 L24:V32 L20:V20 L22:V22 G66:G69 E44:H44 L64:V74 B65:B67 B76:B77 G58:V60 B44:B46 C4:D89 E45:G46">
-    <cfRule type="expression" dxfId="274" priority="677">
+    <cfRule type="expression" dxfId="275" priority="678">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64 L64:V64">
-    <cfRule type="expression" dxfId="273" priority="654">
+    <cfRule type="expression" dxfId="274" priority="655">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69 L69:V69">
-    <cfRule type="expression" dxfId="272" priority="650">
+    <cfRule type="expression" dxfId="273" priority="651">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73 L73:V73">
-    <cfRule type="expression" dxfId="271" priority="648">
+    <cfRule type="expression" dxfId="272" priority="649">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68 L68:V68">
-    <cfRule type="expression" dxfId="270" priority="646">
+    <cfRule type="expression" dxfId="271" priority="647">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87 K87:V87 E87:F87">
-    <cfRule type="expression" dxfId="269" priority="642">
+    <cfRule type="expression" dxfId="270" priority="643">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" dxfId="268" priority="640">
+    <cfRule type="expression" dxfId="269" priority="641">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E73">
+    <cfRule type="expression" dxfId="268" priority="638">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68">
     <cfRule type="expression" dxfId="267" priority="637">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
-    <cfRule type="expression" dxfId="266" priority="636">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B83:B84 J83:V84">
-    <cfRule type="expression" dxfId="265" priority="633">
+    <cfRule type="expression" dxfId="266" priority="634">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:B81 J80:V80 E80:E81">
-    <cfRule type="expression" dxfId="264" priority="631">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E83:F84">
-    <cfRule type="expression" dxfId="263" priority="629">
+    <cfRule type="expression" dxfId="265" priority="632">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E84:F84 E83">
+    <cfRule type="expression" dxfId="264" priority="630">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79 J79:V79">
-    <cfRule type="expression" dxfId="262" priority="627">
+    <cfRule type="expression" dxfId="263" priority="628">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89 J89:V89 E89">
-    <cfRule type="expression" dxfId="261" priority="625">
+    <cfRule type="expression" dxfId="262" priority="626">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F68">
-    <cfRule type="expression" dxfId="260" priority="617">
+    <cfRule type="expression" dxfId="261" priority="618">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62:V62">
-    <cfRule type="expression" dxfId="259" priority="557">
+    <cfRule type="expression" dxfId="260" priority="558">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F73">
-    <cfRule type="expression" dxfId="258" priority="579">
+    <cfRule type="expression" dxfId="259" priority="580">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75:B77 E75:F77">
-    <cfRule type="expression" dxfId="257" priority="543">
+    <cfRule type="expression" dxfId="258" priority="544">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="256" priority="564">
+    <cfRule type="expression" dxfId="257" priority="565">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63 L63:V63">
-    <cfRule type="expression" dxfId="255" priority="565">
+    <cfRule type="expression" dxfId="256" priority="566">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F80:F81">
-    <cfRule type="expression" dxfId="254" priority="577">
+    <cfRule type="expression" dxfId="255" priority="578">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64">
+    <cfRule type="expression" dxfId="254" priority="574">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69:F69">
     <cfRule type="expression" dxfId="253" priority="573">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69:F69">
-    <cfRule type="expression" dxfId="252" priority="572">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E79:F79">
-    <cfRule type="expression" dxfId="251" priority="570">
+    <cfRule type="expression" dxfId="252" priority="571">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63:V63 G63">
-    <cfRule type="expression" dxfId="250" priority="567">
+    <cfRule type="expression" dxfId="251" priority="568">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:V7">
-    <cfRule type="expression" dxfId="249" priority="512">
+    <cfRule type="expression" dxfId="250" priority="513">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F63">
-    <cfRule type="expression" dxfId="248" priority="561">
+    <cfRule type="expression" dxfId="249" priority="562">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:V48">
-    <cfRule type="expression" dxfId="247" priority="681">
+    <cfRule type="expression" dxfId="248" priority="682">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62:V62">
-    <cfRule type="expression" dxfId="246" priority="558">
+    <cfRule type="expression" dxfId="247" priority="559">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:V10">
-    <cfRule type="expression" dxfId="245" priority="503">
+    <cfRule type="expression" dxfId="246" priority="504">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H14 J13:V14 L18:V18">
-    <cfRule type="expression" dxfId="244" priority="549">
+    <cfRule type="expression" dxfId="245" priority="550">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:V14 L18:V18">
-    <cfRule type="expression" dxfId="243" priority="550">
+    <cfRule type="expression" dxfId="244" priority="551">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:G3 B7 E7:G7">
-    <cfRule type="expression" dxfId="242" priority="544">
+    <cfRule type="expression" dxfId="243" priority="545">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K75:V75 L76:V76">
-    <cfRule type="expression" dxfId="241" priority="542">
+    <cfRule type="expression" dxfId="242" priority="543">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J75:V75 L76:V76">
+    <cfRule type="expression" dxfId="241" priority="541">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H75">
     <cfRule type="expression" dxfId="240" priority="540">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H75">
-    <cfRule type="expression" dxfId="239" priority="539">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J78:V78">
-    <cfRule type="expression" dxfId="238" priority="534">
+    <cfRule type="expression" dxfId="239" priority="535">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78 E78:F78">
+    <cfRule type="expression" dxfId="238" priority="538">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K78:V78">
     <cfRule type="expression" dxfId="237" priority="537">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K78:V78">
-    <cfRule type="expression" dxfId="236" priority="536">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H78">
-    <cfRule type="expression" dxfId="235" priority="533">
+    <cfRule type="expression" dxfId="236" priority="534">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="234" priority="526">
+    <cfRule type="expression" dxfId="235" priority="527">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:F30">
+    <cfRule type="expression" dxfId="234" priority="532">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43 E43 L43:V43 G43">
     <cfRule type="expression" dxfId="233" priority="531">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43 E43 L43:V43 G43">
-    <cfRule type="expression" dxfId="232" priority="530">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B4 E4:G4">
+    <cfRule type="expression" dxfId="232" priority="526">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
     <cfRule type="expression" dxfId="231" priority="525">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="230" priority="524">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B6 E6:H6 J6:V6">
-    <cfRule type="expression" dxfId="229" priority="522">
+    <cfRule type="expression" dxfId="230" priority="523">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:V5">
-    <cfRule type="expression" dxfId="228" priority="519">
+    <cfRule type="expression" dxfId="229" priority="520">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:L4">
-    <cfRule type="expression" dxfId="227" priority="514">
+    <cfRule type="expression" dxfId="228" priority="515">
       <formula>K$1=$H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:V4">
-    <cfRule type="expression" dxfId="226" priority="515">
+    <cfRule type="expression" dxfId="227" priority="516">
       <formula>K$1=$I4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:V4">
-    <cfRule type="expression" dxfId="225" priority="516">
+    <cfRule type="expression" dxfId="226" priority="517">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
+    <cfRule type="expression" dxfId="225" priority="510">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:B10 E8:G10">
     <cfRule type="expression" dxfId="224" priority="509">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B10 E8:G10">
-    <cfRule type="expression" dxfId="223" priority="508">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J8:K8">
-    <cfRule type="expression" dxfId="222" priority="506">
+    <cfRule type="expression" dxfId="223" priority="507">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:H15 J15:V15">
-    <cfRule type="expression" dxfId="221" priority="498">
+    <cfRule type="expression" dxfId="222" priority="499">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15 J15:V15">
-    <cfRule type="expression" dxfId="220" priority="495">
+    <cfRule type="expression" dxfId="221" priority="496">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:V15">
-    <cfRule type="expression" dxfId="219" priority="496">
+    <cfRule type="expression" dxfId="220" priority="497">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:G15">
-    <cfRule type="expression" dxfId="218" priority="494">
+    <cfRule type="expression" dxfId="219" priority="495">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="217" priority="491">
+    <cfRule type="expression" dxfId="218" priority="492">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="216" priority="488">
+    <cfRule type="expression" dxfId="217" priority="489">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="215" priority="489">
+    <cfRule type="expression" dxfId="216" priority="490">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49 J49:V49">
-    <cfRule type="expression" dxfId="214" priority="383">
+    <cfRule type="expression" dxfId="215" priority="384">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19 E19:H19 J19:V19">
-    <cfRule type="expression" dxfId="213" priority="484">
+    <cfRule type="expression" dxfId="214" priority="485">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="212" priority="340">
+    <cfRule type="expression" dxfId="213" priority="341">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27 J27:K27">
-    <cfRule type="expression" dxfId="211" priority="446">
+    <cfRule type="expression" dxfId="212" priority="447">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62:J62">
-    <cfRule type="expression" dxfId="210" priority="378">
+    <cfRule type="expression" dxfId="211" priority="379">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20 J20:K20">
-    <cfRule type="expression" dxfId="209" priority="473">
+    <cfRule type="expression" dxfId="210" priority="474">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22 J22:K22">
-    <cfRule type="expression" dxfId="208" priority="468">
+    <cfRule type="expression" dxfId="209" priority="469">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63">
+    <cfRule type="expression" dxfId="208" priority="374">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10729,43 +10741,43 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="206" priority="372">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H24 J24:K24">
-    <cfRule type="expression" dxfId="205" priority="461">
+    <cfRule type="expression" dxfId="206" priority="462">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="204" priority="369">
+    <cfRule type="expression" dxfId="205" priority="370">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25 J25:K25">
-    <cfRule type="expression" dxfId="203" priority="456">
+    <cfRule type="expression" dxfId="204" priority="457">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64 J64">
-    <cfRule type="expression" dxfId="202" priority="367">
+    <cfRule type="expression" dxfId="203" priority="368">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26 J26:K26">
-    <cfRule type="expression" dxfId="201" priority="451">
+    <cfRule type="expression" dxfId="202" priority="452">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
+    <cfRule type="expression" dxfId="201" priority="365">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H65 J65">
     <cfRule type="expression" dxfId="200" priority="364">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H65 J65">
-    <cfRule type="expression" dxfId="199" priority="363">
+  <conditionalFormatting sqref="K66">
+    <cfRule type="expression" dxfId="199" priority="362">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10774,38 +10786,38 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="197" priority="360">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H28 J28:K28">
-    <cfRule type="expression" dxfId="196" priority="441">
+    <cfRule type="expression" dxfId="197" priority="442">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="195" priority="357">
+    <cfRule type="expression" dxfId="196" priority="358">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29 J29:K29">
-    <cfRule type="expression" dxfId="194" priority="436">
+    <cfRule type="expression" dxfId="195" priority="437">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="193" priority="355">
+    <cfRule type="expression" dxfId="194" priority="356">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30 J30:K30">
-    <cfRule type="expression" dxfId="192" priority="431">
+    <cfRule type="expression" dxfId="193" priority="432">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31 J31:K31">
-    <cfRule type="expression" dxfId="191" priority="426">
+    <cfRule type="expression" dxfId="192" priority="427">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K68">
+    <cfRule type="expression" dxfId="191" priority="350">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10814,63 +10826,63 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="189" priority="348">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H32 J32:K32">
-    <cfRule type="expression" dxfId="188" priority="421">
+    <cfRule type="expression" dxfId="189" priority="422">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="187" priority="345">
+    <cfRule type="expression" dxfId="188" priority="346">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69 J69">
-    <cfRule type="expression" dxfId="186" priority="343">
+    <cfRule type="expression" dxfId="187" priority="344">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="185" priority="409">
+    <cfRule type="expression" dxfId="186" priority="410">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="184" priority="341">
+    <cfRule type="expression" dxfId="185" priority="342">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="183" priority="406">
+    <cfRule type="expression" dxfId="184" priority="407">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="182" priority="403">
+    <cfRule type="expression" dxfId="183" priority="404">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70 J70">
-    <cfRule type="expression" dxfId="181" priority="339">
+    <cfRule type="expression" dxfId="182" priority="340">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="180" priority="400">
+    <cfRule type="expression" dxfId="181" priority="401">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:B40 J39:V39 E39:H39 E40:G40 L40:V40">
-    <cfRule type="expression" dxfId="179" priority="397">
+    <cfRule type="expression" dxfId="180" priority="398">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:V41 B41:B43 E43 E41:H41 G43 E42:G42 L42:V43">
-    <cfRule type="expression" dxfId="178" priority="393">
+    <cfRule type="expression" dxfId="179" priority="394">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72">
+    <cfRule type="expression" dxfId="178" priority="338">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10879,98 +10891,98 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="176" priority="336">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E49:G49 B49">
-    <cfRule type="expression" dxfId="175" priority="386">
+    <cfRule type="expression" dxfId="176" priority="387">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I82">
-    <cfRule type="expression" dxfId="174" priority="243">
+    <cfRule type="expression" dxfId="175" priority="244">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
+    <cfRule type="expression" dxfId="174" priority="383">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53 J53">
     <cfRule type="expression" dxfId="173" priority="382">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H53 J53">
-    <cfRule type="expression" dxfId="172" priority="381">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="171" priority="329">
+    <cfRule type="expression" dxfId="172" priority="330">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="170" priority="332">
+    <cfRule type="expression" dxfId="171" priority="333">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72 J72">
-    <cfRule type="expression" dxfId="169" priority="335">
+    <cfRule type="expression" dxfId="170" priority="336">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63 J63">
-    <cfRule type="expression" dxfId="168" priority="371">
+    <cfRule type="expression" dxfId="169" priority="372">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="167" priority="368">
+    <cfRule type="expression" dxfId="168" priority="369">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="166" priority="365">
+    <cfRule type="expression" dxfId="167" priority="366">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66 J66">
-    <cfRule type="expression" dxfId="165" priority="359">
+    <cfRule type="expression" dxfId="166" priority="360">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="164" priority="356">
+    <cfRule type="expression" dxfId="165" priority="357">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68 J68">
-    <cfRule type="expression" dxfId="163" priority="347">
+    <cfRule type="expression" dxfId="164" priority="348">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="162" priority="344">
+    <cfRule type="expression" dxfId="163" priority="345">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="161" priority="333">
+    <cfRule type="expression" dxfId="162" priority="334">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73 J73">
-    <cfRule type="expression" dxfId="160" priority="331">
+    <cfRule type="expression" dxfId="161" priority="332">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74">
+    <cfRule type="expression" dxfId="160" priority="329">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H74 J74">
     <cfRule type="expression" dxfId="159" priority="328">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H74 J74">
-    <cfRule type="expression" dxfId="158" priority="327">
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="158" priority="326">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10979,642 +10991,642 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
+  <conditionalFormatting sqref="H71 J71">
     <cfRule type="expression" dxfId="156" priority="324">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H71 J71">
-    <cfRule type="expression" dxfId="155" priority="323">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G82">
-    <cfRule type="expression" dxfId="154" priority="318">
+    <cfRule type="expression" dxfId="155" priority="319">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J82:V82">
-    <cfRule type="expression" dxfId="153" priority="313">
+    <cfRule type="expression" dxfId="154" priority="314">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82 E82:F82">
+    <cfRule type="expression" dxfId="153" priority="316">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82:V82">
     <cfRule type="expression" dxfId="152" priority="315">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K82:V82">
-    <cfRule type="expression" dxfId="151" priority="314">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="expression" dxfId="150" priority="312">
+    <cfRule type="expression" dxfId="151" priority="313">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79">
-    <cfRule type="expression" dxfId="149" priority="309">
+    <cfRule type="expression" dxfId="150" priority="310">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80">
-    <cfRule type="expression" dxfId="148" priority="307">
+    <cfRule type="expression" dxfId="149" priority="308">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G85">
-    <cfRule type="expression" dxfId="147" priority="304">
+    <cfRule type="expression" dxfId="148" priority="305">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="146" priority="161">
+    <cfRule type="expression" dxfId="147" priority="162">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J85:V85">
-    <cfRule type="expression" dxfId="145" priority="299">
+    <cfRule type="expression" dxfId="146" priority="300">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85 E85:F85">
+    <cfRule type="expression" dxfId="145" priority="302">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K85:V85">
     <cfRule type="expression" dxfId="144" priority="301">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K85:V85">
-    <cfRule type="expression" dxfId="143" priority="300">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="expression" dxfId="142" priority="298">
+    <cfRule type="expression" dxfId="143" priority="299">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="expression" dxfId="141" priority="296">
+    <cfRule type="expression" dxfId="142" priority="297">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G86">
-    <cfRule type="expression" dxfId="140" priority="294">
+    <cfRule type="expression" dxfId="141" priority="295">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="139" priority="151">
+    <cfRule type="expression" dxfId="140" priority="152">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J86:V86">
-    <cfRule type="expression" dxfId="138" priority="289">
+    <cfRule type="expression" dxfId="139" priority="290">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86 E86:F86">
+    <cfRule type="expression" dxfId="138" priority="292">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K86:V86">
     <cfRule type="expression" dxfId="137" priority="291">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K86:V86">
-    <cfRule type="expression" dxfId="136" priority="290">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="expression" dxfId="135" priority="288">
+    <cfRule type="expression" dxfId="136" priority="289">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87">
+    <cfRule type="expression" dxfId="135" priority="287">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H87">
     <cfRule type="expression" dxfId="134" priority="286">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H87">
-    <cfRule type="expression" dxfId="133" priority="285">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G88">
-    <cfRule type="expression" dxfId="132" priority="283">
+    <cfRule type="expression" dxfId="133" priority="284">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="131" priority="140">
+    <cfRule type="expression" dxfId="132" priority="141">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J88:V88">
-    <cfRule type="expression" dxfId="130" priority="278">
+    <cfRule type="expression" dxfId="131" priority="279">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88 E88:F88">
+    <cfRule type="expression" dxfId="130" priority="281">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K88:V88">
     <cfRule type="expression" dxfId="129" priority="280">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K88:V88">
-    <cfRule type="expression" dxfId="128" priority="279">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H88">
-    <cfRule type="expression" dxfId="127" priority="277">
+    <cfRule type="expression" dxfId="128" priority="278">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43">
-    <cfRule type="expression" dxfId="126" priority="275">
+    <cfRule type="expression" dxfId="127" priority="276">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43 J43">
-    <cfRule type="expression" dxfId="125" priority="273">
+    <cfRule type="expression" dxfId="126" priority="274">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:K38">
-    <cfRule type="expression" dxfId="124" priority="270">
+    <cfRule type="expression" dxfId="125" priority="271">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="123" priority="268">
+    <cfRule type="expression" dxfId="124" priority="269">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="expression" dxfId="122" priority="126">
+    <cfRule type="expression" dxfId="123" priority="127">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53">
-    <cfRule type="expression" dxfId="121" priority="264">
+    <cfRule type="expression" dxfId="122" priority="265">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I67">
-    <cfRule type="expression" dxfId="120" priority="257">
+    <cfRule type="expression" dxfId="121" priority="258">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63">
+    <cfRule type="expression" dxfId="120" priority="262">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I64">
     <cfRule type="expression" dxfId="119" priority="261">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I64">
+  <conditionalFormatting sqref="I65">
     <cfRule type="expression" dxfId="118" priority="260">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
+  <conditionalFormatting sqref="I66">
     <cfRule type="expression" dxfId="117" priority="259">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I66">
-    <cfRule type="expression" dxfId="116" priority="258">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I68">
+    <cfRule type="expression" dxfId="116" priority="256">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I69">
     <cfRule type="expression" dxfId="115" priority="255">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I69">
+  <conditionalFormatting sqref="I70">
     <cfRule type="expression" dxfId="114" priority="254">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I70">
+  <conditionalFormatting sqref="I71">
     <cfRule type="expression" dxfId="113" priority="253">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I71">
+  <conditionalFormatting sqref="I72">
     <cfRule type="expression" dxfId="112" priority="252">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I72">
+  <conditionalFormatting sqref="I73">
     <cfRule type="expression" dxfId="111" priority="251">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I73">
+  <conditionalFormatting sqref="I74">
     <cfRule type="expression" dxfId="110" priority="250">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I74">
+  <conditionalFormatting sqref="I75">
     <cfRule type="expression" dxfId="109" priority="249">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I75">
-    <cfRule type="expression" dxfId="108" priority="248">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I78">
+    <cfRule type="expression" dxfId="108" priority="247">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I79">
     <cfRule type="expression" dxfId="107" priority="246">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I79">
+  <conditionalFormatting sqref="I80">
     <cfRule type="expression" dxfId="106" priority="245">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I80">
-    <cfRule type="expression" dxfId="105" priority="244">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I83">
+    <cfRule type="expression" dxfId="105" priority="243">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I85">
     <cfRule type="expression" dxfId="104" priority="242">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I85">
+  <conditionalFormatting sqref="I86">
     <cfRule type="expression" dxfId="103" priority="241">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I86">
+  <conditionalFormatting sqref="I87">
     <cfRule type="expression" dxfId="102" priority="240">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87">
+  <conditionalFormatting sqref="I88">
     <cfRule type="expression" dxfId="101" priority="239">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88">
+  <conditionalFormatting sqref="I89">
     <cfRule type="expression" dxfId="100" priority="238">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I89">
+  <conditionalFormatting sqref="H89">
     <cfRule type="expression" dxfId="99" priority="237">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H89">
+  <conditionalFormatting sqref="I2">
     <cfRule type="expression" dxfId="98" priority="236">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I3">
     <cfRule type="expression" dxfId="97" priority="235">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
+  <conditionalFormatting sqref="I4">
     <cfRule type="expression" dxfId="96" priority="234">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
+  <conditionalFormatting sqref="I5">
     <cfRule type="expression" dxfId="95" priority="233">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
+  <conditionalFormatting sqref="I6">
     <cfRule type="expression" dxfId="94" priority="232">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
+  <conditionalFormatting sqref="I7">
     <cfRule type="expression" dxfId="93" priority="231">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
+  <conditionalFormatting sqref="I8">
     <cfRule type="expression" dxfId="92" priority="230">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
+  <conditionalFormatting sqref="I11">
     <cfRule type="expression" dxfId="91" priority="229">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="90" priority="228">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I13">
+    <cfRule type="expression" dxfId="90" priority="161">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
     <cfRule type="expression" dxfId="89" priority="160">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
+  <conditionalFormatting sqref="I15">
     <cfRule type="expression" dxfId="88" priority="159">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
+  <conditionalFormatting sqref="I16">
     <cfRule type="expression" dxfId="87" priority="158">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
+  <conditionalFormatting sqref="I17">
     <cfRule type="expression" dxfId="86" priority="157">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="85" priority="156">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="84" priority="150">
+    <cfRule type="expression" dxfId="85" priority="151">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
+    <cfRule type="expression" dxfId="84" priority="155">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
     <cfRule type="expression" dxfId="83" priority="154">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
+  <conditionalFormatting sqref="I22">
     <cfRule type="expression" dxfId="82" priority="153">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="81" priority="152">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I25">
+    <cfRule type="expression" dxfId="81" priority="150">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
     <cfRule type="expression" dxfId="80" priority="149">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
+  <conditionalFormatting sqref="I27">
     <cfRule type="expression" dxfId="79" priority="148">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
+  <conditionalFormatting sqref="I28">
     <cfRule type="expression" dxfId="78" priority="147">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
+  <conditionalFormatting sqref="I29">
     <cfRule type="expression" dxfId="77" priority="146">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
+  <conditionalFormatting sqref="I30">
     <cfRule type="expression" dxfId="76" priority="145">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
+  <conditionalFormatting sqref="I31">
     <cfRule type="expression" dxfId="75" priority="144">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
+  <conditionalFormatting sqref="I32">
     <cfRule type="expression" dxfId="74" priority="143">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="73" priority="142">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="72" priority="139">
+    <cfRule type="expression" dxfId="73" priority="140">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50">
-    <cfRule type="expression" dxfId="71" priority="125">
+    <cfRule type="expression" dxfId="72" priority="126">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
+    <cfRule type="expression" dxfId="71" priority="138">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
     <cfRule type="expression" dxfId="70" priority="137">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
+  <conditionalFormatting sqref="I37">
     <cfRule type="expression" dxfId="69" priority="136">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
+  <conditionalFormatting sqref="I38">
     <cfRule type="expression" dxfId="68" priority="135">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
+  <conditionalFormatting sqref="I39">
     <cfRule type="expression" dxfId="67" priority="134">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
+  <conditionalFormatting sqref="I41">
     <cfRule type="expression" dxfId="66" priority="133">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
+  <conditionalFormatting sqref="I43">
     <cfRule type="expression" dxfId="65" priority="132">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="64" priority="131">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="63" priority="129">
+    <cfRule type="expression" dxfId="64" priority="130">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="62" priority="127">
+    <cfRule type="expression" dxfId="63" priority="128">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:V10">
-    <cfRule type="expression" dxfId="61" priority="117">
+    <cfRule type="expression" dxfId="62" priority="118">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="60" priority="106">
+    <cfRule type="expression" dxfId="61" priority="107">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H84">
+    <cfRule type="expression" dxfId="60" priority="116">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I84">
     <cfRule type="expression" dxfId="59" priority="115">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I84">
-    <cfRule type="expression" dxfId="58" priority="114">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J9:K9">
+    <cfRule type="expression" dxfId="58" priority="106">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
     <cfRule type="expression" dxfId="57" priority="105">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="56" priority="104">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="55" priority="107">
+    <cfRule type="expression" dxfId="56" priority="108">
       <formula>K$1=$H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="54" priority="108">
+    <cfRule type="expression" dxfId="55" priority="109">
       <formula>K$1=$I9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="53" priority="102">
+    <cfRule type="expression" dxfId="54" priority="103">
       <formula>K$1=$H10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="52" priority="103">
+    <cfRule type="expression" dxfId="53" priority="104">
       <formula>K$1=$I10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
+    <cfRule type="expression" dxfId="52" priority="102">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:K10">
     <cfRule type="expression" dxfId="51" priority="101">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
+  <conditionalFormatting sqref="I10">
     <cfRule type="expression" dxfId="50" priority="100">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="49" priority="99">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="48" priority="92">
+    <cfRule type="expression" dxfId="49" priority="93">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42:K42 H42">
+    <cfRule type="expression" dxfId="48" priority="88">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I42">
     <cfRule type="expression" dxfId="47" priority="87">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="46" priority="86">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="45" priority="77">
+    <cfRule type="expression" dxfId="46" priority="78">
       <formula>K$1=$H18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="44" priority="78">
+    <cfRule type="expression" dxfId="45" priority="79">
       <formula>K$1=$I18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18 J18:K18">
-    <cfRule type="expression" dxfId="43" priority="79">
+    <cfRule type="expression" dxfId="44" priority="80">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="42" priority="76">
+    <cfRule type="expression" dxfId="43" priority="77">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K76">
+    <cfRule type="expression" dxfId="42" priority="75">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J76:K76">
     <cfRule type="expression" dxfId="41" priority="74">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J76:K76">
+  <conditionalFormatting sqref="H76">
     <cfRule type="expression" dxfId="40" priority="73">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H76">
+  <conditionalFormatting sqref="I76">
     <cfRule type="expression" dxfId="39" priority="72">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="expression" dxfId="38" priority="71">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J40:K40 H40">
+    <cfRule type="expression" dxfId="38" priority="70">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
     <cfRule type="expression" dxfId="37" priority="69">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="36" priority="68">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J81">
+    <cfRule type="expression" dxfId="36" priority="60">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H81">
     <cfRule type="expression" dxfId="35" priority="59">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H81">
+  <conditionalFormatting sqref="I81">
     <cfRule type="expression" dxfId="34" priority="58">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I81">
+  <conditionalFormatting sqref="K81:V81">
     <cfRule type="expression" dxfId="33" priority="57">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="32" priority="56">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="31" priority="54">
+    <cfRule type="expression" dxfId="32" priority="55">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47 G47">
+    <cfRule type="expression" dxfId="31" priority="53">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47:F47">
     <cfRule type="expression" dxfId="30" priority="52">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E47:F47">
+  <conditionalFormatting sqref="B47 E47 G47">
     <cfRule type="expression" dxfId="29" priority="51">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -11624,103 +11636,103 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47 E47 G47">
+  <conditionalFormatting sqref="F47">
     <cfRule type="expression" dxfId="27" priority="49">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
+  <conditionalFormatting sqref="J47:V47 H47">
     <cfRule type="expression" dxfId="26" priority="48">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J47:V47 H47">
-    <cfRule type="expression" dxfId="25" priority="47">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I47">
+    <cfRule type="expression" dxfId="25" priority="46">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21 E21:G21">
     <cfRule type="expression" dxfId="24" priority="45">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21 E21:G21">
-    <cfRule type="expression" dxfId="23" priority="44">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E46:F46">
+    <cfRule type="expression" dxfId="23" priority="41">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J46:V46 H46">
     <cfRule type="expression" dxfId="22" priority="40">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J46:V46 H46">
-    <cfRule type="expression" dxfId="21" priority="39">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="20" priority="37">
+    <cfRule type="expression" dxfId="21" priority="38">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:V21">
-    <cfRule type="expression" dxfId="19" priority="34">
+    <cfRule type="expression" dxfId="20" priority="35">
       <formula>K$1=$H21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="expression" dxfId="18" priority="35">
+    <cfRule type="expression" dxfId="19" priority="36">
       <formula>K$1=$I21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21:V21">
-    <cfRule type="expression" dxfId="17" priority="36">
+    <cfRule type="expression" dxfId="18" priority="37">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21 J21:K21">
+    <cfRule type="expression" dxfId="17" priority="34">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
     <cfRule type="expression" dxfId="16" priority="33">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
+  <conditionalFormatting sqref="F60">
     <cfRule type="expression" dxfId="15" priority="32">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F60">
-    <cfRule type="expression" dxfId="14" priority="31">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G77">
-    <cfRule type="expression" dxfId="13" priority="27">
+    <cfRule type="expression" dxfId="14" priority="28">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77">
+    <cfRule type="expression" dxfId="13" priority="18">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J77:K77">
     <cfRule type="expression" dxfId="12" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J77:K77">
+  <conditionalFormatting sqref="H77">
     <cfRule type="expression" dxfId="11" priority="16">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H77">
+  <conditionalFormatting sqref="I77">
     <cfRule type="expression" dxfId="10" priority="15">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I77">
-    <cfRule type="expression" dxfId="9" priority="14">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="8" priority="21">
+    <cfRule type="expression" dxfId="9" priority="22">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L77:V77">
+    <cfRule type="expression" dxfId="8" priority="20">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11729,37 +11741,37 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="6" priority="18">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B45:G45">
+    <cfRule type="expression" dxfId="6" priority="14">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
     <cfRule type="expression" dxfId="5" priority="13">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
+  <conditionalFormatting sqref="E45:F45">
     <cfRule type="expression" dxfId="4" priority="12">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E45:F45">
-    <cfRule type="expression" dxfId="3" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K45:V45">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>K$1=$H45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45:V45 H45">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F83">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Move Punisher09brm to 1hr earlier payout
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10303"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D902693-A433-BD4F-9AD0-FF60049A12C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D05406-55D5-9A45-A6CF-81AD5DE41DC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11600" yWindow="2680" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1214,7 +1214,14 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="278">
+  <dxfs count="275">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1620,34 +1627,6 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3495,8 +3474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3586,11 +3565,11 @@
         <v>CST</v>
       </c>
       <c r="U1" s="3" t="str">
-        <f>H65</f>
+        <f>H66</f>
         <v>CST</v>
       </c>
       <c r="V1" s="3" t="str">
-        <f>H70</f>
+        <f>H71</f>
         <v>CST</v>
       </c>
     </row>
@@ -7906,23 +7885,23 @@
     </row>
     <row r="58" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="55"/>
-      <c r="B58" s="18" t="s">
-        <v>93</v>
+      <c r="B58" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="C58" s="7">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D58" s="7">
-        <v>57</v>
-      </c>
-      <c r="E58" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="E58" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F58" s="40" t="s">
+      <c r="F58" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G58" s="29" t="s">
-        <v>155</v>
+      <c r="G58" s="22" t="s">
+        <v>124</v>
       </c>
       <c r="H58" s="29" t="s">
         <v>220</v>
@@ -7933,7 +7912,7 @@
       <c r="J58" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K58" s="25">
+      <c r="K58" s="11">
         <f>$I58+Sheet2!B$1/24</f>
         <v>1.375</v>
       </c>
@@ -7985,22 +7964,22 @@
     <row r="59" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="55"/>
       <c r="B59" s="18" t="s">
-        <v>245</v>
+        <v>93</v>
       </c>
       <c r="C59" s="7">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="D59" s="7">
-        <v>99</v>
-      </c>
-      <c r="E59" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="E59" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="F59" s="53" t="s">
+      <c r="F59" s="40" t="s">
         <v>20</v>
       </c>
       <c r="G59" s="29" t="s">
-        <v>246</v>
+        <v>155</v>
       </c>
       <c r="H59" s="29" t="s">
         <v>220</v>
@@ -8063,20 +8042,22 @@
     <row r="60" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="55"/>
       <c r="B60" s="18" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C60" s="7">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="D60" s="7">
-        <v>58</v>
-      </c>
-      <c r="E60" s="53"/>
-      <c r="F60" s="19" t="s">
-        <v>45</v>
+        <v>99</v>
+      </c>
+      <c r="E60" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" s="53" t="s">
+        <v>20</v>
       </c>
       <c r="G60" s="29" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="H60" s="29" t="s">
         <v>220</v>
@@ -8139,22 +8120,20 @@
     <row r="61" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="55"/>
       <c r="B61" s="18" t="s">
-        <v>44</v>
+        <v>241</v>
       </c>
       <c r="C61" s="7">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D61" s="7">
-        <v>59</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>27</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E61" s="53"/>
       <c r="F61" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G61" s="21" t="s">
-        <v>158</v>
+      <c r="G61" s="29" t="s">
+        <v>242</v>
       </c>
       <c r="H61" s="29" t="s">
         <v>220</v>
@@ -8217,97 +8196,97 @@
     <row r="62" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="55"/>
       <c r="B62" s="18" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="C62" s="7">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D62" s="7">
-        <v>60</v>
-      </c>
-      <c r="E62" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="F62" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="G62" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="G62" s="21" t="s">
+        <v>158</v>
+      </c>
       <c r="H62" s="29" t="s">
-        <v>9</v>
+        <v>220</v>
       </c>
       <c r="I62" s="23">
-        <v>0</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="J62" s="26" t="s">
         <v>14</v>
       </c>
       <c r="K62" s="25">
         <f>$I62+Sheet2!B$1/24</f>
-        <v>0.41666666666666669</v>
+        <v>1.375</v>
       </c>
       <c r="L62" s="23">
         <f>$I62+Sheet2!B$2/24</f>
-        <v>0.375</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="M62" s="23">
         <f>$I62+Sheet2!B$3/24</f>
-        <v>0.33333333333333331</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="N62" s="23">
         <f>$I62+Sheet2!B$4/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="O62" s="23">
         <f>$I62+Sheet2!B$5/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="P62" s="23">
         <f>$I62+Sheet2!B$6/24</f>
-        <v>0.125</v>
+        <v>1.0833333333333335</v>
       </c>
       <c r="Q62" s="23">
         <f>$I62+Sheet2!B$7/24</f>
-        <v>8.3333333333333329E-2</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="R62" s="23">
         <f>$I62+Sheet2!B$8/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>1</v>
       </c>
       <c r="S62" s="23">
         <f>$I62+Sheet2!B$9/24</f>
-        <v>-0.16666666666666666</v>
+        <v>0.79166666666666674</v>
       </c>
       <c r="T62" s="23">
         <f>$I62+Sheet2!B$10/24</f>
-        <v>-0.20833333333333334</v>
+        <v>0.75</v>
       </c>
       <c r="U62" s="23">
         <f>$I62+Sheet2!B$11/24</f>
-        <v>-0.25</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="V62" s="23">
         <f>$I62+Sheet2!B$12/24</f>
-        <v>-0.29166666666666669</v>
+        <v>0.66666666666666674</v>
       </c>
     </row>
     <row r="63" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="55"/>
-      <c r="B63" s="35" t="s">
-        <v>94</v>
+      <c r="B63" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="C63" s="7">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D63" s="7">
-        <v>61</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>27</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E63" s="14"/>
       <c r="F63" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G63" s="29" t="s">
-        <v>159</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="G63" s="9"/>
       <c r="H63" s="29" t="s">
         <v>9</v>
       </c>
@@ -8369,13 +8348,13 @@
     <row r="64" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="55"/>
       <c r="B64" s="35" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="C64" s="7">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D64" s="7">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E64" s="14" t="s">
         <v>27</v>
@@ -8384,7 +8363,7 @@
         <v>20</v>
       </c>
       <c r="G64" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H64" s="29" t="s">
         <v>9</v>
@@ -8447,22 +8426,22 @@
     <row r="65" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="55"/>
       <c r="B65" s="35" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C65" s="7">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D65" s="7">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E65" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F65" s="7" t="s">
-        <v>69</v>
+      <c r="F65" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="G65" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H65" s="29" t="s">
         <v>9</v>
@@ -8524,23 +8503,23 @@
     </row>
     <row r="66" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="55"/>
-      <c r="B66" s="18" t="s">
-        <v>88</v>
+      <c r="B66" s="35" t="s">
+        <v>57</v>
       </c>
       <c r="C66" s="7">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D66" s="7">
-        <v>65</v>
-      </c>
-      <c r="E66" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F66" s="40" t="s">
-        <v>20</v>
+      <c r="F66" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="G66" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H66" s="29" t="s">
         <v>9</v>
@@ -8603,13 +8582,13 @@
     <row r="67" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="55"/>
       <c r="B67" s="18" t="s">
-        <v>180</v>
+        <v>88</v>
       </c>
       <c r="C67" s="7">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D67" s="7">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E67" s="39" t="s">
         <v>27</v>
@@ -8618,7 +8597,7 @@
         <v>20</v>
       </c>
       <c r="G67" s="29" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="H67" s="29" t="s">
         <v>9</v>
@@ -8680,23 +8659,23 @@
     </row>
     <row r="68" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="55"/>
-      <c r="B68" s="35" t="s">
-        <v>63</v>
+      <c r="B68" s="18" t="s">
+        <v>180</v>
       </c>
       <c r="C68" s="7">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D68" s="7">
-        <v>67</v>
-      </c>
-      <c r="E68" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E68" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="F68" s="19" t="s">
-        <v>45</v>
+      <c r="F68" s="40" t="s">
+        <v>20</v>
       </c>
       <c r="G68" s="29" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="H68" s="29" t="s">
         <v>9</v>
@@ -8759,22 +8738,22 @@
     <row r="69" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="55"/>
       <c r="B69" s="35" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C69" s="7">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D69" s="7">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E69" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G69" s="27" t="s">
-        <v>165</v>
+        <v>45</v>
+      </c>
+      <c r="G69" s="29" t="s">
+        <v>164</v>
       </c>
       <c r="H69" s="29" t="s">
         <v>9</v>
@@ -8836,23 +8815,23 @@
     </row>
     <row r="70" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="55"/>
-      <c r="B70" s="18" t="s">
-        <v>58</v>
+      <c r="B70" s="35" t="s">
+        <v>61</v>
       </c>
       <c r="C70" s="7">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D70" s="7">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E70" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F70" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G70" s="29" t="s">
-        <v>166</v>
+      <c r="F70" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" s="27" t="s">
+        <v>165</v>
       </c>
       <c r="H70" s="29" t="s">
         <v>9</v>
@@ -8914,23 +8893,23 @@
     </row>
     <row r="71" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="55"/>
-      <c r="B71" s="12" t="s">
-        <v>90</v>
+      <c r="B71" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="C71" s="7">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D71" s="7">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E71" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F71" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G71" s="22" t="s">
-        <v>124</v>
+      <c r="F71" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G71" s="29" t="s">
+        <v>166</v>
       </c>
       <c r="H71" s="29" t="s">
         <v>9</v>
@@ -8945,47 +8924,47 @@
         <f>$I71+Sheet2!B$1/24</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="L71" s="16">
+      <c r="L71" s="23">
         <f>$I71+Sheet2!B$2/24</f>
         <v>0.375</v>
       </c>
-      <c r="M71" s="16">
+      <c r="M71" s="23">
         <f>$I71+Sheet2!B$3/24</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N71" s="16">
+      <c r="N71" s="23">
         <f>$I71+Sheet2!B$4/24</f>
         <v>0.125</v>
       </c>
-      <c r="O71" s="16">
+      <c r="O71" s="23">
         <f>$I71+Sheet2!B$5/24</f>
         <v>0.125</v>
       </c>
-      <c r="P71" s="16">
+      <c r="P71" s="23">
         <f>$I71+Sheet2!B$6/24</f>
         <v>0.125</v>
       </c>
-      <c r="Q71" s="16">
+      <c r="Q71" s="23">
         <f>$I71+Sheet2!B$7/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="R71" s="16">
+      <c r="R71" s="23">
         <f>$I71+Sheet2!B$8/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="S71" s="16">
+      <c r="S71" s="23">
         <f>$I71+Sheet2!B$9/24</f>
         <v>-0.16666666666666666</v>
       </c>
-      <c r="T71" s="16">
+      <c r="T71" s="23">
         <f>$I71+Sheet2!B$10/24</f>
         <v>-0.20833333333333334</v>
       </c>
-      <c r="U71" s="16">
+      <c r="U71" s="23">
         <f>$I71+Sheet2!B$11/24</f>
         <v>-0.25</v>
       </c>
-      <c r="V71" s="16">
+      <c r="V71" s="23">
         <f>$I71+Sheet2!B$12/24</f>
         <v>-0.29166666666666669</v>
       </c>
@@ -10374,11 +10353,11 @@
     <sortCondition ref="D2:D72"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
+      <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
-      <selection sqref="A1:XFD1048576"/>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -10387,1241 +10366,1226 @@
     <mergeCell ref="A51:A88"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V44 K46:V89">
-    <cfRule type="expression" dxfId="277" priority="672">
+    <cfRule type="expression" dxfId="274" priority="673">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K17:V17 K19:V19 K23:V23 K20 K24:K32 K22">
-    <cfRule type="expression" dxfId="276" priority="674">
+    <cfRule type="expression" dxfId="273" priority="675">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K53:V53 G53 G64 G73 G89 E62:G62 G30 B74 E74:G74 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 B70:B72 E70:G72 L40:V40 K87:V87 G87 K79:V80 K83:V84 K89:V89 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B84 J11:V14 J84:V84 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L76:V76 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E84:G84 E61:V61 E65:G65 B50:B62 B40 B81 B48 J48:V48 G75:G80 E24:G29 B20:B38 E5:G5 E48:H48 E81:G81 E76:G77 L24:V32 L20:V20 L22:V22 G66:G69 E44:H44 L64:V74 B65:B67 B76:B77 G58:V60 B44:B46 C4:D89 E45:G46">
-    <cfRule type="expression" dxfId="275" priority="678">
+  <conditionalFormatting sqref="K53:V53 G53 G65 G73 G89 E63:G63 G30 B74 E74:G74 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 L40:V40 K87:V87 G87 K79:V80 K83:V84 K89:V89 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B84 J11:V14 J84:V84 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L76:V76 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E84:G84 E62:V62 E66:G66 B50:B57 B40 B81 B48 J48:V48 G75:G80 E24:G29 B20:B38 E5:G5 E48:H48 E81:G81 E76:G77 L24:V32 L20:V20 L22:V22 G67:G70 E44:H44 B66:B68 B76:B77 G59:V61 B44:B46 C4:D57 E45:G46 B59:B63 H58:V58 B71:B72 E71:G72 L65:V74 C59:D89">
+    <cfRule type="expression" dxfId="272" priority="679">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B65 L65:V65">
+    <cfRule type="expression" dxfId="271" priority="656">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70 L70:V70">
+    <cfRule type="expression" dxfId="270" priority="652">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B73 L73:V73">
+    <cfRule type="expression" dxfId="269" priority="650">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69 L69:V69">
+    <cfRule type="expression" dxfId="268" priority="648">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B87 K87:V87 E87:F87">
+    <cfRule type="expression" dxfId="267" priority="644">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule type="expression" dxfId="266" priority="642">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E73">
+    <cfRule type="expression" dxfId="265" priority="639">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
+    <cfRule type="expression" dxfId="264" priority="638">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B84 J83:V84">
+    <cfRule type="expression" dxfId="263" priority="635">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B80:B81 J80:V80 E80:E81">
+    <cfRule type="expression" dxfId="262" priority="633">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E84:F84 E83">
+    <cfRule type="expression" dxfId="261" priority="631">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B79 J79:V79">
+    <cfRule type="expression" dxfId="260" priority="629">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B89 J89:V89 E89">
+    <cfRule type="expression" dxfId="259" priority="627">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F69">
+    <cfRule type="expression" dxfId="258" priority="619">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63:V63">
+    <cfRule type="expression" dxfId="257" priority="559">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F73">
+    <cfRule type="expression" dxfId="256" priority="581">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B75:B77 E75:F77">
+    <cfRule type="expression" dxfId="255" priority="545">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
+    <cfRule type="expression" dxfId="254" priority="566">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64 L64:V64">
-    <cfRule type="expression" dxfId="274" priority="655">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B69 L69:V69">
-    <cfRule type="expression" dxfId="273" priority="651">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B73 L73:V73">
-    <cfRule type="expression" dxfId="272" priority="649">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B68 L68:V68">
-    <cfRule type="expression" dxfId="271" priority="647">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B87 K87:V87 E87:F87">
-    <cfRule type="expression" dxfId="270" priority="643">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E64">
-    <cfRule type="expression" dxfId="269" priority="641">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E73">
-    <cfRule type="expression" dxfId="268" priority="638">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
-    <cfRule type="expression" dxfId="267" priority="637">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B83:B84 J83:V84">
-    <cfRule type="expression" dxfId="266" priority="634">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B80:B81 J80:V80 E80:E81">
-    <cfRule type="expression" dxfId="265" priority="632">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E84:F84 E83">
-    <cfRule type="expression" dxfId="264" priority="630">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B79 J79:V79">
-    <cfRule type="expression" dxfId="263" priority="628">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B89 J89:V89 E89">
-    <cfRule type="expression" dxfId="262" priority="626">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F68">
-    <cfRule type="expression" dxfId="261" priority="618">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62:V62">
-    <cfRule type="expression" dxfId="260" priority="558">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F73">
-    <cfRule type="expression" dxfId="259" priority="580">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B75:B77 E75:F77">
-    <cfRule type="expression" dxfId="258" priority="544">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="257" priority="565">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B63 L63:V63">
-    <cfRule type="expression" dxfId="256" priority="566">
+    <cfRule type="expression" dxfId="253" priority="567">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F80:F81">
-    <cfRule type="expression" dxfId="255" priority="578">
+    <cfRule type="expression" dxfId="252" priority="579">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F65">
+    <cfRule type="expression" dxfId="251" priority="575">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E70:F70">
+    <cfRule type="expression" dxfId="250" priority="574">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E79:F79">
+    <cfRule type="expression" dxfId="249" priority="572">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L64:V64 G64">
+    <cfRule type="expression" dxfId="248" priority="569">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7:V7">
+    <cfRule type="expression" dxfId="247" priority="514">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64">
-    <cfRule type="expression" dxfId="254" priority="574">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69:F69">
-    <cfRule type="expression" dxfId="253" priority="573">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E79:F79">
-    <cfRule type="expression" dxfId="252" priority="571">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L63:V63 G63">
-    <cfRule type="expression" dxfId="251" priority="568">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7:V7">
-    <cfRule type="expression" dxfId="250" priority="513">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F63">
-    <cfRule type="expression" dxfId="249" priority="562">
+    <cfRule type="expression" dxfId="246" priority="563">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:V48">
-    <cfRule type="expression" dxfId="248" priority="682">
+    <cfRule type="expression" dxfId="245" priority="683">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K62:V62">
-    <cfRule type="expression" dxfId="247" priority="559">
+  <conditionalFormatting sqref="K63:V63">
+    <cfRule type="expression" dxfId="244" priority="560">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:V10">
-    <cfRule type="expression" dxfId="246" priority="504">
+    <cfRule type="expression" dxfId="243" priority="505">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H14 J13:V14 L18:V18">
-    <cfRule type="expression" dxfId="245" priority="550">
+    <cfRule type="expression" dxfId="242" priority="551">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:V14 L18:V18">
-    <cfRule type="expression" dxfId="244" priority="551">
+    <cfRule type="expression" dxfId="241" priority="552">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:G3 B7 E7:G7">
-    <cfRule type="expression" dxfId="243" priority="545">
+    <cfRule type="expression" dxfId="240" priority="546">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K75:V75 L76:V76">
-    <cfRule type="expression" dxfId="242" priority="543">
+    <cfRule type="expression" dxfId="239" priority="544">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J75:V75 L76:V76">
-    <cfRule type="expression" dxfId="241" priority="541">
+    <cfRule type="expression" dxfId="238" priority="542">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75">
-    <cfRule type="expression" dxfId="240" priority="540">
+    <cfRule type="expression" dxfId="237" priority="541">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J78:V78">
-    <cfRule type="expression" dxfId="239" priority="535">
+    <cfRule type="expression" dxfId="236" priority="536">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78 E78:F78">
-    <cfRule type="expression" dxfId="238" priority="538">
+    <cfRule type="expression" dxfId="235" priority="539">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K78:V78">
-    <cfRule type="expression" dxfId="237" priority="537">
+    <cfRule type="expression" dxfId="234" priority="538">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78">
-    <cfRule type="expression" dxfId="236" priority="534">
+    <cfRule type="expression" dxfId="233" priority="535">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="235" priority="527">
+    <cfRule type="expression" dxfId="232" priority="528">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:F30">
-    <cfRule type="expression" dxfId="234" priority="532">
+    <cfRule type="expression" dxfId="231" priority="533">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43 E43 L43:V43 G43">
-    <cfRule type="expression" dxfId="233" priority="531">
+    <cfRule type="expression" dxfId="230" priority="532">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4 E4:G4">
-    <cfRule type="expression" dxfId="232" priority="526">
+    <cfRule type="expression" dxfId="229" priority="527">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="231" priority="525">
+    <cfRule type="expression" dxfId="228" priority="526">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 E6:H6 J6:V6">
-    <cfRule type="expression" dxfId="230" priority="523">
+    <cfRule type="expression" dxfId="227" priority="524">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:V5">
-    <cfRule type="expression" dxfId="229" priority="520">
+    <cfRule type="expression" dxfId="226" priority="521">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:L4">
-    <cfRule type="expression" dxfId="228" priority="515">
+    <cfRule type="expression" dxfId="225" priority="516">
       <formula>K$1=$H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:V4">
-    <cfRule type="expression" dxfId="227" priority="516">
+    <cfRule type="expression" dxfId="224" priority="517">
       <formula>K$1=$I4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:V4">
-    <cfRule type="expression" dxfId="226" priority="517">
+    <cfRule type="expression" dxfId="223" priority="518">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="225" priority="510">
+    <cfRule type="expression" dxfId="222" priority="511">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 E8:G10">
-    <cfRule type="expression" dxfId="224" priority="509">
+    <cfRule type="expression" dxfId="221" priority="510">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:K8">
-    <cfRule type="expression" dxfId="223" priority="507">
+    <cfRule type="expression" dxfId="220" priority="508">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:H15 J15:V15">
-    <cfRule type="expression" dxfId="222" priority="499">
+    <cfRule type="expression" dxfId="219" priority="500">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15 J15:V15">
-    <cfRule type="expression" dxfId="221" priority="496">
+    <cfRule type="expression" dxfId="218" priority="497">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:V15">
-    <cfRule type="expression" dxfId="220" priority="497">
+    <cfRule type="expression" dxfId="217" priority="498">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:G15">
-    <cfRule type="expression" dxfId="219" priority="495">
+    <cfRule type="expression" dxfId="216" priority="496">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="218" priority="492">
+    <cfRule type="expression" dxfId="215" priority="493">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="217" priority="489">
+    <cfRule type="expression" dxfId="214" priority="490">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="216" priority="490">
+    <cfRule type="expression" dxfId="213" priority="491">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49 J49:V49">
-    <cfRule type="expression" dxfId="215" priority="384">
+    <cfRule type="expression" dxfId="212" priority="385">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19 E19:H19 J19:V19">
-    <cfRule type="expression" dxfId="214" priority="485">
+    <cfRule type="expression" dxfId="211" priority="486">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="210" priority="342">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27 J27:K27">
+    <cfRule type="expression" dxfId="209" priority="448">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H63:J63">
+    <cfRule type="expression" dxfId="208" priority="380">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20 J20:K20">
+    <cfRule type="expression" dxfId="207" priority="475">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22 J22:K22">
+    <cfRule type="expression" dxfId="206" priority="470">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="expression" dxfId="205" priority="375">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K64">
+    <cfRule type="expression" dxfId="204" priority="374">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24 J24:K24">
+    <cfRule type="expression" dxfId="203" priority="463">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K65">
+    <cfRule type="expression" dxfId="202" priority="371">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25 J25:K25">
+    <cfRule type="expression" dxfId="201" priority="458">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H65 J65">
+    <cfRule type="expression" dxfId="200" priority="369">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26 J26:K26">
+    <cfRule type="expression" dxfId="199" priority="453">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K66">
+    <cfRule type="expression" dxfId="198" priority="366">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66 J66">
+    <cfRule type="expression" dxfId="197" priority="365">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67">
+    <cfRule type="expression" dxfId="196" priority="363">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67">
+    <cfRule type="expression" dxfId="195" priority="362">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28 J28:K28">
+    <cfRule type="expression" dxfId="194" priority="443">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K68">
+    <cfRule type="expression" dxfId="193" priority="359">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29 J29:K29">
+    <cfRule type="expression" dxfId="192" priority="438">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H68 J68">
+    <cfRule type="expression" dxfId="191" priority="357">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30 J30:K30">
+    <cfRule type="expression" dxfId="190" priority="433">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31 J31:K31">
+    <cfRule type="expression" dxfId="189" priority="428">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="expression" dxfId="188" priority="351">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="expression" dxfId="187" priority="350">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32 J32:K32">
+    <cfRule type="expression" dxfId="186" priority="423">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="213" priority="341">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27 J27:K27">
-    <cfRule type="expression" dxfId="212" priority="447">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H62:J62">
-    <cfRule type="expression" dxfId="211" priority="379">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20 J20:K20">
-    <cfRule type="expression" dxfId="210" priority="474">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22 J22:K22">
-    <cfRule type="expression" dxfId="209" priority="469">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="208" priority="374">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K63">
-    <cfRule type="expression" dxfId="207" priority="373">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24 J24:K24">
-    <cfRule type="expression" dxfId="206" priority="462">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="205" priority="370">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25 J25:K25">
-    <cfRule type="expression" dxfId="204" priority="457">
+    <cfRule type="expression" dxfId="185" priority="347">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H70 J70">
+    <cfRule type="expression" dxfId="184" priority="345">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="expression" dxfId="183" priority="411">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="182" priority="343">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="expression" dxfId="181" priority="408">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
+    <cfRule type="expression" dxfId="180" priority="405">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H71 J71">
+    <cfRule type="expression" dxfId="179" priority="341">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H37">
+    <cfRule type="expression" dxfId="178" priority="402">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:B40 J39:V39 E39:H39 E40:G40 L40:V40">
+    <cfRule type="expression" dxfId="177" priority="399">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41:V41 B41:B43 E43 E41:H41 G43 E42:G42 L42:V43">
+    <cfRule type="expression" dxfId="176" priority="395">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72">
+    <cfRule type="expression" dxfId="175" priority="339">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K72">
+    <cfRule type="expression" dxfId="174" priority="338">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49:G49 B49">
+    <cfRule type="expression" dxfId="173" priority="388">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I82">
+    <cfRule type="expression" dxfId="172" priority="245">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H50">
+    <cfRule type="expression" dxfId="171" priority="384">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53 J53">
+    <cfRule type="expression" dxfId="170" priority="383">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K74">
+    <cfRule type="expression" dxfId="169" priority="331">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K73">
+    <cfRule type="expression" dxfId="168" priority="334">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H72 J72">
+    <cfRule type="expression" dxfId="167" priority="337">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64 J64">
-    <cfRule type="expression" dxfId="203" priority="368">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26 J26:K26">
-    <cfRule type="expression" dxfId="202" priority="452">
+    <cfRule type="expression" dxfId="166" priority="373">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="201" priority="365">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H65 J65">
-    <cfRule type="expression" dxfId="200" priority="364">
+    <cfRule type="expression" dxfId="165" priority="370">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="199" priority="362">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="198" priority="361">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H28 J28:K28">
-    <cfRule type="expression" dxfId="197" priority="442">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="196" priority="358">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29 J29:K29">
-    <cfRule type="expression" dxfId="195" priority="437">
+    <cfRule type="expression" dxfId="164" priority="367">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="194" priority="356">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H30 J30:K30">
-    <cfRule type="expression" dxfId="193" priority="432">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H31 J31:K31">
-    <cfRule type="expression" dxfId="192" priority="427">
+    <cfRule type="expression" dxfId="163" priority="361">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="191" priority="350">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="190" priority="349">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H32 J32:K32">
-    <cfRule type="expression" dxfId="189" priority="422">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="188" priority="346">
+    <cfRule type="expression" dxfId="162" priority="358">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69 J69">
-    <cfRule type="expression" dxfId="187" priority="344">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="186" priority="410">
+    <cfRule type="expression" dxfId="161" priority="349">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="185" priority="342">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="184" priority="407">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="183" priority="404">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H70 J70">
-    <cfRule type="expression" dxfId="182" priority="340">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="181" priority="401">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39:B40 J39:V39 E39:H39 E40:G40 L40:V40">
-    <cfRule type="expression" dxfId="180" priority="398">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J41:V41 B41:B43 E43 E41:H41 G43 E42:G42 L42:V43">
-    <cfRule type="expression" dxfId="179" priority="394">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="178" priority="338">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="177" priority="337">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49:G49 B49">
-    <cfRule type="expression" dxfId="176" priority="387">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I82">
-    <cfRule type="expression" dxfId="175" priority="244">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="174" priority="383">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H53 J53">
-    <cfRule type="expression" dxfId="173" priority="382">
+    <cfRule type="expression" dxfId="160" priority="346">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K73">
+    <cfRule type="expression" dxfId="159" priority="335">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H73 J73">
+    <cfRule type="expression" dxfId="158" priority="333">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="172" priority="330">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="171" priority="333">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H72 J72">
-    <cfRule type="expression" dxfId="170" priority="336">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H63 J63">
-    <cfRule type="expression" dxfId="169" priority="372">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="168" priority="369">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="167" priority="366">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H66 J66">
-    <cfRule type="expression" dxfId="166" priority="360">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="165" priority="357">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H68 J68">
-    <cfRule type="expression" dxfId="164" priority="348">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="163" priority="345">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="162" priority="334">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H73 J73">
-    <cfRule type="expression" dxfId="161" priority="332">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="160" priority="329">
+    <cfRule type="expression" dxfId="157" priority="330">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74 J74">
-    <cfRule type="expression" dxfId="159" priority="328">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="158" priority="326">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="157" priority="325">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H71 J71">
-    <cfRule type="expression" dxfId="156" priority="324">
+    <cfRule type="expression" dxfId="156" priority="329">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82">
-    <cfRule type="expression" dxfId="155" priority="319">
+    <cfRule type="expression" dxfId="155" priority="320">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J82:V82">
-    <cfRule type="expression" dxfId="154" priority="314">
+    <cfRule type="expression" dxfId="154" priority="315">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82 E82:F82">
-    <cfRule type="expression" dxfId="153" priority="316">
+    <cfRule type="expression" dxfId="153" priority="317">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K82:V82">
-    <cfRule type="expression" dxfId="152" priority="315">
+    <cfRule type="expression" dxfId="152" priority="316">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="expression" dxfId="151" priority="313">
+    <cfRule type="expression" dxfId="151" priority="314">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79">
-    <cfRule type="expression" dxfId="150" priority="310">
+    <cfRule type="expression" dxfId="150" priority="311">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80">
-    <cfRule type="expression" dxfId="149" priority="308">
+    <cfRule type="expression" dxfId="149" priority="309">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G85">
-    <cfRule type="expression" dxfId="148" priority="305">
+    <cfRule type="expression" dxfId="148" priority="306">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="147" priority="162">
+    <cfRule type="expression" dxfId="147" priority="163">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J85:V85">
-    <cfRule type="expression" dxfId="146" priority="300">
+    <cfRule type="expression" dxfId="146" priority="301">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85 E85:F85">
-    <cfRule type="expression" dxfId="145" priority="302">
+    <cfRule type="expression" dxfId="145" priority="303">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K85:V85">
-    <cfRule type="expression" dxfId="144" priority="301">
+    <cfRule type="expression" dxfId="144" priority="302">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="expression" dxfId="143" priority="299">
+    <cfRule type="expression" dxfId="143" priority="300">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="expression" dxfId="142" priority="297">
+    <cfRule type="expression" dxfId="142" priority="298">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G86">
-    <cfRule type="expression" dxfId="141" priority="295">
+    <cfRule type="expression" dxfId="141" priority="296">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="140" priority="152">
+    <cfRule type="expression" dxfId="140" priority="153">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J86:V86">
-    <cfRule type="expression" dxfId="139" priority="290">
+    <cfRule type="expression" dxfId="139" priority="291">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86 E86:F86">
-    <cfRule type="expression" dxfId="138" priority="292">
+    <cfRule type="expression" dxfId="138" priority="293">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K86:V86">
-    <cfRule type="expression" dxfId="137" priority="291">
+    <cfRule type="expression" dxfId="137" priority="292">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="expression" dxfId="136" priority="289">
+    <cfRule type="expression" dxfId="136" priority="290">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87">
-    <cfRule type="expression" dxfId="135" priority="287">
+    <cfRule type="expression" dxfId="135" priority="288">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87">
-    <cfRule type="expression" dxfId="134" priority="286">
+    <cfRule type="expression" dxfId="134" priority="287">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88">
-    <cfRule type="expression" dxfId="133" priority="284">
+    <cfRule type="expression" dxfId="133" priority="285">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="132" priority="141">
+    <cfRule type="expression" dxfId="132" priority="142">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J88:V88">
-    <cfRule type="expression" dxfId="131" priority="279">
+    <cfRule type="expression" dxfId="131" priority="280">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88 E88:F88">
-    <cfRule type="expression" dxfId="130" priority="281">
+    <cfRule type="expression" dxfId="130" priority="282">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88:V88">
-    <cfRule type="expression" dxfId="129" priority="280">
+    <cfRule type="expression" dxfId="129" priority="281">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88">
-    <cfRule type="expression" dxfId="128" priority="278">
+    <cfRule type="expression" dxfId="128" priority="279">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43">
-    <cfRule type="expression" dxfId="127" priority="276">
+    <cfRule type="expression" dxfId="127" priority="277">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43 J43">
-    <cfRule type="expression" dxfId="126" priority="274">
+    <cfRule type="expression" dxfId="126" priority="275">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:K38">
-    <cfRule type="expression" dxfId="125" priority="271">
+    <cfRule type="expression" dxfId="125" priority="272">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="124" priority="269">
+    <cfRule type="expression" dxfId="124" priority="270">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="expression" dxfId="123" priority="127">
+    <cfRule type="expression" dxfId="123" priority="128">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53">
-    <cfRule type="expression" dxfId="122" priority="265">
+    <cfRule type="expression" dxfId="122" priority="266">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I68">
+    <cfRule type="expression" dxfId="121" priority="259">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I64">
+    <cfRule type="expression" dxfId="120" priority="263">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I65">
+    <cfRule type="expression" dxfId="119" priority="262">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I66">
+    <cfRule type="expression" dxfId="118" priority="261">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I67">
-    <cfRule type="expression" dxfId="121" priority="258">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I63">
-    <cfRule type="expression" dxfId="120" priority="262">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I64">
-    <cfRule type="expression" dxfId="119" priority="261">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
-    <cfRule type="expression" dxfId="118" priority="260">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I66">
-    <cfRule type="expression" dxfId="117" priority="259">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I68">
-    <cfRule type="expression" dxfId="116" priority="256">
+    <cfRule type="expression" dxfId="117" priority="260">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="115" priority="255">
+    <cfRule type="expression" dxfId="116" priority="257">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="114" priority="254">
+    <cfRule type="expression" dxfId="115" priority="256">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I71">
+    <cfRule type="expression" dxfId="114" priority="255">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I72">
     <cfRule type="expression" dxfId="113" priority="253">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I72">
+  <conditionalFormatting sqref="I73">
     <cfRule type="expression" dxfId="112" priority="252">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I73">
+  <conditionalFormatting sqref="I74">
     <cfRule type="expression" dxfId="111" priority="251">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I74">
+  <conditionalFormatting sqref="I75">
     <cfRule type="expression" dxfId="110" priority="250">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I75">
-    <cfRule type="expression" dxfId="109" priority="249">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I78">
+    <cfRule type="expression" dxfId="109" priority="248">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I79">
     <cfRule type="expression" dxfId="108" priority="247">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I79">
+  <conditionalFormatting sqref="I80">
     <cfRule type="expression" dxfId="107" priority="246">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I80">
-    <cfRule type="expression" dxfId="106" priority="245">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I83">
+    <cfRule type="expression" dxfId="106" priority="244">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I85">
     <cfRule type="expression" dxfId="105" priority="243">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I85">
+  <conditionalFormatting sqref="I86">
     <cfRule type="expression" dxfId="104" priority="242">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I86">
+  <conditionalFormatting sqref="I87">
     <cfRule type="expression" dxfId="103" priority="241">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87">
+  <conditionalFormatting sqref="I88">
     <cfRule type="expression" dxfId="102" priority="240">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88">
+  <conditionalFormatting sqref="I89">
     <cfRule type="expression" dxfId="101" priority="239">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I89">
+  <conditionalFormatting sqref="H89">
     <cfRule type="expression" dxfId="100" priority="238">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H89">
+  <conditionalFormatting sqref="I2">
     <cfRule type="expression" dxfId="99" priority="237">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I3">
     <cfRule type="expression" dxfId="98" priority="236">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
+  <conditionalFormatting sqref="I4">
     <cfRule type="expression" dxfId="97" priority="235">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
+  <conditionalFormatting sqref="I5">
     <cfRule type="expression" dxfId="96" priority="234">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
+  <conditionalFormatting sqref="I6">
     <cfRule type="expression" dxfId="95" priority="233">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
+  <conditionalFormatting sqref="I7">
     <cfRule type="expression" dxfId="94" priority="232">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
+  <conditionalFormatting sqref="I8">
     <cfRule type="expression" dxfId="93" priority="231">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
+  <conditionalFormatting sqref="I11">
     <cfRule type="expression" dxfId="92" priority="230">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="91" priority="229">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I13">
+    <cfRule type="expression" dxfId="91" priority="162">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
     <cfRule type="expression" dxfId="90" priority="161">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
+  <conditionalFormatting sqref="I15">
     <cfRule type="expression" dxfId="89" priority="160">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
+  <conditionalFormatting sqref="I16">
     <cfRule type="expression" dxfId="88" priority="159">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
+  <conditionalFormatting sqref="I17">
     <cfRule type="expression" dxfId="87" priority="158">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="86" priority="157">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="85" priority="151">
+    <cfRule type="expression" dxfId="86" priority="152">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
+    <cfRule type="expression" dxfId="85" priority="156">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
     <cfRule type="expression" dxfId="84" priority="155">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
+  <conditionalFormatting sqref="I22">
     <cfRule type="expression" dxfId="83" priority="154">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="82" priority="153">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I25">
+    <cfRule type="expression" dxfId="82" priority="151">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
     <cfRule type="expression" dxfId="81" priority="150">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
+  <conditionalFormatting sqref="I27">
     <cfRule type="expression" dxfId="80" priority="149">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
+  <conditionalFormatting sqref="I28">
     <cfRule type="expression" dxfId="79" priority="148">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
+  <conditionalFormatting sqref="I29">
     <cfRule type="expression" dxfId="78" priority="147">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
+  <conditionalFormatting sqref="I30">
     <cfRule type="expression" dxfId="77" priority="146">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
+  <conditionalFormatting sqref="I31">
     <cfRule type="expression" dxfId="76" priority="145">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
+  <conditionalFormatting sqref="I32">
     <cfRule type="expression" dxfId="75" priority="144">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="74" priority="143">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="73" priority="140">
+    <cfRule type="expression" dxfId="74" priority="141">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50">
-    <cfRule type="expression" dxfId="72" priority="126">
+    <cfRule type="expression" dxfId="73" priority="127">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
+    <cfRule type="expression" dxfId="72" priority="139">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
     <cfRule type="expression" dxfId="71" priority="138">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
+  <conditionalFormatting sqref="I37">
     <cfRule type="expression" dxfId="70" priority="137">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
+  <conditionalFormatting sqref="I38">
     <cfRule type="expression" dxfId="69" priority="136">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
+  <conditionalFormatting sqref="I39">
     <cfRule type="expression" dxfId="68" priority="135">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
+  <conditionalFormatting sqref="I41">
     <cfRule type="expression" dxfId="67" priority="134">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
+  <conditionalFormatting sqref="I43">
     <cfRule type="expression" dxfId="66" priority="133">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="65" priority="132">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="64" priority="130">
+    <cfRule type="expression" dxfId="65" priority="131">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="63" priority="128">
+    <cfRule type="expression" dxfId="64" priority="129">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:V10">
-    <cfRule type="expression" dxfId="62" priority="118">
+    <cfRule type="expression" dxfId="63" priority="119">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="61" priority="107">
+    <cfRule type="expression" dxfId="62" priority="108">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H84">
+    <cfRule type="expression" dxfId="61" priority="117">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I84">
     <cfRule type="expression" dxfId="60" priority="116">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I84">
-    <cfRule type="expression" dxfId="59" priority="115">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J9:K9">
+    <cfRule type="expression" dxfId="59" priority="107">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
     <cfRule type="expression" dxfId="58" priority="106">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="57" priority="105">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="56" priority="108">
+    <cfRule type="expression" dxfId="57" priority="109">
       <formula>K$1=$H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="55" priority="109">
+    <cfRule type="expression" dxfId="56" priority="110">
       <formula>K$1=$I9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="54" priority="103">
+    <cfRule type="expression" dxfId="55" priority="104">
       <formula>K$1=$H10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="53" priority="104">
+    <cfRule type="expression" dxfId="54" priority="105">
       <formula>K$1=$I10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
+    <cfRule type="expression" dxfId="53" priority="103">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:K10">
     <cfRule type="expression" dxfId="52" priority="102">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
+  <conditionalFormatting sqref="I10">
     <cfRule type="expression" dxfId="51" priority="101">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="50" priority="100">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="49" priority="93">
+    <cfRule type="expression" dxfId="50" priority="94">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42:K42 H42">
+    <cfRule type="expression" dxfId="49" priority="89">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I42">
     <cfRule type="expression" dxfId="48" priority="88">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="47" priority="87">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="46" priority="78">
+    <cfRule type="expression" dxfId="47" priority="79">
       <formula>K$1=$H18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="45" priority="79">
+    <cfRule type="expression" dxfId="46" priority="80">
       <formula>K$1=$I18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18 J18:K18">
-    <cfRule type="expression" dxfId="44" priority="80">
+    <cfRule type="expression" dxfId="45" priority="81">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="43" priority="77">
+    <cfRule type="expression" dxfId="44" priority="78">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K76">
+    <cfRule type="expression" dxfId="43" priority="76">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J76:K76">
     <cfRule type="expression" dxfId="42" priority="75">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J76:K76">
+  <conditionalFormatting sqref="H76">
     <cfRule type="expression" dxfId="41" priority="74">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H76">
+  <conditionalFormatting sqref="I76">
     <cfRule type="expression" dxfId="40" priority="73">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="expression" dxfId="39" priority="72">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J40:K40 H40">
+    <cfRule type="expression" dxfId="39" priority="71">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
     <cfRule type="expression" dxfId="38" priority="70">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="37" priority="69">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J81">
+    <cfRule type="expression" dxfId="37" priority="61">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H81">
     <cfRule type="expression" dxfId="36" priority="60">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H81">
+  <conditionalFormatting sqref="I81">
     <cfRule type="expression" dxfId="35" priority="59">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I81">
+  <conditionalFormatting sqref="K81:V81">
     <cfRule type="expression" dxfId="34" priority="58">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="33" priority="57">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="32" priority="55">
+    <cfRule type="expression" dxfId="33" priority="56">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47 G47">
+    <cfRule type="expression" dxfId="32" priority="54">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47:F47">
     <cfRule type="expression" dxfId="31" priority="53">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E47:F47">
+  <conditionalFormatting sqref="B47 E47 G47">
     <cfRule type="expression" dxfId="30" priority="52">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -11631,103 +11595,103 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47 E47 G47">
+  <conditionalFormatting sqref="F47">
     <cfRule type="expression" dxfId="28" priority="50">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
+  <conditionalFormatting sqref="J47:V47 H47">
     <cfRule type="expression" dxfId="27" priority="49">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J47:V47 H47">
-    <cfRule type="expression" dxfId="26" priority="48">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I47">
+    <cfRule type="expression" dxfId="26" priority="47">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21 E21:G21">
     <cfRule type="expression" dxfId="25" priority="46">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21 E21:G21">
-    <cfRule type="expression" dxfId="24" priority="45">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E46:F46">
+    <cfRule type="expression" dxfId="24" priority="42">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J46:V46 H46">
     <cfRule type="expression" dxfId="23" priority="41">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J46:V46 H46">
-    <cfRule type="expression" dxfId="22" priority="40">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="21" priority="38">
+    <cfRule type="expression" dxfId="22" priority="39">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:V21">
-    <cfRule type="expression" dxfId="20" priority="35">
+    <cfRule type="expression" dxfId="21" priority="36">
       <formula>K$1=$H21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="expression" dxfId="19" priority="36">
+    <cfRule type="expression" dxfId="20" priority="37">
       <formula>K$1=$I21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21:V21">
-    <cfRule type="expression" dxfId="18" priority="37">
+    <cfRule type="expression" dxfId="19" priority="38">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21 J21:K21">
+    <cfRule type="expression" dxfId="18" priority="35">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
     <cfRule type="expression" dxfId="17" priority="34">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
+  <conditionalFormatting sqref="F61">
     <cfRule type="expression" dxfId="16" priority="33">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F60">
-    <cfRule type="expression" dxfId="15" priority="32">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G77">
-    <cfRule type="expression" dxfId="14" priority="28">
+    <cfRule type="expression" dxfId="15" priority="29">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77">
+    <cfRule type="expression" dxfId="14" priority="19">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J77:K77">
     <cfRule type="expression" dxfId="13" priority="18">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J77:K77">
+  <conditionalFormatting sqref="H77">
     <cfRule type="expression" dxfId="12" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H77">
+  <conditionalFormatting sqref="I77">
     <cfRule type="expression" dxfId="11" priority="16">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I77">
-    <cfRule type="expression" dxfId="10" priority="15">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="9" priority="22">
+    <cfRule type="expression" dxfId="10" priority="23">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L77:V77">
+    <cfRule type="expression" dxfId="9" priority="21">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11736,42 +11700,42 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="7" priority="19">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B45:G45">
+    <cfRule type="expression" dxfId="7" priority="15">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
     <cfRule type="expression" dxfId="6" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
+  <conditionalFormatting sqref="E45:F45">
     <cfRule type="expression" dxfId="5" priority="13">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E45:F45">
-    <cfRule type="expression" dxfId="4" priority="12">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K45:V45">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>K$1=$H45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45:V45 H45">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F83">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F83">
+  <conditionalFormatting sqref="B58:G58">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Move Joseph Howan to 1 hour earlier
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10303"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm/Documents/Code/swgoh-squad-arena-payout-bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D05406-55D5-9A45-A6CF-81AD5DE41DC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9BFC16-BF45-B645-A3D9-1ED894A59217}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20260" yWindow="5940" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1199,10 +1199,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1214,28 +1214,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="275">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="278">
     <dxf>
       <fill>
         <patternFill>
@@ -1253,111 +1232,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
@@ -1369,6 +1243,154 @@
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF920000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF920000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3474,8 +3496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3545,7 +3567,7 @@
         <v>CXT</v>
       </c>
       <c r="P1" s="3" t="str">
-        <f>H20</f>
+        <f>H21</f>
         <v>EET</v>
       </c>
       <c r="Q1" s="3" t="str">
@@ -4870,100 +4892,100 @@
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="47"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="18" t="s">
-        <v>203</v>
+        <v>234</v>
       </c>
       <c r="C19" s="7">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D19" s="7">
-        <v>18</v>
-      </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="H19" s="29" t="s">
-        <v>205</v>
+        <v>20</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="G19" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>10</v>
       </c>
       <c r="I19" s="23">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="J19" s="30" t="s">
+        <v>0.625</v>
+      </c>
+      <c r="J19" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K19" s="11">
+      <c r="K19" s="25">
         <f>$I19+Sheet2!B$1/24</f>
-        <v>1.0833333333333333</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="L19" s="23">
         <f>$I19+Sheet2!B$2/24</f>
-        <v>1.0416666666666665</v>
+        <v>1</v>
       </c>
       <c r="M19" s="23">
         <f>$I19+Sheet2!B$3/24</f>
-        <v>1</v>
+        <v>0.95833333333333326</v>
       </c>
       <c r="N19" s="23">
         <f>$I19+Sheet2!B$4/24</f>
-        <v>0.79166666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="O19" s="23">
         <f>$I19+Sheet2!B$5/24</f>
-        <v>0.79166666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="P19" s="23">
         <f>$I19+Sheet2!B$6/24</f>
-        <v>0.79166666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="Q19" s="23">
         <f>$I19+Sheet2!B$7/24</f>
-        <v>0.75</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="R19" s="23">
         <f>$I19+Sheet2!B$8/24</f>
-        <v>0.70833333333333326</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="S19" s="23">
         <f>$I19+Sheet2!B$9/24</f>
-        <v>0.5</v>
+        <v>0.45833333333333337</v>
       </c>
       <c r="T19" s="23">
         <f>$I19+Sheet2!B$10/24</f>
-        <v>0.45833333333333326</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="U19" s="23">
         <f>$I19+Sheet2!B$11/24</f>
-        <v>0.41666666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="V19" s="23">
         <f>$I19+Sheet2!B$12/24</f>
-        <v>0.37499999999999994</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="47"/>
       <c r="B20" s="18" t="s">
-        <v>41</v>
+        <v>203</v>
       </c>
       <c r="C20" s="7">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="7">
-        <v>19</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E20" s="20"/>
       <c r="F20" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>132</v>
+        <v>204</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>99</v>
       </c>
       <c r="H20" s="29" t="s">
         <v>205</v>
@@ -5024,24 +5046,24 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="52"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="18" t="s">
-        <v>234</v>
+        <v>41</v>
       </c>
       <c r="C21" s="7">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="7">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="G21" s="51" t="s">
-        <v>237</v>
+        <v>19</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>132</v>
       </c>
       <c r="H21" s="29" t="s">
         <v>205</v>
@@ -8050,10 +8072,10 @@
       <c r="D60" s="7">
         <v>99</v>
       </c>
-      <c r="E60" s="53" t="s">
+      <c r="E60" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="F60" s="53" t="s">
+      <c r="F60" s="52" t="s">
         <v>20</v>
       </c>
       <c r="G60" s="29" t="s">
@@ -8128,7 +8150,7 @@
       <c r="D61" s="7">
         <v>58</v>
       </c>
-      <c r="E61" s="53"/>
+      <c r="E61" s="52"/>
       <c r="F61" s="19" t="s">
         <v>45</v>
       </c>
@@ -10353,11 +10375,11 @@
     <sortCondition ref="D2:D72"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -10365,1383 +10387,1398 @@
     <mergeCell ref="A25:A50"/>
     <mergeCell ref="A51:A88"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K19:V20 K22:V44 K46:V89">
-    <cfRule type="expression" dxfId="274" priority="673">
+  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K20:V89">
+    <cfRule type="expression" dxfId="277" priority="683">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K17:V17 K19:V19 K23:V23 K20 K24:K32 K22">
-    <cfRule type="expression" dxfId="273" priority="675">
+  <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K17:V17 K20:V20 K23:V23 K24:K32 K21:K22">
+    <cfRule type="expression" dxfId="276" priority="685">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K53:V53 G53 G65 G73 G89 E63:G63 G30 B74 E74:G74 B3 E3:H3 H7 L10:V10 E20:G22 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 L40:V40 K87:V87 G87 K79:V80 K83:V84 K89:V89 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B84 J11:V14 J84:V84 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L76:V76 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E84:G84 E62:V62 E66:G66 B50:B57 B40 B81 B48 J48:V48 G75:G80 E24:G29 B20:B38 E5:G5 E48:H48 E81:G81 E76:G77 L24:V32 L20:V20 L22:V22 G67:G70 E44:H44 B66:B68 B76:B77 G59:V61 B44:B46 C4:D57 E45:G46 B59:B63 H58:V58 B71:B72 E71:G72 L65:V74 C59:D89">
-    <cfRule type="expression" dxfId="272" priority="679">
+  <conditionalFormatting sqref="K53:V53 G53 G65 G73 G89 E63:G63 G30 B74 E74:G74 B3 E3:H3 H7 L10:V10 E23:H23 E31:G32 J23:V23 E33:H33 J33:V37 E50:G50 J50:V50 L40:V40 K87:V87 G87 K79:V80 K83:V84 K89:V89 L38:V38 E34:G38 E51:V52 H2 J2:V3 E40:G40 B84 J11:V14 J84:V84 B5 E54:V57 L16:V16 L42:V42 B42 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J44:V44 L76:V76 B9:B14 E18:G18 E9:G10 E17:H17 E42:G42 E84:G84 E62:V62 E66:G66 B50:B57 B40 B81 B48 J48:V48 G75:G80 E24:G29 E5:G5 E48:H48 E81:G81 E76:G77 L24:V32 L21:V22 G67:G70 E44:H44 B66:B68 B76:B77 G59:V61 B44:B46 C4:D18 E45:G46 B59:B63 H58:V58 B71:B72 E71:G72 L65:V74 C59:D89 E21:G22 B21:B38 C20:D57">
+    <cfRule type="expression" dxfId="275" priority="689">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65 L65:V65">
-    <cfRule type="expression" dxfId="271" priority="656">
+    <cfRule type="expression" dxfId="274" priority="666">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70 L70:V70">
-    <cfRule type="expression" dxfId="270" priority="652">
+    <cfRule type="expression" dxfId="273" priority="662">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73 L73:V73">
-    <cfRule type="expression" dxfId="269" priority="650">
+    <cfRule type="expression" dxfId="272" priority="660">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69 L69:V69">
-    <cfRule type="expression" dxfId="268" priority="648">
+    <cfRule type="expression" dxfId="271" priority="658">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87 K87:V87 E87:F87">
-    <cfRule type="expression" dxfId="267" priority="644">
+    <cfRule type="expression" dxfId="270" priority="654">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="expression" dxfId="266" priority="642">
+    <cfRule type="expression" dxfId="269" priority="652">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E73">
-    <cfRule type="expression" dxfId="265" priority="639">
+    <cfRule type="expression" dxfId="268" priority="649">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69">
-    <cfRule type="expression" dxfId="264" priority="638">
+    <cfRule type="expression" dxfId="267" priority="648">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:B84 J83:V84">
-    <cfRule type="expression" dxfId="263" priority="635">
+    <cfRule type="expression" dxfId="266" priority="645">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:B81 J80:V80 E80:E81">
-    <cfRule type="expression" dxfId="262" priority="633">
+    <cfRule type="expression" dxfId="265" priority="643">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E84:F84 E83">
-    <cfRule type="expression" dxfId="261" priority="631">
+    <cfRule type="expression" dxfId="264" priority="641">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79 J79:V79">
-    <cfRule type="expression" dxfId="260" priority="629">
+    <cfRule type="expression" dxfId="263" priority="639">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89 J89:V89 E89">
-    <cfRule type="expression" dxfId="259" priority="627">
+    <cfRule type="expression" dxfId="262" priority="637">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F69">
-    <cfRule type="expression" dxfId="258" priority="619">
+    <cfRule type="expression" dxfId="261" priority="629">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63:V63">
-    <cfRule type="expression" dxfId="257" priority="559">
+    <cfRule type="expression" dxfId="260" priority="569">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F73">
-    <cfRule type="expression" dxfId="256" priority="581">
+    <cfRule type="expression" dxfId="259" priority="591">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75:B77 E75:F77">
-    <cfRule type="expression" dxfId="255" priority="545">
+    <cfRule type="expression" dxfId="258" priority="555">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" dxfId="254" priority="566">
+    <cfRule type="expression" dxfId="257" priority="576">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64 L64:V64">
-    <cfRule type="expression" dxfId="253" priority="567">
+    <cfRule type="expression" dxfId="256" priority="577">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F80:F81">
-    <cfRule type="expression" dxfId="252" priority="579">
+    <cfRule type="expression" dxfId="255" priority="589">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65">
-    <cfRule type="expression" dxfId="251" priority="575">
+    <cfRule type="expression" dxfId="254" priority="585">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70:F70">
-    <cfRule type="expression" dxfId="250" priority="574">
+    <cfRule type="expression" dxfId="253" priority="584">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E79:F79">
-    <cfRule type="expression" dxfId="249" priority="572">
+    <cfRule type="expression" dxfId="252" priority="582">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L64:V64 G64">
-    <cfRule type="expression" dxfId="248" priority="569">
+    <cfRule type="expression" dxfId="251" priority="579">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:V7">
-    <cfRule type="expression" dxfId="247" priority="514">
+    <cfRule type="expression" dxfId="250" priority="524">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64">
-    <cfRule type="expression" dxfId="246" priority="563">
+    <cfRule type="expression" dxfId="249" priority="573">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:V48">
-    <cfRule type="expression" dxfId="245" priority="683">
+    <cfRule type="expression" dxfId="248" priority="693">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63:V63">
-    <cfRule type="expression" dxfId="244" priority="560">
+    <cfRule type="expression" dxfId="247" priority="570">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:V10">
-    <cfRule type="expression" dxfId="243" priority="505">
+    <cfRule type="expression" dxfId="246" priority="515">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H14 J13:V14 L18:V18">
-    <cfRule type="expression" dxfId="242" priority="551">
+    <cfRule type="expression" dxfId="245" priority="561">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:V14 L18:V18">
+    <cfRule type="expression" dxfId="244" priority="562">
+      <formula>K$1=#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:G3 B7 E7:G7">
+    <cfRule type="expression" dxfId="243" priority="556">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K75:V75 L76:V76">
+    <cfRule type="expression" dxfId="242" priority="554">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J75:V75 L76:V76">
     <cfRule type="expression" dxfId="241" priority="552">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H75">
+    <cfRule type="expression" dxfId="240" priority="551">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J78:V78">
+    <cfRule type="expression" dxfId="239" priority="546">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B78 E78:F78">
+    <cfRule type="expression" dxfId="238" priority="549">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K78:V78">
+    <cfRule type="expression" dxfId="237" priority="548">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H78">
+    <cfRule type="expression" dxfId="236" priority="545">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="expression" dxfId="235" priority="538">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30:F30">
+    <cfRule type="expression" dxfId="234" priority="543">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43 E43 L43:V43 G43">
+    <cfRule type="expression" dxfId="233" priority="542">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4 E4:G4">
+    <cfRule type="expression" dxfId="232" priority="537">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
+    <cfRule type="expression" dxfId="231" priority="536">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6 E6:H6 J6:V6">
+    <cfRule type="expression" dxfId="230" priority="534">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:V5">
+    <cfRule type="expression" dxfId="229" priority="531">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:L4">
+    <cfRule type="expression" dxfId="228" priority="526">
+      <formula>K$1=$H4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:V4">
+    <cfRule type="expression" dxfId="227" priority="527">
+      <formula>K$1=$I4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:V4">
+    <cfRule type="expression" dxfId="226" priority="528">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="expression" dxfId="225" priority="521">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:B10 E8:G10">
+    <cfRule type="expression" dxfId="224" priority="520">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8:K8">
+    <cfRule type="expression" dxfId="223" priority="518">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15 E15:H15 J15:V15">
+    <cfRule type="expression" dxfId="222" priority="510">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15 J15:V15">
+    <cfRule type="expression" dxfId="221" priority="507">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15:V15">
+    <cfRule type="expression" dxfId="220" priority="508">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G3 B7 E7:G7">
-    <cfRule type="expression" dxfId="240" priority="546">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K75:V75 L76:V76">
-    <cfRule type="expression" dxfId="239" priority="544">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J75:V75 L76:V76">
-    <cfRule type="expression" dxfId="238" priority="542">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H75">
-    <cfRule type="expression" dxfId="237" priority="541">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J78:V78">
-    <cfRule type="expression" dxfId="236" priority="536">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B78 E78:F78">
-    <cfRule type="expression" dxfId="235" priority="539">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K78:V78">
-    <cfRule type="expression" dxfId="234" priority="538">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H78">
-    <cfRule type="expression" dxfId="233" priority="535">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="232" priority="528">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30:F30">
-    <cfRule type="expression" dxfId="231" priority="533">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B43 E43 L43:V43 G43">
-    <cfRule type="expression" dxfId="230" priority="532">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4 E4:G4">
-    <cfRule type="expression" dxfId="229" priority="527">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="228" priority="526">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6 E6:H6 J6:V6">
-    <cfRule type="expression" dxfId="227" priority="524">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J5:V5">
-    <cfRule type="expression" dxfId="226" priority="521">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:L4">
-    <cfRule type="expression" dxfId="225" priority="516">
-      <formula>K$1=$H4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:V4">
-    <cfRule type="expression" dxfId="224" priority="517">
-      <formula>K$1=$I4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4:V4">
-    <cfRule type="expression" dxfId="223" priority="518">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="222" priority="511">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B10 E8:G10">
-    <cfRule type="expression" dxfId="221" priority="510">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8:K8">
-    <cfRule type="expression" dxfId="220" priority="508">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15 E15:H15 J15:V15">
-    <cfRule type="expression" dxfId="219" priority="500">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15 J15:V15">
-    <cfRule type="expression" dxfId="218" priority="497">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15:V15">
-    <cfRule type="expression" dxfId="217" priority="498">
+  <conditionalFormatting sqref="B15 E15:G15">
+    <cfRule type="expression" dxfId="219" priority="506">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16 J16:K16">
+    <cfRule type="expression" dxfId="218" priority="503">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16 J16:K16">
+    <cfRule type="expression" dxfId="217" priority="500">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="expression" dxfId="216" priority="501">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 E15:G15">
-    <cfRule type="expression" dxfId="216" priority="496">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="215" priority="493">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="214" priority="490">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="213" priority="491">
-      <formula>K$1=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H49 J49:V49">
-    <cfRule type="expression" dxfId="212" priority="385">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19 E19:H19 J19:V19">
-    <cfRule type="expression" dxfId="211" priority="486">
+    <cfRule type="expression" dxfId="215" priority="395">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20 E20:H20 J20:V20">
+    <cfRule type="expression" dxfId="214" priority="496">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="210" priority="342">
+    <cfRule type="expression" dxfId="213" priority="352">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27 J27:K27">
-    <cfRule type="expression" dxfId="209" priority="448">
+    <cfRule type="expression" dxfId="212" priority="458">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63:J63">
-    <cfRule type="expression" dxfId="208" priority="380">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20 J20:K20">
-    <cfRule type="expression" dxfId="207" priority="475">
+    <cfRule type="expression" dxfId="211" priority="390">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21 J21:K21">
+    <cfRule type="expression" dxfId="210" priority="485">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22 J22:K22">
-    <cfRule type="expression" dxfId="206" priority="470">
+    <cfRule type="expression" dxfId="209" priority="480">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="205" priority="375">
+    <cfRule type="expression" dxfId="208" priority="385">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
-    <cfRule type="expression" dxfId="204" priority="374">
+    <cfRule type="expression" dxfId="207" priority="384">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24 J24:K24">
-    <cfRule type="expression" dxfId="203" priority="463">
+    <cfRule type="expression" dxfId="206" priority="473">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="202" priority="371">
+    <cfRule type="expression" dxfId="205" priority="381">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25 J25:K25">
-    <cfRule type="expression" dxfId="201" priority="458">
+    <cfRule type="expression" dxfId="204" priority="468">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65 J65">
-    <cfRule type="expression" dxfId="200" priority="369">
+    <cfRule type="expression" dxfId="203" priority="379">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26 J26:K26">
-    <cfRule type="expression" dxfId="199" priority="453">
+    <cfRule type="expression" dxfId="202" priority="463">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="198" priority="366">
+    <cfRule type="expression" dxfId="201" priority="376">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66 J66">
-    <cfRule type="expression" dxfId="197" priority="365">
+    <cfRule type="expression" dxfId="200" priority="375">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="196" priority="363">
+    <cfRule type="expression" dxfId="199" priority="373">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="195" priority="362">
+    <cfRule type="expression" dxfId="198" priority="372">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28 J28:K28">
-    <cfRule type="expression" dxfId="194" priority="443">
+    <cfRule type="expression" dxfId="197" priority="453">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="193" priority="359">
+    <cfRule type="expression" dxfId="196" priority="369">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29 J29:K29">
+    <cfRule type="expression" dxfId="195" priority="448">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H68 J68">
+    <cfRule type="expression" dxfId="194" priority="367">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30 J30:K30">
+    <cfRule type="expression" dxfId="193" priority="443">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31 J31:K31">
     <cfRule type="expression" dxfId="192" priority="438">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H68 J68">
-    <cfRule type="expression" dxfId="191" priority="357">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H30 J30:K30">
-    <cfRule type="expression" dxfId="190" priority="433">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H31 J31:K31">
-    <cfRule type="expression" dxfId="189" priority="428">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="188" priority="351">
+    <cfRule type="expression" dxfId="191" priority="361">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="187" priority="350">
+    <cfRule type="expression" dxfId="190" priority="360">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32 J32:K32">
-    <cfRule type="expression" dxfId="186" priority="423">
+    <cfRule type="expression" dxfId="189" priority="433">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="185" priority="347">
+    <cfRule type="expression" dxfId="188" priority="357">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70 J70">
-    <cfRule type="expression" dxfId="184" priority="345">
+    <cfRule type="expression" dxfId="187" priority="355">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="183" priority="411">
+    <cfRule type="expression" dxfId="186" priority="421">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="182" priority="343">
+    <cfRule type="expression" dxfId="185" priority="353">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="181" priority="408">
+    <cfRule type="expression" dxfId="184" priority="418">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="180" priority="405">
+    <cfRule type="expression" dxfId="183" priority="415">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71 J71">
-    <cfRule type="expression" dxfId="179" priority="341">
+    <cfRule type="expression" dxfId="182" priority="351">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="178" priority="402">
+    <cfRule type="expression" dxfId="181" priority="412">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:B40 J39:V39 E39:H39 E40:G40 L40:V40">
-    <cfRule type="expression" dxfId="177" priority="399">
+    <cfRule type="expression" dxfId="180" priority="409">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:V41 B41:B43 E43 E41:H41 G43 E42:G42 L42:V43">
-    <cfRule type="expression" dxfId="176" priority="395">
+    <cfRule type="expression" dxfId="179" priority="405">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="175" priority="339">
+    <cfRule type="expression" dxfId="178" priority="349">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="174" priority="338">
+    <cfRule type="expression" dxfId="177" priority="348">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:G49 B49">
-    <cfRule type="expression" dxfId="173" priority="388">
+    <cfRule type="expression" dxfId="176" priority="398">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I82">
-    <cfRule type="expression" dxfId="172" priority="245">
+    <cfRule type="expression" dxfId="175" priority="255">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="171" priority="384">
+    <cfRule type="expression" dxfId="174" priority="394">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53 J53">
-    <cfRule type="expression" dxfId="170" priority="383">
+    <cfRule type="expression" dxfId="173" priority="393">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="169" priority="331">
+    <cfRule type="expression" dxfId="172" priority="341">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="168" priority="334">
+    <cfRule type="expression" dxfId="171" priority="344">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72 J72">
-    <cfRule type="expression" dxfId="167" priority="337">
+    <cfRule type="expression" dxfId="170" priority="347">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64 J64">
-    <cfRule type="expression" dxfId="166" priority="373">
+    <cfRule type="expression" dxfId="169" priority="383">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="165" priority="370">
+    <cfRule type="expression" dxfId="168" priority="380">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="164" priority="367">
+    <cfRule type="expression" dxfId="167" priority="377">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="163" priority="361">
+    <cfRule type="expression" dxfId="166" priority="371">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="162" priority="358">
+    <cfRule type="expression" dxfId="165" priority="368">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69 J69">
-    <cfRule type="expression" dxfId="161" priority="349">
+    <cfRule type="expression" dxfId="164" priority="359">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="160" priority="346">
+    <cfRule type="expression" dxfId="163" priority="356">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="159" priority="335">
+    <cfRule type="expression" dxfId="162" priority="345">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73 J73">
-    <cfRule type="expression" dxfId="158" priority="333">
+    <cfRule type="expression" dxfId="161" priority="343">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="157" priority="330">
+    <cfRule type="expression" dxfId="160" priority="340">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74 J74">
-    <cfRule type="expression" dxfId="156" priority="329">
+    <cfRule type="expression" dxfId="159" priority="339">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82">
-    <cfRule type="expression" dxfId="155" priority="320">
+    <cfRule type="expression" dxfId="158" priority="330">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J82:V82">
-    <cfRule type="expression" dxfId="154" priority="315">
+    <cfRule type="expression" dxfId="157" priority="325">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82 E82:F82">
-    <cfRule type="expression" dxfId="153" priority="317">
+    <cfRule type="expression" dxfId="156" priority="327">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K82:V82">
-    <cfRule type="expression" dxfId="152" priority="316">
+    <cfRule type="expression" dxfId="155" priority="326">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="expression" dxfId="151" priority="314">
+    <cfRule type="expression" dxfId="154" priority="324">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79">
-    <cfRule type="expression" dxfId="150" priority="311">
+    <cfRule type="expression" dxfId="153" priority="321">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80">
-    <cfRule type="expression" dxfId="149" priority="309">
+    <cfRule type="expression" dxfId="152" priority="319">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G85">
-    <cfRule type="expression" dxfId="148" priority="306">
+    <cfRule type="expression" dxfId="151" priority="316">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="147" priority="163">
+    <cfRule type="expression" dxfId="150" priority="173">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J85:V85">
-    <cfRule type="expression" dxfId="146" priority="301">
+    <cfRule type="expression" dxfId="149" priority="311">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85 E85:F85">
-    <cfRule type="expression" dxfId="145" priority="303">
+    <cfRule type="expression" dxfId="148" priority="313">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K85:V85">
-    <cfRule type="expression" dxfId="144" priority="302">
+    <cfRule type="expression" dxfId="147" priority="312">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="expression" dxfId="143" priority="300">
+    <cfRule type="expression" dxfId="146" priority="310">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="expression" dxfId="142" priority="298">
+    <cfRule type="expression" dxfId="145" priority="308">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G86">
-    <cfRule type="expression" dxfId="141" priority="296">
+    <cfRule type="expression" dxfId="144" priority="306">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="140" priority="153">
+    <cfRule type="expression" dxfId="143" priority="163">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J86:V86">
-    <cfRule type="expression" dxfId="139" priority="291">
+    <cfRule type="expression" dxfId="142" priority="301">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86 E86:F86">
-    <cfRule type="expression" dxfId="138" priority="293">
+    <cfRule type="expression" dxfId="141" priority="303">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K86:V86">
-    <cfRule type="expression" dxfId="137" priority="292">
+    <cfRule type="expression" dxfId="140" priority="302">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="expression" dxfId="136" priority="290">
+    <cfRule type="expression" dxfId="139" priority="300">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87">
-    <cfRule type="expression" dxfId="135" priority="288">
+    <cfRule type="expression" dxfId="138" priority="298">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87">
-    <cfRule type="expression" dxfId="134" priority="287">
+    <cfRule type="expression" dxfId="137" priority="297">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88">
-    <cfRule type="expression" dxfId="133" priority="285">
+    <cfRule type="expression" dxfId="136" priority="295">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="132" priority="142">
+    <cfRule type="expression" dxfId="135" priority="152">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J88:V88">
-    <cfRule type="expression" dxfId="131" priority="280">
+    <cfRule type="expression" dxfId="134" priority="290">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88 E88:F88">
-    <cfRule type="expression" dxfId="130" priority="282">
+    <cfRule type="expression" dxfId="133" priority="292">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88:V88">
-    <cfRule type="expression" dxfId="129" priority="281">
+    <cfRule type="expression" dxfId="132" priority="291">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88">
-    <cfRule type="expression" dxfId="128" priority="279">
+    <cfRule type="expression" dxfId="131" priority="289">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43">
-    <cfRule type="expression" dxfId="127" priority="277">
+    <cfRule type="expression" dxfId="130" priority="287">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43 J43">
-    <cfRule type="expression" dxfId="126" priority="275">
+    <cfRule type="expression" dxfId="129" priority="285">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:K38">
-    <cfRule type="expression" dxfId="125" priority="272">
+    <cfRule type="expression" dxfId="128" priority="282">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="124" priority="270">
+    <cfRule type="expression" dxfId="127" priority="280">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="expression" dxfId="123" priority="128">
+    <cfRule type="expression" dxfId="126" priority="138">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53">
-    <cfRule type="expression" dxfId="122" priority="266">
+    <cfRule type="expression" dxfId="125" priority="276">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I68">
-    <cfRule type="expression" dxfId="121" priority="259">
+    <cfRule type="expression" dxfId="124" priority="269">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64">
-    <cfRule type="expression" dxfId="120" priority="263">
+    <cfRule type="expression" dxfId="123" priority="273">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I65">
-    <cfRule type="expression" dxfId="119" priority="262">
+    <cfRule type="expression" dxfId="122" priority="272">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I66">
-    <cfRule type="expression" dxfId="118" priority="261">
+    <cfRule type="expression" dxfId="121" priority="271">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I67">
-    <cfRule type="expression" dxfId="117" priority="260">
+    <cfRule type="expression" dxfId="120" priority="270">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="116" priority="257">
+    <cfRule type="expression" dxfId="119" priority="267">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="115" priority="256">
+    <cfRule type="expression" dxfId="118" priority="266">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I71">
-    <cfRule type="expression" dxfId="114" priority="255">
+    <cfRule type="expression" dxfId="117" priority="265">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I72">
-    <cfRule type="expression" dxfId="113" priority="253">
+    <cfRule type="expression" dxfId="116" priority="263">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I73">
-    <cfRule type="expression" dxfId="112" priority="252">
+    <cfRule type="expression" dxfId="115" priority="262">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74">
-    <cfRule type="expression" dxfId="111" priority="251">
+    <cfRule type="expression" dxfId="114" priority="261">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I75">
-    <cfRule type="expression" dxfId="110" priority="250">
+    <cfRule type="expression" dxfId="113" priority="260">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I78">
-    <cfRule type="expression" dxfId="109" priority="248">
+    <cfRule type="expression" dxfId="112" priority="258">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I79">
-    <cfRule type="expression" dxfId="108" priority="247">
+    <cfRule type="expression" dxfId="111" priority="257">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I80">
-    <cfRule type="expression" dxfId="107" priority="246">
+    <cfRule type="expression" dxfId="110" priority="256">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I83">
-    <cfRule type="expression" dxfId="106" priority="244">
+    <cfRule type="expression" dxfId="109" priority="254">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I85">
-    <cfRule type="expression" dxfId="105" priority="243">
+    <cfRule type="expression" dxfId="108" priority="253">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I86">
-    <cfRule type="expression" dxfId="104" priority="242">
+    <cfRule type="expression" dxfId="107" priority="252">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I87">
-    <cfRule type="expression" dxfId="103" priority="241">
+    <cfRule type="expression" dxfId="106" priority="251">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I88">
-    <cfRule type="expression" dxfId="102" priority="240">
+    <cfRule type="expression" dxfId="105" priority="250">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I89">
-    <cfRule type="expression" dxfId="101" priority="239">
+    <cfRule type="expression" dxfId="104" priority="249">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="expression" dxfId="100" priority="238">
+    <cfRule type="expression" dxfId="103" priority="248">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="99" priority="237">
+    <cfRule type="expression" dxfId="102" priority="247">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="98" priority="236">
+    <cfRule type="expression" dxfId="101" priority="246">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="expression" dxfId="97" priority="235">
+    <cfRule type="expression" dxfId="100" priority="245">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="96" priority="234">
+    <cfRule type="expression" dxfId="99" priority="244">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="95" priority="233">
+    <cfRule type="expression" dxfId="98" priority="243">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="94" priority="232">
+    <cfRule type="expression" dxfId="97" priority="242">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="93" priority="231">
+    <cfRule type="expression" dxfId="96" priority="241">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="92" priority="230">
+    <cfRule type="expression" dxfId="95" priority="240">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="91" priority="162">
+    <cfRule type="expression" dxfId="94" priority="172">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="expression" dxfId="90" priority="161">
+    <cfRule type="expression" dxfId="93" priority="171">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="expression" dxfId="89" priority="160">
+    <cfRule type="expression" dxfId="92" priority="170">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="88" priority="159">
+    <cfRule type="expression" dxfId="91" priority="169">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="87" priority="158">
+    <cfRule type="expression" dxfId="90" priority="168">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="86" priority="152">
+    <cfRule type="expression" dxfId="89" priority="162">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="expression" dxfId="88" priority="166">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="expression" dxfId="87" priority="165">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
+    <cfRule type="expression" dxfId="86" priority="164">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="expression" dxfId="85" priority="161">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="expression" dxfId="84" priority="160">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="expression" dxfId="83" priority="159">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="expression" dxfId="82" priority="158">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="expression" dxfId="81" priority="157">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30">
+    <cfRule type="expression" dxfId="80" priority="156">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="expression" dxfId="79" priority="155">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="expression" dxfId="78" priority="154">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
+    <cfRule type="expression" dxfId="77" priority="151">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50">
+    <cfRule type="expression" dxfId="76" priority="137">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
+    <cfRule type="expression" dxfId="75" priority="149">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="expression" dxfId="74" priority="148">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="expression" dxfId="73" priority="147">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38">
+    <cfRule type="expression" dxfId="72" priority="146">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="expression" dxfId="71" priority="145">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
+    <cfRule type="expression" dxfId="70" priority="144">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43">
+    <cfRule type="expression" dxfId="69" priority="143">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="expression" dxfId="68" priority="141">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I48">
+    <cfRule type="expression" dxfId="67" priority="139">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:V10">
+    <cfRule type="expression" dxfId="66" priority="129">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="expression" dxfId="65" priority="118">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H84">
+    <cfRule type="expression" dxfId="64" priority="127">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I84">
+    <cfRule type="expression" dxfId="63" priority="126">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:K9">
+    <cfRule type="expression" dxfId="62" priority="117">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="expression" dxfId="61" priority="116">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="60" priority="119">
+      <formula>K$1=$H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="59" priority="120">
+      <formula>K$1=$I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="58" priority="114">
+      <formula>K$1=$H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="57" priority="115">
+      <formula>K$1=$I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="expression" dxfId="56" priority="113">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:K10">
+    <cfRule type="expression" dxfId="55" priority="112">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="expression" dxfId="54" priority="111">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43">
+    <cfRule type="expression" dxfId="53" priority="104">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42:K42 H42">
+    <cfRule type="expression" dxfId="52" priority="99">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I42">
+    <cfRule type="expression" dxfId="51" priority="98">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="50" priority="89">
+      <formula>K$1=$H18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="49" priority="90">
+      <formula>K$1=$I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18 J18:K18">
+    <cfRule type="expression" dxfId="48" priority="91">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="expression" dxfId="47" priority="88">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K76">
+    <cfRule type="expression" dxfId="46" priority="86">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J76:K76">
+    <cfRule type="expression" dxfId="45" priority="85">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H76">
+    <cfRule type="expression" dxfId="44" priority="84">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I76">
+    <cfRule type="expression" dxfId="43" priority="83">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40:K40 H40">
+    <cfRule type="expression" dxfId="42" priority="81">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="expression" dxfId="41" priority="80">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J81">
+    <cfRule type="expression" dxfId="40" priority="71">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H81">
+    <cfRule type="expression" dxfId="39" priority="70">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I81">
+    <cfRule type="expression" dxfId="38" priority="69">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81:V81">
+    <cfRule type="expression" dxfId="37" priority="68">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K81:V81">
+    <cfRule type="expression" dxfId="36" priority="66">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47 G47">
+    <cfRule type="expression" dxfId="35" priority="64">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47:F47">
+    <cfRule type="expression" dxfId="34" priority="63">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47 E47 G47">
+    <cfRule type="expression" dxfId="33" priority="62">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47 E47 G47">
+    <cfRule type="expression" dxfId="32" priority="61">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47">
+    <cfRule type="expression" dxfId="31" priority="60">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J47:V47 H47">
+    <cfRule type="expression" dxfId="30" priority="59">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I47">
+    <cfRule type="expression" dxfId="29" priority="57">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46:F46">
+    <cfRule type="expression" dxfId="28" priority="52">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J46:V46 H46">
+    <cfRule type="expression" dxfId="27" priority="51">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I46">
+    <cfRule type="expression" dxfId="26" priority="49">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F61">
+    <cfRule type="expression" dxfId="25" priority="43">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G77">
+    <cfRule type="expression" dxfId="24" priority="39">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K77">
+    <cfRule type="expression" dxfId="23" priority="29">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J77:K77">
+    <cfRule type="expression" dxfId="22" priority="28">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H77">
+    <cfRule type="expression" dxfId="21" priority="27">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I77">
+    <cfRule type="expression" dxfId="20" priority="26">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L77:V77">
+    <cfRule type="expression" dxfId="19" priority="33">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L77:V77">
+    <cfRule type="expression" dxfId="18" priority="31">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L77:V77">
+    <cfRule type="expression" dxfId="17" priority="30">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45:G45">
+    <cfRule type="expression" dxfId="16" priority="25">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="expression" dxfId="15" priority="24">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45:F45">
+    <cfRule type="expression" dxfId="14" priority="23">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J45:V45 H45">
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I45">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F83">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58:G58">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="expression" dxfId="85" priority="156">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="expression" dxfId="84" priority="155">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="83" priority="154">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="expression" dxfId="82" priority="151">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
-    <cfRule type="expression" dxfId="81" priority="150">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
-    <cfRule type="expression" dxfId="80" priority="149">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="79" priority="148">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="78" priority="147">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="expression" dxfId="77" priority="146">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="expression" dxfId="76" priority="145">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="75" priority="144">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="74" priority="141">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I50">
-    <cfRule type="expression" dxfId="73" priority="127">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="expression" dxfId="72" priority="139">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
-    <cfRule type="expression" dxfId="71" priority="138">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="expression" dxfId="70" priority="137">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="69" priority="136">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="expression" dxfId="68" priority="135">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
-    <cfRule type="expression" dxfId="67" priority="134">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="66" priority="133">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="65" priority="131">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="64" priority="129">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L9:V10">
-    <cfRule type="expression" dxfId="63" priority="119">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="62" priority="108">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H84">
-    <cfRule type="expression" dxfId="61" priority="117">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I84">
-    <cfRule type="expression" dxfId="60" priority="116">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:K9">
-    <cfRule type="expression" dxfId="59" priority="107">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="58" priority="106">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="57" priority="109">
-      <formula>K$1=$H9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="56" priority="110">
-      <formula>K$1=$I9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="55" priority="104">
-      <formula>K$1=$H10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="54" priority="105">
-      <formula>K$1=$I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="53" priority="103">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
-    <cfRule type="expression" dxfId="52" priority="102">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="51" priority="101">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="50" priority="94">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J42:K42 H42">
-    <cfRule type="expression" dxfId="49" priority="89">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="48" priority="88">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="47" priority="79">
-      <formula>K$1=$H18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="46" priority="80">
-      <formula>K$1=$I18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18 J18:K18">
-    <cfRule type="expression" dxfId="45" priority="81">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="44" priority="78">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K76">
-    <cfRule type="expression" dxfId="43" priority="76">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J76:K76">
-    <cfRule type="expression" dxfId="42" priority="75">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H76">
-    <cfRule type="expression" dxfId="41" priority="74">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="expression" dxfId="40" priority="73">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J40:K40 H40">
-    <cfRule type="expression" dxfId="39" priority="71">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="38" priority="70">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J81">
-    <cfRule type="expression" dxfId="37" priority="61">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H81">
-    <cfRule type="expression" dxfId="36" priority="60">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I81">
-    <cfRule type="expression" dxfId="35" priority="59">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="34" priority="58">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K81:V81">
-    <cfRule type="expression" dxfId="33" priority="56">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47 G47">
-    <cfRule type="expression" dxfId="32" priority="54">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47:F47">
-    <cfRule type="expression" dxfId="31" priority="53">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47 E47 G47">
-    <cfRule type="expression" dxfId="30" priority="52">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47 E47 G47">
-    <cfRule type="expression" dxfId="29" priority="51">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
-    <cfRule type="expression" dxfId="28" priority="50">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J47:V47 H47">
-    <cfRule type="expression" dxfId="27" priority="49">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="26" priority="47">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21 E21:G21">
-    <cfRule type="expression" dxfId="25" priority="46">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46:F46">
-    <cfRule type="expression" dxfId="24" priority="42">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J46:V46 H46">
-    <cfRule type="expression" dxfId="23" priority="41">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="22" priority="39">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:V21">
-    <cfRule type="expression" dxfId="21" priority="36">
-      <formula>K$1=$H21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="expression" dxfId="20" priority="37">
-      <formula>K$1=$I21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L21:V21">
-    <cfRule type="expression" dxfId="19" priority="38">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21 J21:K21">
-    <cfRule type="expression" dxfId="18" priority="35">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="expression" dxfId="17" priority="34">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F61">
-    <cfRule type="expression" dxfId="16" priority="33">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G77">
-    <cfRule type="expression" dxfId="15" priority="29">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K77">
-    <cfRule type="expression" dxfId="14" priority="19">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J77:K77">
-    <cfRule type="expression" dxfId="13" priority="18">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="12" priority="17">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I77">
-    <cfRule type="expression" dxfId="11" priority="16">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="10" priority="23">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="9" priority="21">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L77:V77">
-    <cfRule type="expression" dxfId="8" priority="20">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45:G45">
-    <cfRule type="expression" dxfId="7" priority="15">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
-    <cfRule type="expression" dxfId="6" priority="14">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45:F45">
-    <cfRule type="expression" dxfId="5" priority="13">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K45:V45">
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>K$1=$H45</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J45:V45 H45">
-    <cfRule type="expression" dxfId="3" priority="5">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F83">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B58:G58">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:G19">
+    <cfRule type="expression" dxfId="8" priority="10">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19 E19:G19">
+    <cfRule type="expression" dxfId="7" priority="9">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:V19">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>L$1=$H19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:V19">
+    <cfRule type="expression" dxfId="5" priority="8">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:V19">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:V19">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>L$1=#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>K$1=$H19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>K$1=$I19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19 J19:K19">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G21" r:id="rId1" xr:uid="{441BD375-4CFE-1440-B1DD-3FDA85827C47}"/>
+    <hyperlink ref="G19" r:id="rId1" xr:uid="{8A228858-5429-5F4D-B04A-382FDC7D00CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Move DarthHemRhoid to ART payout
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tm/Documents/Code/swgoh-squad-arena-payout-bot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1566DDBC-19DD-DB4F-A650-8C781BC76CBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF267A4E-AAD6-E046-B393-60D982E0AB9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59920" yWindow="2440" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1223,7 +1223,57 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="287">
+  <dxfs count="294">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF920000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3571,7 +3621,7 @@
   <dimension ref="A1:V90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7132,13 +7182,13 @@
     <row r="47" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="55"/>
       <c r="B47" s="18" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="C47" s="7">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D47" s="7">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E47" s="14" t="s">
         <v>27</v>
@@ -7146,8 +7196,8 @@
       <c r="F47" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G47" s="29" t="s">
-        <v>163</v>
+      <c r="G47" s="22" t="s">
+        <v>147</v>
       </c>
       <c r="H47" s="29" t="s">
         <v>216</v>
@@ -7210,22 +7260,22 @@
     <row r="48" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="55"/>
       <c r="B48" s="18" t="s">
-        <v>238</v>
+        <v>60</v>
       </c>
       <c r="C48" s="7">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D48" s="7">
-        <v>45</v>
-      </c>
-      <c r="E48" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>76</v>
+        <v>44</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="G48" s="29" t="s">
-        <v>239</v>
+        <v>163</v>
       </c>
       <c r="H48" s="29" t="s">
         <v>216</v>
@@ -7288,22 +7338,22 @@
     <row r="49" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="55"/>
       <c r="B49" s="18" t="s">
-        <v>108</v>
+        <v>238</v>
       </c>
       <c r="C49" s="7">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D49" s="7">
-        <v>46</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>70</v>
+        <v>45</v>
+      </c>
+      <c r="E49" s="33" t="s">
+        <v>75</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>119</v>
+        <v>76</v>
+      </c>
+      <c r="G49" s="29" t="s">
+        <v>239</v>
       </c>
       <c r="H49" s="29" t="s">
         <v>216</v>
@@ -7363,100 +7413,100 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="50" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="55"/>
       <c r="B50" s="18" t="s">
-        <v>217</v>
+        <v>108</v>
       </c>
       <c r="C50" s="7">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D50" s="7">
-        <v>48</v>
-      </c>
-      <c r="E50" s="20"/>
+        <v>46</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>70</v>
+      </c>
       <c r="F50" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="G50" s="29"/>
+        <v>71</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>119</v>
+      </c>
       <c r="H50" s="29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I50" s="23">
-        <v>0.91666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="J50" s="26" t="s">
         <v>14</v>
       </c>
       <c r="K50" s="25">
         <f>$I50+Sheet2!B$1/24</f>
-        <v>1.3333333333333333</v>
+        <v>1.2916666666666667</v>
       </c>
       <c r="L50" s="23">
         <f>$I50+Sheet2!B$2/24</f>
-        <v>1.2916666666666665</v>
+        <v>1.25</v>
       </c>
       <c r="M50" s="23">
         <f>$I50+Sheet2!B$3/24</f>
-        <v>1.25</v>
+        <v>1.2083333333333333</v>
       </c>
       <c r="N50" s="23">
         <f>$I50+Sheet2!B$4/24</f>
-        <v>1.0416666666666665</v>
+        <v>1</v>
       </c>
       <c r="O50" s="23">
         <f>$I50+Sheet2!B$5/24</f>
-        <v>1.0416666666666665</v>
+        <v>1</v>
       </c>
       <c r="P50" s="23">
         <f>$I50+Sheet2!B$6/24</f>
-        <v>1.0416666666666665</v>
+        <v>1</v>
       </c>
       <c r="Q50" s="23">
         <f>$I50+Sheet2!B$7/24</f>
-        <v>1</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="R50" s="23">
         <f>$I50+Sheet2!B$8/24</f>
-        <v>0.95833333333333326</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="S50" s="23">
         <f>$I50+Sheet2!B$9/24</f>
-        <v>0.75</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="T50" s="23">
         <f>$I50+Sheet2!B$10/24</f>
-        <v>0.70833333333333326</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="U50" s="23">
         <f>$I50+Sheet2!B$11/24</f>
-        <v>0.66666666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="V50" s="23">
         <f>$I50+Sheet2!B$12/24</f>
-        <v>0.625</v>
+        <v>0.58333333333333326</v>
       </c>
     </row>
     <row r="51" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="55"/>
       <c r="B51" s="18" t="s">
-        <v>30</v>
+        <v>217</v>
       </c>
       <c r="C51" s="7">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" s="7">
-        <v>49</v>
-      </c>
-      <c r="E51" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>157</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E51" s="20"/>
+      <c r="F51" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G51" s="29"/>
       <c r="H51" s="29" t="s">
         <v>218</v>
       </c>
@@ -7516,99 +7566,99 @@
       </c>
     </row>
     <row r="52" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="56"/>
+      <c r="A52" s="55"/>
       <c r="B52" s="18" t="s">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="C52" s="7">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D52" s="7">
-        <v>50</v>
-      </c>
-      <c r="E52" s="20"/>
-      <c r="F52" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="G52" s="29"/>
+        <v>49</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>157</v>
+      </c>
       <c r="H52" s="29" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I52" s="23">
-        <v>0.95833333333333337</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="J52" s="26" t="s">
         <v>14</v>
       </c>
       <c r="K52" s="25">
         <f>$I52+Sheet2!B$1/24</f>
-        <v>1.375</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="L52" s="23">
         <f>$I52+Sheet2!B$2/24</f>
-        <v>1.3333333333333335</v>
+        <v>1.2916666666666665</v>
       </c>
       <c r="M52" s="23">
         <f>$I52+Sheet2!B$3/24</f>
-        <v>1.2916666666666667</v>
+        <v>1.25</v>
       </c>
       <c r="N52" s="23">
         <f>$I52+Sheet2!B$4/24</f>
-        <v>1.0833333333333335</v>
+        <v>1.0416666666666665</v>
       </c>
       <c r="O52" s="23">
         <f>$I52+Sheet2!B$5/24</f>
-        <v>1.0833333333333335</v>
+        <v>1.0416666666666665</v>
       </c>
       <c r="P52" s="23">
         <f>$I52+Sheet2!B$6/24</f>
-        <v>1.0833333333333335</v>
+        <v>1.0416666666666665</v>
       </c>
       <c r="Q52" s="23">
         <f>$I52+Sheet2!B$7/24</f>
-        <v>1.0416666666666667</v>
+        <v>1</v>
       </c>
       <c r="R52" s="23">
         <f>$I52+Sheet2!B$8/24</f>
-        <v>1</v>
+        <v>0.95833333333333326</v>
       </c>
       <c r="S52" s="23">
         <f>$I52+Sheet2!B$9/24</f>
-        <v>0.79166666666666674</v>
+        <v>0.75</v>
       </c>
       <c r="T52" s="23">
         <f>$I52+Sheet2!B$10/24</f>
-        <v>0.75</v>
+        <v>0.70833333333333326</v>
       </c>
       <c r="U52" s="23">
         <f>$I52+Sheet2!B$11/24</f>
-        <v>0.70833333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="V52" s="23">
         <f>$I52+Sheet2!B$12/24</f>
-        <v>0.66666666666666674</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="53" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="56"/>
       <c r="B53" s="18" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="C53" s="7">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D53" s="7">
-        <v>51</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F53" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G53" s="22" t="s">
-        <v>147</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E53" s="20"/>
+      <c r="F53" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="G53" s="29"/>
       <c r="H53" s="29" t="s">
         <v>220</v>
       </c>
@@ -10527,1449 +10577,1484 @@
     <sortCondition ref="D2:D73"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
-    <mergeCell ref="A26:A51"/>
-    <mergeCell ref="A52:A89"/>
+    <mergeCell ref="A26:A52"/>
+    <mergeCell ref="A53:A89"/>
   </mergeCells>
-  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K20:V21 K23:V43 K45:V90">
-    <cfRule type="expression" dxfId="286" priority="694">
+  <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K20:V21 K23:V43 K45:V46 K48:V90">
+    <cfRule type="expression" dxfId="293" priority="701">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K17:V17 K20:V20 K24:V24 K25:K33 K21 K23">
-    <cfRule type="expression" dxfId="285" priority="696">
+    <cfRule type="expression" dxfId="292" priority="703">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K54:V54 G54 G66 G74 G90 E64:G64 G31 B75 E75:G75 B3 E3:H3 H7 L10:V10 E24:H24 E32:G33 J24:V24 E34:H34 J34:V38 E51:G51 J51:V51 L41:V41 K88:V88 G88 K80:V81 K84:V85 K90:V90 L39:V39 E35:G39 E52:V53 H2 J2:V3 E41:G41 B85 J11:V14 J85:V85 B5 E55:V58 L16:V16 L43:V43 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J46:V46 L77:V77 B9:B14 E18:G18 E9:G10 E17:H17 E85:G85 E63:V63 E67:G67 B41 B82 B43:B44 G76:G81 E25:G30 E5:G5 E82:G82 E77:G78 L25:V33 L21:V21 G68:G71 E46:H46 B67:B69 B77:B78 B46:B48 C4:D18 E47:G48 B51:B64 B72:B73 E72:G73 L66:V75 E21:G23 B21:B39 E43:G44 C20:D90 L23:V23 G59:V62">
-    <cfRule type="expression" dxfId="284" priority="700">
+  <conditionalFormatting sqref="K54:V54 G54 G66 G74 G90 E64:G64 G31 B75 E75:G75 B3 E3:H3 H7 L10:V10 E24:H24 E32:G33 J24:V24 E34:H34 J34:V38 E52:G52 J52:V52 L41:V41 K88:V88 G88 K80:V81 K84:V85 K90:V90 L39:V39 E35:G39 E53:V53 H2 J2:V3 E41:G41 B85 J11:V14 J85:V85 B5 E55:V58 L16:V16 L43:V43 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J46:V46 L77:V77 B9:B14 E18:G18 E9:G10 E17:H17 E85:G85 E63:V63 E67:G67 B41 B82 B43:B44 G76:G81 E25:G30 E5:G5 E82:G82 E77:G78 L25:V33 L21:V21 G68:G71 E46:H46 B67:B69 B77:B78 B46 C4:D18 E48:G49 B72:B73 E72:G73 L66:V75 E21:G23 B21:B39 E43:G44 C20:D46 L23:V23 G59:V62 B48:B49 B52:B64 C48:D90">
+    <cfRule type="expression" dxfId="291" priority="707">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66 L66:V66">
-    <cfRule type="expression" dxfId="283" priority="677">
+    <cfRule type="expression" dxfId="290" priority="684">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71 L71:V71">
-    <cfRule type="expression" dxfId="282" priority="673">
+    <cfRule type="expression" dxfId="289" priority="680">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74 L74:V74">
-    <cfRule type="expression" dxfId="281" priority="671">
+    <cfRule type="expression" dxfId="288" priority="678">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70 L70:V70">
-    <cfRule type="expression" dxfId="280" priority="669">
+    <cfRule type="expression" dxfId="287" priority="676">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88 K88:V88 E88:F88">
-    <cfRule type="expression" dxfId="279" priority="665">
+    <cfRule type="expression" dxfId="286" priority="672">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="expression" dxfId="278" priority="663">
+    <cfRule type="expression" dxfId="285" priority="670">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74">
-    <cfRule type="expression" dxfId="277" priority="660">
+    <cfRule type="expression" dxfId="284" priority="667">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70">
-    <cfRule type="expression" dxfId="276" priority="659">
+    <cfRule type="expression" dxfId="283" priority="666">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84:B85 J84:V85">
-    <cfRule type="expression" dxfId="275" priority="656">
+    <cfRule type="expression" dxfId="282" priority="663">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81:B82 J81:V81 E81:E82">
-    <cfRule type="expression" dxfId="274" priority="654">
+    <cfRule type="expression" dxfId="281" priority="661">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85:F85 E84">
-    <cfRule type="expression" dxfId="273" priority="652">
+    <cfRule type="expression" dxfId="280" priority="659">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80 J80:V80">
-    <cfRule type="expression" dxfId="272" priority="650">
+    <cfRule type="expression" dxfId="279" priority="657">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90 J90:V90 E90">
-    <cfRule type="expression" dxfId="271" priority="648">
+    <cfRule type="expression" dxfId="278" priority="655">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70">
-    <cfRule type="expression" dxfId="270" priority="640">
+    <cfRule type="expression" dxfId="277" priority="647">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64:V64">
-    <cfRule type="expression" dxfId="269" priority="580">
+    <cfRule type="expression" dxfId="276" priority="587">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F74">
-    <cfRule type="expression" dxfId="268" priority="602">
+    <cfRule type="expression" dxfId="275" priority="609">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76:B78 E76:F78">
-    <cfRule type="expression" dxfId="267" priority="566">
+    <cfRule type="expression" dxfId="274" priority="573">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="expression" dxfId="266" priority="587">
+    <cfRule type="expression" dxfId="273" priority="594">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65 L65:V65">
-    <cfRule type="expression" dxfId="265" priority="588">
+    <cfRule type="expression" dxfId="272" priority="595">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81:F82">
-    <cfRule type="expression" dxfId="264" priority="600">
+    <cfRule type="expression" dxfId="271" priority="607">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66">
-    <cfRule type="expression" dxfId="263" priority="596">
+    <cfRule type="expression" dxfId="270" priority="603">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E71:F71">
-    <cfRule type="expression" dxfId="262" priority="595">
+    <cfRule type="expression" dxfId="269" priority="602">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E80:F80">
-    <cfRule type="expression" dxfId="261" priority="593">
+    <cfRule type="expression" dxfId="268" priority="600">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L65:V65 G65">
-    <cfRule type="expression" dxfId="260" priority="590">
+    <cfRule type="expression" dxfId="267" priority="597">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:V7">
-    <cfRule type="expression" dxfId="259" priority="535">
+    <cfRule type="expression" dxfId="266" priority="542">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65">
-    <cfRule type="expression" dxfId="258" priority="584">
+    <cfRule type="expression" dxfId="265" priority="591">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64:V64">
-    <cfRule type="expression" dxfId="257" priority="581">
+    <cfRule type="expression" dxfId="264" priority="588">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:V10">
-    <cfRule type="expression" dxfId="256" priority="526">
+    <cfRule type="expression" dxfId="263" priority="533">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H14 J13:V14 L18:V18">
-    <cfRule type="expression" dxfId="255" priority="572">
+    <cfRule type="expression" dxfId="262" priority="579">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:V14 L18:V18">
-    <cfRule type="expression" dxfId="254" priority="573">
+    <cfRule type="expression" dxfId="261" priority="580">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:G3 B7 E7:G7">
-    <cfRule type="expression" dxfId="253" priority="567">
+    <cfRule type="expression" dxfId="260" priority="574">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K76:V76 L77:V77">
-    <cfRule type="expression" dxfId="252" priority="565">
+    <cfRule type="expression" dxfId="259" priority="572">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76:V76 L77:V77">
-    <cfRule type="expression" dxfId="251" priority="563">
+    <cfRule type="expression" dxfId="258" priority="570">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H76">
-    <cfRule type="expression" dxfId="250" priority="562">
+    <cfRule type="expression" dxfId="257" priority="569">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J79:V79">
-    <cfRule type="expression" dxfId="249" priority="557">
+    <cfRule type="expression" dxfId="256" priority="564">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79 E79:F79">
-    <cfRule type="expression" dxfId="248" priority="560">
+    <cfRule type="expression" dxfId="255" priority="567">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K79:V79">
-    <cfRule type="expression" dxfId="247" priority="559">
+    <cfRule type="expression" dxfId="254" priority="566">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79">
-    <cfRule type="expression" dxfId="246" priority="556">
+    <cfRule type="expression" dxfId="253" priority="563">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="245" priority="549">
+    <cfRule type="expression" dxfId="252" priority="556">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:F31">
-    <cfRule type="expression" dxfId="244" priority="554">
+    <cfRule type="expression" dxfId="251" priority="561">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45 E45 L45:V45 G45">
-    <cfRule type="expression" dxfId="243" priority="553">
+    <cfRule type="expression" dxfId="250" priority="560">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4 E4:G4">
-    <cfRule type="expression" dxfId="242" priority="548">
+    <cfRule type="expression" dxfId="249" priority="555">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="241" priority="547">
+    <cfRule type="expression" dxfId="248" priority="554">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 E6:H6 J6:V6">
-    <cfRule type="expression" dxfId="240" priority="545">
+    <cfRule type="expression" dxfId="247" priority="552">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:V5">
-    <cfRule type="expression" dxfId="239" priority="542">
+    <cfRule type="expression" dxfId="246" priority="549">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:L4">
-    <cfRule type="expression" dxfId="238" priority="537">
+    <cfRule type="expression" dxfId="245" priority="544">
       <formula>K$1=$H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:V4">
-    <cfRule type="expression" dxfId="237" priority="538">
+    <cfRule type="expression" dxfId="244" priority="545">
       <formula>K$1=$I4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:V4">
-    <cfRule type="expression" dxfId="236" priority="539">
+    <cfRule type="expression" dxfId="243" priority="546">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="235" priority="532">
+    <cfRule type="expression" dxfId="242" priority="539">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 E8:G10">
-    <cfRule type="expression" dxfId="234" priority="531">
+    <cfRule type="expression" dxfId="241" priority="538">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:K8">
-    <cfRule type="expression" dxfId="233" priority="529">
+    <cfRule type="expression" dxfId="240" priority="536">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:H15 J15:V15">
-    <cfRule type="expression" dxfId="232" priority="521">
+    <cfRule type="expression" dxfId="239" priority="528">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15 J15:V15">
-    <cfRule type="expression" dxfId="231" priority="518">
+    <cfRule type="expression" dxfId="238" priority="525">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:V15">
-    <cfRule type="expression" dxfId="230" priority="519">
+    <cfRule type="expression" dxfId="237" priority="526">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:G15">
-    <cfRule type="expression" dxfId="229" priority="517">
+    <cfRule type="expression" dxfId="236" priority="524">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="228" priority="514">
+    <cfRule type="expression" dxfId="235" priority="521">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="227" priority="511">
+    <cfRule type="expression" dxfId="234" priority="518">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="226" priority="512">
+    <cfRule type="expression" dxfId="233" priority="519">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H50 J50:V50">
-    <cfRule type="expression" dxfId="225" priority="406">
+  <conditionalFormatting sqref="H51 J51:V51">
+    <cfRule type="expression" dxfId="232" priority="413">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20 E20:H20 J20:V20">
-    <cfRule type="expression" dxfId="224" priority="507">
+    <cfRule type="expression" dxfId="231" priority="514">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="223" priority="363">
+    <cfRule type="expression" dxfId="230" priority="370">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28 J28:K28">
-    <cfRule type="expression" dxfId="222" priority="469">
+    <cfRule type="expression" dxfId="229" priority="476">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64:J64">
-    <cfRule type="expression" dxfId="221" priority="401">
+    <cfRule type="expression" dxfId="228" priority="408">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21 J21:K21">
-    <cfRule type="expression" dxfId="220" priority="496">
+    <cfRule type="expression" dxfId="227" priority="503">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23 J23:K23">
-    <cfRule type="expression" dxfId="219" priority="491">
+    <cfRule type="expression" dxfId="226" priority="498">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="218" priority="396">
+    <cfRule type="expression" dxfId="225" priority="403">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="217" priority="395">
+    <cfRule type="expression" dxfId="224" priority="402">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25 J25:K25">
-    <cfRule type="expression" dxfId="216" priority="484">
+    <cfRule type="expression" dxfId="223" priority="491">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="215" priority="392">
+    <cfRule type="expression" dxfId="222" priority="399">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26 J26:K26">
-    <cfRule type="expression" dxfId="214" priority="479">
+    <cfRule type="expression" dxfId="221" priority="486">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66 J66">
-    <cfRule type="expression" dxfId="213" priority="390">
+    <cfRule type="expression" dxfId="220" priority="397">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27 J27:K27">
-    <cfRule type="expression" dxfId="212" priority="474">
+    <cfRule type="expression" dxfId="219" priority="481">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="211" priority="387">
+    <cfRule type="expression" dxfId="218" priority="394">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="210" priority="386">
+    <cfRule type="expression" dxfId="217" priority="393">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="209" priority="384">
+    <cfRule type="expression" dxfId="216" priority="391">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="208" priority="383">
+    <cfRule type="expression" dxfId="215" priority="390">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29 J29:K29">
-    <cfRule type="expression" dxfId="207" priority="464">
+    <cfRule type="expression" dxfId="214" priority="471">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="206" priority="380">
+    <cfRule type="expression" dxfId="213" priority="387">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30 J30:K30">
-    <cfRule type="expression" dxfId="205" priority="459">
+    <cfRule type="expression" dxfId="212" priority="466">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69 J69">
-    <cfRule type="expression" dxfId="204" priority="378">
+    <cfRule type="expression" dxfId="211" priority="385">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31 J31:K31">
-    <cfRule type="expression" dxfId="203" priority="454">
+    <cfRule type="expression" dxfId="210" priority="461">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32 J32:K32">
-    <cfRule type="expression" dxfId="202" priority="449">
+    <cfRule type="expression" dxfId="209" priority="456">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="201" priority="372">
+    <cfRule type="expression" dxfId="208" priority="379">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="200" priority="371">
+    <cfRule type="expression" dxfId="207" priority="378">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33 J33:K33">
-    <cfRule type="expression" dxfId="199" priority="444">
+    <cfRule type="expression" dxfId="206" priority="451">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="198" priority="368">
+    <cfRule type="expression" dxfId="205" priority="375">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71 J71">
-    <cfRule type="expression" dxfId="197" priority="366">
+    <cfRule type="expression" dxfId="204" priority="373">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="196" priority="432">
+    <cfRule type="expression" dxfId="203" priority="439">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="195" priority="364">
+    <cfRule type="expression" dxfId="202" priority="371">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="194" priority="429">
+    <cfRule type="expression" dxfId="201" priority="436">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="193" priority="426">
+    <cfRule type="expression" dxfId="200" priority="433">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72 J72">
-    <cfRule type="expression" dxfId="192" priority="362">
+    <cfRule type="expression" dxfId="199" priority="369">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="191" priority="423">
+    <cfRule type="expression" dxfId="198" priority="430">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40:B41 J40:V40 E40:H40 E41:G41 L41:V41">
-    <cfRule type="expression" dxfId="190" priority="420">
+    <cfRule type="expression" dxfId="197" priority="427">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42:V42 B42:B45 E45 E42:H42 G45 E43:G44 L43:V43 L45:V45">
-    <cfRule type="expression" dxfId="189" priority="416">
+    <cfRule type="expression" dxfId="196" priority="423">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="188" priority="360">
+    <cfRule type="expression" dxfId="195" priority="367">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="187" priority="359">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E50:G50 B50">
-    <cfRule type="expression" dxfId="186" priority="409">
+    <cfRule type="expression" dxfId="194" priority="366">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51:G51 B51">
+    <cfRule type="expression" dxfId="193" priority="416">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I83">
-    <cfRule type="expression" dxfId="185" priority="266">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
-    <cfRule type="expression" dxfId="184" priority="405">
+    <cfRule type="expression" dxfId="192" priority="273">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H52">
+    <cfRule type="expression" dxfId="191" priority="412">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54 J54">
-    <cfRule type="expression" dxfId="183" priority="404">
+    <cfRule type="expression" dxfId="190" priority="411">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K75">
-    <cfRule type="expression" dxfId="182" priority="352">
+    <cfRule type="expression" dxfId="189" priority="359">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="181" priority="355">
+    <cfRule type="expression" dxfId="188" priority="362">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73 J73">
-    <cfRule type="expression" dxfId="180" priority="358">
+    <cfRule type="expression" dxfId="187" priority="365">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65 J65">
-    <cfRule type="expression" dxfId="179" priority="394">
+    <cfRule type="expression" dxfId="186" priority="401">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="178" priority="391">
+    <cfRule type="expression" dxfId="185" priority="398">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="177" priority="388">
+    <cfRule type="expression" dxfId="184" priority="395">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68 J68">
-    <cfRule type="expression" dxfId="176" priority="382">
+    <cfRule type="expression" dxfId="183" priority="389">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="175" priority="379">
+    <cfRule type="expression" dxfId="182" priority="386">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70 J70">
-    <cfRule type="expression" dxfId="174" priority="370">
+    <cfRule type="expression" dxfId="181" priority="377">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="173" priority="367">
+    <cfRule type="expression" dxfId="180" priority="374">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="172" priority="356">
+    <cfRule type="expression" dxfId="179" priority="363">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74 J74">
-    <cfRule type="expression" dxfId="171" priority="354">
+    <cfRule type="expression" dxfId="178" priority="361">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K75">
-    <cfRule type="expression" dxfId="170" priority="351">
+    <cfRule type="expression" dxfId="177" priority="358">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75 J75">
-    <cfRule type="expression" dxfId="169" priority="350">
+    <cfRule type="expression" dxfId="176" priority="357">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G83">
-    <cfRule type="expression" dxfId="168" priority="341">
+    <cfRule type="expression" dxfId="175" priority="348">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J83:V83">
-    <cfRule type="expression" dxfId="167" priority="336">
+    <cfRule type="expression" dxfId="174" priority="343">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83 E83:F83">
-    <cfRule type="expression" dxfId="166" priority="338">
+    <cfRule type="expression" dxfId="173" priority="345">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K83:V83">
-    <cfRule type="expression" dxfId="165" priority="337">
+    <cfRule type="expression" dxfId="172" priority="344">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="expression" dxfId="164" priority="335">
+    <cfRule type="expression" dxfId="171" priority="342">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80">
-    <cfRule type="expression" dxfId="163" priority="332">
+    <cfRule type="expression" dxfId="170" priority="339">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81">
-    <cfRule type="expression" dxfId="162" priority="330">
+    <cfRule type="expression" dxfId="169" priority="337">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G86">
-    <cfRule type="expression" dxfId="161" priority="327">
+    <cfRule type="expression" dxfId="168" priority="334">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="160" priority="184">
+    <cfRule type="expression" dxfId="167" priority="191">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J86:V86">
-    <cfRule type="expression" dxfId="159" priority="322">
+    <cfRule type="expression" dxfId="166" priority="329">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86 E86:F86">
-    <cfRule type="expression" dxfId="158" priority="324">
+    <cfRule type="expression" dxfId="165" priority="331">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K86:V86">
-    <cfRule type="expression" dxfId="157" priority="323">
+    <cfRule type="expression" dxfId="164" priority="330">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="expression" dxfId="156" priority="321">
+    <cfRule type="expression" dxfId="163" priority="328">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H84">
-    <cfRule type="expression" dxfId="155" priority="319">
+    <cfRule type="expression" dxfId="162" priority="326">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G87">
-    <cfRule type="expression" dxfId="154" priority="317">
+    <cfRule type="expression" dxfId="161" priority="324">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="153" priority="174">
+    <cfRule type="expression" dxfId="160" priority="181">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87:V87">
-    <cfRule type="expression" dxfId="152" priority="312">
+    <cfRule type="expression" dxfId="159" priority="319">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87 E87:F87">
-    <cfRule type="expression" dxfId="151" priority="314">
+    <cfRule type="expression" dxfId="158" priority="321">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K87:V87">
-    <cfRule type="expression" dxfId="150" priority="313">
+    <cfRule type="expression" dxfId="157" priority="320">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87">
-    <cfRule type="expression" dxfId="149" priority="311">
+    <cfRule type="expression" dxfId="156" priority="318">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J88">
-    <cfRule type="expression" dxfId="148" priority="309">
+    <cfRule type="expression" dxfId="155" priority="316">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88">
-    <cfRule type="expression" dxfId="147" priority="308">
+    <cfRule type="expression" dxfId="154" priority="315">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G89">
-    <cfRule type="expression" dxfId="146" priority="306">
+    <cfRule type="expression" dxfId="153" priority="313">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="145" priority="163">
+    <cfRule type="expression" dxfId="152" priority="170">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J89:V89">
-    <cfRule type="expression" dxfId="144" priority="301">
+    <cfRule type="expression" dxfId="151" priority="308">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89 E89:F89">
-    <cfRule type="expression" dxfId="143" priority="303">
+    <cfRule type="expression" dxfId="150" priority="310">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K89:V89">
-    <cfRule type="expression" dxfId="142" priority="302">
+    <cfRule type="expression" dxfId="149" priority="309">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="expression" dxfId="141" priority="300">
+    <cfRule type="expression" dxfId="148" priority="307">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45">
-    <cfRule type="expression" dxfId="140" priority="298">
+    <cfRule type="expression" dxfId="147" priority="305">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45 J45">
-    <cfRule type="expression" dxfId="139" priority="296">
+    <cfRule type="expression" dxfId="146" priority="303">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39:K39">
-    <cfRule type="expression" dxfId="138" priority="293">
+    <cfRule type="expression" dxfId="145" priority="300">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="expression" dxfId="137" priority="291">
+    <cfRule type="expression" dxfId="144" priority="298">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I51">
+    <cfRule type="expression" dxfId="143" priority="156">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I54">
+    <cfRule type="expression" dxfId="142" priority="294">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I69">
+    <cfRule type="expression" dxfId="141" priority="287">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I65">
+    <cfRule type="expression" dxfId="140" priority="291">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I66">
+    <cfRule type="expression" dxfId="139" priority="290">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I67">
+    <cfRule type="expression" dxfId="138" priority="289">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I68">
+    <cfRule type="expression" dxfId="137" priority="288">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I70">
+    <cfRule type="expression" dxfId="136" priority="285">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I71">
+    <cfRule type="expression" dxfId="135" priority="284">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I72">
+    <cfRule type="expression" dxfId="134" priority="283">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I73">
+    <cfRule type="expression" dxfId="133" priority="281">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I74">
+    <cfRule type="expression" dxfId="132" priority="280">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I75">
+    <cfRule type="expression" dxfId="131" priority="279">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I76">
+    <cfRule type="expression" dxfId="130" priority="278">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I79">
+    <cfRule type="expression" dxfId="129" priority="276">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I80">
+    <cfRule type="expression" dxfId="128" priority="275">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I81">
+    <cfRule type="expression" dxfId="127" priority="274">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I84">
+    <cfRule type="expression" dxfId="126" priority="272">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I86">
+    <cfRule type="expression" dxfId="125" priority="271">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I87">
+    <cfRule type="expression" dxfId="124" priority="270">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I88">
+    <cfRule type="expression" dxfId="123" priority="269">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I89">
+    <cfRule type="expression" dxfId="122" priority="268">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I90">
+    <cfRule type="expression" dxfId="121" priority="267">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H90">
+    <cfRule type="expression" dxfId="120" priority="266">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="expression" dxfId="119" priority="265">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="expression" dxfId="118" priority="264">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="expression" dxfId="117" priority="263">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="expression" dxfId="116" priority="262">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6">
+    <cfRule type="expression" dxfId="115" priority="261">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="expression" dxfId="114" priority="260">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="expression" dxfId="113" priority="259">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="expression" dxfId="112" priority="258">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="expression" dxfId="111" priority="190">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="expression" dxfId="110" priority="189">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
+    <cfRule type="expression" dxfId="109" priority="188">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="expression" dxfId="108" priority="187">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="expression" dxfId="107" priority="186">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="expression" dxfId="106" priority="180">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="expression" dxfId="105" priority="184">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="expression" dxfId="104" priority="183">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="expression" dxfId="103" priority="182">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="expression" dxfId="102" priority="179">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="expression" dxfId="101" priority="178">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="expression" dxfId="100" priority="177">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="expression" dxfId="99" priority="176">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30">
+    <cfRule type="expression" dxfId="98" priority="175">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="expression" dxfId="97" priority="174">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="expression" dxfId="96" priority="173">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33">
+    <cfRule type="expression" dxfId="95" priority="172">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
+    <cfRule type="expression" dxfId="94" priority="169">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I52">
+    <cfRule type="expression" dxfId="93" priority="155">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="expression" dxfId="92" priority="167">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="expression" dxfId="91" priority="166">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38">
+    <cfRule type="expression" dxfId="90" priority="165">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="expression" dxfId="89" priority="164">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40">
+    <cfRule type="expression" dxfId="88" priority="163">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I42">
+    <cfRule type="expression" dxfId="87" priority="162">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I45">
+    <cfRule type="expression" dxfId="86" priority="161">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I46">
+    <cfRule type="expression" dxfId="85" priority="159">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:V10">
+    <cfRule type="expression" dxfId="84" priority="147">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="expression" dxfId="83" priority="136">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H85">
+    <cfRule type="expression" dxfId="82" priority="145">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I85">
+    <cfRule type="expression" dxfId="81" priority="144">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:K9">
+    <cfRule type="expression" dxfId="80" priority="135">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="expression" dxfId="79" priority="134">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="78" priority="137">
+      <formula>K$1=$H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="77" priority="138">
+      <formula>K$1=$I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="76" priority="132">
+      <formula>K$1=$H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="expression" dxfId="75" priority="133">
+      <formula>K$1=$I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="expression" dxfId="74" priority="131">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:K10">
+    <cfRule type="expression" dxfId="73" priority="130">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
+    <cfRule type="expression" dxfId="72" priority="129">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45">
+    <cfRule type="expression" dxfId="71" priority="122">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43:K43 H43">
+    <cfRule type="expression" dxfId="70" priority="117">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43">
+    <cfRule type="expression" dxfId="69" priority="116">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="68" priority="107">
+      <formula>K$1=$H18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="expression" dxfId="67" priority="108">
+      <formula>K$1=$I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18 J18:K18">
+    <cfRule type="expression" dxfId="66" priority="109">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="expression" dxfId="65" priority="106">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K77">
+    <cfRule type="expression" dxfId="64" priority="104">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J77:K77">
+    <cfRule type="expression" dxfId="63" priority="103">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H77">
+    <cfRule type="expression" dxfId="62" priority="102">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I77">
+    <cfRule type="expression" dxfId="61" priority="101">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41:K41 H41">
+    <cfRule type="expression" dxfId="60" priority="99">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
+    <cfRule type="expression" dxfId="59" priority="98">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J82">
+    <cfRule type="expression" dxfId="58" priority="89">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H82">
+    <cfRule type="expression" dxfId="57" priority="88">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I82">
+    <cfRule type="expression" dxfId="56" priority="87">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82:V82">
+    <cfRule type="expression" dxfId="55" priority="86">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K82:V82">
+    <cfRule type="expression" dxfId="54" priority="84">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50 G50">
+    <cfRule type="expression" dxfId="53" priority="82">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50:F50">
+    <cfRule type="expression" dxfId="52" priority="81">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50 E50 G50">
+    <cfRule type="expression" dxfId="51" priority="80">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50 E50 G50">
+    <cfRule type="expression" dxfId="50" priority="79">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F50">
+    <cfRule type="expression" dxfId="49" priority="78">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J50:V50 H50">
+    <cfRule type="expression" dxfId="48" priority="77">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50">
-    <cfRule type="expression" dxfId="136" priority="149">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I54">
-    <cfRule type="expression" dxfId="135" priority="287">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="134" priority="280">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
-    <cfRule type="expression" dxfId="133" priority="284">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I66">
-    <cfRule type="expression" dxfId="132" priority="283">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I67">
-    <cfRule type="expression" dxfId="131" priority="282">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I68">
-    <cfRule type="expression" dxfId="130" priority="281">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="129" priority="278">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I71">
-    <cfRule type="expression" dxfId="128" priority="277">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I72">
-    <cfRule type="expression" dxfId="127" priority="276">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I73">
-    <cfRule type="expression" dxfId="126" priority="274">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I74">
-    <cfRule type="expression" dxfId="125" priority="273">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I75">
-    <cfRule type="expression" dxfId="124" priority="272">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
-    <cfRule type="expression" dxfId="123" priority="271">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I79">
-    <cfRule type="expression" dxfId="122" priority="269">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I80">
-    <cfRule type="expression" dxfId="121" priority="268">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I81">
-    <cfRule type="expression" dxfId="120" priority="267">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I84">
-    <cfRule type="expression" dxfId="119" priority="265">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I86">
-    <cfRule type="expression" dxfId="118" priority="264">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I87">
-    <cfRule type="expression" dxfId="117" priority="263">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I88">
-    <cfRule type="expression" dxfId="116" priority="262">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I89">
-    <cfRule type="expression" dxfId="115" priority="261">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I90">
-    <cfRule type="expression" dxfId="114" priority="260">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H90">
-    <cfRule type="expression" dxfId="113" priority="259">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="112" priority="258">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="111" priority="257">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="expression" dxfId="110" priority="256">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="109" priority="255">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="108" priority="254">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="107" priority="253">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="106" priority="252">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="105" priority="251">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="expression" dxfId="104" priority="183">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="expression" dxfId="103" priority="182">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="expression" dxfId="102" priority="181">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="expression" dxfId="101" priority="180">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="100" priority="179">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="expression" dxfId="99" priority="173">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20">
-    <cfRule type="expression" dxfId="98" priority="177">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
-    <cfRule type="expression" dxfId="97" priority="176">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="96" priority="175">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26">
-    <cfRule type="expression" dxfId="95" priority="172">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
-    <cfRule type="expression" dxfId="94" priority="171">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="93" priority="170">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="92" priority="169">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="expression" dxfId="91" priority="168">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="expression" dxfId="90" priority="167">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="89" priority="166">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="88" priority="165">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="expression" dxfId="87" priority="162">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I51">
-    <cfRule type="expression" dxfId="86" priority="148">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
-    <cfRule type="expression" dxfId="85" priority="160">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="expression" dxfId="84" priority="159">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="83" priority="158">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
-    <cfRule type="expression" dxfId="82" priority="157">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
-    <cfRule type="expression" dxfId="81" priority="156">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" dxfId="80" priority="155">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
-    <cfRule type="expression" dxfId="79" priority="154">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="78" priority="152">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L9:V10">
-    <cfRule type="expression" dxfId="77" priority="140">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="76" priority="129">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H85">
-    <cfRule type="expression" dxfId="75" priority="138">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I85">
-    <cfRule type="expression" dxfId="74" priority="137">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:K9">
-    <cfRule type="expression" dxfId="73" priority="128">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="72" priority="127">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="71" priority="130">
-      <formula>K$1=$H9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="70" priority="131">
-      <formula>K$1=$I9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="69" priority="125">
-      <formula>K$1=$H10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="68" priority="126">
-      <formula>K$1=$I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="67" priority="124">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
-    <cfRule type="expression" dxfId="66" priority="123">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="65" priority="122">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45">
-    <cfRule type="expression" dxfId="64" priority="115">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J43:K43 H43">
-    <cfRule type="expression" dxfId="63" priority="110">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
-    <cfRule type="expression" dxfId="62" priority="109">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="61" priority="100">
-      <formula>K$1=$H18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="60" priority="101">
-      <formula>K$1=$I18</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18 J18:K18">
-    <cfRule type="expression" dxfId="59" priority="102">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="58" priority="99">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K77">
-    <cfRule type="expression" dxfId="57" priority="97">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J77:K77">
-    <cfRule type="expression" dxfId="56" priority="96">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="55" priority="95">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I77">
-    <cfRule type="expression" dxfId="54" priority="94">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J41:K41 H41">
-    <cfRule type="expression" dxfId="53" priority="92">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
-    <cfRule type="expression" dxfId="52" priority="91">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J82">
-    <cfRule type="expression" dxfId="51" priority="82">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H82">
-    <cfRule type="expression" dxfId="50" priority="81">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I82">
-    <cfRule type="expression" dxfId="49" priority="80">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82:V82">
-    <cfRule type="expression" dxfId="48" priority="79">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K82:V82">
-    <cfRule type="expression" dxfId="47" priority="77">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49 G49">
-    <cfRule type="expression" dxfId="46" priority="75">
+    <cfRule type="expression" dxfId="47" priority="75">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:F49">
-    <cfRule type="expression" dxfId="45" priority="74">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49 E49 G49">
-    <cfRule type="expression" dxfId="44" priority="73">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49 E49 G49">
-    <cfRule type="expression" dxfId="43" priority="72">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
-    <cfRule type="expression" dxfId="42" priority="71">
+    <cfRule type="expression" dxfId="46" priority="70">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49:V49 H49">
-    <cfRule type="expression" dxfId="41" priority="70">
+    <cfRule type="expression" dxfId="45" priority="69">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="expression" dxfId="40" priority="68">
+    <cfRule type="expression" dxfId="44" priority="67">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F61">
+    <cfRule type="expression" dxfId="43" priority="61">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G78">
+    <cfRule type="expression" dxfId="42" priority="57">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K78">
+    <cfRule type="expression" dxfId="41" priority="47">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J78:K78">
+    <cfRule type="expression" dxfId="40" priority="46">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H78">
+    <cfRule type="expression" dxfId="39" priority="45">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I78">
+    <cfRule type="expression" dxfId="38" priority="44">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L78:V78">
+    <cfRule type="expression" dxfId="37" priority="51">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L78:V78">
+    <cfRule type="expression" dxfId="36" priority="49">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L78:V78">
+    <cfRule type="expression" dxfId="35" priority="48">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48:G48">
+    <cfRule type="expression" dxfId="34" priority="43">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48">
+    <cfRule type="expression" dxfId="33" priority="42">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:F48">
-    <cfRule type="expression" dxfId="39" priority="63">
+    <cfRule type="expression" dxfId="32" priority="41">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:V48 H48">
-    <cfRule type="expression" dxfId="38" priority="62">
+    <cfRule type="expression" dxfId="31" priority="33">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48">
-    <cfRule type="expression" dxfId="37" priority="60">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F61">
-    <cfRule type="expression" dxfId="36" priority="54">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G78">
-    <cfRule type="expression" dxfId="35" priority="50">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K78">
-    <cfRule type="expression" dxfId="34" priority="40">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J78:K78">
-    <cfRule type="expression" dxfId="33" priority="39">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H78">
-    <cfRule type="expression" dxfId="32" priority="38">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I78">
-    <cfRule type="expression" dxfId="31" priority="37">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L78:V78">
-    <cfRule type="expression" dxfId="30" priority="44">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L78:V78">
-    <cfRule type="expression" dxfId="29" priority="42">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L78:V78">
-    <cfRule type="expression" dxfId="28" priority="41">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47:G47">
-    <cfRule type="expression" dxfId="27" priority="36">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="26" priority="35">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47:F47">
-    <cfRule type="expression" dxfId="25" priority="34">
-      <formula>MOD(ROW(),2)=1</formula>
+    <cfRule type="expression" dxfId="30" priority="31">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F84">
+    <cfRule type="expression" dxfId="29" priority="30">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:G22">
+    <cfRule type="expression" dxfId="28" priority="29">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="expression" dxfId="27" priority="19">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:G19">
+    <cfRule type="expression" dxfId="26" priority="28">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19 E19:G19">
+    <cfRule type="expression" dxfId="25" priority="27">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:V19">
+    <cfRule type="expression" dxfId="24" priority="25">
+      <formula>L$1=$H19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:V19">
+    <cfRule type="expression" dxfId="23" priority="26">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:V19">
+    <cfRule type="expression" dxfId="22" priority="23">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19:V19">
+    <cfRule type="expression" dxfId="21" priority="24">
+      <formula>L$1=#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="expression" dxfId="20" priority="20">
+      <formula>K$1=$H19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>K$1=$I19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19 J19:K19">
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K44:V44">
+    <cfRule type="expression" dxfId="17" priority="17">
+      <formula>K$1=$H44</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L44:V44">
+    <cfRule type="expression" dxfId="16" priority="18">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L44:V44">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J44:K44 H44">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22:V22">
+    <cfRule type="expression" dxfId="12" priority="11">
+      <formula>K$1=$H22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>K$1=$I22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L22:V22">
+    <cfRule type="expression" dxfId="10" priority="13">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22 J22:K22">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47:E47 G47">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47:V47">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>K$1=$H47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J47:V47 H47">
-    <cfRule type="expression" dxfId="24" priority="26">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="23" priority="24">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F84">
-    <cfRule type="expression" dxfId="22" priority="23">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22:G22">
-    <cfRule type="expression" dxfId="21" priority="22">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
-    <cfRule type="expression" dxfId="20" priority="12">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:G19">
-    <cfRule type="expression" dxfId="19" priority="21">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19 E19:G19">
-    <cfRule type="expression" dxfId="18" priority="20">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L19:V19">
-    <cfRule type="expression" dxfId="17" priority="18">
-      <formula>L$1=$H19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L19:V19">
-    <cfRule type="expression" dxfId="16" priority="19">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L19:V19">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L19:V19">
-    <cfRule type="expression" dxfId="14" priority="17">
-      <formula>L$1=#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19">
-    <cfRule type="expression" dxfId="13" priority="13">
-      <formula>K$1=$H19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19">
-    <cfRule type="expression" dxfId="12" priority="14">
-      <formula>K$1=$I19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H19 J19:K19">
-    <cfRule type="expression" dxfId="11" priority="15">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K44:V44">
-    <cfRule type="expression" dxfId="10" priority="10">
-      <formula>K$1=$H44</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L44:V44">
-    <cfRule type="expression" dxfId="9" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L44:V44">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J44:K44 H44">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K22:V22">
-    <cfRule type="expression" dxfId="5" priority="4">
-      <formula>K$1=$H22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K22">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>K$1=$I22</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L22:V22">
-    <cfRule type="expression" dxfId="3" priority="6">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22 J22:K22">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
+  <conditionalFormatting sqref="F47">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E62">
+  <conditionalFormatting sqref="F47">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Mark Mistborn as enemy
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB926E92-B4D8-E44F-8B38-368519D67FA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C538CA7C-A0F7-E94F-8B5B-67484EE15E11}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="59920" yWindow="2420" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1229,7 +1229,14 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="301">
+  <dxfs count="302">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3677,7 +3684,7 @@
   <dimension ref="A1:V91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7020,7 +7027,7 @@
         <v>27</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>151</v>
@@ -10711,11 +10718,11 @@
     <sortCondition ref="D2:D74"/>
   </sortState>
   <customSheetViews>
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" hiddenColumns="1">
       <selection sqref="A1:XFD1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -10724,342 +10731,347 @@
     <mergeCell ref="A54:A90"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:L3 L10:V10 K5:L8 L9 K11:L14 K13:V17 L18:V18 K20:V21 K23:V42 K44:V44 K46:V49 K51:V91">
-    <cfRule type="expression" dxfId="300" priority="715">
+    <cfRule type="expression" dxfId="301" priority="716">
       <formula>K$1=$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:V3 K5:V8 L9:V10 K11:V15 K16 K17:V17 K20:V20 K24:V24 K25:K33 K21 K23">
-    <cfRule type="expression" dxfId="299" priority="717">
+    <cfRule type="expression" dxfId="300" priority="718">
       <formula>K$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K55:V55 G55 G67 G75 G91 E65:G65 G31 B76 E76:G76 B3 E3:H3 H7 L10:V10 E24:H24 E32:G33 J24:V24 E34:H34 J34:V38 E53:G53 J53:V53 L41:V41 K89:V89 G89 K81:V82 K85:V86 K91:V91 L39:V39 E35:G39 E54:V54 H2 J2:V3 E41:G41 B86 J11:V14 J86:V86 B5 E56:V59 L16:V16 L44:V44 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J47:V47 L78:V78 B9:B14 E18:G18 E9:G10 E17:H17 E86:G86 E64:V64 E68:G68 B41 B83 B44:B45 G77:G82 E25:G30 E5:G5 E83:G83 E78:G79 L25:V33 L21:V21 G69:G72 E47:H47 B68:B70 B78:B79 C4:D18 B73:B74 E73:G74 L67:V76 E21:G23 B21:B39 E44:G45 C20:D42 L23:V23 G60:V63 B47:B50 B53:B65 C44:D91 E48:G50">
-    <cfRule type="expression" dxfId="298" priority="721">
+  <conditionalFormatting sqref="K55:V55 G55 G67 G75 G91 E65:G65 G31 B76 E76:G76 B3 E3:H3 H7 L10:V10 E24:H24 E32:G33 J24:V24 E34:H34 J34:V38 E53:G53 J53:V53 L41:V41 K89:V89 G89 K81:V82 K85:V86 K91:V91 L39:V39 E35:G39 E54:V54 H2 J2:V3 E41:G41 B86 J11:V14 J86:V86 B5 E56:V59 L16:V16 L44:V44 J17:V17 E11:H14 E16:G16 L18:V18 B16:B18 J47:V47 L78:V78 B9:B14 E18:G18 E9:G10 E17:H17 E86:G86 E64:V64 E68:G68 B41 B83 B44:B45 G77:G82 E25:G30 E5:G5 E83:G83 E78:G79 L25:V33 L21:V21 G69:G72 E47:H47 B68:B70 B78:B79 C4:D18 B73:B74 E73:G74 L67:V76 E21:G23 B21:B39 E45:G45 C20:D42 L23:V23 G60:V63 B47:B50 B53:B65 C44:D91 E48:G50 E44 G44">
+    <cfRule type="expression" dxfId="299" priority="722">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67 L67:V67">
-    <cfRule type="expression" dxfId="297" priority="698">
+    <cfRule type="expression" dxfId="298" priority="699">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72 L72:V72">
-    <cfRule type="expression" dxfId="296" priority="694">
+    <cfRule type="expression" dxfId="297" priority="695">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75 L75:V75">
-    <cfRule type="expression" dxfId="295" priority="692">
+    <cfRule type="expression" dxfId="296" priority="693">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71 L71:V71">
-    <cfRule type="expression" dxfId="294" priority="690">
+    <cfRule type="expression" dxfId="295" priority="691">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89 K89:V89 E89:F89">
-    <cfRule type="expression" dxfId="293" priority="686">
+    <cfRule type="expression" dxfId="294" priority="687">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="expression" dxfId="292" priority="684">
+    <cfRule type="expression" dxfId="293" priority="685">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E75">
+    <cfRule type="expression" dxfId="292" priority="682">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71">
     <cfRule type="expression" dxfId="291" priority="681">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E71">
-    <cfRule type="expression" dxfId="290" priority="680">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B85:B86 J85:V86">
-    <cfRule type="expression" dxfId="289" priority="677">
+    <cfRule type="expression" dxfId="290" priority="678">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82:B83 J82:V82 E82:E83">
-    <cfRule type="expression" dxfId="288" priority="675">
+    <cfRule type="expression" dxfId="289" priority="676">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86:F86 E85">
-    <cfRule type="expression" dxfId="287" priority="673">
+    <cfRule type="expression" dxfId="288" priority="674">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81 J81:V81">
-    <cfRule type="expression" dxfId="286" priority="671">
+    <cfRule type="expression" dxfId="287" priority="672">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91 J91:V91 E91">
-    <cfRule type="expression" dxfId="285" priority="669">
+    <cfRule type="expression" dxfId="286" priority="670">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71">
-    <cfRule type="expression" dxfId="284" priority="661">
+    <cfRule type="expression" dxfId="285" priority="662">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65:V65">
-    <cfRule type="expression" dxfId="283" priority="601">
+    <cfRule type="expression" dxfId="284" priority="602">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F75">
-    <cfRule type="expression" dxfId="282" priority="623">
+    <cfRule type="expression" dxfId="283" priority="624">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77:B79 E77:F79">
-    <cfRule type="expression" dxfId="281" priority="587">
+    <cfRule type="expression" dxfId="282" priority="588">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="expression" dxfId="280" priority="608">
+    <cfRule type="expression" dxfId="281" priority="609">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66 L66:V66">
-    <cfRule type="expression" dxfId="279" priority="609">
+    <cfRule type="expression" dxfId="280" priority="610">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F82:F83">
-    <cfRule type="expression" dxfId="278" priority="621">
+    <cfRule type="expression" dxfId="279" priority="622">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F67">
+    <cfRule type="expression" dxfId="278" priority="618">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E72:F72">
     <cfRule type="expression" dxfId="277" priority="617">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E72:F72">
-    <cfRule type="expression" dxfId="276" priority="616">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E81:F81">
-    <cfRule type="expression" dxfId="275" priority="614">
+    <cfRule type="expression" dxfId="276" priority="615">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L66:V66 G66">
-    <cfRule type="expression" dxfId="274" priority="611">
+    <cfRule type="expression" dxfId="275" priority="612">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:V7">
-    <cfRule type="expression" dxfId="273" priority="556">
+    <cfRule type="expression" dxfId="274" priority="557">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66">
-    <cfRule type="expression" dxfId="272" priority="605">
+    <cfRule type="expression" dxfId="273" priority="606">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65:V65">
-    <cfRule type="expression" dxfId="271" priority="602">
+    <cfRule type="expression" dxfId="272" priority="603">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:V10">
-    <cfRule type="expression" dxfId="270" priority="547">
+    <cfRule type="expression" dxfId="271" priority="548">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H14 J13:V14 L18:V18">
-    <cfRule type="expression" dxfId="269" priority="593">
+    <cfRule type="expression" dxfId="270" priority="594">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:V14 L18:V18">
-    <cfRule type="expression" dxfId="268" priority="594">
+    <cfRule type="expression" dxfId="269" priority="595">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:G3 B7 E7:G7">
-    <cfRule type="expression" dxfId="267" priority="588">
+    <cfRule type="expression" dxfId="268" priority="589">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77:V77 L78:V78">
-    <cfRule type="expression" dxfId="266" priority="586">
+    <cfRule type="expression" dxfId="267" priority="587">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J77:V77 L78:V78">
+    <cfRule type="expression" dxfId="266" priority="585">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H77">
     <cfRule type="expression" dxfId="265" priority="584">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="264" priority="583">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J80:V80">
-    <cfRule type="expression" dxfId="263" priority="578">
+    <cfRule type="expression" dxfId="264" priority="579">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80 E80:F80">
+    <cfRule type="expression" dxfId="263" priority="582">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K80:V80">
     <cfRule type="expression" dxfId="262" priority="581">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K80:V80">
-    <cfRule type="expression" dxfId="261" priority="580">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H80">
-    <cfRule type="expression" dxfId="260" priority="577">
+    <cfRule type="expression" dxfId="261" priority="578">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="259" priority="570">
+    <cfRule type="expression" dxfId="260" priority="571">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:F31">
+    <cfRule type="expression" dxfId="259" priority="576">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46 E46 L46:V46 G46">
     <cfRule type="expression" dxfId="258" priority="575">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B46 E46 L46:V46 G46">
-    <cfRule type="expression" dxfId="257" priority="574">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B4 E4:G4">
+    <cfRule type="expression" dxfId="257" priority="570">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
     <cfRule type="expression" dxfId="256" priority="569">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="255" priority="568">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B6 E6:H6 J6:V6">
-    <cfRule type="expression" dxfId="254" priority="566">
+    <cfRule type="expression" dxfId="255" priority="567">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:V5">
-    <cfRule type="expression" dxfId="253" priority="563">
+    <cfRule type="expression" dxfId="254" priority="564">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:L4">
-    <cfRule type="expression" dxfId="252" priority="558">
+    <cfRule type="expression" dxfId="253" priority="559">
       <formula>K$1=$H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:V4">
-    <cfRule type="expression" dxfId="251" priority="559">
+    <cfRule type="expression" dxfId="252" priority="560">
       <formula>K$1=$I4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:V4">
-    <cfRule type="expression" dxfId="250" priority="560">
+    <cfRule type="expression" dxfId="251" priority="561">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
+    <cfRule type="expression" dxfId="250" priority="554">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:B10 E8:G10">
     <cfRule type="expression" dxfId="249" priority="553">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:B10 E8:G10">
-    <cfRule type="expression" dxfId="248" priority="552">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J8:K8">
-    <cfRule type="expression" dxfId="247" priority="550">
+    <cfRule type="expression" dxfId="248" priority="551">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:H15 J15:V15">
-    <cfRule type="expression" dxfId="246" priority="542">
+    <cfRule type="expression" dxfId="247" priority="543">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15 J15:V15">
-    <cfRule type="expression" dxfId="245" priority="539">
+    <cfRule type="expression" dxfId="246" priority="540">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:V15">
-    <cfRule type="expression" dxfId="244" priority="540">
+    <cfRule type="expression" dxfId="245" priority="541">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 E15:G15">
-    <cfRule type="expression" dxfId="243" priority="538">
+    <cfRule type="expression" dxfId="244" priority="539">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="242" priority="535">
+    <cfRule type="expression" dxfId="243" priority="536">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16 J16:K16">
-    <cfRule type="expression" dxfId="241" priority="532">
+    <cfRule type="expression" dxfId="242" priority="533">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="expression" dxfId="240" priority="533">
+    <cfRule type="expression" dxfId="241" priority="534">
       <formula>K$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52 J52:V52">
-    <cfRule type="expression" dxfId="239" priority="427">
+    <cfRule type="expression" dxfId="240" priority="428">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20 E20:H20 J20:V20">
-    <cfRule type="expression" dxfId="238" priority="528">
+    <cfRule type="expression" dxfId="239" priority="529">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="237" priority="384">
+    <cfRule type="expression" dxfId="238" priority="385">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28 J28:K28">
-    <cfRule type="expression" dxfId="236" priority="490">
+    <cfRule type="expression" dxfId="237" priority="491">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65:J65">
-    <cfRule type="expression" dxfId="235" priority="422">
+    <cfRule type="expression" dxfId="236" priority="423">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21 J21:K21">
-    <cfRule type="expression" dxfId="234" priority="517">
+    <cfRule type="expression" dxfId="235" priority="518">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23 J23:K23">
-    <cfRule type="expression" dxfId="233" priority="512">
+    <cfRule type="expression" dxfId="234" priority="513">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K66">
+    <cfRule type="expression" dxfId="233" priority="418">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11068,43 +11080,43 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K66">
-    <cfRule type="expression" dxfId="231" priority="416">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H25 J25:K25">
-    <cfRule type="expression" dxfId="230" priority="505">
+    <cfRule type="expression" dxfId="231" priority="506">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="229" priority="413">
+    <cfRule type="expression" dxfId="230" priority="414">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26 J26:K26">
-    <cfRule type="expression" dxfId="228" priority="500">
+    <cfRule type="expression" dxfId="229" priority="501">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67 J67">
-    <cfRule type="expression" dxfId="227" priority="411">
+    <cfRule type="expression" dxfId="228" priority="412">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27 J27:K27">
-    <cfRule type="expression" dxfId="226" priority="495">
+    <cfRule type="expression" dxfId="227" priority="496">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
+    <cfRule type="expression" dxfId="226" priority="409">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H68 J68">
     <cfRule type="expression" dxfId="225" priority="408">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H68 J68">
-    <cfRule type="expression" dxfId="224" priority="407">
+  <conditionalFormatting sqref="K69">
+    <cfRule type="expression" dxfId="224" priority="406">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11113,38 +11125,38 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="expression" dxfId="222" priority="404">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H29 J29:K29">
-    <cfRule type="expression" dxfId="221" priority="485">
+    <cfRule type="expression" dxfId="222" priority="486">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="220" priority="401">
+    <cfRule type="expression" dxfId="221" priority="402">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30 J30:K30">
-    <cfRule type="expression" dxfId="219" priority="480">
+    <cfRule type="expression" dxfId="220" priority="481">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70 J70">
-    <cfRule type="expression" dxfId="218" priority="399">
+    <cfRule type="expression" dxfId="219" priority="400">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31 J31:K31">
-    <cfRule type="expression" dxfId="217" priority="475">
+    <cfRule type="expression" dxfId="218" priority="476">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32 J32:K32">
-    <cfRule type="expression" dxfId="216" priority="470">
+    <cfRule type="expression" dxfId="217" priority="471">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K71">
+    <cfRule type="expression" dxfId="216" priority="394">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11153,63 +11165,63 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="214" priority="392">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H33 J33:K33">
-    <cfRule type="expression" dxfId="213" priority="465">
+    <cfRule type="expression" dxfId="214" priority="466">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="212" priority="389">
+    <cfRule type="expression" dxfId="213" priority="390">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72 J72">
-    <cfRule type="expression" dxfId="211" priority="387">
+    <cfRule type="expression" dxfId="212" priority="388">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="210" priority="453">
+    <cfRule type="expression" dxfId="211" priority="454">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73">
-    <cfRule type="expression" dxfId="209" priority="385">
+    <cfRule type="expression" dxfId="210" priority="386">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="208" priority="450">
+    <cfRule type="expression" dxfId="209" priority="451">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="207" priority="447">
+    <cfRule type="expression" dxfId="208" priority="448">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73 J73">
-    <cfRule type="expression" dxfId="206" priority="383">
+    <cfRule type="expression" dxfId="207" priority="384">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="205" priority="444">
+    <cfRule type="expression" dxfId="206" priority="445">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40:B41 J40:V40 E40:H40 E41:G41 L41:V41">
-    <cfRule type="expression" dxfId="204" priority="441">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J42:V42 B42 E46 E42:H42 G46 E44:G45 L44:V44 L46:V46 B44:B46">
-    <cfRule type="expression" dxfId="203" priority="437">
+    <cfRule type="expression" dxfId="205" priority="442">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J42:V42 B42 E46 E42:H42 G46 E45:G45 L44:V44 L46:V46 B44:B46 E44 G44">
+    <cfRule type="expression" dxfId="204" priority="438">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K74">
+    <cfRule type="expression" dxfId="203" priority="382">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11218,717 +11230,717 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K74">
-    <cfRule type="expression" dxfId="201" priority="380">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E52:G52 B52">
-    <cfRule type="expression" dxfId="200" priority="430">
+    <cfRule type="expression" dxfId="201" priority="431">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I84">
-    <cfRule type="expression" dxfId="199" priority="287">
+    <cfRule type="expression" dxfId="200" priority="288">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
+    <cfRule type="expression" dxfId="199" priority="427">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H55 J55">
     <cfRule type="expression" dxfId="198" priority="426">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H55 J55">
-    <cfRule type="expression" dxfId="197" priority="425">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K76">
-    <cfRule type="expression" dxfId="196" priority="373">
+    <cfRule type="expression" dxfId="197" priority="374">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K75">
-    <cfRule type="expression" dxfId="195" priority="376">
+    <cfRule type="expression" dxfId="196" priority="377">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74 J74">
-    <cfRule type="expression" dxfId="194" priority="379">
+    <cfRule type="expression" dxfId="195" priority="380">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66 J66">
-    <cfRule type="expression" dxfId="193" priority="415">
+    <cfRule type="expression" dxfId="194" priority="416">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67">
-    <cfRule type="expression" dxfId="192" priority="412">
+    <cfRule type="expression" dxfId="193" priority="413">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="expression" dxfId="191" priority="409">
+    <cfRule type="expression" dxfId="192" priority="410">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69 J69">
-    <cfRule type="expression" dxfId="190" priority="403">
+    <cfRule type="expression" dxfId="191" priority="404">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="expression" dxfId="189" priority="400">
+    <cfRule type="expression" dxfId="190" priority="401">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71 J71">
-    <cfRule type="expression" dxfId="188" priority="391">
+    <cfRule type="expression" dxfId="189" priority="392">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="expression" dxfId="187" priority="388">
+    <cfRule type="expression" dxfId="188" priority="389">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K75">
-    <cfRule type="expression" dxfId="186" priority="377">
+    <cfRule type="expression" dxfId="187" priority="378">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75 J75">
-    <cfRule type="expression" dxfId="185" priority="375">
+    <cfRule type="expression" dxfId="186" priority="376">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K76">
+    <cfRule type="expression" dxfId="185" priority="373">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H76 J76">
     <cfRule type="expression" dxfId="184" priority="372">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H76 J76">
-    <cfRule type="expression" dxfId="183" priority="371">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G84">
-    <cfRule type="expression" dxfId="182" priority="362">
+    <cfRule type="expression" dxfId="183" priority="363">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J84:V84">
-    <cfRule type="expression" dxfId="181" priority="357">
+    <cfRule type="expression" dxfId="182" priority="358">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84 E84:F84">
+    <cfRule type="expression" dxfId="181" priority="360">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K84:V84">
     <cfRule type="expression" dxfId="180" priority="359">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K84:V84">
-    <cfRule type="expression" dxfId="179" priority="358">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H84">
-    <cfRule type="expression" dxfId="178" priority="356">
+    <cfRule type="expression" dxfId="179" priority="357">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81">
-    <cfRule type="expression" dxfId="177" priority="353">
+    <cfRule type="expression" dxfId="178" priority="354">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="expression" dxfId="176" priority="351">
+    <cfRule type="expression" dxfId="177" priority="352">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G87">
-    <cfRule type="expression" dxfId="175" priority="348">
+    <cfRule type="expression" dxfId="176" priority="349">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="174" priority="205">
+    <cfRule type="expression" dxfId="175" priority="206">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87:V87">
-    <cfRule type="expression" dxfId="173" priority="343">
+    <cfRule type="expression" dxfId="174" priority="344">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87 E87:F87">
+    <cfRule type="expression" dxfId="173" priority="346">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K87:V87">
     <cfRule type="expression" dxfId="172" priority="345">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K87:V87">
-    <cfRule type="expression" dxfId="171" priority="344">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H87">
-    <cfRule type="expression" dxfId="170" priority="342">
+    <cfRule type="expression" dxfId="171" priority="343">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="expression" dxfId="169" priority="340">
+    <cfRule type="expression" dxfId="170" priority="341">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88">
-    <cfRule type="expression" dxfId="168" priority="338">
+    <cfRule type="expression" dxfId="169" priority="339">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24">
-    <cfRule type="expression" dxfId="167" priority="195">
+    <cfRule type="expression" dxfId="168" priority="196">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J88:V88">
-    <cfRule type="expression" dxfId="166" priority="333">
+    <cfRule type="expression" dxfId="167" priority="334">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88 E88:F88">
+    <cfRule type="expression" dxfId="166" priority="336">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K88:V88">
     <cfRule type="expression" dxfId="165" priority="335">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K88:V88">
-    <cfRule type="expression" dxfId="164" priority="334">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H88">
-    <cfRule type="expression" dxfId="163" priority="332">
+    <cfRule type="expression" dxfId="164" priority="333">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J89">
+    <cfRule type="expression" dxfId="163" priority="331">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H89">
     <cfRule type="expression" dxfId="162" priority="330">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H89">
-    <cfRule type="expression" dxfId="161" priority="329">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G90">
-    <cfRule type="expression" dxfId="160" priority="327">
+    <cfRule type="expression" dxfId="161" priority="328">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34">
-    <cfRule type="expression" dxfId="159" priority="184">
+    <cfRule type="expression" dxfId="160" priority="185">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J90:V90">
-    <cfRule type="expression" dxfId="158" priority="322">
+    <cfRule type="expression" dxfId="159" priority="323">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90 E90:F90">
+    <cfRule type="expression" dxfId="158" priority="325">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K90:V90">
     <cfRule type="expression" dxfId="157" priority="324">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K90:V90">
-    <cfRule type="expression" dxfId="156" priority="323">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H90">
-    <cfRule type="expression" dxfId="155" priority="321">
+    <cfRule type="expression" dxfId="156" priority="322">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46">
-    <cfRule type="expression" dxfId="154" priority="319">
+    <cfRule type="expression" dxfId="155" priority="320">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46 J46">
-    <cfRule type="expression" dxfId="153" priority="317">
+    <cfRule type="expression" dxfId="154" priority="318">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39:K39">
-    <cfRule type="expression" dxfId="152" priority="314">
+    <cfRule type="expression" dxfId="153" priority="315">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="expression" dxfId="151" priority="312">
+    <cfRule type="expression" dxfId="152" priority="313">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52">
-    <cfRule type="expression" dxfId="150" priority="170">
+    <cfRule type="expression" dxfId="151" priority="171">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I55">
-    <cfRule type="expression" dxfId="149" priority="308">
+    <cfRule type="expression" dxfId="150" priority="309">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="148" priority="301">
+    <cfRule type="expression" dxfId="149" priority="302">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I66">
+    <cfRule type="expression" dxfId="148" priority="306">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I67">
     <cfRule type="expression" dxfId="147" priority="305">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I67">
+  <conditionalFormatting sqref="I68">
     <cfRule type="expression" dxfId="146" priority="304">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I68">
+  <conditionalFormatting sqref="I69">
     <cfRule type="expression" dxfId="145" priority="303">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I69">
-    <cfRule type="expression" dxfId="144" priority="302">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I71">
+    <cfRule type="expression" dxfId="144" priority="300">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I72">
     <cfRule type="expression" dxfId="143" priority="299">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I72">
+  <conditionalFormatting sqref="I73">
     <cfRule type="expression" dxfId="142" priority="298">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I73">
-    <cfRule type="expression" dxfId="141" priority="297">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I74">
+    <cfRule type="expression" dxfId="141" priority="296">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I75">
     <cfRule type="expression" dxfId="140" priority="295">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I75">
+  <conditionalFormatting sqref="I76">
     <cfRule type="expression" dxfId="139" priority="294">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I76">
+  <conditionalFormatting sqref="I77">
     <cfRule type="expression" dxfId="138" priority="293">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I77">
-    <cfRule type="expression" dxfId="137" priority="292">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I80">
+    <cfRule type="expression" dxfId="137" priority="291">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I81">
     <cfRule type="expression" dxfId="136" priority="290">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I81">
+  <conditionalFormatting sqref="I82">
     <cfRule type="expression" dxfId="135" priority="289">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I82">
-    <cfRule type="expression" dxfId="134" priority="288">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I85">
+    <cfRule type="expression" dxfId="134" priority="287">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I87">
     <cfRule type="expression" dxfId="133" priority="286">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87">
+  <conditionalFormatting sqref="I88">
     <cfRule type="expression" dxfId="132" priority="285">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88">
+  <conditionalFormatting sqref="I89">
     <cfRule type="expression" dxfId="131" priority="284">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I89">
+  <conditionalFormatting sqref="I90">
     <cfRule type="expression" dxfId="130" priority="283">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I90">
+  <conditionalFormatting sqref="I91">
     <cfRule type="expression" dxfId="129" priority="282">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I91">
+  <conditionalFormatting sqref="H91">
     <cfRule type="expression" dxfId="128" priority="281">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H91">
+  <conditionalFormatting sqref="I2">
     <cfRule type="expression" dxfId="127" priority="280">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I3">
     <cfRule type="expression" dxfId="126" priority="279">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
+  <conditionalFormatting sqref="I4">
     <cfRule type="expression" dxfId="125" priority="278">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
+  <conditionalFormatting sqref="I5">
     <cfRule type="expression" dxfId="124" priority="277">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
+  <conditionalFormatting sqref="I6">
     <cfRule type="expression" dxfId="123" priority="276">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
+  <conditionalFormatting sqref="I7">
     <cfRule type="expression" dxfId="122" priority="275">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
+  <conditionalFormatting sqref="I8">
     <cfRule type="expression" dxfId="121" priority="274">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
+  <conditionalFormatting sqref="I11">
     <cfRule type="expression" dxfId="120" priority="273">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="119" priority="272">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I13">
+    <cfRule type="expression" dxfId="119" priority="205">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
     <cfRule type="expression" dxfId="118" priority="204">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
+  <conditionalFormatting sqref="I15">
     <cfRule type="expression" dxfId="117" priority="203">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
+  <conditionalFormatting sqref="I16">
     <cfRule type="expression" dxfId="116" priority="202">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
+  <conditionalFormatting sqref="I17">
     <cfRule type="expression" dxfId="115" priority="201">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="expression" dxfId="114" priority="200">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="expression" dxfId="113" priority="194">
+    <cfRule type="expression" dxfId="114" priority="195">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
+    <cfRule type="expression" dxfId="113" priority="199">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
     <cfRule type="expression" dxfId="112" priority="198">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
+  <conditionalFormatting sqref="I23">
     <cfRule type="expression" dxfId="111" priority="197">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="110" priority="196">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I26">
+    <cfRule type="expression" dxfId="110" priority="194">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
     <cfRule type="expression" dxfId="109" priority="193">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27">
+  <conditionalFormatting sqref="I28">
     <cfRule type="expression" dxfId="108" priority="192">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
+  <conditionalFormatting sqref="I29">
     <cfRule type="expression" dxfId="107" priority="191">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
+  <conditionalFormatting sqref="I30">
     <cfRule type="expression" dxfId="106" priority="190">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
+  <conditionalFormatting sqref="I31">
     <cfRule type="expression" dxfId="105" priority="189">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
+  <conditionalFormatting sqref="I32">
     <cfRule type="expression" dxfId="104" priority="188">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
+  <conditionalFormatting sqref="I33">
     <cfRule type="expression" dxfId="103" priority="187">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="102" priority="186">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="expression" dxfId="101" priority="183">
+    <cfRule type="expression" dxfId="102" priority="184">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53">
-    <cfRule type="expression" dxfId="100" priority="169">
+    <cfRule type="expression" dxfId="101" priority="170">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
+    <cfRule type="expression" dxfId="100" priority="182">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
     <cfRule type="expression" dxfId="99" priority="181">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
+  <conditionalFormatting sqref="I38">
     <cfRule type="expression" dxfId="98" priority="180">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
+  <conditionalFormatting sqref="I39">
     <cfRule type="expression" dxfId="97" priority="179">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
+  <conditionalFormatting sqref="I40">
     <cfRule type="expression" dxfId="96" priority="178">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40">
+  <conditionalFormatting sqref="I42">
     <cfRule type="expression" dxfId="95" priority="177">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
+  <conditionalFormatting sqref="I46">
     <cfRule type="expression" dxfId="94" priority="176">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
-    <cfRule type="expression" dxfId="93" priority="175">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="expression" dxfId="92" priority="173">
+    <cfRule type="expression" dxfId="93" priority="174">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:V10">
-    <cfRule type="expression" dxfId="91" priority="161">
+    <cfRule type="expression" dxfId="92" priority="162">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="90" priority="150">
+    <cfRule type="expression" dxfId="91" priority="151">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
+    <cfRule type="expression" dxfId="90" priority="160">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I86">
     <cfRule type="expression" dxfId="89" priority="159">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I86">
-    <cfRule type="expression" dxfId="88" priority="158">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J9:K9">
+    <cfRule type="expression" dxfId="88" priority="150">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
     <cfRule type="expression" dxfId="87" priority="149">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="86" priority="148">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="85" priority="151">
+    <cfRule type="expression" dxfId="86" priority="152">
       <formula>K$1=$H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="84" priority="152">
+    <cfRule type="expression" dxfId="85" priority="153">
       <formula>K$1=$I9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="83" priority="146">
+    <cfRule type="expression" dxfId="84" priority="147">
       <formula>K$1=$H10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="82" priority="147">
+    <cfRule type="expression" dxfId="83" priority="148">
       <formula>K$1=$I10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
+    <cfRule type="expression" dxfId="82" priority="146">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:K10">
     <cfRule type="expression" dxfId="81" priority="145">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J10:K10">
+  <conditionalFormatting sqref="I10">
     <cfRule type="expression" dxfId="80" priority="144">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="79" priority="143">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F46">
-    <cfRule type="expression" dxfId="78" priority="136">
+    <cfRule type="expression" dxfId="79" priority="137">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:K44 H44">
+    <cfRule type="expression" dxfId="78" priority="132">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
     <cfRule type="expression" dxfId="77" priority="131">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
-    <cfRule type="expression" dxfId="76" priority="130">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="75" priority="121">
+    <cfRule type="expression" dxfId="76" priority="122">
       <formula>K$1=$H18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="74" priority="122">
+    <cfRule type="expression" dxfId="75" priority="123">
       <formula>K$1=$I18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18 J18:K18">
-    <cfRule type="expression" dxfId="73" priority="123">
+    <cfRule type="expression" dxfId="74" priority="124">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="expression" dxfId="72" priority="120">
+    <cfRule type="expression" dxfId="73" priority="121">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K78">
+    <cfRule type="expression" dxfId="72" priority="119">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J78:K78">
     <cfRule type="expression" dxfId="71" priority="118">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J78:K78">
+  <conditionalFormatting sqref="H78">
     <cfRule type="expression" dxfId="70" priority="117">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H78">
+  <conditionalFormatting sqref="I78">
     <cfRule type="expression" dxfId="69" priority="116">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I78">
-    <cfRule type="expression" dxfId="68" priority="115">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J41:K41 H41">
+    <cfRule type="expression" dxfId="68" priority="114">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
     <cfRule type="expression" dxfId="67" priority="113">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I41">
-    <cfRule type="expression" dxfId="66" priority="112">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J83">
+    <cfRule type="expression" dxfId="66" priority="104">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H83">
     <cfRule type="expression" dxfId="65" priority="103">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H83">
+  <conditionalFormatting sqref="I83">
     <cfRule type="expression" dxfId="64" priority="102">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I83">
+  <conditionalFormatting sqref="K83:V83">
     <cfRule type="expression" dxfId="63" priority="101">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K83:V83">
-    <cfRule type="expression" dxfId="62" priority="100">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K83:V83">
-    <cfRule type="expression" dxfId="61" priority="98">
+    <cfRule type="expression" dxfId="62" priority="99">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51 G51">
+    <cfRule type="expression" dxfId="61" priority="97">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51:F51">
     <cfRule type="expression" dxfId="60" priority="96">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51:F51">
+  <conditionalFormatting sqref="B51 E51 G51">
     <cfRule type="expression" dxfId="59" priority="95">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -11938,73 +11950,73 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51 E51 G51">
+  <conditionalFormatting sqref="F51">
     <cfRule type="expression" dxfId="57" priority="93">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F51">
+  <conditionalFormatting sqref="J51:V51 H51">
     <cfRule type="expression" dxfId="56" priority="92">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J51:V51 H51">
-    <cfRule type="expression" dxfId="55" priority="91">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I51">
-    <cfRule type="expression" dxfId="54" priority="89">
+    <cfRule type="expression" dxfId="55" priority="90">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:F50">
+    <cfRule type="expression" dxfId="54" priority="85">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J49:V49 H49">
     <cfRule type="expression" dxfId="53" priority="84">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J49:V49 H49">
-    <cfRule type="expression" dxfId="52" priority="83">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="expression" dxfId="51" priority="81">
+    <cfRule type="expression" dxfId="52" priority="82">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F62">
-    <cfRule type="expression" dxfId="50" priority="75">
+    <cfRule type="expression" dxfId="51" priority="76">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G79">
-    <cfRule type="expression" dxfId="49" priority="71">
+    <cfRule type="expression" dxfId="50" priority="72">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K79">
+    <cfRule type="expression" dxfId="49" priority="62">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J79:K79">
     <cfRule type="expression" dxfId="48" priority="61">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J79:K79">
+  <conditionalFormatting sqref="H79">
     <cfRule type="expression" dxfId="47" priority="60">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H79">
+  <conditionalFormatting sqref="I79">
     <cfRule type="expression" dxfId="46" priority="59">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I79">
-    <cfRule type="expression" dxfId="45" priority="58">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L79:V79">
-    <cfRule type="expression" dxfId="44" priority="65">
+    <cfRule type="expression" dxfId="45" priority="66">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L79:V79">
+    <cfRule type="expression" dxfId="44" priority="64">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12013,152 +12025,152 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L79:V79">
-    <cfRule type="expression" dxfId="42" priority="62">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B48:G48">
+    <cfRule type="expression" dxfId="42" priority="58">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48">
     <cfRule type="expression" dxfId="41" priority="57">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48">
+  <conditionalFormatting sqref="E48:F48">
     <cfRule type="expression" dxfId="40" priority="56">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48:F48">
-    <cfRule type="expression" dxfId="39" priority="55">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J48:V48 H48">
-    <cfRule type="expression" dxfId="38" priority="47">
+    <cfRule type="expression" dxfId="39" priority="48">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48">
+    <cfRule type="expression" dxfId="38" priority="46">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F85">
     <cfRule type="expression" dxfId="37" priority="45">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F85">
+  <conditionalFormatting sqref="B22:G22">
     <cfRule type="expression" dxfId="36" priority="44">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:G22">
-    <cfRule type="expression" dxfId="35" priority="43">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="expression" dxfId="34" priority="33">
+    <cfRule type="expression" dxfId="35" priority="34">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:G19">
+    <cfRule type="expression" dxfId="34" priority="43">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19 E19:G19">
     <cfRule type="expression" dxfId="33" priority="42">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19 E19:G19">
-    <cfRule type="expression" dxfId="32" priority="41">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L19:V19">
-    <cfRule type="expression" dxfId="31" priority="39">
+    <cfRule type="expression" dxfId="32" priority="40">
       <formula>L$1=$H19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19:V19">
-    <cfRule type="expression" dxfId="30" priority="40">
+    <cfRule type="expression" dxfId="31" priority="41">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19:V19">
-    <cfRule type="expression" dxfId="29" priority="37">
+    <cfRule type="expression" dxfId="30" priority="38">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19:V19">
-    <cfRule type="expression" dxfId="28" priority="38">
+    <cfRule type="expression" dxfId="29" priority="39">
       <formula>L$1=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="expression" dxfId="27" priority="34">
+    <cfRule type="expression" dxfId="28" priority="35">
       <formula>K$1=$H19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="expression" dxfId="26" priority="35">
+    <cfRule type="expression" dxfId="27" priority="36">
       <formula>K$1=$I19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19 J19:K19">
-    <cfRule type="expression" dxfId="25" priority="36">
+    <cfRule type="expression" dxfId="26" priority="37">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:V45">
-    <cfRule type="expression" dxfId="24" priority="31">
+    <cfRule type="expression" dxfId="25" priority="32">
       <formula>K$1=$H45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45:V45">
-    <cfRule type="expression" dxfId="23" priority="32">
+    <cfRule type="expression" dxfId="24" priority="33">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45:V45">
+    <cfRule type="expression" dxfId="23" priority="31">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J45:K45 H45">
     <cfRule type="expression" dxfId="22" priority="30">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J45:K45 H45">
+  <conditionalFormatting sqref="I45">
     <cfRule type="expression" dxfId="21" priority="29">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
-    <cfRule type="expression" dxfId="20" priority="28">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K22:V22">
-    <cfRule type="expression" dxfId="19" priority="25">
+    <cfRule type="expression" dxfId="20" priority="26">
       <formula>K$1=$H22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="expression" dxfId="18" priority="26">
+    <cfRule type="expression" dxfId="19" priority="27">
       <formula>K$1=$I22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22:V22">
-    <cfRule type="expression" dxfId="17" priority="27">
+    <cfRule type="expression" dxfId="18" priority="28">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22 J22:K22">
+    <cfRule type="expression" dxfId="17" priority="25">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
     <cfRule type="expression" dxfId="16" priority="24">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
+  <conditionalFormatting sqref="E63">
     <cfRule type="expression" dxfId="15" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="14" priority="22">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B43:E43 G43">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43">
     <cfRule type="expression" dxfId="13" priority="14">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -12173,32 +12185,32 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="10" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K43:V43">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>K$1=$H43</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L43:V43">
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L43:V43">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43:K43 H43">
     <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J43:K43 H43">
+  <conditionalFormatting sqref="I43">
     <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43">
+  <conditionalFormatting sqref="E50:F50">
     <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -12208,22 +12220,22 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E50:F50">
+  <conditionalFormatting sqref="K50:V50">
     <cfRule type="expression" dxfId="3" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K50:V50">
+      <formula>K$1=$H50</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J50:V50 H50">
     <cfRule type="expression" dxfId="2" priority="3">
-      <formula>K$1=$H50</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J50:V50 H50">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I50">
+  <conditionalFormatting sqref="F44">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Rename SF Sersa to SF Bekesar; mark Miguel as enemy
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troymurray/Documents/Code/swgoh-squad-arena-payout-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C538CA7C-A0F7-E94F-8B5B-67484EE15E11}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD4445A-51D9-CE4C-8BBA-E8E8806A79DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="59920" yWindow="2420" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="selected" guid="{6B6C704A-4C22-4616-B5BC-59850AE98E27}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="250">
   <si>
     <t>Name</t>
   </si>
@@ -180,9 +180,6 @@
     <t>:rage:</t>
   </si>
   <si>
-    <t>SF Sersa</t>
-  </si>
-  <si>
     <t>SF Berne</t>
   </si>
   <si>
@@ -354,9 +351,6 @@
     <t>:clock8:</t>
   </si>
   <si>
-    <t>:flag_mx:</t>
-  </si>
-  <si>
     <t>Tardigrada</t>
   </si>
   <si>
@@ -793,6 +787,9 @@
   </si>
   <si>
     <t>https://swgoh.gg/p/343913881/</t>
+  </si>
+  <si>
+    <t>SF Bekesar</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1226,14 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="302">
+  <dxfs count="303">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF305496"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3683,8 +3687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3787,7 +3791,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -3797,10 +3801,10 @@
       </c>
       <c r="E2" s="20"/>
       <c r="F2" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>12</v>
@@ -3863,7 +3867,7 @@
     <row r="3" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="47"/>
       <c r="B3" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="7">
         <v>2</v>
@@ -3878,7 +3882,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>12</v>
@@ -3941,7 +3945,7 @@
     <row r="4" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C4" s="7">
         <v>3</v>
@@ -3951,13 +3955,13 @@
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I4" s="23">
         <v>0.33333333333333331</v>
@@ -4017,7 +4021,7 @@
     <row r="5" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5" s="7">
         <v>4</v>
@@ -4027,10 +4031,10 @@
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>25</v>
@@ -4102,13 +4106,13 @@
         <v>5</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>25</v>
@@ -4171,7 +4175,7 @@
     <row r="7" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C7" s="7">
         <v>6</v>
@@ -4181,11 +4185,11 @@
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G7" s="29"/>
       <c r="H7" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I7" s="23">
         <v>0.41666666666666669</v>
@@ -4245,7 +4249,7 @@
     <row r="8" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C8" s="7">
         <v>7</v>
@@ -4255,11 +4259,11 @@
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G8" s="29"/>
       <c r="H8" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I8" s="23">
         <v>0.45833333333333331</v>
@@ -4328,16 +4332,16 @@
         <v>8</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I9" s="23">
         <v>0.45833333333333331</v>
@@ -4397,7 +4401,7 @@
     <row r="10" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
       <c r="B10" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="7">
         <v>9</v>
@@ -4406,16 +4410,16 @@
         <v>9</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I10" s="23">
         <v>0.45833333333333331</v>
@@ -4475,7 +4479,7 @@
     <row r="11" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="43"/>
       <c r="B11" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C11" s="7">
         <v>10</v>
@@ -4485,11 +4489,11 @@
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I11" s="23">
         <v>0.5</v>
@@ -4549,7 +4553,7 @@
     <row r="12" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="7">
         <v>11</v>
@@ -4558,14 +4562,14 @@
         <v>11</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I12" s="23">
         <v>0.5</v>
@@ -4625,7 +4629,7 @@
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="47"/>
       <c r="B13" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13" s="7">
         <v>12</v>
@@ -4637,13 +4641,13 @@
         <v>27</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I13" s="23">
         <v>0.5</v>
@@ -4703,7 +4707,7 @@
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="47"/>
       <c r="B14" s="18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C14" s="7">
         <v>13</v>
@@ -4713,11 +4717,11 @@
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I14" s="23">
         <v>0.54166666666666663</v>
@@ -4777,7 +4781,7 @@
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="47"/>
       <c r="B15" s="18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C15" s="7">
         <v>14</v>
@@ -4787,11 +4791,11 @@
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I15" s="23">
         <v>0.58333333333333337</v>
@@ -4866,10 +4870,10 @@
         <v>18</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I16" s="23">
         <v>0.58333333333333337</v>
@@ -4929,7 +4933,7 @@
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="43"/>
       <c r="B17" s="36" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C17" s="7">
         <v>16</v>
@@ -4939,7 +4943,7 @@
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="27" t="s">
@@ -5018,7 +5022,7 @@
         <v>20</v>
       </c>
       <c r="G18" s="45" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H18" s="27" t="s">
         <v>10</v>
@@ -5081,7 +5085,7 @@
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="53"/>
       <c r="B19" s="18" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C19" s="7">
         <v>20</v>
@@ -5090,13 +5094,13 @@
         <v>20</v>
       </c>
       <c r="E19" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="G19" s="51" t="s">
         <v>235</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="G19" s="51" t="s">
-        <v>237</v>
       </c>
       <c r="H19" s="27" t="s">
         <v>10</v>
@@ -5159,7 +5163,7 @@
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="47"/>
       <c r="B20" s="18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C20" s="7">
         <v>18</v>
@@ -5169,13 +5173,13 @@
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H20" s="29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I20" s="23">
         <v>0.66666666666666663</v>
@@ -5247,13 +5251,13 @@
         <v>19</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G21" s="22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I21" s="23">
         <v>0.66666666666666663</v>
@@ -5313,7 +5317,7 @@
     <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="54"/>
       <c r="B22" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="7">
         <v>70</v>
@@ -5328,10 +5332,10 @@
         <v>20</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I22" s="23">
   